<commit_message>
Latest trades added and updated rosters/picks
</commit_message>
<xml_diff>
--- a/OffSeason.xlsx
+++ b/OffSeason.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="664">
   <si>
     <t>Chubber for Chubb - John Olson</t>
   </si>
@@ -2007,6 +2007,18 @@
   </si>
   <si>
     <t>2021 3rd (vanja)</t>
+  </si>
+  <si>
+    <t>Sony</t>
+  </si>
+  <si>
+    <t>2020 4.x</t>
+  </si>
+  <si>
+    <t>2021 2nd (Vanja)</t>
+  </si>
+  <si>
+    <t>2021 3rd (alan)</t>
   </si>
 </sst>
 </file>
@@ -2205,7 +2217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2238,21 +2250,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2260,10 +2257,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2548,8 +2563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11:K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2564,11 +2579,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="F1" t="s">
         <v>42</v>
       </c>
@@ -2589,37 +2604,37 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="K2" t="s">
         <v>77</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="N2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="O2" t="s">
         <v>112</v>
       </c>
-      <c r="R2" s="21" t="s">
+      <c r="R2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="S2" t="s">
         <v>144</v>
       </c>
-      <c r="V2" s="21" t="s">
+      <c r="V2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="W2" t="s">
@@ -2630,27 +2645,27 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="23"/>
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="21"/>
+      <c r="F3" s="23"/>
       <c r="G3" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="21"/>
+      <c r="J3" s="23"/>
       <c r="K3" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="21"/>
+      <c r="N3" s="23"/>
       <c r="O3" t="s">
         <v>104</v>
       </c>
-      <c r="R3" s="21"/>
+      <c r="R3" s="23"/>
       <c r="S3" t="s">
         <v>145</v>
       </c>
-      <c r="V3" s="21"/>
+      <c r="V3" s="23"/>
       <c r="W3" t="s">
         <v>179</v>
       </c>
@@ -2659,35 +2674,35 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="21"/>
+      <c r="F4" s="23"/>
       <c r="G4" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="24" t="s">
         <v>5</v>
       </c>
       <c r="K4" t="s">
         <v>248</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="N4" s="24" t="s">
         <v>5</v>
       </c>
       <c r="O4" t="s">
         <v>113</v>
       </c>
-      <c r="R4" s="20" t="s">
+      <c r="R4" s="24" t="s">
         <v>5</v>
       </c>
       <c r="S4" t="s">
         <v>146</v>
       </c>
-      <c r="V4" s="21"/>
+      <c r="V4" s="23"/>
       <c r="W4" t="s">
         <v>180</v>
       </c>
@@ -2696,27 +2711,27 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="24"/>
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="23"/>
       <c r="G5" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="20"/>
+      <c r="J5" s="24"/>
       <c r="K5" t="s">
         <v>81</v>
       </c>
-      <c r="N5" s="20"/>
+      <c r="N5" s="24"/>
       <c r="O5" t="s">
         <v>114</v>
       </c>
-      <c r="R5" s="20"/>
+      <c r="R5" s="24"/>
       <c r="S5" t="s">
         <v>147</v>
       </c>
-      <c r="V5" s="21"/>
+      <c r="V5" s="23"/>
       <c r="W5" t="s">
         <v>181</v>
       </c>
@@ -2725,29 +2740,29 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="20"/>
+      <c r="B6" s="24"/>
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="24" t="s">
         <v>5</v>
       </c>
       <c r="G6" t="s">
         <v>215</v>
       </c>
-      <c r="J6" s="20"/>
+      <c r="J6" s="24"/>
       <c r="K6" t="s">
         <v>82</v>
       </c>
-      <c r="N6" s="20"/>
+      <c r="N6" s="24"/>
       <c r="O6" t="s">
         <v>115</v>
       </c>
-      <c r="R6" s="20"/>
+      <c r="R6" s="24"/>
       <c r="S6" t="s">
         <v>148</v>
       </c>
-      <c r="V6" s="20" t="s">
+      <c r="V6" s="24" t="s">
         <v>5</v>
       </c>
       <c r="W6" t="s">
@@ -2758,27 +2773,27 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="20"/>
+      <c r="B7" s="24"/>
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="20"/>
+      <c r="F7" s="24"/>
       <c r="G7" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="20"/>
+      <c r="J7" s="24"/>
       <c r="K7" t="s">
         <v>84</v>
       </c>
-      <c r="N7" s="20"/>
+      <c r="N7" s="24"/>
       <c r="O7" t="s">
         <v>116</v>
       </c>
-      <c r="R7" s="20"/>
+      <c r="R7" s="24"/>
       <c r="S7" t="s">
         <v>149</v>
       </c>
-      <c r="V7" s="20"/>
+      <c r="V7" s="24"/>
       <c r="W7" t="s">
         <v>250</v>
       </c>
@@ -2787,27 +2802,27 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="20"/>
+      <c r="B8" s="24"/>
       <c r="C8" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="20"/>
+      <c r="F8" s="24"/>
       <c r="G8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J8" s="20"/>
+        <v>50</v>
+      </c>
+      <c r="J8" s="24"/>
       <c r="K8" t="s">
-        <v>85</v>
-      </c>
-      <c r="N8" s="20"/>
+        <v>48</v>
+      </c>
+      <c r="N8" s="24"/>
       <c r="O8" t="s">
         <v>117</v>
       </c>
-      <c r="R8" s="20"/>
+      <c r="R8" s="24"/>
       <c r="S8" t="s">
         <v>150</v>
       </c>
-      <c r="V8" s="20"/>
+      <c r="V8" s="24"/>
       <c r="W8" t="s">
         <v>184</v>
       </c>
@@ -2816,27 +2831,27 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="20"/>
+      <c r="B9" s="24"/>
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="20"/>
+      <c r="F9" s="24"/>
       <c r="G9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J9" s="20"/>
+        <v>49</v>
+      </c>
+      <c r="J9" s="24"/>
       <c r="K9" t="s">
-        <v>10</v>
-      </c>
-      <c r="N9" s="20"/>
+        <v>85</v>
+      </c>
+      <c r="N9" s="24"/>
       <c r="O9" t="s">
         <v>118</v>
       </c>
-      <c r="R9" s="20"/>
+      <c r="R9" s="24"/>
       <c r="S9" t="s">
         <v>151</v>
       </c>
-      <c r="V9" s="20"/>
+      <c r="V9" s="24"/>
       <c r="W9" t="s">
         <v>252</v>
       </c>
@@ -2845,31 +2860,35 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="20"/>
+      <c r="F10" s="25" t="s">
+        <v>12</v>
+      </c>
       <c r="G10" t="s">
-        <v>49</v>
-      </c>
-      <c r="J10" s="20"/>
+        <v>54</v>
+      </c>
+      <c r="J10" s="25" t="s">
+        <v>12</v>
+      </c>
       <c r="K10" t="s">
-        <v>48</v>
-      </c>
-      <c r="N10" s="20"/>
+        <v>188</v>
+      </c>
+      <c r="N10" s="24"/>
       <c r="O10" t="s">
         <v>119</v>
       </c>
-      <c r="R10" s="23" t="s">
+      <c r="R10" s="25" t="s">
         <v>12</v>
       </c>
       <c r="S10" t="s">
         <v>152</v>
       </c>
-      <c r="V10" s="20"/>
+      <c r="V10" s="24"/>
       <c r="W10" t="s">
         <v>186</v>
       </c>
@@ -2878,33 +2897,29 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="23"/>
+      <c r="B11" s="25"/>
       <c r="C11" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="23" t="s">
-        <v>12</v>
-      </c>
+      <c r="F11" s="25"/>
       <c r="G11" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="23" t="s">
-        <v>12</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="J11" s="25"/>
       <c r="K11" t="s">
         <v>88</v>
       </c>
-      <c r="N11" s="23" t="s">
+      <c r="N11" s="25" t="s">
         <v>12</v>
       </c>
       <c r="O11" t="s">
         <v>120</v>
       </c>
-      <c r="R11" s="23"/>
+      <c r="R11" s="25"/>
       <c r="S11" t="s">
         <v>153</v>
       </c>
-      <c r="V11" s="20"/>
+      <c r="V11" s="24"/>
       <c r="W11" t="s">
         <v>187</v>
       </c>
@@ -2913,27 +2928,27 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="23"/>
+      <c r="B12" s="25"/>
       <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="23"/>
+      <c r="F12" s="25"/>
       <c r="G12" t="s">
-        <v>56</v>
-      </c>
-      <c r="J12" s="23"/>
+        <v>58</v>
+      </c>
+      <c r="J12" s="25"/>
       <c r="K12" t="s">
         <v>16</v>
       </c>
-      <c r="N12" s="23"/>
+      <c r="N12" s="25"/>
       <c r="O12" t="s">
         <v>121</v>
       </c>
-      <c r="R12" s="23"/>
+      <c r="R12" s="25"/>
       <c r="S12" t="s">
         <v>154</v>
       </c>
-      <c r="V12" s="20"/>
+      <c r="V12" s="24"/>
       <c r="W12" t="s">
         <v>53</v>
       </c>
@@ -2942,58 +2957,58 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="23"/>
+      <c r="B13" s="25"/>
       <c r="C13" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="23"/>
+      <c r="F13" s="25"/>
       <c r="G13" t="s">
-        <v>58</v>
-      </c>
-      <c r="J13" s="23"/>
+        <v>59</v>
+      </c>
+      <c r="J13" s="25"/>
       <c r="K13" t="s">
         <v>17</v>
       </c>
-      <c r="N13" s="23"/>
+      <c r="N13" s="25"/>
       <c r="O13" t="s">
         <v>122</v>
       </c>
-      <c r="R13" s="23"/>
+      <c r="R13" s="25"/>
       <c r="S13" t="s">
         <v>155</v>
       </c>
-      <c r="V13" s="23" t="s">
-        <v>12</v>
-      </c>
+      <c r="V13" s="24"/>
       <c r="W13" t="s">
-        <v>188</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="23"/>
+      <c r="B14" s="25"/>
       <c r="C14" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="23"/>
+      <c r="F14" s="25"/>
       <c r="G14" t="s">
-        <v>59</v>
-      </c>
-      <c r="J14" s="23"/>
+        <v>226</v>
+      </c>
+      <c r="J14" s="25"/>
       <c r="K14" t="s">
         <v>22</v>
       </c>
-      <c r="N14" s="23"/>
+      <c r="N14" s="25"/>
       <c r="O14" t="s">
         <v>123</v>
       </c>
-      <c r="R14" s="23"/>
+      <c r="R14" s="25"/>
       <c r="S14" t="s">
         <v>156</v>
       </c>
-      <c r="V14" s="23"/>
+      <c r="V14" s="29" t="s">
+        <v>12</v>
+      </c>
       <c r="W14" t="s">
         <v>256</v>
       </c>
@@ -3002,27 +3017,27 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="23"/>
+      <c r="B15" s="25"/>
       <c r="C15" t="s">
         <v>87</v>
       </c>
-      <c r="F15" s="23"/>
+      <c r="F15" s="25"/>
       <c r="G15" t="s">
-        <v>226</v>
-      </c>
-      <c r="J15" s="23"/>
+        <v>225</v>
+      </c>
+      <c r="J15" s="25"/>
       <c r="K15" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="23"/>
+      <c r="N15" s="25"/>
       <c r="O15" t="s">
         <v>124</v>
       </c>
-      <c r="R15" s="23"/>
+      <c r="R15" s="25"/>
       <c r="S15" t="s">
         <v>157</v>
       </c>
-      <c r="V15" s="23"/>
+      <c r="V15" s="29"/>
       <c r="W15" t="s">
         <v>189</v>
       </c>
@@ -3031,31 +3046,33 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="23"/>
+      <c r="F16" s="26" t="s">
+        <v>18</v>
+      </c>
       <c r="G16" t="s">
-        <v>225</v>
-      </c>
-      <c r="J16" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="26" t="s">
         <v>18</v>
       </c>
       <c r="K16" t="s">
         <v>95</v>
       </c>
-      <c r="N16" s="23"/>
+      <c r="N16" s="25"/>
       <c r="O16" t="s">
         <v>125</v>
       </c>
-      <c r="R16" s="23"/>
+      <c r="R16" s="25"/>
       <c r="S16" t="s">
         <v>158</v>
       </c>
-      <c r="V16" s="23"/>
+      <c r="V16" s="29"/>
       <c r="W16" t="s">
         <v>190</v>
       </c>
@@ -3064,31 +3081,29 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="22"/>
+      <c r="B17" s="26"/>
       <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="22" t="s">
-        <v>18</v>
-      </c>
+      <c r="F17" s="26"/>
       <c r="G17" t="s">
-        <v>60</v>
-      </c>
-      <c r="J17" s="22"/>
+        <v>62</v>
+      </c>
+      <c r="J17" s="26"/>
       <c r="K17" t="s">
         <v>96</v>
       </c>
-      <c r="N17" s="22" t="s">
+      <c r="N17" s="26" t="s">
         <v>18</v>
       </c>
       <c r="O17" t="s">
         <v>126</v>
       </c>
-      <c r="R17" s="23"/>
+      <c r="R17" s="25"/>
       <c r="S17" t="s">
         <v>159</v>
       </c>
-      <c r="V17" s="23"/>
+      <c r="V17" s="29"/>
       <c r="W17" t="s">
         <v>191</v>
       </c>
@@ -3097,27 +3112,27 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="22"/>
+      <c r="B18" s="26"/>
       <c r="C18" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="22"/>
+      <c r="F18" s="26"/>
       <c r="G18" t="s">
-        <v>62</v>
-      </c>
-      <c r="J18" s="22"/>
+        <v>63</v>
+      </c>
+      <c r="J18" s="26"/>
       <c r="K18" t="s">
         <v>97</v>
       </c>
-      <c r="N18" s="22"/>
+      <c r="N18" s="26"/>
       <c r="O18" t="s">
         <v>127</v>
       </c>
-      <c r="R18" s="23"/>
+      <c r="R18" s="25"/>
       <c r="S18" t="s">
         <v>160</v>
       </c>
-      <c r="V18" s="23"/>
+      <c r="V18" s="29"/>
       <c r="W18" t="s">
         <v>91</v>
       </c>
@@ -3126,31 +3141,33 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="27" t="s">
         <v>24</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="22"/>
+      <c r="F19" s="27" t="s">
+        <v>24</v>
+      </c>
       <c r="G19" t="s">
-        <v>63</v>
-      </c>
-      <c r="J19" s="22"/>
+        <v>64</v>
+      </c>
+      <c r="J19" s="26"/>
       <c r="K19" t="s">
         <v>98</v>
       </c>
-      <c r="N19" s="24" t="s">
+      <c r="N19" s="27" t="s">
         <v>24</v>
       </c>
       <c r="O19" t="s">
         <v>128</v>
       </c>
-      <c r="R19" s="23"/>
+      <c r="R19" s="25"/>
       <c r="S19" t="s">
         <v>161</v>
       </c>
-      <c r="V19" s="23"/>
+      <c r="V19" s="29"/>
       <c r="W19" t="s">
         <v>261</v>
       </c>
@@ -3159,33 +3176,31 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="24"/>
+      <c r="B20" s="27"/>
       <c r="C20" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="24" t="s">
-        <v>24</v>
-      </c>
+      <c r="F20" s="27"/>
       <c r="G20" t="s">
-        <v>64</v>
-      </c>
-      <c r="J20" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="J20" s="27" t="s">
         <v>24</v>
       </c>
       <c r="K20" t="s">
         <v>99</v>
       </c>
-      <c r="N20" s="24"/>
+      <c r="N20" s="27"/>
       <c r="O20" t="s">
         <v>129</v>
       </c>
-      <c r="R20" s="22" t="s">
+      <c r="R20" s="26" t="s">
         <v>18</v>
       </c>
       <c r="S20" t="s">
         <v>162</v>
       </c>
-      <c r="V20" s="23"/>
+      <c r="V20" s="29"/>
       <c r="W20" t="s">
         <v>94</v>
       </c>
@@ -3194,27 +3209,27 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="24"/>
+      <c r="B21" s="27"/>
       <c r="C21" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="24"/>
+      <c r="F21" s="27"/>
       <c r="G21" t="s">
-        <v>65</v>
-      </c>
-      <c r="J21" s="24"/>
+        <v>66</v>
+      </c>
+      <c r="J21" s="27"/>
       <c r="K21" t="s">
         <v>28</v>
       </c>
-      <c r="N21" s="24"/>
+      <c r="N21" s="27"/>
       <c r="O21" t="s">
         <v>130</v>
       </c>
-      <c r="R21" s="22"/>
+      <c r="R21" s="26"/>
       <c r="S21" t="s">
         <v>163</v>
       </c>
-      <c r="V21" s="23"/>
+      <c r="V21" s="29"/>
       <c r="W21" t="s">
         <v>192</v>
       </c>
@@ -3223,29 +3238,29 @@
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="24"/>
+      <c r="B22" s="27"/>
       <c r="C22" t="s">
         <v>100</v>
       </c>
-      <c r="F22" s="24"/>
+      <c r="F22" s="27"/>
       <c r="G22" t="s">
-        <v>66</v>
-      </c>
-      <c r="J22" s="24"/>
+        <v>67</v>
+      </c>
+      <c r="J22" s="27"/>
       <c r="K22" t="s">
         <v>29</v>
       </c>
-      <c r="N22" s="24"/>
+      <c r="N22" s="27"/>
       <c r="O22" t="s">
         <v>131</v>
       </c>
-      <c r="R22" s="24" t="s">
+      <c r="R22" s="27" t="s">
         <v>24</v>
       </c>
       <c r="S22" t="s">
         <v>164</v>
       </c>
-      <c r="V22" s="23"/>
+      <c r="V22" s="29"/>
       <c r="W22" t="s">
         <v>193</v>
       </c>
@@ -3254,31 +3269,33 @@
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="20" t="s">
         <v>30</v>
       </c>
       <c r="C23" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="24"/>
+      <c r="F23" s="20" t="s">
+        <v>30</v>
+      </c>
       <c r="G23" t="s">
-        <v>67</v>
-      </c>
-      <c r="J23" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="J23" s="20" t="s">
         <v>30</v>
       </c>
       <c r="K23" t="s">
         <v>103</v>
       </c>
-      <c r="N23" s="24"/>
+      <c r="N23" s="27"/>
       <c r="O23" t="s">
         <v>132</v>
       </c>
-      <c r="R23" s="24"/>
+      <c r="R23" s="27"/>
       <c r="S23" t="s">
         <v>165</v>
       </c>
-      <c r="V23" s="23"/>
+      <c r="V23" s="29"/>
       <c r="W23" t="s">
         <v>195</v>
       </c>
@@ -3287,31 +3304,29 @@
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="25"/>
+      <c r="B24" s="20"/>
       <c r="C24" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="25" t="s">
-        <v>30</v>
-      </c>
+      <c r="F24" s="20"/>
       <c r="G24" t="s">
-        <v>69</v>
-      </c>
-      <c r="J24" s="25"/>
+        <v>70</v>
+      </c>
+      <c r="J24" s="20"/>
       <c r="K24" t="s">
         <v>104</v>
       </c>
-      <c r="N24" s="25" t="s">
+      <c r="N24" s="20" t="s">
         <v>30</v>
       </c>
       <c r="O24" t="s">
         <v>133</v>
       </c>
-      <c r="R24" s="24"/>
+      <c r="R24" s="27"/>
       <c r="S24" t="s">
         <v>166</v>
       </c>
-      <c r="V24" s="23"/>
+      <c r="V24" s="29"/>
       <c r="W24" t="s">
         <v>196</v>
       </c>
@@ -3320,27 +3335,27 @@
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="25"/>
+      <c r="B25" s="20"/>
       <c r="C25" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="25"/>
+      <c r="F25" s="20"/>
       <c r="G25" t="s">
-        <v>70</v>
-      </c>
-      <c r="J25" s="25"/>
+        <v>71</v>
+      </c>
+      <c r="J25" s="20"/>
       <c r="K25" t="s">
         <v>105</v>
       </c>
-      <c r="N25" s="25"/>
+      <c r="N25" s="20"/>
       <c r="O25" t="s">
         <v>134</v>
       </c>
-      <c r="R25" s="24"/>
+      <c r="R25" s="27"/>
       <c r="S25" t="s">
         <v>167</v>
       </c>
-      <c r="V25" s="22" t="s">
+      <c r="V25" s="26" t="s">
         <v>18</v>
       </c>
       <c r="W25" t="s">
@@ -3351,31 +3366,31 @@
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="21" t="s">
         <v>36</v>
       </c>
       <c r="C26" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="25"/>
+      <c r="F26" s="20"/>
       <c r="G26" t="s">
-        <v>71</v>
-      </c>
-      <c r="J26" s="25"/>
+        <v>68</v>
+      </c>
+      <c r="J26" s="20"/>
       <c r="K26" t="s">
         <v>106</v>
       </c>
-      <c r="N26" s="25"/>
+      <c r="N26" s="20"/>
       <c r="O26" t="s">
         <v>135</v>
       </c>
-      <c r="R26" s="25" t="s">
+      <c r="R26" s="20" t="s">
         <v>30</v>
       </c>
       <c r="S26" t="s">
         <v>168</v>
       </c>
-      <c r="V26" s="22"/>
+      <c r="V26" s="26"/>
       <c r="W26" t="s">
         <v>198</v>
       </c>
@@ -3384,29 +3399,31 @@
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="26"/>
+      <c r="B27" s="21"/>
       <c r="C27" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="25"/>
+      <c r="F27" s="21" t="s">
+        <v>36</v>
+      </c>
       <c r="G27" t="s">
-        <v>68</v>
-      </c>
-      <c r="J27" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="J27" s="21" t="s">
         <v>36</v>
       </c>
       <c r="K27" t="s">
         <v>40</v>
       </c>
-      <c r="N27" s="25"/>
+      <c r="N27" s="20"/>
       <c r="O27" t="s">
         <v>136</v>
       </c>
-      <c r="R27" s="25"/>
+      <c r="R27" s="20"/>
       <c r="S27" t="s">
         <v>169</v>
       </c>
-      <c r="V27" s="22"/>
+      <c r="V27" s="26"/>
       <c r="W27" t="s">
         <v>199</v>
       </c>
@@ -3415,29 +3432,27 @@
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="26"/>
+      <c r="B28" s="21"/>
       <c r="C28" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="26" t="s">
-        <v>36</v>
-      </c>
+      <c r="F28" s="21"/>
       <c r="G28" t="s">
-        <v>72</v>
-      </c>
-      <c r="J28" s="26"/>
+        <v>73</v>
+      </c>
+      <c r="J28" s="21"/>
       <c r="K28" t="s">
         <v>108</v>
       </c>
-      <c r="N28" s="25"/>
+      <c r="N28" s="20"/>
       <c r="O28" t="s">
         <v>137</v>
       </c>
-      <c r="R28" s="25"/>
+      <c r="R28" s="20"/>
       <c r="S28" t="s">
         <v>170</v>
       </c>
-      <c r="V28" s="24" t="s">
+      <c r="V28" s="27" t="s">
         <v>24</v>
       </c>
       <c r="W28" t="s">
@@ -3448,27 +3463,27 @@
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="26"/>
+      <c r="B29" s="21"/>
       <c r="C29" t="s">
         <v>107</v>
       </c>
-      <c r="F29" s="26"/>
+      <c r="F29" s="21"/>
       <c r="G29" t="s">
-        <v>73</v>
-      </c>
-      <c r="J29" s="26"/>
+        <v>74</v>
+      </c>
+      <c r="J29" s="21"/>
       <c r="K29" t="s">
         <v>110</v>
       </c>
-      <c r="N29" s="25"/>
+      <c r="N29" s="20"/>
       <c r="O29" t="s">
         <v>138</v>
       </c>
-      <c r="R29" s="25"/>
+      <c r="R29" s="20"/>
       <c r="S29" t="s">
         <v>171</v>
       </c>
-      <c r="V29" s="24"/>
+      <c r="V29" s="27"/>
       <c r="W29" t="s">
         <v>201</v>
       </c>
@@ -3477,25 +3492,25 @@
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="F30" s="26"/>
+      <c r="F30" s="21"/>
       <c r="G30" t="s">
-        <v>74</v>
-      </c>
-      <c r="J30" s="26"/>
+        <v>75</v>
+      </c>
+      <c r="J30" s="21"/>
       <c r="K30" t="s">
         <v>41</v>
       </c>
-      <c r="N30" s="26" t="s">
+      <c r="N30" s="21" t="s">
         <v>36</v>
       </c>
       <c r="O30" t="s">
         <v>139</v>
       </c>
-      <c r="R30" s="25"/>
+      <c r="R30" s="20"/>
       <c r="S30" t="s">
         <v>172</v>
       </c>
-      <c r="V30" s="24"/>
+      <c r="V30" s="27"/>
       <c r="W30" t="s">
         <v>202</v>
       </c>
@@ -3504,35 +3519,35 @@
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="F31" s="26"/>
+      <c r="F31" s="21"/>
       <c r="G31" t="s">
-        <v>75</v>
-      </c>
-      <c r="N31" s="26"/>
+        <v>275</v>
+      </c>
+      <c r="N31" s="21"/>
       <c r="O31" t="s">
         <v>140</v>
       </c>
-      <c r="R31" s="26" t="s">
+      <c r="R31" s="21" t="s">
         <v>36</v>
       </c>
       <c r="S31" t="s">
         <v>173</v>
       </c>
-      <c r="V31" s="24"/>
+      <c r="V31" s="27"/>
       <c r="W31" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="N32" s="26"/>
+      <c r="N32" s="21"/>
       <c r="O32" t="s">
         <v>141</v>
       </c>
-      <c r="R32" s="26"/>
+      <c r="R32" s="21"/>
       <c r="S32" t="s">
         <v>174</v>
       </c>
-      <c r="V32" s="25" t="s">
+      <c r="V32" s="20" t="s">
         <v>30</v>
       </c>
       <c r="W32" t="s">
@@ -3540,43 +3555,43 @@
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="N33" s="26"/>
+      <c r="N33" s="21"/>
       <c r="O33" t="s">
         <v>142</v>
       </c>
-      <c r="R33" s="26"/>
+      <c r="R33" s="21"/>
       <c r="S33" t="s">
         <v>175</v>
       </c>
-      <c r="V33" s="25"/>
+      <c r="V33" s="20"/>
       <c r="W33" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="R34" s="26"/>
+      <c r="R34" s="21"/>
       <c r="S34" t="s">
         <v>176</v>
       </c>
-      <c r="V34" s="25"/>
+      <c r="V34" s="20"/>
       <c r="W34" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V35" s="25"/>
+      <c r="V35" s="20"/>
       <c r="W35" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V36" s="25"/>
+      <c r="V36" s="20"/>
       <c r="W36" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V37" s="26" t="s">
+      <c r="V37" s="21" t="s">
         <v>36</v>
       </c>
       <c r="W37" t="s">
@@ -3584,21 +3599,26 @@
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V38" s="26"/>
+      <c r="V38" s="21"/>
       <c r="W38" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V39" s="26"/>
+      <c r="V39" s="21"/>
       <c r="W39" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V40" s="26"/>
+      <c r="V40" s="21"/>
       <c r="W40" t="s">
         <v>211</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="G41" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.35">
@@ -3617,48 +3637,48 @@
       <c r="R43" t="s">
         <v>315</v>
       </c>
-      <c r="V43" s="28" t="s">
+      <c r="V43" s="22" t="s">
         <v>316</v>
       </c>
-      <c r="W43" s="28"/>
-      <c r="X43" s="28"/>
-      <c r="Y43" s="28"/>
+      <c r="W43" s="22"/>
+      <c r="X43" s="22"/>
+      <c r="Y43" s="22"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>1</v>
       </c>
-      <c r="B44" s="21" t="s">
+      <c r="B44" s="23" t="s">
         <v>1</v>
       </c>
       <c r="C44" t="s">
         <v>44</v>
       </c>
-      <c r="F44" s="21" t="s">
+      <c r="F44" s="23" t="s">
         <v>1</v>
       </c>
       <c r="G44" t="s">
         <v>246</v>
       </c>
-      <c r="J44" s="21" t="s">
+      <c r="J44" s="23" t="s">
         <v>1</v>
       </c>
       <c r="K44" t="s">
         <v>280</v>
       </c>
-      <c r="N44" s="21" t="s">
+      <c r="N44" s="23" t="s">
         <v>1</v>
       </c>
       <c r="O44" t="s">
         <v>317</v>
       </c>
-      <c r="R44" s="21" t="s">
+      <c r="R44" s="23" t="s">
         <v>1</v>
       </c>
       <c r="S44" t="s">
         <v>348</v>
       </c>
-      <c r="V44" s="21" t="s">
+      <c r="V44" s="23" t="s">
         <v>1</v>
       </c>
       <c r="W44" t="s">
@@ -3669,27 +3689,27 @@
       <c r="A45" s="1">
         <v>2</v>
       </c>
-      <c r="B45" s="21"/>
+      <c r="B45" s="23"/>
       <c r="C45" t="s">
         <v>214</v>
       </c>
-      <c r="F45" s="21"/>
+      <c r="F45" s="23"/>
       <c r="G45" t="s">
         <v>247</v>
       </c>
-      <c r="J45" s="21"/>
+      <c r="J45" s="23"/>
       <c r="K45" t="s">
         <v>281</v>
       </c>
-      <c r="N45" s="21"/>
+      <c r="N45" s="23"/>
       <c r="O45" t="s">
         <v>318</v>
       </c>
-      <c r="R45" s="21"/>
+      <c r="R45" s="23"/>
       <c r="S45" t="s">
         <v>349</v>
       </c>
-      <c r="V45" s="21"/>
+      <c r="V45" s="23"/>
       <c r="W45" t="s">
         <v>379</v>
       </c>
@@ -3698,27 +3718,27 @@
       <c r="A46" s="1">
         <v>3</v>
       </c>
-      <c r="B46" s="21"/>
+      <c r="B46" s="23"/>
       <c r="C46" t="s">
         <v>213</v>
       </c>
-      <c r="F46" s="21"/>
+      <c r="F46" s="23"/>
       <c r="G46" t="s">
         <v>79</v>
       </c>
-      <c r="J46" s="21"/>
+      <c r="J46" s="23"/>
       <c r="K46" t="s">
         <v>282</v>
       </c>
-      <c r="N46" s="21"/>
+      <c r="N46" s="23"/>
       <c r="O46" t="s">
         <v>319</v>
       </c>
-      <c r="R46" s="21"/>
+      <c r="R46" s="23"/>
       <c r="S46" t="s">
         <v>78</v>
       </c>
-      <c r="V46" s="21"/>
+      <c r="V46" s="23"/>
       <c r="W46" t="s">
         <v>380</v>
       </c>
@@ -3727,35 +3747,35 @@
       <c r="A47" s="1">
         <v>4</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C47" t="s">
         <v>216</v>
       </c>
-      <c r="F47" s="20" t="s">
+      <c r="F47" s="24" t="s">
         <v>5</v>
       </c>
       <c r="G47" t="s">
         <v>183</v>
       </c>
-      <c r="J47" s="20" t="s">
+      <c r="J47" s="24" t="s">
         <v>5</v>
       </c>
       <c r="K47" t="s">
         <v>283</v>
       </c>
-      <c r="N47" s="20" t="s">
+      <c r="N47" s="24" t="s">
         <v>5</v>
       </c>
       <c r="O47" t="s">
         <v>320</v>
       </c>
-      <c r="R47" s="21"/>
+      <c r="R47" s="23"/>
       <c r="S47" t="s">
         <v>350</v>
       </c>
-      <c r="V47" s="20" t="s">
+      <c r="V47" s="24" t="s">
         <v>5</v>
       </c>
       <c r="W47" t="s">
@@ -3766,29 +3786,29 @@
       <c r="A48" s="1">
         <v>5</v>
       </c>
-      <c r="B48" s="20"/>
+      <c r="B48" s="24"/>
       <c r="C48" t="s">
         <v>217</v>
       </c>
-      <c r="F48" s="20"/>
+      <c r="F48" s="24"/>
       <c r="G48" t="s">
         <v>321</v>
       </c>
-      <c r="J48" s="20"/>
+      <c r="J48" s="24"/>
       <c r="K48" t="s">
         <v>284</v>
       </c>
-      <c r="N48" s="20"/>
+      <c r="N48" s="24"/>
       <c r="O48" t="s">
         <v>251</v>
       </c>
-      <c r="R48" s="20" t="s">
+      <c r="R48" s="24" t="s">
         <v>5</v>
       </c>
       <c r="S48" t="s">
         <v>351</v>
       </c>
-      <c r="V48" s="20"/>
+      <c r="V48" s="24"/>
       <c r="W48" t="s">
         <v>382</v>
       </c>
@@ -3797,27 +3817,27 @@
       <c r="A49" s="1">
         <v>6</v>
       </c>
-      <c r="B49" s="20"/>
+      <c r="B49" s="24"/>
       <c r="C49" t="s">
         <v>221</v>
       </c>
-      <c r="F49" s="20"/>
+      <c r="F49" s="24"/>
       <c r="G49" t="s">
         <v>185</v>
       </c>
-      <c r="J49" s="20"/>
+      <c r="J49" s="24"/>
       <c r="K49" t="s">
         <v>285</v>
       </c>
-      <c r="N49" s="20"/>
+      <c r="N49" s="24"/>
       <c r="O49" t="s">
         <v>322</v>
       </c>
-      <c r="R49" s="20"/>
+      <c r="R49" s="24"/>
       <c r="S49" t="s">
         <v>352</v>
       </c>
-      <c r="V49" s="20"/>
+      <c r="V49" s="24"/>
       <c r="W49" t="s">
         <v>383</v>
       </c>
@@ -3826,31 +3846,31 @@
       <c r="A50" s="1">
         <v>7</v>
       </c>
-      <c r="B50" s="20"/>
+      <c r="B50" s="24"/>
       <c r="C50" t="s">
         <v>222</v>
       </c>
-      <c r="F50" s="20"/>
+      <c r="F50" s="24"/>
       <c r="G50" t="s">
         <v>249</v>
       </c>
-      <c r="J50" s="23" t="s">
+      <c r="J50" s="25" t="s">
         <v>12</v>
       </c>
       <c r="K50" t="s">
         <v>286</v>
       </c>
-      <c r="N50" s="23" t="s">
+      <c r="N50" s="25" t="s">
         <v>12</v>
       </c>
       <c r="O50" t="s">
         <v>323</v>
       </c>
-      <c r="R50" s="20"/>
+      <c r="R50" s="24"/>
       <c r="S50" t="s">
         <v>353</v>
       </c>
-      <c r="V50" s="20"/>
+      <c r="V50" s="24"/>
       <c r="W50" t="s">
         <v>384</v>
       </c>
@@ -3859,29 +3879,29 @@
       <c r="A51" s="1">
         <v>8</v>
       </c>
-      <c r="B51" s="23" t="s">
+      <c r="B51" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C51" t="s">
         <v>57</v>
       </c>
-      <c r="F51" s="20"/>
+      <c r="F51" s="24"/>
       <c r="G51" t="s">
         <v>253</v>
       </c>
-      <c r="J51" s="23"/>
+      <c r="J51" s="25"/>
       <c r="K51" t="s">
         <v>287</v>
       </c>
-      <c r="N51" s="23"/>
+      <c r="N51" s="25"/>
       <c r="O51" t="s">
         <v>324</v>
       </c>
-      <c r="R51" s="20"/>
+      <c r="R51" s="24"/>
       <c r="S51" t="s">
         <v>354</v>
       </c>
-      <c r="V51" s="20"/>
+      <c r="V51" s="24"/>
       <c r="W51" t="s">
         <v>385</v>
       </c>
@@ -3890,27 +3910,27 @@
       <c r="A52" s="1">
         <v>9</v>
       </c>
-      <c r="B52" s="23"/>
+      <c r="B52" s="25"/>
       <c r="C52" t="s">
         <v>218</v>
       </c>
-      <c r="F52" s="20"/>
+      <c r="F52" s="24"/>
       <c r="G52" t="s">
         <v>254</v>
       </c>
-      <c r="J52" s="23"/>
+      <c r="J52" s="25"/>
       <c r="K52" t="s">
         <v>288</v>
       </c>
-      <c r="N52" s="23"/>
+      <c r="N52" s="25"/>
       <c r="O52" t="s">
         <v>325</v>
       </c>
-      <c r="R52" s="20"/>
+      <c r="R52" s="24"/>
       <c r="S52" t="s">
         <v>355</v>
       </c>
-      <c r="V52" s="23" t="s">
+      <c r="V52" s="25" t="s">
         <v>12</v>
       </c>
       <c r="W52" t="s">
@@ -3921,29 +3941,29 @@
       <c r="A53" s="1">
         <v>10</v>
       </c>
-      <c r="B53" s="23"/>
+      <c r="B53" s="25"/>
       <c r="C53" t="s">
         <v>219</v>
       </c>
-      <c r="F53" s="20"/>
+      <c r="F53" s="24"/>
       <c r="G53" t="s">
         <v>255</v>
       </c>
-      <c r="J53" s="23"/>
+      <c r="J53" s="25"/>
       <c r="K53" t="s">
         <v>289</v>
       </c>
-      <c r="N53" s="23"/>
+      <c r="N53" s="25"/>
       <c r="O53" t="s">
         <v>326</v>
       </c>
-      <c r="R53" s="23" t="s">
+      <c r="R53" s="25" t="s">
         <v>12</v>
       </c>
       <c r="S53" t="s">
         <v>356</v>
       </c>
-      <c r="V53" s="23"/>
+      <c r="V53" s="25"/>
       <c r="W53" t="s">
         <v>387</v>
       </c>
@@ -3952,27 +3972,27 @@
       <c r="A54" s="1">
         <v>11</v>
       </c>
-      <c r="B54" s="23"/>
+      <c r="B54" s="25"/>
       <c r="C54" t="s">
         <v>93</v>
       </c>
-      <c r="F54" s="20"/>
+      <c r="F54" s="24"/>
       <c r="G54" t="s">
         <v>83</v>
       </c>
-      <c r="J54" s="23"/>
+      <c r="J54" s="25"/>
       <c r="K54" t="s">
         <v>290</v>
       </c>
-      <c r="N54" s="23"/>
+      <c r="N54" s="25"/>
       <c r="O54" t="s">
         <v>327</v>
       </c>
-      <c r="R54" s="23"/>
+      <c r="R54" s="25"/>
       <c r="S54" t="s">
         <v>357</v>
       </c>
-      <c r="V54" s="23"/>
+      <c r="V54" s="25"/>
       <c r="W54" t="s">
         <v>388</v>
       </c>
@@ -3981,29 +4001,29 @@
       <c r="A55" s="1">
         <v>12</v>
       </c>
-      <c r="B55" s="23"/>
+      <c r="B55" s="25"/>
       <c r="C55" t="s">
         <v>220</v>
       </c>
-      <c r="F55" s="23" t="s">
+      <c r="F55" s="25" t="s">
         <v>12</v>
       </c>
       <c r="G55" t="s">
         <v>194</v>
       </c>
-      <c r="J55" s="23"/>
+      <c r="J55" s="25"/>
       <c r="K55" t="s">
         <v>291</v>
       </c>
-      <c r="N55" s="23"/>
+      <c r="N55" s="25"/>
       <c r="O55" t="s">
         <v>328</v>
       </c>
-      <c r="R55" s="23"/>
+      <c r="R55" s="25"/>
       <c r="S55" t="s">
         <v>358</v>
       </c>
-      <c r="V55" s="23"/>
+      <c r="V55" s="25"/>
       <c r="W55" t="s">
         <v>389</v>
       </c>
@@ -4012,27 +4032,27 @@
       <c r="A56" s="1">
         <v>13</v>
       </c>
-      <c r="B56" s="23"/>
+      <c r="B56" s="25"/>
       <c r="C56" t="s">
         <v>223</v>
       </c>
-      <c r="F56" s="23"/>
+      <c r="F56" s="25"/>
       <c r="G56" t="s">
         <v>258</v>
       </c>
-      <c r="J56" s="23"/>
+      <c r="J56" s="25"/>
       <c r="K56" t="s">
         <v>292</v>
       </c>
-      <c r="N56" s="23"/>
+      <c r="N56" s="25"/>
       <c r="O56" t="s">
         <v>329</v>
       </c>
-      <c r="R56" s="23"/>
+      <c r="R56" s="25"/>
       <c r="S56" t="s">
         <v>359</v>
       </c>
-      <c r="V56" s="23"/>
+      <c r="V56" s="25"/>
       <c r="W56" t="s">
         <v>390</v>
       </c>
@@ -4041,27 +4061,27 @@
       <c r="A57" s="1">
         <v>14</v>
       </c>
-      <c r="B57" s="23"/>
+      <c r="B57" s="25"/>
       <c r="C57" t="s">
         <v>224</v>
       </c>
-      <c r="F57" s="23"/>
+      <c r="F57" s="25"/>
       <c r="G57" t="s">
         <v>90</v>
       </c>
-      <c r="J57" s="23"/>
+      <c r="J57" s="25"/>
       <c r="K57" t="s">
         <v>293</v>
       </c>
-      <c r="N57" s="23"/>
+      <c r="N57" s="25"/>
       <c r="O57" t="s">
         <v>257</v>
       </c>
-      <c r="R57" s="23"/>
+      <c r="R57" s="25"/>
       <c r="S57" t="s">
         <v>360</v>
       </c>
-      <c r="V57" s="23"/>
+      <c r="V57" s="25"/>
       <c r="W57" t="s">
         <v>391</v>
       </c>
@@ -4070,27 +4090,27 @@
       <c r="A58" s="1">
         <v>15</v>
       </c>
-      <c r="B58" s="23"/>
+      <c r="B58" s="25"/>
       <c r="C58" t="s">
         <v>227</v>
       </c>
-      <c r="F58" s="23"/>
+      <c r="F58" s="25"/>
       <c r="G58" t="s">
         <v>260</v>
       </c>
-      <c r="J58" s="23"/>
+      <c r="J58" s="25"/>
       <c r="K58" t="s">
         <v>294</v>
       </c>
-      <c r="N58" s="23"/>
+      <c r="N58" s="25"/>
       <c r="O58" t="s">
         <v>263</v>
       </c>
-      <c r="R58" s="23"/>
+      <c r="R58" s="25"/>
       <c r="S58" t="s">
         <v>361</v>
       </c>
-      <c r="V58" s="23"/>
+      <c r="V58" s="25"/>
       <c r="W58" t="s">
         <v>392</v>
       </c>
@@ -4099,27 +4119,27 @@
       <c r="A59" s="1">
         <v>16</v>
       </c>
-      <c r="B59" s="23"/>
+      <c r="B59" s="25"/>
       <c r="C59" t="s">
         <v>228</v>
       </c>
-      <c r="F59" s="23"/>
+      <c r="F59" s="25"/>
       <c r="G59" t="s">
         <v>262</v>
       </c>
-      <c r="J59" s="23"/>
+      <c r="J59" s="25"/>
       <c r="K59" t="s">
         <v>295</v>
       </c>
-      <c r="N59" s="23"/>
+      <c r="N59" s="25"/>
       <c r="O59" t="s">
         <v>330</v>
       </c>
-      <c r="R59" s="23"/>
+      <c r="R59" s="25"/>
       <c r="S59" t="s">
         <v>362</v>
       </c>
-      <c r="V59" s="23"/>
+      <c r="V59" s="25"/>
       <c r="W59" t="s">
         <v>393</v>
       </c>
@@ -4128,21 +4148,21 @@
       <c r="A60" s="1">
         <v>17</v>
       </c>
-      <c r="B60" s="23"/>
+      <c r="B60" s="25"/>
       <c r="C60" t="s">
         <v>229</v>
       </c>
-      <c r="F60" s="23"/>
+      <c r="F60" s="25"/>
       <c r="G60" t="s">
         <v>259</v>
       </c>
-      <c r="J60" s="22" t="s">
+      <c r="J60" s="26" t="s">
         <v>18</v>
       </c>
       <c r="K60" t="s">
         <v>296</v>
       </c>
-      <c r="N60" s="22" t="s">
+      <c r="N60" s="26" t="s">
         <v>18</v>
       </c>
       <c r="O60" t="s">
@@ -4154,7 +4174,7 @@
       <c r="S60" t="s">
         <v>363</v>
       </c>
-      <c r="V60" s="22" t="s">
+      <c r="V60" s="26" t="s">
         <v>18</v>
       </c>
       <c r="W60" t="s">
@@ -4165,29 +4185,29 @@
       <c r="A61" s="1">
         <v>18</v>
       </c>
-      <c r="B61" s="23"/>
+      <c r="B61" s="25"/>
       <c r="C61" t="s">
         <v>55</v>
       </c>
-      <c r="F61" s="23"/>
+      <c r="F61" s="25"/>
       <c r="G61" t="s">
         <v>92</v>
       </c>
-      <c r="J61" s="22"/>
+      <c r="J61" s="26"/>
       <c r="K61" t="s">
         <v>297</v>
       </c>
-      <c r="N61" s="22"/>
+      <c r="N61" s="26"/>
       <c r="O61" t="s">
         <v>332</v>
       </c>
-      <c r="R61" s="24" t="s">
+      <c r="R61" s="27" t="s">
         <v>24</v>
       </c>
       <c r="S61" t="s">
         <v>364</v>
       </c>
-      <c r="V61" s="22"/>
+      <c r="V61" s="26"/>
       <c r="W61" t="s">
         <v>395</v>
       </c>
@@ -4196,31 +4216,31 @@
       <c r="A62" s="1">
         <v>19</v>
       </c>
-      <c r="B62" s="22" t="s">
+      <c r="B62" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C62" t="s">
         <v>233</v>
       </c>
-      <c r="F62" s="22" t="s">
+      <c r="F62" s="26" t="s">
         <v>18</v>
       </c>
       <c r="G62" t="s">
         <v>264</v>
       </c>
-      <c r="J62" s="22"/>
+      <c r="J62" s="26"/>
       <c r="K62" t="s">
         <v>298</v>
       </c>
-      <c r="N62" s="22"/>
+      <c r="N62" s="26"/>
       <c r="O62" t="s">
         <v>333</v>
       </c>
-      <c r="R62" s="24"/>
+      <c r="R62" s="27"/>
       <c r="S62" t="s">
         <v>365</v>
       </c>
-      <c r="V62" s="22"/>
+      <c r="V62" s="26"/>
       <c r="W62" t="s">
         <v>396</v>
       </c>
@@ -4229,29 +4249,29 @@
       <c r="A63" s="1">
         <v>20</v>
       </c>
-      <c r="B63" s="22"/>
+      <c r="B63" s="26"/>
       <c r="C63" t="s">
         <v>230</v>
       </c>
-      <c r="F63" s="22"/>
+      <c r="F63" s="26"/>
       <c r="G63" t="s">
         <v>265</v>
       </c>
-      <c r="J63" s="24" t="s">
+      <c r="J63" s="27" t="s">
         <v>24</v>
       </c>
       <c r="K63" t="s">
         <v>299</v>
       </c>
-      <c r="N63" s="22"/>
+      <c r="N63" s="26"/>
       <c r="O63" t="s">
         <v>334</v>
       </c>
-      <c r="R63" s="24"/>
+      <c r="R63" s="27"/>
       <c r="S63" t="s">
         <v>366</v>
       </c>
-      <c r="V63" s="22"/>
+      <c r="V63" s="26"/>
       <c r="W63" t="s">
         <v>397</v>
       </c>
@@ -4260,27 +4280,27 @@
       <c r="A64" s="1">
         <v>21</v>
       </c>
-      <c r="B64" s="22"/>
+      <c r="B64" s="26"/>
       <c r="C64" t="s">
         <v>231</v>
       </c>
-      <c r="F64" s="22"/>
+      <c r="F64" s="26"/>
       <c r="G64" t="s">
         <v>266</v>
       </c>
-      <c r="J64" s="24"/>
+      <c r="J64" s="27"/>
       <c r="K64" t="s">
         <v>300</v>
       </c>
-      <c r="N64" s="22"/>
+      <c r="N64" s="26"/>
       <c r="O64" t="s">
         <v>335</v>
       </c>
-      <c r="R64" s="24"/>
+      <c r="R64" s="27"/>
       <c r="S64" t="s">
         <v>367</v>
       </c>
-      <c r="V64" s="24" t="s">
+      <c r="V64" s="27" t="s">
         <v>24</v>
       </c>
       <c r="W64" t="s">
@@ -4291,29 +4311,29 @@
       <c r="A65" s="1">
         <v>22</v>
       </c>
-      <c r="B65" s="22"/>
+      <c r="B65" s="26"/>
       <c r="C65" t="s">
         <v>232</v>
       </c>
-      <c r="F65" s="22"/>
+      <c r="F65" s="26"/>
       <c r="G65" t="s">
         <v>267</v>
       </c>
-      <c r="J65" s="24"/>
+      <c r="J65" s="27"/>
       <c r="K65" t="s">
         <v>301</v>
       </c>
-      <c r="N65" s="24" t="s">
+      <c r="N65" s="27" t="s">
         <v>24</v>
       </c>
       <c r="O65" t="s">
         <v>336</v>
       </c>
-      <c r="R65" s="24"/>
+      <c r="R65" s="27"/>
       <c r="S65" t="s">
         <v>368</v>
       </c>
-      <c r="V65" s="24"/>
+      <c r="V65" s="27"/>
       <c r="W65" t="s">
         <v>399</v>
       </c>
@@ -4322,31 +4342,31 @@
       <c r="A66" s="1">
         <v>23</v>
       </c>
-      <c r="B66" s="22"/>
+      <c r="B66" s="26"/>
       <c r="C66" t="s">
         <v>61</v>
       </c>
-      <c r="F66" s="24" t="s">
+      <c r="F66" s="27" t="s">
         <v>24</v>
       </c>
       <c r="G66" t="s">
         <v>268</v>
       </c>
-      <c r="J66" s="24"/>
+      <c r="J66" s="27"/>
       <c r="K66" t="s">
         <v>302</v>
       </c>
-      <c r="N66" s="24"/>
+      <c r="N66" s="27"/>
       <c r="O66" t="s">
         <v>337</v>
       </c>
-      <c r="R66" s="25" t="s">
+      <c r="R66" s="20" t="s">
         <v>30</v>
       </c>
       <c r="S66" t="s">
         <v>369</v>
       </c>
-      <c r="V66" s="24"/>
+      <c r="V66" s="27"/>
       <c r="W66" t="s">
         <v>400</v>
       </c>
@@ -4355,29 +4375,29 @@
       <c r="A67" s="1">
         <v>24</v>
       </c>
-      <c r="B67" s="24" t="s">
+      <c r="B67" s="27" t="s">
         <v>24</v>
       </c>
       <c r="C67" t="s">
         <v>102</v>
       </c>
-      <c r="F67" s="24"/>
+      <c r="F67" s="27"/>
       <c r="G67" t="s">
         <v>269</v>
       </c>
-      <c r="J67" s="24"/>
+      <c r="J67" s="27"/>
       <c r="K67" t="s">
         <v>303</v>
       </c>
-      <c r="N67" s="24"/>
+      <c r="N67" s="27"/>
       <c r="O67" t="s">
         <v>338</v>
       </c>
-      <c r="R67" s="25"/>
+      <c r="R67" s="20"/>
       <c r="S67" t="s">
         <v>370</v>
       </c>
-      <c r="V67" s="24"/>
+      <c r="V67" s="27"/>
       <c r="W67" t="s">
         <v>401</v>
       </c>
@@ -4386,27 +4406,27 @@
       <c r="A68" s="1">
         <v>25</v>
       </c>
-      <c r="B68" s="24"/>
+      <c r="B68" s="27"/>
       <c r="C68" t="s">
         <v>234</v>
       </c>
-      <c r="F68" s="24"/>
+      <c r="F68" s="27"/>
       <c r="G68" t="s">
         <v>270</v>
       </c>
-      <c r="J68" s="24"/>
+      <c r="J68" s="27"/>
       <c r="K68" t="s">
         <v>304</v>
       </c>
-      <c r="N68" s="24"/>
+      <c r="N68" s="27"/>
       <c r="O68" t="s">
         <v>342</v>
       </c>
-      <c r="R68" s="25"/>
+      <c r="R68" s="20"/>
       <c r="S68" t="s">
         <v>371</v>
       </c>
-      <c r="V68" s="25" t="s">
+      <c r="V68" s="20" t="s">
         <v>30</v>
       </c>
       <c r="W68" t="s">
@@ -4417,29 +4437,29 @@
       <c r="A69" s="1">
         <v>26</v>
       </c>
-      <c r="B69" s="24"/>
+      <c r="B69" s="27"/>
       <c r="C69" t="s">
         <v>235</v>
       </c>
-      <c r="F69" s="24"/>
+      <c r="F69" s="27"/>
       <c r="G69" t="s">
         <v>101</v>
       </c>
-      <c r="J69" s="24"/>
+      <c r="J69" s="27"/>
       <c r="K69" t="s">
         <v>305</v>
       </c>
-      <c r="N69" s="25" t="s">
+      <c r="N69" s="20" t="s">
         <v>30</v>
       </c>
       <c r="O69" t="s">
         <v>339</v>
       </c>
-      <c r="R69" s="25"/>
+      <c r="R69" s="20"/>
       <c r="S69" t="s">
         <v>372</v>
       </c>
-      <c r="V69" s="25"/>
+      <c r="V69" s="20"/>
       <c r="W69" t="s">
         <v>403</v>
       </c>
@@ -4448,33 +4468,33 @@
       <c r="A70" s="1">
         <v>27</v>
       </c>
-      <c r="B70" s="24"/>
+      <c r="B70" s="27"/>
       <c r="C70" t="s">
         <v>236</v>
       </c>
-      <c r="F70" s="25" t="s">
+      <c r="F70" s="20" t="s">
         <v>30</v>
       </c>
       <c r="G70" t="s">
         <v>271</v>
       </c>
-      <c r="J70" s="25" t="s">
+      <c r="J70" s="20" t="s">
         <v>30</v>
       </c>
       <c r="K70" t="s">
         <v>306</v>
       </c>
-      <c r="N70" s="25"/>
+      <c r="N70" s="20"/>
       <c r="O70" t="s">
         <v>340</v>
       </c>
-      <c r="R70" s="26" t="s">
+      <c r="R70" s="21" t="s">
         <v>36</v>
       </c>
       <c r="S70" t="s">
         <v>373</v>
       </c>
-      <c r="V70" s="25"/>
+      <c r="V70" s="20"/>
       <c r="W70" t="s">
         <v>404</v>
       </c>
@@ -4483,27 +4503,27 @@
       <c r="A71" s="1">
         <v>28</v>
       </c>
-      <c r="B71" s="24"/>
+      <c r="B71" s="27"/>
       <c r="C71" t="s">
         <v>237</v>
       </c>
-      <c r="F71" s="25"/>
+      <c r="F71" s="20"/>
       <c r="G71" t="s">
         <v>272</v>
       </c>
-      <c r="J71" s="25"/>
+      <c r="J71" s="20"/>
       <c r="K71" t="s">
         <v>307</v>
       </c>
-      <c r="N71" s="25"/>
+      <c r="N71" s="20"/>
       <c r="O71" t="s">
         <v>341</v>
       </c>
-      <c r="R71" s="26"/>
+      <c r="R71" s="21"/>
       <c r="S71" t="s">
         <v>374</v>
       </c>
-      <c r="V71" s="25"/>
+      <c r="V71" s="20"/>
       <c r="W71" t="s">
         <v>405</v>
       </c>
@@ -4512,27 +4532,27 @@
       <c r="A72" s="1">
         <v>29</v>
       </c>
-      <c r="B72" s="24"/>
+      <c r="B72" s="27"/>
       <c r="C72" t="s">
         <v>238</v>
       </c>
-      <c r="F72" s="25"/>
+      <c r="F72" s="20"/>
       <c r="G72" t="s">
         <v>273</v>
       </c>
-      <c r="J72" s="25"/>
+      <c r="J72" s="20"/>
       <c r="K72" t="s">
         <v>308</v>
       </c>
-      <c r="N72" s="25"/>
+      <c r="N72" s="20"/>
       <c r="O72" t="s">
         <v>343</v>
       </c>
-      <c r="R72" s="26"/>
+      <c r="R72" s="21"/>
       <c r="S72" t="s">
         <v>375</v>
       </c>
-      <c r="V72" s="25"/>
+      <c r="V72" s="20"/>
       <c r="W72" t="s">
         <v>406</v>
       </c>
@@ -4541,31 +4561,31 @@
       <c r="A73" s="1">
         <v>30</v>
       </c>
-      <c r="B73" s="25" t="s">
+      <c r="B73" s="20" t="s">
         <v>30</v>
       </c>
       <c r="C73" t="s">
         <v>34</v>
       </c>
-      <c r="F73" s="25"/>
+      <c r="F73" s="20"/>
       <c r="G73" t="s">
         <v>274</v>
       </c>
-      <c r="J73" s="25"/>
+      <c r="J73" s="20"/>
       <c r="K73" t="s">
         <v>309</v>
       </c>
-      <c r="N73" s="26" t="s">
+      <c r="N73" s="21" t="s">
         <v>36</v>
       </c>
       <c r="O73" t="s">
         <v>344</v>
       </c>
-      <c r="R73" s="26"/>
+      <c r="R73" s="21"/>
       <c r="S73" t="s">
         <v>376</v>
       </c>
-      <c r="V73" s="26" t="s">
+      <c r="V73" s="21" t="s">
         <v>36</v>
       </c>
       <c r="W73" t="s">
@@ -4573,119 +4593,184 @@
       </c>
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B74" s="25"/>
+      <c r="B74" s="20"/>
       <c r="C74" t="s">
         <v>239</v>
       </c>
-      <c r="F74" s="26" t="s">
+      <c r="F74" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="G74" t="s">
-        <v>275</v>
-      </c>
-      <c r="J74" s="26" t="s">
+      <c r="J74" s="21" t="s">
         <v>36</v>
       </c>
       <c r="K74" t="s">
         <v>310</v>
       </c>
-      <c r="N74" s="26"/>
+      <c r="N74" s="21"/>
       <c r="O74" t="s">
         <v>345</v>
       </c>
-      <c r="R74" s="26"/>
+      <c r="R74" s="21"/>
       <c r="S74" t="s">
         <v>377</v>
       </c>
-      <c r="V74" s="26"/>
+      <c r="V74" s="21"/>
       <c r="W74" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B75" s="25"/>
+      <c r="B75" s="20"/>
       <c r="C75" t="s">
         <v>240</v>
       </c>
-      <c r="F75" s="26"/>
+      <c r="F75" s="21"/>
       <c r="G75" t="s">
         <v>276</v>
       </c>
-      <c r="J75" s="26"/>
+      <c r="J75" s="21"/>
       <c r="K75" t="s">
         <v>311</v>
       </c>
-      <c r="N75" s="26"/>
+      <c r="N75" s="21"/>
       <c r="O75" t="s">
         <v>346</v>
       </c>
-      <c r="V75" s="26"/>
+      <c r="V75" s="21"/>
       <c r="W75" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B76" s="25"/>
+      <c r="B76" s="20"/>
       <c r="C76" t="s">
         <v>241</v>
       </c>
-      <c r="F76" s="26"/>
+      <c r="F76" s="21"/>
       <c r="G76" t="s">
         <v>277</v>
       </c>
-      <c r="J76" s="26"/>
+      <c r="J76" s="21"/>
       <c r="K76" t="s">
         <v>312</v>
       </c>
-      <c r="N76" s="26"/>
+      <c r="N76" s="21"/>
       <c r="O76" t="s">
         <v>347</v>
       </c>
-      <c r="V76" s="26"/>
+      <c r="V76" s="21"/>
       <c r="W76" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="77" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B77" s="26" t="s">
+      <c r="B77" s="21" t="s">
         <v>36</v>
       </c>
       <c r="C77" t="s">
         <v>109</v>
       </c>
-      <c r="F77" s="26"/>
+      <c r="F77" s="21"/>
       <c r="G77" t="s">
         <v>278</v>
       </c>
-      <c r="J77" s="26"/>
+      <c r="J77" s="21"/>
       <c r="K77" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B78" s="26"/>
+      <c r="B78" s="21"/>
       <c r="C78" t="s">
         <v>242</v>
       </c>
-      <c r="F78" s="26"/>
+      <c r="F78" s="21"/>
       <c r="G78" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B79" s="26"/>
+      <c r="B79" s="21"/>
       <c r="C79" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B80" s="26"/>
+      <c r="B80" s="21"/>
       <c r="C80" t="s">
         <v>244</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="85">
+  <mergeCells count="84">
+    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="V6:V13"/>
+    <mergeCell ref="J10:J15"/>
+    <mergeCell ref="J4:J9"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="F10:F15"/>
+    <mergeCell ref="J20:J22"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="F47:F54"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="F55:F61"/>
+    <mergeCell ref="B51:B61"/>
+    <mergeCell ref="F62:F65"/>
+    <mergeCell ref="J70:J73"/>
+    <mergeCell ref="J74:J77"/>
+    <mergeCell ref="N44:N46"/>
+    <mergeCell ref="N47:N49"/>
+    <mergeCell ref="N60:N64"/>
+    <mergeCell ref="N65:N68"/>
+    <mergeCell ref="N69:N72"/>
+    <mergeCell ref="N73:N76"/>
+    <mergeCell ref="N50:N59"/>
+    <mergeCell ref="J60:J62"/>
+    <mergeCell ref="J50:J59"/>
+    <mergeCell ref="J63:J69"/>
+    <mergeCell ref="F70:F73"/>
+    <mergeCell ref="F66:F69"/>
+    <mergeCell ref="F74:F78"/>
+    <mergeCell ref="B67:B72"/>
+    <mergeCell ref="B73:B76"/>
+    <mergeCell ref="B77:B80"/>
+    <mergeCell ref="V2:V5"/>
+    <mergeCell ref="V25:V27"/>
+    <mergeCell ref="V28:V31"/>
+    <mergeCell ref="R44:R47"/>
+    <mergeCell ref="J27:J30"/>
+    <mergeCell ref="N24:N29"/>
+    <mergeCell ref="N30:N33"/>
+    <mergeCell ref="R26:R30"/>
+    <mergeCell ref="J44:J46"/>
+    <mergeCell ref="J47:J49"/>
+    <mergeCell ref="J23:J26"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="R4:R9"/>
+    <mergeCell ref="R10:R19"/>
+    <mergeCell ref="R20:R21"/>
+    <mergeCell ref="R22:R25"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="N4:N10"/>
+    <mergeCell ref="N11:N16"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="N19:N23"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="B2:B3"/>
     <mergeCell ref="V68:V72"/>
     <mergeCell ref="V73:V76"/>
     <mergeCell ref="R66:R69"/>
@@ -4700,77 +4785,8 @@
     <mergeCell ref="V37:V40"/>
     <mergeCell ref="R61:R65"/>
     <mergeCell ref="V32:V36"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="N4:N10"/>
-    <mergeCell ref="N11:N16"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="N19:N23"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="R4:R9"/>
-    <mergeCell ref="R10:R19"/>
-    <mergeCell ref="R20:R21"/>
-    <mergeCell ref="R22:R25"/>
     <mergeCell ref="R48:R52"/>
     <mergeCell ref="R53:R59"/>
-    <mergeCell ref="R44:R47"/>
-    <mergeCell ref="J27:J30"/>
-    <mergeCell ref="N24:N29"/>
-    <mergeCell ref="N30:N33"/>
-    <mergeCell ref="R26:R30"/>
-    <mergeCell ref="J44:J46"/>
-    <mergeCell ref="J47:J49"/>
-    <mergeCell ref="J23:J26"/>
-    <mergeCell ref="V2:V5"/>
-    <mergeCell ref="V25:V27"/>
-    <mergeCell ref="V28:V31"/>
-    <mergeCell ref="V6:V12"/>
-    <mergeCell ref="V13:V24"/>
-    <mergeCell ref="F70:F73"/>
-    <mergeCell ref="F66:F69"/>
-    <mergeCell ref="F74:F78"/>
-    <mergeCell ref="B67:B72"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="B77:B80"/>
-    <mergeCell ref="J70:J73"/>
-    <mergeCell ref="J74:J77"/>
-    <mergeCell ref="N44:N46"/>
-    <mergeCell ref="N47:N49"/>
-    <mergeCell ref="N60:N64"/>
-    <mergeCell ref="N65:N68"/>
-    <mergeCell ref="N69:N72"/>
-    <mergeCell ref="N73:N76"/>
-    <mergeCell ref="N50:N59"/>
-    <mergeCell ref="J60:J62"/>
-    <mergeCell ref="J50:J59"/>
-    <mergeCell ref="J63:J69"/>
-    <mergeCell ref="J20:J22"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="F47:F54"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="F55:F61"/>
-    <mergeCell ref="B51:B61"/>
-    <mergeCell ref="F62:F65"/>
-    <mergeCell ref="J4:J10"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="F11:F16"/>
-    <mergeCell ref="F6:F10"/>
-    <mergeCell ref="J11:J15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4781,7 +4797,7 @@
   <dimension ref="A1:Z50"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4802,36 +4818,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="E1" s="28" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="E1" s="22" t="s">
         <v>412</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
       <c r="J1" t="s">
         <v>411</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="O1" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="T1" s="28" t="s">
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="T1" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="X1" s="28" t="s">
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="X1" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -4843,6 +4859,9 @@
       <c r="E2" t="s">
         <v>590</v>
       </c>
+      <c r="F2" t="s">
+        <v>508</v>
+      </c>
       <c r="J2" t="s">
         <v>556</v>
       </c>
@@ -4934,9 +4953,6 @@
       <c r="X4" t="s">
         <v>416</v>
       </c>
-      <c r="Y4" t="s">
-        <v>539</v>
-      </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -5000,6 +5016,9 @@
       <c r="B7" t="s">
         <v>489</v>
       </c>
+      <c r="E7" t="s">
+        <v>622</v>
+      </c>
       <c r="K7" t="s">
         <v>493</v>
       </c>
@@ -5012,66 +5031,65 @@
         <v>490</v>
       </c>
       <c r="E8" t="s">
-        <v>600</v>
+        <v>419</v>
       </c>
       <c r="K8" t="s">
-        <v>494</v>
+        <v>539</v>
       </c>
       <c r="T8" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="E9" t="s">
-        <v>622</v>
-      </c>
       <c r="K9" t="s">
-        <v>509</v>
+        <v>494</v>
       </c>
       <c r="T9" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="E10" t="s">
-        <v>419</v>
-      </c>
       <c r="K10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="K11" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="K12" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
       <c r="E17" t="s">
         <v>420</v>
       </c>
-      <c r="I17" s="28" t="s">
+      <c r="I17" s="22" t="s">
         <v>421</v>
       </c>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="N17" s="28" t="s">
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="N17" s="22" t="s">
         <v>314</v>
       </c>
-      <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="28"/>
-      <c r="S17" s="28" t="s">
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="S17" s="22" t="s">
         <v>315</v>
       </c>
-      <c r="T17" s="28"/>
-      <c r="U17" s="28"/>
-      <c r="V17" s="28"/>
+      <c r="T17" s="22"/>
+      <c r="U17" s="22"/>
+      <c r="V17" s="22"/>
       <c r="X17" t="s">
         <v>316</v>
       </c>
@@ -5125,7 +5143,7 @@
         <v>629</v>
       </c>
       <c r="F19" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="J19" t="s">
         <v>630</v>
@@ -5160,7 +5178,7 @@
         <v>598</v>
       </c>
       <c r="F20" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="J20" t="s">
         <v>603</v>
@@ -5198,7 +5216,7 @@
         <v>429</v>
       </c>
       <c r="F21" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="J21" t="s">
         <v>426</v>
@@ -5232,9 +5250,6 @@
       <c r="E22" t="s">
         <v>594</v>
       </c>
-      <c r="F22" t="s">
-        <v>501</v>
-      </c>
       <c r="K22" t="s">
         <v>516</v>
       </c>
@@ -5259,7 +5274,7 @@
         <v>619</v>
       </c>
       <c r="E23" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="O23" t="s">
         <v>609</v>
@@ -5270,7 +5285,7 @@
         <v>632</v>
       </c>
       <c r="E24" t="s">
-        <v>624</v>
+        <v>604</v>
       </c>
       <c r="O24" t="s">
         <v>431</v>
@@ -5281,7 +5296,7 @@
         <v>432</v>
       </c>
       <c r="E25" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
       <c r="O25" t="s">
         <v>433</v>
@@ -5289,6 +5304,11 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="E26" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="E27" t="s">
         <v>434</v>
       </c>
     </row>
@@ -5593,10 +5613,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K104"/>
+  <dimension ref="A1:K115"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6202,6 +6222,58 @@
         <v>35</v>
       </c>
     </row>
+    <row r="106" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" s="5" t="s">
+        <v>651</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" s="10"/>
+      <c r="B108" s="11" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="B109" s="11" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A110" s="7"/>
+      <c r="B110" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" s="5" t="s">
+        <v>578</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="B114" s="11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A115" s="7"/>
+      <c r="B115" s="8" t="s">
+        <v>663</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
More trades and updated picks
</commit_message>
<xml_diff>
--- a/OffSeason.xlsx
+++ b/OffSeason.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="667">
   <si>
     <t>Chubber for Chubb - John Olson</t>
   </si>
@@ -2019,6 +2019,15 @@
   </si>
   <si>
     <t>2021 3rd (alan)</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>2020 2 snow happens (lottery)</t>
+  </si>
+  <si>
+    <t>2021 3rd (John O)</t>
   </si>
 </sst>
 </file>
@@ -2250,6 +2259,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2276,9 +2288,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2564,7 +2573,7 @@
   <dimension ref="A1:Y80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2579,11 +2588,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
       <c r="F1" t="s">
         <v>42</v>
       </c>
@@ -2604,37 +2613,37 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="24" t="s">
         <v>1</v>
       </c>
       <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="24" t="s">
         <v>1</v>
       </c>
       <c r="K2" t="s">
         <v>77</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="24" t="s">
         <v>1</v>
       </c>
       <c r="O2" t="s">
         <v>112</v>
       </c>
-      <c r="R2" s="23" t="s">
+      <c r="R2" s="24" t="s">
         <v>1</v>
       </c>
       <c r="S2" t="s">
         <v>144</v>
       </c>
-      <c r="V2" s="23" t="s">
+      <c r="V2" s="24" t="s">
         <v>1</v>
       </c>
       <c r="W2" t="s">
@@ -2645,27 +2654,27 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="24"/>
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="23"/>
+      <c r="F3" s="24"/>
       <c r="G3" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="23"/>
+      <c r="J3" s="24"/>
       <c r="K3" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="23"/>
+      <c r="N3" s="24"/>
       <c r="O3" t="s">
         <v>104</v>
       </c>
-      <c r="R3" s="23"/>
+      <c r="R3" s="24"/>
       <c r="S3" t="s">
         <v>145</v>
       </c>
-      <c r="V3" s="23"/>
+      <c r="V3" s="24"/>
       <c r="W3" t="s">
         <v>179</v>
       </c>
@@ -2674,35 +2683,35 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="25" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="23"/>
+      <c r="F4" s="24"/>
       <c r="G4" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="25" t="s">
         <v>5</v>
       </c>
       <c r="K4" t="s">
         <v>248</v>
       </c>
-      <c r="N4" s="24" t="s">
+      <c r="N4" s="25" t="s">
         <v>5</v>
       </c>
       <c r="O4" t="s">
         <v>113</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="25" t="s">
         <v>5</v>
       </c>
       <c r="S4" t="s">
         <v>146</v>
       </c>
-      <c r="V4" s="23"/>
+      <c r="V4" s="24"/>
       <c r="W4" t="s">
         <v>180</v>
       </c>
@@ -2711,27 +2720,27 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="25"/>
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="23"/>
+      <c r="F5" s="24"/>
       <c r="G5" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="24"/>
+      <c r="J5" s="25"/>
       <c r="K5" t="s">
         <v>81</v>
       </c>
-      <c r="N5" s="24"/>
+      <c r="N5" s="25"/>
       <c r="O5" t="s">
         <v>114</v>
       </c>
-      <c r="R5" s="24"/>
+      <c r="R5" s="25"/>
       <c r="S5" t="s">
         <v>147</v>
       </c>
-      <c r="V5" s="23"/>
+      <c r="V5" s="24"/>
       <c r="W5" t="s">
         <v>181</v>
       </c>
@@ -2740,29 +2749,29 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="25"/>
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="25" t="s">
         <v>5</v>
       </c>
       <c r="G6" t="s">
         <v>215</v>
       </c>
-      <c r="J6" s="24"/>
+      <c r="J6" s="25"/>
       <c r="K6" t="s">
         <v>82</v>
       </c>
-      <c r="N6" s="24"/>
+      <c r="N6" s="25"/>
       <c r="O6" t="s">
         <v>115</v>
       </c>
-      <c r="R6" s="24"/>
+      <c r="R6" s="25"/>
       <c r="S6" t="s">
         <v>148</v>
       </c>
-      <c r="V6" s="24" t="s">
+      <c r="V6" s="25" t="s">
         <v>5</v>
       </c>
       <c r="W6" t="s">
@@ -2773,27 +2782,27 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="24"/>
+      <c r="B7" s="25"/>
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="24"/>
+      <c r="F7" s="25"/>
       <c r="G7" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="24"/>
+      <c r="J7" s="25"/>
       <c r="K7" t="s">
         <v>84</v>
       </c>
-      <c r="N7" s="24"/>
+      <c r="N7" s="25"/>
       <c r="O7" t="s">
         <v>116</v>
       </c>
-      <c r="R7" s="24"/>
+      <c r="R7" s="25"/>
       <c r="S7" t="s">
         <v>149</v>
       </c>
-      <c r="V7" s="24"/>
+      <c r="V7" s="25"/>
       <c r="W7" t="s">
         <v>250</v>
       </c>
@@ -2802,27 +2811,27 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="24"/>
+      <c r="B8" s="25"/>
       <c r="C8" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="25"/>
       <c r="G8" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="24"/>
+      <c r="J8" s="25"/>
       <c r="K8" t="s">
         <v>48</v>
       </c>
-      <c r="N8" s="24"/>
+      <c r="N8" s="25"/>
       <c r="O8" t="s">
         <v>117</v>
       </c>
-      <c r="R8" s="24"/>
+      <c r="R8" s="25"/>
       <c r="S8" t="s">
         <v>150</v>
       </c>
-      <c r="V8" s="24"/>
+      <c r="V8" s="25"/>
       <c r="W8" t="s">
         <v>184</v>
       </c>
@@ -2831,27 +2840,27 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="24"/>
+      <c r="B9" s="25"/>
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="24"/>
+      <c r="F9" s="25"/>
       <c r="G9" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="24"/>
+      <c r="J9" s="25"/>
       <c r="K9" t="s">
         <v>85</v>
       </c>
-      <c r="N9" s="24"/>
+      <c r="N9" s="25"/>
       <c r="O9" t="s">
         <v>118</v>
       </c>
-      <c r="R9" s="24"/>
+      <c r="R9" s="25"/>
       <c r="S9" t="s">
         <v>151</v>
       </c>
-      <c r="V9" s="24"/>
+      <c r="V9" s="25"/>
       <c r="W9" t="s">
         <v>252</v>
       </c>
@@ -2860,35 +2869,35 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="26" t="s">
         <v>12</v>
       </c>
       <c r="G10" t="s">
         <v>54</v>
       </c>
-      <c r="J10" s="25" t="s">
+      <c r="J10" s="26" t="s">
         <v>12</v>
       </c>
       <c r="K10" t="s">
         <v>188</v>
       </c>
-      <c r="N10" s="24"/>
+      <c r="N10" s="25"/>
       <c r="O10" t="s">
         <v>119</v>
       </c>
-      <c r="R10" s="25" t="s">
+      <c r="R10" s="26" t="s">
         <v>12</v>
       </c>
       <c r="S10" t="s">
         <v>152</v>
       </c>
-      <c r="V10" s="24"/>
+      <c r="V10" s="25"/>
       <c r="W10" t="s">
         <v>186</v>
       </c>
@@ -2897,29 +2906,29 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="25"/>
+      <c r="B11" s="26"/>
       <c r="C11" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="25"/>
+      <c r="F11" s="26"/>
       <c r="G11" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="25"/>
+      <c r="J11" s="26"/>
       <c r="K11" t="s">
         <v>88</v>
       </c>
-      <c r="N11" s="25" t="s">
+      <c r="N11" s="26" t="s">
         <v>12</v>
       </c>
       <c r="O11" t="s">
         <v>120</v>
       </c>
-      <c r="R11" s="25"/>
+      <c r="R11" s="26"/>
       <c r="S11" t="s">
         <v>153</v>
       </c>
-      <c r="V11" s="24"/>
+      <c r="V11" s="25"/>
       <c r="W11" t="s">
         <v>187</v>
       </c>
@@ -2928,27 +2937,27 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="25"/>
+      <c r="B12" s="26"/>
       <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="25"/>
+      <c r="F12" s="26"/>
       <c r="G12" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="25"/>
+      <c r="J12" s="26"/>
       <c r="K12" t="s">
         <v>16</v>
       </c>
-      <c r="N12" s="25"/>
+      <c r="N12" s="26"/>
       <c r="O12" t="s">
         <v>121</v>
       </c>
-      <c r="R12" s="25"/>
+      <c r="R12" s="26"/>
       <c r="S12" t="s">
         <v>154</v>
       </c>
-      <c r="V12" s="24"/>
+      <c r="V12" s="25"/>
       <c r="W12" t="s">
         <v>53</v>
       </c>
@@ -2957,27 +2966,27 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="25"/>
+      <c r="B13" s="26"/>
       <c r="C13" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="25"/>
+      <c r="F13" s="26"/>
       <c r="G13" t="s">
         <v>59</v>
       </c>
-      <c r="J13" s="25"/>
+      <c r="J13" s="26"/>
       <c r="K13" t="s">
         <v>17</v>
       </c>
-      <c r="N13" s="25"/>
+      <c r="N13" s="26"/>
       <c r="O13" t="s">
         <v>122</v>
       </c>
-      <c r="R13" s="25"/>
+      <c r="R13" s="26"/>
       <c r="S13" t="s">
         <v>155</v>
       </c>
-      <c r="V13" s="24"/>
+      <c r="V13" s="25"/>
       <c r="W13" t="s">
         <v>10</v>
       </c>
@@ -2986,27 +2995,27 @@
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="25"/>
+      <c r="B14" s="26"/>
       <c r="C14" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="25"/>
+      <c r="F14" s="26"/>
       <c r="G14" t="s">
         <v>226</v>
       </c>
-      <c r="J14" s="25"/>
+      <c r="J14" s="26"/>
       <c r="K14" t="s">
         <v>22</v>
       </c>
-      <c r="N14" s="25"/>
+      <c r="N14" s="26"/>
       <c r="O14" t="s">
         <v>123</v>
       </c>
-      <c r="R14" s="25"/>
+      <c r="R14" s="26"/>
       <c r="S14" t="s">
         <v>156</v>
       </c>
-      <c r="V14" s="29" t="s">
+      <c r="V14" s="20" t="s">
         <v>12</v>
       </c>
       <c r="W14" t="s">
@@ -3017,27 +3026,27 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="25"/>
+      <c r="B15" s="26"/>
       <c r="C15" t="s">
         <v>87</v>
       </c>
-      <c r="F15" s="25"/>
+      <c r="F15" s="26"/>
       <c r="G15" t="s">
         <v>225</v>
       </c>
-      <c r="J15" s="25"/>
+      <c r="J15" s="26"/>
       <c r="K15" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="25"/>
+      <c r="N15" s="26"/>
       <c r="O15" t="s">
         <v>124</v>
       </c>
-      <c r="R15" s="25"/>
+      <c r="R15" s="26"/>
       <c r="S15" t="s">
         <v>157</v>
       </c>
-      <c r="V15" s="29"/>
+      <c r="V15" s="20"/>
       <c r="W15" t="s">
         <v>189</v>
       </c>
@@ -3046,33 +3055,33 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="27" t="s">
         <v>18</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="27" t="s">
         <v>18</v>
       </c>
       <c r="G16" t="s">
         <v>60</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="27" t="s">
         <v>18</v>
       </c>
       <c r="K16" t="s">
         <v>95</v>
       </c>
-      <c r="N16" s="25"/>
+      <c r="N16" s="26"/>
       <c r="O16" t="s">
         <v>125</v>
       </c>
-      <c r="R16" s="25"/>
+      <c r="R16" s="26"/>
       <c r="S16" t="s">
         <v>158</v>
       </c>
-      <c r="V16" s="29"/>
+      <c r="V16" s="20"/>
       <c r="W16" t="s">
         <v>190</v>
       </c>
@@ -3081,29 +3090,29 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="26"/>
+      <c r="B17" s="27"/>
       <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="26"/>
+      <c r="F17" s="27"/>
       <c r="G17" t="s">
         <v>62</v>
       </c>
-      <c r="J17" s="26"/>
+      <c r="J17" s="27"/>
       <c r="K17" t="s">
-        <v>96</v>
-      </c>
-      <c r="N17" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="N17" s="27" t="s">
         <v>18</v>
       </c>
       <c r="O17" t="s">
         <v>126</v>
       </c>
-      <c r="R17" s="25"/>
+      <c r="R17" s="26"/>
       <c r="S17" t="s">
         <v>159</v>
       </c>
-      <c r="V17" s="29"/>
+      <c r="V17" s="20"/>
       <c r="W17" t="s">
         <v>191</v>
       </c>
@@ -3112,27 +3121,27 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="26"/>
+      <c r="B18" s="27"/>
       <c r="C18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="26"/>
+        <v>96</v>
+      </c>
+      <c r="F18" s="27"/>
       <c r="G18" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="26"/>
+      <c r="J18" s="27"/>
       <c r="K18" t="s">
         <v>97</v>
       </c>
-      <c r="N18" s="26"/>
+      <c r="N18" s="27"/>
       <c r="O18" t="s">
         <v>127</v>
       </c>
-      <c r="R18" s="25"/>
+      <c r="R18" s="26"/>
       <c r="S18" t="s">
         <v>160</v>
       </c>
-      <c r="V18" s="29"/>
+      <c r="V18" s="20"/>
       <c r="W18" t="s">
         <v>91</v>
       </c>
@@ -3141,33 +3150,33 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="28" t="s">
         <v>24</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="28" t="s">
         <v>24</v>
       </c>
       <c r="G19" t="s">
         <v>64</v>
       </c>
-      <c r="J19" s="26"/>
+      <c r="J19" s="27"/>
       <c r="K19" t="s">
         <v>98</v>
       </c>
-      <c r="N19" s="27" t="s">
+      <c r="N19" s="28" t="s">
         <v>24</v>
       </c>
       <c r="O19" t="s">
         <v>128</v>
       </c>
-      <c r="R19" s="25"/>
+      <c r="R19" s="26"/>
       <c r="S19" t="s">
         <v>161</v>
       </c>
-      <c r="V19" s="29"/>
+      <c r="V19" s="20"/>
       <c r="W19" t="s">
         <v>261</v>
       </c>
@@ -3176,31 +3185,31 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="27"/>
+      <c r="B20" s="28"/>
       <c r="C20" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="27"/>
+      <c r="F20" s="28"/>
       <c r="G20" t="s">
         <v>65</v>
       </c>
-      <c r="J20" s="27" t="s">
+      <c r="J20" s="28" t="s">
         <v>24</v>
       </c>
       <c r="K20" t="s">
         <v>99</v>
       </c>
-      <c r="N20" s="27"/>
+      <c r="N20" s="28"/>
       <c r="O20" t="s">
         <v>129</v>
       </c>
-      <c r="R20" s="26" t="s">
+      <c r="R20" s="27" t="s">
         <v>18</v>
       </c>
       <c r="S20" t="s">
         <v>162</v>
       </c>
-      <c r="V20" s="29"/>
+      <c r="V20" s="20"/>
       <c r="W20" t="s">
         <v>94</v>
       </c>
@@ -3209,27 +3218,27 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="27"/>
+      <c r="B21" s="28"/>
       <c r="C21" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="27"/>
+      <c r="F21" s="28"/>
       <c r="G21" t="s">
         <v>66</v>
       </c>
-      <c r="J21" s="27"/>
+      <c r="J21" s="28"/>
       <c r="K21" t="s">
         <v>28</v>
       </c>
-      <c r="N21" s="27"/>
+      <c r="N21" s="28"/>
       <c r="O21" t="s">
         <v>130</v>
       </c>
-      <c r="R21" s="26"/>
+      <c r="R21" s="27"/>
       <c r="S21" t="s">
         <v>163</v>
       </c>
-      <c r="V21" s="29"/>
+      <c r="V21" s="20"/>
       <c r="W21" t="s">
         <v>192</v>
       </c>
@@ -3238,29 +3247,29 @@
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="27"/>
+      <c r="B22" s="28"/>
       <c r="C22" t="s">
         <v>100</v>
       </c>
-      <c r="F22" s="27"/>
+      <c r="F22" s="28"/>
       <c r="G22" t="s">
         <v>67</v>
       </c>
-      <c r="J22" s="27"/>
+      <c r="J22" s="28"/>
       <c r="K22" t="s">
         <v>29</v>
       </c>
-      <c r="N22" s="27"/>
+      <c r="N22" s="28"/>
       <c r="O22" t="s">
         <v>131</v>
       </c>
-      <c r="R22" s="27" t="s">
+      <c r="R22" s="28" t="s">
         <v>24</v>
       </c>
       <c r="S22" t="s">
         <v>164</v>
       </c>
-      <c r="V22" s="29"/>
+      <c r="V22" s="20"/>
       <c r="W22" t="s">
         <v>193</v>
       </c>
@@ -3269,33 +3278,33 @@
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C23" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="21" t="s">
         <v>30</v>
       </c>
       <c r="G23" t="s">
         <v>69</v>
       </c>
-      <c r="J23" s="20" t="s">
+      <c r="J23" s="21" t="s">
         <v>30</v>
       </c>
       <c r="K23" t="s">
         <v>103</v>
       </c>
-      <c r="N23" s="27"/>
+      <c r="N23" s="28"/>
       <c r="O23" t="s">
         <v>132</v>
       </c>
-      <c r="R23" s="27"/>
+      <c r="R23" s="28"/>
       <c r="S23" t="s">
         <v>165</v>
       </c>
-      <c r="V23" s="29"/>
+      <c r="V23" s="20"/>
       <c r="W23" t="s">
         <v>195</v>
       </c>
@@ -3304,29 +3313,29 @@
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="20"/>
+      <c r="B24" s="21"/>
       <c r="C24" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="20"/>
+      <c r="F24" s="21"/>
       <c r="G24" t="s">
         <v>70</v>
       </c>
-      <c r="J24" s="20"/>
+      <c r="J24" s="21"/>
       <c r="K24" t="s">
         <v>104</v>
       </c>
-      <c r="N24" s="20" t="s">
+      <c r="N24" s="21" t="s">
         <v>30</v>
       </c>
       <c r="O24" t="s">
         <v>133</v>
       </c>
-      <c r="R24" s="27"/>
+      <c r="R24" s="28"/>
       <c r="S24" t="s">
         <v>166</v>
       </c>
-      <c r="V24" s="29"/>
+      <c r="V24" s="20"/>
       <c r="W24" t="s">
         <v>196</v>
       </c>
@@ -3335,27 +3344,27 @@
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="20"/>
+      <c r="B25" s="21"/>
       <c r="C25" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="20"/>
+      <c r="F25" s="21"/>
       <c r="G25" t="s">
         <v>71</v>
       </c>
-      <c r="J25" s="20"/>
+      <c r="J25" s="21"/>
       <c r="K25" t="s">
         <v>105</v>
       </c>
-      <c r="N25" s="20"/>
+      <c r="N25" s="21"/>
       <c r="O25" t="s">
         <v>134</v>
       </c>
-      <c r="R25" s="27"/>
+      <c r="R25" s="28"/>
       <c r="S25" t="s">
         <v>167</v>
       </c>
-      <c r="V25" s="26" t="s">
+      <c r="V25" s="27" t="s">
         <v>18</v>
       </c>
       <c r="W25" t="s">
@@ -3366,31 +3375,31 @@
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="22" t="s">
         <v>36</v>
       </c>
       <c r="C26" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="20"/>
+      <c r="F26" s="21"/>
       <c r="G26" t="s">
         <v>68</v>
       </c>
-      <c r="J26" s="20"/>
+      <c r="J26" s="21"/>
       <c r="K26" t="s">
         <v>106</v>
       </c>
-      <c r="N26" s="20"/>
+      <c r="N26" s="21"/>
       <c r="O26" t="s">
         <v>135</v>
       </c>
-      <c r="R26" s="20" t="s">
+      <c r="R26" s="21" t="s">
         <v>30</v>
       </c>
       <c r="S26" t="s">
         <v>168</v>
       </c>
-      <c r="V26" s="26"/>
+      <c r="V26" s="27"/>
       <c r="W26" t="s">
         <v>198</v>
       </c>
@@ -3399,31 +3408,31 @@
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="21"/>
+      <c r="B27" s="22"/>
       <c r="C27" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="21" t="s">
+      <c r="F27" s="22" t="s">
         <v>36</v>
       </c>
       <c r="G27" t="s">
         <v>72</v>
       </c>
-      <c r="J27" s="21" t="s">
+      <c r="J27" s="22" t="s">
         <v>36</v>
       </c>
       <c r="K27" t="s">
         <v>40</v>
       </c>
-      <c r="N27" s="20"/>
+      <c r="N27" s="21"/>
       <c r="O27" t="s">
         <v>136</v>
       </c>
-      <c r="R27" s="20"/>
+      <c r="R27" s="21"/>
       <c r="S27" t="s">
         <v>169</v>
       </c>
-      <c r="V27" s="26"/>
+      <c r="V27" s="27"/>
       <c r="W27" t="s">
         <v>199</v>
       </c>
@@ -3432,27 +3441,27 @@
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="21"/>
+      <c r="B28" s="22"/>
       <c r="C28" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="21"/>
+      <c r="F28" s="22"/>
       <c r="G28" t="s">
         <v>73</v>
       </c>
-      <c r="J28" s="21"/>
+      <c r="J28" s="22"/>
       <c r="K28" t="s">
         <v>108</v>
       </c>
-      <c r="N28" s="20"/>
+      <c r="N28" s="21"/>
       <c r="O28" t="s">
         <v>137</v>
       </c>
-      <c r="R28" s="20"/>
+      <c r="R28" s="21"/>
       <c r="S28" t="s">
         <v>170</v>
       </c>
-      <c r="V28" s="27" t="s">
+      <c r="V28" s="28" t="s">
         <v>24</v>
       </c>
       <c r="W28" t="s">
@@ -3463,27 +3472,27 @@
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="21"/>
+      <c r="B29" s="22"/>
       <c r="C29" t="s">
         <v>107</v>
       </c>
-      <c r="F29" s="21"/>
+      <c r="F29" s="22"/>
       <c r="G29" t="s">
         <v>74</v>
       </c>
-      <c r="J29" s="21"/>
+      <c r="J29" s="22"/>
       <c r="K29" t="s">
         <v>110</v>
       </c>
-      <c r="N29" s="20"/>
+      <c r="N29" s="21"/>
       <c r="O29" t="s">
         <v>138</v>
       </c>
-      <c r="R29" s="20"/>
+      <c r="R29" s="21"/>
       <c r="S29" t="s">
         <v>171</v>
       </c>
-      <c r="V29" s="27"/>
+      <c r="V29" s="28"/>
       <c r="W29" t="s">
         <v>201</v>
       </c>
@@ -3492,25 +3501,25 @@
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="F30" s="21"/>
+      <c r="F30" s="22"/>
       <c r="G30" t="s">
         <v>75</v>
       </c>
-      <c r="J30" s="21"/>
+      <c r="J30" s="22"/>
       <c r="K30" t="s">
         <v>41</v>
       </c>
-      <c r="N30" s="21" t="s">
+      <c r="N30" s="22" t="s">
         <v>36</v>
       </c>
       <c r="O30" t="s">
         <v>139</v>
       </c>
-      <c r="R30" s="20"/>
+      <c r="R30" s="21"/>
       <c r="S30" t="s">
         <v>172</v>
       </c>
-      <c r="V30" s="27"/>
+      <c r="V30" s="28"/>
       <c r="W30" t="s">
         <v>202</v>
       </c>
@@ -3519,35 +3528,35 @@
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="F31" s="21"/>
+      <c r="F31" s="22"/>
       <c r="G31" t="s">
         <v>275</v>
       </c>
-      <c r="N31" s="21"/>
+      <c r="N31" s="22"/>
       <c r="O31" t="s">
         <v>140</v>
       </c>
-      <c r="R31" s="21" t="s">
+      <c r="R31" s="22" t="s">
         <v>36</v>
       </c>
       <c r="S31" t="s">
         <v>173</v>
       </c>
-      <c r="V31" s="27"/>
+      <c r="V31" s="28"/>
       <c r="W31" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="N32" s="21"/>
+      <c r="N32" s="22"/>
       <c r="O32" t="s">
         <v>141</v>
       </c>
-      <c r="R32" s="21"/>
+      <c r="R32" s="22"/>
       <c r="S32" t="s">
         <v>174</v>
       </c>
-      <c r="V32" s="20" t="s">
+      <c r="V32" s="21" t="s">
         <v>30</v>
       </c>
       <c r="W32" t="s">
@@ -3555,43 +3564,43 @@
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="N33" s="21"/>
+      <c r="N33" s="22"/>
       <c r="O33" t="s">
         <v>142</v>
       </c>
-      <c r="R33" s="21"/>
+      <c r="R33" s="22"/>
       <c r="S33" t="s">
         <v>175</v>
       </c>
-      <c r="V33" s="20"/>
+      <c r="V33" s="21"/>
       <c r="W33" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="R34" s="21"/>
+      <c r="R34" s="22"/>
       <c r="S34" t="s">
         <v>176</v>
       </c>
-      <c r="V34" s="20"/>
+      <c r="V34" s="21"/>
       <c r="W34" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V35" s="20"/>
+      <c r="V35" s="21"/>
       <c r="W35" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V36" s="20"/>
+      <c r="V36" s="21"/>
       <c r="W36" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V37" s="21" t="s">
+      <c r="V37" s="22" t="s">
         <v>36</v>
       </c>
       <c r="W37" t="s">
@@ -3599,26 +3608,21 @@
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V38" s="21"/>
+      <c r="V38" s="22"/>
       <c r="W38" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V39" s="21"/>
+      <c r="V39" s="22"/>
       <c r="W39" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V40" s="21"/>
+      <c r="V40" s="22"/>
       <c r="W40" t="s">
         <v>211</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="G41" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.35">
@@ -3637,48 +3641,48 @@
       <c r="R43" t="s">
         <v>315</v>
       </c>
-      <c r="V43" s="22" t="s">
+      <c r="V43" s="23" t="s">
         <v>316</v>
       </c>
-      <c r="W43" s="22"/>
-      <c r="X43" s="22"/>
-      <c r="Y43" s="22"/>
+      <c r="W43" s="23"/>
+      <c r="X43" s="23"/>
+      <c r="Y43" s="23"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>1</v>
       </c>
-      <c r="B44" s="23" t="s">
+      <c r="B44" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C44" t="s">
         <v>44</v>
       </c>
-      <c r="F44" s="23" t="s">
+      <c r="F44" s="24" t="s">
         <v>1</v>
       </c>
       <c r="G44" t="s">
         <v>246</v>
       </c>
-      <c r="J44" s="23" t="s">
+      <c r="J44" s="24" t="s">
         <v>1</v>
       </c>
       <c r="K44" t="s">
         <v>280</v>
       </c>
-      <c r="N44" s="23" t="s">
+      <c r="N44" s="24" t="s">
         <v>1</v>
       </c>
       <c r="O44" t="s">
         <v>317</v>
       </c>
-      <c r="R44" s="23" t="s">
+      <c r="R44" s="24" t="s">
         <v>1</v>
       </c>
       <c r="S44" t="s">
         <v>348</v>
       </c>
-      <c r="V44" s="23" t="s">
+      <c r="V44" s="24" t="s">
         <v>1</v>
       </c>
       <c r="W44" t="s">
@@ -3689,27 +3693,27 @@
       <c r="A45" s="1">
         <v>2</v>
       </c>
-      <c r="B45" s="23"/>
+      <c r="B45" s="24"/>
       <c r="C45" t="s">
         <v>214</v>
       </c>
-      <c r="F45" s="23"/>
+      <c r="F45" s="24"/>
       <c r="G45" t="s">
         <v>247</v>
       </c>
-      <c r="J45" s="23"/>
+      <c r="J45" s="24"/>
       <c r="K45" t="s">
         <v>281</v>
       </c>
-      <c r="N45" s="23"/>
+      <c r="N45" s="24"/>
       <c r="O45" t="s">
         <v>318</v>
       </c>
-      <c r="R45" s="23"/>
+      <c r="R45" s="24"/>
       <c r="S45" t="s">
         <v>349</v>
       </c>
-      <c r="V45" s="23"/>
+      <c r="V45" s="24"/>
       <c r="W45" t="s">
         <v>379</v>
       </c>
@@ -3718,27 +3722,27 @@
       <c r="A46" s="1">
         <v>3</v>
       </c>
-      <c r="B46" s="23"/>
+      <c r="B46" s="24"/>
       <c r="C46" t="s">
         <v>213</v>
       </c>
-      <c r="F46" s="23"/>
+      <c r="F46" s="24"/>
       <c r="G46" t="s">
         <v>79</v>
       </c>
-      <c r="J46" s="23"/>
+      <c r="J46" s="24"/>
       <c r="K46" t="s">
         <v>282</v>
       </c>
-      <c r="N46" s="23"/>
+      <c r="N46" s="24"/>
       <c r="O46" t="s">
         <v>319</v>
       </c>
-      <c r="R46" s="23"/>
+      <c r="R46" s="24"/>
       <c r="S46" t="s">
         <v>78</v>
       </c>
-      <c r="V46" s="23"/>
+      <c r="V46" s="24"/>
       <c r="W46" t="s">
         <v>380</v>
       </c>
@@ -3747,35 +3751,35 @@
       <c r="A47" s="1">
         <v>4</v>
       </c>
-      <c r="B47" s="24" t="s">
+      <c r="B47" s="25" t="s">
         <v>5</v>
       </c>
       <c r="C47" t="s">
         <v>216</v>
       </c>
-      <c r="F47" s="24" t="s">
+      <c r="F47" s="25" t="s">
         <v>5</v>
       </c>
       <c r="G47" t="s">
         <v>183</v>
       </c>
-      <c r="J47" s="24" t="s">
+      <c r="J47" s="25" t="s">
         <v>5</v>
       </c>
       <c r="K47" t="s">
         <v>283</v>
       </c>
-      <c r="N47" s="24" t="s">
+      <c r="N47" s="25" t="s">
         <v>5</v>
       </c>
       <c r="O47" t="s">
         <v>320</v>
       </c>
-      <c r="R47" s="23"/>
+      <c r="R47" s="24"/>
       <c r="S47" t="s">
         <v>350</v>
       </c>
-      <c r="V47" s="24" t="s">
+      <c r="V47" s="25" t="s">
         <v>5</v>
       </c>
       <c r="W47" t="s">
@@ -3786,29 +3790,29 @@
       <c r="A48" s="1">
         <v>5</v>
       </c>
-      <c r="B48" s="24"/>
+      <c r="B48" s="25"/>
       <c r="C48" t="s">
         <v>217</v>
       </c>
-      <c r="F48" s="24"/>
+      <c r="F48" s="25"/>
       <c r="G48" t="s">
         <v>321</v>
       </c>
-      <c r="J48" s="24"/>
+      <c r="J48" s="25"/>
       <c r="K48" t="s">
         <v>284</v>
       </c>
-      <c r="N48" s="24"/>
+      <c r="N48" s="25"/>
       <c r="O48" t="s">
         <v>251</v>
       </c>
-      <c r="R48" s="24" t="s">
+      <c r="R48" s="25" t="s">
         <v>5</v>
       </c>
       <c r="S48" t="s">
         <v>351</v>
       </c>
-      <c r="V48" s="24"/>
+      <c r="V48" s="25"/>
       <c r="W48" t="s">
         <v>382</v>
       </c>
@@ -3817,27 +3821,27 @@
       <c r="A49" s="1">
         <v>6</v>
       </c>
-      <c r="B49" s="24"/>
+      <c r="B49" s="25"/>
       <c r="C49" t="s">
         <v>221</v>
       </c>
-      <c r="F49" s="24"/>
+      <c r="F49" s="25"/>
       <c r="G49" t="s">
         <v>185</v>
       </c>
-      <c r="J49" s="24"/>
+      <c r="J49" s="25"/>
       <c r="K49" t="s">
         <v>285</v>
       </c>
-      <c r="N49" s="24"/>
+      <c r="N49" s="25"/>
       <c r="O49" t="s">
         <v>322</v>
       </c>
-      <c r="R49" s="24"/>
+      <c r="R49" s="25"/>
       <c r="S49" t="s">
         <v>352</v>
       </c>
-      <c r="V49" s="24"/>
+      <c r="V49" s="25"/>
       <c r="W49" t="s">
         <v>383</v>
       </c>
@@ -3846,31 +3850,31 @@
       <c r="A50" s="1">
         <v>7</v>
       </c>
-      <c r="B50" s="24"/>
+      <c r="B50" s="25"/>
       <c r="C50" t="s">
         <v>222</v>
       </c>
-      <c r="F50" s="24"/>
+      <c r="F50" s="25"/>
       <c r="G50" t="s">
         <v>249</v>
       </c>
-      <c r="J50" s="25" t="s">
+      <c r="J50" s="26" t="s">
         <v>12</v>
       </c>
       <c r="K50" t="s">
         <v>286</v>
       </c>
-      <c r="N50" s="25" t="s">
+      <c r="N50" s="26" t="s">
         <v>12</v>
       </c>
       <c r="O50" t="s">
         <v>323</v>
       </c>
-      <c r="R50" s="24"/>
+      <c r="R50" s="25"/>
       <c r="S50" t="s">
         <v>353</v>
       </c>
-      <c r="V50" s="24"/>
+      <c r="V50" s="25"/>
       <c r="W50" t="s">
         <v>384</v>
       </c>
@@ -3879,29 +3883,29 @@
       <c r="A51" s="1">
         <v>8</v>
       </c>
-      <c r="B51" s="25" t="s">
+      <c r="B51" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C51" t="s">
         <v>57</v>
       </c>
-      <c r="F51" s="24"/>
+      <c r="F51" s="25"/>
       <c r="G51" t="s">
         <v>253</v>
       </c>
-      <c r="J51" s="25"/>
+      <c r="J51" s="26"/>
       <c r="K51" t="s">
         <v>287</v>
       </c>
-      <c r="N51" s="25"/>
+      <c r="N51" s="26"/>
       <c r="O51" t="s">
         <v>324</v>
       </c>
-      <c r="R51" s="24"/>
+      <c r="R51" s="25"/>
       <c r="S51" t="s">
         <v>354</v>
       </c>
-      <c r="V51" s="24"/>
+      <c r="V51" s="25"/>
       <c r="W51" t="s">
         <v>385</v>
       </c>
@@ -3910,27 +3914,27 @@
       <c r="A52" s="1">
         <v>9</v>
       </c>
-      <c r="B52" s="25"/>
+      <c r="B52" s="26"/>
       <c r="C52" t="s">
         <v>218</v>
       </c>
-      <c r="F52" s="24"/>
+      <c r="F52" s="25"/>
       <c r="G52" t="s">
         <v>254</v>
       </c>
-      <c r="J52" s="25"/>
+      <c r="J52" s="26"/>
       <c r="K52" t="s">
         <v>288</v>
       </c>
-      <c r="N52" s="25"/>
+      <c r="N52" s="26"/>
       <c r="O52" t="s">
         <v>325</v>
       </c>
-      <c r="R52" s="24"/>
+      <c r="R52" s="25"/>
       <c r="S52" t="s">
         <v>355</v>
       </c>
-      <c r="V52" s="25" t="s">
+      <c r="V52" s="26" t="s">
         <v>12</v>
       </c>
       <c r="W52" t="s">
@@ -3941,29 +3945,29 @@
       <c r="A53" s="1">
         <v>10</v>
       </c>
-      <c r="B53" s="25"/>
+      <c r="B53" s="26"/>
       <c r="C53" t="s">
         <v>219</v>
       </c>
-      <c r="F53" s="24"/>
+      <c r="F53" s="25"/>
       <c r="G53" t="s">
         <v>255</v>
       </c>
-      <c r="J53" s="25"/>
+      <c r="J53" s="26"/>
       <c r="K53" t="s">
         <v>289</v>
       </c>
-      <c r="N53" s="25"/>
+      <c r="N53" s="26"/>
       <c r="O53" t="s">
         <v>326</v>
       </c>
-      <c r="R53" s="25" t="s">
+      <c r="R53" s="26" t="s">
         <v>12</v>
       </c>
       <c r="S53" t="s">
         <v>356</v>
       </c>
-      <c r="V53" s="25"/>
+      <c r="V53" s="26"/>
       <c r="W53" t="s">
         <v>387</v>
       </c>
@@ -3972,27 +3976,27 @@
       <c r="A54" s="1">
         <v>11</v>
       </c>
-      <c r="B54" s="25"/>
+      <c r="B54" s="26"/>
       <c r="C54" t="s">
         <v>93</v>
       </c>
-      <c r="F54" s="24"/>
+      <c r="F54" s="25"/>
       <c r="G54" t="s">
         <v>83</v>
       </c>
-      <c r="J54" s="25"/>
+      <c r="J54" s="26"/>
       <c r="K54" t="s">
         <v>290</v>
       </c>
-      <c r="N54" s="25"/>
+      <c r="N54" s="26"/>
       <c r="O54" t="s">
         <v>327</v>
       </c>
-      <c r="R54" s="25"/>
+      <c r="R54" s="26"/>
       <c r="S54" t="s">
         <v>357</v>
       </c>
-      <c r="V54" s="25"/>
+      <c r="V54" s="26"/>
       <c r="W54" t="s">
         <v>388</v>
       </c>
@@ -4001,29 +4005,27 @@
       <c r="A55" s="1">
         <v>12</v>
       </c>
-      <c r="B55" s="25"/>
+      <c r="B55" s="26"/>
       <c r="C55" t="s">
         <v>220</v>
       </c>
-      <c r="F55" s="25" t="s">
-        <v>12</v>
-      </c>
+      <c r="F55" s="25"/>
       <c r="G55" t="s">
-        <v>194</v>
-      </c>
-      <c r="J55" s="25"/>
+        <v>51</v>
+      </c>
+      <c r="J55" s="26"/>
       <c r="K55" t="s">
         <v>291</v>
       </c>
-      <c r="N55" s="25"/>
+      <c r="N55" s="26"/>
       <c r="O55" t="s">
         <v>328</v>
       </c>
-      <c r="R55" s="25"/>
+      <c r="R55" s="26"/>
       <c r="S55" t="s">
         <v>358</v>
       </c>
-      <c r="V55" s="25"/>
+      <c r="V55" s="26"/>
       <c r="W55" t="s">
         <v>389</v>
       </c>
@@ -4032,27 +4034,29 @@
       <c r="A56" s="1">
         <v>13</v>
       </c>
-      <c r="B56" s="25"/>
+      <c r="B56" s="26"/>
       <c r="C56" t="s">
         <v>223</v>
       </c>
-      <c r="F56" s="25"/>
+      <c r="F56" s="26" t="s">
+        <v>12</v>
+      </c>
       <c r="G56" t="s">
-        <v>258</v>
-      </c>
-      <c r="J56" s="25"/>
+        <v>194</v>
+      </c>
+      <c r="J56" s="26"/>
       <c r="K56" t="s">
         <v>292</v>
       </c>
-      <c r="N56" s="25"/>
+      <c r="N56" s="26"/>
       <c r="O56" t="s">
         <v>329</v>
       </c>
-      <c r="R56" s="25"/>
+      <c r="R56" s="26"/>
       <c r="S56" t="s">
         <v>359</v>
       </c>
-      <c r="V56" s="25"/>
+      <c r="V56" s="26"/>
       <c r="W56" t="s">
         <v>390</v>
       </c>
@@ -4061,27 +4065,27 @@
       <c r="A57" s="1">
         <v>14</v>
       </c>
-      <c r="B57" s="25"/>
+      <c r="B57" s="26"/>
       <c r="C57" t="s">
         <v>224</v>
       </c>
-      <c r="F57" s="25"/>
+      <c r="F57" s="26"/>
       <c r="G57" t="s">
-        <v>90</v>
-      </c>
-      <c r="J57" s="25"/>
+        <v>258</v>
+      </c>
+      <c r="J57" s="26"/>
       <c r="K57" t="s">
         <v>293</v>
       </c>
-      <c r="N57" s="25"/>
+      <c r="N57" s="26"/>
       <c r="O57" t="s">
         <v>257</v>
       </c>
-      <c r="R57" s="25"/>
+      <c r="R57" s="26"/>
       <c r="S57" t="s">
         <v>360</v>
       </c>
-      <c r="V57" s="25"/>
+      <c r="V57" s="26"/>
       <c r="W57" t="s">
         <v>391</v>
       </c>
@@ -4090,27 +4094,27 @@
       <c r="A58" s="1">
         <v>15</v>
       </c>
-      <c r="B58" s="25"/>
+      <c r="B58" s="26"/>
       <c r="C58" t="s">
         <v>227</v>
       </c>
-      <c r="F58" s="25"/>
+      <c r="F58" s="26"/>
       <c r="G58" t="s">
-        <v>260</v>
-      </c>
-      <c r="J58" s="25"/>
+        <v>90</v>
+      </c>
+      <c r="J58" s="26"/>
       <c r="K58" t="s">
         <v>294</v>
       </c>
-      <c r="N58" s="25"/>
+      <c r="N58" s="26"/>
       <c r="O58" t="s">
         <v>263</v>
       </c>
-      <c r="R58" s="25"/>
+      <c r="R58" s="26"/>
       <c r="S58" t="s">
         <v>361</v>
       </c>
-      <c r="V58" s="25"/>
+      <c r="V58" s="26"/>
       <c r="W58" t="s">
         <v>392</v>
       </c>
@@ -4119,27 +4123,27 @@
       <c r="A59" s="1">
         <v>16</v>
       </c>
-      <c r="B59" s="25"/>
+      <c r="B59" s="26"/>
       <c r="C59" t="s">
         <v>228</v>
       </c>
-      <c r="F59" s="25"/>
+      <c r="F59" s="26"/>
       <c r="G59" t="s">
-        <v>262</v>
-      </c>
-      <c r="J59" s="25"/>
+        <v>260</v>
+      </c>
+      <c r="J59" s="26"/>
       <c r="K59" t="s">
         <v>295</v>
       </c>
-      <c r="N59" s="25"/>
+      <c r="N59" s="26"/>
       <c r="O59" t="s">
         <v>330</v>
       </c>
-      <c r="R59" s="25"/>
+      <c r="R59" s="26"/>
       <c r="S59" t="s">
         <v>362</v>
       </c>
-      <c r="V59" s="25"/>
+      <c r="V59" s="26"/>
       <c r="W59" t="s">
         <v>393</v>
       </c>
@@ -4148,21 +4152,21 @@
       <c r="A60" s="1">
         <v>17</v>
       </c>
-      <c r="B60" s="25"/>
+      <c r="B60" s="26"/>
       <c r="C60" t="s">
         <v>229</v>
       </c>
-      <c r="F60" s="25"/>
+      <c r="F60" s="26"/>
       <c r="G60" t="s">
-        <v>259</v>
-      </c>
-      <c r="J60" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="J60" s="27" t="s">
         <v>18</v>
       </c>
       <c r="K60" t="s">
         <v>296</v>
       </c>
-      <c r="N60" s="26" t="s">
+      <c r="N60" s="27" t="s">
         <v>18</v>
       </c>
       <c r="O60" t="s">
@@ -4174,7 +4178,7 @@
       <c r="S60" t="s">
         <v>363</v>
       </c>
-      <c r="V60" s="26" t="s">
+      <c r="V60" s="27" t="s">
         <v>18</v>
       </c>
       <c r="W60" t="s">
@@ -4185,29 +4189,29 @@
       <c r="A61" s="1">
         <v>18</v>
       </c>
-      <c r="B61" s="25"/>
+      <c r="B61" s="26"/>
       <c r="C61" t="s">
         <v>55</v>
       </c>
-      <c r="F61" s="25"/>
+      <c r="F61" s="26"/>
       <c r="G61" t="s">
-        <v>92</v>
-      </c>
-      <c r="J61" s="26"/>
+        <v>259</v>
+      </c>
+      <c r="J61" s="27"/>
       <c r="K61" t="s">
         <v>297</v>
       </c>
-      <c r="N61" s="26"/>
+      <c r="N61" s="27"/>
       <c r="O61" t="s">
         <v>332</v>
       </c>
-      <c r="R61" s="27" t="s">
+      <c r="R61" s="28" t="s">
         <v>24</v>
       </c>
       <c r="S61" t="s">
         <v>364</v>
       </c>
-      <c r="V61" s="26"/>
+      <c r="V61" s="27"/>
       <c r="W61" t="s">
         <v>395</v>
       </c>
@@ -4216,31 +4220,29 @@
       <c r="A62" s="1">
         <v>19</v>
       </c>
-      <c r="B62" s="26" t="s">
+      <c r="B62" s="27" t="s">
         <v>18</v>
       </c>
       <c r="C62" t="s">
         <v>233</v>
       </c>
-      <c r="F62" s="26" t="s">
-        <v>18</v>
-      </c>
+      <c r="F62" s="26"/>
       <c r="G62" t="s">
-        <v>264</v>
-      </c>
-      <c r="J62" s="26"/>
+        <v>92</v>
+      </c>
+      <c r="J62" s="27"/>
       <c r="K62" t="s">
         <v>298</v>
       </c>
-      <c r="N62" s="26"/>
+      <c r="N62" s="27"/>
       <c r="O62" t="s">
         <v>333</v>
       </c>
-      <c r="R62" s="27"/>
+      <c r="R62" s="28"/>
       <c r="S62" t="s">
         <v>365</v>
       </c>
-      <c r="V62" s="26"/>
+      <c r="V62" s="27"/>
       <c r="W62" t="s">
         <v>396</v>
       </c>
@@ -4249,29 +4251,31 @@
       <c r="A63" s="1">
         <v>20</v>
       </c>
-      <c r="B63" s="26"/>
+      <c r="B63" s="27"/>
       <c r="C63" t="s">
         <v>230</v>
       </c>
-      <c r="F63" s="26"/>
+      <c r="F63" s="27" t="s">
+        <v>18</v>
+      </c>
       <c r="G63" t="s">
-        <v>265</v>
-      </c>
-      <c r="J63" s="27" t="s">
+        <v>264</v>
+      </c>
+      <c r="J63" s="28" t="s">
         <v>24</v>
       </c>
       <c r="K63" t="s">
         <v>299</v>
       </c>
-      <c r="N63" s="26"/>
+      <c r="N63" s="27"/>
       <c r="O63" t="s">
         <v>334</v>
       </c>
-      <c r="R63" s="27"/>
+      <c r="R63" s="28"/>
       <c r="S63" t="s">
         <v>366</v>
       </c>
-      <c r="V63" s="26"/>
+      <c r="V63" s="27"/>
       <c r="W63" t="s">
         <v>397</v>
       </c>
@@ -4280,27 +4284,27 @@
       <c r="A64" s="1">
         <v>21</v>
       </c>
-      <c r="B64" s="26"/>
+      <c r="B64" s="27"/>
       <c r="C64" t="s">
         <v>231</v>
       </c>
-      <c r="F64" s="26"/>
+      <c r="F64" s="27"/>
       <c r="G64" t="s">
-        <v>266</v>
-      </c>
-      <c r="J64" s="27"/>
+        <v>265</v>
+      </c>
+      <c r="J64" s="28"/>
       <c r="K64" t="s">
         <v>300</v>
       </c>
-      <c r="N64" s="26"/>
+      <c r="N64" s="27"/>
       <c r="O64" t="s">
         <v>335</v>
       </c>
-      <c r="R64" s="27"/>
+      <c r="R64" s="28"/>
       <c r="S64" t="s">
         <v>367</v>
       </c>
-      <c r="V64" s="27" t="s">
+      <c r="V64" s="28" t="s">
         <v>24</v>
       </c>
       <c r="W64" t="s">
@@ -4311,29 +4315,29 @@
       <c r="A65" s="1">
         <v>22</v>
       </c>
-      <c r="B65" s="26"/>
+      <c r="B65" s="27"/>
       <c r="C65" t="s">
         <v>232</v>
       </c>
-      <c r="F65" s="26"/>
+      <c r="F65" s="27"/>
       <c r="G65" t="s">
-        <v>267</v>
-      </c>
-      <c r="J65" s="27"/>
+        <v>266</v>
+      </c>
+      <c r="J65" s="28"/>
       <c r="K65" t="s">
         <v>301</v>
       </c>
-      <c r="N65" s="27" t="s">
+      <c r="N65" s="28" t="s">
         <v>24</v>
       </c>
       <c r="O65" t="s">
         <v>336</v>
       </c>
-      <c r="R65" s="27"/>
+      <c r="R65" s="28"/>
       <c r="S65" t="s">
         <v>368</v>
       </c>
-      <c r="V65" s="27"/>
+      <c r="V65" s="28"/>
       <c r="W65" t="s">
         <v>399</v>
       </c>
@@ -4342,31 +4346,29 @@
       <c r="A66" s="1">
         <v>23</v>
       </c>
-      <c r="B66" s="26"/>
+      <c r="B66" s="27"/>
       <c r="C66" t="s">
         <v>61</v>
       </c>
-      <c r="F66" s="27" t="s">
-        <v>24</v>
-      </c>
+      <c r="F66" s="27"/>
       <c r="G66" t="s">
-        <v>268</v>
-      </c>
-      <c r="J66" s="27"/>
+        <v>267</v>
+      </c>
+      <c r="J66" s="28"/>
       <c r="K66" t="s">
         <v>302</v>
       </c>
-      <c r="N66" s="27"/>
+      <c r="N66" s="28"/>
       <c r="O66" t="s">
         <v>337</v>
       </c>
-      <c r="R66" s="20" t="s">
+      <c r="R66" s="21" t="s">
         <v>30</v>
       </c>
       <c r="S66" t="s">
         <v>369</v>
       </c>
-      <c r="V66" s="27"/>
+      <c r="V66" s="28"/>
       <c r="W66" t="s">
         <v>400</v>
       </c>
@@ -4375,29 +4377,31 @@
       <c r="A67" s="1">
         <v>24</v>
       </c>
-      <c r="B67" s="27" t="s">
+      <c r="B67" s="28" t="s">
         <v>24</v>
       </c>
       <c r="C67" t="s">
         <v>102</v>
       </c>
-      <c r="F67" s="27"/>
+      <c r="F67" s="28" t="s">
+        <v>24</v>
+      </c>
       <c r="G67" t="s">
-        <v>269</v>
-      </c>
-      <c r="J67" s="27"/>
+        <v>268</v>
+      </c>
+      <c r="J67" s="28"/>
       <c r="K67" t="s">
         <v>303</v>
       </c>
-      <c r="N67" s="27"/>
+      <c r="N67" s="28"/>
       <c r="O67" t="s">
         <v>338</v>
       </c>
-      <c r="R67" s="20"/>
+      <c r="R67" s="21"/>
       <c r="S67" t="s">
         <v>370</v>
       </c>
-      <c r="V67" s="27"/>
+      <c r="V67" s="28"/>
       <c r="W67" t="s">
         <v>401</v>
       </c>
@@ -4406,27 +4410,27 @@
       <c r="A68" s="1">
         <v>25</v>
       </c>
-      <c r="B68" s="27"/>
+      <c r="B68" s="28"/>
       <c r="C68" t="s">
         <v>234</v>
       </c>
-      <c r="F68" s="27"/>
+      <c r="F68" s="28"/>
       <c r="G68" t="s">
-        <v>270</v>
-      </c>
-      <c r="J68" s="27"/>
+        <v>269</v>
+      </c>
+      <c r="J68" s="28"/>
       <c r="K68" t="s">
         <v>304</v>
       </c>
-      <c r="N68" s="27"/>
+      <c r="N68" s="28"/>
       <c r="O68" t="s">
         <v>342</v>
       </c>
-      <c r="R68" s="20"/>
+      <c r="R68" s="21"/>
       <c r="S68" t="s">
         <v>371</v>
       </c>
-      <c r="V68" s="20" t="s">
+      <c r="V68" s="21" t="s">
         <v>30</v>
       </c>
       <c r="W68" t="s">
@@ -4437,29 +4441,29 @@
       <c r="A69" s="1">
         <v>26</v>
       </c>
-      <c r="B69" s="27"/>
+      <c r="B69" s="28"/>
       <c r="C69" t="s">
         <v>235</v>
       </c>
-      <c r="F69" s="27"/>
+      <c r="F69" s="28"/>
       <c r="G69" t="s">
-        <v>101</v>
-      </c>
-      <c r="J69" s="27"/>
+        <v>270</v>
+      </c>
+      <c r="J69" s="28"/>
       <c r="K69" t="s">
         <v>305</v>
       </c>
-      <c r="N69" s="20" t="s">
+      <c r="N69" s="21" t="s">
         <v>30</v>
       </c>
       <c r="O69" t="s">
         <v>339</v>
       </c>
-      <c r="R69" s="20"/>
+      <c r="R69" s="21"/>
       <c r="S69" t="s">
         <v>372</v>
       </c>
-      <c r="V69" s="20"/>
+      <c r="V69" s="21"/>
       <c r="W69" t="s">
         <v>403</v>
       </c>
@@ -4468,33 +4472,31 @@
       <c r="A70" s="1">
         <v>27</v>
       </c>
-      <c r="B70" s="27"/>
+      <c r="B70" s="28"/>
       <c r="C70" t="s">
         <v>236</v>
       </c>
-      <c r="F70" s="20" t="s">
-        <v>30</v>
-      </c>
+      <c r="F70" s="28"/>
       <c r="G70" t="s">
-        <v>271</v>
-      </c>
-      <c r="J70" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="J70" s="21" t="s">
         <v>30</v>
       </c>
       <c r="K70" t="s">
         <v>306</v>
       </c>
-      <c r="N70" s="20"/>
+      <c r="N70" s="21"/>
       <c r="O70" t="s">
         <v>340</v>
       </c>
-      <c r="R70" s="21" t="s">
+      <c r="R70" s="22" t="s">
         <v>36</v>
       </c>
       <c r="S70" t="s">
         <v>373</v>
       </c>
-      <c r="V70" s="20"/>
+      <c r="V70" s="21"/>
       <c r="W70" t="s">
         <v>404</v>
       </c>
@@ -4503,27 +4505,29 @@
       <c r="A71" s="1">
         <v>28</v>
       </c>
-      <c r="B71" s="27"/>
+      <c r="B71" s="28"/>
       <c r="C71" t="s">
         <v>237</v>
       </c>
-      <c r="F71" s="20"/>
+      <c r="F71" s="21" t="s">
+        <v>30</v>
+      </c>
       <c r="G71" t="s">
-        <v>272</v>
-      </c>
-      <c r="J71" s="20"/>
+        <v>271</v>
+      </c>
+      <c r="J71" s="21"/>
       <c r="K71" t="s">
         <v>307</v>
       </c>
-      <c r="N71" s="20"/>
+      <c r="N71" s="21"/>
       <c r="O71" t="s">
         <v>341</v>
       </c>
-      <c r="R71" s="21"/>
+      <c r="R71" s="22"/>
       <c r="S71" t="s">
         <v>374</v>
       </c>
-      <c r="V71" s="20"/>
+      <c r="V71" s="21"/>
       <c r="W71" t="s">
         <v>405</v>
       </c>
@@ -4532,27 +4536,27 @@
       <c r="A72" s="1">
         <v>29</v>
       </c>
-      <c r="B72" s="27"/>
+      <c r="B72" s="28"/>
       <c r="C72" t="s">
         <v>238</v>
       </c>
-      <c r="F72" s="20"/>
+      <c r="F72" s="21"/>
       <c r="G72" t="s">
-        <v>273</v>
-      </c>
-      <c r="J72" s="20"/>
+        <v>272</v>
+      </c>
+      <c r="J72" s="21"/>
       <c r="K72" t="s">
         <v>308</v>
       </c>
-      <c r="N72" s="20"/>
+      <c r="N72" s="21"/>
       <c r="O72" t="s">
         <v>343</v>
       </c>
-      <c r="R72" s="21"/>
+      <c r="R72" s="22"/>
       <c r="S72" t="s">
         <v>375</v>
       </c>
-      <c r="V72" s="20"/>
+      <c r="V72" s="21"/>
       <c r="W72" t="s">
         <v>406</v>
       </c>
@@ -4561,31 +4565,31 @@
       <c r="A73" s="1">
         <v>30</v>
       </c>
-      <c r="B73" s="20" t="s">
+      <c r="B73" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C73" t="s">
         <v>34</v>
       </c>
-      <c r="F73" s="20"/>
+      <c r="F73" s="21"/>
       <c r="G73" t="s">
-        <v>274</v>
-      </c>
-      <c r="J73" s="20"/>
+        <v>273</v>
+      </c>
+      <c r="J73" s="21"/>
       <c r="K73" t="s">
         <v>309</v>
       </c>
-      <c r="N73" s="21" t="s">
+      <c r="N73" s="22" t="s">
         <v>36</v>
       </c>
       <c r="O73" t="s">
         <v>344</v>
       </c>
-      <c r="R73" s="21"/>
+      <c r="R73" s="22"/>
       <c r="S73" t="s">
         <v>376</v>
       </c>
-      <c r="V73" s="21" t="s">
+      <c r="V73" s="22" t="s">
         <v>36</v>
       </c>
       <c r="W73" t="s">
@@ -4593,126 +4597,134 @@
       </c>
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B74" s="20"/>
+      <c r="B74" s="21"/>
       <c r="C74" t="s">
         <v>239</v>
       </c>
-      <c r="F74" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J74" s="21" t="s">
+      <c r="F74" s="21"/>
+      <c r="G74" t="s">
+        <v>274</v>
+      </c>
+      <c r="J74" s="22" t="s">
         <v>36</v>
       </c>
       <c r="K74" t="s">
         <v>310</v>
       </c>
-      <c r="N74" s="21"/>
+      <c r="N74" s="22"/>
       <c r="O74" t="s">
         <v>345</v>
       </c>
-      <c r="R74" s="21"/>
+      <c r="R74" s="22"/>
       <c r="S74" t="s">
         <v>377</v>
       </c>
-      <c r="V74" s="21"/>
+      <c r="V74" s="22"/>
       <c r="W74" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B75" s="20"/>
+      <c r="B75" s="21"/>
       <c r="C75" t="s">
         <v>240</v>
       </c>
-      <c r="F75" s="21"/>
+      <c r="F75" s="22" t="s">
+        <v>36</v>
+      </c>
       <c r="G75" t="s">
         <v>276</v>
       </c>
-      <c r="J75" s="21"/>
+      <c r="J75" s="22"/>
       <c r="K75" t="s">
         <v>311</v>
       </c>
-      <c r="N75" s="21"/>
+      <c r="N75" s="22"/>
       <c r="O75" t="s">
         <v>346</v>
       </c>
-      <c r="V75" s="21"/>
+      <c r="V75" s="22"/>
       <c r="W75" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B76" s="20"/>
+      <c r="B76" s="21"/>
       <c r="C76" t="s">
         <v>241</v>
       </c>
-      <c r="F76" s="21"/>
+      <c r="F76" s="22"/>
       <c r="G76" t="s">
         <v>277</v>
       </c>
-      <c r="J76" s="21"/>
+      <c r="J76" s="22"/>
       <c r="K76" t="s">
         <v>312</v>
       </c>
-      <c r="N76" s="21"/>
+      <c r="N76" s="22"/>
       <c r="O76" t="s">
         <v>347</v>
       </c>
-      <c r="V76" s="21"/>
+      <c r="V76" s="22"/>
       <c r="W76" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="77" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B77" s="21" t="s">
+      <c r="B77" s="22" t="s">
         <v>36</v>
       </c>
       <c r="C77" t="s">
         <v>109</v>
       </c>
-      <c r="F77" s="21"/>
+      <c r="F77" s="22"/>
       <c r="G77" t="s">
         <v>278</v>
       </c>
-      <c r="J77" s="21"/>
+      <c r="J77" s="22"/>
       <c r="K77" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B78" s="21"/>
+      <c r="B78" s="22"/>
       <c r="C78" t="s">
         <v>242</v>
       </c>
-      <c r="F78" s="21"/>
+      <c r="F78" s="22"/>
       <c r="G78" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B79" s="21"/>
+      <c r="B79" s="22"/>
       <c r="C79" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B80" s="21"/>
+      <c r="B80" s="22"/>
       <c r="C80" t="s">
         <v>244</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="V25:V27"/>
+    <mergeCell ref="V28:V31"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="R4:R9"/>
+    <mergeCell ref="R10:R19"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="F10:F15"/>
+    <mergeCell ref="J20:J22"/>
+    <mergeCell ref="V2:V5"/>
     <mergeCell ref="F6:F9"/>
     <mergeCell ref="V6:V13"/>
     <mergeCell ref="J10:J15"/>
     <mergeCell ref="J4:J9"/>
     <mergeCell ref="F2:F5"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="F10:F15"/>
-    <mergeCell ref="J20:J22"/>
     <mergeCell ref="B44:B46"/>
     <mergeCell ref="B62:B66"/>
     <mergeCell ref="F16:F18"/>
@@ -4722,11 +4734,12 @@
     <mergeCell ref="F19:F22"/>
     <mergeCell ref="F23:F26"/>
     <mergeCell ref="B47:B50"/>
-    <mergeCell ref="F47:F54"/>
     <mergeCell ref="F44:F46"/>
-    <mergeCell ref="F55:F61"/>
+    <mergeCell ref="F56:F62"/>
     <mergeCell ref="B51:B61"/>
-    <mergeCell ref="F62:F65"/>
+    <mergeCell ref="F63:F66"/>
+    <mergeCell ref="F47:F55"/>
+    <mergeCell ref="F27:F31"/>
     <mergeCell ref="J70:J73"/>
     <mergeCell ref="J74:J77"/>
     <mergeCell ref="N44:N46"/>
@@ -4739,15 +4752,12 @@
     <mergeCell ref="J60:J62"/>
     <mergeCell ref="J50:J59"/>
     <mergeCell ref="J63:J69"/>
-    <mergeCell ref="F70:F73"/>
-    <mergeCell ref="F66:F69"/>
-    <mergeCell ref="F74:F78"/>
+    <mergeCell ref="F71:F74"/>
+    <mergeCell ref="F67:F70"/>
     <mergeCell ref="B67:B72"/>
     <mergeCell ref="B73:B76"/>
     <mergeCell ref="B77:B80"/>
-    <mergeCell ref="V2:V5"/>
-    <mergeCell ref="V25:V27"/>
-    <mergeCell ref="V28:V31"/>
+    <mergeCell ref="F75:F78"/>
     <mergeCell ref="R44:R47"/>
     <mergeCell ref="J27:J30"/>
     <mergeCell ref="N24:N29"/>
@@ -4756,9 +4766,6 @@
     <mergeCell ref="J44:J46"/>
     <mergeCell ref="J47:J49"/>
     <mergeCell ref="J23:J26"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="R4:R9"/>
-    <mergeCell ref="R10:R19"/>
     <mergeCell ref="R20:R21"/>
     <mergeCell ref="R22:R25"/>
     <mergeCell ref="N2:N3"/>
@@ -4797,7 +4804,7 @@
   <dimension ref="A1:Z50"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4818,36 +4825,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="E1" s="22" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="E1" s="23" t="s">
         <v>412</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
       <c r="J1" t="s">
         <v>411</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="O1" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="T1" s="22" t="s">
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="T1" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="X1" s="22" t="s">
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="X1" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -4886,7 +4893,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>413</v>
+        <v>596</v>
       </c>
       <c r="B3" t="s">
         <v>487</v>
@@ -4933,7 +4940,7 @@
         <v>496</v>
       </c>
       <c r="J4" t="s">
-        <v>596</v>
+        <v>413</v>
       </c>
       <c r="K4" t="s">
         <v>492</v>
@@ -4991,7 +4998,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E6" t="s">
         <v>606</v>
@@ -5014,7 +5021,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E7" t="s">
         <v>622</v>
@@ -5027,9 +5034,6 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>490</v>
-      </c>
       <c r="E8" t="s">
         <v>419</v>
       </c>
@@ -5055,41 +5059,46 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="K11" t="s">
-        <v>510</v>
+        <v>491</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="K12" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="K13" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
       <c r="E17" t="s">
         <v>420</v>
       </c>
-      <c r="I17" s="22" t="s">
+      <c r="I17" s="23" t="s">
         <v>421</v>
       </c>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="N17" s="22" t="s">
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="N17" s="23" t="s">
         <v>314</v>
       </c>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="S17" s="22" t="s">
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="S17" s="23" t="s">
         <v>315</v>
       </c>
-      <c r="T17" s="22"/>
-      <c r="U17" s="22"/>
-      <c r="V17" s="22"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
       <c r="X17" t="s">
         <v>316</v>
       </c>
@@ -5613,10 +5622,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K115"/>
+  <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+    <sheetView topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118:B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6274,6 +6283,41 @@
         <v>663</v>
       </c>
     </row>
+    <row r="117" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" s="5" t="s">
+        <v>578</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" s="10"/>
+      <c r="B119" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="B120" s="11" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" s="10"/>
+      <c r="B121" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A122" s="7"/>
+      <c r="B122" s="8" t="s">
+        <v>666</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
picks updated accordingly after last trades.
Good catch Vanja
</commit_message>
<xml_diff>
--- a/OffSeason.xlsx
+++ b/OffSeason.xlsx
@@ -2304,14 +2304,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2322,14 +2319,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2615,7 +2615,7 @@
   <dimension ref="A1:Y80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="C10" sqref="C10:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2630,11 +2630,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
       <c r="F1" t="s">
         <v>42</v>
       </c>
@@ -2655,37 +2655,37 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="K2" t="s">
         <v>77</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="O2" t="s">
         <v>112</v>
       </c>
-      <c r="R2" s="23" t="s">
+      <c r="R2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="S2" t="s">
         <v>144</v>
       </c>
-      <c r="V2" s="23" t="s">
+      <c r="V2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="W2" t="s">
@@ -2696,27 +2696,27 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="22"/>
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="23"/>
+      <c r="F3" s="22"/>
       <c r="G3" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="23"/>
+      <c r="J3" s="22"/>
       <c r="K3" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="23"/>
+      <c r="N3" s="22"/>
       <c r="O3" t="s">
         <v>104</v>
       </c>
-      <c r="R3" s="23"/>
+      <c r="R3" s="22"/>
       <c r="S3" t="s">
         <v>145</v>
       </c>
-      <c r="V3" s="23"/>
+      <c r="V3" s="22"/>
       <c r="W3" t="s">
         <v>179</v>
       </c>
@@ -2725,35 +2725,35 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="23"/>
+      <c r="F4" s="22"/>
       <c r="G4" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="23" t="s">
         <v>5</v>
       </c>
       <c r="K4" t="s">
         <v>248</v>
       </c>
-      <c r="N4" s="24" t="s">
+      <c r="N4" s="23" t="s">
         <v>5</v>
       </c>
       <c r="O4" t="s">
         <v>113</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="23" t="s">
         <v>5</v>
       </c>
       <c r="S4" t="s">
         <v>146</v>
       </c>
-      <c r="V4" s="23"/>
+      <c r="V4" s="22"/>
       <c r="W4" t="s">
         <v>180</v>
       </c>
@@ -2762,27 +2762,27 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="23"/>
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="23"/>
+      <c r="F5" s="22"/>
       <c r="G5" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="24"/>
+      <c r="J5" s="23"/>
       <c r="K5" t="s">
         <v>81</v>
       </c>
-      <c r="N5" s="24"/>
+      <c r="N5" s="23"/>
       <c r="O5" t="s">
         <v>114</v>
       </c>
-      <c r="R5" s="24"/>
+      <c r="R5" s="23"/>
       <c r="S5" t="s">
         <v>147</v>
       </c>
-      <c r="V5" s="23"/>
+      <c r="V5" s="22"/>
       <c r="W5" t="s">
         <v>181</v>
       </c>
@@ -2791,29 +2791,29 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="23"/>
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="23" t="s">
         <v>5</v>
       </c>
       <c r="G6" t="s">
         <v>215</v>
       </c>
-      <c r="J6" s="24"/>
+      <c r="J6" s="23"/>
       <c r="K6" t="s">
         <v>82</v>
       </c>
-      <c r="N6" s="24"/>
+      <c r="N6" s="23"/>
       <c r="O6" t="s">
         <v>115</v>
       </c>
-      <c r="R6" s="24"/>
+      <c r="R6" s="23"/>
       <c r="S6" t="s">
         <v>148</v>
       </c>
-      <c r="V6" s="24" t="s">
+      <c r="V6" s="23" t="s">
         <v>5</v>
       </c>
       <c r="W6" t="s">
@@ -2824,27 +2824,27 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="24"/>
+      <c r="B7" s="23"/>
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="24"/>
+      <c r="F7" s="23"/>
       <c r="G7" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="24"/>
+      <c r="J7" s="23"/>
       <c r="K7" t="s">
         <v>84</v>
       </c>
-      <c r="N7" s="24"/>
+      <c r="N7" s="23"/>
       <c r="O7" t="s">
         <v>116</v>
       </c>
-      <c r="R7" s="24"/>
+      <c r="R7" s="23"/>
       <c r="S7" t="s">
         <v>149</v>
       </c>
-      <c r="V7" s="24"/>
+      <c r="V7" s="23"/>
       <c r="W7" t="s">
         <v>250</v>
       </c>
@@ -2853,27 +2853,27 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="24"/>
+      <c r="B8" s="23"/>
       <c r="C8" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="23"/>
       <c r="G8" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="24"/>
+      <c r="J8" s="23"/>
       <c r="K8" t="s">
         <v>48</v>
       </c>
-      <c r="N8" s="24"/>
+      <c r="N8" s="23"/>
       <c r="O8" t="s">
         <v>117</v>
       </c>
-      <c r="R8" s="24"/>
+      <c r="R8" s="23"/>
       <c r="S8" t="s">
         <v>150</v>
       </c>
-      <c r="V8" s="24"/>
+      <c r="V8" s="23"/>
       <c r="W8" t="s">
         <v>184</v>
       </c>
@@ -2882,27 +2882,27 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="24"/>
+      <c r="B9" s="23"/>
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="24"/>
+      <c r="F9" s="23"/>
       <c r="G9" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="24"/>
+      <c r="J9" s="23"/>
       <c r="K9" t="s">
         <v>85</v>
       </c>
-      <c r="N9" s="24"/>
+      <c r="N9" s="23"/>
       <c r="O9" t="s">
         <v>118</v>
       </c>
-      <c r="R9" s="24"/>
+      <c r="R9" s="23"/>
       <c r="S9" t="s">
         <v>151</v>
       </c>
-      <c r="V9" s="24"/>
+      <c r="V9" s="23"/>
       <c r="W9" t="s">
         <v>252</v>
       </c>
@@ -2911,35 +2911,35 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G10" t="s">
         <v>54</v>
       </c>
-      <c r="J10" s="25" t="s">
+      <c r="J10" s="24" t="s">
         <v>12</v>
       </c>
       <c r="K10" t="s">
         <v>15</v>
       </c>
-      <c r="N10" s="24"/>
+      <c r="N10" s="23"/>
       <c r="O10" t="s">
         <v>119</v>
       </c>
-      <c r="R10" s="25" t="s">
+      <c r="R10" s="24" t="s">
         <v>12</v>
       </c>
       <c r="S10" t="s">
         <v>152</v>
       </c>
-      <c r="V10" s="24"/>
+      <c r="V10" s="23"/>
       <c r="W10" t="s">
         <v>186</v>
       </c>
@@ -2948,29 +2948,29 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="25"/>
+      <c r="B11" s="24"/>
       <c r="C11" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="25"/>
+      <c r="F11" s="24"/>
       <c r="G11" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="25"/>
+      <c r="J11" s="24"/>
       <c r="K11" t="s">
         <v>188</v>
       </c>
-      <c r="N11" s="25" t="s">
+      <c r="N11" s="24" t="s">
         <v>12</v>
       </c>
       <c r="O11" t="s">
         <v>120</v>
       </c>
-      <c r="R11" s="25"/>
+      <c r="R11" s="24"/>
       <c r="S11" t="s">
         <v>153</v>
       </c>
-      <c r="V11" s="24"/>
+      <c r="V11" s="23"/>
       <c r="W11" t="s">
         <v>187</v>
       </c>
@@ -2979,27 +2979,27 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="25"/>
+      <c r="B12" s="24"/>
       <c r="C12" t="s">
         <v>86</v>
       </c>
-      <c r="F12" s="25"/>
+      <c r="F12" s="24"/>
       <c r="G12" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="25"/>
+      <c r="J12" s="24"/>
       <c r="K12" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="25"/>
+      <c r="N12" s="24"/>
       <c r="O12" t="s">
         <v>121</v>
       </c>
-      <c r="R12" s="25"/>
+      <c r="R12" s="24"/>
       <c r="S12" t="s">
         <v>154</v>
       </c>
-      <c r="V12" s="24"/>
+      <c r="V12" s="23"/>
       <c r="W12" t="s">
         <v>53</v>
       </c>
@@ -3008,27 +3008,27 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="25"/>
+      <c r="B13" s="24"/>
       <c r="C13" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="25"/>
+      <c r="F13" s="24"/>
       <c r="G13" t="s">
         <v>59</v>
       </c>
-      <c r="J13" s="25"/>
+      <c r="J13" s="24"/>
       <c r="K13" t="s">
         <v>88</v>
       </c>
-      <c r="N13" s="25"/>
+      <c r="N13" s="24"/>
       <c r="O13" t="s">
         <v>122</v>
       </c>
-      <c r="R13" s="25"/>
+      <c r="R13" s="24"/>
       <c r="S13" t="s">
         <v>155</v>
       </c>
-      <c r="V13" s="24"/>
+      <c r="V13" s="23"/>
       <c r="W13" t="s">
         <v>10</v>
       </c>
@@ -3037,27 +3037,27 @@
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="25"/>
+      <c r="B14" s="24"/>
       <c r="C14" t="s">
         <v>87</v>
       </c>
-      <c r="F14" s="25"/>
+      <c r="F14" s="24"/>
       <c r="G14" t="s">
         <v>226</v>
       </c>
-      <c r="J14" s="25"/>
+      <c r="J14" s="24"/>
       <c r="K14" t="s">
         <v>16</v>
       </c>
-      <c r="N14" s="25"/>
+      <c r="N14" s="24"/>
       <c r="O14" t="s">
         <v>123</v>
       </c>
-      <c r="R14" s="25"/>
+      <c r="R14" s="24"/>
       <c r="S14" t="s">
         <v>156</v>
       </c>
-      <c r="V14" s="25" t="s">
+      <c r="V14" s="24" t="s">
         <v>12</v>
       </c>
       <c r="W14" t="s">
@@ -3068,29 +3068,29 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="25"/>
+      <c r="F15" s="24"/>
       <c r="G15" t="s">
         <v>225</v>
       </c>
-      <c r="J15" s="25"/>
+      <c r="J15" s="24"/>
       <c r="K15" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="25"/>
+      <c r="N15" s="24"/>
       <c r="O15" t="s">
         <v>124</v>
       </c>
-      <c r="R15" s="25"/>
+      <c r="R15" s="24"/>
       <c r="S15" t="s">
         <v>157</v>
       </c>
-      <c r="V15" s="25"/>
+      <c r="V15" s="24"/>
       <c r="W15" t="s">
         <v>189</v>
       </c>
@@ -3099,29 +3099,29 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="26"/>
+      <c r="B16" s="20"/>
       <c r="C16" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="20" t="s">
         <v>18</v>
       </c>
       <c r="G16" t="s">
         <v>60</v>
       </c>
-      <c r="J16" s="25"/>
+      <c r="J16" s="24"/>
       <c r="K16" t="s">
         <v>259</v>
       </c>
-      <c r="N16" s="25"/>
+      <c r="N16" s="24"/>
       <c r="O16" t="s">
         <v>125</v>
       </c>
-      <c r="R16" s="25"/>
+      <c r="R16" s="24"/>
       <c r="S16" t="s">
         <v>158</v>
       </c>
-      <c r="V16" s="25"/>
+      <c r="V16" s="24"/>
       <c r="W16" t="s">
         <v>190</v>
       </c>
@@ -3130,31 +3130,31 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="26"/>
+      <c r="B17" s="20"/>
       <c r="C17" t="s">
         <v>96</v>
       </c>
-      <c r="F17" s="26"/>
+      <c r="F17" s="20"/>
       <c r="G17" t="s">
         <v>62</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="20" t="s">
         <v>18</v>
       </c>
       <c r="K17" t="s">
         <v>95</v>
       </c>
-      <c r="N17" s="26" t="s">
+      <c r="N17" s="20" t="s">
         <v>18</v>
       </c>
       <c r="O17" t="s">
         <v>126</v>
       </c>
-      <c r="R17" s="25"/>
+      <c r="R17" s="24"/>
       <c r="S17" t="s">
         <v>159</v>
       </c>
-      <c r="V17" s="25"/>
+      <c r="V17" s="24"/>
       <c r="W17" t="s">
         <v>191</v>
       </c>
@@ -3163,29 +3163,29 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="26"/>
+      <c r="F18" s="20"/>
       <c r="G18" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="26"/>
+      <c r="J18" s="20"/>
       <c r="K18" t="s">
         <v>21</v>
       </c>
-      <c r="N18" s="26"/>
+      <c r="N18" s="20"/>
       <c r="O18" t="s">
         <v>127</v>
       </c>
-      <c r="R18" s="25"/>
+      <c r="R18" s="24"/>
       <c r="S18" t="s">
         <v>160</v>
       </c>
-      <c r="V18" s="25"/>
+      <c r="V18" s="24"/>
       <c r="W18" t="s">
         <v>91</v>
       </c>
@@ -3194,31 +3194,31 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="27"/>
+      <c r="B19" s="21"/>
       <c r="C19" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="21" t="s">
         <v>24</v>
       </c>
       <c r="G19" t="s">
         <v>64</v>
       </c>
-      <c r="J19" s="26"/>
+      <c r="J19" s="20"/>
       <c r="K19" t="s">
         <v>98</v>
       </c>
-      <c r="N19" s="27" t="s">
+      <c r="N19" s="21" t="s">
         <v>24</v>
       </c>
       <c r="O19" t="s">
         <v>128</v>
       </c>
-      <c r="R19" s="25"/>
+      <c r="R19" s="24"/>
       <c r="S19" t="s">
         <v>161</v>
       </c>
-      <c r="V19" s="25"/>
+      <c r="V19" s="24"/>
       <c r="W19" t="s">
         <v>261</v>
       </c>
@@ -3227,31 +3227,31 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="27"/>
+      <c r="B20" s="21"/>
       <c r="C20" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="27"/>
+      <c r="F20" s="21"/>
       <c r="G20" t="s">
         <v>65</v>
       </c>
-      <c r="J20" s="27" t="s">
+      <c r="J20" s="21" t="s">
         <v>24</v>
       </c>
       <c r="K20" t="s">
         <v>99</v>
       </c>
-      <c r="N20" s="27"/>
+      <c r="N20" s="21"/>
       <c r="O20" t="s">
         <v>129</v>
       </c>
-      <c r="R20" s="26" t="s">
+      <c r="R20" s="20" t="s">
         <v>18</v>
       </c>
       <c r="S20" t="s">
         <v>162</v>
       </c>
-      <c r="V20" s="25"/>
+      <c r="V20" s="24"/>
       <c r="W20" t="s">
         <v>94</v>
       </c>
@@ -3260,27 +3260,27 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="27"/>
+      <c r="B21" s="21"/>
       <c r="C21" t="s">
         <v>100</v>
       </c>
-      <c r="F21" s="27"/>
+      <c r="F21" s="21"/>
       <c r="G21" t="s">
         <v>66</v>
       </c>
-      <c r="J21" s="27"/>
+      <c r="J21" s="21"/>
       <c r="K21" t="s">
         <v>28</v>
       </c>
-      <c r="N21" s="27"/>
+      <c r="N21" s="21"/>
       <c r="O21" t="s">
         <v>130</v>
       </c>
-      <c r="R21" s="26"/>
+      <c r="R21" s="20"/>
       <c r="S21" t="s">
         <v>163</v>
       </c>
-      <c r="V21" s="25"/>
+      <c r="V21" s="24"/>
       <c r="W21" t="s">
         <v>192</v>
       </c>
@@ -3289,31 +3289,31 @@
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="26" t="s">
         <v>30</v>
       </c>
       <c r="C22" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="27"/>
+      <c r="F22" s="21"/>
       <c r="G22" t="s">
         <v>67</v>
       </c>
-      <c r="J22" s="27"/>
+      <c r="J22" s="21"/>
       <c r="K22" t="s">
         <v>29</v>
       </c>
-      <c r="N22" s="27"/>
+      <c r="N22" s="21"/>
       <c r="O22" t="s">
         <v>131</v>
       </c>
-      <c r="R22" s="27" t="s">
+      <c r="R22" s="21" t="s">
         <v>24</v>
       </c>
       <c r="S22" t="s">
         <v>164</v>
       </c>
-      <c r="V22" s="25"/>
+      <c r="V22" s="24"/>
       <c r="W22" t="s">
         <v>193</v>
       </c>
@@ -3322,31 +3322,31 @@
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="20"/>
+      <c r="B23" s="26"/>
       <c r="C23" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="26" t="s">
         <v>30</v>
       </c>
       <c r="G23" t="s">
         <v>69</v>
       </c>
-      <c r="J23" s="20" t="s">
+      <c r="J23" s="26" t="s">
         <v>30</v>
       </c>
       <c r="K23" t="s">
         <v>103</v>
       </c>
-      <c r="N23" s="27"/>
+      <c r="N23" s="21"/>
       <c r="O23" t="s">
         <v>132</v>
       </c>
-      <c r="R23" s="27"/>
+      <c r="R23" s="21"/>
       <c r="S23" t="s">
         <v>165</v>
       </c>
-      <c r="V23" s="25"/>
+      <c r="V23" s="24"/>
       <c r="W23" t="s">
         <v>195</v>
       </c>
@@ -3355,29 +3355,29 @@
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="20"/>
+      <c r="B24" s="26"/>
       <c r="C24" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="20"/>
+      <c r="F24" s="26"/>
       <c r="G24" t="s">
         <v>70</v>
       </c>
-      <c r="J24" s="20"/>
+      <c r="J24" s="26"/>
       <c r="K24" t="s">
         <v>104</v>
       </c>
-      <c r="N24" s="20" t="s">
+      <c r="N24" s="26" t="s">
         <v>30</v>
       </c>
       <c r="O24" t="s">
         <v>133</v>
       </c>
-      <c r="R24" s="27"/>
+      <c r="R24" s="21"/>
       <c r="S24" t="s">
         <v>166</v>
       </c>
-      <c r="V24" s="25"/>
+      <c r="V24" s="24"/>
       <c r="W24" t="s">
         <v>196</v>
       </c>
@@ -3386,29 +3386,29 @@
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="25" t="s">
         <v>36</v>
       </c>
       <c r="C25" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="20"/>
+      <c r="F25" s="26"/>
       <c r="G25" t="s">
         <v>71</v>
       </c>
-      <c r="J25" s="20"/>
+      <c r="J25" s="26"/>
       <c r="K25" t="s">
         <v>105</v>
       </c>
-      <c r="N25" s="20"/>
+      <c r="N25" s="26"/>
       <c r="O25" t="s">
         <v>134</v>
       </c>
-      <c r="R25" s="27"/>
+      <c r="R25" s="21"/>
       <c r="S25" t="s">
         <v>167</v>
       </c>
-      <c r="V25" s="26" t="s">
+      <c r="V25" s="20" t="s">
         <v>18</v>
       </c>
       <c r="W25" t="s">
@@ -3419,29 +3419,29 @@
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="21"/>
+      <c r="B26" s="25"/>
       <c r="C26" t="s">
         <v>38</v>
       </c>
-      <c r="F26" s="20"/>
+      <c r="F26" s="26"/>
       <c r="G26" t="s">
         <v>68</v>
       </c>
-      <c r="J26" s="20"/>
+      <c r="J26" s="26"/>
       <c r="K26" t="s">
         <v>106</v>
       </c>
-      <c r="N26" s="20"/>
+      <c r="N26" s="26"/>
       <c r="O26" t="s">
         <v>135</v>
       </c>
-      <c r="R26" s="20" t="s">
+      <c r="R26" s="26" t="s">
         <v>30</v>
       </c>
       <c r="S26" t="s">
         <v>168</v>
       </c>
-      <c r="V26" s="26"/>
+      <c r="V26" s="20"/>
       <c r="W26" t="s">
         <v>198</v>
       </c>
@@ -3450,31 +3450,31 @@
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="21"/>
+      <c r="B27" s="25"/>
       <c r="C27" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="21" t="s">
+      <c r="F27" s="25" t="s">
         <v>36</v>
       </c>
       <c r="G27" t="s">
         <v>72</v>
       </c>
-      <c r="J27" s="21" t="s">
+      <c r="J27" s="25" t="s">
         <v>36</v>
       </c>
       <c r="K27" t="s">
         <v>40</v>
       </c>
-      <c r="N27" s="20"/>
+      <c r="N27" s="26"/>
       <c r="O27" t="s">
         <v>136</v>
       </c>
-      <c r="R27" s="20"/>
+      <c r="R27" s="26"/>
       <c r="S27" t="s">
         <v>169</v>
       </c>
-      <c r="V27" s="26"/>
+      <c r="V27" s="20"/>
       <c r="W27" t="s">
         <v>199</v>
       </c>
@@ -3483,27 +3483,27 @@
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="21"/>
+      <c r="B28" s="25"/>
       <c r="C28" t="s">
         <v>107</v>
       </c>
-      <c r="F28" s="21"/>
+      <c r="F28" s="25"/>
       <c r="G28" t="s">
         <v>73</v>
       </c>
-      <c r="J28" s="21"/>
+      <c r="J28" s="25"/>
       <c r="K28" t="s">
         <v>108</v>
       </c>
-      <c r="N28" s="20"/>
+      <c r="N28" s="26"/>
       <c r="O28" t="s">
         <v>137</v>
       </c>
-      <c r="R28" s="20"/>
+      <c r="R28" s="26"/>
       <c r="S28" t="s">
         <v>170</v>
       </c>
-      <c r="V28" s="27" t="s">
+      <c r="V28" s="21" t="s">
         <v>24</v>
       </c>
       <c r="W28" t="s">
@@ -3514,23 +3514,23 @@
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="F29" s="21"/>
+      <c r="F29" s="25"/>
       <c r="G29" t="s">
         <v>74</v>
       </c>
-      <c r="J29" s="21"/>
+      <c r="J29" s="25"/>
       <c r="K29" t="s">
         <v>110</v>
       </c>
-      <c r="N29" s="20"/>
+      <c r="N29" s="26"/>
       <c r="O29" t="s">
         <v>138</v>
       </c>
-      <c r="R29" s="20"/>
+      <c r="R29" s="26"/>
       <c r="S29" t="s">
         <v>171</v>
       </c>
-      <c r="V29" s="27"/>
+      <c r="V29" s="21"/>
       <c r="W29" t="s">
         <v>201</v>
       </c>
@@ -3539,25 +3539,25 @@
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="F30" s="21"/>
+      <c r="F30" s="25"/>
       <c r="G30" t="s">
         <v>75</v>
       </c>
-      <c r="J30" s="21"/>
+      <c r="J30" s="25"/>
       <c r="K30" t="s">
         <v>41</v>
       </c>
-      <c r="N30" s="21" t="s">
+      <c r="N30" s="25" t="s">
         <v>36</v>
       </c>
       <c r="O30" t="s">
         <v>139</v>
       </c>
-      <c r="R30" s="20"/>
+      <c r="R30" s="26"/>
       <c r="S30" t="s">
         <v>172</v>
       </c>
-      <c r="V30" s="27"/>
+      <c r="V30" s="21"/>
       <c r="W30" t="s">
         <v>202</v>
       </c>
@@ -3566,35 +3566,35 @@
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="F31" s="21"/>
+      <c r="F31" s="25"/>
       <c r="G31" t="s">
         <v>275</v>
       </c>
-      <c r="N31" s="21"/>
+      <c r="N31" s="25"/>
       <c r="O31" t="s">
         <v>140</v>
       </c>
-      <c r="R31" s="21" t="s">
+      <c r="R31" s="25" t="s">
         <v>36</v>
       </c>
       <c r="S31" t="s">
         <v>173</v>
       </c>
-      <c r="V31" s="27"/>
+      <c r="V31" s="21"/>
       <c r="W31" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="N32" s="21"/>
+      <c r="N32" s="25"/>
       <c r="O32" t="s">
         <v>141</v>
       </c>
-      <c r="R32" s="21"/>
+      <c r="R32" s="25"/>
       <c r="S32" t="s">
         <v>174</v>
       </c>
-      <c r="V32" s="20" t="s">
+      <c r="V32" s="26" t="s">
         <v>30</v>
       </c>
       <c r="W32" t="s">
@@ -3602,43 +3602,43 @@
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="N33" s="21"/>
+      <c r="N33" s="25"/>
       <c r="O33" t="s">
         <v>142</v>
       </c>
-      <c r="R33" s="21"/>
+      <c r="R33" s="25"/>
       <c r="S33" t="s">
         <v>175</v>
       </c>
-      <c r="V33" s="20"/>
+      <c r="V33" s="26"/>
       <c r="W33" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="R34" s="21"/>
+      <c r="R34" s="25"/>
       <c r="S34" t="s">
         <v>176</v>
       </c>
-      <c r="V34" s="20"/>
+      <c r="V34" s="26"/>
       <c r="W34" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V35" s="20"/>
+      <c r="V35" s="26"/>
       <c r="W35" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V36" s="20"/>
+      <c r="V36" s="26"/>
       <c r="W36" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V37" s="21" t="s">
+      <c r="V37" s="25" t="s">
         <v>36</v>
       </c>
       <c r="W37" t="s">
@@ -3646,19 +3646,19 @@
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V38" s="21"/>
+      <c r="V38" s="25"/>
       <c r="W38" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V39" s="21"/>
+      <c r="V39" s="25"/>
       <c r="W39" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V40" s="21"/>
+      <c r="V40" s="25"/>
       <c r="W40" t="s">
         <v>211</v>
       </c>
@@ -3679,48 +3679,48 @@
       <c r="R43" t="s">
         <v>315</v>
       </c>
-      <c r="V43" s="22" t="s">
+      <c r="V43" s="28" t="s">
         <v>316</v>
       </c>
-      <c r="W43" s="22"/>
-      <c r="X43" s="22"/>
-      <c r="Y43" s="22"/>
+      <c r="W43" s="28"/>
+      <c r="X43" s="28"/>
+      <c r="Y43" s="28"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>1</v>
       </c>
-      <c r="B44" s="23" t="s">
+      <c r="B44" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C44" t="s">
         <v>44</v>
       </c>
-      <c r="F44" s="23" t="s">
+      <c r="F44" s="22" t="s">
         <v>1</v>
       </c>
       <c r="G44" t="s">
         <v>246</v>
       </c>
-      <c r="J44" s="23" t="s">
+      <c r="J44" s="22" t="s">
         <v>1</v>
       </c>
       <c r="K44" t="s">
         <v>280</v>
       </c>
-      <c r="N44" s="23" t="s">
+      <c r="N44" s="22" t="s">
         <v>1</v>
       </c>
       <c r="O44" t="s">
         <v>317</v>
       </c>
-      <c r="R44" s="23" t="s">
+      <c r="R44" s="22" t="s">
         <v>1</v>
       </c>
       <c r="S44" t="s">
         <v>348</v>
       </c>
-      <c r="V44" s="23" t="s">
+      <c r="V44" s="22" t="s">
         <v>1</v>
       </c>
       <c r="W44" t="s">
@@ -3731,27 +3731,27 @@
       <c r="A45" s="1">
         <v>2</v>
       </c>
-      <c r="B45" s="23"/>
+      <c r="B45" s="22"/>
       <c r="C45" t="s">
         <v>214</v>
       </c>
-      <c r="F45" s="23"/>
+      <c r="F45" s="22"/>
       <c r="G45" t="s">
         <v>247</v>
       </c>
-      <c r="J45" s="23"/>
+      <c r="J45" s="22"/>
       <c r="K45" t="s">
         <v>281</v>
       </c>
-      <c r="N45" s="23"/>
+      <c r="N45" s="22"/>
       <c r="O45" t="s">
         <v>318</v>
       </c>
-      <c r="R45" s="23"/>
+      <c r="R45" s="22"/>
       <c r="S45" t="s">
         <v>349</v>
       </c>
-      <c r="V45" s="23"/>
+      <c r="V45" s="22"/>
       <c r="W45" t="s">
         <v>379</v>
       </c>
@@ -3760,27 +3760,27 @@
       <c r="A46" s="1">
         <v>3</v>
       </c>
-      <c r="B46" s="23"/>
+      <c r="B46" s="22"/>
       <c r="C46" t="s">
         <v>213</v>
       </c>
-      <c r="F46" s="23"/>
+      <c r="F46" s="22"/>
       <c r="G46" t="s">
         <v>79</v>
       </c>
-      <c r="J46" s="23"/>
+      <c r="J46" s="22"/>
       <c r="K46" t="s">
         <v>282</v>
       </c>
-      <c r="N46" s="23"/>
+      <c r="N46" s="22"/>
       <c r="O46" t="s">
         <v>319</v>
       </c>
-      <c r="R46" s="23"/>
+      <c r="R46" s="22"/>
       <c r="S46" t="s">
         <v>78</v>
       </c>
-      <c r="V46" s="23"/>
+      <c r="V46" s="22"/>
       <c r="W46" t="s">
         <v>380</v>
       </c>
@@ -3789,35 +3789,35 @@
       <c r="A47" s="1">
         <v>4</v>
       </c>
-      <c r="B47" s="24" t="s">
+      <c r="B47" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C47" t="s">
         <v>216</v>
       </c>
-      <c r="F47" s="24" t="s">
+      <c r="F47" s="23" t="s">
         <v>5</v>
       </c>
       <c r="G47" t="s">
         <v>183</v>
       </c>
-      <c r="J47" s="24" t="s">
+      <c r="J47" s="23" t="s">
         <v>5</v>
       </c>
       <c r="K47" t="s">
         <v>283</v>
       </c>
-      <c r="N47" s="24" t="s">
+      <c r="N47" s="23" t="s">
         <v>5</v>
       </c>
       <c r="O47" t="s">
         <v>320</v>
       </c>
-      <c r="R47" s="23"/>
+      <c r="R47" s="22"/>
       <c r="S47" t="s">
         <v>350</v>
       </c>
-      <c r="V47" s="24" t="s">
+      <c r="V47" s="23" t="s">
         <v>5</v>
       </c>
       <c r="W47" t="s">
@@ -3828,29 +3828,29 @@
       <c r="A48" s="1">
         <v>5</v>
       </c>
-      <c r="B48" s="24"/>
+      <c r="B48" s="23"/>
       <c r="C48" t="s">
         <v>217</v>
       </c>
-      <c r="F48" s="24"/>
+      <c r="F48" s="23"/>
       <c r="G48" t="s">
         <v>321</v>
       </c>
-      <c r="J48" s="24"/>
+      <c r="J48" s="23"/>
       <c r="K48" t="s">
         <v>284</v>
       </c>
-      <c r="N48" s="24"/>
+      <c r="N48" s="23"/>
       <c r="O48" t="s">
         <v>251</v>
       </c>
-      <c r="R48" s="24" t="s">
+      <c r="R48" s="23" t="s">
         <v>5</v>
       </c>
       <c r="S48" t="s">
         <v>351</v>
       </c>
-      <c r="V48" s="24"/>
+      <c r="V48" s="23"/>
       <c r="W48" t="s">
         <v>382</v>
       </c>
@@ -3859,27 +3859,27 @@
       <c r="A49" s="1">
         <v>6</v>
       </c>
-      <c r="B49" s="24"/>
+      <c r="B49" s="23"/>
       <c r="C49" t="s">
         <v>221</v>
       </c>
-      <c r="F49" s="24"/>
+      <c r="F49" s="23"/>
       <c r="G49" t="s">
         <v>185</v>
       </c>
-      <c r="J49" s="24"/>
+      <c r="J49" s="23"/>
       <c r="K49" t="s">
         <v>285</v>
       </c>
-      <c r="N49" s="24"/>
+      <c r="N49" s="23"/>
       <c r="O49" t="s">
         <v>322</v>
       </c>
-      <c r="R49" s="24"/>
+      <c r="R49" s="23"/>
       <c r="S49" t="s">
         <v>352</v>
       </c>
-      <c r="V49" s="24"/>
+      <c r="V49" s="23"/>
       <c r="W49" t="s">
         <v>383</v>
       </c>
@@ -3888,31 +3888,31 @@
       <c r="A50" s="1">
         <v>7</v>
       </c>
-      <c r="B50" s="24"/>
+      <c r="B50" s="23"/>
       <c r="C50" t="s">
         <v>222</v>
       </c>
-      <c r="F50" s="24"/>
+      <c r="F50" s="23"/>
       <c r="G50" t="s">
         <v>249</v>
       </c>
-      <c r="J50" s="25" t="s">
+      <c r="J50" s="24" t="s">
         <v>12</v>
       </c>
       <c r="K50" t="s">
         <v>286</v>
       </c>
-      <c r="N50" s="25" t="s">
+      <c r="N50" s="24" t="s">
         <v>12</v>
       </c>
       <c r="O50" t="s">
         <v>323</v>
       </c>
-      <c r="R50" s="24"/>
+      <c r="R50" s="23"/>
       <c r="S50" t="s">
         <v>353</v>
       </c>
-      <c r="V50" s="24"/>
+      <c r="V50" s="23"/>
       <c r="W50" t="s">
         <v>384</v>
       </c>
@@ -3921,29 +3921,29 @@
       <c r="A51" s="1">
         <v>8</v>
       </c>
-      <c r="B51" s="25" t="s">
+      <c r="B51" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C51" t="s">
         <v>57</v>
       </c>
-      <c r="F51" s="24"/>
+      <c r="F51" s="23"/>
       <c r="G51" t="s">
         <v>253</v>
       </c>
-      <c r="J51" s="25"/>
+      <c r="J51" s="24"/>
       <c r="K51" t="s">
         <v>287</v>
       </c>
-      <c r="N51" s="25"/>
+      <c r="N51" s="24"/>
       <c r="O51" t="s">
         <v>324</v>
       </c>
-      <c r="R51" s="24"/>
+      <c r="R51" s="23"/>
       <c r="S51" t="s">
         <v>354</v>
       </c>
-      <c r="V51" s="24"/>
+      <c r="V51" s="23"/>
       <c r="W51" t="s">
         <v>385</v>
       </c>
@@ -3952,27 +3952,27 @@
       <c r="A52" s="1">
         <v>9</v>
       </c>
-      <c r="B52" s="25"/>
+      <c r="B52" s="24"/>
       <c r="C52" t="s">
         <v>218</v>
       </c>
-      <c r="F52" s="24"/>
+      <c r="F52" s="23"/>
       <c r="G52" t="s">
         <v>254</v>
       </c>
-      <c r="J52" s="25"/>
+      <c r="J52" s="24"/>
       <c r="K52" t="s">
         <v>288</v>
       </c>
-      <c r="N52" s="25"/>
+      <c r="N52" s="24"/>
       <c r="O52" t="s">
         <v>325</v>
       </c>
-      <c r="R52" s="24"/>
+      <c r="R52" s="23"/>
       <c r="S52" t="s">
         <v>355</v>
       </c>
-      <c r="V52" s="25" t="s">
+      <c r="V52" s="24" t="s">
         <v>12</v>
       </c>
       <c r="W52" t="s">
@@ -3983,29 +3983,29 @@
       <c r="A53" s="1">
         <v>10</v>
       </c>
-      <c r="B53" s="25"/>
+      <c r="B53" s="24"/>
       <c r="C53" t="s">
         <v>219</v>
       </c>
-      <c r="F53" s="24"/>
+      <c r="F53" s="23"/>
       <c r="G53" t="s">
         <v>255</v>
       </c>
-      <c r="J53" s="25"/>
+      <c r="J53" s="24"/>
       <c r="K53" t="s">
         <v>289</v>
       </c>
-      <c r="N53" s="25"/>
+      <c r="N53" s="24"/>
       <c r="O53" t="s">
         <v>326</v>
       </c>
-      <c r="R53" s="25" t="s">
+      <c r="R53" s="24" t="s">
         <v>12</v>
       </c>
       <c r="S53" t="s">
         <v>356</v>
       </c>
-      <c r="V53" s="25"/>
+      <c r="V53" s="24"/>
       <c r="W53" t="s">
         <v>387</v>
       </c>
@@ -4014,27 +4014,27 @@
       <c r="A54" s="1">
         <v>11</v>
       </c>
-      <c r="B54" s="25"/>
+      <c r="B54" s="24"/>
       <c r="C54" t="s">
         <v>93</v>
       </c>
-      <c r="F54" s="24"/>
+      <c r="F54" s="23"/>
       <c r="G54" t="s">
         <v>83</v>
       </c>
-      <c r="J54" s="25"/>
+      <c r="J54" s="24"/>
       <c r="K54" t="s">
         <v>290</v>
       </c>
-      <c r="N54" s="25"/>
+      <c r="N54" s="24"/>
       <c r="O54" t="s">
         <v>327</v>
       </c>
-      <c r="R54" s="25"/>
+      <c r="R54" s="24"/>
       <c r="S54" t="s">
         <v>357</v>
       </c>
-      <c r="V54" s="25"/>
+      <c r="V54" s="24"/>
       <c r="W54" t="s">
         <v>388</v>
       </c>
@@ -4043,27 +4043,27 @@
       <c r="A55" s="1">
         <v>12</v>
       </c>
-      <c r="B55" s="25"/>
+      <c r="B55" s="24"/>
       <c r="C55" t="s">
         <v>220</v>
       </c>
-      <c r="F55" s="24"/>
+      <c r="F55" s="23"/>
       <c r="G55" t="s">
         <v>51</v>
       </c>
-      <c r="J55" s="25"/>
+      <c r="J55" s="24"/>
       <c r="K55" t="s">
         <v>291</v>
       </c>
-      <c r="N55" s="25"/>
+      <c r="N55" s="24"/>
       <c r="O55" t="s">
         <v>328</v>
       </c>
-      <c r="R55" s="25"/>
+      <c r="R55" s="24"/>
       <c r="S55" t="s">
         <v>358</v>
       </c>
-      <c r="V55" s="25"/>
+      <c r="V55" s="24"/>
       <c r="W55" t="s">
         <v>389</v>
       </c>
@@ -4072,29 +4072,29 @@
       <c r="A56" s="1">
         <v>13</v>
       </c>
-      <c r="B56" s="25"/>
+      <c r="B56" s="24"/>
       <c r="C56" t="s">
         <v>223</v>
       </c>
-      <c r="F56" s="25" t="s">
+      <c r="F56" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G56" t="s">
         <v>194</v>
       </c>
-      <c r="J56" s="25"/>
+      <c r="J56" s="24"/>
       <c r="K56" t="s">
         <v>292</v>
       </c>
-      <c r="N56" s="25"/>
+      <c r="N56" s="24"/>
       <c r="O56" t="s">
         <v>329</v>
       </c>
-      <c r="R56" s="25"/>
+      <c r="R56" s="24"/>
       <c r="S56" t="s">
         <v>359</v>
       </c>
-      <c r="V56" s="25"/>
+      <c r="V56" s="24"/>
       <c r="W56" t="s">
         <v>390</v>
       </c>
@@ -4103,27 +4103,27 @@
       <c r="A57" s="1">
         <v>14</v>
       </c>
-      <c r="B57" s="25"/>
+      <c r="B57" s="24"/>
       <c r="C57" t="s">
         <v>224</v>
       </c>
-      <c r="F57" s="25"/>
+      <c r="F57" s="24"/>
       <c r="G57" t="s">
         <v>258</v>
       </c>
-      <c r="J57" s="25"/>
+      <c r="J57" s="24"/>
       <c r="K57" t="s">
         <v>293</v>
       </c>
-      <c r="N57" s="25"/>
+      <c r="N57" s="24"/>
       <c r="O57" t="s">
         <v>257</v>
       </c>
-      <c r="R57" s="25"/>
+      <c r="R57" s="24"/>
       <c r="S57" t="s">
         <v>360</v>
       </c>
-      <c r="V57" s="25"/>
+      <c r="V57" s="24"/>
       <c r="W57" t="s">
         <v>391</v>
       </c>
@@ -4132,27 +4132,27 @@
       <c r="A58" s="1">
         <v>15</v>
       </c>
-      <c r="B58" s="25"/>
+      <c r="B58" s="24"/>
       <c r="C58" t="s">
         <v>227</v>
       </c>
-      <c r="F58" s="25"/>
+      <c r="F58" s="24"/>
       <c r="G58" t="s">
         <v>22</v>
       </c>
-      <c r="J58" s="25"/>
+      <c r="J58" s="24"/>
       <c r="K58" t="s">
         <v>294</v>
       </c>
-      <c r="N58" s="25"/>
+      <c r="N58" s="24"/>
       <c r="O58" t="s">
         <v>263</v>
       </c>
-      <c r="R58" s="25"/>
+      <c r="R58" s="24"/>
       <c r="S58" t="s">
         <v>361</v>
       </c>
-      <c r="V58" s="25"/>
+      <c r="V58" s="24"/>
       <c r="W58" t="s">
         <v>392</v>
       </c>
@@ -4161,27 +4161,27 @@
       <c r="A59" s="1">
         <v>16</v>
       </c>
-      <c r="B59" s="25"/>
+      <c r="B59" s="24"/>
       <c r="C59" t="s">
         <v>228</v>
       </c>
-      <c r="F59" s="25"/>
+      <c r="F59" s="24"/>
       <c r="G59" t="s">
         <v>90</v>
       </c>
-      <c r="J59" s="25"/>
+      <c r="J59" s="24"/>
       <c r="K59" t="s">
         <v>295</v>
       </c>
-      <c r="N59" s="25"/>
+      <c r="N59" s="24"/>
       <c r="O59" t="s">
         <v>330</v>
       </c>
-      <c r="R59" s="25"/>
+      <c r="R59" s="24"/>
       <c r="S59" t="s">
         <v>362</v>
       </c>
-      <c r="V59" s="25"/>
+      <c r="V59" s="24"/>
       <c r="W59" t="s">
         <v>393</v>
       </c>
@@ -4190,21 +4190,21 @@
       <c r="A60" s="1">
         <v>17</v>
       </c>
-      <c r="B60" s="25"/>
+      <c r="B60" s="24"/>
       <c r="C60" t="s">
         <v>229</v>
       </c>
-      <c r="F60" s="25"/>
+      <c r="F60" s="24"/>
       <c r="G60" t="s">
         <v>260</v>
       </c>
-      <c r="J60" s="26" t="s">
+      <c r="J60" s="20" t="s">
         <v>18</v>
       </c>
       <c r="K60" t="s">
         <v>296</v>
       </c>
-      <c r="N60" s="26" t="s">
+      <c r="N60" s="20" t="s">
         <v>18</v>
       </c>
       <c r="O60" t="s">
@@ -4216,7 +4216,7 @@
       <c r="S60" t="s">
         <v>363</v>
       </c>
-      <c r="V60" s="26" t="s">
+      <c r="V60" s="20" t="s">
         <v>18</v>
       </c>
       <c r="W60" t="s">
@@ -4227,29 +4227,29 @@
       <c r="A61" s="1">
         <v>18</v>
       </c>
-      <c r="B61" s="25"/>
+      <c r="B61" s="24"/>
       <c r="C61" t="s">
         <v>55</v>
       </c>
-      <c r="F61" s="25"/>
+      <c r="F61" s="24"/>
       <c r="G61" t="s">
         <v>262</v>
       </c>
-      <c r="J61" s="26"/>
+      <c r="J61" s="20"/>
       <c r="K61" t="s">
         <v>297</v>
       </c>
-      <c r="N61" s="26"/>
+      <c r="N61" s="20"/>
       <c r="O61" t="s">
         <v>332</v>
       </c>
-      <c r="R61" s="27" t="s">
+      <c r="R61" s="21" t="s">
         <v>24</v>
       </c>
       <c r="S61" t="s">
         <v>364</v>
       </c>
-      <c r="V61" s="26"/>
+      <c r="V61" s="20"/>
       <c r="W61" t="s">
         <v>395</v>
       </c>
@@ -4258,29 +4258,29 @@
       <c r="A62" s="1">
         <v>19</v>
       </c>
-      <c r="B62" s="26" t="s">
+      <c r="B62" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C62" t="s">
         <v>233</v>
       </c>
-      <c r="F62" s="25"/>
+      <c r="F62" s="24"/>
       <c r="G62" t="s">
         <v>92</v>
       </c>
-      <c r="J62" s="26"/>
+      <c r="J62" s="20"/>
       <c r="K62" t="s">
         <v>298</v>
       </c>
-      <c r="N62" s="26"/>
+      <c r="N62" s="20"/>
       <c r="O62" t="s">
         <v>333</v>
       </c>
-      <c r="R62" s="27"/>
+      <c r="R62" s="21"/>
       <c r="S62" t="s">
         <v>365</v>
       </c>
-      <c r="V62" s="26"/>
+      <c r="V62" s="20"/>
       <c r="W62" t="s">
         <v>396</v>
       </c>
@@ -4289,31 +4289,31 @@
       <c r="A63" s="1">
         <v>20</v>
       </c>
-      <c r="B63" s="26"/>
+      <c r="B63" s="20"/>
       <c r="C63" t="s">
         <v>230</v>
       </c>
-      <c r="F63" s="26" t="s">
+      <c r="F63" s="20" t="s">
         <v>18</v>
       </c>
       <c r="G63" t="s">
         <v>264</v>
       </c>
-      <c r="J63" s="27" t="s">
+      <c r="J63" s="21" t="s">
         <v>24</v>
       </c>
       <c r="K63" t="s">
         <v>299</v>
       </c>
-      <c r="N63" s="26"/>
+      <c r="N63" s="20"/>
       <c r="O63" t="s">
         <v>334</v>
       </c>
-      <c r="R63" s="27"/>
+      <c r="R63" s="21"/>
       <c r="S63" t="s">
         <v>366</v>
       </c>
-      <c r="V63" s="26"/>
+      <c r="V63" s="20"/>
       <c r="W63" t="s">
         <v>397</v>
       </c>
@@ -4322,27 +4322,27 @@
       <c r="A64" s="1">
         <v>21</v>
       </c>
-      <c r="B64" s="26"/>
+      <c r="B64" s="20"/>
       <c r="C64" t="s">
         <v>231</v>
       </c>
-      <c r="F64" s="26"/>
+      <c r="F64" s="20"/>
       <c r="G64" t="s">
         <v>265</v>
       </c>
-      <c r="J64" s="27"/>
+      <c r="J64" s="21"/>
       <c r="K64" t="s">
         <v>300</v>
       </c>
-      <c r="N64" s="26"/>
+      <c r="N64" s="20"/>
       <c r="O64" t="s">
         <v>335</v>
       </c>
-      <c r="R64" s="27"/>
+      <c r="R64" s="21"/>
       <c r="S64" t="s">
         <v>367</v>
       </c>
-      <c r="V64" s="27" t="s">
+      <c r="V64" s="21" t="s">
         <v>24</v>
       </c>
       <c r="W64" t="s">
@@ -4353,29 +4353,29 @@
       <c r="A65" s="1">
         <v>22</v>
       </c>
-      <c r="B65" s="26"/>
+      <c r="B65" s="20"/>
       <c r="C65" t="s">
         <v>232</v>
       </c>
-      <c r="F65" s="26"/>
+      <c r="F65" s="20"/>
       <c r="G65" t="s">
         <v>97</v>
       </c>
-      <c r="J65" s="27"/>
+      <c r="J65" s="21"/>
       <c r="K65" t="s">
         <v>301</v>
       </c>
-      <c r="N65" s="27" t="s">
+      <c r="N65" s="21" t="s">
         <v>24</v>
       </c>
       <c r="O65" t="s">
         <v>336</v>
       </c>
-      <c r="R65" s="27"/>
+      <c r="R65" s="21"/>
       <c r="S65" t="s">
         <v>368</v>
       </c>
-      <c r="V65" s="27"/>
+      <c r="V65" s="21"/>
       <c r="W65" t="s">
         <v>399</v>
       </c>
@@ -4384,29 +4384,29 @@
       <c r="A66" s="1">
         <v>23</v>
       </c>
-      <c r="B66" s="26"/>
+      <c r="B66" s="20"/>
       <c r="C66" t="s">
         <v>61</v>
       </c>
-      <c r="F66" s="26"/>
+      <c r="F66" s="20"/>
       <c r="G66" t="s">
         <v>266</v>
       </c>
-      <c r="J66" s="27"/>
+      <c r="J66" s="21"/>
       <c r="K66" t="s">
         <v>302</v>
       </c>
-      <c r="N66" s="27"/>
+      <c r="N66" s="21"/>
       <c r="O66" t="s">
         <v>337</v>
       </c>
-      <c r="R66" s="20" t="s">
+      <c r="R66" s="26" t="s">
         <v>30</v>
       </c>
       <c r="S66" t="s">
         <v>369</v>
       </c>
-      <c r="V66" s="27"/>
+      <c r="V66" s="21"/>
       <c r="W66" t="s">
         <v>400</v>
       </c>
@@ -4415,29 +4415,29 @@
       <c r="A67" s="1">
         <v>24</v>
       </c>
-      <c r="B67" s="27" t="s">
+      <c r="B67" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C67" t="s">
         <v>102</v>
       </c>
-      <c r="F67" s="26"/>
+      <c r="F67" s="20"/>
       <c r="G67" t="s">
         <v>267</v>
       </c>
-      <c r="J67" s="27"/>
+      <c r="J67" s="21"/>
       <c r="K67" t="s">
         <v>303</v>
       </c>
-      <c r="N67" s="27"/>
+      <c r="N67" s="21"/>
       <c r="O67" t="s">
         <v>338</v>
       </c>
-      <c r="R67" s="20"/>
+      <c r="R67" s="26"/>
       <c r="S67" t="s">
         <v>370</v>
       </c>
-      <c r="V67" s="27"/>
+      <c r="V67" s="21"/>
       <c r="W67" t="s">
         <v>401</v>
       </c>
@@ -4446,29 +4446,29 @@
       <c r="A68" s="1">
         <v>25</v>
       </c>
-      <c r="B68" s="27"/>
+      <c r="B68" s="21"/>
       <c r="C68" t="s">
         <v>234</v>
       </c>
-      <c r="F68" s="27" t="s">
+      <c r="F68" s="21" t="s">
         <v>24</v>
       </c>
       <c r="G68" t="s">
         <v>268</v>
       </c>
-      <c r="J68" s="27"/>
+      <c r="J68" s="21"/>
       <c r="K68" t="s">
         <v>304</v>
       </c>
-      <c r="N68" s="27"/>
+      <c r="N68" s="21"/>
       <c r="O68" t="s">
         <v>342</v>
       </c>
-      <c r="R68" s="20"/>
+      <c r="R68" s="26"/>
       <c r="S68" t="s">
         <v>371</v>
       </c>
-      <c r="V68" s="20" t="s">
+      <c r="V68" s="26" t="s">
         <v>30</v>
       </c>
       <c r="W68" t="s">
@@ -4479,29 +4479,29 @@
       <c r="A69" s="1">
         <v>26</v>
       </c>
-      <c r="B69" s="27"/>
+      <c r="B69" s="21"/>
       <c r="C69" t="s">
         <v>235</v>
       </c>
-      <c r="F69" s="27"/>
+      <c r="F69" s="21"/>
       <c r="G69" t="s">
         <v>269</v>
       </c>
-      <c r="J69" s="27"/>
+      <c r="J69" s="21"/>
       <c r="K69" t="s">
         <v>305</v>
       </c>
-      <c r="N69" s="20" t="s">
+      <c r="N69" s="26" t="s">
         <v>30</v>
       </c>
       <c r="O69" t="s">
         <v>339</v>
       </c>
-      <c r="R69" s="20"/>
+      <c r="R69" s="26"/>
       <c r="S69" t="s">
         <v>372</v>
       </c>
-      <c r="V69" s="20"/>
+      <c r="V69" s="26"/>
       <c r="W69" t="s">
         <v>403</v>
       </c>
@@ -4510,31 +4510,31 @@
       <c r="A70" s="1">
         <v>27</v>
       </c>
-      <c r="B70" s="27"/>
+      <c r="B70" s="21"/>
       <c r="C70" t="s">
         <v>236</v>
       </c>
-      <c r="F70" s="27"/>
+      <c r="F70" s="21"/>
       <c r="G70" t="s">
         <v>270</v>
       </c>
-      <c r="J70" s="20" t="s">
+      <c r="J70" s="26" t="s">
         <v>30</v>
       </c>
       <c r="K70" t="s">
         <v>306</v>
       </c>
-      <c r="N70" s="20"/>
+      <c r="N70" s="26"/>
       <c r="O70" t="s">
         <v>340</v>
       </c>
-      <c r="R70" s="21" t="s">
+      <c r="R70" s="25" t="s">
         <v>36</v>
       </c>
       <c r="S70" t="s">
         <v>373</v>
       </c>
-      <c r="V70" s="20"/>
+      <c r="V70" s="26"/>
       <c r="W70" t="s">
         <v>404</v>
       </c>
@@ -4543,27 +4543,27 @@
       <c r="A71" s="1">
         <v>28</v>
       </c>
-      <c r="B71" s="27"/>
+      <c r="B71" s="21"/>
       <c r="C71" t="s">
         <v>237</v>
       </c>
-      <c r="F71" s="27"/>
+      <c r="F71" s="21"/>
       <c r="G71" t="s">
         <v>101</v>
       </c>
-      <c r="J71" s="20"/>
+      <c r="J71" s="26"/>
       <c r="K71" t="s">
         <v>307</v>
       </c>
-      <c r="N71" s="20"/>
+      <c r="N71" s="26"/>
       <c r="O71" t="s">
         <v>341</v>
       </c>
-      <c r="R71" s="21"/>
+      <c r="R71" s="25"/>
       <c r="S71" t="s">
         <v>374</v>
       </c>
-      <c r="V71" s="20"/>
+      <c r="V71" s="26"/>
       <c r="W71" t="s">
         <v>405</v>
       </c>
@@ -4572,29 +4572,29 @@
       <c r="A72" s="1">
         <v>29</v>
       </c>
-      <c r="B72" s="27"/>
+      <c r="B72" s="21"/>
       <c r="C72" t="s">
         <v>238</v>
       </c>
-      <c r="F72" s="20" t="s">
+      <c r="F72" s="26" t="s">
         <v>30</v>
       </c>
       <c r="G72" t="s">
         <v>271</v>
       </c>
-      <c r="J72" s="20"/>
+      <c r="J72" s="26"/>
       <c r="K72" t="s">
         <v>308</v>
       </c>
-      <c r="N72" s="20"/>
+      <c r="N72" s="26"/>
       <c r="O72" t="s">
         <v>343</v>
       </c>
-      <c r="R72" s="21"/>
+      <c r="R72" s="25"/>
       <c r="S72" t="s">
         <v>375</v>
       </c>
-      <c r="V72" s="20"/>
+      <c r="V72" s="26"/>
       <c r="W72" t="s">
         <v>406</v>
       </c>
@@ -4603,31 +4603,31 @@
       <c r="A73" s="1">
         <v>30</v>
       </c>
-      <c r="B73" s="20" t="s">
+      <c r="B73" s="26" t="s">
         <v>30</v>
       </c>
       <c r="C73" t="s">
         <v>34</v>
       </c>
-      <c r="F73" s="20"/>
+      <c r="F73" s="26"/>
       <c r="G73" t="s">
         <v>272</v>
       </c>
-      <c r="J73" s="20"/>
+      <c r="J73" s="26"/>
       <c r="K73" t="s">
         <v>309</v>
       </c>
-      <c r="N73" s="21" t="s">
+      <c r="N73" s="25" t="s">
         <v>36</v>
       </c>
       <c r="O73" t="s">
         <v>344</v>
       </c>
-      <c r="R73" s="21"/>
+      <c r="R73" s="25"/>
       <c r="S73" t="s">
         <v>376</v>
       </c>
-      <c r="V73" s="21" t="s">
+      <c r="V73" s="25" t="s">
         <v>36</v>
       </c>
       <c r="W73" t="s">
@@ -4635,144 +4635,171 @@
       </c>
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B74" s="20"/>
+      <c r="B74" s="26"/>
       <c r="C74" t="s">
         <v>239</v>
       </c>
-      <c r="F74" s="20"/>
+      <c r="F74" s="26"/>
       <c r="G74" t="s">
         <v>273</v>
       </c>
-      <c r="J74" s="21" t="s">
+      <c r="J74" s="25" t="s">
         <v>36</v>
       </c>
       <c r="K74" t="s">
         <v>310</v>
       </c>
-      <c r="N74" s="21"/>
+      <c r="N74" s="25"/>
       <c r="O74" t="s">
         <v>345</v>
       </c>
-      <c r="R74" s="21"/>
+      <c r="R74" s="25"/>
       <c r="S74" t="s">
         <v>377</v>
       </c>
-      <c r="V74" s="21"/>
+      <c r="V74" s="25"/>
       <c r="W74" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B75" s="20"/>
+      <c r="B75" s="26"/>
       <c r="C75" t="s">
         <v>240</v>
       </c>
-      <c r="F75" s="20"/>
+      <c r="F75" s="26"/>
       <c r="G75" t="s">
         <v>274</v>
       </c>
-      <c r="J75" s="21"/>
+      <c r="J75" s="25"/>
       <c r="K75" t="s">
         <v>311</v>
       </c>
-      <c r="N75" s="21"/>
+      <c r="N75" s="25"/>
       <c r="O75" t="s">
         <v>346</v>
       </c>
-      <c r="V75" s="21"/>
+      <c r="V75" s="25"/>
       <c r="W75" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B76" s="20"/>
+      <c r="B76" s="26"/>
       <c r="C76" t="s">
         <v>241</v>
       </c>
-      <c r="F76" s="21" t="s">
+      <c r="F76" s="25" t="s">
         <v>36</v>
       </c>
       <c r="G76" t="s">
         <v>276</v>
       </c>
-      <c r="J76" s="21"/>
+      <c r="J76" s="25"/>
       <c r="K76" t="s">
         <v>312</v>
       </c>
-      <c r="N76" s="21"/>
+      <c r="N76" s="25"/>
       <c r="O76" t="s">
         <v>347</v>
       </c>
-      <c r="V76" s="21"/>
+      <c r="V76" s="25"/>
       <c r="W76" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="77" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B77" s="21" t="s">
+      <c r="B77" s="25" t="s">
         <v>36</v>
       </c>
       <c r="C77" t="s">
         <v>109</v>
       </c>
-      <c r="F77" s="21"/>
+      <c r="F77" s="25"/>
       <c r="G77" t="s">
         <v>277</v>
       </c>
-      <c r="J77" s="21"/>
+      <c r="J77" s="25"/>
       <c r="K77" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B78" s="21"/>
+      <c r="B78" s="25"/>
       <c r="C78" t="s">
         <v>242</v>
       </c>
-      <c r="F78" s="21"/>
+      <c r="F78" s="25"/>
       <c r="G78" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B79" s="21"/>
+      <c r="B79" s="25"/>
       <c r="C79" t="s">
         <v>243</v>
       </c>
-      <c r="F79" s="21"/>
+      <c r="F79" s="25"/>
       <c r="G79" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B80" s="21"/>
+      <c r="B80" s="25"/>
       <c r="C80" t="s">
         <v>244</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="V25:V27"/>
-    <mergeCell ref="V28:V31"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="R4:R9"/>
-    <mergeCell ref="R10:R19"/>
-    <mergeCell ref="V2:V5"/>
-    <mergeCell ref="V6:V13"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="N4:N10"/>
-    <mergeCell ref="N11:N16"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="V14:V24"/>
-    <mergeCell ref="F63:F67"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="F10:F15"/>
-    <mergeCell ref="J20:J22"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="J4:J9"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="J10:J16"/>
+    <mergeCell ref="V68:V72"/>
+    <mergeCell ref="V73:V76"/>
+    <mergeCell ref="R66:R69"/>
+    <mergeCell ref="R70:R74"/>
+    <mergeCell ref="R31:R34"/>
+    <mergeCell ref="V43:Y43"/>
+    <mergeCell ref="V44:V46"/>
+    <mergeCell ref="V47:V51"/>
+    <mergeCell ref="V52:V59"/>
+    <mergeCell ref="V60:V63"/>
+    <mergeCell ref="V64:V67"/>
+    <mergeCell ref="V37:V40"/>
+    <mergeCell ref="R61:R65"/>
+    <mergeCell ref="V32:V36"/>
+    <mergeCell ref="R48:R52"/>
+    <mergeCell ref="R53:R59"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="R44:R47"/>
+    <mergeCell ref="J27:J30"/>
+    <mergeCell ref="N24:N29"/>
+    <mergeCell ref="N30:N33"/>
+    <mergeCell ref="R26:R30"/>
+    <mergeCell ref="J44:J46"/>
+    <mergeCell ref="J47:J49"/>
+    <mergeCell ref="J23:J26"/>
+    <mergeCell ref="R22:R25"/>
+    <mergeCell ref="N19:N23"/>
+    <mergeCell ref="R20:R21"/>
+    <mergeCell ref="F72:F75"/>
+    <mergeCell ref="F68:F71"/>
+    <mergeCell ref="B67:B72"/>
+    <mergeCell ref="B73:B76"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="F56:F62"/>
+    <mergeCell ref="B51:B61"/>
+    <mergeCell ref="F47:F55"/>
+    <mergeCell ref="F27:F31"/>
     <mergeCell ref="B77:B80"/>
     <mergeCell ref="F76:F79"/>
     <mergeCell ref="J70:J73"/>
@@ -4789,54 +4816,27 @@
     <mergeCell ref="J63:J69"/>
     <mergeCell ref="B44:B46"/>
     <mergeCell ref="B62:B66"/>
-    <mergeCell ref="F72:F75"/>
-    <mergeCell ref="F68:F71"/>
-    <mergeCell ref="B67:B72"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="F56:F62"/>
-    <mergeCell ref="B51:B61"/>
-    <mergeCell ref="F47:F55"/>
-    <mergeCell ref="F27:F31"/>
-    <mergeCell ref="R44:R47"/>
-    <mergeCell ref="J27:J30"/>
-    <mergeCell ref="N24:N29"/>
-    <mergeCell ref="N30:N33"/>
-    <mergeCell ref="R26:R30"/>
-    <mergeCell ref="J44:J46"/>
-    <mergeCell ref="J47:J49"/>
-    <mergeCell ref="J23:J26"/>
-    <mergeCell ref="R22:R25"/>
-    <mergeCell ref="N19:N23"/>
-    <mergeCell ref="R20:R21"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="V68:V72"/>
-    <mergeCell ref="V73:V76"/>
-    <mergeCell ref="R66:R69"/>
-    <mergeCell ref="R70:R74"/>
-    <mergeCell ref="R31:R34"/>
-    <mergeCell ref="V43:Y43"/>
-    <mergeCell ref="V44:V46"/>
-    <mergeCell ref="V47:V51"/>
-    <mergeCell ref="V52:V59"/>
-    <mergeCell ref="V60:V63"/>
-    <mergeCell ref="V64:V67"/>
-    <mergeCell ref="V37:V40"/>
-    <mergeCell ref="R61:R65"/>
-    <mergeCell ref="V32:V36"/>
-    <mergeCell ref="R48:R52"/>
-    <mergeCell ref="R53:R59"/>
+    <mergeCell ref="F63:F67"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="F10:F15"/>
+    <mergeCell ref="J20:J22"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="J4:J9"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="J10:J16"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="N4:N10"/>
+    <mergeCell ref="N11:N16"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="V14:V24"/>
+    <mergeCell ref="V25:V27"/>
+    <mergeCell ref="V28:V31"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="R4:R9"/>
+    <mergeCell ref="R10:R19"/>
+    <mergeCell ref="V2:V5"/>
+    <mergeCell ref="V6:V13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4846,8 +4846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4868,36 +4868,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="E1" s="22" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="E1" s="28" t="s">
         <v>412</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
       <c r="J1" t="s">
         <v>411</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="O1" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="T1" s="22" t="s">
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="T1" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="X1" s="22" t="s">
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="X1" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -4910,7 +4910,7 @@
         <v>555</v>
       </c>
       <c r="F2" t="s">
-        <v>508</v>
+        <v>492</v>
       </c>
       <c r="J2" t="s">
         <v>413</v>
@@ -4945,13 +4945,13 @@
         <v>414</v>
       </c>
       <c r="F3" t="s">
-        <v>538</v>
+        <v>487</v>
       </c>
       <c r="J3" t="s">
         <v>596</v>
       </c>
       <c r="K3" t="s">
-        <v>492</v>
+        <v>537</v>
       </c>
       <c r="O3" t="s">
         <v>641</v>
@@ -4973,6 +4973,9 @@
       <c r="A4" t="s">
         <v>556</v>
       </c>
+      <c r="B4" t="s">
+        <v>489</v>
+      </c>
       <c r="E4" t="s">
         <v>591</v>
       </c>
@@ -4983,7 +4986,7 @@
         <v>611</v>
       </c>
       <c r="K4" t="s">
-        <v>537</v>
+        <v>508</v>
       </c>
       <c r="O4" t="s">
         <v>642</v>
@@ -5005,6 +5008,9 @@
       <c r="A5" t="s">
         <v>592</v>
       </c>
+      <c r="B5" t="s">
+        <v>490</v>
+      </c>
       <c r="E5" t="s">
         <v>621</v>
       </c>
@@ -5015,7 +5021,7 @@
         <v>568</v>
       </c>
       <c r="K5" t="s">
-        <v>487</v>
+        <v>538</v>
       </c>
       <c r="O5" t="s">
         <v>643</v>
@@ -5037,18 +5043,12 @@
       <c r="A6" t="s">
         <v>573</v>
       </c>
-      <c r="B6" t="s">
-        <v>489</v>
-      </c>
       <c r="E6" t="s">
         <v>606</v>
       </c>
       <c r="K6" t="s">
         <v>503</v>
       </c>
-      <c r="L6" t="s">
-        <v>498</v>
-      </c>
       <c r="P6" t="s">
         <v>521</v>
       </c>
@@ -5063,17 +5063,11 @@
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>490</v>
-      </c>
       <c r="E7" t="s">
         <v>622</v>
       </c>
       <c r="K7" t="s">
         <v>528</v>
-      </c>
-      <c r="L7" t="s">
-        <v>488</v>
       </c>
       <c r="T7" t="s">
         <v>616</v>
@@ -5091,42 +5085,50 @@
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="K9" t="s">
+        <v>498</v>
+      </c>
       <c r="T9" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="K10" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="K11" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
       <c r="E17" t="s">
         <v>420</v>
       </c>
-      <c r="I17" s="22" t="s">
+      <c r="I17" s="28" t="s">
         <v>421</v>
       </c>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="N17" s="22" t="s">
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="N17" s="28" t="s">
         <v>314</v>
       </c>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="S17" s="22" t="s">
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
+      <c r="S17" s="28" t="s">
         <v>315</v>
       </c>
-      <c r="T17" s="22"/>
-      <c r="U17" s="22"/>
-      <c r="V17" s="22"/>
+      <c r="T17" s="28"/>
+      <c r="U17" s="28"/>
+      <c r="V17" s="28"/>
       <c r="X17" t="s">
         <v>316</v>
       </c>
@@ -5661,7 +5663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A138" workbookViewId="0">
       <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
did save on last commit
</commit_message>
<xml_diff>
--- a/OffSeason.xlsx
+++ b/OffSeason.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="724">
   <si>
     <t>Chubber for Chubb - John Olson</t>
   </si>
@@ -1319,9 +1319,6 @@
     <t>2020 4th Snow Happens</t>
   </si>
   <si>
-    <t>start 4th own</t>
-  </si>
-  <si>
     <t>2020 3rd Snow Happens</t>
   </si>
   <si>
@@ -2187,6 +2184,21 @@
   </si>
   <si>
     <t>Cam sends</t>
+  </si>
+  <si>
+    <t>Alan sends</t>
+  </si>
+  <si>
+    <t>Andrew Sends</t>
+  </si>
+  <si>
+    <t>2020 4th (andrew)</t>
+  </si>
+  <si>
+    <t>2020 4th Slick Daddy Club</t>
+  </si>
+  <si>
+    <t>2020 5th Slick Daddy Club</t>
   </si>
 </sst>
 </file>
@@ -2427,19 +2439,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2449,10 +2461,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2737,8 +2749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" topLeftCell="G15" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2754,11 +2766,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="F1" t="s">
         <v>42</v>
       </c>
@@ -2779,37 +2791,37 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="K2" t="s">
         <v>77</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="O2" t="s">
         <v>112</v>
       </c>
-      <c r="R2" s="24" t="s">
+      <c r="R2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="S2" t="s">
         <v>144</v>
       </c>
-      <c r="V2" s="24" t="s">
+      <c r="V2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="W2" t="s">
@@ -2820,27 +2832,27 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="24"/>
+      <c r="B3" s="23"/>
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="24"/>
+      <c r="F3" s="23"/>
       <c r="G3" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="24"/>
+      <c r="J3" s="23"/>
       <c r="K3" t="s">
         <v>214</v>
       </c>
-      <c r="N3" s="24"/>
+      <c r="N3" s="23"/>
       <c r="O3" t="s">
         <v>104</v>
       </c>
-      <c r="R3" s="24"/>
+      <c r="R3" s="23"/>
       <c r="S3" t="s">
         <v>145</v>
       </c>
-      <c r="V3" s="24"/>
+      <c r="V3" s="23"/>
       <c r="W3" t="s">
         <v>180</v>
       </c>
@@ -2849,33 +2861,33 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="24"/>
+      <c r="B4" s="23"/>
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="24"/>
+      <c r="F4" s="23"/>
       <c r="G4" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="24" t="s">
         <v>5</v>
       </c>
       <c r="K4" t="s">
         <v>248</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="24" t="s">
         <v>5</v>
       </c>
       <c r="O4" t="s">
         <v>113</v>
       </c>
-      <c r="R4" s="21" t="s">
+      <c r="R4" s="24" t="s">
         <v>5</v>
       </c>
       <c r="S4" t="s">
         <v>146</v>
       </c>
-      <c r="V4" s="24"/>
+      <c r="V4" s="23"/>
       <c r="W4" t="s">
         <v>181</v>
       </c>
@@ -2884,29 +2896,29 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="24"/>
+      <c r="F5" s="23"/>
       <c r="G5" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="24"/>
       <c r="K5" t="s">
         <v>81</v>
       </c>
-      <c r="N5" s="21"/>
+      <c r="N5" s="24"/>
       <c r="O5" t="s">
         <v>114</v>
       </c>
-      <c r="R5" s="21"/>
+      <c r="R5" s="24"/>
       <c r="S5" t="s">
         <v>147</v>
       </c>
-      <c r="V5" s="21" t="s">
+      <c r="V5" s="24" t="s">
         <v>5</v>
       </c>
       <c r="W5" t="s">
@@ -2917,29 +2929,29 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="21"/>
+      <c r="B6" s="24"/>
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="24" t="s">
         <v>5</v>
       </c>
       <c r="G6" t="s">
         <v>215</v>
       </c>
-      <c r="J6" s="21"/>
+      <c r="J6" s="24"/>
       <c r="K6" t="s">
         <v>82</v>
       </c>
-      <c r="N6" s="21"/>
+      <c r="N6" s="24"/>
       <c r="O6" t="s">
         <v>115</v>
       </c>
-      <c r="R6" s="21"/>
+      <c r="R6" s="24"/>
       <c r="S6" t="s">
         <v>148</v>
       </c>
-      <c r="V6" s="21"/>
+      <c r="V6" s="24"/>
       <c r="W6" t="s">
         <v>250</v>
       </c>
@@ -2948,27 +2960,27 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="21"/>
+      <c r="B7" s="24"/>
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="24"/>
       <c r="G7" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="21"/>
+      <c r="J7" s="24"/>
       <c r="K7" t="s">
         <v>352</v>
       </c>
-      <c r="N7" s="21"/>
+      <c r="N7" s="24"/>
       <c r="O7" t="s">
         <v>116</v>
       </c>
-      <c r="R7" s="21"/>
+      <c r="R7" s="24"/>
       <c r="S7" t="s">
         <v>149</v>
       </c>
-      <c r="V7" s="21"/>
+      <c r="V7" s="24"/>
       <c r="W7" t="s">
         <v>184</v>
       </c>
@@ -2977,27 +2989,27 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="21"/>
+      <c r="B8" s="24"/>
       <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="24"/>
       <c r="G8" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="21"/>
+      <c r="J8" s="24"/>
       <c r="K8" t="s">
         <v>85</v>
       </c>
-      <c r="N8" s="21"/>
+      <c r="N8" s="24"/>
       <c r="O8" t="s">
         <v>117</v>
       </c>
-      <c r="R8" s="21"/>
+      <c r="R8" s="24"/>
       <c r="S8" t="s">
         <v>150</v>
       </c>
-      <c r="V8" s="21"/>
+      <c r="V8" s="24"/>
       <c r="W8" t="s">
         <v>252</v>
       </c>
@@ -3006,62 +3018,62 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="21"/>
+      <c r="B9" s="24"/>
       <c r="C9" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="24"/>
       <c r="G9" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="22" t="s">
+      <c r="J9" s="25" t="s">
         <v>12</v>
       </c>
       <c r="K9" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="21"/>
+      <c r="N9" s="24"/>
       <c r="O9" t="s">
         <v>118</v>
       </c>
-      <c r="R9" s="21"/>
+      <c r="R9" s="24"/>
       <c r="S9" t="s">
         <v>151</v>
       </c>
-      <c r="V9" s="21"/>
+      <c r="V9" s="24"/>
       <c r="W9" t="s">
-        <v>186</v>
+        <v>385</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="21"/>
+      <c r="B10" s="24"/>
       <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="25" t="s">
         <v>12</v>
       </c>
       <c r="G10" t="s">
         <v>54</v>
       </c>
-      <c r="J10" s="22"/>
+      <c r="J10" s="25"/>
       <c r="K10" t="s">
         <v>188</v>
       </c>
-      <c r="N10" s="21"/>
+      <c r="N10" s="24"/>
       <c r="O10" t="s">
         <v>119</v>
       </c>
-      <c r="R10" s="22" t="s">
+      <c r="R10" s="25" t="s">
         <v>12</v>
       </c>
       <c r="S10" t="s">
         <v>152</v>
       </c>
-      <c r="V10" s="21"/>
+      <c r="V10" s="24"/>
       <c r="W10" t="s">
         <v>187</v>
       </c>
@@ -3070,31 +3082,31 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="22"/>
+      <c r="F11" s="25"/>
       <c r="G11" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="22"/>
+      <c r="J11" s="25"/>
       <c r="K11" t="s">
         <v>17</v>
       </c>
-      <c r="N11" s="22" t="s">
+      <c r="N11" s="25" t="s">
         <v>12</v>
       </c>
       <c r="O11" t="s">
         <v>120</v>
       </c>
-      <c r="R11" s="22"/>
+      <c r="R11" s="25"/>
       <c r="S11" t="s">
         <v>153</v>
       </c>
-      <c r="V11" s="21"/>
+      <c r="V11" s="24"/>
       <c r="W11" t="s">
         <v>53</v>
       </c>
@@ -3103,27 +3115,27 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="22"/>
+      <c r="B12" s="25"/>
       <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="22"/>
+      <c r="F12" s="25"/>
       <c r="G12" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="22"/>
+      <c r="J12" s="25"/>
       <c r="K12" t="s">
         <v>88</v>
       </c>
-      <c r="N12" s="22"/>
+      <c r="N12" s="25"/>
       <c r="O12" t="s">
         <v>121</v>
       </c>
-      <c r="R12" s="22"/>
+      <c r="R12" s="25"/>
       <c r="S12" t="s">
         <v>154</v>
       </c>
-      <c r="V12" s="21"/>
+      <c r="V12" s="24"/>
       <c r="W12" t="s">
         <v>10</v>
       </c>
@@ -3132,27 +3144,27 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="22"/>
+      <c r="B13" s="25"/>
       <c r="C13" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="22"/>
+      <c r="F13" s="25"/>
       <c r="G13" t="s">
         <v>59</v>
       </c>
-      <c r="J13" s="22"/>
+      <c r="J13" s="25"/>
       <c r="K13" t="s">
         <v>16</v>
       </c>
-      <c r="N13" s="22"/>
+      <c r="N13" s="25"/>
       <c r="O13" t="s">
         <v>122</v>
       </c>
-      <c r="R13" s="22"/>
+      <c r="R13" s="25"/>
       <c r="S13" t="s">
         <v>155</v>
       </c>
-      <c r="V13" s="22" t="s">
+      <c r="V13" s="25" t="s">
         <v>12</v>
       </c>
       <c r="W13" t="s">
@@ -3163,27 +3175,27 @@
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="22"/>
+      <c r="B14" s="25"/>
       <c r="C14" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="22"/>
+      <c r="F14" s="25"/>
       <c r="G14" t="s">
         <v>226</v>
       </c>
-      <c r="J14" s="22"/>
+      <c r="J14" s="25"/>
       <c r="K14" t="s">
         <v>22</v>
       </c>
-      <c r="N14" s="22"/>
+      <c r="N14" s="25"/>
       <c r="O14" t="s">
         <v>123</v>
       </c>
-      <c r="R14" s="22"/>
+      <c r="R14" s="25"/>
       <c r="S14" t="s">
         <v>156</v>
       </c>
-      <c r="V14" s="22"/>
+      <c r="V14" s="25"/>
       <c r="W14" t="s">
         <v>189</v>
       </c>
@@ -3192,27 +3204,27 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="22"/>
+      <c r="B15" s="25"/>
       <c r="C15" t="s">
         <v>87</v>
       </c>
-      <c r="F15" s="22"/>
+      <c r="F15" s="25"/>
       <c r="G15" t="s">
         <v>225</v>
       </c>
-      <c r="J15" s="22"/>
+      <c r="J15" s="25"/>
       <c r="K15" t="s">
         <v>194</v>
       </c>
-      <c r="N15" s="22"/>
+      <c r="N15" s="25"/>
       <c r="O15" t="s">
         <v>124</v>
       </c>
-      <c r="R15" s="22"/>
+      <c r="R15" s="25"/>
       <c r="S15" t="s">
         <v>157</v>
       </c>
-      <c r="V15" s="22"/>
+      <c r="V15" s="25"/>
       <c r="W15" t="s">
         <v>190</v>
       </c>
@@ -3221,31 +3233,31 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="21" t="s">
         <v>18</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F16" s="21" t="s">
         <v>18</v>
       </c>
       <c r="G16" t="s">
         <v>60</v>
       </c>
-      <c r="J16" s="22"/>
+      <c r="J16" s="25"/>
       <c r="K16" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="22"/>
+      <c r="N16" s="25"/>
       <c r="O16" t="s">
         <v>125</v>
       </c>
-      <c r="R16" s="22"/>
+      <c r="R16" s="25"/>
       <c r="S16" t="s">
         <v>158</v>
       </c>
-      <c r="V16" s="22"/>
+      <c r="V16" s="25"/>
       <c r="W16" t="s">
         <v>191</v>
       </c>
@@ -3254,31 +3266,31 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="23"/>
+      <c r="B17" s="21"/>
       <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="23"/>
+      <c r="F17" s="21"/>
       <c r="G17" t="s">
         <v>62</v>
       </c>
-      <c r="J17" s="23" t="s">
+      <c r="J17" s="21" t="s">
         <v>18</v>
       </c>
       <c r="K17" t="s">
         <v>95</v>
       </c>
-      <c r="N17" s="23" t="s">
+      <c r="N17" s="21" t="s">
         <v>18</v>
       </c>
       <c r="O17" t="s">
         <v>126</v>
       </c>
-      <c r="R17" s="22"/>
+      <c r="R17" s="25"/>
       <c r="S17" t="s">
         <v>159</v>
       </c>
-      <c r="V17" s="22"/>
+      <c r="V17" s="25"/>
       <c r="W17" t="s">
         <v>91</v>
       </c>
@@ -3287,27 +3299,27 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="23"/>
+      <c r="B18" s="21"/>
       <c r="C18" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="23"/>
+      <c r="F18" s="21"/>
       <c r="G18" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="23"/>
+      <c r="J18" s="21"/>
       <c r="K18" t="s">
         <v>98</v>
       </c>
-      <c r="N18" s="23"/>
+      <c r="N18" s="21"/>
       <c r="O18" t="s">
         <v>127</v>
       </c>
-      <c r="R18" s="22"/>
+      <c r="R18" s="25"/>
       <c r="S18" t="s">
         <v>160</v>
       </c>
-      <c r="V18" s="22"/>
+      <c r="V18" s="25"/>
       <c r="W18" t="s">
         <v>261</v>
       </c>
@@ -3316,33 +3328,33 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="22" t="s">
         <v>24</v>
       </c>
       <c r="G19" t="s">
         <v>64</v>
       </c>
-      <c r="J19" s="23"/>
+      <c r="J19" s="21"/>
       <c r="K19" t="s">
         <v>333</v>
       </c>
-      <c r="N19" s="25" t="s">
+      <c r="N19" s="22" t="s">
         <v>24</v>
       </c>
       <c r="O19" t="s">
         <v>128</v>
       </c>
-      <c r="R19" s="22"/>
+      <c r="R19" s="25"/>
       <c r="S19" t="s">
         <v>161</v>
       </c>
-      <c r="V19" s="22"/>
+      <c r="V19" s="25"/>
       <c r="W19" t="s">
         <v>94</v>
       </c>
@@ -3351,31 +3363,31 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="25"/>
+      <c r="B20" s="22"/>
       <c r="C20" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="25"/>
+      <c r="F20" s="22"/>
       <c r="G20" t="s">
         <v>65</v>
       </c>
-      <c r="J20" s="25" t="s">
+      <c r="J20" s="22" t="s">
         <v>24</v>
       </c>
       <c r="K20" t="s">
         <v>99</v>
       </c>
-      <c r="N20" s="25"/>
+      <c r="N20" s="22"/>
       <c r="O20" t="s">
         <v>129</v>
       </c>
-      <c r="R20" s="23" t="s">
+      <c r="R20" s="21" t="s">
         <v>18</v>
       </c>
       <c r="S20" t="s">
         <v>162</v>
       </c>
-      <c r="V20" s="22"/>
+      <c r="V20" s="25"/>
       <c r="W20" t="s">
         <v>193</v>
       </c>
@@ -3384,27 +3396,27 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="25"/>
+      <c r="B21" s="22"/>
       <c r="C21" t="s">
         <v>100</v>
       </c>
-      <c r="F21" s="25"/>
+      <c r="F21" s="22"/>
       <c r="G21" t="s">
         <v>66</v>
       </c>
-      <c r="J21" s="25"/>
+      <c r="J21" s="22"/>
       <c r="K21" t="s">
         <v>28</v>
       </c>
-      <c r="N21" s="25"/>
+      <c r="N21" s="22"/>
       <c r="O21" t="s">
         <v>130</v>
       </c>
-      <c r="R21" s="23"/>
+      <c r="R21" s="21"/>
       <c r="S21" t="s">
         <v>163</v>
       </c>
-      <c r="V21" s="22"/>
+      <c r="V21" s="25"/>
       <c r="W21" t="s">
         <v>195</v>
       </c>
@@ -3419,25 +3431,25 @@
       <c r="C22" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="25"/>
+      <c r="F22" s="22"/>
       <c r="G22" t="s">
         <v>67</v>
       </c>
-      <c r="J22" s="25"/>
+      <c r="J22" s="22"/>
       <c r="K22" t="s">
         <v>29</v>
       </c>
-      <c r="N22" s="25"/>
+      <c r="N22" s="22"/>
       <c r="O22" t="s">
         <v>131</v>
       </c>
-      <c r="R22" s="25" t="s">
+      <c r="R22" s="22" t="s">
         <v>24</v>
       </c>
       <c r="S22" t="s">
         <v>164</v>
       </c>
-      <c r="V22" s="22"/>
+      <c r="V22" s="25"/>
       <c r="W22" t="s">
         <v>196</v>
       </c>
@@ -3456,19 +3468,19 @@
       <c r="G23" t="s">
         <v>69</v>
       </c>
-      <c r="J23" s="25"/>
+      <c r="J23" s="22"/>
       <c r="K23" t="s">
         <v>27</v>
       </c>
-      <c r="N23" s="25"/>
+      <c r="N23" s="22"/>
       <c r="O23" t="s">
         <v>132</v>
       </c>
-      <c r="R23" s="25"/>
+      <c r="R23" s="22"/>
       <c r="S23" t="s">
         <v>165</v>
       </c>
-      <c r="V23" s="23" t="s">
+      <c r="V23" s="21" t="s">
         <v>18</v>
       </c>
       <c r="W23" t="s">
@@ -3499,11 +3511,11 @@
       <c r="O24" t="s">
         <v>133</v>
       </c>
-      <c r="R24" s="25"/>
+      <c r="R24" s="22"/>
       <c r="S24" t="s">
         <v>166</v>
       </c>
-      <c r="V24" s="23"/>
+      <c r="V24" s="21"/>
       <c r="W24" t="s">
         <v>198</v>
       </c>
@@ -3530,11 +3542,11 @@
       <c r="O25" t="s">
         <v>134</v>
       </c>
-      <c r="R25" s="25"/>
+      <c r="R25" s="22"/>
       <c r="S25" t="s">
         <v>167</v>
       </c>
-      <c r="V25" s="23"/>
+      <c r="V25" s="21"/>
       <c r="W25" t="s">
         <v>199</v>
       </c>
@@ -3565,7 +3577,7 @@
       <c r="S26" t="s">
         <v>168</v>
       </c>
-      <c r="V26" s="25" t="s">
+      <c r="V26" s="22" t="s">
         <v>24</v>
       </c>
       <c r="W26" t="s">
@@ -3598,7 +3610,7 @@
       <c r="S27" t="s">
         <v>169</v>
       </c>
-      <c r="V27" s="25"/>
+      <c r="V27" s="22"/>
       <c r="W27" t="s">
         <v>201</v>
       </c>
@@ -3629,7 +3641,7 @@
       <c r="S28" t="s">
         <v>170</v>
       </c>
-      <c r="V28" s="25"/>
+      <c r="V28" s="22"/>
       <c r="W28" t="s">
         <v>202</v>
       </c>
@@ -3654,7 +3666,7 @@
       <c r="S29" t="s">
         <v>171</v>
       </c>
-      <c r="V29" s="25"/>
+      <c r="V29" s="22"/>
       <c r="W29" t="s">
         <v>203</v>
       </c>
@@ -3764,18 +3776,12 @@
     <row r="36" spans="1:25" x14ac:dyDescent="0.35">
       <c r="V36" s="27"/>
       <c r="W36" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.35">
       <c r="V37" s="27"/>
       <c r="W37" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V38" s="27"/>
-      <c r="W38" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3787,7 +3793,7 @@
         <v>245</v>
       </c>
       <c r="J43" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N43" t="s">
         <v>314</v>
@@ -3795,48 +3801,48 @@
       <c r="R43" t="s">
         <v>315</v>
       </c>
-      <c r="V43" s="28" t="s">
+      <c r="V43" s="29" t="s">
         <v>316</v>
       </c>
-      <c r="W43" s="28"/>
-      <c r="X43" s="28"/>
-      <c r="Y43" s="28"/>
+      <c r="W43" s="29"/>
+      <c r="X43" s="29"/>
+      <c r="Y43" s="29"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>1</v>
       </c>
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="23" t="s">
         <v>1</v>
       </c>
       <c r="C44" t="s">
         <v>44</v>
       </c>
-      <c r="F44" s="24" t="s">
+      <c r="F44" s="23" t="s">
         <v>1</v>
       </c>
       <c r="G44" t="s">
         <v>246</v>
       </c>
-      <c r="J44" s="24" t="s">
+      <c r="J44" s="23" t="s">
         <v>1</v>
       </c>
       <c r="K44" t="s">
         <v>280</v>
       </c>
-      <c r="N44" s="24" t="s">
+      <c r="N44" s="23" t="s">
         <v>1</v>
       </c>
       <c r="O44" t="s">
         <v>317</v>
       </c>
-      <c r="R44" s="24" t="s">
+      <c r="R44" s="23" t="s">
         <v>1</v>
       </c>
       <c r="S44" t="s">
         <v>348</v>
       </c>
-      <c r="V44" s="24" t="s">
+      <c r="V44" s="23" t="s">
         <v>1</v>
       </c>
       <c r="W44" t="s">
@@ -3847,27 +3853,27 @@
       <c r="A45" s="1">
         <v>2</v>
       </c>
-      <c r="B45" s="24"/>
+      <c r="B45" s="23"/>
       <c r="C45" t="s">
         <v>179</v>
       </c>
-      <c r="F45" s="24"/>
+      <c r="F45" s="23"/>
       <c r="G45" t="s">
         <v>247</v>
       </c>
-      <c r="J45" s="24"/>
+      <c r="J45" s="23"/>
       <c r="K45" t="s">
         <v>281</v>
       </c>
-      <c r="N45" s="24"/>
+      <c r="N45" s="23"/>
       <c r="O45" t="s">
         <v>318</v>
       </c>
-      <c r="R45" s="24"/>
+      <c r="R45" s="23"/>
       <c r="S45" t="s">
         <v>349</v>
       </c>
-      <c r="V45" s="24"/>
+      <c r="V45" s="23"/>
       <c r="W45" t="s">
         <v>379</v>
       </c>
@@ -3876,27 +3882,27 @@
       <c r="A46" s="1">
         <v>3</v>
       </c>
-      <c r="B46" s="24"/>
+      <c r="B46" s="23"/>
       <c r="C46" t="s">
         <v>213</v>
       </c>
-      <c r="F46" s="24"/>
+      <c r="F46" s="23"/>
       <c r="G46" t="s">
         <v>79</v>
       </c>
-      <c r="J46" s="24"/>
+      <c r="J46" s="23"/>
       <c r="K46" t="s">
         <v>282</v>
       </c>
-      <c r="N46" s="24"/>
+      <c r="N46" s="23"/>
       <c r="O46" t="s">
         <v>319</v>
       </c>
-      <c r="R46" s="24"/>
+      <c r="R46" s="23"/>
       <c r="S46" t="s">
         <v>78</v>
       </c>
-      <c r="V46" s="24"/>
+      <c r="V46" s="23"/>
       <c r="W46" t="s">
         <v>380</v>
       </c>
@@ -3905,35 +3911,35 @@
       <c r="A47" s="1">
         <v>4</v>
       </c>
-      <c r="B47" s="21" t="s">
+      <c r="B47" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C47" t="s">
         <v>216</v>
       </c>
-      <c r="F47" s="21" t="s">
+      <c r="F47" s="24" t="s">
         <v>5</v>
       </c>
       <c r="G47" t="s">
         <v>183</v>
       </c>
-      <c r="J47" s="21" t="s">
+      <c r="J47" s="24" t="s">
         <v>5</v>
       </c>
       <c r="K47" t="s">
         <v>283</v>
       </c>
-      <c r="N47" s="21" t="s">
+      <c r="N47" s="24" t="s">
         <v>5</v>
       </c>
       <c r="O47" t="s">
         <v>320</v>
       </c>
-      <c r="R47" s="24"/>
+      <c r="R47" s="23"/>
       <c r="S47" t="s">
         <v>350</v>
       </c>
-      <c r="V47" s="21" t="s">
+      <c r="V47" s="24" t="s">
         <v>5</v>
       </c>
       <c r="W47" t="s">
@@ -3944,29 +3950,29 @@
       <c r="A48" s="1">
         <v>5</v>
       </c>
-      <c r="B48" s="21"/>
+      <c r="B48" s="24"/>
       <c r="C48" t="s">
         <v>217</v>
       </c>
-      <c r="F48" s="21"/>
+      <c r="F48" s="24"/>
       <c r="G48" t="s">
         <v>84</v>
       </c>
-      <c r="J48" s="21"/>
+      <c r="J48" s="24"/>
       <c r="K48" t="s">
         <v>284</v>
       </c>
-      <c r="N48" s="21"/>
+      <c r="N48" s="24"/>
       <c r="O48" t="s">
         <v>251</v>
       </c>
-      <c r="R48" s="21" t="s">
+      <c r="R48" s="24" t="s">
         <v>5</v>
       </c>
       <c r="S48" t="s">
         <v>351</v>
       </c>
-      <c r="V48" s="21"/>
+      <c r="V48" s="24"/>
       <c r="W48" t="s">
         <v>382</v>
       </c>
@@ -3975,28 +3981,28 @@
       <c r="A49" s="1">
         <v>6</v>
       </c>
-      <c r="B49" s="21"/>
+      <c r="B49" s="24"/>
       <c r="C49" t="s">
         <v>221</v>
       </c>
       <c r="D49" s="20"/>
-      <c r="F49" s="21"/>
+      <c r="F49" s="24"/>
       <c r="G49" t="s">
         <v>51</v>
       </c>
-      <c r="J49" s="21"/>
+      <c r="J49" s="24"/>
       <c r="K49" t="s">
         <v>285</v>
       </c>
-      <c r="N49" s="21"/>
+      <c r="N49" s="24"/>
       <c r="O49" t="s">
         <v>322</v>
       </c>
-      <c r="R49" s="21"/>
+      <c r="R49" s="24"/>
       <c r="S49" t="s">
         <v>48</v>
       </c>
-      <c r="V49" s="21"/>
+      <c r="V49" s="24"/>
       <c r="W49" t="s">
         <v>383</v>
       </c>
@@ -4005,31 +4011,31 @@
       <c r="A50" s="1">
         <v>7</v>
       </c>
-      <c r="B50" s="21"/>
+      <c r="B50" s="24"/>
       <c r="C50" t="s">
         <v>222</v>
       </c>
-      <c r="F50" s="21"/>
+      <c r="F50" s="24"/>
       <c r="G50" t="s">
         <v>321</v>
       </c>
-      <c r="J50" s="22" t="s">
+      <c r="J50" s="25" t="s">
         <v>12</v>
       </c>
       <c r="K50" t="s">
         <v>286</v>
       </c>
-      <c r="N50" s="22" t="s">
+      <c r="N50" s="25" t="s">
         <v>12</v>
       </c>
       <c r="O50" t="s">
         <v>323</v>
       </c>
-      <c r="R50" s="21"/>
+      <c r="R50" s="24"/>
       <c r="S50" t="s">
         <v>353</v>
       </c>
-      <c r="V50" s="21"/>
+      <c r="V50" s="24"/>
       <c r="W50" t="s">
         <v>384</v>
       </c>
@@ -4038,56 +4044,56 @@
       <c r="A51" s="1">
         <v>8</v>
       </c>
-      <c r="B51" s="21"/>
+      <c r="B51" s="24"/>
       <c r="C51" t="s">
         <v>253</v>
       </c>
-      <c r="F51" s="21"/>
+      <c r="F51" s="24"/>
       <c r="G51" t="s">
         <v>254</v>
       </c>
-      <c r="J51" s="22"/>
+      <c r="J51" s="25"/>
       <c r="K51" t="s">
         <v>287</v>
       </c>
-      <c r="N51" s="22"/>
+      <c r="N51" s="25"/>
       <c r="O51" t="s">
         <v>324</v>
       </c>
-      <c r="R51" s="21"/>
+      <c r="R51" s="24"/>
       <c r="S51" t="s">
         <v>354</v>
       </c>
-      <c r="V51" s="21"/>
+      <c r="V51" s="24"/>
       <c r="W51" t="s">
-        <v>385</v>
+        <v>186</v>
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>9</v>
       </c>
-      <c r="B52" s="21"/>
+      <c r="B52" s="24"/>
       <c r="C52" t="s">
         <v>83</v>
       </c>
-      <c r="F52" s="21"/>
+      <c r="F52" s="24"/>
       <c r="G52" t="s">
         <v>249</v>
       </c>
-      <c r="J52" s="22"/>
+      <c r="J52" s="25"/>
       <c r="K52" t="s">
         <v>288</v>
       </c>
-      <c r="N52" s="22"/>
+      <c r="N52" s="25"/>
       <c r="O52" t="s">
         <v>325</v>
       </c>
-      <c r="R52" s="21"/>
+      <c r="R52" s="24"/>
       <c r="S52" t="s">
         <v>355</v>
       </c>
-      <c r="V52" s="22" t="s">
+      <c r="V52" s="25" t="s">
         <v>12</v>
       </c>
       <c r="W52" t="s">
@@ -4098,31 +4104,31 @@
       <c r="A53" s="1">
         <v>10</v>
       </c>
-      <c r="B53" s="22" t="s">
+      <c r="B53" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C53" t="s">
         <v>57</v>
       </c>
-      <c r="F53" s="21"/>
+      <c r="F53" s="24"/>
       <c r="G53" t="s">
         <v>255</v>
       </c>
-      <c r="J53" s="22"/>
+      <c r="J53" s="25"/>
       <c r="K53" t="s">
         <v>289</v>
       </c>
-      <c r="N53" s="22"/>
+      <c r="N53" s="25"/>
       <c r="O53" t="s">
         <v>326</v>
       </c>
-      <c r="R53" s="22" t="s">
+      <c r="R53" s="25" t="s">
         <v>12</v>
       </c>
       <c r="S53" t="s">
         <v>356</v>
       </c>
-      <c r="V53" s="22"/>
+      <c r="V53" s="25"/>
       <c r="W53" t="s">
         <v>387</v>
       </c>
@@ -4131,27 +4137,27 @@
       <c r="A54" s="1">
         <v>11</v>
       </c>
-      <c r="B54" s="22"/>
+      <c r="B54" s="25"/>
       <c r="C54" t="s">
         <v>93</v>
       </c>
-      <c r="F54" s="21"/>
+      <c r="F54" s="24"/>
       <c r="G54" t="s">
         <v>185</v>
       </c>
-      <c r="J54" s="22"/>
+      <c r="J54" s="25"/>
       <c r="K54" t="s">
         <v>290</v>
       </c>
-      <c r="N54" s="22"/>
+      <c r="N54" s="25"/>
       <c r="O54" t="s">
         <v>327</v>
       </c>
-      <c r="R54" s="22"/>
+      <c r="R54" s="25"/>
       <c r="S54" t="s">
         <v>357</v>
       </c>
-      <c r="V54" s="22"/>
+      <c r="V54" s="25"/>
       <c r="W54" t="s">
         <v>388</v>
       </c>
@@ -4160,29 +4166,29 @@
       <c r="A55" s="1">
         <v>12</v>
       </c>
-      <c r="B55" s="22"/>
+      <c r="B55" s="25"/>
       <c r="C55" t="s">
         <v>218</v>
       </c>
-      <c r="F55" s="22" t="s">
+      <c r="F55" s="25" t="s">
         <v>12</v>
       </c>
       <c r="G55" t="s">
         <v>219</v>
       </c>
-      <c r="J55" s="22"/>
+      <c r="J55" s="25"/>
       <c r="K55" t="s">
         <v>291</v>
       </c>
-      <c r="N55" s="22"/>
+      <c r="N55" s="25"/>
       <c r="O55" t="s">
         <v>328</v>
       </c>
-      <c r="R55" s="22"/>
+      <c r="R55" s="25"/>
       <c r="S55" t="s">
         <v>358</v>
       </c>
-      <c r="V55" s="22"/>
+      <c r="V55" s="25"/>
       <c r="W55" t="s">
         <v>389</v>
       </c>
@@ -4191,27 +4197,27 @@
       <c r="A56" s="1">
         <v>13</v>
       </c>
-      <c r="B56" s="22"/>
+      <c r="B56" s="25"/>
       <c r="C56" t="s">
         <v>220</v>
       </c>
-      <c r="F56" s="22"/>
+      <c r="F56" s="25"/>
       <c r="G56" t="s">
         <v>228</v>
       </c>
-      <c r="J56" s="22"/>
+      <c r="J56" s="25"/>
       <c r="K56" t="s">
         <v>292</v>
       </c>
-      <c r="N56" s="22"/>
+      <c r="N56" s="25"/>
       <c r="O56" t="s">
         <v>329</v>
       </c>
-      <c r="R56" s="22"/>
+      <c r="R56" s="25"/>
       <c r="S56" t="s">
         <v>359</v>
       </c>
-      <c r="V56" s="22"/>
+      <c r="V56" s="25"/>
       <c r="W56" t="s">
         <v>390</v>
       </c>
@@ -4220,27 +4226,27 @@
       <c r="A57" s="1">
         <v>14</v>
       </c>
-      <c r="B57" s="22"/>
+      <c r="B57" s="25"/>
       <c r="C57" t="s">
         <v>223</v>
       </c>
-      <c r="F57" s="22"/>
+      <c r="F57" s="25"/>
       <c r="G57" t="s">
         <v>258</v>
       </c>
-      <c r="J57" s="22"/>
+      <c r="J57" s="25"/>
       <c r="K57" t="s">
         <v>293</v>
       </c>
-      <c r="N57" s="22"/>
+      <c r="N57" s="25"/>
       <c r="O57" t="s">
         <v>257</v>
       </c>
-      <c r="R57" s="22"/>
+      <c r="R57" s="25"/>
       <c r="S57" t="s">
         <v>360</v>
       </c>
-      <c r="V57" s="22"/>
+      <c r="V57" s="25"/>
       <c r="W57" t="s">
         <v>391</v>
       </c>
@@ -4249,27 +4255,27 @@
       <c r="A58" s="1">
         <v>15</v>
       </c>
-      <c r="B58" s="22"/>
+      <c r="B58" s="25"/>
       <c r="C58" t="s">
         <v>224</v>
       </c>
-      <c r="F58" s="22"/>
+      <c r="F58" s="25"/>
       <c r="G58" t="s">
         <v>90</v>
       </c>
-      <c r="J58" s="22"/>
+      <c r="J58" s="25"/>
       <c r="K58" t="s">
         <v>294</v>
       </c>
-      <c r="N58" s="22"/>
+      <c r="N58" s="25"/>
       <c r="O58" t="s">
         <v>263</v>
       </c>
-      <c r="R58" s="22"/>
+      <c r="R58" s="25"/>
       <c r="S58" t="s">
         <v>361</v>
       </c>
-      <c r="V58" s="22"/>
+      <c r="V58" s="25"/>
       <c r="W58" t="s">
         <v>392</v>
       </c>
@@ -4278,27 +4284,27 @@
       <c r="A59" s="1">
         <v>16</v>
       </c>
-      <c r="B59" s="22"/>
+      <c r="B59" s="25"/>
       <c r="C59" t="s">
         <v>227</v>
       </c>
-      <c r="F59" s="22"/>
+      <c r="F59" s="25"/>
       <c r="G59" t="s">
         <v>262</v>
       </c>
-      <c r="J59" s="22"/>
+      <c r="J59" s="25"/>
       <c r="K59" t="s">
         <v>295</v>
       </c>
-      <c r="N59" s="22"/>
+      <c r="N59" s="25"/>
       <c r="O59" t="s">
         <v>330</v>
       </c>
-      <c r="R59" s="22"/>
+      <c r="R59" s="25"/>
       <c r="S59" t="s">
         <v>362</v>
       </c>
-      <c r="V59" s="22"/>
+      <c r="V59" s="25"/>
       <c r="W59" t="s">
         <v>393</v>
       </c>
@@ -4307,31 +4313,31 @@
       <c r="A60" s="1">
         <v>17</v>
       </c>
-      <c r="B60" s="22"/>
+      <c r="B60" s="25"/>
       <c r="C60" t="s">
         <v>229</v>
       </c>
-      <c r="F60" s="22"/>
+      <c r="F60" s="25"/>
       <c r="G60" t="s">
         <v>260</v>
       </c>
-      <c r="J60" s="23" t="s">
+      <c r="J60" s="21" t="s">
         <v>18</v>
       </c>
       <c r="K60" t="s">
         <v>296</v>
       </c>
-      <c r="N60" s="23" t="s">
+      <c r="N60" s="21" t="s">
         <v>18</v>
       </c>
       <c r="O60" t="s">
         <v>331</v>
       </c>
-      <c r="R60" s="22"/>
+      <c r="R60" s="25"/>
       <c r="S60" t="s">
         <v>192</v>
       </c>
-      <c r="V60" s="23" t="s">
+      <c r="V60" s="21" t="s">
         <v>18</v>
       </c>
       <c r="W60" t="s">
@@ -4342,19 +4348,19 @@
       <c r="A61" s="1">
         <v>18</v>
       </c>
-      <c r="B61" s="22"/>
+      <c r="B61" s="25"/>
       <c r="C61" t="s">
         <v>55</v>
       </c>
-      <c r="F61" s="22"/>
+      <c r="F61" s="25"/>
       <c r="G61" t="s">
         <v>92</v>
       </c>
-      <c r="J61" s="23"/>
+      <c r="J61" s="21"/>
       <c r="K61" t="s">
         <v>297</v>
       </c>
-      <c r="N61" s="23"/>
+      <c r="N61" s="21"/>
       <c r="O61" t="s">
         <v>332</v>
       </c>
@@ -4364,7 +4370,7 @@
       <c r="S61" t="s">
         <v>363</v>
       </c>
-      <c r="V61" s="23"/>
+      <c r="V61" s="21"/>
       <c r="W61" t="s">
         <v>395</v>
       </c>
@@ -4373,31 +4379,31 @@
       <c r="A62" s="1">
         <v>19</v>
       </c>
-      <c r="B62" s="23" t="s">
+      <c r="B62" s="21" t="s">
         <v>18</v>
       </c>
       <c r="C62" t="s">
         <v>233</v>
       </c>
-      <c r="F62" s="22"/>
+      <c r="F62" s="25"/>
       <c r="G62" t="s">
         <v>259</v>
       </c>
-      <c r="J62" s="23"/>
+      <c r="J62" s="21"/>
       <c r="K62" t="s">
         <v>298</v>
       </c>
-      <c r="N62" s="23"/>
+      <c r="N62" s="21"/>
       <c r="O62" t="s">
         <v>334</v>
       </c>
-      <c r="R62" s="25" t="s">
+      <c r="R62" s="22" t="s">
         <v>24</v>
       </c>
       <c r="S62" t="s">
         <v>364</v>
       </c>
-      <c r="V62" s="23"/>
+      <c r="V62" s="21"/>
       <c r="W62" t="s">
         <v>396</v>
       </c>
@@ -4406,31 +4412,31 @@
       <c r="A63" s="1">
         <v>20</v>
       </c>
-      <c r="B63" s="23"/>
+      <c r="B63" s="21"/>
       <c r="C63" t="s">
         <v>230</v>
       </c>
-      <c r="F63" s="23" t="s">
+      <c r="F63" s="21" t="s">
         <v>18</v>
       </c>
       <c r="G63" t="s">
         <v>264</v>
       </c>
-      <c r="J63" s="25" t="s">
+      <c r="J63" s="22" t="s">
         <v>24</v>
       </c>
       <c r="K63" t="s">
         <v>299</v>
       </c>
-      <c r="N63" s="23"/>
+      <c r="N63" s="21"/>
       <c r="O63" t="s">
         <v>335</v>
       </c>
-      <c r="R63" s="25"/>
+      <c r="R63" s="22"/>
       <c r="S63" t="s">
         <v>365</v>
       </c>
-      <c r="V63" s="23"/>
+      <c r="V63" s="21"/>
       <c r="W63" t="s">
         <v>397</v>
       </c>
@@ -4439,29 +4445,29 @@
       <c r="A64" s="1">
         <v>21</v>
       </c>
-      <c r="B64" s="23"/>
+      <c r="B64" s="21"/>
       <c r="C64" t="s">
         <v>231</v>
       </c>
-      <c r="F64" s="23"/>
+      <c r="F64" s="21"/>
       <c r="G64" t="s">
         <v>265</v>
       </c>
-      <c r="J64" s="25"/>
+      <c r="J64" s="22"/>
       <c r="K64" t="s">
         <v>300</v>
       </c>
-      <c r="N64" s="25" t="s">
+      <c r="N64" s="22" t="s">
         <v>24</v>
       </c>
       <c r="O64" t="s">
         <v>336</v>
       </c>
-      <c r="R64" s="25"/>
+      <c r="R64" s="22"/>
       <c r="S64" t="s">
         <v>366</v>
       </c>
-      <c r="V64" s="25" t="s">
+      <c r="V64" s="22" t="s">
         <v>24</v>
       </c>
       <c r="W64" t="s">
@@ -4472,27 +4478,27 @@
       <c r="A65" s="1">
         <v>22</v>
       </c>
-      <c r="B65" s="23"/>
+      <c r="B65" s="21"/>
       <c r="C65" t="s">
         <v>232</v>
       </c>
-      <c r="F65" s="23"/>
+      <c r="F65" s="21"/>
       <c r="G65" t="s">
         <v>97</v>
       </c>
-      <c r="J65" s="25"/>
+      <c r="J65" s="22"/>
       <c r="K65" t="s">
         <v>301</v>
       </c>
-      <c r="N65" s="25"/>
+      <c r="N65" s="22"/>
       <c r="O65" t="s">
         <v>337</v>
       </c>
-      <c r="R65" s="25"/>
+      <c r="R65" s="22"/>
       <c r="S65" t="s">
         <v>367</v>
       </c>
-      <c r="V65" s="25"/>
+      <c r="V65" s="22"/>
       <c r="W65" t="s">
         <v>399</v>
       </c>
@@ -4501,27 +4507,27 @@
       <c r="A66" s="1">
         <v>23</v>
       </c>
-      <c r="B66" s="23"/>
+      <c r="B66" s="21"/>
       <c r="C66" t="s">
         <v>61</v>
       </c>
-      <c r="F66" s="23"/>
+      <c r="F66" s="21"/>
       <c r="G66" t="s">
         <v>266</v>
       </c>
-      <c r="J66" s="25"/>
+      <c r="J66" s="22"/>
       <c r="K66" t="s">
         <v>302</v>
       </c>
-      <c r="N66" s="25"/>
+      <c r="N66" s="22"/>
       <c r="O66" t="s">
         <v>338</v>
       </c>
-      <c r="R66" s="25"/>
+      <c r="R66" s="22"/>
       <c r="S66" t="s">
         <v>368</v>
       </c>
-      <c r="V66" s="25"/>
+      <c r="V66" s="22"/>
       <c r="W66" t="s">
         <v>400</v>
       </c>
@@ -4530,19 +4536,19 @@
       <c r="A67" s="1">
         <v>24</v>
       </c>
-      <c r="B67" s="23"/>
+      <c r="B67" s="21"/>
       <c r="C67" t="s">
         <v>267</v>
       </c>
-      <c r="F67" s="23"/>
+      <c r="F67" s="21"/>
       <c r="G67" t="s">
         <v>21</v>
       </c>
-      <c r="J67" s="25"/>
+      <c r="J67" s="22"/>
       <c r="K67" t="s">
         <v>303</v>
       </c>
-      <c r="N67" s="25"/>
+      <c r="N67" s="22"/>
       <c r="O67" t="s">
         <v>342</v>
       </c>
@@ -4552,7 +4558,7 @@
       <c r="S67" t="s">
         <v>369</v>
       </c>
-      <c r="V67" s="25"/>
+      <c r="V67" s="22"/>
       <c r="W67" t="s">
         <v>401</v>
       </c>
@@ -4561,19 +4567,19 @@
       <c r="A68" s="1">
         <v>25</v>
       </c>
-      <c r="B68" s="25" t="s">
+      <c r="B68" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C68" t="s">
         <v>102</v>
       </c>
-      <c r="F68" s="25" t="s">
+      <c r="F68" s="22" t="s">
         <v>24</v>
       </c>
       <c r="G68" t="s">
         <v>268</v>
       </c>
-      <c r="J68" s="25"/>
+      <c r="J68" s="22"/>
       <c r="K68" t="s">
         <v>304</v>
       </c>
@@ -4598,15 +4604,15 @@
       <c r="A69" s="1">
         <v>26</v>
       </c>
-      <c r="B69" s="25"/>
+      <c r="B69" s="22"/>
       <c r="C69" t="s">
         <v>234</v>
       </c>
-      <c r="F69" s="25"/>
+      <c r="F69" s="22"/>
       <c r="G69" t="s">
         <v>269</v>
       </c>
-      <c r="J69" s="25"/>
+      <c r="J69" s="22"/>
       <c r="K69" t="s">
         <v>305</v>
       </c>
@@ -4627,11 +4633,11 @@
       <c r="A70" s="1">
         <v>27</v>
       </c>
-      <c r="B70" s="25"/>
+      <c r="B70" s="22"/>
       <c r="C70" t="s">
         <v>235</v>
       </c>
-      <c r="F70" s="25"/>
+      <c r="F70" s="22"/>
       <c r="G70" t="s">
         <v>270</v>
       </c>
@@ -4658,11 +4664,11 @@
       <c r="A71" s="1">
         <v>28</v>
       </c>
-      <c r="B71" s="25"/>
+      <c r="B71" s="22"/>
       <c r="C71" t="s">
         <v>236</v>
       </c>
-      <c r="F71" s="25"/>
+      <c r="F71" s="22"/>
       <c r="G71" t="s">
         <v>101</v>
       </c>
@@ -4689,7 +4695,7 @@
       <c r="A72" s="1">
         <v>29</v>
       </c>
-      <c r="B72" s="25"/>
+      <c r="B72" s="22"/>
       <c r="C72" t="s">
         <v>237</v>
       </c>
@@ -4722,7 +4728,7 @@
       <c r="A73" s="1">
         <v>30</v>
       </c>
-      <c r="B73" s="25"/>
+      <c r="B73" s="22"/>
       <c r="C73" t="s">
         <v>238</v>
       </c>
@@ -4838,6 +4844,10 @@
       <c r="K77" t="s">
         <v>313</v>
       </c>
+      <c r="V77" s="27"/>
+      <c r="W77" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B78" s="27" t="s">
@@ -4875,37 +4885,44 @@
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="V23:V25"/>
-    <mergeCell ref="R20:R21"/>
-    <mergeCell ref="V26:V29"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="R4:R9"/>
-    <mergeCell ref="R10:R19"/>
-    <mergeCell ref="V5:V12"/>
-    <mergeCell ref="V2:V4"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="N4:N10"/>
-    <mergeCell ref="N11:N16"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="J70:J73"/>
-    <mergeCell ref="J74:J77"/>
-    <mergeCell ref="N44:N46"/>
-    <mergeCell ref="N47:N49"/>
-    <mergeCell ref="N64:N67"/>
-    <mergeCell ref="N68:N71"/>
-    <mergeCell ref="N72:N75"/>
-    <mergeCell ref="N50:N59"/>
-    <mergeCell ref="J60:J62"/>
-    <mergeCell ref="J50:J59"/>
-    <mergeCell ref="J63:J69"/>
-    <mergeCell ref="N60:N63"/>
-    <mergeCell ref="F72:F75"/>
-    <mergeCell ref="F68:F71"/>
-    <mergeCell ref="B68:B73"/>
-    <mergeCell ref="B74:B77"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="F76:F79"/>
+    <mergeCell ref="V73:V77"/>
+    <mergeCell ref="V35:V37"/>
+    <mergeCell ref="B47:B52"/>
+    <mergeCell ref="B53:B61"/>
+    <mergeCell ref="B62:B67"/>
+    <mergeCell ref="F47:F54"/>
+    <mergeCell ref="F55:F62"/>
+    <mergeCell ref="F63:F67"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="J4:J8"/>
+    <mergeCell ref="J9:J16"/>
+    <mergeCell ref="F10:F15"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="R53:R60"/>
+    <mergeCell ref="V13:V22"/>
+    <mergeCell ref="V68:V72"/>
+    <mergeCell ref="R67:R70"/>
+    <mergeCell ref="R71:R75"/>
+    <mergeCell ref="R31:R34"/>
+    <mergeCell ref="V43:Y43"/>
+    <mergeCell ref="V44:V46"/>
+    <mergeCell ref="V47:V51"/>
+    <mergeCell ref="V52:V59"/>
+    <mergeCell ref="V60:V63"/>
+    <mergeCell ref="V64:V67"/>
+    <mergeCell ref="R62:R66"/>
+    <mergeCell ref="V30:V34"/>
     <mergeCell ref="R48:R52"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B5:B10"/>
@@ -4922,44 +4939,37 @@
     <mergeCell ref="N19:N23"/>
     <mergeCell ref="F44:F46"/>
     <mergeCell ref="B44:B46"/>
-    <mergeCell ref="R53:R60"/>
-    <mergeCell ref="V13:V22"/>
-    <mergeCell ref="V68:V72"/>
-    <mergeCell ref="V73:V76"/>
-    <mergeCell ref="R67:R70"/>
-    <mergeCell ref="R71:R75"/>
-    <mergeCell ref="R31:R34"/>
-    <mergeCell ref="V43:Y43"/>
-    <mergeCell ref="V44:V46"/>
-    <mergeCell ref="V47:V51"/>
-    <mergeCell ref="V52:V59"/>
-    <mergeCell ref="V60:V63"/>
-    <mergeCell ref="V64:V67"/>
-    <mergeCell ref="V35:V38"/>
-    <mergeCell ref="R62:R66"/>
-    <mergeCell ref="V30:V34"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="F27:F31"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="J4:J8"/>
-    <mergeCell ref="J9:J16"/>
-    <mergeCell ref="F10:F15"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B47:B52"/>
-    <mergeCell ref="B53:B61"/>
-    <mergeCell ref="B62:B67"/>
-    <mergeCell ref="F47:F54"/>
-    <mergeCell ref="F55:F62"/>
-    <mergeCell ref="F63:F67"/>
+    <mergeCell ref="F72:F75"/>
+    <mergeCell ref="F68:F71"/>
+    <mergeCell ref="B68:B73"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="F76:F79"/>
+    <mergeCell ref="J70:J73"/>
+    <mergeCell ref="J74:J77"/>
+    <mergeCell ref="N44:N46"/>
+    <mergeCell ref="N47:N49"/>
+    <mergeCell ref="N64:N67"/>
+    <mergeCell ref="N68:N71"/>
+    <mergeCell ref="N72:N75"/>
+    <mergeCell ref="N50:N59"/>
+    <mergeCell ref="J60:J62"/>
+    <mergeCell ref="J50:J59"/>
+    <mergeCell ref="J63:J69"/>
+    <mergeCell ref="N60:N63"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="N4:N10"/>
+    <mergeCell ref="N11:N16"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="V23:V25"/>
+    <mergeCell ref="R20:R21"/>
+    <mergeCell ref="V26:V29"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="R4:R9"/>
+    <mergeCell ref="R10:R19"/>
+    <mergeCell ref="V5:V12"/>
+    <mergeCell ref="V2:V4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -4970,8 +4980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z50"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4992,221 +5002,224 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="E1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="E1" s="29" t="s">
         <v>412</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
       <c r="J1" t="s">
         <v>411</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="O1" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="T1" s="28" t="s">
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="T1" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="X1" s="28" t="s">
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="X1" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>415</v>
       </c>
       <c r="B2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E2" t="s">
+        <v>553</v>
+      </c>
+      <c r="F2" t="s">
+        <v>490</v>
+      </c>
+      <c r="J2" t="s">
         <v>554</v>
       </c>
-      <c r="F2" t="s">
-        <v>491</v>
-      </c>
-      <c r="J2" t="s">
-        <v>555</v>
-      </c>
       <c r="K2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="O2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="P2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="T2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="U2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="X2" t="s">
-        <v>594</v>
+        <v>722</v>
       </c>
       <c r="Y2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E3" t="s">
         <v>414</v>
       </c>
       <c r="F3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J3" t="s">
         <v>413</v>
       </c>
       <c r="K3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="O3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="P3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="T3" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="U3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="X3" t="s">
-        <v>604</v>
+        <v>593</v>
       </c>
       <c r="Y3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
+        <v>535</v>
+      </c>
+      <c r="E4" t="s">
+        <v>589</v>
+      </c>
+      <c r="F4" t="s">
+        <v>497</v>
+      </c>
+      <c r="J4" t="s">
+        <v>599</v>
+      </c>
+      <c r="K4" t="s">
         <v>536</v>
       </c>
-      <c r="E4" t="s">
-        <v>590</v>
-      </c>
-      <c r="F4" t="s">
-        <v>498</v>
-      </c>
-      <c r="J4" t="s">
-        <v>600</v>
-      </c>
-      <c r="K4" t="s">
-        <v>537</v>
-      </c>
       <c r="O4" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="P4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="T4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="U4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="X4" t="s">
-        <v>416</v>
+        <v>603</v>
       </c>
       <c r="Y4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F5" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G5" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="J5" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="K5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="O5" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="P5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="T5" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="U5" t="s">
-        <v>534</v>
+        <v>533</v>
+      </c>
+      <c r="X5" t="s">
+        <v>416</v>
       </c>
       <c r="Y5" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B6" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="K6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="P6" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="T6" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="U6" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E7" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F7" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="K7" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="T7" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.35">
@@ -5214,52 +5227,52 @@
         <v>419</v>
       </c>
       <c r="K8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="T8" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="K9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="T9" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="K11" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="29" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
       <c r="E17" t="s">
         <v>420</v>
       </c>
-      <c r="I17" s="28" t="s">
+      <c r="I17" s="29" t="s">
         <v>421</v>
       </c>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="N17" s="28" t="s">
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="N17" s="29" t="s">
         <v>314</v>
       </c>
-      <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="28"/>
-      <c r="S17" s="28" t="s">
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="S17" s="29" t="s">
         <v>315</v>
       </c>
-      <c r="T17" s="28"/>
-      <c r="U17" s="28"/>
-      <c r="V17" s="28"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="29"/>
+      <c r="V17" s="29"/>
       <c r="X17" t="s">
         <v>316</v>
       </c>
@@ -5269,305 +5282,308 @@
         <v>417</v>
       </c>
       <c r="B18" t="s">
+        <v>509</v>
+      </c>
+      <c r="E18" t="s">
+        <v>594</v>
+      </c>
+      <c r="F18" t="s">
+        <v>502</v>
+      </c>
+      <c r="J18" t="s">
+        <v>595</v>
+      </c>
+      <c r="K18" t="s">
         <v>510</v>
-      </c>
-      <c r="E18" t="s">
-        <v>595</v>
-      </c>
-      <c r="F18" t="s">
-        <v>503</v>
-      </c>
-      <c r="J18" t="s">
-        <v>596</v>
-      </c>
-      <c r="K18" t="s">
-        <v>511</v>
       </c>
       <c r="O18" t="s">
         <v>424</v>
       </c>
       <c r="P18" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T18" t="s">
         <v>422</v>
       </c>
       <c r="U18" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="X18" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="Y18" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B19" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E19" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F19" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="J19" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="K19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="O19" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="P19" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="T19" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="U19" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="X19" t="s">
         <v>423</v>
       </c>
       <c r="Y19" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>598</v>
+      </c>
+      <c r="B20" t="s">
+        <v>702</v>
+      </c>
+      <c r="E20" t="s">
         <v>599</v>
       </c>
-      <c r="B20" t="s">
-        <v>703</v>
-      </c>
-      <c r="E20" t="s">
-        <v>600</v>
-      </c>
       <c r="F20" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="J20" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="K20" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="O20" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="P20" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="T20" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="X20" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="Y20" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E21" t="s">
         <v>429</v>
       </c>
       <c r="F21" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="J21" t="s">
         <v>426</v>
       </c>
       <c r="K21" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="O21" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="P21" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="T21" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="X21" t="s">
         <v>428</v>
       </c>
       <c r="Y21" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E22" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F22" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="K22" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="O22" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="P22" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="T22" t="s">
         <v>425</v>
       </c>
-      <c r="X22" t="s">
-        <v>430</v>
-      </c>
       <c r="Y22" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E23" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F23" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="O23" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="P23" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="T23" t="s">
         <v>427</v>
       </c>
       <c r="U23" t="s">
-        <v>688</v>
+        <v>687</v>
+      </c>
+      <c r="X23" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E24" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F24" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="O24" t="s">
-        <v>431</v>
+        <v>430</v>
+      </c>
+      <c r="X24" t="s">
+        <v>702</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E25" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="O25" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E26" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.35">
       <c r="C30" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.35">
       <c r="C31" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.35">
       <c r="C32" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C33" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C34" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C35" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C36" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C37" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="38" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C38" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C39" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J39" s="17" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="K39" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.35">
       <c r="J40" s="18" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="K40" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="41" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="J41" s="19" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="K41" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.35">
@@ -5575,7 +5591,7 @@
         <v>4</v>
       </c>
       <c r="J42" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.35">
@@ -5583,7 +5599,7 @@
         <v>5</v>
       </c>
       <c r="J43" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.35">
@@ -5591,7 +5607,7 @@
         <v>6</v>
       </c>
       <c r="J44" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.35">
@@ -5599,7 +5615,7 @@
         <v>7</v>
       </c>
       <c r="J45" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="46" spans="3:11" x14ac:dyDescent="0.35">
@@ -5607,7 +5623,7 @@
         <v>8</v>
       </c>
       <c r="J46" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.35">
@@ -5615,7 +5631,7 @@
         <v>9</v>
       </c>
       <c r="J47" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.35">
@@ -5623,7 +5639,7 @@
         <v>10</v>
       </c>
       <c r="J48" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="49" spans="9:10" x14ac:dyDescent="0.35">
@@ -5631,7 +5647,7 @@
         <v>11</v>
       </c>
       <c r="J49" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="50" spans="9:10" x14ac:dyDescent="0.35">
@@ -5639,7 +5655,7 @@
         <v>12</v>
       </c>
       <c r="J50" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
   </sheetData>
@@ -5655,6 +5671,7 @@
     <mergeCell ref="T1:V1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5675,134 +5692,134 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>439</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>440</v>
+      </c>
+      <c r="B2" t="s">
         <v>441</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="4" t="s">
         <v>442</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B3" t="s">
+        <v>443</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>444</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>445</v>
+      </c>
+      <c r="B4" t="s">
         <v>446</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="4" t="s">
         <v>447</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>448</v>
+      </c>
+      <c r="B5" t="s">
         <v>449</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="4" t="s">
         <v>450</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B6" t="s">
+        <v>451</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>452</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B7" t="s">
+        <v>453</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>454</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B8" t="s">
+        <v>455</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>456</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>457</v>
+      </c>
+      <c r="B9" t="s">
         <v>458</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="4" t="s">
         <v>459</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B10" t="s">
+        <v>460</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>461</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>462</v>
+      </c>
+      <c r="B11" t="s">
         <v>463</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="4" t="s">
         <v>464</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>465</v>
+      </c>
+      <c r="B12" t="s">
         <v>466</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="4" t="s">
         <v>467</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>468</v>
       </c>
     </row>
   </sheetData>
@@ -5825,10 +5842,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K216"/>
+  <dimension ref="A1:K221"/>
   <sheetViews>
-    <sheetView topLeftCell="A203" workbookViewId="0">
-      <selection activeCell="B213" sqref="B213"/>
+    <sheetView topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="C219" sqref="C219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5848,7 +5865,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>226</v>
@@ -5856,7 +5873,7 @@
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>44</v>
@@ -5865,10 +5882,10 @@
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -5881,13 +5898,13 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="10"/>
       <c r="B5" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="10"/>
       <c r="B6" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -5896,7 +5913,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>90</v>
@@ -5905,19 +5922,19 @@
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="10"/>
       <c r="B11" s="11" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -5929,37 +5946,37 @@
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="7"/>
       <c r="B17" s="8" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>86</v>
@@ -5974,7 +5991,7 @@
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="10"/>
       <c r="B21" s="11" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -5986,7 +6003,7 @@
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="10"/>
       <c r="B23" s="11" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -5998,19 +6015,19 @@
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="10"/>
       <c r="B25" s="12" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="10"/>
       <c r="B26" s="11" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="10"/>
       <c r="B27" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -6019,7 +6036,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>17</v>
@@ -6034,31 +6051,31 @@
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="10"/>
       <c r="B31" s="11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="10"/>
       <c r="B32" s="11" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="10"/>
       <c r="B33" s="12" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="10"/>
       <c r="B34" s="12" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="10"/>
       <c r="B35" s="12" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -6070,13 +6087,13 @@
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="10"/>
       <c r="B37" s="12" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="10"/>
       <c r="B38" s="11" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -6088,13 +6105,13 @@
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="10"/>
       <c r="B40" s="11" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="10"/>
       <c r="B41" s="11" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -6112,7 +6129,7 @@
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="10"/>
       <c r="B44" s="12" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6124,27 +6141,27 @@
     <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
+        <v>561</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>562</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="10"/>
       <c r="B48" s="11" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="10"/>
       <c r="B49" s="11" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="7" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>225</v>
@@ -6153,28 +6170,28 @@
     <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="10"/>
       <c r="B54" s="15" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="10"/>
       <c r="B55" s="15" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="10"/>
       <c r="B56" s="15" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -6183,7 +6200,7 @@
     </row>
     <row r="58" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="7" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B58" s="16" t="s">
         <v>321</v>
@@ -6192,24 +6209,24 @@
     <row r="60" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>573</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="7" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>48</v>
@@ -6218,33 +6235,33 @@
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="10"/>
       <c r="B65" s="11" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="10" t="s">
+        <v>576</v>
+      </c>
+      <c r="B66" s="11" t="s">
         <v>577</v>
-      </c>
-      <c r="B66" s="11" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="10"/>
       <c r="B67" s="11" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="7"/>
       <c r="B68" s="8" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>183</v>
@@ -6253,27 +6270,27 @@
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="10"/>
       <c r="B71" s="11" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="10"/>
       <c r="B72" s="11" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="10"/>
       <c r="B73" s="11" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="10" t="s">
+        <v>586</v>
+      </c>
+      <c r="B74" s="11" t="s">
         <v>587</v>
-      </c>
-      <c r="B74" s="11" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -6309,13 +6326,13 @@
     <row r="80" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="7"/>
       <c r="B80" s="8" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>78</v>
@@ -6323,16 +6340,16 @@
     </row>
     <row r="84" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="7" t="s">
+        <v>643</v>
+      </c>
+      <c r="B84" s="8" t="s">
         <v>644</v>
-      </c>
-      <c r="B84" s="8" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>215</v>
@@ -6340,7 +6357,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="10" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B88" s="11" t="s">
         <v>57</v>
@@ -6349,13 +6366,13 @@
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="10"/>
       <c r="B89" s="11" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="10"/>
       <c r="B90" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6367,7 +6384,7 @@
     <row r="92" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>93</v>
@@ -6382,7 +6399,7 @@
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="10"/>
       <c r="B95" s="11" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -6393,42 +6410,42 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="10" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="10"/>
       <c r="B98" s="11" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="10"/>
       <c r="B99" s="11" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="7"/>
       <c r="B100" s="8" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="B103" s="6" t="s">
         <v>654</v>
-      </c>
-      <c r="B103" s="6" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="7" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B104" s="8" t="s">
         <v>35</v>
@@ -6437,24 +6454,24 @@
     <row r="106" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="10"/>
       <c r="B108" s="11" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="10" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6466,7 +6483,7 @@
     <row r="112" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B113" s="6" t="s">
         <v>10</v>
@@ -6474,7 +6491,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="10" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B114" s="11" t="s">
         <v>188</v>
@@ -6483,16 +6500,16 @@
     <row r="115" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A115" s="7"/>
       <c r="B115" s="8" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
@@ -6503,10 +6520,10 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="10" t="s">
+        <v>659</v>
+      </c>
+      <c r="B120" s="11" t="s">
         <v>660</v>
-      </c>
-      <c r="B120" s="11" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
@@ -6518,16 +6535,16 @@
     <row r="122" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A122" s="7"/>
       <c r="B122" s="8" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
@@ -6539,158 +6556,158 @@
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" s="10"/>
       <c r="B126" s="11" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" s="10"/>
       <c r="B127" s="11" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" s="10"/>
       <c r="B128" s="11" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" s="10" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" s="10"/>
       <c r="B130" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A131" s="7"/>
       <c r="B131" s="8" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" s="10"/>
       <c r="B134" s="11" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" s="10"/>
       <c r="B135" s="11" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A136" s="7" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" s="10" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B139" s="11" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A140" s="7"/>
       <c r="B140" s="8" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" s="10"/>
       <c r="B143" s="11" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" s="10"/>
       <c r="B144" s="11" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" s="10"/>
       <c r="B145" s="11" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" s="10" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B146" s="11" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" s="10"/>
       <c r="B147" s="11" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A148" s="7"/>
       <c r="B148" s="8" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" s="10"/>
       <c r="B151" s="11" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" s="10" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B152" s="11" t="s">
         <v>15</v>
@@ -6699,19 +6716,19 @@
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" s="10"/>
       <c r="B153" s="11" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A154" s="7"/>
       <c r="B154" s="8" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" s="5" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B156" s="6" t="s">
         <v>192</v>
@@ -6719,25 +6736,25 @@
     </row>
     <row r="157" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A157" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="10"/>
       <c r="B160" s="11" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
@@ -6748,51 +6765,51 @@
     </row>
     <row r="162" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A162" s="7" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="5" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" s="10"/>
       <c r="B165" s="11" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" s="10"/>
       <c r="B166" s="11" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" s="10" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B167" s="11" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A168" s="7"/>
       <c r="B168" s="8" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B170" s="6" t="s">
         <v>48</v>
@@ -6801,12 +6818,12 @@
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" s="10"/>
       <c r="B171" s="11" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" s="10" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B172" s="11" t="s">
         <v>352</v>
@@ -6815,65 +6832,65 @@
     <row r="173" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A173" s="7"/>
       <c r="B173" s="8" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" s="5" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" s="10" t="s">
+        <v>690</v>
+      </c>
+      <c r="B176" s="11" t="s">
         <v>691</v>
-      </c>
-      <c r="B176" s="11" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A177" s="7"/>
       <c r="B177" s="8" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" s="5" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" s="10"/>
       <c r="B180" s="11" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" s="10"/>
       <c r="B181" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" s="10"/>
       <c r="B182" s="11" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" s="10" t="s">
+        <v>695</v>
+      </c>
+      <c r="B183" s="11" t="s">
         <v>696</v>
-      </c>
-      <c r="B183" s="11" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6885,18 +6902,18 @@
     <row r="185" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" s="5" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" s="10" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B187" s="11" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6908,10 +6925,10 @@
     <row r="189" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" s="5" t="s">
+        <v>703</v>
+      </c>
+      <c r="B190" s="6" t="s">
         <v>704</v>
-      </c>
-      <c r="B190" s="6" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
@@ -6923,30 +6940,30 @@
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" s="10"/>
       <c r="B192" s="11" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" s="10"/>
       <c r="B193" s="11" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" s="10"/>
       <c r="B194" s="11" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" s="10"/>
       <c r="B195" s="11" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" s="10" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B196" s="11" t="s">
         <v>219</v>
@@ -6955,37 +6972,37 @@
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" s="10"/>
       <c r="B197" s="11" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" s="10"/>
       <c r="B198" s="11" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" s="10"/>
       <c r="B199" s="11" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" s="10"/>
       <c r="B200" s="11" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A201" s="7"/>
       <c r="B201" s="8" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" s="5" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B203" s="6" t="s">
         <v>214</v>
@@ -6993,7 +7010,7 @@
     </row>
     <row r="204" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A204" s="7" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B204" s="8" t="s">
         <v>179</v>
@@ -7002,27 +7019,27 @@
     <row r="205" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" s="5" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B206" s="6" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" s="10"/>
       <c r="B207" s="11" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" s="10"/>
       <c r="B208" s="11" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A209" s="7" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B209" s="8" t="s">
         <v>21</v>
@@ -7031,15 +7048,15 @@
     <row r="210" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" s="5" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B211" s="6" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" s="10" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B212" s="11" t="s">
         <v>27</v>
@@ -7048,24 +7065,53 @@
     <row r="213" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A213" s="7"/>
       <c r="B213" s="8" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" s="5" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B215" s="6" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A216" s="7" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B216" s="8" t="s">
         <v>333</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A218" s="5" t="s">
+        <v>719</v>
+      </c>
+      <c r="B218" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A219" s="10"/>
+      <c r="B219" s="11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A220" s="10" t="s">
+        <v>720</v>
+      </c>
+      <c r="B220" s="11" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A221" s="7"/>
+      <c r="B221" s="8" t="s">
+        <v>721</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
couple trades and correct pick issue
moved wrong pick from Vanja to Ben and it was corrected
</commit_message>
<xml_diff>
--- a/OffSeason.xlsx
+++ b/OffSeason.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Rosters" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="747">
   <si>
     <t>Chubber for Chubb - John Olson</t>
   </si>
@@ -2250,6 +2250,24 @@
   </si>
   <si>
     <t>2021 4th Cam</t>
+  </si>
+  <si>
+    <t>Alan trades</t>
+  </si>
+  <si>
+    <t>Adam trades</t>
+  </si>
+  <si>
+    <t>Garner Minshaw</t>
+  </si>
+  <si>
+    <t>2020 4th (MikeW)</t>
+  </si>
+  <si>
+    <t>John trades</t>
+  </si>
+  <si>
+    <t>2021 3 (MikeW)</t>
   </si>
 </sst>
 </file>
@@ -2491,13 +2509,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2514,6 +2526,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2801,8 +2819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I67" sqref="I67"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2843,68 +2861,68 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="K2" t="s">
         <v>77</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="O2" t="s">
         <v>112</v>
       </c>
-      <c r="R2" s="23" t="s">
+      <c r="R2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="S2" t="s">
         <v>144</v>
       </c>
-      <c r="V2" s="23" t="s">
+      <c r="V2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="W2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="22"/>
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="23"/>
+      <c r="F3" s="22"/>
       <c r="G3" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="23"/>
+      <c r="J3" s="22"/>
       <c r="K3" t="s">
         <v>214</v>
       </c>
-      <c r="N3" s="23"/>
+      <c r="N3" s="22"/>
       <c r="O3" t="s">
         <v>104</v>
       </c>
-      <c r="R3" s="23"/>
+      <c r="R3" s="22"/>
       <c r="S3" t="s">
         <v>145</v>
       </c>
-      <c r="V3" s="23"/>
+      <c r="V3" s="22"/>
       <c r="W3" t="s">
         <v>180</v>
       </c>
@@ -2913,33 +2931,33 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="23"/>
+      <c r="B4" s="22"/>
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="23"/>
+      <c r="F4" s="22"/>
       <c r="G4" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="28" t="s">
         <v>5</v>
       </c>
       <c r="K4" t="s">
         <v>248</v>
       </c>
-      <c r="N4" s="24" t="s">
+      <c r="N4" s="28" t="s">
         <v>5</v>
       </c>
       <c r="O4" t="s">
         <v>113</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="28" t="s">
         <v>5</v>
       </c>
       <c r="S4" t="s">
         <v>146</v>
       </c>
-      <c r="V4" s="23"/>
+      <c r="V4" s="22"/>
       <c r="W4" t="s">
         <v>181</v>
       </c>
@@ -2948,29 +2966,29 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="23"/>
+      <c r="F5" s="22"/>
       <c r="G5" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="24"/>
+      <c r="J5" s="28"/>
       <c r="K5" t="s">
         <v>81</v>
       </c>
-      <c r="N5" s="24"/>
+      <c r="N5" s="28"/>
       <c r="O5" t="s">
         <v>114</v>
       </c>
-      <c r="R5" s="24"/>
+      <c r="R5" s="28"/>
       <c r="S5" t="s">
         <v>147</v>
       </c>
-      <c r="V5" s="24" t="s">
+      <c r="V5" s="28" t="s">
         <v>5</v>
       </c>
       <c r="W5" t="s">
@@ -2981,29 +2999,29 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="28"/>
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="28" t="s">
         <v>5</v>
       </c>
       <c r="G6" t="s">
         <v>215</v>
       </c>
-      <c r="J6" s="24"/>
+      <c r="J6" s="28"/>
       <c r="K6" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="24"/>
+      <c r="N6" s="28"/>
       <c r="O6" t="s">
         <v>115</v>
       </c>
-      <c r="R6" s="24"/>
+      <c r="R6" s="28"/>
       <c r="S6" t="s">
         <v>148</v>
       </c>
-      <c r="V6" s="24"/>
+      <c r="V6" s="28"/>
       <c r="W6" t="s">
         <v>250</v>
       </c>
@@ -3012,27 +3030,27 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="24"/>
+      <c r="B7" s="28"/>
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="24"/>
+      <c r="F7" s="28"/>
       <c r="G7" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="24"/>
+      <c r="J7" s="28"/>
       <c r="K7" t="s">
         <v>352</v>
       </c>
-      <c r="N7" s="24"/>
+      <c r="N7" s="28"/>
       <c r="O7" t="s">
         <v>116</v>
       </c>
-      <c r="R7" s="24"/>
+      <c r="R7" s="28"/>
       <c r="S7" t="s">
         <v>149</v>
       </c>
-      <c r="V7" s="24"/>
+      <c r="V7" s="28"/>
       <c r="W7" t="s">
         <v>184</v>
       </c>
@@ -3041,27 +3059,27 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="24"/>
+      <c r="B8" s="28"/>
       <c r="C8" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="28"/>
       <c r="G8" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="24"/>
+      <c r="J8" s="28"/>
       <c r="K8" t="s">
         <v>85</v>
       </c>
-      <c r="N8" s="24"/>
+      <c r="N8" s="28"/>
       <c r="O8" t="s">
         <v>117</v>
       </c>
-      <c r="R8" s="24"/>
+      <c r="R8" s="28"/>
       <c r="S8" t="s">
         <v>150</v>
       </c>
-      <c r="V8" s="24"/>
+      <c r="V8" s="28"/>
       <c r="W8" t="s">
         <v>252</v>
       </c>
@@ -3070,27 +3088,27 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="24"/>
+      <c r="B9" s="28"/>
       <c r="C9" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="24"/>
+      <c r="F9" s="28"/>
       <c r="G9" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="24"/>
+      <c r="J9" s="28"/>
       <c r="K9" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="24"/>
+      <c r="N9" s="28"/>
       <c r="O9" t="s">
         <v>118</v>
       </c>
-      <c r="R9" s="24"/>
+      <c r="R9" s="28"/>
       <c r="S9" t="s">
         <v>151</v>
       </c>
-      <c r="V9" s="24"/>
+      <c r="V9" s="28"/>
       <c r="W9" t="s">
         <v>385</v>
       </c>
@@ -3099,35 +3117,35 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="23" t="s">
         <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G10" t="s">
         <v>194</v>
       </c>
-      <c r="J10" s="25" t="s">
+      <c r="J10" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K10" t="s">
         <v>15</v>
       </c>
-      <c r="N10" s="24"/>
+      <c r="N10" s="28"/>
       <c r="O10" t="s">
         <v>119</v>
       </c>
-      <c r="R10" s="25" t="s">
+      <c r="R10" s="23" t="s">
         <v>12</v>
       </c>
       <c r="S10" t="s">
         <v>152</v>
       </c>
-      <c r="V10" s="24"/>
+      <c r="V10" s="28"/>
       <c r="W10" t="s">
         <v>187</v>
       </c>
@@ -3136,29 +3154,29 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="25"/>
+      <c r="B11" s="23"/>
       <c r="C11" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="25"/>
+      <c r="F11" s="23"/>
       <c r="G11" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="25"/>
+      <c r="J11" s="23"/>
       <c r="K11" t="s">
         <v>188</v>
       </c>
-      <c r="N11" s="25" t="s">
+      <c r="N11" s="23" t="s">
         <v>12</v>
       </c>
       <c r="O11" t="s">
         <v>120</v>
       </c>
-      <c r="R11" s="25"/>
+      <c r="R11" s="23"/>
       <c r="S11" t="s">
         <v>153</v>
       </c>
-      <c r="V11" s="24"/>
+      <c r="V11" s="28"/>
       <c r="W11" t="s">
         <v>53</v>
       </c>
@@ -3167,27 +3185,27 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="25"/>
+      <c r="B12" s="23"/>
       <c r="C12" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="25"/>
+      <c r="F12" s="23"/>
       <c r="G12" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="25"/>
+      <c r="J12" s="23"/>
       <c r="K12" t="s">
         <v>86</v>
       </c>
-      <c r="N12" s="25"/>
+      <c r="N12" s="23"/>
       <c r="O12" t="s">
         <v>121</v>
       </c>
-      <c r="R12" s="25"/>
+      <c r="R12" s="23"/>
       <c r="S12" t="s">
         <v>154</v>
       </c>
-      <c r="V12" s="24"/>
+      <c r="V12" s="28"/>
       <c r="W12" t="s">
         <v>10</v>
       </c>
@@ -3196,27 +3214,27 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="25"/>
+      <c r="B13" s="23"/>
       <c r="C13" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="25"/>
+      <c r="F13" s="23"/>
       <c r="G13" t="s">
         <v>59</v>
       </c>
-      <c r="J13" s="25"/>
+      <c r="J13" s="23"/>
       <c r="K13" t="s">
         <v>88</v>
       </c>
-      <c r="N13" s="25"/>
+      <c r="N13" s="23"/>
       <c r="O13" t="s">
         <v>122</v>
       </c>
-      <c r="R13" s="25"/>
+      <c r="R13" s="23"/>
       <c r="S13" t="s">
         <v>155</v>
       </c>
-      <c r="V13" s="25" t="s">
+      <c r="V13" s="23" t="s">
         <v>12</v>
       </c>
       <c r="W13" t="s">
@@ -3227,27 +3245,27 @@
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="25"/>
+      <c r="B14" s="23"/>
       <c r="C14" t="s">
         <v>87</v>
       </c>
-      <c r="F14" s="25"/>
+      <c r="F14" s="23"/>
       <c r="G14" t="s">
         <v>226</v>
       </c>
-      <c r="J14" s="25"/>
+      <c r="J14" s="23"/>
       <c r="K14" t="s">
         <v>16</v>
       </c>
-      <c r="N14" s="25"/>
+      <c r="N14" s="23"/>
       <c r="O14" t="s">
         <v>123</v>
       </c>
-      <c r="R14" s="25"/>
+      <c r="R14" s="23"/>
       <c r="S14" t="s">
         <v>156</v>
       </c>
-      <c r="V14" s="25"/>
+      <c r="V14" s="23"/>
       <c r="W14" t="s">
         <v>189</v>
       </c>
@@ -3256,27 +3274,27 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="25"/>
+      <c r="B15" s="23"/>
       <c r="C15" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="25"/>
+      <c r="F15" s="23"/>
       <c r="G15" t="s">
         <v>225</v>
       </c>
-      <c r="J15" s="25"/>
+      <c r="J15" s="23"/>
       <c r="K15" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="25"/>
+      <c r="N15" s="23"/>
       <c r="O15" t="s">
         <v>124</v>
       </c>
-      <c r="R15" s="25"/>
+      <c r="R15" s="23"/>
       <c r="S15" t="s">
         <v>157</v>
       </c>
-      <c r="V15" s="25"/>
+      <c r="V15" s="23"/>
       <c r="W15" t="s">
         <v>190</v>
       </c>
@@ -3285,31 +3303,31 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="29" t="s">
         <v>18</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="29" t="s">
         <v>18</v>
       </c>
       <c r="G16" t="s">
         <v>60</v>
       </c>
-      <c r="J16" s="25"/>
+      <c r="J16" s="23"/>
       <c r="K16" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="25"/>
+      <c r="N16" s="23"/>
       <c r="O16" t="s">
         <v>125</v>
       </c>
-      <c r="R16" s="25"/>
+      <c r="R16" s="23"/>
       <c r="S16" t="s">
         <v>158</v>
       </c>
-      <c r="V16" s="25"/>
+      <c r="V16" s="23"/>
       <c r="W16" t="s">
         <v>191</v>
       </c>
@@ -3318,31 +3336,31 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="22"/>
+      <c r="B17" s="29"/>
       <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="22"/>
+      <c r="F17" s="29"/>
       <c r="G17" t="s">
         <v>62</v>
       </c>
-      <c r="J17" s="22" t="s">
+      <c r="J17" s="29" t="s">
         <v>18</v>
       </c>
       <c r="K17" t="s">
         <v>95</v>
       </c>
-      <c r="N17" s="22" t="s">
+      <c r="N17" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O17" t="s">
         <v>126</v>
       </c>
-      <c r="R17" s="25"/>
+      <c r="R17" s="23"/>
       <c r="S17" t="s">
         <v>159</v>
       </c>
-      <c r="V17" s="25"/>
+      <c r="V17" s="23"/>
       <c r="W17" t="s">
         <v>91</v>
       </c>
@@ -3351,27 +3369,27 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="22"/>
+      <c r="B18" s="29"/>
       <c r="C18" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="22"/>
+      <c r="F18" s="29"/>
       <c r="G18" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="22"/>
+      <c r="J18" s="29"/>
       <c r="K18" t="s">
         <v>98</v>
       </c>
-      <c r="N18" s="22"/>
+      <c r="N18" s="29"/>
       <c r="O18" t="s">
         <v>127</v>
       </c>
-      <c r="R18" s="25"/>
+      <c r="R18" s="23"/>
       <c r="S18" t="s">
         <v>160</v>
       </c>
-      <c r="V18" s="25"/>
+      <c r="V18" s="23"/>
       <c r="W18" t="s">
         <v>261</v>
       </c>
@@ -3380,33 +3398,33 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="25" t="s">
         <v>24</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="25" t="s">
         <v>24</v>
       </c>
       <c r="G19" t="s">
         <v>64</v>
       </c>
-      <c r="J19" s="22"/>
+      <c r="J19" s="29"/>
       <c r="K19" t="s">
         <v>333</v>
       </c>
-      <c r="N19" s="27" t="s">
+      <c r="N19" s="25" t="s">
         <v>24</v>
       </c>
       <c r="O19" t="s">
         <v>128</v>
       </c>
-      <c r="R19" s="25"/>
+      <c r="R19" s="23"/>
       <c r="S19" t="s">
         <v>161</v>
       </c>
-      <c r="V19" s="25"/>
+      <c r="V19" s="23"/>
       <c r="W19" t="s">
         <v>94</v>
       </c>
@@ -3415,31 +3433,31 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="27"/>
+      <c r="B20" s="25"/>
       <c r="C20" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="27"/>
+      <c r="F20" s="25"/>
       <c r="G20" t="s">
         <v>65</v>
       </c>
-      <c r="J20" s="27" t="s">
+      <c r="J20" s="25" t="s">
         <v>24</v>
       </c>
       <c r="K20" t="s">
         <v>99</v>
       </c>
-      <c r="N20" s="27"/>
+      <c r="N20" s="25"/>
       <c r="O20" t="s">
         <v>129</v>
       </c>
-      <c r="R20" s="22" t="s">
+      <c r="R20" s="29" t="s">
         <v>18</v>
       </c>
       <c r="S20" t="s">
         <v>162</v>
       </c>
-      <c r="V20" s="25"/>
+      <c r="V20" s="23"/>
       <c r="W20" t="s">
         <v>193</v>
       </c>
@@ -3448,27 +3466,27 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="27"/>
+      <c r="B21" s="25"/>
       <c r="C21" t="s">
         <v>100</v>
       </c>
-      <c r="F21" s="27"/>
+      <c r="F21" s="25"/>
       <c r="G21" t="s">
         <v>66</v>
       </c>
-      <c r="J21" s="27"/>
+      <c r="J21" s="25"/>
       <c r="K21" t="s">
         <v>28</v>
       </c>
-      <c r="N21" s="27"/>
+      <c r="N21" s="25"/>
       <c r="O21" t="s">
         <v>130</v>
       </c>
-      <c r="R21" s="22"/>
+      <c r="R21" s="29"/>
       <c r="S21" t="s">
         <v>163</v>
       </c>
-      <c r="V21" s="25"/>
+      <c r="V21" s="23"/>
       <c r="W21" t="s">
         <v>195</v>
       </c>
@@ -3477,31 +3495,31 @@
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="24" t="s">
         <v>30</v>
       </c>
       <c r="C22" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="27"/>
+      <c r="F22" s="25"/>
       <c r="G22" t="s">
         <v>67</v>
       </c>
-      <c r="J22" s="27"/>
+      <c r="J22" s="25"/>
       <c r="K22" t="s">
         <v>29</v>
       </c>
-      <c r="N22" s="27"/>
+      <c r="N22" s="25"/>
       <c r="O22" t="s">
         <v>131</v>
       </c>
-      <c r="R22" s="27" t="s">
+      <c r="R22" s="25" t="s">
         <v>24</v>
       </c>
       <c r="S22" t="s">
         <v>164</v>
       </c>
-      <c r="V22" s="25"/>
+      <c r="V22" s="23"/>
       <c r="W22" t="s">
         <v>196</v>
       </c>
@@ -3510,29 +3528,29 @@
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="26"/>
+      <c r="B23" s="24"/>
       <c r="C23" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="24" t="s">
         <v>30</v>
       </c>
       <c r="G23" t="s">
         <v>69</v>
       </c>
-      <c r="J23" s="27"/>
+      <c r="J23" s="25"/>
       <c r="K23" t="s">
         <v>27</v>
       </c>
-      <c r="N23" s="27"/>
+      <c r="N23" s="25"/>
       <c r="O23" t="s">
         <v>132</v>
       </c>
-      <c r="R23" s="27"/>
+      <c r="R23" s="25"/>
       <c r="S23" t="s">
         <v>165</v>
       </c>
-      <c r="V23" s="22" t="s">
+      <c r="V23" s="29" t="s">
         <v>18</v>
       </c>
       <c r="W23" t="s">
@@ -3543,31 +3561,31 @@
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="26"/>
+      <c r="B24" s="24"/>
       <c r="C24" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="26"/>
+      <c r="F24" s="24"/>
       <c r="G24" t="s">
         <v>70</v>
       </c>
-      <c r="J24" s="26" t="s">
+      <c r="J24" s="24" t="s">
         <v>30</v>
       </c>
       <c r="K24" t="s">
         <v>103</v>
       </c>
-      <c r="N24" s="26" t="s">
+      <c r="N24" s="24" t="s">
         <v>30</v>
       </c>
       <c r="O24" t="s">
         <v>133</v>
       </c>
-      <c r="R24" s="27"/>
+      <c r="R24" s="25"/>
       <c r="S24" t="s">
         <v>166</v>
       </c>
-      <c r="V24" s="22"/>
+      <c r="V24" s="29"/>
       <c r="W24" t="s">
         <v>198</v>
       </c>
@@ -3576,27 +3594,27 @@
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="26"/>
+      <c r="B25" s="24"/>
       <c r="C25" t="s">
         <v>104</v>
       </c>
-      <c r="F25" s="26"/>
+      <c r="F25" s="24"/>
       <c r="G25" t="s">
         <v>71</v>
       </c>
-      <c r="J25" s="26"/>
+      <c r="J25" s="24"/>
       <c r="K25" t="s">
         <v>105</v>
       </c>
-      <c r="N25" s="26"/>
+      <c r="N25" s="24"/>
       <c r="O25" t="s">
         <v>134</v>
       </c>
-      <c r="R25" s="27"/>
+      <c r="R25" s="25"/>
       <c r="S25" t="s">
         <v>167</v>
       </c>
-      <c r="V25" s="22"/>
+      <c r="V25" s="29"/>
       <c r="W25" t="s">
         <v>199</v>
       </c>
@@ -3605,31 +3623,31 @@
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="26" t="s">
         <v>36</v>
       </c>
       <c r="C26" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="26"/>
+      <c r="F26" s="24"/>
       <c r="G26" t="s">
         <v>68</v>
       </c>
-      <c r="J26" s="26"/>
+      <c r="J26" s="24"/>
       <c r="K26" t="s">
         <v>106</v>
       </c>
-      <c r="N26" s="26"/>
+      <c r="N26" s="24"/>
       <c r="O26" t="s">
         <v>135</v>
       </c>
-      <c r="R26" s="26" t="s">
+      <c r="R26" s="24" t="s">
         <v>30</v>
       </c>
       <c r="S26" t="s">
         <v>168</v>
       </c>
-      <c r="V26" s="27" t="s">
+      <c r="V26" s="25" t="s">
         <v>24</v>
       </c>
       <c r="W26" t="s">
@@ -3640,31 +3658,31 @@
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="28"/>
+      <c r="B27" s="26"/>
       <c r="C27" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="28" t="s">
+      <c r="F27" s="26" t="s">
         <v>36</v>
       </c>
       <c r="G27" t="s">
         <v>72</v>
       </c>
-      <c r="J27" s="28" t="s">
+      <c r="J27" s="26" t="s">
         <v>36</v>
       </c>
       <c r="K27" t="s">
         <v>40</v>
       </c>
-      <c r="N27" s="26"/>
+      <c r="N27" s="24"/>
       <c r="O27" t="s">
         <v>136</v>
       </c>
-      <c r="R27" s="26"/>
+      <c r="R27" s="24"/>
       <c r="S27" t="s">
         <v>169</v>
       </c>
-      <c r="V27" s="27"/>
+      <c r="V27" s="25"/>
       <c r="W27" t="s">
         <v>201</v>
       </c>
@@ -3673,27 +3691,27 @@
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="28"/>
+      <c r="B28" s="26"/>
       <c r="C28" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="28"/>
+      <c r="F28" s="26"/>
       <c r="G28" t="s">
         <v>73</v>
       </c>
-      <c r="J28" s="28"/>
+      <c r="J28" s="26"/>
       <c r="K28" t="s">
         <v>108</v>
       </c>
-      <c r="N28" s="26"/>
+      <c r="N28" s="24"/>
       <c r="O28" t="s">
         <v>137</v>
       </c>
-      <c r="R28" s="26"/>
+      <c r="R28" s="24"/>
       <c r="S28" t="s">
         <v>170</v>
       </c>
-      <c r="V28" s="27"/>
+      <c r="V28" s="25"/>
       <c r="W28" t="s">
         <v>202</v>
       </c>
@@ -3702,27 +3720,27 @@
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="28"/>
+      <c r="B29" s="26"/>
       <c r="C29" t="s">
         <v>107</v>
       </c>
-      <c r="F29" s="28"/>
+      <c r="F29" s="26"/>
       <c r="G29" t="s">
         <v>74</v>
       </c>
-      <c r="J29" s="28"/>
+      <c r="J29" s="26"/>
       <c r="K29" t="s">
         <v>110</v>
       </c>
-      <c r="N29" s="26"/>
+      <c r="N29" s="24"/>
       <c r="O29" t="s">
         <v>138</v>
       </c>
-      <c r="R29" s="26"/>
+      <c r="R29" s="24"/>
       <c r="S29" t="s">
         <v>171</v>
       </c>
-      <c r="V29" s="27"/>
+      <c r="V29" s="25"/>
       <c r="W29" t="s">
         <v>203</v>
       </c>
@@ -3731,25 +3749,25 @@
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="F30" s="28"/>
+      <c r="F30" s="26"/>
       <c r="G30" t="s">
         <v>75</v>
       </c>
-      <c r="J30" s="28"/>
+      <c r="J30" s="26"/>
       <c r="K30" t="s">
         <v>41</v>
       </c>
-      <c r="N30" s="28" t="s">
+      <c r="N30" s="26" t="s">
         <v>36</v>
       </c>
       <c r="O30" t="s">
         <v>139</v>
       </c>
-      <c r="R30" s="26"/>
+      <c r="R30" s="24"/>
       <c r="S30" t="s">
         <v>172</v>
       </c>
-      <c r="V30" s="26" t="s">
+      <c r="V30" s="24" t="s">
         <v>30</v>
       </c>
       <c r="W30" t="s">
@@ -3760,65 +3778,65 @@
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="26"/>
       <c r="G31" t="s">
         <v>275</v>
       </c>
-      <c r="N31" s="28"/>
+      <c r="N31" s="26"/>
       <c r="O31" t="s">
         <v>140</v>
       </c>
-      <c r="R31" s="28" t="s">
+      <c r="R31" s="26" t="s">
         <v>36</v>
       </c>
       <c r="S31" t="s">
         <v>173</v>
       </c>
-      <c r="V31" s="26"/>
+      <c r="V31" s="24"/>
       <c r="W31" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="N32" s="28"/>
+      <c r="N32" s="26"/>
       <c r="O32" t="s">
         <v>141</v>
       </c>
-      <c r="R32" s="28"/>
+      <c r="R32" s="26"/>
       <c r="S32" t="s">
         <v>174</v>
       </c>
-      <c r="V32" s="26"/>
+      <c r="V32" s="24"/>
       <c r="W32" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="N33" s="28"/>
+      <c r="N33" s="26"/>
       <c r="O33" t="s">
         <v>142</v>
       </c>
-      <c r="R33" s="28"/>
+      <c r="R33" s="26"/>
       <c r="S33" t="s">
         <v>175</v>
       </c>
-      <c r="V33" s="26"/>
+      <c r="V33" s="24"/>
       <c r="W33" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="R34" s="28"/>
+      <c r="R34" s="26"/>
       <c r="S34" t="s">
         <v>176</v>
       </c>
-      <c r="V34" s="26"/>
+      <c r="V34" s="24"/>
       <c r="W34" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V35" s="28" t="s">
+      <c r="V35" s="26" t="s">
         <v>36</v>
       </c>
       <c r="W35" t="s">
@@ -3826,13 +3844,13 @@
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V36" s="28"/>
+      <c r="V36" s="26"/>
       <c r="W36" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="V37" s="28"/>
+      <c r="V37" s="26"/>
       <c r="W37" t="s">
         <v>211</v>
       </c>
@@ -3853,48 +3871,48 @@
       <c r="R43" t="s">
         <v>315</v>
       </c>
-      <c r="V43" s="29" t="s">
+      <c r="V43" s="27" t="s">
         <v>316</v>
       </c>
-      <c r="W43" s="29"/>
-      <c r="X43" s="29"/>
-      <c r="Y43" s="29"/>
+      <c r="W43" s="27"/>
+      <c r="X43" s="27"/>
+      <c r="Y43" s="27"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>1</v>
       </c>
-      <c r="B44" s="23" t="s">
+      <c r="B44" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C44" t="s">
         <v>44</v>
       </c>
-      <c r="F44" s="23" t="s">
+      <c r="F44" s="22" t="s">
         <v>1</v>
       </c>
       <c r="G44" t="s">
         <v>246</v>
       </c>
-      <c r="J44" s="23" t="s">
+      <c r="J44" s="22" t="s">
         <v>1</v>
       </c>
       <c r="K44" t="s">
         <v>280</v>
       </c>
-      <c r="N44" s="23" t="s">
+      <c r="N44" s="22" t="s">
         <v>1</v>
       </c>
       <c r="O44" t="s">
         <v>317</v>
       </c>
-      <c r="R44" s="23" t="s">
+      <c r="R44" s="22" t="s">
         <v>1</v>
       </c>
       <c r="S44" t="s">
         <v>348</v>
       </c>
-      <c r="V44" s="23" t="s">
+      <c r="V44" s="22" t="s">
         <v>1</v>
       </c>
       <c r="W44" t="s">
@@ -3905,27 +3923,27 @@
       <c r="A45" s="1">
         <v>2</v>
       </c>
-      <c r="B45" s="23"/>
+      <c r="B45" s="22"/>
       <c r="C45" t="s">
-        <v>179</v>
-      </c>
-      <c r="F45" s="23"/>
+        <v>178</v>
+      </c>
+      <c r="F45" s="22"/>
       <c r="G45" t="s">
         <v>247</v>
       </c>
-      <c r="J45" s="23"/>
+      <c r="J45" s="22"/>
       <c r="K45" t="s">
         <v>281</v>
       </c>
-      <c r="N45" s="23"/>
+      <c r="N45" s="22"/>
       <c r="O45" t="s">
         <v>318</v>
       </c>
-      <c r="R45" s="23"/>
+      <c r="R45" s="22"/>
       <c r="S45" t="s">
         <v>349</v>
       </c>
-      <c r="V45" s="23"/>
+      <c r="V45" s="22"/>
       <c r="W45" t="s">
         <v>379</v>
       </c>
@@ -3934,27 +3952,27 @@
       <c r="A46" s="1">
         <v>3</v>
       </c>
-      <c r="B46" s="23"/>
+      <c r="B46" s="22"/>
       <c r="C46" t="s">
         <v>213</v>
       </c>
-      <c r="F46" s="23"/>
+      <c r="F46" s="22"/>
       <c r="G46" t="s">
         <v>79</v>
       </c>
-      <c r="J46" s="23"/>
+      <c r="J46" s="22"/>
       <c r="K46" t="s">
         <v>282</v>
       </c>
-      <c r="N46" s="23"/>
+      <c r="N46" s="22"/>
       <c r="O46" t="s">
         <v>319</v>
       </c>
-      <c r="R46" s="23"/>
+      <c r="R46" s="22"/>
       <c r="S46" t="s">
         <v>78</v>
       </c>
-      <c r="V46" s="23"/>
+      <c r="V46" s="22"/>
       <c r="W46" t="s">
         <v>380</v>
       </c>
@@ -3963,35 +3981,35 @@
       <c r="A47" s="1">
         <v>4</v>
       </c>
-      <c r="B47" s="24" t="s">
+      <c r="B47" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C47" t="s">
         <v>216</v>
       </c>
-      <c r="F47" s="24" t="s">
+      <c r="F47" s="28" t="s">
         <v>5</v>
       </c>
       <c r="G47" t="s">
         <v>183</v>
       </c>
-      <c r="J47" s="24" t="s">
+      <c r="J47" s="28" t="s">
         <v>5</v>
       </c>
       <c r="K47" t="s">
         <v>283</v>
       </c>
-      <c r="N47" s="24" t="s">
+      <c r="N47" s="28" t="s">
         <v>5</v>
       </c>
       <c r="O47" t="s">
         <v>320</v>
       </c>
-      <c r="R47" s="23"/>
+      <c r="R47" s="22"/>
       <c r="S47" t="s">
         <v>350</v>
       </c>
-      <c r="V47" s="24" t="s">
+      <c r="V47" s="28" t="s">
         <v>5</v>
       </c>
       <c r="W47" t="s">
@@ -4002,29 +4020,29 @@
       <c r="A48" s="1">
         <v>5</v>
       </c>
-      <c r="B48" s="24"/>
+      <c r="B48" s="28"/>
       <c r="C48" t="s">
         <v>217</v>
       </c>
-      <c r="F48" s="24"/>
+      <c r="F48" s="28"/>
       <c r="G48" t="s">
         <v>84</v>
       </c>
-      <c r="J48" s="24"/>
+      <c r="J48" s="28"/>
       <c r="K48" t="s">
         <v>284</v>
       </c>
-      <c r="N48" s="24"/>
+      <c r="N48" s="28"/>
       <c r="O48" t="s">
         <v>251</v>
       </c>
-      <c r="R48" s="24" t="s">
+      <c r="R48" s="28" t="s">
         <v>5</v>
       </c>
       <c r="S48" t="s">
         <v>351</v>
       </c>
-      <c r="V48" s="24"/>
+      <c r="V48" s="28"/>
       <c r="W48" t="s">
         <v>382</v>
       </c>
@@ -4033,28 +4051,28 @@
       <c r="A49" s="1">
         <v>6</v>
       </c>
-      <c r="B49" s="24"/>
+      <c r="B49" s="28"/>
       <c r="C49" t="s">
         <v>221</v>
       </c>
       <c r="D49" s="20"/>
-      <c r="F49" s="24"/>
+      <c r="F49" s="28"/>
       <c r="G49" t="s">
         <v>51</v>
       </c>
-      <c r="J49" s="24"/>
+      <c r="J49" s="28"/>
       <c r="K49" t="s">
         <v>285</v>
       </c>
-      <c r="N49" s="24"/>
+      <c r="N49" s="28"/>
       <c r="O49" t="s">
         <v>322</v>
       </c>
-      <c r="R49" s="24"/>
+      <c r="R49" s="28"/>
       <c r="S49" t="s">
         <v>48</v>
       </c>
-      <c r="V49" s="24"/>
+      <c r="V49" s="28"/>
       <c r="W49" t="s">
         <v>383</v>
       </c>
@@ -4063,31 +4081,31 @@
       <c r="A50" s="1">
         <v>7</v>
       </c>
-      <c r="B50" s="24"/>
+      <c r="B50" s="28"/>
       <c r="C50" t="s">
         <v>222</v>
       </c>
-      <c r="F50" s="24"/>
+      <c r="F50" s="28"/>
       <c r="G50" t="s">
         <v>321</v>
       </c>
-      <c r="J50" s="25" t="s">
+      <c r="J50" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K50" t="s">
         <v>286</v>
       </c>
-      <c r="N50" s="25" t="s">
+      <c r="N50" s="23" t="s">
         <v>12</v>
       </c>
       <c r="O50" t="s">
         <v>323</v>
       </c>
-      <c r="R50" s="24"/>
+      <c r="R50" s="28"/>
       <c r="S50" t="s">
         <v>353</v>
       </c>
-      <c r="V50" s="24"/>
+      <c r="V50" s="28"/>
       <c r="W50" t="s">
         <v>384</v>
       </c>
@@ -4096,27 +4114,27 @@
       <c r="A51" s="1">
         <v>8</v>
       </c>
-      <c r="B51" s="24"/>
+      <c r="B51" s="28"/>
       <c r="C51" t="s">
         <v>253</v>
       </c>
-      <c r="F51" s="24"/>
+      <c r="F51" s="28"/>
       <c r="G51" t="s">
         <v>254</v>
       </c>
-      <c r="J51" s="25"/>
+      <c r="J51" s="23"/>
       <c r="K51" t="s">
         <v>287</v>
       </c>
-      <c r="N51" s="25"/>
+      <c r="N51" s="23"/>
       <c r="O51" t="s">
         <v>324</v>
       </c>
-      <c r="R51" s="24"/>
+      <c r="R51" s="28"/>
       <c r="S51" t="s">
         <v>354</v>
       </c>
-      <c r="V51" s="24"/>
+      <c r="V51" s="28"/>
       <c r="W51" t="s">
         <v>186</v>
       </c>
@@ -4125,27 +4143,27 @@
       <c r="A52" s="1">
         <v>9</v>
       </c>
-      <c r="B52" s="24"/>
+      <c r="B52" s="28"/>
       <c r="C52" t="s">
         <v>83</v>
       </c>
-      <c r="F52" s="24"/>
+      <c r="F52" s="28"/>
       <c r="G52" t="s">
         <v>249</v>
       </c>
-      <c r="J52" s="25"/>
+      <c r="J52" s="23"/>
       <c r="K52" t="s">
         <v>288</v>
       </c>
-      <c r="N52" s="25"/>
+      <c r="N52" s="23"/>
       <c r="O52" t="s">
         <v>325</v>
       </c>
-      <c r="R52" s="24"/>
+      <c r="R52" s="28"/>
       <c r="S52" t="s">
         <v>355</v>
       </c>
-      <c r="V52" s="25" t="s">
+      <c r="V52" s="23" t="s">
         <v>12</v>
       </c>
       <c r="W52" t="s">
@@ -4156,31 +4174,31 @@
       <c r="A53" s="1">
         <v>10</v>
       </c>
-      <c r="B53" s="25" t="s">
+      <c r="B53" s="23" t="s">
         <v>12</v>
       </c>
       <c r="C53" t="s">
         <v>57</v>
       </c>
-      <c r="F53" s="24"/>
+      <c r="F53" s="28"/>
       <c r="G53" t="s">
         <v>255</v>
       </c>
-      <c r="J53" s="25"/>
+      <c r="J53" s="23"/>
       <c r="K53" t="s">
         <v>289</v>
       </c>
-      <c r="N53" s="25"/>
+      <c r="N53" s="23"/>
       <c r="O53" t="s">
         <v>326</v>
       </c>
-      <c r="R53" s="25" t="s">
+      <c r="R53" s="23" t="s">
         <v>12</v>
       </c>
       <c r="S53" t="s">
         <v>356</v>
       </c>
-      <c r="V53" s="25"/>
+      <c r="V53" s="23"/>
       <c r="W53" t="s">
         <v>387</v>
       </c>
@@ -4189,27 +4207,27 @@
       <c r="A54" s="1">
         <v>11</v>
       </c>
-      <c r="B54" s="25"/>
+      <c r="B54" s="23"/>
       <c r="C54" t="s">
         <v>93</v>
       </c>
-      <c r="F54" s="24"/>
+      <c r="F54" s="28"/>
       <c r="G54" t="s">
         <v>185</v>
       </c>
-      <c r="J54" s="25"/>
+      <c r="J54" s="23"/>
       <c r="K54" t="s">
         <v>290</v>
       </c>
-      <c r="N54" s="25"/>
+      <c r="N54" s="23"/>
       <c r="O54" t="s">
         <v>327</v>
       </c>
-      <c r="R54" s="25"/>
+      <c r="R54" s="23"/>
       <c r="S54" t="s">
         <v>357</v>
       </c>
-      <c r="V54" s="25"/>
+      <c r="V54" s="23"/>
       <c r="W54" t="s">
         <v>388</v>
       </c>
@@ -4218,29 +4236,29 @@
       <c r="A55" s="1">
         <v>12</v>
       </c>
-      <c r="B55" s="25"/>
+      <c r="B55" s="23"/>
       <c r="C55" t="s">
         <v>218</v>
       </c>
-      <c r="F55" s="25" t="s">
+      <c r="F55" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G55" t="s">
         <v>219</v>
       </c>
-      <c r="J55" s="25"/>
+      <c r="J55" s="23"/>
       <c r="K55" t="s">
         <v>291</v>
       </c>
-      <c r="N55" s="25"/>
+      <c r="N55" s="23"/>
       <c r="O55" t="s">
         <v>328</v>
       </c>
-      <c r="R55" s="25"/>
+      <c r="R55" s="23"/>
       <c r="S55" t="s">
         <v>358</v>
       </c>
-      <c r="V55" s="25"/>
+      <c r="V55" s="23"/>
       <c r="W55" t="s">
         <v>389</v>
       </c>
@@ -4249,27 +4267,27 @@
       <c r="A56" s="1">
         <v>13</v>
       </c>
-      <c r="B56" s="25"/>
+      <c r="B56" s="23"/>
       <c r="C56" t="s">
         <v>220</v>
       </c>
-      <c r="F56" s="25"/>
+      <c r="F56" s="23"/>
       <c r="G56" t="s">
         <v>228</v>
       </c>
-      <c r="J56" s="25"/>
+      <c r="J56" s="23"/>
       <c r="K56" t="s">
         <v>292</v>
       </c>
-      <c r="N56" s="25"/>
+      <c r="N56" s="23"/>
       <c r="O56" t="s">
         <v>329</v>
       </c>
-      <c r="R56" s="25"/>
+      <c r="R56" s="23"/>
       <c r="S56" t="s">
         <v>359</v>
       </c>
-      <c r="V56" s="25"/>
+      <c r="V56" s="23"/>
       <c r="W56" t="s">
         <v>390</v>
       </c>
@@ -4278,27 +4296,27 @@
       <c r="A57" s="1">
         <v>14</v>
       </c>
-      <c r="B57" s="25"/>
+      <c r="B57" s="23"/>
       <c r="C57" t="s">
         <v>223</v>
       </c>
-      <c r="F57" s="25"/>
+      <c r="F57" s="23"/>
       <c r="G57" t="s">
         <v>258</v>
       </c>
-      <c r="J57" s="25"/>
+      <c r="J57" s="23"/>
       <c r="K57" t="s">
         <v>293</v>
       </c>
-      <c r="N57" s="25"/>
+      <c r="N57" s="23"/>
       <c r="O57" t="s">
         <v>257</v>
       </c>
-      <c r="R57" s="25"/>
+      <c r="R57" s="23"/>
       <c r="S57" t="s">
         <v>360</v>
       </c>
-      <c r="V57" s="25"/>
+      <c r="V57" s="23"/>
       <c r="W57" t="s">
         <v>391</v>
       </c>
@@ -4307,27 +4325,27 @@
       <c r="A58" s="1">
         <v>15</v>
       </c>
-      <c r="B58" s="25"/>
+      <c r="B58" s="23"/>
       <c r="C58" t="s">
         <v>224</v>
       </c>
-      <c r="F58" s="25"/>
+      <c r="F58" s="23"/>
       <c r="G58" t="s">
         <v>90</v>
       </c>
-      <c r="J58" s="25"/>
+      <c r="J58" s="23"/>
       <c r="K58" t="s">
         <v>294</v>
       </c>
-      <c r="N58" s="25"/>
+      <c r="N58" s="23"/>
       <c r="O58" t="s">
         <v>263</v>
       </c>
-      <c r="R58" s="25"/>
+      <c r="R58" s="23"/>
       <c r="S58" t="s">
         <v>361</v>
       </c>
-      <c r="V58" s="25"/>
+      <c r="V58" s="23"/>
       <c r="W58" t="s">
         <v>392</v>
       </c>
@@ -4336,27 +4354,27 @@
       <c r="A59" s="1">
         <v>16</v>
       </c>
-      <c r="B59" s="25"/>
+      <c r="B59" s="23"/>
       <c r="C59" t="s">
         <v>227</v>
       </c>
-      <c r="F59" s="25"/>
+      <c r="F59" s="23"/>
       <c r="G59" t="s">
         <v>262</v>
       </c>
-      <c r="J59" s="25"/>
+      <c r="J59" s="23"/>
       <c r="K59" t="s">
         <v>295</v>
       </c>
-      <c r="N59" s="25"/>
+      <c r="N59" s="23"/>
       <c r="O59" t="s">
         <v>330</v>
       </c>
-      <c r="R59" s="25"/>
+      <c r="R59" s="23"/>
       <c r="S59" t="s">
         <v>362</v>
       </c>
-      <c r="V59" s="25"/>
+      <c r="V59" s="23"/>
       <c r="W59" t="s">
         <v>393</v>
       </c>
@@ -4365,31 +4383,31 @@
       <c r="A60" s="1">
         <v>17</v>
       </c>
-      <c r="B60" s="25"/>
+      <c r="B60" s="23"/>
       <c r="C60" t="s">
         <v>229</v>
       </c>
-      <c r="F60" s="25"/>
+      <c r="F60" s="23"/>
       <c r="G60" t="s">
         <v>260</v>
       </c>
-      <c r="J60" s="22" t="s">
+      <c r="J60" s="29" t="s">
         <v>18</v>
       </c>
       <c r="K60" t="s">
         <v>296</v>
       </c>
-      <c r="N60" s="22" t="s">
+      <c r="N60" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O60" t="s">
         <v>331</v>
       </c>
-      <c r="R60" s="25"/>
+      <c r="R60" s="23"/>
       <c r="S60" t="s">
         <v>192</v>
       </c>
-      <c r="V60" s="22" t="s">
+      <c r="V60" s="29" t="s">
         <v>18</v>
       </c>
       <c r="W60" t="s">
@@ -4400,19 +4418,19 @@
       <c r="A61" s="1">
         <v>18</v>
       </c>
-      <c r="B61" s="25"/>
+      <c r="B61" s="23"/>
       <c r="C61" t="s">
         <v>55</v>
       </c>
-      <c r="F61" s="25"/>
+      <c r="F61" s="23"/>
       <c r="G61" t="s">
         <v>92</v>
       </c>
-      <c r="J61" s="22"/>
+      <c r="J61" s="29"/>
       <c r="K61" t="s">
         <v>297</v>
       </c>
-      <c r="N61" s="22"/>
+      <c r="N61" s="29"/>
       <c r="O61" t="s">
         <v>332</v>
       </c>
@@ -4422,7 +4440,7 @@
       <c r="S61" t="s">
         <v>363</v>
       </c>
-      <c r="V61" s="22"/>
+      <c r="V61" s="29"/>
       <c r="W61" t="s">
         <v>395</v>
       </c>
@@ -4431,31 +4449,31 @@
       <c r="A62" s="1">
         <v>19</v>
       </c>
-      <c r="B62" s="22" t="s">
+      <c r="B62" s="29" t="s">
         <v>18</v>
       </c>
       <c r="C62" t="s">
         <v>233</v>
       </c>
-      <c r="F62" s="25"/>
+      <c r="F62" s="23"/>
       <c r="G62" t="s">
         <v>259</v>
       </c>
-      <c r="J62" s="22"/>
+      <c r="J62" s="29"/>
       <c r="K62" t="s">
         <v>298</v>
       </c>
-      <c r="N62" s="22"/>
+      <c r="N62" s="29"/>
       <c r="O62" t="s">
         <v>334</v>
       </c>
-      <c r="R62" s="27" t="s">
+      <c r="R62" s="25" t="s">
         <v>24</v>
       </c>
       <c r="S62" t="s">
         <v>364</v>
       </c>
-      <c r="V62" s="22"/>
+      <c r="V62" s="29"/>
       <c r="W62" t="s">
         <v>396</v>
       </c>
@@ -4464,31 +4482,31 @@
       <c r="A63" s="1">
         <v>20</v>
       </c>
-      <c r="B63" s="22"/>
+      <c r="B63" s="29"/>
       <c r="C63" t="s">
         <v>230</v>
       </c>
-      <c r="F63" s="22" t="s">
+      <c r="F63" s="29" t="s">
         <v>18</v>
       </c>
       <c r="G63" t="s">
         <v>264</v>
       </c>
-      <c r="J63" s="27" t="s">
+      <c r="J63" s="25" t="s">
         <v>24</v>
       </c>
       <c r="K63" t="s">
         <v>299</v>
       </c>
-      <c r="N63" s="22"/>
+      <c r="N63" s="29"/>
       <c r="O63" t="s">
         <v>335</v>
       </c>
-      <c r="R63" s="27"/>
+      <c r="R63" s="25"/>
       <c r="S63" t="s">
         <v>365</v>
       </c>
-      <c r="V63" s="22"/>
+      <c r="V63" s="29"/>
       <c r="W63" t="s">
         <v>397</v>
       </c>
@@ -4497,29 +4515,29 @@
       <c r="A64" s="1">
         <v>21</v>
       </c>
-      <c r="B64" s="22"/>
+      <c r="B64" s="29"/>
       <c r="C64" t="s">
         <v>231</v>
       </c>
-      <c r="F64" s="22"/>
+      <c r="F64" s="29"/>
       <c r="G64" t="s">
         <v>265</v>
       </c>
-      <c r="J64" s="27"/>
+      <c r="J64" s="25"/>
       <c r="K64" t="s">
         <v>300</v>
       </c>
-      <c r="N64" s="27" t="s">
+      <c r="N64" s="25" t="s">
         <v>24</v>
       </c>
       <c r="O64" t="s">
         <v>336</v>
       </c>
-      <c r="R64" s="27"/>
+      <c r="R64" s="25"/>
       <c r="S64" t="s">
         <v>366</v>
       </c>
-      <c r="V64" s="27" t="s">
+      <c r="V64" s="25" t="s">
         <v>24</v>
       </c>
       <c r="W64" t="s">
@@ -4530,27 +4548,27 @@
       <c r="A65" s="1">
         <v>22</v>
       </c>
-      <c r="B65" s="22"/>
+      <c r="B65" s="29"/>
       <c r="C65" t="s">
         <v>232</v>
       </c>
-      <c r="F65" s="22"/>
+      <c r="F65" s="29"/>
       <c r="G65" t="s">
         <v>97</v>
       </c>
-      <c r="J65" s="27"/>
+      <c r="J65" s="25"/>
       <c r="K65" t="s">
         <v>301</v>
       </c>
-      <c r="N65" s="27"/>
+      <c r="N65" s="25"/>
       <c r="O65" t="s">
         <v>337</v>
       </c>
-      <c r="R65" s="27"/>
+      <c r="R65" s="25"/>
       <c r="S65" t="s">
         <v>367</v>
       </c>
-      <c r="V65" s="27"/>
+      <c r="V65" s="25"/>
       <c r="W65" t="s">
         <v>399</v>
       </c>
@@ -4559,27 +4577,27 @@
       <c r="A66" s="1">
         <v>23</v>
       </c>
-      <c r="B66" s="22"/>
+      <c r="B66" s="29"/>
       <c r="C66" t="s">
         <v>61</v>
       </c>
-      <c r="F66" s="22"/>
+      <c r="F66" s="29"/>
       <c r="G66" t="s">
         <v>266</v>
       </c>
-      <c r="J66" s="27"/>
+      <c r="J66" s="25"/>
       <c r="K66" t="s">
         <v>302</v>
       </c>
-      <c r="N66" s="27"/>
+      <c r="N66" s="25"/>
       <c r="O66" t="s">
         <v>338</v>
       </c>
-      <c r="R66" s="27"/>
+      <c r="R66" s="25"/>
       <c r="S66" t="s">
         <v>368</v>
       </c>
-      <c r="V66" s="27"/>
+      <c r="V66" s="25"/>
       <c r="W66" t="s">
         <v>400</v>
       </c>
@@ -4588,29 +4606,29 @@
       <c r="A67" s="1">
         <v>24</v>
       </c>
-      <c r="B67" s="22"/>
+      <c r="B67" s="29"/>
       <c r="C67" t="s">
         <v>267</v>
       </c>
-      <c r="F67" s="22"/>
+      <c r="F67" s="29"/>
       <c r="G67" t="s">
         <v>21</v>
       </c>
-      <c r="J67" s="27"/>
+      <c r="J67" s="25"/>
       <c r="K67" t="s">
         <v>303</v>
       </c>
-      <c r="N67" s="27"/>
+      <c r="N67" s="25"/>
       <c r="O67" t="s">
         <v>342</v>
       </c>
-      <c r="R67" s="26" t="s">
+      <c r="R67" s="24" t="s">
         <v>30</v>
       </c>
       <c r="S67" t="s">
         <v>369</v>
       </c>
-      <c r="V67" s="27"/>
+      <c r="V67" s="25"/>
       <c r="W67" t="s">
         <v>401</v>
       </c>
@@ -4619,33 +4637,33 @@
       <c r="A68" s="1">
         <v>25</v>
       </c>
-      <c r="B68" s="27" t="s">
+      <c r="B68" s="25" t="s">
         <v>24</v>
       </c>
       <c r="C68" t="s">
         <v>102</v>
       </c>
-      <c r="F68" s="27" t="s">
+      <c r="F68" s="25" t="s">
         <v>24</v>
       </c>
       <c r="G68" t="s">
         <v>268</v>
       </c>
-      <c r="J68" s="27"/>
+      <c r="J68" s="25"/>
       <c r="K68" t="s">
         <v>304</v>
       </c>
-      <c r="N68" s="26" t="s">
+      <c r="N68" s="24" t="s">
         <v>30</v>
       </c>
       <c r="O68" t="s">
         <v>339</v>
       </c>
-      <c r="R68" s="26"/>
+      <c r="R68" s="24"/>
       <c r="S68" t="s">
         <v>370</v>
       </c>
-      <c r="V68" s="26" t="s">
+      <c r="V68" s="24" t="s">
         <v>30</v>
       </c>
       <c r="W68" t="s">
@@ -4656,27 +4674,27 @@
       <c r="A69" s="1">
         <v>26</v>
       </c>
-      <c r="B69" s="27"/>
+      <c r="B69" s="25"/>
       <c r="C69" t="s">
         <v>234</v>
       </c>
-      <c r="F69" s="27"/>
+      <c r="F69" s="25"/>
       <c r="G69" t="s">
         <v>269</v>
       </c>
-      <c r="J69" s="27"/>
+      <c r="J69" s="25"/>
       <c r="K69" t="s">
         <v>305</v>
       </c>
-      <c r="N69" s="26"/>
+      <c r="N69" s="24"/>
       <c r="O69" t="s">
         <v>340</v>
       </c>
-      <c r="R69" s="26"/>
+      <c r="R69" s="24"/>
       <c r="S69" t="s">
         <v>371</v>
       </c>
-      <c r="V69" s="26"/>
+      <c r="V69" s="24"/>
       <c r="W69" t="s">
         <v>403</v>
       </c>
@@ -4685,29 +4703,29 @@
       <c r="A70" s="1">
         <v>27</v>
       </c>
-      <c r="B70" s="27"/>
+      <c r="B70" s="25"/>
       <c r="C70" t="s">
         <v>235</v>
       </c>
-      <c r="F70" s="27"/>
+      <c r="F70" s="25"/>
       <c r="G70" t="s">
         <v>270</v>
       </c>
-      <c r="J70" s="26" t="s">
+      <c r="J70" s="24" t="s">
         <v>30</v>
       </c>
       <c r="K70" t="s">
         <v>306</v>
       </c>
-      <c r="N70" s="26"/>
+      <c r="N70" s="24"/>
       <c r="O70" t="s">
         <v>341</v>
       </c>
-      <c r="R70" s="26"/>
+      <c r="R70" s="24"/>
       <c r="S70" t="s">
         <v>372</v>
       </c>
-      <c r="V70" s="26"/>
+      <c r="V70" s="24"/>
       <c r="W70" t="s">
         <v>404</v>
       </c>
@@ -4716,29 +4734,29 @@
       <c r="A71" s="1">
         <v>28</v>
       </c>
-      <c r="B71" s="27"/>
+      <c r="B71" s="25"/>
       <c r="C71" t="s">
         <v>236</v>
       </c>
-      <c r="F71" s="27"/>
+      <c r="F71" s="25"/>
       <c r="G71" t="s">
         <v>101</v>
       </c>
-      <c r="J71" s="26"/>
+      <c r="J71" s="24"/>
       <c r="K71" t="s">
         <v>307</v>
       </c>
-      <c r="N71" s="26"/>
+      <c r="N71" s="24"/>
       <c r="O71" t="s">
         <v>343</v>
       </c>
-      <c r="R71" s="28" t="s">
+      <c r="R71" s="26" t="s">
         <v>36</v>
       </c>
       <c r="S71" t="s">
         <v>373</v>
       </c>
-      <c r="V71" s="26"/>
+      <c r="V71" s="24"/>
       <c r="W71" t="s">
         <v>405</v>
       </c>
@@ -4747,29 +4765,29 @@
       <c r="A72" s="1">
         <v>29</v>
       </c>
-      <c r="B72" s="27"/>
+      <c r="B72" s="25"/>
       <c r="C72" t="s">
         <v>237</v>
       </c>
-      <c r="F72" s="26" t="s">
+      <c r="F72" s="24" t="s">
         <v>30</v>
       </c>
       <c r="G72" t="s">
         <v>272</v>
       </c>
-      <c r="J72" s="26"/>
+      <c r="J72" s="24"/>
       <c r="K72" t="s">
         <v>308</v>
       </c>
-      <c r="N72" s="26"/>
+      <c r="N72" s="24"/>
       <c r="O72" t="s">
         <v>271</v>
       </c>
-      <c r="R72" s="28"/>
+      <c r="R72" s="26"/>
       <c r="S72" t="s">
         <v>374</v>
       </c>
-      <c r="V72" s="26"/>
+      <c r="V72" s="24"/>
       <c r="W72" t="s">
         <v>406</v>
       </c>
@@ -4778,29 +4796,29 @@
       <c r="A73" s="1">
         <v>30</v>
       </c>
-      <c r="B73" s="27"/>
+      <c r="B73" s="25"/>
       <c r="C73" t="s">
         <v>238</v>
       </c>
-      <c r="F73" s="26"/>
+      <c r="F73" s="24"/>
       <c r="G73" t="s">
         <v>273</v>
       </c>
-      <c r="J73" s="26"/>
+      <c r="J73" s="24"/>
       <c r="K73" t="s">
         <v>309</v>
       </c>
-      <c r="N73" s="28" t="s">
+      <c r="N73" s="26" t="s">
         <v>36</v>
       </c>
       <c r="O73" t="s">
         <v>344</v>
       </c>
-      <c r="R73" s="28"/>
+      <c r="R73" s="26"/>
       <c r="S73" t="s">
         <v>375</v>
       </c>
-      <c r="V73" s="28" t="s">
+      <c r="V73" s="26" t="s">
         <v>36</v>
       </c>
       <c r="W73" t="s">
@@ -4808,140 +4826,190 @@
       </c>
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B74" s="26" t="s">
+      <c r="B74" s="24" t="s">
         <v>30</v>
       </c>
       <c r="C74" t="s">
         <v>34</v>
       </c>
-      <c r="F74" s="26"/>
+      <c r="F74" s="24"/>
       <c r="G74" t="s">
         <v>274</v>
       </c>
-      <c r="J74" s="28" t="s">
+      <c r="J74" s="26" t="s">
         <v>36</v>
       </c>
       <c r="K74" t="s">
         <v>310</v>
       </c>
-      <c r="N74" s="28"/>
+      <c r="N74" s="26"/>
       <c r="O74" t="s">
         <v>345</v>
       </c>
-      <c r="R74" s="28"/>
+      <c r="R74" s="26"/>
       <c r="S74" t="s">
         <v>376</v>
       </c>
-      <c r="V74" s="28"/>
+      <c r="V74" s="26"/>
       <c r="W74" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B75" s="26"/>
+      <c r="B75" s="24"/>
       <c r="C75" t="s">
         <v>239</v>
       </c>
-      <c r="F75" s="28" t="s">
+      <c r="F75" s="26" t="s">
         <v>36</v>
       </c>
       <c r="G75" t="s">
         <v>276</v>
       </c>
-      <c r="J75" s="28"/>
+      <c r="J75" s="26"/>
       <c r="K75" t="s">
         <v>311</v>
       </c>
-      <c r="N75" s="28"/>
+      <c r="N75" s="26"/>
       <c r="O75" t="s">
         <v>346</v>
       </c>
-      <c r="R75" s="28"/>
+      <c r="R75" s="26"/>
       <c r="S75" t="s">
         <v>377</v>
       </c>
-      <c r="V75" s="28"/>
+      <c r="V75" s="26"/>
       <c r="W75" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B76" s="26"/>
+      <c r="B76" s="24"/>
       <c r="C76" t="s">
         <v>240</v>
       </c>
-      <c r="F76" s="28"/>
+      <c r="F76" s="26"/>
       <c r="G76" t="s">
         <v>277</v>
       </c>
-      <c r="J76" s="28"/>
+      <c r="J76" s="26"/>
       <c r="K76" t="s">
         <v>312</v>
       </c>
-      <c r="N76" s="28"/>
+      <c r="N76" s="26"/>
       <c r="O76" t="s">
         <v>347</v>
       </c>
-      <c r="V76" s="28"/>
+      <c r="V76" s="26"/>
       <c r="W76" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="77" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B77" s="26"/>
+      <c r="B77" s="24"/>
       <c r="C77" t="s">
         <v>241</v>
       </c>
-      <c r="F77" s="28"/>
+      <c r="F77" s="26"/>
       <c r="G77" t="s">
         <v>278</v>
       </c>
-      <c r="J77" s="28"/>
+      <c r="J77" s="26"/>
       <c r="K77" t="s">
         <v>313</v>
       </c>
-      <c r="V77" s="28"/>
+      <c r="V77" s="26"/>
       <c r="W77" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B78" s="28" t="s">
+      <c r="B78" s="26" t="s">
         <v>36</v>
       </c>
       <c r="C78" t="s">
         <v>109</v>
       </c>
-      <c r="F78" s="28"/>
+      <c r="F78" s="26"/>
       <c r="G78" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B79" s="28"/>
+      <c r="B79" s="26"/>
       <c r="C79" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B80" s="28"/>
+      <c r="B80" s="26"/>
       <c r="C80" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B81" s="28"/>
+      <c r="B81" s="26"/>
       <c r="C81" t="s">
         <v>244</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="85">
+    <mergeCell ref="F63:F67"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="F68:F71"/>
+    <mergeCell ref="B68:B73"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="J4:J9"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="F27:F31"/>
     <mergeCell ref="F72:F74"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="B62:B67"/>
+    <mergeCell ref="F47:F54"/>
+    <mergeCell ref="F55:F62"/>
+    <mergeCell ref="F10:F15"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="R4:R9"/>
+    <mergeCell ref="V73:V77"/>
+    <mergeCell ref="V35:V37"/>
+    <mergeCell ref="R53:R60"/>
+    <mergeCell ref="V26:V29"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="V52:V59"/>
+    <mergeCell ref="V60:V63"/>
+    <mergeCell ref="V64:V67"/>
+    <mergeCell ref="R62:R66"/>
+    <mergeCell ref="V30:V34"/>
+    <mergeCell ref="R48:R52"/>
     <mergeCell ref="N68:N72"/>
-    <mergeCell ref="V2:V4"/>
-    <mergeCell ref="V13:V22"/>
-    <mergeCell ref="J10:J16"/>
+    <mergeCell ref="V68:V72"/>
+    <mergeCell ref="R67:R70"/>
+    <mergeCell ref="R71:R75"/>
+    <mergeCell ref="V23:V25"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="N4:N10"/>
+    <mergeCell ref="N11:N16"/>
+    <mergeCell ref="J27:J30"/>
+    <mergeCell ref="N24:N29"/>
+    <mergeCell ref="N30:N33"/>
+    <mergeCell ref="J44:J46"/>
     <mergeCell ref="B78:B81"/>
     <mergeCell ref="F75:F78"/>
     <mergeCell ref="J70:J73"/>
@@ -4957,71 +5025,21 @@
     <mergeCell ref="N60:N63"/>
     <mergeCell ref="B47:B52"/>
     <mergeCell ref="B53:B61"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="N4:N10"/>
-    <mergeCell ref="N11:N16"/>
+    <mergeCell ref="J47:J49"/>
+    <mergeCell ref="V2:V4"/>
+    <mergeCell ref="V13:V22"/>
+    <mergeCell ref="J10:J16"/>
     <mergeCell ref="R44:R47"/>
-    <mergeCell ref="J27:J30"/>
-    <mergeCell ref="N24:N29"/>
-    <mergeCell ref="N30:N33"/>
     <mergeCell ref="R26:R30"/>
-    <mergeCell ref="J44:J46"/>
-    <mergeCell ref="J47:J49"/>
     <mergeCell ref="R22:R25"/>
     <mergeCell ref="N19:N23"/>
-    <mergeCell ref="V68:V72"/>
-    <mergeCell ref="R67:R70"/>
-    <mergeCell ref="R71:R75"/>
     <mergeCell ref="R31:R34"/>
     <mergeCell ref="V43:Y43"/>
     <mergeCell ref="V44:V46"/>
     <mergeCell ref="V47:V51"/>
-    <mergeCell ref="V52:V59"/>
-    <mergeCell ref="V60:V63"/>
-    <mergeCell ref="V64:V67"/>
-    <mergeCell ref="R62:R66"/>
-    <mergeCell ref="V30:V34"/>
-    <mergeCell ref="R48:R52"/>
-    <mergeCell ref="V73:V77"/>
-    <mergeCell ref="V35:V37"/>
-    <mergeCell ref="R53:R60"/>
-    <mergeCell ref="V26:V29"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="F27:F31"/>
-    <mergeCell ref="V23:V25"/>
     <mergeCell ref="R20:R21"/>
     <mergeCell ref="R10:R19"/>
     <mergeCell ref="V5:V12"/>
-    <mergeCell ref="F10:F15"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="R4:R9"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="F68:F71"/>
-    <mergeCell ref="B68:B73"/>
-    <mergeCell ref="B74:B77"/>
-    <mergeCell ref="B62:B67"/>
-    <mergeCell ref="F47:F54"/>
-    <mergeCell ref="F55:F62"/>
-    <mergeCell ref="F63:F67"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="J4:J9"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="J24:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -5033,7 +5051,7 @@
   <dimension ref="A1:Z50"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5041,7 +5059,7 @@
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.90625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.7265625" customWidth="1"/>
     <col min="10" max="10" width="29" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.26953125" bestFit="1" customWidth="1"/>
@@ -5054,36 +5072,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="E1" s="29" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="E1" s="27" t="s">
         <v>412</v>
       </c>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
       <c r="J1" t="s">
         <v>411</v>
       </c>
-      <c r="O1" s="29" t="s">
+      <c r="O1" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="T1" s="29" t="s">
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="T1" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="X1" s="29" t="s">
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="X1" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -5124,6 +5142,9 @@
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>599</v>
+      </c>
       <c r="B3" t="s">
         <v>500</v>
       </c>
@@ -5152,10 +5173,7 @@
         <v>531</v>
       </c>
       <c r="X3" t="s">
-        <v>593</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>528</v>
+        <v>417</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
@@ -5166,13 +5184,10 @@
         <v>413</v>
       </c>
       <c r="F4" t="s">
-        <v>492</v>
-      </c>
-      <c r="J4" t="s">
-        <v>599</v>
+        <v>491</v>
       </c>
       <c r="K4" t="s">
-        <v>491</v>
+        <v>527</v>
       </c>
       <c r="O4" t="s">
         <v>637</v>
@@ -5187,7 +5202,7 @@
         <v>532</v>
       </c>
       <c r="X4" t="s">
-        <v>603</v>
+        <v>593</v>
       </c>
       <c r="Y4" t="s">
         <v>539</v>
@@ -5213,7 +5228,7 @@
         <v>709</v>
       </c>
       <c r="K5" t="s">
-        <v>538</v>
+        <v>492</v>
       </c>
       <c r="O5" t="s">
         <v>638</v>
@@ -5228,7 +5243,7 @@
         <v>533</v>
       </c>
       <c r="X5" t="s">
-        <v>416</v>
+        <v>603</v>
       </c>
       <c r="Y5" t="s">
         <v>699</v>
@@ -5244,6 +5259,9 @@
       <c r="F6" t="s">
         <v>494</v>
       </c>
+      <c r="K6" t="s">
+        <v>538</v>
+      </c>
       <c r="P6" t="s">
         <v>519</v>
       </c>
@@ -5252,6 +5270,9 @@
       </c>
       <c r="U6" t="s">
         <v>534</v>
+      </c>
+      <c r="X6" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
@@ -5264,19 +5285,22 @@
       <c r="F7" t="s">
         <v>529</v>
       </c>
+      <c r="K7" t="s">
+        <v>668</v>
+      </c>
       <c r="T7" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>527</v>
-      </c>
       <c r="E8" t="s">
         <v>419</v>
       </c>
       <c r="F8" t="s">
         <v>686</v>
+      </c>
+      <c r="K8" t="s">
+        <v>431</v>
       </c>
       <c r="T8" t="s">
         <v>625</v>
@@ -5296,42 +5320,39 @@
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
       <c r="E17" t="s">
         <v>420</v>
       </c>
-      <c r="I17" s="29" t="s">
+      <c r="I17" s="27" t="s">
         <v>421</v>
       </c>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="N17" s="29" t="s">
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="N17" s="27" t="s">
         <v>314</v>
       </c>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
-      <c r="S17" s="29" t="s">
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27"/>
+      <c r="S17" s="27" t="s">
         <v>315</v>
       </c>
-      <c r="T17" s="29"/>
-      <c r="U17" s="29"/>
-      <c r="V17" s="29"/>
+      <c r="T17" s="27"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="27"/>
       <c r="X17" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>417</v>
-      </c>
       <c r="B18" t="s">
-        <v>509</v>
+        <v>528</v>
       </c>
       <c r="E18" t="s">
         <v>594</v>
@@ -5369,7 +5390,7 @@
         <v>596</v>
       </c>
       <c r="B19" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="E19" t="s">
         <v>609</v>
@@ -5407,7 +5428,7 @@
         <v>598</v>
       </c>
       <c r="B20" t="s">
-        <v>700</v>
+        <v>504</v>
       </c>
       <c r="E20" t="s">
         <v>429</v>
@@ -5440,6 +5461,9 @@
     <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>611</v>
+      </c>
+      <c r="B21" t="s">
+        <v>700</v>
       </c>
       <c r="E21" t="s">
         <v>592</v>
@@ -5891,10 +5915,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K262"/>
+  <dimension ref="A1:K270"/>
   <sheetViews>
-    <sheetView topLeftCell="A249" workbookViewId="0">
-      <selection activeCell="C261" sqref="C261"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C267" sqref="C267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7413,6 +7437,52 @@
         <v>740</v>
       </c>
     </row>
+    <row r="263" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A264" s="5" t="s">
+        <v>741</v>
+      </c>
+      <c r="B264" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A265" s="10"/>
+      <c r="B265" s="11" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A266" s="10" t="s">
+        <v>742</v>
+      </c>
+      <c r="B266" s="11" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A267" s="7"/>
+      <c r="B267" s="8" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A269" s="5" t="s">
+        <v>745</v>
+      </c>
+      <c r="B269" s="6" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A270" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="B270" s="8" t="s">
+        <v>599</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
3 Trades including a 3 Team trade
HUGE trades
</commit_message>
<xml_diff>
--- a/OffSeason.xlsx
+++ b/OffSeason.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sdwg-my.sharepoint.com/personal/john_olson_agtegra_com/Documents/Documents 1/Football/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="8_{587C1225-B75F-4676-884C-6424DEF11A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93BC11FB-5A41-4B02-BF93-1DEDC89E1845}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{ECA9F46E-F317-4CC4-8E17-E8E8FEC0C4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B117613A-D9C8-47F2-9CB2-8102E335D0CF}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rosters" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="650">
   <si>
     <t>Vanja Dolas - CeeDee Nuts</t>
   </si>
@@ -1575,9 +1575,6 @@
     <t>2022 5 AlanP</t>
   </si>
   <si>
-    <t>2021 2.7 Andrew</t>
-  </si>
-  <si>
     <t>2022 5 BenL</t>
   </si>
   <si>
@@ -1927,6 +1924,60 @@
   </si>
   <si>
     <t>Benny Snell</t>
+  </si>
+  <si>
+    <t>Brandon</t>
+  </si>
+  <si>
+    <t>2022 1 Alan</t>
+  </si>
+  <si>
+    <t>2022 2 (Vanja)</t>
+  </si>
+  <si>
+    <t>2021 2.8 Andrew</t>
+  </si>
+  <si>
+    <t>3 team trade</t>
+  </si>
+  <si>
+    <t>John Sends</t>
+  </si>
+  <si>
+    <t>JK Dobbins</t>
+  </si>
+  <si>
+    <t>John Receives</t>
+  </si>
+  <si>
+    <t>2021 1.6</t>
+  </si>
+  <si>
+    <t>Jared Receives</t>
+  </si>
+  <si>
+    <t>Jared Sends</t>
+  </si>
+  <si>
+    <t>2022 3 Jared</t>
+  </si>
+  <si>
+    <t>Vanja Sends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 2 MikeR </t>
+  </si>
+  <si>
+    <t>Vanja Receives</t>
+  </si>
+  <si>
+    <t>Kenny Gollady</t>
+  </si>
+  <si>
+    <t>2022 3rd Jared</t>
+  </si>
+  <si>
+    <t>2021 2.8</t>
   </si>
 </sst>
 </file>
@@ -2169,29 +2220,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2578,336 +2629,336 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.54296875" customWidth="1"/>
-    <col min="6" max="6" width="19.1796875" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="10" max="10" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.81640625" customWidth="1"/>
-    <col min="22" max="22" width="22.453125" customWidth="1"/>
-    <col min="23" max="23" width="11.1796875" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.85546875" customWidth="1"/>
+    <col min="22" max="22" width="22.42578125" customWidth="1"/>
+    <col min="23" max="23" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="E1" s="26" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="E1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="26"/>
+      <c r="F1" s="32"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="26"/>
+      <c r="N1" s="32"/>
       <c r="O1" s="1"/>
-      <c r="Q1" s="26" t="s">
+      <c r="Q1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="26"/>
+      <c r="R1" s="32"/>
       <c r="S1" s="1"/>
-      <c r="U1" s="26" t="s">
+      <c r="U1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="26"/>
+      <c r="V1" s="32"/>
       <c r="W1" s="1"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="M2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="N2" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="27" t="s">
+      <c r="Q2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="R2" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="27" t="s">
+      <c r="U2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="V2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A3" s="27"/>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="25"/>
       <c r="B3" t="s">
         <v>209</v>
       </c>
-      <c r="E3" s="27"/>
+      <c r="E3" s="25"/>
       <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="27"/>
+      <c r="I3" s="25"/>
       <c r="J3" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="27"/>
+      <c r="M3" s="25"/>
       <c r="N3" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="27"/>
+      <c r="Q3" s="25"/>
       <c r="R3" t="s">
         <v>17</v>
       </c>
-      <c r="U3" s="27"/>
+      <c r="U3" s="25"/>
       <c r="V3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A4" s="25" t="s">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="28" t="s">
         <v>20</v>
       </c>
       <c r="J4" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="27"/>
+      <c r="M4" s="25"/>
       <c r="N4" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" s="27"/>
+      <c r="Q4" s="25"/>
       <c r="R4" t="s">
         <v>24</v>
       </c>
-      <c r="U4" s="27"/>
+      <c r="U4" s="25"/>
       <c r="V4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A5" s="25"/>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
       <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="28"/>
       <c r="F5" t="s">
         <v>227</v>
       </c>
-      <c r="I5" s="25"/>
+      <c r="I5" s="28"/>
       <c r="J5" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="25" t="s">
+      <c r="M5" s="28" t="s">
         <v>20</v>
       </c>
       <c r="N5" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="25" t="s">
+      <c r="Q5" s="28" t="s">
         <v>20</v>
       </c>
       <c r="R5" t="s">
         <v>30</v>
       </c>
-      <c r="U5" s="25" t="s">
+      <c r="U5" s="28" t="s">
         <v>20</v>
       </c>
       <c r="V5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A6" s="25"/>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
       <c r="B6" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="28"/>
       <c r="F6" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="25"/>
+      <c r="I6" s="28"/>
       <c r="J6" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="25"/>
+      <c r="M6" s="28"/>
       <c r="N6" t="s">
         <v>35</v>
       </c>
-      <c r="Q6" s="25"/>
+      <c r="Q6" s="28"/>
       <c r="R6" t="s">
         <v>36</v>
       </c>
-      <c r="U6" s="25"/>
+      <c r="U6" s="28"/>
       <c r="V6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A7" s="25"/>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
       <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="28"/>
       <c r="F7" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="25"/>
+      <c r="I7" s="28"/>
       <c r="J7" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="25"/>
+      <c r="M7" s="28"/>
       <c r="N7" t="s">
         <v>41</v>
       </c>
-      <c r="Q7" s="25"/>
+      <c r="Q7" s="28"/>
       <c r="R7" t="s">
         <v>42</v>
       </c>
-      <c r="U7" s="25"/>
+      <c r="U7" s="28"/>
       <c r="V7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>44</v>
       </c>
       <c r="B8" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="25"/>
+      <c r="E8" s="28"/>
       <c r="F8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="I8" s="28"/>
       <c r="J8" t="s">
         <v>47</v>
       </c>
-      <c r="M8" s="25"/>
+      <c r="M8" s="28"/>
       <c r="N8" t="s">
         <v>48</v>
       </c>
-      <c r="Q8" s="25"/>
+      <c r="Q8" s="28"/>
       <c r="R8" t="s">
         <v>49</v>
       </c>
-      <c r="U8" s="25"/>
+      <c r="U8" s="28"/>
       <c r="V8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="30"/>
       <c r="B9" t="s">
-        <v>294</v>
-      </c>
-      <c r="E9" s="25"/>
+        <v>51</v>
+      </c>
+      <c r="E9" s="28"/>
       <c r="F9" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9" s="25"/>
+        <v>58</v>
+      </c>
+      <c r="I9" s="28"/>
       <c r="J9" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="25"/>
+      <c r="M9" s="28"/>
       <c r="N9" t="s">
         <v>54</v>
       </c>
-      <c r="Q9" s="25"/>
+      <c r="Q9" s="28"/>
       <c r="R9" t="s">
         <v>55</v>
       </c>
-      <c r="U9" s="25"/>
+      <c r="U9" s="28"/>
       <c r="V9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="30"/>
       <c r="B10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="25"/>
+        <v>281</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>44</v>
+      </c>
       <c r="F10" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="25"/>
+        <v>64</v>
+      </c>
+      <c r="I10" s="28"/>
       <c r="J10" t="s">
         <v>59</v>
       </c>
-      <c r="M10" s="25"/>
+      <c r="M10" s="28"/>
       <c r="N10" t="s">
         <v>60</v>
       </c>
-      <c r="Q10" s="25"/>
+      <c r="Q10" s="28"/>
       <c r="R10" t="s">
         <v>61</v>
       </c>
-      <c r="U10" s="25"/>
+      <c r="U10" s="28"/>
       <c r="V10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="30"/>
       <c r="B11" t="s">
-        <v>281</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>44</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="E11" s="30"/>
       <c r="F11" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" s="25"/>
+        <v>70</v>
+      </c>
+      <c r="I11" s="28"/>
       <c r="J11" t="s">
         <v>65</v>
       </c>
-      <c r="M11" s="25"/>
+      <c r="M11" s="28"/>
       <c r="N11" t="s">
         <v>66</v>
       </c>
-      <c r="Q11" s="25"/>
+      <c r="Q11" s="28"/>
       <c r="R11" t="s">
         <v>67</v>
       </c>
@@ -2918,14 +2969,14 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="30"/>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="I12" s="30" t="s">
         <v>44</v>
@@ -2950,14 +3001,14 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="30"/>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>270</v>
       </c>
       <c r="E13" s="30"/>
       <c r="F13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="I13" s="30"/>
       <c r="J13" t="s">
@@ -2976,14 +3027,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="30"/>
       <c r="B14" t="s">
         <v>81</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="I14" s="30"/>
       <c r="J14" t="s">
@@ -3002,14 +3053,14 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="30"/>
       <c r="B15" t="s">
         <v>87</v>
       </c>
       <c r="E15" s="30"/>
       <c r="F15" t="s">
-        <v>95</v>
+        <v>294</v>
       </c>
       <c r="I15" s="30"/>
       <c r="J15" t="s">
@@ -3028,14 +3079,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A16" s="32" t="s">
-        <v>93</v>
-      </c>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="30"/>
       <c r="B16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E16" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="E16" s="31" t="s">
         <v>93</v>
       </c>
       <c r="F16" t="s">
@@ -3058,12 +3107,14 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A17" s="32"/>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
+        <v>93</v>
+      </c>
       <c r="B17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E17" s="32"/>
+        <v>94</v>
+      </c>
+      <c r="E17" s="31"/>
       <c r="F17" t="s">
         <v>107</v>
       </c>
@@ -3084,12 +3135,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A18" s="32"/>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="31"/>
       <c r="B18" t="s">
-        <v>106</v>
-      </c>
-      <c r="E18" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="29" t="s">
         <v>113</v>
       </c>
       <c r="F18" t="s">
@@ -3112,12 +3163,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A19" s="32"/>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="31"/>
       <c r="B19" t="s">
-        <v>112</v>
-      </c>
-      <c r="E19" s="31"/>
+        <v>106</v>
+      </c>
+      <c r="E19" s="29"/>
       <c r="F19" t="s">
         <v>126</v>
       </c>
@@ -3125,33 +3176,29 @@
       <c r="J19" t="s">
         <v>115</v>
       </c>
-      <c r="M19" s="32" t="s">
-        <v>93</v>
-      </c>
+      <c r="M19" s="30"/>
       <c r="N19" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q19" s="32" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q19" s="31" t="s">
         <v>93</v>
       </c>
       <c r="R19" t="s">
         <v>117</v>
       </c>
-      <c r="U19" s="32" t="s">
+      <c r="U19" s="31" t="s">
         <v>93</v>
       </c>
       <c r="V19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A20" s="31" t="s">
-        <v>113</v>
-      </c>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="31"/>
       <c r="B20" t="s">
-        <v>119</v>
-      </c>
-      <c r="E20" s="31"/>
+        <v>112</v>
+      </c>
+      <c r="E20" s="29"/>
       <c r="F20" t="s">
         <v>132</v>
       </c>
@@ -3161,413 +3208,417 @@
       <c r="J20" t="s">
         <v>121</v>
       </c>
-      <c r="M20" s="32"/>
+      <c r="M20" s="31" t="s">
+        <v>93</v>
+      </c>
       <c r="N20" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q20" s="32"/>
+        <v>116</v>
+      </c>
+      <c r="Q20" s="31"/>
       <c r="R20" t="s">
         <v>123</v>
       </c>
-      <c r="U20" s="32"/>
+      <c r="U20" s="31"/>
       <c r="V20" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A21" s="31"/>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>113</v>
+      </c>
       <c r="B21" t="s">
-        <v>131</v>
-      </c>
-      <c r="E21" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="27" t="s">
         <v>137</v>
       </c>
       <c r="F21" t="s">
         <v>139</v>
       </c>
-      <c r="I21" s="31" t="s">
+      <c r="I21" s="29" t="s">
         <v>113</v>
       </c>
       <c r="J21" t="s">
         <v>127</v>
       </c>
-      <c r="M21" s="32"/>
+      <c r="M21" s="31"/>
       <c r="N21" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q21" s="32"/>
+        <v>122</v>
+      </c>
+      <c r="Q21" s="31"/>
       <c r="R21" t="s">
         <v>129</v>
       </c>
-      <c r="U21" s="31" t="s">
+      <c r="U21" s="29" t="s">
         <v>113</v>
       </c>
       <c r="V21" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A22" s="31"/>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="29"/>
       <c r="B22" t="s">
-        <v>114</v>
-      </c>
-      <c r="E22" s="28"/>
+        <v>131</v>
+      </c>
+      <c r="E22" s="27"/>
       <c r="F22" t="s">
         <v>145</v>
       </c>
-      <c r="I22" s="31"/>
+      <c r="I22" s="29"/>
       <c r="J22" t="s">
         <v>133</v>
       </c>
-      <c r="M22" s="32"/>
+      <c r="M22" s="31"/>
       <c r="N22" t="s">
         <v>134</v>
       </c>
-      <c r="Q22" s="31" t="s">
+      <c r="Q22" s="29" t="s">
         <v>113</v>
       </c>
       <c r="R22" t="s">
         <v>135</v>
       </c>
-      <c r="U22" s="31"/>
+      <c r="U22" s="29"/>
       <c r="V22" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A23" s="28" t="s">
-        <v>137</v>
-      </c>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="29"/>
       <c r="B23" t="s">
-        <v>138</v>
-      </c>
-      <c r="E23" s="28"/>
+        <v>114</v>
+      </c>
+      <c r="E23" s="27"/>
       <c r="F23" t="s">
         <v>151</v>
       </c>
-      <c r="I23" s="31"/>
+      <c r="I23" s="29"/>
       <c r="J23" t="s">
         <v>140</v>
       </c>
-      <c r="M23" s="31" t="s">
+      <c r="M23" s="29" t="s">
         <v>113</v>
       </c>
       <c r="N23" t="s">
         <v>141</v>
       </c>
-      <c r="Q23" s="31"/>
+      <c r="Q23" s="29"/>
       <c r="R23" t="s">
         <v>142</v>
       </c>
-      <c r="U23" s="31"/>
+      <c r="U23" s="29"/>
       <c r="V23" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A24" s="28"/>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
+        <v>137</v>
+      </c>
       <c r="B24" t="s">
-        <v>144</v>
-      </c>
-      <c r="E24" s="28"/>
+        <v>138</v>
+      </c>
+      <c r="E24" s="27"/>
       <c r="F24" t="s">
         <v>157</v>
       </c>
-      <c r="I24" s="31"/>
+      <c r="I24" s="29"/>
       <c r="J24" t="s">
         <v>146</v>
       </c>
-      <c r="M24" s="31"/>
+      <c r="M24" s="29"/>
       <c r="N24" t="s">
         <v>147</v>
       </c>
-      <c r="Q24" s="31"/>
+      <c r="Q24" s="29"/>
       <c r="R24" t="s">
         <v>148</v>
       </c>
-      <c r="U24" s="31"/>
+      <c r="U24" s="29"/>
       <c r="V24" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A25" s="28"/>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="27"/>
       <c r="B25" t="s">
-        <v>150</v>
-      </c>
-      <c r="E25" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="E25" s="26" t="s">
         <v>167</v>
       </c>
       <c r="F25" t="s">
         <v>169</v>
       </c>
-      <c r="I25" s="28" t="s">
+      <c r="I25" s="27" t="s">
         <v>137</v>
       </c>
       <c r="J25" t="s">
         <v>152</v>
       </c>
-      <c r="M25" s="31"/>
+      <c r="M25" s="29"/>
       <c r="N25" t="s">
         <v>153</v>
       </c>
-      <c r="Q25" s="31"/>
+      <c r="Q25" s="29"/>
       <c r="R25" t="s">
         <v>154</v>
       </c>
-      <c r="U25" s="28" t="s">
+      <c r="U25" s="27" t="s">
         <v>137</v>
       </c>
       <c r="V25" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A26" s="28"/>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="27"/>
       <c r="B26" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="29"/>
+        <v>150</v>
+      </c>
+      <c r="E26" s="26"/>
       <c r="F26" t="s">
         <v>175</v>
       </c>
-      <c r="I26" s="28"/>
+      <c r="I26" s="27"/>
       <c r="J26" t="s">
         <v>158</v>
       </c>
-      <c r="M26" s="28" t="s">
+      <c r="M26" s="27" t="s">
         <v>137</v>
       </c>
       <c r="N26" t="s">
         <v>159</v>
       </c>
-      <c r="Q26" s="28" t="s">
+      <c r="Q26" s="27" t="s">
         <v>137</v>
       </c>
       <c r="R26" t="s">
         <v>160</v>
       </c>
-      <c r="U26" s="28"/>
+      <c r="U26" s="27"/>
       <c r="V26" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A27" s="29" t="s">
-        <v>167</v>
-      </c>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="27"/>
       <c r="B27" t="s">
-        <v>193</v>
-      </c>
-      <c r="E27" s="29"/>
+        <v>9</v>
+      </c>
+      <c r="E27" s="26"/>
       <c r="F27" t="s">
         <v>181</v>
       </c>
-      <c r="I27" s="28"/>
+      <c r="I27" s="27"/>
       <c r="J27" t="s">
         <v>163</v>
       </c>
-      <c r="M27" s="28"/>
+      <c r="M27" s="27"/>
       <c r="N27" t="s">
         <v>164</v>
       </c>
-      <c r="Q27" s="28"/>
+      <c r="Q27" s="27"/>
       <c r="R27" t="s">
         <v>165</v>
       </c>
-      <c r="U27" s="28"/>
+      <c r="U27" s="27"/>
       <c r="V27" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A28" s="29"/>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
+        <v>167</v>
+      </c>
       <c r="B28" t="s">
-        <v>174</v>
-      </c>
-      <c r="E28" s="29"/>
-      <c r="F28" t="s">
-        <v>187</v>
-      </c>
-      <c r="I28" s="28"/>
+        <v>193</v>
+      </c>
+      <c r="I28" s="27"/>
       <c r="J28" t="s">
         <v>170</v>
       </c>
-      <c r="M28" s="28"/>
+      <c r="M28" s="27"/>
       <c r="N28" t="s">
         <v>171</v>
       </c>
-      <c r="Q28" s="28"/>
+      <c r="Q28" s="27"/>
       <c r="R28" t="s">
         <v>172</v>
       </c>
-      <c r="U28" s="28"/>
+      <c r="U28" s="27"/>
       <c r="V28" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A29" s="29"/>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="26"/>
       <c r="B29" t="s">
-        <v>192</v>
-      </c>
-      <c r="I29" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="I29" s="26" t="s">
         <v>167</v>
       </c>
       <c r="J29" t="s">
         <v>176</v>
       </c>
-      <c r="M29" s="28"/>
+      <c r="M29" s="27"/>
       <c r="N29" t="s">
         <v>177</v>
       </c>
-      <c r="Q29" s="28"/>
+      <c r="Q29" s="27"/>
       <c r="R29" t="s">
         <v>178</v>
       </c>
-      <c r="U29" s="29" t="s">
+      <c r="U29" s="26" t="s">
         <v>167</v>
       </c>
       <c r="V29" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A30" s="29"/>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
       <c r="B30" t="s">
-        <v>180</v>
-      </c>
-      <c r="I30" s="29"/>
+        <v>192</v>
+      </c>
+      <c r="I30" s="26"/>
       <c r="J30" t="s">
         <v>182</v>
       </c>
-      <c r="M30" s="29" t="s">
+      <c r="M30" s="26" t="s">
         <v>167</v>
       </c>
       <c r="N30" t="s">
         <v>183</v>
       </c>
-      <c r="Q30" s="29" t="s">
+      <c r="Q30" s="26" t="s">
         <v>167</v>
       </c>
       <c r="R30" t="s">
         <v>184</v>
       </c>
-      <c r="U30" s="29"/>
+      <c r="U30" s="26"/>
       <c r="V30" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A31" s="29"/>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="26"/>
       <c r="B31" t="s">
-        <v>186</v>
-      </c>
-      <c r="I31" s="29"/>
+        <v>180</v>
+      </c>
+      <c r="I31" s="26"/>
       <c r="J31" t="s">
         <v>188</v>
       </c>
-      <c r="M31" s="29"/>
+      <c r="M31" s="26"/>
       <c r="N31" t="s">
         <v>189</v>
       </c>
-      <c r="Q31" s="29"/>
+      <c r="Q31" s="26"/>
       <c r="R31" t="s">
         <v>190</v>
       </c>
-      <c r="U31" s="29"/>
+      <c r="U31" s="26"/>
       <c r="V31" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A32" s="29"/>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" s="26"/>
       <c r="B32" t="s">
-        <v>168</v>
-      </c>
-      <c r="I32" s="29"/>
+        <v>186</v>
+      </c>
+      <c r="I32" s="26"/>
       <c r="J32" t="s">
         <v>194</v>
       </c>
-      <c r="M32" s="29"/>
+      <c r="M32" s="26"/>
       <c r="N32" t="s">
         <v>195</v>
       </c>
-      <c r="Q32" s="29"/>
+      <c r="Q32" s="26"/>
       <c r="R32" t="s">
         <v>196</v>
       </c>
-      <c r="U32" s="29"/>
+      <c r="U32" s="26"/>
       <c r="V32" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="I33" s="29"/>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33" s="26"/>
+      <c r="B33" t="s">
+        <v>168</v>
+      </c>
+      <c r="I33" s="26"/>
       <c r="J33" t="s">
         <v>198</v>
       </c>
-      <c r="M33" s="29"/>
+      <c r="M33" s="26"/>
       <c r="N33" t="s">
         <v>199</v>
       </c>
-      <c r="Q33" s="29"/>
+      <c r="Q33" s="26"/>
       <c r="R33" t="s">
         <v>200</v>
       </c>
-      <c r="U33" s="29"/>
+      <c r="U33" s="26"/>
       <c r="V33" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="Q34" s="29"/>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q34" s="26"/>
       <c r="R34" t="s">
         <v>202</v>
       </c>
       <c r="U34" s="3"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A40" s="26" t="s">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A40" s="32" t="s">
         <v>203</v>
       </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="E40" s="26" t="s">
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="E40" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
-      <c r="I40" s="26" t="s">
-        <v>606</v>
-      </c>
-      <c r="J40" s="26"/>
-      <c r="K40" s="26"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="I40" s="32" t="s">
+        <v>605</v>
+      </c>
+      <c r="J40" s="32"/>
+      <c r="K40" s="32"/>
       <c r="L40" s="1"/>
-      <c r="M40" s="26" t="s">
+      <c r="M40" s="32" t="s">
         <v>205</v>
       </c>
-      <c r="N40" s="26"/>
+      <c r="N40" s="32"/>
       <c r="O40" s="1"/>
-      <c r="Q40" s="26" t="s">
+      <c r="Q40" s="32" t="s">
         <v>206</v>
       </c>
-      <c r="R40" s="26"/>
+      <c r="R40" s="32"/>
       <c r="S40" s="1"/>
-      <c r="U40" s="26" t="s">
+      <c r="U40" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="V40" s="26"/>
+      <c r="V40" s="32"/>
       <c r="W40" s="1"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A41" s="27" t="s">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A41" s="25" t="s">
         <v>6</v>
       </c>
       <c r="B41" t="s">
         <v>208</v>
       </c>
-      <c r="E41" s="27" t="s">
+      <c r="E41" s="25" t="s">
         <v>6</v>
       </c>
       <c r="F41" t="s">
@@ -3579,265 +3630,265 @@
       <c r="J41" t="s">
         <v>216</v>
       </c>
-      <c r="M41" s="27" t="s">
+      <c r="M41" s="25" t="s">
         <v>6</v>
       </c>
       <c r="N41" t="s">
         <v>211</v>
       </c>
-      <c r="Q41" s="27" t="s">
+      <c r="Q41" s="25" t="s">
         <v>6</v>
       </c>
       <c r="R41" t="s">
         <v>212</v>
       </c>
-      <c r="U41" s="27" t="s">
+      <c r="U41" s="25" t="s">
         <v>6</v>
       </c>
       <c r="V41" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A42" s="27"/>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A42" s="25"/>
       <c r="B42" t="s">
         <v>214</v>
       </c>
-      <c r="E42" s="27"/>
+      <c r="E42" s="25"/>
       <c r="F42" t="s">
         <v>19</v>
       </c>
-      <c r="I42" s="25" t="s">
+      <c r="I42" s="28" t="s">
         <v>20</v>
       </c>
       <c r="J42" t="s">
         <v>222</v>
       </c>
-      <c r="M42" s="27"/>
+      <c r="M42" s="25"/>
       <c r="N42" t="s">
         <v>217</v>
       </c>
-      <c r="Q42" s="27"/>
+      <c r="Q42" s="25"/>
       <c r="R42" t="s">
         <v>218</v>
       </c>
-      <c r="U42" s="27"/>
+      <c r="U42" s="25"/>
       <c r="V42" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A43" s="27"/>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A43" s="25"/>
       <c r="B43" t="s">
         <v>220</v>
       </c>
-      <c r="E43" s="27"/>
+      <c r="E43" s="25"/>
       <c r="F43" t="s">
         <v>215</v>
       </c>
-      <c r="I43" s="25"/>
+      <c r="I43" s="28"/>
       <c r="J43" t="s">
-        <v>245</v>
-      </c>
-      <c r="M43" s="27"/>
+        <v>46</v>
+      </c>
+      <c r="M43" s="25"/>
       <c r="N43" t="s">
         <v>223</v>
       </c>
-      <c r="Q43" s="25" t="s">
+      <c r="Q43" s="28" t="s">
         <v>20</v>
       </c>
       <c r="R43" t="s">
         <v>224</v>
       </c>
-      <c r="U43" s="27"/>
+      <c r="U43" s="25"/>
       <c r="V43" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A44" s="25" t="s">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A44" s="28" t="s">
         <v>20</v>
       </c>
       <c r="B44" t="s">
         <v>226</v>
       </c>
-      <c r="E44" s="27"/>
+      <c r="E44" s="25"/>
       <c r="F44" t="s">
         <v>221</v>
       </c>
-      <c r="I44" s="25"/>
+      <c r="I44" s="28"/>
       <c r="J44" t="s">
-        <v>234</v>
-      </c>
-      <c r="M44" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="M44" s="28" t="s">
         <v>20</v>
       </c>
       <c r="N44" t="s">
         <v>229</v>
       </c>
-      <c r="Q44" s="25"/>
+      <c r="Q44" s="28"/>
       <c r="R44" t="s">
         <v>230</v>
       </c>
-      <c r="U44" s="25" t="s">
+      <c r="U44" s="28" t="s">
         <v>20</v>
       </c>
       <c r="V44" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A45" s="25"/>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A45" s="28"/>
       <c r="B45" t="s">
-        <v>232</v>
-      </c>
-      <c r="E45" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="E45" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F45" t="s">
-        <v>233</v>
-      </c>
-      <c r="I45" s="25"/>
+        <v>239</v>
+      </c>
+      <c r="I45" s="28"/>
       <c r="J45" t="s">
-        <v>246</v>
-      </c>
-      <c r="M45" s="25"/>
+        <v>234</v>
+      </c>
+      <c r="M45" s="28"/>
       <c r="N45" t="s">
         <v>235</v>
       </c>
-      <c r="Q45" s="25"/>
+      <c r="Q45" s="28"/>
       <c r="R45" t="s">
         <v>236</v>
       </c>
-      <c r="U45" s="25"/>
+      <c r="U45" s="28"/>
       <c r="V45" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A46" s="25"/>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A46" s="28"/>
       <c r="B46" t="s">
-        <v>238</v>
-      </c>
-      <c r="E46" s="25"/>
+        <v>232</v>
+      </c>
+      <c r="E46" s="28"/>
       <c r="F46" t="s">
-        <v>239</v>
-      </c>
-      <c r="I46" s="25"/>
+        <v>251</v>
+      </c>
+      <c r="I46" s="28"/>
       <c r="J46" t="s">
         <v>252</v>
       </c>
-      <c r="M46" s="25"/>
+      <c r="M46" s="28"/>
       <c r="N46" t="s">
         <v>241</v>
       </c>
-      <c r="Q46" s="25"/>
+      <c r="Q46" s="28"/>
       <c r="R46" t="s">
         <v>242</v>
       </c>
-      <c r="U46" s="25"/>
+      <c r="U46" s="28"/>
       <c r="V46" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A47" s="25"/>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A47" s="28"/>
       <c r="B47" t="s">
-        <v>244</v>
-      </c>
-      <c r="E47" s="25"/>
+        <v>238</v>
+      </c>
+      <c r="E47" s="28"/>
       <c r="F47" t="s">
-        <v>251</v>
-      </c>
-      <c r="I47" s="25"/>
+        <v>257</v>
+      </c>
+      <c r="I47" s="28"/>
       <c r="J47" t="s">
         <v>258</v>
       </c>
-      <c r="M47" s="25"/>
+      <c r="M47" s="28"/>
       <c r="N47" t="s">
         <v>247</v>
       </c>
-      <c r="Q47" s="25"/>
+      <c r="Q47" s="28"/>
       <c r="R47" t="s">
         <v>248</v>
       </c>
-      <c r="U47" s="25"/>
+      <c r="U47" s="28"/>
       <c r="V47" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A48" s="25"/>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A48" s="28"/>
       <c r="B48" t="s">
-        <v>250</v>
-      </c>
-      <c r="E48" s="25"/>
+        <v>244</v>
+      </c>
+      <c r="E48" s="28"/>
       <c r="F48" t="s">
-        <v>257</v>
-      </c>
-      <c r="I48" s="25"/>
+        <v>263</v>
+      </c>
+      <c r="I48" s="28"/>
       <c r="J48" t="s">
         <v>264</v>
       </c>
-      <c r="M48" s="25"/>
+      <c r="M48" s="28"/>
       <c r="N48" t="s">
         <v>253</v>
       </c>
-      <c r="Q48" s="25"/>
+      <c r="Q48" s="28"/>
       <c r="R48" t="s">
         <v>254</v>
       </c>
-      <c r="U48" s="25"/>
+      <c r="U48" s="28"/>
       <c r="V48" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A49" s="25"/>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A49" s="28"/>
       <c r="B49" t="s">
-        <v>256</v>
-      </c>
-      <c r="E49" s="25"/>
+        <v>250</v>
+      </c>
+      <c r="E49" s="28"/>
       <c r="F49" t="s">
-        <v>263</v>
-      </c>
-      <c r="I49" s="25"/>
+        <v>240</v>
+      </c>
+      <c r="I49" s="28"/>
       <c r="J49" t="s">
         <v>228</v>
       </c>
-      <c r="M49" s="25"/>
+      <c r="M49" s="28"/>
       <c r="N49" t="s">
         <v>259</v>
       </c>
-      <c r="Q49" s="25"/>
+      <c r="Q49" s="28"/>
       <c r="R49" t="s">
         <v>260</v>
       </c>
-      <c r="U49" s="25"/>
+      <c r="U49" s="28"/>
       <c r="V49" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A50" s="25"/>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A50" s="28"/>
       <c r="B50" t="s">
-        <v>262</v>
-      </c>
-      <c r="E50" s="25"/>
+        <v>256</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>44</v>
+      </c>
       <c r="F50" t="s">
-        <v>240</v>
-      </c>
-      <c r="I50" s="30" t="s">
-        <v>44</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="I50" s="28"/>
       <c r="J50" t="s">
-        <v>76</v>
-      </c>
-      <c r="M50" s="25"/>
+        <v>246</v>
+      </c>
+      <c r="M50" s="28"/>
       <c r="N50" t="s">
         <v>265</v>
       </c>
-      <c r="Q50" s="25"/>
+      <c r="Q50" s="28"/>
       <c r="R50" t="s">
         <v>266</v>
       </c>
@@ -3848,22 +3899,20 @@
         <v>261</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A51" s="30" t="s">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A51" s="28"/>
+      <c r="B51" t="s">
+        <v>262</v>
+      </c>
+      <c r="E51" s="30"/>
+      <c r="F51" t="s">
+        <v>275</v>
+      </c>
+      <c r="I51" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B51" t="s">
-        <v>268</v>
-      </c>
-      <c r="E51" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="F51" t="s">
-        <v>269</v>
-      </c>
-      <c r="I51" s="30"/>
       <c r="J51" t="s">
-        <v>276</v>
+        <v>76</v>
       </c>
       <c r="M51" s="30" t="s">
         <v>44</v>
@@ -3882,22 +3931,22 @@
         <v>267</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A52" s="30"/>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A52" s="30" t="s">
+        <v>44</v>
+      </c>
       <c r="B52" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E52" s="30"/>
       <c r="F52" t="s">
-        <v>275</v>
+        <v>63</v>
       </c>
       <c r="I52" s="30"/>
       <c r="J52" t="s">
-        <v>300</v>
-      </c>
-      <c r="M52" s="30" t="s">
-        <v>44</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="M52" s="30"/>
       <c r="N52" t="s">
         <v>277</v>
       </c>
@@ -3910,22 +3959,20 @@
         <v>273</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="30"/>
       <c r="B53" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="E53" s="30"/>
       <c r="F53" t="s">
-        <v>63</v>
+        <v>287</v>
       </c>
       <c r="I53" s="30"/>
       <c r="J53" t="s">
-        <v>51</v>
-      </c>
-      <c r="M53" s="30" t="s">
-        <v>44</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="M53" s="30"/>
       <c r="N53" t="s">
         <v>283</v>
       </c>
@@ -3938,22 +3985,20 @@
         <v>279</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="30"/>
       <c r="B54" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E54" s="30"/>
       <c r="F54" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="I54" s="30"/>
       <c r="J54" t="s">
         <v>288</v>
       </c>
-      <c r="M54" s="30" t="s">
-        <v>44</v>
-      </c>
+      <c r="M54" s="30"/>
       <c r="N54" t="s">
         <v>289</v>
       </c>
@@ -3966,22 +4011,20 @@
         <v>285</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="30"/>
       <c r="B55" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="E55" s="30"/>
       <c r="F55" t="s">
-        <v>293</v>
+        <v>312</v>
       </c>
       <c r="I55" s="30"/>
       <c r="J55" t="s">
-        <v>282</v>
-      </c>
-      <c r="M55" s="30" t="s">
-        <v>44</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="M55" s="30"/>
       <c r="N55" t="s">
         <v>295</v>
       </c>
@@ -3994,24 +4037,22 @@
         <v>291</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="30"/>
       <c r="B56" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="E56" s="30"/>
       <c r="F56" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I56" s="30"/>
       <c r="J56" t="s">
-        <v>306</v>
-      </c>
-      <c r="M56" s="30" t="s">
-        <v>44</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="M56" s="30"/>
       <c r="N56" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="Q56" s="30"/>
       <c r="R56" t="s">
@@ -4022,24 +4063,24 @@
         <v>297</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="30"/>
       <c r="B57" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="E57" s="30"/>
       <c r="F57" t="s">
-        <v>305</v>
-      </c>
-      <c r="I57" s="30"/>
+        <v>317</v>
+      </c>
+      <c r="I57" s="31" t="s">
+        <v>93</v>
+      </c>
       <c r="J57" t="s">
-        <v>270</v>
-      </c>
-      <c r="M57" s="30" t="s">
-        <v>44</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="M57" s="30"/>
       <c r="N57" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="Q57" s="30"/>
       <c r="R57" t="s">
@@ -4050,24 +4091,24 @@
         <v>303</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="30"/>
       <c r="B58" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="E58" s="30"/>
       <c r="F58" t="s">
-        <v>311</v>
-      </c>
-      <c r="I58" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="I58" s="31"/>
+      <c r="J58" t="s">
+        <v>353</v>
+      </c>
+      <c r="M58" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="J58" t="s">
-        <v>318</v>
-      </c>
-      <c r="M58" s="30"/>
       <c r="N58" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="Q58" s="30"/>
       <c r="R58" t="s">
@@ -4078,24 +4119,22 @@
         <v>309</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="30"/>
       <c r="B59" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="E59" s="30"/>
       <c r="F59" t="s">
-        <v>317</v>
-      </c>
-      <c r="I59" s="32"/>
+        <v>329</v>
+      </c>
+      <c r="I59" s="31"/>
       <c r="J59" t="s">
-        <v>353</v>
-      </c>
-      <c r="M59" s="32" t="s">
-        <v>93</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="M59" s="31"/>
       <c r="N59" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="Q59" s="30"/>
       <c r="R59" t="s">
@@ -4106,76 +4145,78 @@
         <v>315</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" s="30"/>
       <c r="B60" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="E60" s="30"/>
       <c r="F60" t="s">
-        <v>323</v>
-      </c>
-      <c r="I60" s="32"/>
+        <v>335</v>
+      </c>
+      <c r="I60" s="31"/>
       <c r="J60" t="s">
-        <v>330</v>
-      </c>
-      <c r="M60" s="32"/>
+        <v>336</v>
+      </c>
+      <c r="M60" s="31"/>
       <c r="N60" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="Q60" s="30"/>
       <c r="R60" t="s">
         <v>326</v>
       </c>
-      <c r="U60" s="32" t="s">
+      <c r="U60" s="31" t="s">
         <v>93</v>
       </c>
       <c r="V60" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A61" s="32" t="s">
-        <v>93</v>
-      </c>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A61" s="30"/>
       <c r="B61" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="E61" s="30"/>
       <c r="F61" t="s">
-        <v>329</v>
-      </c>
-      <c r="I61" s="32"/>
+        <v>299</v>
+      </c>
+      <c r="I61" s="31"/>
       <c r="J61" t="s">
-        <v>336</v>
-      </c>
-      <c r="M61" s="32"/>
+        <v>324</v>
+      </c>
+      <c r="M61" s="31"/>
       <c r="N61" t="s">
-        <v>331</v>
+        <v>128</v>
       </c>
       <c r="Q61" s="30"/>
       <c r="R61" t="s">
         <v>332</v>
       </c>
-      <c r="U61" s="32"/>
+      <c r="U61" s="31"/>
       <c r="V61" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A62" s="32"/>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A62" s="30"/>
       <c r="B62" t="s">
-        <v>334</v>
-      </c>
-      <c r="E62" s="30"/>
+        <v>305</v>
+      </c>
+      <c r="E62" s="31" t="s">
+        <v>93</v>
+      </c>
       <c r="F62" t="s">
-        <v>335</v>
-      </c>
-      <c r="I62" s="32"/>
+        <v>341</v>
+      </c>
+      <c r="I62" s="29" t="s">
+        <v>113</v>
+      </c>
       <c r="J62" t="s">
-        <v>324</v>
-      </c>
-      <c r="M62" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="M62" s="29" t="s">
         <v>113</v>
       </c>
       <c r="N62" t="s">
@@ -4185,29 +4226,29 @@
       <c r="R62" t="s">
         <v>338</v>
       </c>
-      <c r="U62" s="31" t="s">
+      <c r="U62" s="29" t="s">
         <v>113</v>
       </c>
       <c r="V62" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A63" s="32"/>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A63" s="31" t="s">
+        <v>93</v>
+      </c>
       <c r="B63" t="s">
-        <v>340</v>
-      </c>
-      <c r="E63" s="30"/>
+        <v>328</v>
+      </c>
+      <c r="E63" s="31"/>
       <c r="F63" t="s">
-        <v>299</v>
-      </c>
-      <c r="I63" s="31" t="s">
-        <v>113</v>
-      </c>
+        <v>347</v>
+      </c>
+      <c r="I63" s="29"/>
       <c r="J63" t="s">
-        <v>342</v>
-      </c>
-      <c r="M63" s="31"/>
+        <v>348</v>
+      </c>
+      <c r="M63" s="29"/>
       <c r="N63" t="s">
         <v>343</v>
       </c>
@@ -4215,421 +4256,395 @@
       <c r="R63" t="s">
         <v>344</v>
       </c>
-      <c r="U63" s="31"/>
+      <c r="U63" s="29"/>
       <c r="V63" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A64" s="32"/>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A64" s="31"/>
       <c r="B64" t="s">
-        <v>346</v>
-      </c>
-      <c r="E64" s="32" t="s">
-        <v>93</v>
-      </c>
+        <v>334</v>
+      </c>
+      <c r="E64" s="31"/>
       <c r="F64" t="s">
-        <v>341</v>
-      </c>
-      <c r="I64" s="31"/>
+        <v>359</v>
+      </c>
+      <c r="I64" s="29"/>
       <c r="J64" t="s">
-        <v>348</v>
-      </c>
-      <c r="M64" s="31"/>
+        <v>354</v>
+      </c>
+      <c r="M64" s="29"/>
       <c r="N64" t="s">
         <v>349</v>
       </c>
-      <c r="Q64" s="32" t="s">
+      <c r="Q64" s="31" t="s">
         <v>93</v>
       </c>
       <c r="R64" t="s">
         <v>350</v>
       </c>
-      <c r="U64" s="31"/>
+      <c r="U64" s="29"/>
       <c r="V64" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A65" s="31" t="s">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A65" s="31"/>
+      <c r="B65" t="s">
+        <v>340</v>
+      </c>
+      <c r="E65" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="B65" t="s">
-        <v>352</v>
-      </c>
-      <c r="E65" s="32"/>
       <c r="F65" t="s">
-        <v>347</v>
-      </c>
-      <c r="I65" s="31"/>
+        <v>365</v>
+      </c>
+      <c r="I65" s="29"/>
       <c r="J65" t="s">
-        <v>354</v>
-      </c>
-      <c r="M65" s="28" t="s">
+        <v>360</v>
+      </c>
+      <c r="M65" s="27" t="s">
         <v>137</v>
       </c>
       <c r="N65" t="s">
         <v>355</v>
       </c>
-      <c r="Q65" s="32"/>
+      <c r="Q65" s="31"/>
       <c r="R65" t="s">
         <v>356</v>
       </c>
-      <c r="U65" s="28" t="s">
+      <c r="U65" s="27" t="s">
         <v>137</v>
       </c>
       <c r="V65" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" s="31"/>
       <c r="B66" t="s">
-        <v>358</v>
-      </c>
-      <c r="E66" s="32"/>
+        <v>346</v>
+      </c>
+      <c r="E66" s="29"/>
       <c r="F66" t="s">
-        <v>359</v>
-      </c>
-      <c r="I66" s="31"/>
+        <v>371</v>
+      </c>
+      <c r="I66" s="27" t="s">
+        <v>137</v>
+      </c>
       <c r="J66" t="s">
-        <v>360</v>
-      </c>
-      <c r="M66" s="28"/>
+        <v>372</v>
+      </c>
+      <c r="M66" s="27"/>
       <c r="N66" t="s">
         <v>361</v>
       </c>
-      <c r="Q66" s="31" t="s">
+      <c r="Q66" s="29" t="s">
         <v>113</v>
       </c>
       <c r="R66" t="s">
         <v>362</v>
       </c>
-      <c r="U66" s="28"/>
+      <c r="U66" s="27"/>
       <c r="V66" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A67" s="31"/>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A67" s="29" t="s">
+        <v>113</v>
+      </c>
       <c r="B67" t="s">
-        <v>364</v>
-      </c>
-      <c r="E67" s="31" t="s">
-        <v>113</v>
-      </c>
+        <v>352</v>
+      </c>
+      <c r="E67" s="29"/>
       <c r="F67" t="s">
-        <v>365</v>
-      </c>
-      <c r="I67" s="28" t="s">
-        <v>137</v>
-      </c>
+        <v>377</v>
+      </c>
+      <c r="I67" s="27"/>
       <c r="J67" t="s">
-        <v>372</v>
-      </c>
-      <c r="M67" s="28"/>
+        <v>384</v>
+      </c>
+      <c r="M67" s="27"/>
       <c r="N67" t="s">
         <v>156</v>
       </c>
-      <c r="Q67" s="31"/>
+      <c r="Q67" s="29"/>
       <c r="R67" t="s">
         <v>368</v>
       </c>
-      <c r="U67" s="28"/>
+      <c r="U67" s="27"/>
       <c r="V67" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A68" s="28" t="s">
-        <v>137</v>
-      </c>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A68" s="29"/>
       <c r="B68" t="s">
-        <v>370</v>
-      </c>
-      <c r="E68" s="31"/>
+        <v>358</v>
+      </c>
+      <c r="E68" s="29"/>
       <c r="F68" t="s">
-        <v>371</v>
-      </c>
-      <c r="I68" s="28"/>
+        <v>125</v>
+      </c>
+      <c r="I68" s="27"/>
       <c r="J68" t="s">
-        <v>384</v>
-      </c>
-      <c r="M68" s="28"/>
+        <v>162</v>
+      </c>
+      <c r="M68" s="27"/>
       <c r="N68" t="s">
         <v>373</v>
       </c>
-      <c r="Q68" s="31"/>
+      <c r="Q68" s="29"/>
       <c r="R68" t="s">
         <v>374</v>
       </c>
-      <c r="U68" s="28"/>
+      <c r="U68" s="27"/>
       <c r="V68" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A69" s="28"/>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A69" s="29"/>
       <c r="B69" t="s">
-        <v>376</v>
-      </c>
-      <c r="E69" s="31"/>
+        <v>364</v>
+      </c>
+      <c r="E69" s="27" t="s">
+        <v>137</v>
+      </c>
       <c r="F69" t="s">
-        <v>377</v>
-      </c>
-      <c r="I69" s="28"/>
+        <v>383</v>
+      </c>
+      <c r="I69" s="27"/>
       <c r="J69" t="s">
-        <v>162</v>
-      </c>
-      <c r="M69" s="28"/>
+        <v>407</v>
+      </c>
+      <c r="M69" s="27"/>
       <c r="N69" t="s">
         <v>379</v>
       </c>
-      <c r="Q69" s="31"/>
+      <c r="Q69" s="29"/>
       <c r="R69" t="s">
         <v>380</v>
       </c>
-      <c r="U69" s="28"/>
+      <c r="U69" s="27"/>
       <c r="V69" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A70" s="28"/>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A70" s="27" t="s">
+        <v>137</v>
+      </c>
       <c r="B70" t="s">
-        <v>382</v>
-      </c>
-      <c r="E70" s="31"/>
+        <v>370</v>
+      </c>
+      <c r="E70" s="27"/>
       <c r="F70" t="s">
-        <v>125</v>
-      </c>
-      <c r="I70" s="28"/>
+        <v>389</v>
+      </c>
+      <c r="I70" s="27"/>
       <c r="J70" t="s">
-        <v>407</v>
-      </c>
-      <c r="M70" s="28"/>
+        <v>366</v>
+      </c>
+      <c r="M70" s="27"/>
       <c r="N70" t="s">
         <v>367</v>
       </c>
-      <c r="Q70" s="28" t="s">
+      <c r="Q70" s="27" t="s">
         <v>137</v>
       </c>
       <c r="R70" t="s">
         <v>386</v>
       </c>
-      <c r="U70" s="29" t="s">
+      <c r="U70" s="26" t="s">
         <v>167</v>
       </c>
       <c r="V70" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A71" s="28"/>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A71" s="27"/>
       <c r="B71" t="s">
-        <v>388</v>
-      </c>
-      <c r="E71" s="28" t="s">
-        <v>137</v>
-      </c>
+        <v>376</v>
+      </c>
+      <c r="E71" s="27"/>
       <c r="F71" t="s">
-        <v>383</v>
-      </c>
-      <c r="I71" s="28"/>
+        <v>395</v>
+      </c>
+      <c r="I71" s="27"/>
       <c r="J71" t="s">
-        <v>366</v>
-      </c>
-      <c r="M71" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="M71" s="26" t="s">
         <v>167</v>
       </c>
       <c r="N71" t="s">
         <v>385</v>
       </c>
-      <c r="Q71" s="28"/>
+      <c r="Q71" s="27"/>
       <c r="R71" t="s">
         <v>392</v>
       </c>
-      <c r="U71" s="29"/>
+      <c r="U71" s="26"/>
       <c r="V71" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A72" s="29" t="s">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A72" s="27"/>
+      <c r="B72" t="s">
+        <v>382</v>
+      </c>
+      <c r="E72" s="27"/>
+      <c r="F72" t="s">
+        <v>401</v>
+      </c>
+      <c r="I72" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="B72" t="s">
-        <v>394</v>
-      </c>
-      <c r="E72" s="28"/>
-      <c r="F72" t="s">
-        <v>389</v>
-      </c>
-      <c r="I72" s="28"/>
       <c r="J72" t="s">
-        <v>378</v>
-      </c>
-      <c r="M72" s="29"/>
+        <v>390</v>
+      </c>
+      <c r="M72" s="26"/>
       <c r="N72" t="s">
         <v>391</v>
       </c>
-      <c r="Q72" s="28"/>
+      <c r="Q72" s="27"/>
       <c r="R72" t="s">
         <v>398</v>
       </c>
-      <c r="U72" s="29"/>
+      <c r="U72" s="26"/>
       <c r="V72" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A73" s="29"/>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A73" s="27"/>
       <c r="B73" t="s">
-        <v>400</v>
-      </c>
-      <c r="E73" s="28"/>
+        <v>388</v>
+      </c>
+      <c r="E73" s="26" t="s">
+        <v>167</v>
+      </c>
       <c r="F73" t="s">
-        <v>395</v>
-      </c>
-      <c r="I73" s="29" t="s">
-        <v>167</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="I73" s="26"/>
       <c r="J73" t="s">
-        <v>390</v>
-      </c>
-      <c r="M73" s="29"/>
+        <v>402</v>
+      </c>
+      <c r="M73" s="26"/>
       <c r="N73" t="s">
         <v>397</v>
       </c>
-      <c r="Q73" s="28"/>
+      <c r="Q73" s="27"/>
       <c r="R73" t="s">
         <v>403</v>
       </c>
-      <c r="U73" s="29"/>
+      <c r="U73" s="26"/>
       <c r="V73" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A74" s="29"/>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A74" s="26" t="s">
+        <v>167</v>
+      </c>
       <c r="B74" t="s">
-        <v>405</v>
-      </c>
-      <c r="E74" s="28"/>
+        <v>394</v>
+      </c>
+      <c r="E74" s="26"/>
       <c r="F74" t="s">
-        <v>401</v>
-      </c>
-      <c r="I74" s="29"/>
+        <v>410</v>
+      </c>
+      <c r="I74" s="26"/>
       <c r="J74" t="s">
-        <v>402</v>
-      </c>
-      <c r="Q74" s="29" t="s">
+        <v>411</v>
+      </c>
+      <c r="Q74" s="26" t="s">
         <v>167</v>
       </c>
       <c r="R74" t="s">
         <v>408</v>
       </c>
-      <c r="U74" s="29"/>
+      <c r="U74" s="26"/>
       <c r="V74" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A75" s="29"/>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A75" s="26"/>
       <c r="B75" t="s">
-        <v>409</v>
-      </c>
-      <c r="E75" s="29" t="s">
-        <v>167</v>
-      </c>
+        <v>400</v>
+      </c>
+      <c r="E75" s="26"/>
       <c r="F75" t="s">
-        <v>406</v>
-      </c>
-      <c r="I75" s="29"/>
+        <v>413</v>
+      </c>
+      <c r="I75" s="26"/>
       <c r="J75" t="s">
-        <v>411</v>
-      </c>
-      <c r="Q75" s="29"/>
+        <v>187</v>
+      </c>
+      <c r="Q75" s="26"/>
       <c r="R75" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="E76" s="29"/>
-      <c r="F76" t="s">
-        <v>410</v>
-      </c>
-      <c r="I76" s="29"/>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A76" s="26"/>
+      <c r="B76" t="s">
+        <v>405</v>
+      </c>
+      <c r="I76" s="26"/>
       <c r="J76" t="s">
         <v>396</v>
       </c>
-      <c r="Q76" s="29"/>
+      <c r="Q76" s="26"/>
       <c r="R76" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="E77" s="29"/>
-      <c r="F77" t="s">
-        <v>413</v>
-      </c>
-      <c r="Q77" s="29"/>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A77" s="26"/>
+      <c r="B77" t="s">
+        <v>409</v>
+      </c>
+      <c r="Q77" s="26"/>
       <c r="R77" t="s">
         <v>415</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="E41:E44"/>
-    <mergeCell ref="I73:I76"/>
-    <mergeCell ref="E21:E24"/>
-    <mergeCell ref="Q74:Q77"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="E25:E28"/>
-    <mergeCell ref="A8:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="M65:M70"/>
-    <mergeCell ref="E67:E70"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="M41:M43"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="M51:M58"/>
-    <mergeCell ref="M59:M61"/>
-    <mergeCell ref="U41:U43"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="U40:V40"/>
-    <mergeCell ref="U44:U49"/>
-    <mergeCell ref="U60:U61"/>
-    <mergeCell ref="U50:U59"/>
-    <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="Q43:Q50"/>
-    <mergeCell ref="E64:E66"/>
-    <mergeCell ref="I50:I57"/>
-    <mergeCell ref="I58:I62"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="M12:M18"/>
-    <mergeCell ref="E11:E15"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="A51:A60"/>
-    <mergeCell ref="I29:I33"/>
-    <mergeCell ref="I42:I49"/>
-    <mergeCell ref="E45:E50"/>
-    <mergeCell ref="M44:M50"/>
-    <mergeCell ref="E51:E63"/>
-    <mergeCell ref="U70:U74"/>
-    <mergeCell ref="E71:E74"/>
-    <mergeCell ref="M71:M73"/>
-    <mergeCell ref="Q70:Q73"/>
-    <mergeCell ref="E75:E77"/>
-    <mergeCell ref="I67:I72"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="U2:U4"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="E10:E15"/>
+    <mergeCell ref="Q5:Q11"/>
+    <mergeCell ref="U5:U10"/>
+    <mergeCell ref="U11:U18"/>
+    <mergeCell ref="Q12:Q18"/>
+    <mergeCell ref="U62:U64"/>
+    <mergeCell ref="Q64:Q65"/>
+    <mergeCell ref="U65:U69"/>
+    <mergeCell ref="Q66:Q69"/>
+    <mergeCell ref="Q19:Q21"/>
+    <mergeCell ref="E73:E75"/>
+    <mergeCell ref="I66:I71"/>
     <mergeCell ref="M30:M33"/>
     <mergeCell ref="U19:U20"/>
     <mergeCell ref="I21:I24"/>
@@ -4642,38 +4657,62 @@
     <mergeCell ref="Q26:Q29"/>
     <mergeCell ref="Q30:Q34"/>
     <mergeCell ref="I12:I19"/>
+    <mergeCell ref="U29:U33"/>
+    <mergeCell ref="Q51:Q63"/>
+    <mergeCell ref="M44:M50"/>
+    <mergeCell ref="U70:U74"/>
+    <mergeCell ref="E69:E72"/>
+    <mergeCell ref="M71:M73"/>
+    <mergeCell ref="Q70:Q73"/>
+    <mergeCell ref="M62:M64"/>
+    <mergeCell ref="I62:I65"/>
+    <mergeCell ref="I51:I56"/>
+    <mergeCell ref="I42:I50"/>
+    <mergeCell ref="I72:I76"/>
+    <mergeCell ref="E45:E49"/>
+    <mergeCell ref="E50:E61"/>
+    <mergeCell ref="M51:M57"/>
+    <mergeCell ref="M58:M61"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="I29:I33"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="A44:A51"/>
+    <mergeCell ref="A52:A62"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="M40:N40"/>
     <mergeCell ref="I4:I11"/>
     <mergeCell ref="M5:M11"/>
-    <mergeCell ref="U29:U33"/>
-    <mergeCell ref="Q51:Q63"/>
-    <mergeCell ref="Q5:Q11"/>
-    <mergeCell ref="U5:U10"/>
-    <mergeCell ref="U11:U18"/>
-    <mergeCell ref="Q12:Q18"/>
-    <mergeCell ref="U62:U64"/>
-    <mergeCell ref="M62:M64"/>
-    <mergeCell ref="I63:I66"/>
-    <mergeCell ref="Q64:Q65"/>
-    <mergeCell ref="U65:U69"/>
-    <mergeCell ref="Q66:Q69"/>
-    <mergeCell ref="M19:M22"/>
-    <mergeCell ref="Q19:Q21"/>
-    <mergeCell ref="A44:A50"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="U2:U4"/>
-    <mergeCell ref="E4:E10"/>
+    <mergeCell ref="E4:E9"/>
+    <mergeCell ref="M20:M22"/>
+    <mergeCell ref="M12:M19"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="U41:U43"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="U40:V40"/>
+    <mergeCell ref="U44:U49"/>
+    <mergeCell ref="U60:U61"/>
+    <mergeCell ref="U50:U59"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="Q43:Q50"/>
+    <mergeCell ref="E62:E64"/>
+    <mergeCell ref="I57:I61"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="E41:E44"/>
+    <mergeCell ref="E21:E24"/>
+    <mergeCell ref="Q74:Q77"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="M65:M70"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="M41:M43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4682,69 +4721,69 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S29"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="8" max="8" width="15.54296875" customWidth="1"/>
-    <col min="9" max="9" width="14.81640625" customWidth="1"/>
-    <col min="10" max="10" width="18.26953125" customWidth="1"/>
-    <col min="12" max="12" width="16.81640625" customWidth="1"/>
-    <col min="13" max="13" width="18.453125" customWidth="1"/>
-    <col min="15" max="15" width="16.81640625" customWidth="1"/>
-    <col min="16" max="16" width="17.453125" customWidth="1"/>
-    <col min="17" max="17" width="7.81640625" customWidth="1"/>
-    <col min="18" max="18" width="14.81640625" customWidth="1"/>
-    <col min="19" max="19" width="20.7265625" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" customWidth="1"/>
+    <col min="17" max="17" width="7.85546875" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="E1" s="26" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="E1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="26"/>
+      <c r="F1" s="32"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="26"/>
-      <c r="O1" s="26" t="s">
+      <c r="M1" s="32"/>
+      <c r="O1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="26"/>
-      <c r="R1" s="26" t="s">
+      <c r="P1" s="32"/>
+      <c r="R1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="26"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S1" s="32"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>416</v>
+        <v>448</v>
       </c>
       <c r="C2" t="s">
-        <v>449</v>
+        <v>493</v>
       </c>
       <c r="E2" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F2" t="s">
         <v>418</v>
@@ -4756,7 +4795,7 @@
         <v>420</v>
       </c>
       <c r="L2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="M2" t="s">
         <v>421</v>
@@ -4774,12 +4813,9 @@
         <v>425</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>501</v>
-      </c>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>493</v>
+        <v>450</v>
       </c>
       <c r="E3" t="s">
         <v>484</v>
@@ -4812,12 +4848,12 @@
         <v>436</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>448</v>
-      </c>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>459</v>
+        <v>460</v>
+      </c>
+      <c r="E4" t="s">
+        <v>416</v>
       </c>
       <c r="F4" t="s">
         <v>439</v>
@@ -4847,9 +4883,12 @@
         <v>447</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>490</v>
+        <v>459</v>
+      </c>
+      <c r="E5" t="s">
+        <v>492</v>
       </c>
       <c r="F5" t="s">
         <v>417</v>
@@ -4879,9 +4918,9 @@
         <v>458</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>473</v>
+        <v>490</v>
       </c>
       <c r="F6" t="s">
         <v>427</v>
@@ -4911,9 +4950,9 @@
         <v>468</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>475</v>
+        <v>502</v>
       </c>
       <c r="F7" t="s">
         <v>485</v>
@@ -4925,96 +4964,87 @@
         <v>472</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>473</v>
+      </c>
       <c r="F8" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>475</v>
+      </c>
       <c r="F9" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="E17" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="I17" s="32" t="s">
+        <v>605</v>
+      </c>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="M17" s="32"/>
+      <c r="O17" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="P17" s="32"/>
+      <c r="R17" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="S17" s="32"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>635</v>
+      </c>
+      <c r="C18" t="s">
+        <v>438</v>
+      </c>
+      <c r="E18" t="s">
+        <v>624</v>
+      </c>
+      <c r="F18" t="s">
+        <v>481</v>
+      </c>
+      <c r="I18" t="s">
+        <v>507</v>
+      </c>
+      <c r="J18" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="F12" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="F13" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="F14" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="F15" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="E17" s="26" t="s">
-        <v>204</v>
-      </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="I17" s="26" t="s">
-        <v>606</v>
-      </c>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26" t="s">
-        <v>205</v>
-      </c>
-      <c r="M17" s="26"/>
-      <c r="O17" s="26" t="s">
-        <v>206</v>
-      </c>
-      <c r="P17" s="26"/>
-      <c r="R17" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="S17" s="26"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
-        <v>480</v>
-      </c>
-      <c r="C18" t="s">
-        <v>481</v>
-      </c>
-      <c r="E18" t="s">
-        <v>625</v>
-      </c>
-      <c r="F18" t="s">
-        <v>495</v>
-      </c>
-      <c r="I18" t="s">
-        <v>492</v>
-      </c>
-      <c r="J18" t="s">
-        <v>438</v>
-      </c>
       <c r="L18" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="M18" t="s">
         <v>487</v>
@@ -5026,21 +5056,24 @@
         <v>489</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>480</v>
+      </c>
       <c r="C19" t="s">
         <v>491</v>
       </c>
       <c r="E19" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F19" t="s">
-        <v>474</v>
+        <v>495</v>
       </c>
       <c r="I19" t="s">
-        <v>507</v>
+        <v>621</v>
       </c>
       <c r="J19" t="s">
-        <v>502</v>
+        <v>449</v>
       </c>
       <c r="L19" t="s">
         <v>496</v>
@@ -5049,15 +5082,15 @@
         <v>497</v>
       </c>
       <c r="R19" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>482</v>
       </c>
       <c r="F20" t="s">
-        <v>500</v>
+        <v>474</v>
       </c>
       <c r="I20" t="s">
         <v>622</v>
@@ -5078,15 +5111,15 @@
         <v>506</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>499</v>
       </c>
       <c r="F21" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="I21" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="J21" t="s">
         <v>510</v>
@@ -5095,7 +5128,7 @@
         <v>511</v>
       </c>
       <c r="O21" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="P21" t="s">
         <v>512</v>
@@ -5104,7 +5137,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>514</v>
       </c>
@@ -5112,69 +5145,67 @@
         <v>494</v>
       </c>
       <c r="F22" t="s">
+        <v>508</v>
+      </c>
+      <c r="I22" t="s">
+        <v>501</v>
+      </c>
+      <c r="J22" t="s">
+        <v>517</v>
+      </c>
+      <c r="O22" t="s">
+        <v>518</v>
+      </c>
+      <c r="S22" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>520</v>
+      </c>
+      <c r="F23" t="s">
         <v>469</v>
-      </c>
-      <c r="I22" t="s">
-        <v>627</v>
-      </c>
-      <c r="J22" t="s">
-        <v>518</v>
-      </c>
-      <c r="O22" t="s">
-        <v>519</v>
-      </c>
-      <c r="S22" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="E23" t="s">
-        <v>515</v>
-      </c>
-      <c r="F23" t="s">
-        <v>516</v>
       </c>
       <c r="I23" t="s">
         <v>509</v>
       </c>
       <c r="O23" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>521</v>
+        <v>627</v>
+      </c>
+      <c r="F24" t="s">
+        <v>515</v>
       </c>
       <c r="I24" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="O24" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
         <v>526</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="E29" t="s">
-        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -5205,153 +5236,153 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1796875" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" customWidth="1"/>
-    <col min="3" max="3" width="29.81640625" customWidth="1"/>
-    <col min="4" max="4" width="24.1796875" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B1" t="s">
         <v>528</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="4" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>531</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" t="s">
         <v>533</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>535</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="C3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>538</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>540</v>
       </c>
-      <c r="D4" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>541</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="4" t="s">
         <v>542</v>
       </c>
-      <c r="C5" s="4" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>609</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>544</v>
       </c>
-      <c r="B6" t="s">
-        <v>610</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>545</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="4" t="s">
         <v>546</v>
       </c>
-      <c r="C7" s="4" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>548</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="4" t="s">
         <v>549</v>
       </c>
-      <c r="C8" s="4" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>551</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="C9" s="4" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>554</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="4" t="s">
         <v>555</v>
       </c>
-      <c r="C10" s="4" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>557</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="4" t="s">
         <v>558</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>559</v>
       </c>
-      <c r="D11" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>560</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="4" t="s">
         <v>561</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>562</v>
       </c>
     </row>
   </sheetData>
@@ -5376,682 +5407,931 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B116"/>
+  <dimension ref="A1:B157"/>
   <sheetViews>
-    <sheetView topLeftCell="A104" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D151" sqref="D151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" customWidth="1"/>
-    <col min="2" max="2" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>563</v>
       </c>
-      <c r="B1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>565</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="10" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="10" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
+        <v>568</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>569</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="8" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>571</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>572</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="10" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="9" t="s">
+      <c r="B16" s="10" t="s">
         <v>575</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="10" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="8" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="10" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="10" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="10" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="10" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="8" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="10" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B37" s="8" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
+      <c r="B39" s="6" t="s">
         <v>585</v>
       </c>
-      <c r="B39" s="6" t="s">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="7" t="s">
+      <c r="B40" s="8" t="s">
         <v>587</v>
       </c>
-      <c r="B40" s="8" t="s">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>577</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="5" t="s">
-        <v>578</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
       <c r="B43" s="10" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="B44" s="10" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="8" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
       <c r="B49" s="10" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
       <c r="B53" s="10" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="8" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="9"/>
       <c r="B58" s="10" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="9"/>
       <c r="B59" s="10" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B60" s="10" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="8" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
       <c r="B64" s="14" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
+        <v>562</v>
+      </c>
+      <c r="B65" s="14" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="13" t="s">
-        <v>563</v>
-      </c>
-      <c r="B65" s="14" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="15"/>
       <c r="B66" s="16" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
+        <v>599</v>
+      </c>
+      <c r="B68" s="19" t="s">
         <v>600</v>
       </c>
-      <c r="B68" s="19" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="9"/>
       <c r="B69" s="20" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="21" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="21" t="s">
+      <c r="B70" s="22" t="s">
         <v>603</v>
       </c>
-      <c r="B70" s="22" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B72" s="19" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="21" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B73" s="22" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B75" s="19" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="21" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B76" s="22" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
+        <v>606</v>
+      </c>
+      <c r="B78" s="19" t="s">
         <v>607</v>
       </c>
-      <c r="B78" s="19" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="79" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="21" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B79" s="22" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="18" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B81" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="9"/>
       <c r="B82" s="20" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="9"/>
       <c r="B83" s="20" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B84" s="20" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="9"/>
       <c r="B85" s="20" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="21"/>
       <c r="B86" s="22" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="18" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B88" s="19" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="9"/>
       <c r="B89" s="20" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="9"/>
       <c r="B90" s="24" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B91" s="20" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="21"/>
       <c r="B92" s="22" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="18" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B94" s="19" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="9"/>
       <c r="B95" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="9"/>
       <c r="B96" s="20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B97" s="20" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="21"/>
       <c r="B98" s="22" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="18" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B100" s="19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="9"/>
       <c r="B101" s="20" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="9"/>
       <c r="B102" s="20" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B103" s="20" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="21"/>
       <c r="B104" s="22" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="18" t="s">
+        <v>602</v>
+      </c>
+      <c r="B106" s="19" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" s="18" t="s">
-        <v>603</v>
-      </c>
-      <c r="B106" s="19" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="9"/>
       <c r="B107" s="20" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="9"/>
       <c r="B108" s="20" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="9"/>
       <c r="B109" s="20" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B110" s="20" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="21"/>
       <c r="B111" s="22" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="18" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B113" s="19" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="9" t="s">
+        <v>606</v>
+      </c>
+      <c r="B114" s="20" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A114" s="9" t="s">
-        <v>607</v>
-      </c>
-      <c r="B114" s="20" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="9"/>
       <c r="B115" s="20" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="21"/>
       <c r="B116" s="22" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="18" t="s">
         <v>632</v>
+      </c>
+      <c r="B118" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="21" t="s">
+        <v>592</v>
+      </c>
+      <c r="B119" s="22" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="18" t="s">
+        <v>574</v>
+      </c>
+      <c r="B121" s="19" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="B122" s="20" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="9"/>
+      <c r="B123" s="20" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="9"/>
+      <c r="B124" s="20" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="21"/>
+      <c r="B125" s="22" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B127" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="18" t="s">
+        <v>637</v>
+      </c>
+      <c r="B128" s="19" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="9"/>
+      <c r="B129" s="20" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="9"/>
+      <c r="B130" s="20" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="9"/>
+      <c r="B131" s="20" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="9"/>
+      <c r="B132" s="20" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="9" t="s">
+        <v>639</v>
+      </c>
+      <c r="B133" s="20" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="9"/>
+      <c r="B134" s="20" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="9"/>
+      <c r="B135" s="20" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="9" t="s">
+        <v>641</v>
+      </c>
+      <c r="B136" s="20" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="9"/>
+      <c r="B137" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="9"/>
+      <c r="B138" s="20" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="9"/>
+      <c r="B139" s="20" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="9"/>
+      <c r="B140" s="20" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="9"/>
+      <c r="B141" s="20" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="9" t="s">
+        <v>642</v>
+      </c>
+      <c r="B142" s="20" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="9"/>
+      <c r="B143" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="9"/>
+      <c r="B144" s="20" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="9"/>
+      <c r="B145" s="20" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="9"/>
+      <c r="B146" s="20" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="9" t="s">
+        <v>644</v>
+      </c>
+      <c r="B147" s="20" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="9"/>
+      <c r="B148" s="20" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="9"/>
+      <c r="B149" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="9"/>
+      <c r="B150" s="20" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="9"/>
+      <c r="B151" s="20" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="9" t="s">
+        <v>646</v>
+      </c>
+      <c r="B152" s="20" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="9"/>
+      <c r="B153" s="20" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="9"/>
+      <c r="B154" s="20" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="9"/>
+      <c r="B155" s="20" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="9"/>
+      <c r="B156" s="20" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="21"/>
+      <c r="B157" s="22" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trade up! TE on the move!
</commit_message>
<xml_diff>
--- a/OffSeason.xlsx
+++ b/OffSeason.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sdwg-my.sharepoint.com/personal/john_olson_agtegra_com/Documents/Documents 1/Football/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{ECA9F46E-F317-4CC4-8E17-E8E8FEC0C4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FD5E9EF-C50B-4DAD-9A1A-D6A70CA800AC}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{ECA9F46E-F317-4CC4-8E17-E8E8FEC0C4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6811CD6-6CE5-4F95-BB5B-018FFB497015}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rosters" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="657">
   <si>
     <t>Vanja Dolas - CeeDee Nuts</t>
   </si>
@@ -1993,6 +1993,12 @@
   </si>
   <si>
     <t>2022 2 John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jared </t>
   </si>
 </sst>
 </file>
@@ -2235,16 +2241,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2257,6 +2257,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2642,10 +2648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W77"/>
+  <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2661,71 +2667,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="E1" s="25" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="E1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="25"/>
+      <c r="F1" s="31"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="25"/>
+      <c r="N1" s="31"/>
       <c r="O1" s="1"/>
-      <c r="Q1" s="25" t="s">
+      <c r="Q1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="25"/>
+      <c r="R1" s="31"/>
       <c r="S1" s="1"/>
-      <c r="U1" s="25" t="s">
+      <c r="U1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="25"/>
+      <c r="V1" s="31"/>
       <c r="W1" s="1"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="N2" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="26" t="s">
+      <c r="Q2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="R2" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="26" t="s">
+      <c r="U2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="V2" t="s">
@@ -2733,89 +2739,89 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
+      <c r="A3" s="25"/>
       <c r="B3" t="s">
         <v>209</v>
       </c>
-      <c r="E3" s="26"/>
+      <c r="E3" s="25"/>
       <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="26"/>
+      <c r="I3" s="25"/>
       <c r="J3" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="26"/>
+      <c r="M3" s="25"/>
       <c r="N3" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="26"/>
+      <c r="Q3" s="25"/>
       <c r="R3" t="s">
         <v>17</v>
       </c>
-      <c r="U3" s="26"/>
+      <c r="U3" s="25"/>
       <c r="V3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="28" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="I4" s="28" t="s">
         <v>20</v>
       </c>
       <c r="J4" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="26"/>
+      <c r="M4" s="25"/>
       <c r="N4" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" s="26"/>
+      <c r="Q4" s="25"/>
       <c r="R4" t="s">
         <v>24</v>
       </c>
-      <c r="U4" s="26"/>
+      <c r="U4" s="25"/>
       <c r="V4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
+      <c r="A5" s="28"/>
       <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="28"/>
       <c r="F5" t="s">
         <v>227</v>
       </c>
-      <c r="I5" s="30"/>
+      <c r="I5" s="28"/>
       <c r="J5" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="30" t="s">
+      <c r="M5" s="28" t="s">
         <v>20</v>
       </c>
       <c r="N5" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="30" t="s">
+      <c r="Q5" s="28" t="s">
         <v>20</v>
       </c>
       <c r="R5" t="s">
         <v>30</v>
       </c>
-      <c r="U5" s="30" t="s">
+      <c r="U5" s="28" t="s">
         <v>20</v>
       </c>
       <c r="V5" t="s">
@@ -2823,161 +2829,161 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="28"/>
       <c r="B6" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="30"/>
+      <c r="E6" s="28"/>
       <c r="F6" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="30"/>
+      <c r="I6" s="28"/>
       <c r="J6" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="30"/>
+      <c r="M6" s="28"/>
       <c r="N6" t="s">
         <v>35</v>
       </c>
-      <c r="Q6" s="30"/>
+      <c r="Q6" s="28"/>
       <c r="R6" t="s">
         <v>36</v>
       </c>
-      <c r="U6" s="30"/>
+      <c r="U6" s="28"/>
       <c r="V6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="28"/>
       <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="30"/>
+      <c r="E7" s="28"/>
       <c r="F7" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="30"/>
+      <c r="I7" s="28"/>
       <c r="J7" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="30"/>
+      <c r="M7" s="28"/>
       <c r="N7" t="s">
         <v>41</v>
       </c>
-      <c r="Q7" s="30"/>
+      <c r="Q7" s="28"/>
       <c r="R7" t="s">
         <v>42</v>
       </c>
-      <c r="U7" s="30"/>
+      <c r="U7" s="28"/>
       <c r="V7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="32" t="s">
         <v>44</v>
       </c>
       <c r="B8" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="30"/>
+      <c r="E8" s="28"/>
       <c r="F8" t="s">
         <v>52</v>
       </c>
-      <c r="I8" s="30"/>
+      <c r="I8" s="28"/>
       <c r="J8" t="s">
         <v>47</v>
       </c>
-      <c r="M8" s="30"/>
+      <c r="M8" s="28"/>
       <c r="N8" t="s">
         <v>48</v>
       </c>
-      <c r="Q8" s="30"/>
+      <c r="Q8" s="28"/>
       <c r="R8" t="s">
         <v>49</v>
       </c>
-      <c r="U8" s="30"/>
+      <c r="U8" s="28"/>
       <c r="V8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
+      <c r="A9" s="32"/>
       <c r="B9" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="30"/>
+      <c r="E9" s="28"/>
       <c r="F9" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="30"/>
+      <c r="I9" s="28"/>
       <c r="J9" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="30"/>
+      <c r="M9" s="28"/>
       <c r="N9" t="s">
         <v>54</v>
       </c>
-      <c r="Q9" s="30"/>
+      <c r="Q9" s="28"/>
       <c r="R9" t="s">
         <v>55</v>
       </c>
-      <c r="U9" s="30"/>
+      <c r="U9" s="28"/>
       <c r="V9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="32"/>
       <c r="B10" t="s">
         <v>281</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="32" t="s">
         <v>44</v>
       </c>
       <c r="F10" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="30"/>
+      <c r="I10" s="28"/>
       <c r="J10" t="s">
         <v>59</v>
       </c>
-      <c r="M10" s="30"/>
+      <c r="M10" s="28"/>
       <c r="N10" t="s">
         <v>60</v>
       </c>
-      <c r="Q10" s="30"/>
+      <c r="Q10" s="28"/>
       <c r="R10" t="s">
         <v>61</v>
       </c>
-      <c r="U10" s="30"/>
+      <c r="U10" s="28"/>
       <c r="V10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
+      <c r="A11" s="32"/>
       <c r="B11" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="28"/>
+      <c r="E11" s="32"/>
       <c r="F11" t="s">
         <v>70</v>
       </c>
-      <c r="I11" s="30"/>
+      <c r="I11" s="28"/>
       <c r="J11" t="s">
         <v>65</v>
       </c>
-      <c r="M11" s="30"/>
+      <c r="M11" s="28"/>
       <c r="N11" t="s">
         <v>66</v>
       </c>
-      <c r="Q11" s="30"/>
+      <c r="Q11" s="28"/>
       <c r="R11" t="s">
         <v>67</v>
       </c>
-      <c r="U11" s="28" t="s">
+      <c r="U11" s="32" t="s">
         <v>44</v>
       </c>
       <c r="V11" t="s">
@@ -2985,223 +2991,223 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
+      <c r="A12" s="32"/>
       <c r="B12" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="32"/>
       <c r="F12" t="s">
         <v>88</v>
       </c>
-      <c r="I12" s="28" t="s">
+      <c r="I12" s="32" t="s">
         <v>44</v>
       </c>
       <c r="J12" t="s">
         <v>71</v>
       </c>
-      <c r="M12" s="28" t="s">
+      <c r="M12" s="32" t="s">
         <v>44</v>
       </c>
       <c r="N12" t="s">
         <v>72</v>
       </c>
-      <c r="Q12" s="28" t="s">
+      <c r="Q12" s="32" t="s">
         <v>44</v>
       </c>
       <c r="R12" t="s">
         <v>73</v>
       </c>
-      <c r="U12" s="28"/>
+      <c r="U12" s="32"/>
       <c r="V12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
+      <c r="A13" s="32"/>
       <c r="B13" t="s">
         <v>270</v>
       </c>
-      <c r="E13" s="28"/>
+      <c r="E13" s="32"/>
       <c r="F13" t="s">
         <v>82</v>
       </c>
-      <c r="I13" s="28"/>
+      <c r="I13" s="32"/>
       <c r="J13" t="s">
         <v>77</v>
       </c>
-      <c r="M13" s="28"/>
+      <c r="M13" s="32"/>
       <c r="N13" t="s">
         <v>78</v>
       </c>
-      <c r="Q13" s="28"/>
+      <c r="Q13" s="32"/>
       <c r="R13" t="s">
         <v>79</v>
       </c>
-      <c r="U13" s="28"/>
+      <c r="U13" s="32"/>
       <c r="V13" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+      <c r="A14" s="32"/>
       <c r="B14" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="28"/>
+      <c r="E14" s="32"/>
       <c r="F14" t="s">
         <v>95</v>
       </c>
-      <c r="I14" s="28"/>
+      <c r="I14" s="32"/>
       <c r="J14" t="s">
         <v>83</v>
       </c>
-      <c r="M14" s="28"/>
+      <c r="M14" s="32"/>
       <c r="N14" t="s">
         <v>84</v>
       </c>
-      <c r="Q14" s="28"/>
+      <c r="Q14" s="32"/>
       <c r="R14" t="s">
         <v>85</v>
       </c>
-      <c r="U14" s="28"/>
+      <c r="U14" s="32"/>
       <c r="V14" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
+      <c r="A15" s="32"/>
       <c r="B15" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="28"/>
+      <c r="E15" s="32"/>
       <c r="F15" t="s">
         <v>294</v>
       </c>
-      <c r="I15" s="28"/>
+      <c r="I15" s="32"/>
       <c r="J15" t="s">
         <v>89</v>
       </c>
-      <c r="M15" s="28"/>
+      <c r="M15" s="32"/>
       <c r="N15" t="s">
         <v>90</v>
       </c>
-      <c r="Q15" s="28"/>
+      <c r="Q15" s="32"/>
       <c r="R15" t="s">
         <v>91</v>
       </c>
-      <c r="U15" s="28"/>
+      <c r="U15" s="32"/>
       <c r="V15" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
+      <c r="A16" s="32"/>
       <c r="B16" t="s">
         <v>282</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="30" t="s">
         <v>93</v>
       </c>
       <c r="F16" t="s">
         <v>101</v>
       </c>
-      <c r="I16" s="28"/>
+      <c r="I16" s="32"/>
       <c r="J16" t="s">
         <v>96</v>
       </c>
-      <c r="M16" s="28"/>
+      <c r="M16" s="32"/>
       <c r="N16" t="s">
         <v>97</v>
       </c>
-      <c r="Q16" s="28"/>
+      <c r="Q16" s="32"/>
       <c r="R16" t="s">
         <v>98</v>
       </c>
-      <c r="U16" s="28"/>
+      <c r="U16" s="32"/>
       <c r="V16" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="30" t="s">
         <v>93</v>
       </c>
       <c r="B17" t="s">
         <v>94</v>
       </c>
-      <c r="E17" s="32"/>
+      <c r="E17" s="30"/>
       <c r="F17" t="s">
         <v>107</v>
       </c>
-      <c r="I17" s="28"/>
+      <c r="I17" s="32"/>
       <c r="J17" t="s">
         <v>102</v>
       </c>
-      <c r="M17" s="28"/>
+      <c r="M17" s="32"/>
       <c r="N17" t="s">
         <v>103</v>
       </c>
-      <c r="Q17" s="28"/>
+      <c r="Q17" s="32"/>
       <c r="R17" t="s">
         <v>104</v>
       </c>
-      <c r="U17" s="28"/>
+      <c r="U17" s="32"/>
       <c r="V17" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
+      <c r="A18" s="30"/>
       <c r="B18" t="s">
         <v>100</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="29" t="s">
         <v>113</v>
       </c>
       <c r="F18" t="s">
         <v>120</v>
       </c>
-      <c r="I18" s="28"/>
+      <c r="I18" s="32"/>
       <c r="J18" t="s">
         <v>108</v>
       </c>
-      <c r="M18" s="28"/>
+      <c r="M18" s="32"/>
       <c r="N18" t="s">
         <v>109</v>
       </c>
-      <c r="Q18" s="28"/>
+      <c r="Q18" s="32"/>
       <c r="R18" t="s">
         <v>110</v>
       </c>
-      <c r="U18" s="28"/>
+      <c r="U18" s="32"/>
       <c r="V18" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
+      <c r="A19" s="30"/>
       <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="E19" s="31"/>
+      <c r="E19" s="29"/>
       <c r="F19" t="s">
         <v>126</v>
       </c>
-      <c r="I19" s="28"/>
+      <c r="I19" s="32"/>
       <c r="J19" t="s">
         <v>115</v>
       </c>
-      <c r="M19" s="28"/>
+      <c r="M19" s="32"/>
       <c r="N19" t="s">
         <v>301</v>
       </c>
-      <c r="Q19" s="32" t="s">
+      <c r="Q19" s="30" t="s">
         <v>93</v>
       </c>
       <c r="R19" t="s">
         <v>117</v>
       </c>
-      <c r="U19" s="32" t="s">
+      <c r="U19" s="30" t="s">
         <v>93</v>
       </c>
       <c r="V19" t="s">
@@ -3209,11 +3215,11 @@
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
+      <c r="A20" s="30"/>
       <c r="B20" t="s">
         <v>112</v>
       </c>
-      <c r="E20" s="31"/>
+      <c r="E20" s="29"/>
       <c r="F20" t="s">
         <v>132</v>
       </c>
@@ -3223,49 +3229,49 @@
       <c r="J20" t="s">
         <v>121</v>
       </c>
-      <c r="M20" s="32" t="s">
+      <c r="M20" s="30" t="s">
         <v>93</v>
       </c>
       <c r="N20" t="s">
         <v>116</v>
       </c>
-      <c r="Q20" s="32"/>
+      <c r="Q20" s="30"/>
       <c r="R20" t="s">
         <v>123</v>
       </c>
-      <c r="U20" s="32"/>
+      <c r="U20" s="30"/>
       <c r="V20" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="29" t="s">
         <v>113</v>
       </c>
       <c r="B21" t="s">
         <v>119</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="26" t="s">
         <v>137</v>
       </c>
       <c r="F21" t="s">
         <v>139</v>
       </c>
-      <c r="I21" s="31" t="s">
+      <c r="I21" s="29" t="s">
         <v>113</v>
       </c>
       <c r="J21" t="s">
         <v>127</v>
       </c>
-      <c r="M21" s="32"/>
+      <c r="M21" s="30"/>
       <c r="N21" t="s">
         <v>122</v>
       </c>
-      <c r="Q21" s="32"/>
+      <c r="Q21" s="30"/>
       <c r="R21" t="s">
         <v>129</v>
       </c>
-      <c r="U21" s="31" t="s">
+      <c r="U21" s="29" t="s">
         <v>113</v>
       </c>
       <c r="V21" t="s">
@@ -3273,115 +3279,115 @@
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+      <c r="A22" s="29"/>
       <c r="B22" t="s">
         <v>131</v>
       </c>
-      <c r="E22" s="27"/>
+      <c r="E22" s="26"/>
       <c r="F22" t="s">
         <v>145</v>
       </c>
-      <c r="I22" s="31"/>
+      <c r="I22" s="29"/>
       <c r="J22" t="s">
         <v>133</v>
       </c>
-      <c r="M22" s="32"/>
+      <c r="M22" s="30"/>
       <c r="N22" t="s">
         <v>134</v>
       </c>
-      <c r="Q22" s="31" t="s">
+      <c r="Q22" s="29" t="s">
         <v>113</v>
       </c>
       <c r="R22" t="s">
         <v>135</v>
       </c>
-      <c r="U22" s="31"/>
+      <c r="U22" s="29"/>
       <c r="V22" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
+      <c r="A23" s="29"/>
       <c r="B23" t="s">
         <v>114</v>
       </c>
-      <c r="E23" s="27"/>
+      <c r="E23" s="26"/>
       <c r="F23" t="s">
         <v>151</v>
       </c>
-      <c r="I23" s="31"/>
+      <c r="I23" s="29"/>
       <c r="J23" t="s">
         <v>140</v>
       </c>
-      <c r="M23" s="31" t="s">
+      <c r="M23" s="29" t="s">
         <v>113</v>
       </c>
       <c r="N23" t="s">
         <v>141</v>
       </c>
-      <c r="Q23" s="31"/>
+      <c r="Q23" s="29"/>
       <c r="R23" t="s">
         <v>142</v>
       </c>
-      <c r="U23" s="31"/>
+      <c r="U23" s="29"/>
       <c r="V23" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="26" t="s">
         <v>137</v>
       </c>
       <c r="B24" t="s">
         <v>138</v>
       </c>
-      <c r="E24" s="27"/>
+      <c r="E24" s="26"/>
       <c r="F24" t="s">
         <v>157</v>
       </c>
-      <c r="I24" s="31"/>
+      <c r="I24" s="29"/>
       <c r="J24" t="s">
         <v>146</v>
       </c>
-      <c r="M24" s="31"/>
+      <c r="M24" s="29"/>
       <c r="N24" t="s">
         <v>147</v>
       </c>
-      <c r="Q24" s="31"/>
+      <c r="Q24" s="29"/>
       <c r="R24" t="s">
         <v>148</v>
       </c>
-      <c r="U24" s="31"/>
+      <c r="U24" s="29"/>
       <c r="V24" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
+      <c r="A25" s="26"/>
       <c r="B25" t="s">
         <v>144</v>
       </c>
-      <c r="E25" s="29" t="s">
+      <c r="E25" s="27" t="s">
         <v>167</v>
       </c>
       <c r="F25" t="s">
         <v>169</v>
       </c>
-      <c r="I25" s="27" t="s">
+      <c r="I25" s="26" t="s">
         <v>137</v>
       </c>
       <c r="J25" t="s">
         <v>152</v>
       </c>
-      <c r="M25" s="31"/>
+      <c r="M25" s="29"/>
       <c r="N25" t="s">
         <v>153</v>
       </c>
-      <c r="Q25" s="31"/>
+      <c r="Q25" s="29"/>
       <c r="R25" t="s">
         <v>154</v>
       </c>
-      <c r="U25" s="27" t="s">
+      <c r="U25" s="26" t="s">
         <v>137</v>
       </c>
       <c r="V25" t="s">
@@ -3389,105 +3395,105 @@
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
+      <c r="A26" s="26"/>
       <c r="B26" t="s">
         <v>150</v>
       </c>
-      <c r="E26" s="29"/>
+      <c r="E26" s="27"/>
       <c r="F26" t="s">
         <v>175</v>
       </c>
-      <c r="I26" s="27"/>
+      <c r="I26" s="26"/>
       <c r="J26" t="s">
         <v>158</v>
       </c>
-      <c r="M26" s="27" t="s">
+      <c r="M26" s="26" t="s">
         <v>137</v>
       </c>
       <c r="N26" t="s">
         <v>159</v>
       </c>
-      <c r="Q26" s="27" t="s">
+      <c r="Q26" s="26" t="s">
         <v>137</v>
       </c>
       <c r="R26" t="s">
         <v>160</v>
       </c>
-      <c r="U26" s="27"/>
+      <c r="U26" s="26"/>
       <c r="V26" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
+      <c r="A27" s="26"/>
       <c r="B27" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="29"/>
+      <c r="E27" s="27"/>
       <c r="F27" t="s">
         <v>181</v>
       </c>
-      <c r="I27" s="27"/>
+      <c r="I27" s="26"/>
       <c r="J27" t="s">
         <v>163</v>
       </c>
-      <c r="M27" s="27"/>
+      <c r="M27" s="26"/>
       <c r="N27" t="s">
         <v>164</v>
       </c>
-      <c r="Q27" s="27"/>
+      <c r="Q27" s="26"/>
       <c r="R27" t="s">
         <v>165</v>
       </c>
-      <c r="U27" s="27"/>
+      <c r="U27" s="26"/>
       <c r="V27" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="27" t="s">
         <v>167</v>
       </c>
       <c r="B28" t="s">
         <v>193</v>
       </c>
-      <c r="I28" s="27"/>
+      <c r="I28" s="26"/>
       <c r="J28" t="s">
         <v>170</v>
       </c>
-      <c r="M28" s="27"/>
+      <c r="M28" s="26"/>
       <c r="N28" t="s">
         <v>171</v>
       </c>
-      <c r="Q28" s="27"/>
+      <c r="Q28" s="26"/>
       <c r="R28" t="s">
         <v>172</v>
       </c>
-      <c r="U28" s="27"/>
+      <c r="U28" s="26"/>
       <c r="V28" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
+      <c r="A29" s="27"/>
       <c r="B29" t="s">
         <v>174</v>
       </c>
-      <c r="I29" s="29" t="s">
+      <c r="I29" s="27" t="s">
         <v>167</v>
       </c>
       <c r="J29" t="s">
         <v>176</v>
       </c>
-      <c r="M29" s="27"/>
+      <c r="M29" s="26"/>
       <c r="N29" t="s">
         <v>177</v>
       </c>
-      <c r="Q29" s="27"/>
+      <c r="Q29" s="26"/>
       <c r="R29" t="s">
         <v>178</v>
       </c>
-      <c r="U29" s="29" t="s">
+      <c r="U29" s="27" t="s">
         <v>167</v>
       </c>
       <c r="V29" t="s">
@@ -3495,145 +3501,145 @@
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
+      <c r="A30" s="27"/>
       <c r="B30" t="s">
         <v>192</v>
       </c>
-      <c r="I30" s="29"/>
+      <c r="I30" s="27"/>
       <c r="J30" t="s">
         <v>182</v>
       </c>
-      <c r="M30" s="29" t="s">
+      <c r="M30" s="27" t="s">
         <v>167</v>
       </c>
       <c r="N30" t="s">
         <v>183</v>
       </c>
-      <c r="Q30" s="29" t="s">
+      <c r="Q30" s="27" t="s">
         <v>167</v>
       </c>
       <c r="R30" t="s">
         <v>184</v>
       </c>
-      <c r="U30" s="29"/>
+      <c r="U30" s="27"/>
       <c r="V30" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
+      <c r="A31" s="27"/>
       <c r="B31" t="s">
         <v>180</v>
       </c>
-      <c r="I31" s="29"/>
+      <c r="I31" s="27"/>
       <c r="J31" t="s">
         <v>188</v>
       </c>
-      <c r="M31" s="29"/>
+      <c r="M31" s="27"/>
       <c r="N31" t="s">
         <v>189</v>
       </c>
-      <c r="Q31" s="29"/>
+      <c r="Q31" s="27"/>
       <c r="R31" t="s">
         <v>190</v>
       </c>
-      <c r="U31" s="29"/>
+      <c r="U31" s="27"/>
       <c r="V31" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
+      <c r="A32" s="27"/>
       <c r="B32" t="s">
         <v>186</v>
       </c>
-      <c r="I32" s="29"/>
+      <c r="I32" s="27"/>
       <c r="J32" t="s">
         <v>194</v>
       </c>
-      <c r="M32" s="29"/>
+      <c r="M32" s="27"/>
       <c r="N32" t="s">
         <v>195</v>
       </c>
-      <c r="Q32" s="29"/>
+      <c r="Q32" s="27"/>
       <c r="R32" t="s">
         <v>196</v>
       </c>
-      <c r="U32" s="29"/>
+      <c r="U32" s="27"/>
       <c r="V32" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
+      <c r="A33" s="27"/>
       <c r="B33" t="s">
         <v>168</v>
       </c>
-      <c r="I33" s="29"/>
+      <c r="I33" s="27"/>
       <c r="J33" t="s">
         <v>198</v>
       </c>
-      <c r="M33" s="29"/>
+      <c r="M33" s="27"/>
       <c r="N33" t="s">
         <v>199</v>
       </c>
-      <c r="Q33" s="29"/>
+      <c r="Q33" s="27"/>
       <c r="R33" t="s">
         <v>200</v>
       </c>
-      <c r="U33" s="29"/>
+      <c r="U33" s="27"/>
       <c r="V33" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="Q34" s="29"/>
+      <c r="Q34" s="27"/>
       <c r="R34" t="s">
         <v>202</v>
       </c>
       <c r="U34" s="3"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="E40" s="25" t="s">
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="E40" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="I40" s="25" t="s">
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="I40" s="31" t="s">
         <v>605</v>
       </c>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="31"/>
       <c r="L40" s="1"/>
-      <c r="M40" s="25" t="s">
+      <c r="M40" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="N40" s="25"/>
+      <c r="N40" s="31"/>
       <c r="O40" s="1"/>
-      <c r="Q40" s="25" t="s">
+      <c r="Q40" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="R40" s="25"/>
+      <c r="R40" s="31"/>
       <c r="S40" s="1"/>
-      <c r="U40" s="25" t="s">
+      <c r="U40" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="V40" s="25"/>
+      <c r="V40" s="31"/>
       <c r="W40" s="1"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A41" s="26" t="s">
+      <c r="A41" s="25" t="s">
         <v>6</v>
       </c>
       <c r="B41" t="s">
         <v>208</v>
       </c>
-      <c r="E41" s="26" t="s">
+      <c r="E41" s="25" t="s">
         <v>6</v>
       </c>
       <c r="F41" t="s">
@@ -3645,19 +3651,19 @@
       <c r="J41" t="s">
         <v>216</v>
       </c>
-      <c r="M41" s="26" t="s">
+      <c r="M41" s="25" t="s">
         <v>6</v>
       </c>
       <c r="N41" t="s">
         <v>211</v>
       </c>
-      <c r="Q41" s="26" t="s">
+      <c r="Q41" s="25" t="s">
         <v>6</v>
       </c>
       <c r="R41" t="s">
         <v>212</v>
       </c>
-      <c r="U41" s="26" t="s">
+      <c r="U41" s="25" t="s">
         <v>6</v>
       </c>
       <c r="V41" t="s">
@@ -3665,87 +3671,87 @@
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+      <c r="A42" s="25"/>
       <c r="B42" t="s">
         <v>214</v>
       </c>
-      <c r="E42" s="26"/>
+      <c r="E42" s="25"/>
       <c r="F42" t="s">
         <v>19</v>
       </c>
-      <c r="I42" s="30" t="s">
+      <c r="I42" s="28" t="s">
         <v>20</v>
       </c>
       <c r="J42" t="s">
         <v>222</v>
       </c>
-      <c r="M42" s="26"/>
+      <c r="M42" s="25"/>
       <c r="N42" t="s">
         <v>217</v>
       </c>
-      <c r="Q42" s="26"/>
+      <c r="Q42" s="25"/>
       <c r="R42" t="s">
         <v>218</v>
       </c>
-      <c r="U42" s="26"/>
+      <c r="U42" s="25"/>
       <c r="V42" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
+      <c r="A43" s="25"/>
       <c r="B43" t="s">
         <v>220</v>
       </c>
-      <c r="E43" s="26"/>
+      <c r="E43" s="25"/>
       <c r="F43" t="s">
         <v>215</v>
       </c>
-      <c r="I43" s="30"/>
+      <c r="I43" s="28"/>
       <c r="J43" t="s">
         <v>46</v>
       </c>
-      <c r="M43" s="26"/>
+      <c r="M43" s="25"/>
       <c r="N43" t="s">
         <v>223</v>
       </c>
-      <c r="Q43" s="30" t="s">
+      <c r="Q43" s="28" t="s">
         <v>20</v>
       </c>
       <c r="R43" t="s">
         <v>224</v>
       </c>
-      <c r="U43" s="26"/>
+      <c r="U43" s="25"/>
       <c r="V43" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A44" s="30" t="s">
+      <c r="A44" s="28" t="s">
         <v>20</v>
       </c>
       <c r="B44" t="s">
         <v>226</v>
       </c>
-      <c r="E44" s="26"/>
+      <c r="E44" s="25"/>
       <c r="F44" t="s">
         <v>221</v>
       </c>
-      <c r="I44" s="30"/>
+      <c r="I44" s="28"/>
       <c r="J44" t="s">
         <v>245</v>
       </c>
-      <c r="M44" s="30" t="s">
+      <c r="M44" s="28" t="s">
         <v>20</v>
       </c>
       <c r="N44" t="s">
         <v>229</v>
       </c>
-      <c r="Q44" s="30"/>
+      <c r="Q44" s="28"/>
       <c r="R44" t="s">
         <v>230</v>
       </c>
-      <c r="U44" s="30" t="s">
+      <c r="U44" s="28" t="s">
         <v>20</v>
       </c>
       <c r="V44" t="s">
@@ -3753,161 +3759,161 @@
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
+      <c r="A45" s="28"/>
       <c r="B45" t="s">
         <v>233</v>
       </c>
-      <c r="E45" s="30" t="s">
+      <c r="E45" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F45" t="s">
         <v>239</v>
       </c>
-      <c r="I45" s="30"/>
+      <c r="I45" s="28"/>
       <c r="J45" t="s">
         <v>234</v>
       </c>
-      <c r="M45" s="30"/>
+      <c r="M45" s="28"/>
       <c r="N45" t="s">
         <v>235</v>
       </c>
-      <c r="Q45" s="30"/>
+      <c r="Q45" s="28"/>
       <c r="R45" t="s">
         <v>236</v>
       </c>
-      <c r="U45" s="30"/>
+      <c r="U45" s="28"/>
       <c r="V45" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A46" s="30"/>
+      <c r="A46" s="28"/>
       <c r="B46" t="s">
         <v>232</v>
       </c>
-      <c r="E46" s="30"/>
+      <c r="E46" s="28"/>
       <c r="F46" t="s">
         <v>251</v>
       </c>
-      <c r="I46" s="30"/>
+      <c r="I46" s="28"/>
       <c r="J46" t="s">
         <v>252</v>
       </c>
-      <c r="M46" s="30"/>
+      <c r="M46" s="28"/>
       <c r="N46" t="s">
         <v>241</v>
       </c>
-      <c r="Q46" s="30"/>
+      <c r="Q46" s="28"/>
       <c r="R46" t="s">
         <v>242</v>
       </c>
-      <c r="U46" s="30"/>
+      <c r="U46" s="28"/>
       <c r="V46" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A47" s="30"/>
+      <c r="A47" s="28"/>
       <c r="B47" t="s">
         <v>238</v>
       </c>
-      <c r="E47" s="30"/>
+      <c r="E47" s="28"/>
       <c r="F47" t="s">
         <v>257</v>
       </c>
-      <c r="I47" s="30"/>
+      <c r="I47" s="28"/>
       <c r="J47" t="s">
         <v>258</v>
       </c>
-      <c r="M47" s="30"/>
+      <c r="M47" s="28"/>
       <c r="N47" t="s">
         <v>247</v>
       </c>
-      <c r="Q47" s="30"/>
+      <c r="Q47" s="28"/>
       <c r="R47" t="s">
         <v>248</v>
       </c>
-      <c r="U47" s="30"/>
+      <c r="U47" s="28"/>
       <c r="V47" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
+      <c r="A48" s="28"/>
       <c r="B48" t="s">
         <v>244</v>
       </c>
-      <c r="E48" s="30"/>
+      <c r="E48" s="28"/>
       <c r="F48" t="s">
         <v>263</v>
       </c>
-      <c r="I48" s="30"/>
+      <c r="I48" s="28"/>
       <c r="J48" t="s">
         <v>264</v>
       </c>
-      <c r="M48" s="30"/>
+      <c r="M48" s="28"/>
       <c r="N48" t="s">
         <v>253</v>
       </c>
-      <c r="Q48" s="30"/>
+      <c r="Q48" s="28"/>
       <c r="R48" t="s">
         <v>254</v>
       </c>
-      <c r="U48" s="30"/>
+      <c r="U48" s="28"/>
       <c r="V48" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
+      <c r="A49" s="28"/>
       <c r="B49" t="s">
         <v>250</v>
       </c>
-      <c r="E49" s="30"/>
+      <c r="E49" s="28"/>
       <c r="F49" t="s">
         <v>240</v>
       </c>
-      <c r="I49" s="30"/>
+      <c r="I49" s="28"/>
       <c r="J49" t="s">
         <v>228</v>
       </c>
-      <c r="M49" s="30"/>
+      <c r="M49" s="28"/>
       <c r="N49" t="s">
         <v>259</v>
       </c>
-      <c r="Q49" s="30"/>
+      <c r="Q49" s="28"/>
       <c r="R49" t="s">
         <v>260</v>
       </c>
-      <c r="U49" s="30"/>
+      <c r="U49" s="28"/>
       <c r="V49" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A50" s="30"/>
+      <c r="A50" s="28"/>
       <c r="B50" t="s">
         <v>256</v>
       </c>
-      <c r="E50" s="28" t="s">
+      <c r="E50" s="32" t="s">
         <v>44</v>
       </c>
       <c r="F50" t="s">
         <v>269</v>
       </c>
-      <c r="I50" s="30"/>
+      <c r="I50" s="28"/>
       <c r="J50" t="s">
         <v>246</v>
       </c>
-      <c r="M50" s="30"/>
+      <c r="M50" s="28"/>
       <c r="N50" t="s">
         <v>265</v>
       </c>
-      <c r="Q50" s="30"/>
+      <c r="Q50" s="28"/>
       <c r="R50" t="s">
         <v>266</v>
       </c>
-      <c r="U50" s="28" t="s">
+      <c r="U50" s="32" t="s">
         <v>44</v>
       </c>
       <c r="V50" t="s">
@@ -3915,273 +3921,273 @@
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A51" s="30"/>
+      <c r="A51" s="28"/>
       <c r="B51" t="s">
         <v>262</v>
       </c>
-      <c r="E51" s="28"/>
+      <c r="E51" s="32"/>
       <c r="F51" t="s">
         <v>275</v>
       </c>
-      <c r="I51" s="28" t="s">
+      <c r="I51" s="32" t="s">
         <v>44</v>
       </c>
       <c r="J51" t="s">
         <v>76</v>
       </c>
-      <c r="M51" s="28" t="s">
+      <c r="M51" s="32" t="s">
         <v>44</v>
       </c>
       <c r="N51" t="s">
         <v>271</v>
       </c>
-      <c r="Q51" s="28" t="s">
+      <c r="Q51" s="32" t="s">
         <v>44</v>
       </c>
       <c r="R51" t="s">
         <v>272</v>
       </c>
-      <c r="U51" s="28"/>
+      <c r="U51" s="32"/>
       <c r="V51" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A52" s="28" t="s">
+      <c r="A52" s="32" t="s">
         <v>44</v>
       </c>
       <c r="B52" t="s">
         <v>268</v>
       </c>
-      <c r="E52" s="28"/>
+      <c r="E52" s="32"/>
       <c r="F52" t="s">
         <v>63</v>
       </c>
-      <c r="I52" s="28"/>
+      <c r="I52" s="32"/>
       <c r="J52" t="s">
         <v>276</v>
       </c>
-      <c r="M52" s="28"/>
+      <c r="M52" s="32"/>
       <c r="N52" t="s">
         <v>277</v>
       </c>
-      <c r="Q52" s="28"/>
+      <c r="Q52" s="32"/>
       <c r="R52" t="s">
         <v>278</v>
       </c>
-      <c r="U52" s="28"/>
+      <c r="U52" s="32"/>
       <c r="V52" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A53" s="28"/>
+      <c r="A53" s="32"/>
       <c r="B53" t="s">
         <v>274</v>
       </c>
-      <c r="E53" s="28"/>
+      <c r="E53" s="32"/>
       <c r="F53" t="s">
         <v>287</v>
       </c>
-      <c r="I53" s="28"/>
+      <c r="I53" s="32"/>
       <c r="J53" t="s">
         <v>300</v>
       </c>
-      <c r="M53" s="28"/>
+      <c r="M53" s="32"/>
       <c r="N53" t="s">
         <v>283</v>
       </c>
-      <c r="Q53" s="28"/>
+      <c r="Q53" s="32"/>
       <c r="R53" t="s">
         <v>284</v>
       </c>
-      <c r="U53" s="28"/>
+      <c r="U53" s="32"/>
       <c r="V53" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A54" s="28"/>
+      <c r="A54" s="32"/>
       <c r="B54" t="s">
         <v>280</v>
       </c>
-      <c r="E54" s="28"/>
+      <c r="E54" s="32"/>
       <c r="F54" t="s">
         <v>293</v>
       </c>
-      <c r="I54" s="28"/>
+      <c r="I54" s="32"/>
       <c r="J54" t="s">
         <v>288</v>
       </c>
-      <c r="M54" s="28"/>
+      <c r="M54" s="32"/>
       <c r="N54" t="s">
         <v>289</v>
       </c>
-      <c r="Q54" s="28"/>
+      <c r="Q54" s="32"/>
       <c r="R54" t="s">
         <v>290</v>
       </c>
-      <c r="U54" s="28"/>
+      <c r="U54" s="32"/>
       <c r="V54" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A55" s="28"/>
+      <c r="A55" s="32"/>
       <c r="B55" t="s">
         <v>286</v>
       </c>
-      <c r="E55" s="28"/>
+      <c r="E55" s="32"/>
       <c r="F55" t="s">
         <v>312</v>
       </c>
-      <c r="I55" s="28"/>
+      <c r="I55" s="32"/>
       <c r="J55" t="s">
         <v>306</v>
       </c>
-      <c r="M55" s="28"/>
+      <c r="M55" s="32"/>
       <c r="N55" t="s">
         <v>295</v>
       </c>
-      <c r="Q55" s="28"/>
+      <c r="Q55" s="32"/>
       <c r="R55" t="s">
         <v>296</v>
       </c>
-      <c r="U55" s="28"/>
+      <c r="U55" s="32"/>
       <c r="V55" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A56" s="28"/>
+      <c r="A56" s="32"/>
       <c r="B56" t="s">
         <v>292</v>
       </c>
-      <c r="E56" s="28"/>
+      <c r="E56" s="32"/>
       <c r="F56" t="s">
         <v>311</v>
       </c>
-      <c r="I56" s="28"/>
+      <c r="I56" s="32"/>
       <c r="J56" t="s">
         <v>57</v>
       </c>
-      <c r="M56" s="28"/>
+      <c r="M56" s="32"/>
       <c r="N56" t="s">
         <v>307</v>
       </c>
-      <c r="Q56" s="28"/>
+      <c r="Q56" s="32"/>
       <c r="R56" t="s">
         <v>302</v>
       </c>
-      <c r="U56" s="28"/>
+      <c r="U56" s="32"/>
       <c r="V56" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A57" s="28"/>
+      <c r="A57" s="32"/>
       <c r="B57" t="s">
         <v>298</v>
       </c>
-      <c r="E57" s="28"/>
+      <c r="E57" s="32"/>
       <c r="F57" t="s">
         <v>317</v>
       </c>
-      <c r="I57" s="32" t="s">
+      <c r="I57" s="30" t="s">
         <v>93</v>
       </c>
       <c r="J57" t="s">
         <v>318</v>
       </c>
-      <c r="M57" s="28"/>
+      <c r="M57" s="32"/>
       <c r="N57" t="s">
         <v>313</v>
       </c>
-      <c r="Q57" s="28"/>
+      <c r="Q57" s="32"/>
       <c r="R57" t="s">
         <v>308</v>
       </c>
-      <c r="U57" s="28"/>
+      <c r="U57" s="32"/>
       <c r="V57" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A58" s="28"/>
+      <c r="A58" s="32"/>
       <c r="B58" t="s">
         <v>304</v>
       </c>
-      <c r="E58" s="28"/>
+      <c r="E58" s="32"/>
       <c r="F58" t="s">
         <v>323</v>
       </c>
-      <c r="I58" s="32"/>
+      <c r="I58" s="30"/>
       <c r="J58" t="s">
         <v>353</v>
       </c>
-      <c r="M58" s="32" t="s">
+      <c r="M58" s="30" t="s">
         <v>93</v>
       </c>
       <c r="N58" t="s">
         <v>319</v>
       </c>
-      <c r="Q58" s="28"/>
+      <c r="Q58" s="32"/>
       <c r="R58" t="s">
         <v>314</v>
       </c>
-      <c r="U58" s="28"/>
+      <c r="U58" s="32"/>
       <c r="V58" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A59" s="28"/>
+      <c r="A59" s="32"/>
       <c r="B59" t="s">
         <v>310</v>
       </c>
-      <c r="E59" s="28"/>
+      <c r="E59" s="32"/>
       <c r="F59" t="s">
         <v>329</v>
       </c>
-      <c r="I59" s="32"/>
+      <c r="I59" s="30"/>
       <c r="J59" t="s">
-        <v>330</v>
-      </c>
-      <c r="M59" s="32"/>
+        <v>336</v>
+      </c>
+      <c r="M59" s="30"/>
       <c r="N59" t="s">
         <v>325</v>
       </c>
-      <c r="Q59" s="28"/>
+      <c r="Q59" s="32"/>
       <c r="R59" t="s">
         <v>320</v>
       </c>
-      <c r="U59" s="28"/>
+      <c r="U59" s="32"/>
       <c r="V59" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A60" s="28"/>
+      <c r="A60" s="32"/>
       <c r="B60" t="s">
         <v>316</v>
       </c>
-      <c r="E60" s="28"/>
+      <c r="E60" s="32"/>
       <c r="F60" t="s">
         <v>335</v>
       </c>
-      <c r="I60" s="32"/>
+      <c r="I60" s="30"/>
       <c r="J60" t="s">
-        <v>336</v>
-      </c>
-      <c r="M60" s="32"/>
+        <v>324</v>
+      </c>
+      <c r="M60" s="30"/>
       <c r="N60" t="s">
         <v>331</v>
       </c>
-      <c r="Q60" s="28"/>
+      <c r="Q60" s="32"/>
       <c r="R60" t="s">
         <v>326</v>
       </c>
-      <c r="U60" s="32" t="s">
+      <c r="U60" s="30" t="s">
         <v>93</v>
       </c>
       <c r="V60" t="s">
@@ -4189,59 +4195,59 @@
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A61" s="28"/>
+      <c r="A61" s="32"/>
       <c r="B61" t="s">
         <v>322</v>
       </c>
-      <c r="E61" s="28"/>
+      <c r="E61" s="32"/>
       <c r="F61" t="s">
         <v>299</v>
       </c>
-      <c r="I61" s="32"/>
+      <c r="I61" s="29" t="s">
+        <v>113</v>
+      </c>
       <c r="J61" t="s">
-        <v>324</v>
-      </c>
-      <c r="M61" s="32"/>
+        <v>342</v>
+      </c>
+      <c r="M61" s="30"/>
       <c r="N61" t="s">
         <v>128</v>
       </c>
-      <c r="Q61" s="28"/>
+      <c r="Q61" s="32"/>
       <c r="R61" t="s">
         <v>332</v>
       </c>
-      <c r="U61" s="32"/>
+      <c r="U61" s="30"/>
       <c r="V61" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A62" s="28"/>
+      <c r="A62" s="32"/>
       <c r="B62" t="s">
         <v>305</v>
       </c>
-      <c r="E62" s="32" t="s">
+      <c r="E62" s="30" t="s">
         <v>93</v>
       </c>
       <c r="F62" t="s">
         <v>341</v>
       </c>
-      <c r="I62" s="31" t="s">
-        <v>113</v>
-      </c>
+      <c r="I62" s="29"/>
       <c r="J62" t="s">
-        <v>342</v>
-      </c>
-      <c r="M62" s="31" t="s">
+        <v>348</v>
+      </c>
+      <c r="M62" s="29" t="s">
         <v>113</v>
       </c>
       <c r="N62" t="s">
         <v>337</v>
       </c>
-      <c r="Q62" s="28"/>
+      <c r="Q62" s="32"/>
       <c r="R62" t="s">
         <v>338</v>
       </c>
-      <c r="U62" s="31" t="s">
+      <c r="U62" s="29" t="s">
         <v>113</v>
       </c>
       <c r="V62" t="s">
@@ -4249,87 +4255,89 @@
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A63" s="32" t="s">
+      <c r="A63" s="30" t="s">
         <v>93</v>
       </c>
       <c r="B63" t="s">
         <v>328</v>
       </c>
-      <c r="E63" s="32"/>
+      <c r="E63" s="30"/>
       <c r="F63" t="s">
         <v>347</v>
       </c>
-      <c r="I63" s="31"/>
+      <c r="I63" s="29"/>
       <c r="J63" t="s">
-        <v>348</v>
-      </c>
-      <c r="M63" s="31"/>
+        <v>354</v>
+      </c>
+      <c r="M63" s="29"/>
       <c r="N63" t="s">
         <v>343</v>
       </c>
-      <c r="Q63" s="28"/>
+      <c r="Q63" s="32"/>
       <c r="R63" t="s">
         <v>344</v>
       </c>
-      <c r="U63" s="31"/>
+      <c r="U63" s="29"/>
       <c r="V63" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A64" s="32"/>
+      <c r="A64" s="30"/>
       <c r="B64" t="s">
         <v>334</v>
       </c>
-      <c r="E64" s="32"/>
+      <c r="E64" s="30"/>
       <c r="F64" t="s">
         <v>359</v>
       </c>
-      <c r="I64" s="31"/>
+      <c r="I64" s="29"/>
       <c r="J64" t="s">
-        <v>354</v>
-      </c>
-      <c r="M64" s="31"/>
+        <v>360</v>
+      </c>
+      <c r="M64" s="29"/>
       <c r="N64" t="s">
         <v>349</v>
       </c>
-      <c r="Q64" s="32" t="s">
+      <c r="Q64" s="30" t="s">
         <v>93</v>
       </c>
       <c r="R64" t="s">
         <v>350</v>
       </c>
-      <c r="U64" s="31"/>
+      <c r="U64" s="29"/>
       <c r="V64" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A65" s="32"/>
+      <c r="A65" s="30"/>
       <c r="B65" t="s">
         <v>340</v>
       </c>
-      <c r="E65" s="31" t="s">
+      <c r="E65" s="29" t="s">
         <v>113</v>
       </c>
       <c r="F65" t="s">
         <v>365</v>
       </c>
-      <c r="I65" s="31"/>
+      <c r="I65" s="26" t="s">
+        <v>137</v>
+      </c>
       <c r="J65" t="s">
-        <v>360</v>
-      </c>
-      <c r="M65" s="27" t="s">
+        <v>372</v>
+      </c>
+      <c r="M65" s="26" t="s">
         <v>137</v>
       </c>
       <c r="N65" t="s">
         <v>355</v>
       </c>
-      <c r="Q65" s="32"/>
+      <c r="Q65" s="30"/>
       <c r="R65" t="s">
         <v>356</v>
       </c>
-      <c r="U65" s="27" t="s">
+      <c r="U65" s="26" t="s">
         <v>137</v>
       </c>
       <c r="V65" t="s">
@@ -4337,143 +4345,139 @@
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A66" s="32"/>
+      <c r="A66" s="30"/>
       <c r="B66" t="s">
         <v>346</v>
       </c>
-      <c r="E66" s="31"/>
+      <c r="E66" s="29"/>
       <c r="F66" t="s">
         <v>371</v>
       </c>
-      <c r="I66" s="27" t="s">
-        <v>137</v>
-      </c>
+      <c r="I66" s="26"/>
       <c r="J66" t="s">
-        <v>372</v>
-      </c>
-      <c r="M66" s="27"/>
+        <v>384</v>
+      </c>
+      <c r="M66" s="26"/>
       <c r="N66" t="s">
         <v>361</v>
       </c>
-      <c r="Q66" s="31" t="s">
+      <c r="Q66" s="29" t="s">
         <v>113</v>
       </c>
       <c r="R66" t="s">
         <v>362</v>
       </c>
-      <c r="U66" s="27"/>
+      <c r="U66" s="26"/>
       <c r="V66" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A67" s="31" t="s">
-        <v>113</v>
-      </c>
+      <c r="A67" s="30"/>
       <c r="B67" t="s">
-        <v>352</v>
-      </c>
-      <c r="E67" s="31"/>
+        <v>330</v>
+      </c>
+      <c r="E67" s="29"/>
       <c r="F67" t="s">
         <v>377</v>
       </c>
-      <c r="I67" s="27"/>
+      <c r="I67" s="26"/>
       <c r="J67" t="s">
-        <v>384</v>
-      </c>
-      <c r="M67" s="27"/>
+        <v>162</v>
+      </c>
+      <c r="M67" s="26"/>
       <c r="N67" t="s">
         <v>156</v>
       </c>
-      <c r="Q67" s="31"/>
+      <c r="Q67" s="29"/>
       <c r="R67" t="s">
         <v>368</v>
       </c>
-      <c r="U67" s="27"/>
+      <c r="U67" s="26"/>
       <c r="V67" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A68" s="31"/>
+      <c r="A68" s="29" t="s">
+        <v>113</v>
+      </c>
       <c r="B68" t="s">
-        <v>358</v>
-      </c>
-      <c r="E68" s="31"/>
+        <v>352</v>
+      </c>
+      <c r="E68" s="29"/>
       <c r="F68" t="s">
         <v>125</v>
       </c>
-      <c r="I68" s="27"/>
+      <c r="I68" s="26"/>
       <c r="J68" t="s">
-        <v>162</v>
-      </c>
-      <c r="M68" s="27"/>
+        <v>407</v>
+      </c>
+      <c r="M68" s="26"/>
       <c r="N68" t="s">
         <v>373</v>
       </c>
-      <c r="Q68" s="31"/>
+      <c r="Q68" s="29"/>
       <c r="R68" t="s">
         <v>374</v>
       </c>
-      <c r="U68" s="27"/>
+      <c r="U68" s="26"/>
       <c r="V68" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A69" s="31"/>
+      <c r="A69" s="29"/>
       <c r="B69" t="s">
-        <v>364</v>
-      </c>
-      <c r="E69" s="27" t="s">
+        <v>358</v>
+      </c>
+      <c r="E69" s="26" t="s">
         <v>137</v>
       </c>
       <c r="F69" t="s">
         <v>383</v>
       </c>
-      <c r="I69" s="27"/>
+      <c r="I69" s="26"/>
       <c r="J69" t="s">
-        <v>407</v>
-      </c>
-      <c r="M69" s="27"/>
+        <v>366</v>
+      </c>
+      <c r="M69" s="26"/>
       <c r="N69" t="s">
         <v>379</v>
       </c>
-      <c r="Q69" s="31"/>
+      <c r="Q69" s="29"/>
       <c r="R69" t="s">
         <v>380</v>
       </c>
-      <c r="U69" s="27"/>
+      <c r="U69" s="26"/>
       <c r="V69" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A70" s="27" t="s">
-        <v>137</v>
-      </c>
+      <c r="A70" s="29"/>
       <c r="B70" t="s">
-        <v>370</v>
-      </c>
-      <c r="E70" s="27"/>
+        <v>364</v>
+      </c>
+      <c r="E70" s="26"/>
       <c r="F70" t="s">
         <v>389</v>
       </c>
-      <c r="I70" s="27"/>
+      <c r="I70" s="26"/>
       <c r="J70" t="s">
-        <v>366</v>
-      </c>
-      <c r="M70" s="27"/>
+        <v>378</v>
+      </c>
+      <c r="M70" s="26"/>
       <c r="N70" t="s">
         <v>367</v>
       </c>
-      <c r="Q70" s="27" t="s">
+      <c r="Q70" s="26" t="s">
         <v>137</v>
       </c>
       <c r="R70" t="s">
         <v>386</v>
       </c>
-      <c r="U70" s="29" t="s">
+      <c r="U70" s="27" t="s">
         <v>167</v>
       </c>
       <c r="V70" t="s">
@@ -4481,237 +4485,163 @@
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A71" s="27"/>
+      <c r="A71" s="26" t="s">
+        <v>137</v>
+      </c>
       <c r="B71" t="s">
-        <v>376</v>
-      </c>
-      <c r="E71" s="27"/>
+        <v>370</v>
+      </c>
+      <c r="E71" s="26"/>
       <c r="F71" t="s">
         <v>395</v>
       </c>
-      <c r="I71" s="27"/>
+      <c r="I71" s="27" t="s">
+        <v>167</v>
+      </c>
       <c r="J71" t="s">
-        <v>378</v>
-      </c>
-      <c r="M71" s="29" t="s">
+        <v>390</v>
+      </c>
+      <c r="M71" s="27" t="s">
         <v>167</v>
       </c>
       <c r="N71" t="s">
         <v>385</v>
       </c>
-      <c r="Q71" s="27"/>
+      <c r="Q71" s="26"/>
       <c r="R71" t="s">
         <v>392</v>
       </c>
-      <c r="U71" s="29"/>
+      <c r="U71" s="27"/>
       <c r="V71" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A72" s="27"/>
+      <c r="A72" s="26"/>
       <c r="B72" t="s">
-        <v>382</v>
-      </c>
-      <c r="E72" s="27"/>
+        <v>376</v>
+      </c>
+      <c r="E72" s="26"/>
       <c r="F72" t="s">
         <v>401</v>
       </c>
-      <c r="I72" s="29" t="s">
-        <v>167</v>
-      </c>
+      <c r="I72" s="27"/>
       <c r="J72" t="s">
-        <v>390</v>
-      </c>
-      <c r="M72" s="29"/>
+        <v>402</v>
+      </c>
+      <c r="M72" s="27"/>
       <c r="N72" t="s">
         <v>391</v>
       </c>
-      <c r="Q72" s="27"/>
+      <c r="Q72" s="26"/>
       <c r="R72" t="s">
         <v>398</v>
       </c>
-      <c r="U72" s="29"/>
+      <c r="U72" s="27"/>
       <c r="V72" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A73" s="27"/>
+      <c r="A73" s="26"/>
       <c r="B73" t="s">
-        <v>388</v>
-      </c>
-      <c r="E73" s="29" t="s">
+        <v>382</v>
+      </c>
+      <c r="E73" s="27" t="s">
         <v>167</v>
       </c>
       <c r="F73" t="s">
         <v>406</v>
       </c>
-      <c r="I73" s="29"/>
+      <c r="I73" s="27"/>
       <c r="J73" t="s">
-        <v>402</v>
-      </c>
-      <c r="M73" s="29"/>
+        <v>411</v>
+      </c>
+      <c r="M73" s="27"/>
       <c r="N73" t="s">
         <v>397</v>
       </c>
-      <c r="Q73" s="27"/>
+      <c r="Q73" s="26"/>
       <c r="R73" t="s">
         <v>403</v>
       </c>
-      <c r="U73" s="29"/>
+      <c r="U73" s="27"/>
       <c r="V73" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A74" s="29" t="s">
-        <v>167</v>
-      </c>
+      <c r="A74" s="26"/>
       <c r="B74" t="s">
-        <v>394</v>
-      </c>
-      <c r="E74" s="29"/>
+        <v>388</v>
+      </c>
+      <c r="E74" s="27"/>
       <c r="F74" t="s">
         <v>410</v>
       </c>
-      <c r="I74" s="29"/>
+      <c r="I74" s="27"/>
       <c r="J74" t="s">
-        <v>411</v>
-      </c>
-      <c r="Q74" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q74" s="27" t="s">
         <v>167</v>
       </c>
       <c r="R74" t="s">
         <v>408</v>
       </c>
-      <c r="U74" s="29"/>
+      <c r="U74" s="27"/>
       <c r="V74" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A75" s="29"/>
+      <c r="A75" s="27" t="s">
+        <v>167</v>
+      </c>
       <c r="B75" t="s">
-        <v>400</v>
-      </c>
-      <c r="E75" s="29"/>
+        <v>394</v>
+      </c>
+      <c r="E75" s="27"/>
       <c r="F75" t="s">
         <v>413</v>
       </c>
-      <c r="I75" s="29"/>
+      <c r="I75" s="27"/>
       <c r="J75" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q75" s="29"/>
+        <v>396</v>
+      </c>
+      <c r="Q75" s="27"/>
       <c r="R75" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A76" s="29"/>
+      <c r="A76" s="27"/>
       <c r="B76" t="s">
-        <v>405</v>
-      </c>
-      <c r="I76" s="29"/>
-      <c r="J76" t="s">
-        <v>396</v>
-      </c>
-      <c r="Q76" s="29"/>
+        <v>400</v>
+      </c>
+      <c r="Q76" s="27"/>
       <c r="R76" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A77" s="29"/>
+      <c r="A77" s="27"/>
       <c r="B77" t="s">
-        <v>409</v>
-      </c>
-      <c r="Q77" s="29"/>
+        <v>405</v>
+      </c>
+      <c r="Q77" s="27"/>
       <c r="R77" t="s">
         <v>415</v>
       </c>
     </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A78" s="27"/>
+      <c r="B78" t="s">
+        <v>409</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="E41:E44"/>
-    <mergeCell ref="E21:E24"/>
-    <mergeCell ref="Q74:Q77"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A28:A33"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="M65:M70"/>
-    <mergeCell ref="E65:E68"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="M41:M43"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="U41:U43"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="U40:V40"/>
-    <mergeCell ref="U44:U49"/>
-    <mergeCell ref="U60:U61"/>
-    <mergeCell ref="U50:U59"/>
-    <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="Q43:Q50"/>
-    <mergeCell ref="E62:E64"/>
-    <mergeCell ref="I57:I61"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="I4:I11"/>
-    <mergeCell ref="M5:M11"/>
-    <mergeCell ref="E4:E9"/>
-    <mergeCell ref="M20:M22"/>
-    <mergeCell ref="M12:M19"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="I29:I33"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="A44:A51"/>
-    <mergeCell ref="A52:A62"/>
-    <mergeCell ref="M44:M50"/>
-    <mergeCell ref="U70:U74"/>
-    <mergeCell ref="E69:E72"/>
-    <mergeCell ref="M71:M73"/>
-    <mergeCell ref="Q70:Q73"/>
-    <mergeCell ref="M62:M64"/>
-    <mergeCell ref="I62:I65"/>
-    <mergeCell ref="I51:I56"/>
-    <mergeCell ref="I42:I50"/>
-    <mergeCell ref="I72:I76"/>
-    <mergeCell ref="E45:E49"/>
-    <mergeCell ref="E50:E61"/>
-    <mergeCell ref="M51:M57"/>
-    <mergeCell ref="M58:M61"/>
-    <mergeCell ref="E73:E75"/>
-    <mergeCell ref="I66:I71"/>
-    <mergeCell ref="M30:M33"/>
-    <mergeCell ref="U19:U20"/>
-    <mergeCell ref="I21:I24"/>
-    <mergeCell ref="U21:U24"/>
-    <mergeCell ref="Q22:Q25"/>
-    <mergeCell ref="M23:M25"/>
-    <mergeCell ref="I25:I28"/>
-    <mergeCell ref="U25:U28"/>
-    <mergeCell ref="M26:M29"/>
-    <mergeCell ref="Q26:Q29"/>
-    <mergeCell ref="Q30:Q34"/>
-    <mergeCell ref="I12:I19"/>
-    <mergeCell ref="U29:U33"/>
-    <mergeCell ref="Q51:Q63"/>
-    <mergeCell ref="U5:U10"/>
-    <mergeCell ref="U11:U18"/>
-    <mergeCell ref="Q12:Q18"/>
-    <mergeCell ref="U62:U64"/>
-    <mergeCell ref="Q64:Q65"/>
-    <mergeCell ref="U65:U69"/>
-    <mergeCell ref="Q66:Q69"/>
-    <mergeCell ref="Q19:Q21"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="I2:I3"/>
@@ -4728,6 +4658,84 @@
     <mergeCell ref="E25:E27"/>
     <mergeCell ref="E10:E15"/>
     <mergeCell ref="Q5:Q11"/>
+    <mergeCell ref="Q30:Q34"/>
+    <mergeCell ref="I12:I19"/>
+    <mergeCell ref="U29:U33"/>
+    <mergeCell ref="Q51:Q63"/>
+    <mergeCell ref="U5:U10"/>
+    <mergeCell ref="U11:U18"/>
+    <mergeCell ref="Q12:Q18"/>
+    <mergeCell ref="U62:U64"/>
+    <mergeCell ref="Q64:Q65"/>
+    <mergeCell ref="U65:U69"/>
+    <mergeCell ref="Q66:Q69"/>
+    <mergeCell ref="Q19:Q21"/>
+    <mergeCell ref="I57:I60"/>
+    <mergeCell ref="U19:U20"/>
+    <mergeCell ref="I21:I24"/>
+    <mergeCell ref="U21:U24"/>
+    <mergeCell ref="Q22:Q25"/>
+    <mergeCell ref="M23:M25"/>
+    <mergeCell ref="I25:I28"/>
+    <mergeCell ref="U25:U28"/>
+    <mergeCell ref="M26:M29"/>
+    <mergeCell ref="Q26:Q29"/>
+    <mergeCell ref="U70:U74"/>
+    <mergeCell ref="E69:E72"/>
+    <mergeCell ref="M71:M73"/>
+    <mergeCell ref="Q70:Q73"/>
+    <mergeCell ref="M62:M64"/>
+    <mergeCell ref="I61:I64"/>
+    <mergeCell ref="I71:I75"/>
+    <mergeCell ref="E73:E75"/>
+    <mergeCell ref="I65:I70"/>
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="I29:I33"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="A44:A51"/>
+    <mergeCell ref="A52:A62"/>
+    <mergeCell ref="I51:I56"/>
+    <mergeCell ref="I42:I50"/>
+    <mergeCell ref="E45:E49"/>
+    <mergeCell ref="E50:E61"/>
+    <mergeCell ref="A63:A67"/>
+    <mergeCell ref="I4:I11"/>
+    <mergeCell ref="M5:M11"/>
+    <mergeCell ref="E4:E9"/>
+    <mergeCell ref="M20:M22"/>
+    <mergeCell ref="M12:M19"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="M44:M50"/>
+    <mergeCell ref="M51:M57"/>
+    <mergeCell ref="M58:M61"/>
+    <mergeCell ref="M30:M33"/>
+    <mergeCell ref="U41:U43"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="U40:V40"/>
+    <mergeCell ref="U44:U49"/>
+    <mergeCell ref="U60:U61"/>
+    <mergeCell ref="U50:U59"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="Q43:Q50"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="E41:E44"/>
+    <mergeCell ref="E21:E24"/>
+    <mergeCell ref="Q74:Q77"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="M65:M70"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="M41:M43"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="E62:E64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4738,8 +4746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4761,34 +4769,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="E1" s="25" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="E1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="25"/>
+      <c r="F1" s="31"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="25"/>
-      <c r="O1" s="25" t="s">
+      <c r="M1" s="31"/>
+      <c r="O1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="25"/>
-      <c r="R1" s="25" t="s">
+      <c r="P1" s="31"/>
+      <c r="R1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="25"/>
+      <c r="S1" s="31"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -5001,40 +5009,40 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="E17" s="25" t="s">
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="E17" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="I17" s="25" t="s">
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="I17" s="31" t="s">
         <v>605</v>
       </c>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25" t="s">
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="M17" s="25"/>
-      <c r="O17" s="25" t="s">
+      <c r="M17" s="31"/>
+      <c r="O17" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="P17" s="25"/>
-      <c r="R17" s="25" t="s">
+      <c r="P17" s="31"/>
+      <c r="R17" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="S17" s="25"/>
+      <c r="S17" s="31"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>635</v>
+        <v>480</v>
       </c>
       <c r="C18" t="s">
-        <v>438</v>
+        <v>498</v>
       </c>
       <c r="E18" t="s">
         <v>624</v>
@@ -5062,9 +5070,6 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>480</v>
-      </c>
       <c r="C19" t="s">
         <v>491</v>
       </c>
@@ -5078,7 +5083,7 @@
         <v>621</v>
       </c>
       <c r="J19" t="s">
-        <v>477</v>
+        <v>438</v>
       </c>
       <c r="L19" t="s">
         <v>496</v>
@@ -5104,7 +5109,7 @@
         <v>622</v>
       </c>
       <c r="J20" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="O20" t="s">
         <v>504</v>
@@ -5127,10 +5132,10 @@
         <v>470</v>
       </c>
       <c r="I21" t="s">
-        <v>626</v>
+        <v>635</v>
       </c>
       <c r="J21" t="s">
-        <v>498</v>
+        <v>478</v>
       </c>
       <c r="L21" t="s">
         <v>511</v>
@@ -5153,10 +5158,7 @@
         <v>500</v>
       </c>
       <c r="I22" t="s">
-        <v>501</v>
-      </c>
-      <c r="J22" t="s">
-        <v>510</v>
+        <v>626</v>
       </c>
       <c r="O22" t="s">
         <v>518</v>
@@ -5173,10 +5175,10 @@
         <v>508</v>
       </c>
       <c r="I23" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="J23" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="O23" t="s">
         <v>521</v>
@@ -5190,7 +5192,10 @@
         <v>469</v>
       </c>
       <c r="I24" t="s">
-        <v>516</v>
+        <v>509</v>
+      </c>
+      <c r="J24" t="s">
+        <v>517</v>
       </c>
       <c r="O24" t="s">
         <v>523</v>
@@ -5202,6 +5207,9 @@
       </c>
       <c r="F25" t="s">
         <v>515</v>
+      </c>
+      <c r="I25" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -5244,7 +5252,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5276,9 +5284,6 @@
       <c r="C2" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="D2" t="s">
-        <v>533</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -5289,6 +5294,9 @@
       </c>
       <c r="C3" s="4" t="s">
         <v>536</v>
+      </c>
+      <c r="D3" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5418,10 +5426,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B169"/>
+  <dimension ref="A1:B174"/>
   <sheetViews>
-    <sheetView topLeftCell="A144" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView tabSelected="1" topLeftCell="A147" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A176" sqref="A176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6426,6 +6434,35 @@
         <v>654</v>
       </c>
     </row>
+    <row r="170" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="18" t="s">
+        <v>655</v>
+      </c>
+      <c r="B171" s="19" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="9"/>
+      <c r="B172" s="20" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="9" t="s">
+        <v>656</v>
+      </c>
+      <c r="B173" s="20" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="21"/>
+      <c r="B174" s="22" t="s">
+        <v>498</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
two trades! Picks are on the move!
2.5
for
2.8
Micah Kiser
Christian Kirksey

2.2
2.6
3.9
for
Mike Williams
Devontae Booker
2022 3 AdamW
2022 3 MikeR
2022 4 Jared
</commit_message>
<xml_diff>
--- a/OffSeason.xlsx
+++ b/OffSeason.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sdwg-my.sharepoint.com/personal/john_olson_agtegra_com/Documents/Documents 1/Football/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="8_{ECA9F46E-F317-4CC4-8E17-E8E8FEC0C4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67B48BA0-4C37-40B1-B8DF-F08667C699E2}"/>
+  <xr:revisionPtr revIDLastSave="139" documentId="8_{ECA9F46E-F317-4CC4-8E17-E8E8FEC0C4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{061B4D5D-CEBD-4AF8-A8C9-04ADDF22582C}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rosters" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Managers" sheetId="3" r:id="rId3"/>
     <sheet name="Off-Season Trades" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="662">
   <si>
     <t>Vanja Dolas - CeeDee Nuts</t>
   </si>
@@ -2008,6 +2008,12 @@
   </si>
   <si>
     <t>Jared trades</t>
+  </si>
+  <si>
+    <t>Christian Kirksey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam </t>
   </si>
 </sst>
 </file>
@@ -2250,6 +2256,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2263,15 +2278,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2657,10 +2663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W78"/>
+  <dimension ref="A1:W79"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41:H43"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12:N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2676,71 +2682,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="E1" s="31" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="E1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="31"/>
+      <c r="F1" s="27"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="31" t="s">
+      <c r="M1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="31"/>
+      <c r="N1" s="27"/>
       <c r="O1" s="1"/>
-      <c r="Q1" s="31" t="s">
+      <c r="Q1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="31"/>
+      <c r="R1" s="27"/>
       <c r="S1" s="1"/>
-      <c r="U1" s="31" t="s">
+      <c r="U1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="31"/>
+      <c r="V1" s="27"/>
       <c r="W1" s="1"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="28" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="28" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="28" t="s">
         <v>6</v>
       </c>
       <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="28" t="s">
         <v>6</v>
       </c>
       <c r="N2" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="25" t="s">
+      <c r="Q2" s="28" t="s">
         <v>6</v>
       </c>
       <c r="R2" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="25" t="s">
+      <c r="U2" s="28" t="s">
         <v>6</v>
       </c>
       <c r="V2" t="s">
@@ -2748,89 +2754,89 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
+      <c r="A3" s="28"/>
       <c r="B3" t="s">
         <v>209</v>
       </c>
-      <c r="E3" s="25"/>
+      <c r="E3" s="28"/>
       <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="25"/>
+      <c r="I3" s="28"/>
       <c r="J3" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="25"/>
+      <c r="M3" s="28"/>
       <c r="N3" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="25"/>
+      <c r="Q3" s="28"/>
       <c r="R3" t="s">
         <v>17</v>
       </c>
-      <c r="U3" s="25"/>
+      <c r="U3" s="28"/>
       <c r="V3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="31" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="31" t="s">
         <v>20</v>
       </c>
       <c r="J4" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="25"/>
+      <c r="M4" s="28"/>
       <c r="N4" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" s="25"/>
+      <c r="Q4" s="28"/>
       <c r="R4" t="s">
         <v>24</v>
       </c>
-      <c r="U4" s="25"/>
+      <c r="U4" s="28"/>
       <c r="V4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
+      <c r="A5" s="31"/>
       <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="28"/>
+      <c r="E5" s="31"/>
       <c r="F5" t="s">
         <v>227</v>
       </c>
-      <c r="I5" s="28"/>
+      <c r="I5" s="31"/>
       <c r="J5" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="28" t="s">
+      <c r="M5" s="31" t="s">
         <v>20</v>
       </c>
       <c r="N5" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="28" t="s">
+      <c r="Q5" s="31" t="s">
         <v>20</v>
       </c>
       <c r="R5" t="s">
         <v>30</v>
       </c>
-      <c r="U5" s="28" t="s">
+      <c r="U5" s="31" t="s">
         <v>20</v>
       </c>
       <c r="V5" t="s">
@@ -2838,161 +2844,161 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
+      <c r="A6" s="31"/>
       <c r="B6" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="28"/>
+      <c r="E6" s="31"/>
       <c r="F6" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="28"/>
+      <c r="I6" s="31"/>
       <c r="J6" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="28"/>
+      <c r="M6" s="31"/>
       <c r="N6" t="s">
         <v>35</v>
       </c>
-      <c r="Q6" s="28"/>
+      <c r="Q6" s="31"/>
       <c r="R6" t="s">
         <v>36</v>
       </c>
-      <c r="U6" s="28"/>
+      <c r="U6" s="31"/>
       <c r="V6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+      <c r="A7" s="31"/>
       <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="28"/>
+      <c r="E7" s="31"/>
       <c r="F7" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="28"/>
+      <c r="I7" s="31"/>
       <c r="J7" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="28"/>
+      <c r="M7" s="31"/>
       <c r="N7" t="s">
         <v>41</v>
       </c>
-      <c r="Q7" s="28"/>
+      <c r="Q7" s="31"/>
       <c r="R7" t="s">
         <v>42</v>
       </c>
-      <c r="U7" s="28"/>
+      <c r="U7" s="31"/>
       <c r="V7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="26" t="s">
         <v>44</v>
       </c>
       <c r="B8" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="28"/>
+      <c r="E8" s="31"/>
       <c r="F8" t="s">
         <v>52</v>
       </c>
-      <c r="I8" s="28"/>
+      <c r="I8" s="31"/>
       <c r="J8" t="s">
         <v>47</v>
       </c>
-      <c r="M8" s="28"/>
+      <c r="M8" s="31"/>
       <c r="N8" t="s">
         <v>48</v>
       </c>
-      <c r="Q8" s="28"/>
+      <c r="Q8" s="31"/>
       <c r="R8" t="s">
         <v>49</v>
       </c>
-      <c r="U8" s="28"/>
+      <c r="U8" s="31"/>
       <c r="V8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="A9" s="26"/>
       <c r="B9" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="28"/>
+      <c r="E9" s="31"/>
       <c r="F9" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="28"/>
+      <c r="I9" s="31"/>
       <c r="J9" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="28"/>
+      <c r="M9" s="31"/>
       <c r="N9" t="s">
         <v>54</v>
       </c>
-      <c r="Q9" s="28"/>
+      <c r="Q9" s="31"/>
       <c r="R9" t="s">
         <v>55</v>
       </c>
-      <c r="U9" s="28"/>
+      <c r="U9" s="31"/>
       <c r="V9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="26"/>
       <c r="B10" t="s">
         <v>281</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="26" t="s">
         <v>44</v>
       </c>
       <c r="F10" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="28"/>
+      <c r="I10" s="31"/>
       <c r="J10" t="s">
         <v>59</v>
       </c>
-      <c r="M10" s="28"/>
+      <c r="M10" s="31"/>
       <c r="N10" t="s">
         <v>60</v>
       </c>
-      <c r="Q10" s="28"/>
+      <c r="Q10" s="31"/>
       <c r="R10" t="s">
         <v>61</v>
       </c>
-      <c r="U10" s="28"/>
+      <c r="U10" s="31"/>
       <c r="V10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="26"/>
       <c r="B11" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="32"/>
+      <c r="E11" s="26"/>
       <c r="F11" t="s">
         <v>70</v>
       </c>
-      <c r="I11" s="28"/>
+      <c r="I11" s="31"/>
       <c r="J11" t="s">
         <v>65</v>
       </c>
-      <c r="M11" s="28"/>
+      <c r="M11" s="31"/>
       <c r="N11" t="s">
         <v>66</v>
       </c>
-      <c r="Q11" s="28"/>
+      <c r="Q11" s="31"/>
       <c r="R11" t="s">
         <v>67</v>
       </c>
-      <c r="U11" s="32" t="s">
+      <c r="U11" s="26" t="s">
         <v>44</v>
       </c>
       <c r="V11" t="s">
@@ -3000,225 +3006,225 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="26"/>
       <c r="B12" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="26"/>
       <c r="F12" t="s">
         <v>88</v>
       </c>
-      <c r="I12" s="32" t="s">
+      <c r="I12" s="26" t="s">
         <v>44</v>
       </c>
       <c r="J12" t="s">
         <v>71</v>
       </c>
-      <c r="M12" s="32" t="s">
+      <c r="M12" s="26" t="s">
         <v>44</v>
       </c>
       <c r="N12" t="s">
         <v>72</v>
       </c>
-      <c r="Q12" s="32" t="s">
+      <c r="Q12" s="26" t="s">
         <v>44</v>
       </c>
       <c r="R12" t="s">
         <v>73</v>
       </c>
-      <c r="U12" s="32"/>
+      <c r="U12" s="26"/>
       <c r="V12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="26"/>
       <c r="B13" t="s">
         <v>270</v>
       </c>
-      <c r="E13" s="32"/>
+      <c r="E13" s="26"/>
       <c r="F13" t="s">
         <v>82</v>
       </c>
-      <c r="I13" s="32"/>
+      <c r="I13" s="26"/>
       <c r="J13" t="s">
         <v>77</v>
       </c>
-      <c r="M13" s="32"/>
+      <c r="M13" s="26"/>
       <c r="N13" t="s">
         <v>78</v>
       </c>
-      <c r="Q13" s="32"/>
+      <c r="Q13" s="26"/>
       <c r="R13" t="s">
         <v>79</v>
       </c>
-      <c r="U13" s="32"/>
+      <c r="U13" s="26"/>
       <c r="V13" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="26"/>
       <c r="B14" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="32"/>
+      <c r="E14" s="26"/>
       <c r="F14" t="s">
         <v>95</v>
       </c>
-      <c r="I14" s="32"/>
+      <c r="I14" s="26"/>
       <c r="J14" t="s">
         <v>83</v>
       </c>
-      <c r="M14" s="32"/>
+      <c r="M14" s="26"/>
       <c r="N14" t="s">
         <v>84</v>
       </c>
-      <c r="Q14" s="32"/>
+      <c r="Q14" s="26"/>
       <c r="R14" t="s">
         <v>85</v>
       </c>
-      <c r="U14" s="32"/>
+      <c r="U14" s="26"/>
       <c r="V14" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+      <c r="A15" s="26"/>
       <c r="B15" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="32"/>
+      <c r="E15" s="26"/>
       <c r="F15" t="s">
         <v>294</v>
       </c>
-      <c r="I15" s="32"/>
+      <c r="I15" s="26"/>
       <c r="J15" t="s">
         <v>89</v>
       </c>
-      <c r="M15" s="32"/>
+      <c r="M15" s="26"/>
       <c r="N15" t="s">
         <v>90</v>
       </c>
-      <c r="Q15" s="32"/>
+      <c r="Q15" s="26"/>
       <c r="R15" t="s">
         <v>91</v>
       </c>
-      <c r="U15" s="32"/>
+      <c r="U15" s="26"/>
       <c r="V15" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="25" t="s">
         <v>93</v>
       </c>
       <c r="B16" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="25" t="s">
         <v>93</v>
       </c>
       <c r="F16" t="s">
         <v>101</v>
       </c>
-      <c r="I16" s="32"/>
+      <c r="I16" s="26"/>
       <c r="J16" t="s">
         <v>96</v>
       </c>
-      <c r="M16" s="32"/>
+      <c r="M16" s="26"/>
       <c r="N16" t="s">
         <v>97</v>
       </c>
-      <c r="Q16" s="32"/>
+      <c r="Q16" s="26"/>
       <c r="R16" t="s">
         <v>98</v>
       </c>
-      <c r="U16" s="32"/>
+      <c r="U16" s="26"/>
       <c r="V16" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
+      <c r="A17" s="25"/>
       <c r="B17" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="30"/>
+      <c r="E17" s="25"/>
       <c r="F17" t="s">
         <v>107</v>
       </c>
-      <c r="I17" s="32"/>
+      <c r="I17" s="26"/>
       <c r="J17" t="s">
         <v>102</v>
       </c>
-      <c r="M17" s="32"/>
+      <c r="M17" s="26"/>
       <c r="N17" t="s">
         <v>103</v>
       </c>
-      <c r="Q17" s="32"/>
+      <c r="Q17" s="26"/>
       <c r="R17" t="s">
         <v>104</v>
       </c>
-      <c r="U17" s="32"/>
+      <c r="U17" s="26"/>
       <c r="V17" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
+      <c r="A18" s="25"/>
       <c r="B18" t="s">
         <v>112</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="32" t="s">
         <v>113</v>
       </c>
       <c r="F18" t="s">
         <v>120</v>
       </c>
-      <c r="I18" s="32"/>
+      <c r="I18" s="26"/>
       <c r="J18" t="s">
         <v>108</v>
       </c>
-      <c r="M18" s="32"/>
+      <c r="M18" s="26"/>
       <c r="N18" t="s">
         <v>109</v>
       </c>
-      <c r="Q18" s="32"/>
+      <c r="Q18" s="26"/>
       <c r="R18" t="s">
         <v>110</v>
       </c>
-      <c r="U18" s="32"/>
+      <c r="U18" s="26"/>
       <c r="V18" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="32" t="s">
         <v>113</v>
       </c>
       <c r="B19" t="s">
         <v>119</v>
       </c>
-      <c r="E19" s="29"/>
+      <c r="E19" s="32"/>
       <c r="F19" t="s">
         <v>126</v>
       </c>
-      <c r="I19" s="32"/>
+      <c r="I19" s="26"/>
       <c r="J19" t="s">
         <v>115</v>
       </c>
-      <c r="M19" s="32"/>
+      <c r="M19" s="26"/>
       <c r="N19" t="s">
         <v>301</v>
       </c>
-      <c r="Q19" s="30" t="s">
+      <c r="Q19" s="25" t="s">
         <v>93</v>
       </c>
       <c r="R19" t="s">
         <v>117</v>
       </c>
-      <c r="U19" s="30" t="s">
+      <c r="U19" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V19" t="s">
@@ -3226,11 +3232,11 @@
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="A20" s="32"/>
       <c r="B20" t="s">
         <v>131</v>
       </c>
-      <c r="E20" s="29"/>
+      <c r="E20" s="32"/>
       <c r="F20" t="s">
         <v>132</v>
       </c>
@@ -3240,47 +3246,47 @@
       <c r="J20" t="s">
         <v>121</v>
       </c>
-      <c r="M20" s="30" t="s">
+      <c r="M20" s="25" t="s">
         <v>93</v>
       </c>
       <c r="N20" t="s">
         <v>116</v>
       </c>
-      <c r="Q20" s="30"/>
+      <c r="Q20" s="25"/>
       <c r="R20" t="s">
         <v>123</v>
       </c>
-      <c r="U20" s="30"/>
+      <c r="U20" s="25"/>
       <c r="V20" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="A21" s="32"/>
       <c r="B21" t="s">
         <v>114</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="29" t="s">
         <v>137</v>
       </c>
       <c r="F21" t="s">
         <v>139</v>
       </c>
-      <c r="I21" s="29" t="s">
+      <c r="I21" s="32" t="s">
         <v>113</v>
       </c>
       <c r="J21" t="s">
         <v>127</v>
       </c>
-      <c r="M21" s="30"/>
+      <c r="M21" s="25"/>
       <c r="N21" t="s">
         <v>122</v>
       </c>
-      <c r="Q21" s="30"/>
+      <c r="Q21" s="25"/>
       <c r="R21" t="s">
         <v>129</v>
       </c>
-      <c r="U21" s="29" t="s">
+      <c r="U21" s="32" t="s">
         <v>113</v>
       </c>
       <c r="V21" t="s">
@@ -3288,115 +3294,115 @@
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="29" t="s">
         <v>137</v>
       </c>
       <c r="B22" t="s">
         <v>138</v>
       </c>
-      <c r="E22" s="26"/>
+      <c r="E22" s="29"/>
       <c r="F22" t="s">
         <v>145</v>
       </c>
-      <c r="I22" s="29"/>
+      <c r="I22" s="32"/>
       <c r="J22" t="s">
         <v>133</v>
       </c>
-      <c r="M22" s="30"/>
+      <c r="M22" s="25"/>
       <c r="N22" t="s">
         <v>134</v>
       </c>
-      <c r="Q22" s="29" t="s">
+      <c r="Q22" s="32" t="s">
         <v>113</v>
       </c>
       <c r="R22" t="s">
         <v>135</v>
       </c>
-      <c r="U22" s="29"/>
+      <c r="U22" s="32"/>
       <c r="V22" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
+      <c r="A23" s="29"/>
       <c r="B23" t="s">
         <v>144</v>
       </c>
-      <c r="E23" s="26"/>
+      <c r="E23" s="29"/>
       <c r="F23" t="s">
         <v>151</v>
       </c>
-      <c r="I23" s="29"/>
+      <c r="I23" s="32"/>
       <c r="J23" t="s">
         <v>140</v>
       </c>
-      <c r="M23" s="29" t="s">
+      <c r="M23" s="32" t="s">
         <v>113</v>
       </c>
       <c r="N23" t="s">
         <v>141</v>
       </c>
-      <c r="Q23" s="29"/>
+      <c r="Q23" s="32"/>
       <c r="R23" t="s">
         <v>142</v>
       </c>
-      <c r="U23" s="29"/>
+      <c r="U23" s="32"/>
       <c r="V23" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
+      <c r="A24" s="29"/>
       <c r="B24" t="s">
         <v>150</v>
       </c>
-      <c r="E24" s="26"/>
+      <c r="E24" s="29"/>
       <c r="F24" t="s">
         <v>157</v>
       </c>
-      <c r="I24" s="29"/>
+      <c r="I24" s="32"/>
       <c r="J24" t="s">
         <v>146</v>
       </c>
-      <c r="M24" s="29"/>
+      <c r="M24" s="32"/>
       <c r="N24" t="s">
         <v>147</v>
       </c>
-      <c r="Q24" s="29"/>
+      <c r="Q24" s="32"/>
       <c r="R24" t="s">
         <v>148</v>
       </c>
-      <c r="U24" s="29"/>
+      <c r="U24" s="32"/>
       <c r="V24" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
+      <c r="A25" s="29"/>
       <c r="B25" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="27" t="s">
+      <c r="E25" s="30" t="s">
         <v>167</v>
       </c>
       <c r="F25" t="s">
         <v>169</v>
       </c>
-      <c r="I25" s="26" t="s">
+      <c r="I25" s="29" t="s">
         <v>137</v>
       </c>
       <c r="J25" t="s">
         <v>152</v>
       </c>
-      <c r="M25" s="29"/>
+      <c r="M25" s="32"/>
       <c r="N25" t="s">
         <v>153</v>
       </c>
-      <c r="Q25" s="29"/>
+      <c r="Q25" s="32"/>
       <c r="R25" t="s">
         <v>154</v>
       </c>
-      <c r="U25" s="26" t="s">
+      <c r="U25" s="29" t="s">
         <v>137</v>
       </c>
       <c r="V25" t="s">
@@ -3404,105 +3410,105 @@
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="30" t="s">
         <v>167</v>
       </c>
       <c r="B26" t="s">
         <v>193</v>
       </c>
-      <c r="E26" s="27"/>
+      <c r="E26" s="30"/>
       <c r="F26" t="s">
         <v>175</v>
       </c>
-      <c r="I26" s="26"/>
+      <c r="I26" s="29"/>
       <c r="J26" t="s">
         <v>158</v>
       </c>
-      <c r="M26" s="26" t="s">
+      <c r="M26" s="29" t="s">
         <v>137</v>
       </c>
       <c r="N26" t="s">
         <v>159</v>
       </c>
-      <c r="Q26" s="26" t="s">
+      <c r="Q26" s="29" t="s">
         <v>137</v>
       </c>
       <c r="R26" t="s">
         <v>160</v>
       </c>
-      <c r="U26" s="26"/>
+      <c r="U26" s="29"/>
       <c r="V26" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
+      <c r="A27" s="30"/>
       <c r="B27" t="s">
         <v>174</v>
       </c>
-      <c r="E27" s="27"/>
+      <c r="E27" s="30"/>
       <c r="F27" t="s">
         <v>181</v>
       </c>
-      <c r="I27" s="26"/>
+      <c r="I27" s="29"/>
       <c r="J27" t="s">
         <v>163</v>
       </c>
-      <c r="M27" s="26"/>
+      <c r="M27" s="29"/>
       <c r="N27" t="s">
         <v>164</v>
       </c>
-      <c r="Q27" s="26"/>
+      <c r="Q27" s="29"/>
       <c r="R27" t="s">
         <v>165</v>
       </c>
-      <c r="U27" s="26"/>
+      <c r="U27" s="29"/>
       <c r="V27" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
+      <c r="A28" s="30"/>
       <c r="B28" t="s">
         <v>192</v>
       </c>
-      <c r="I28" s="26"/>
+      <c r="I28" s="29"/>
       <c r="J28" t="s">
         <v>170</v>
       </c>
-      <c r="M28" s="26"/>
+      <c r="M28" s="29"/>
       <c r="N28" t="s">
         <v>171</v>
       </c>
-      <c r="Q28" s="26"/>
+      <c r="Q28" s="29"/>
       <c r="R28" t="s">
         <v>172</v>
       </c>
-      <c r="U28" s="26"/>
+      <c r="U28" s="29"/>
       <c r="V28" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
+      <c r="A29" s="30"/>
       <c r="B29" t="s">
         <v>180</v>
       </c>
-      <c r="I29" s="27" t="s">
+      <c r="I29" s="30" t="s">
         <v>167</v>
       </c>
       <c r="J29" t="s">
         <v>176</v>
       </c>
-      <c r="M29" s="26"/>
+      <c r="M29" s="29"/>
       <c r="N29" t="s">
         <v>177</v>
       </c>
-      <c r="Q29" s="26"/>
+      <c r="Q29" s="29"/>
       <c r="R29" t="s">
         <v>178</v>
       </c>
-      <c r="U29" s="27" t="s">
+      <c r="U29" s="30" t="s">
         <v>167</v>
       </c>
       <c r="V29" t="s">
@@ -3510,137 +3516,131 @@
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
-      <c r="B30" t="s">
-        <v>186</v>
-      </c>
-      <c r="I30" s="27"/>
+      <c r="A30" s="30"/>
+      <c r="I30" s="30"/>
       <c r="J30" t="s">
         <v>182</v>
       </c>
-      <c r="M30" s="27" t="s">
+      <c r="M30" s="30" t="s">
         <v>167</v>
       </c>
       <c r="N30" t="s">
         <v>183</v>
       </c>
-      <c r="Q30" s="27" t="s">
+      <c r="Q30" s="30" t="s">
         <v>167</v>
       </c>
       <c r="R30" t="s">
         <v>184</v>
       </c>
-      <c r="U30" s="27"/>
+      <c r="U30" s="30"/>
       <c r="V30" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
-      <c r="B31" t="s">
-        <v>168</v>
-      </c>
-      <c r="I31" s="27"/>
+      <c r="A31" s="30"/>
+      <c r="I31" s="30"/>
       <c r="J31" t="s">
         <v>188</v>
       </c>
-      <c r="M31" s="27"/>
+      <c r="M31" s="30"/>
       <c r="N31" t="s">
         <v>189</v>
       </c>
-      <c r="Q31" s="27"/>
+      <c r="Q31" s="30"/>
       <c r="R31" t="s">
         <v>190</v>
       </c>
-      <c r="U31" s="27"/>
+      <c r="U31" s="30"/>
       <c r="V31" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="I32" s="27"/>
+      <c r="I32" s="30"/>
       <c r="J32" t="s">
         <v>194</v>
       </c>
-      <c r="M32" s="27"/>
+      <c r="M32" s="30"/>
       <c r="N32" t="s">
         <v>195</v>
       </c>
-      <c r="Q32" s="27"/>
+      <c r="Q32" s="30"/>
       <c r="R32" t="s">
         <v>196</v>
       </c>
-      <c r="U32" s="27"/>
+      <c r="U32" s="30"/>
       <c r="V32" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="I33" s="27"/>
+      <c r="I33" s="30"/>
       <c r="J33" t="s">
         <v>198</v>
       </c>
-      <c r="M33" s="27"/>
+      <c r="M33" s="30"/>
       <c r="N33" t="s">
         <v>199</v>
       </c>
-      <c r="Q33" s="27"/>
+      <c r="Q33" s="30"/>
       <c r="R33" t="s">
         <v>200</v>
       </c>
-      <c r="U33" s="27"/>
+      <c r="U33" s="30"/>
       <c r="V33" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="Q34" s="27"/>
+      <c r="Q34" s="30"/>
       <c r="R34" t="s">
         <v>202</v>
       </c>
       <c r="U34" s="3"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="E40" s="31" t="s">
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="E40" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="I40" s="31" t="s">
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="I40" s="27" t="s">
         <v>605</v>
       </c>
-      <c r="J40" s="31"/>
-      <c r="K40" s="31"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
       <c r="L40" s="1"/>
-      <c r="M40" s="31" t="s">
+      <c r="M40" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="N40" s="31"/>
+      <c r="N40" s="27"/>
       <c r="O40" s="1"/>
-      <c r="Q40" s="31" t="s">
+      <c r="Q40" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="R40" s="31"/>
+      <c r="R40" s="27"/>
       <c r="S40" s="1"/>
-      <c r="U40" s="31" t="s">
+      <c r="U40" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="V40" s="31"/>
+      <c r="V40" s="27"/>
       <c r="W40" s="1"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="28" t="s">
         <v>6</v>
       </c>
       <c r="B41" t="s">
         <v>208</v>
       </c>
-      <c r="E41" s="25" t="s">
+      <c r="E41" s="28" t="s">
         <v>6</v>
       </c>
       <c r="F41" t="s">
@@ -3652,19 +3652,19 @@
       <c r="J41" t="s">
         <v>216</v>
       </c>
-      <c r="M41" s="25" t="s">
+      <c r="M41" s="28" t="s">
         <v>6</v>
       </c>
       <c r="N41" t="s">
         <v>211</v>
       </c>
-      <c r="Q41" s="25" t="s">
+      <c r="Q41" s="28" t="s">
         <v>6</v>
       </c>
       <c r="R41" t="s">
         <v>212</v>
       </c>
-      <c r="U41" s="25" t="s">
+      <c r="U41" s="28" t="s">
         <v>6</v>
       </c>
       <c r="V41" t="s">
@@ -3672,87 +3672,87 @@
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
+      <c r="A42" s="28"/>
       <c r="B42" t="s">
         <v>214</v>
       </c>
-      <c r="E42" s="25"/>
+      <c r="E42" s="28"/>
       <c r="F42" t="s">
         <v>19</v>
       </c>
-      <c r="I42" s="28" t="s">
+      <c r="I42" s="31" t="s">
         <v>20</v>
       </c>
       <c r="J42" t="s">
         <v>222</v>
       </c>
-      <c r="M42" s="25"/>
+      <c r="M42" s="28"/>
       <c r="N42" t="s">
         <v>217</v>
       </c>
-      <c r="Q42" s="25"/>
+      <c r="Q42" s="28"/>
       <c r="R42" t="s">
         <v>218</v>
       </c>
-      <c r="U42" s="25"/>
+      <c r="U42" s="28"/>
       <c r="V42" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
+      <c r="A43" s="28"/>
       <c r="B43" t="s">
         <v>220</v>
       </c>
-      <c r="E43" s="25"/>
+      <c r="E43" s="28"/>
       <c r="F43" t="s">
         <v>215</v>
       </c>
-      <c r="I43" s="28"/>
+      <c r="I43" s="31"/>
       <c r="J43" t="s">
         <v>46</v>
       </c>
-      <c r="M43" s="25"/>
+      <c r="M43" s="28"/>
       <c r="N43" t="s">
         <v>223</v>
       </c>
-      <c r="Q43" s="28" t="s">
+      <c r="Q43" s="31" t="s">
         <v>20</v>
       </c>
       <c r="R43" t="s">
         <v>224</v>
       </c>
-      <c r="U43" s="25"/>
+      <c r="U43" s="28"/>
       <c r="V43" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="31" t="s">
         <v>20</v>
       </c>
       <c r="B44" t="s">
         <v>226</v>
       </c>
-      <c r="E44" s="25"/>
+      <c r="E44" s="28"/>
       <c r="F44" t="s">
         <v>221</v>
       </c>
-      <c r="I44" s="28"/>
+      <c r="I44" s="31"/>
       <c r="J44" t="s">
         <v>245</v>
       </c>
-      <c r="M44" s="28" t="s">
+      <c r="M44" s="31" t="s">
         <v>20</v>
       </c>
       <c r="N44" t="s">
         <v>229</v>
       </c>
-      <c r="Q44" s="28"/>
+      <c r="Q44" s="31"/>
       <c r="R44" t="s">
         <v>230</v>
       </c>
-      <c r="U44" s="28" t="s">
+      <c r="U44" s="31" t="s">
         <v>20</v>
       </c>
       <c r="V44" t="s">
@@ -3760,161 +3760,161 @@
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A45" s="28"/>
+      <c r="A45" s="31"/>
       <c r="B45" t="s">
         <v>233</v>
       </c>
-      <c r="E45" s="28" t="s">
+      <c r="E45" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F45" t="s">
         <v>239</v>
       </c>
-      <c r="I45" s="28"/>
+      <c r="I45" s="31"/>
       <c r="J45" t="s">
         <v>234</v>
       </c>
-      <c r="M45" s="28"/>
+      <c r="M45" s="31"/>
       <c r="N45" t="s">
         <v>235</v>
       </c>
-      <c r="Q45" s="28"/>
+      <c r="Q45" s="31"/>
       <c r="R45" t="s">
         <v>236</v>
       </c>
-      <c r="U45" s="28"/>
+      <c r="U45" s="31"/>
       <c r="V45" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A46" s="28"/>
+      <c r="A46" s="31"/>
       <c r="B46" t="s">
         <v>232</v>
       </c>
-      <c r="E46" s="28"/>
+      <c r="E46" s="31"/>
       <c r="F46" t="s">
         <v>251</v>
       </c>
-      <c r="I46" s="28"/>
+      <c r="I46" s="31"/>
       <c r="J46" t="s">
         <v>252</v>
       </c>
-      <c r="M46" s="28"/>
+      <c r="M46" s="31"/>
       <c r="N46" t="s">
         <v>241</v>
       </c>
-      <c r="Q46" s="28"/>
+      <c r="Q46" s="31"/>
       <c r="R46" t="s">
         <v>242</v>
       </c>
-      <c r="U46" s="28"/>
+      <c r="U46" s="31"/>
       <c r="V46" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A47" s="28"/>
+      <c r="A47" s="31"/>
       <c r="B47" t="s">
         <v>238</v>
       </c>
-      <c r="E47" s="28"/>
+      <c r="E47" s="31"/>
       <c r="F47" t="s">
         <v>257</v>
       </c>
-      <c r="I47" s="28"/>
+      <c r="I47" s="31"/>
       <c r="J47" t="s">
         <v>258</v>
       </c>
-      <c r="M47" s="28"/>
+      <c r="M47" s="31"/>
       <c r="N47" t="s">
         <v>247</v>
       </c>
-      <c r="Q47" s="28"/>
+      <c r="Q47" s="31"/>
       <c r="R47" t="s">
         <v>248</v>
       </c>
-      <c r="U47" s="28"/>
+      <c r="U47" s="31"/>
       <c r="V47" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A48" s="28"/>
+      <c r="A48" s="31"/>
       <c r="B48" t="s">
         <v>244</v>
       </c>
-      <c r="E48" s="28"/>
+      <c r="E48" s="31"/>
       <c r="F48" t="s">
         <v>263</v>
       </c>
-      <c r="I48" s="28"/>
+      <c r="I48" s="31"/>
       <c r="J48" t="s">
         <v>264</v>
       </c>
-      <c r="M48" s="28"/>
+      <c r="M48" s="31"/>
       <c r="N48" t="s">
         <v>253</v>
       </c>
-      <c r="Q48" s="28"/>
+      <c r="Q48" s="31"/>
       <c r="R48" t="s">
         <v>254</v>
       </c>
-      <c r="U48" s="28"/>
+      <c r="U48" s="31"/>
       <c r="V48" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A49" s="28"/>
+      <c r="A49" s="31"/>
       <c r="B49" t="s">
         <v>250</v>
       </c>
-      <c r="E49" s="28"/>
+      <c r="E49" s="31"/>
       <c r="F49" t="s">
         <v>240</v>
       </c>
-      <c r="I49" s="28"/>
+      <c r="I49" s="31"/>
       <c r="J49" t="s">
         <v>228</v>
       </c>
-      <c r="M49" s="28"/>
+      <c r="M49" s="31"/>
       <c r="N49" t="s">
         <v>259</v>
       </c>
-      <c r="Q49" s="28"/>
+      <c r="Q49" s="31"/>
       <c r="R49" t="s">
         <v>260</v>
       </c>
-      <c r="U49" s="28"/>
+      <c r="U49" s="31"/>
       <c r="V49" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A50" s="28"/>
+      <c r="A50" s="31"/>
       <c r="B50" t="s">
         <v>256</v>
       </c>
-      <c r="E50" s="32" t="s">
+      <c r="E50" s="26" t="s">
         <v>44</v>
       </c>
       <c r="F50" t="s">
         <v>269</v>
       </c>
-      <c r="I50" s="28"/>
+      <c r="I50" s="31"/>
       <c r="J50" t="s">
         <v>246</v>
       </c>
-      <c r="M50" s="28"/>
+      <c r="M50" s="31"/>
       <c r="N50" t="s">
         <v>265</v>
       </c>
-      <c r="Q50" s="28"/>
+      <c r="Q50" s="31"/>
       <c r="R50" t="s">
         <v>266</v>
       </c>
-      <c r="U50" s="32" t="s">
+      <c r="U50" s="26" t="s">
         <v>44</v>
       </c>
       <c r="V50" t="s">
@@ -3922,273 +3922,273 @@
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A51" s="28"/>
+      <c r="A51" s="31"/>
       <c r="B51" t="s">
         <v>262</v>
       </c>
-      <c r="E51" s="32"/>
+      <c r="E51" s="26"/>
       <c r="F51" t="s">
         <v>275</v>
       </c>
-      <c r="I51" s="32" t="s">
+      <c r="I51" s="26" t="s">
         <v>44</v>
       </c>
       <c r="J51" t="s">
         <v>76</v>
       </c>
-      <c r="M51" s="32" t="s">
+      <c r="M51" s="26" t="s">
         <v>44</v>
       </c>
       <c r="N51" t="s">
         <v>271</v>
       </c>
-      <c r="Q51" s="32" t="s">
+      <c r="Q51" s="26" t="s">
         <v>44</v>
       </c>
       <c r="R51" t="s">
         <v>272</v>
       </c>
-      <c r="U51" s="32"/>
+      <c r="U51" s="26"/>
       <c r="V51" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A52" s="32" t="s">
+      <c r="A52" s="26" t="s">
         <v>44</v>
       </c>
       <c r="B52" t="s">
         <v>268</v>
       </c>
-      <c r="E52" s="32"/>
+      <c r="E52" s="26"/>
       <c r="F52" t="s">
         <v>63</v>
       </c>
-      <c r="I52" s="32"/>
+      <c r="I52" s="26"/>
       <c r="J52" t="s">
         <v>276</v>
       </c>
-      <c r="M52" s="32"/>
+      <c r="M52" s="26"/>
       <c r="N52" t="s">
         <v>277</v>
       </c>
-      <c r="Q52" s="32"/>
+      <c r="Q52" s="26"/>
       <c r="R52" t="s">
         <v>278</v>
       </c>
-      <c r="U52" s="32"/>
+      <c r="U52" s="26"/>
       <c r="V52" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A53" s="32"/>
+      <c r="A53" s="26"/>
       <c r="B53" t="s">
         <v>274</v>
       </c>
-      <c r="E53" s="32"/>
+      <c r="E53" s="26"/>
       <c r="F53" t="s">
         <v>287</v>
       </c>
-      <c r="I53" s="32"/>
+      <c r="I53" s="26"/>
       <c r="J53" t="s">
         <v>300</v>
       </c>
-      <c r="M53" s="32"/>
+      <c r="M53" s="26"/>
       <c r="N53" t="s">
         <v>283</v>
       </c>
-      <c r="Q53" s="32"/>
+      <c r="Q53" s="26"/>
       <c r="R53" t="s">
         <v>284</v>
       </c>
-      <c r="U53" s="32"/>
+      <c r="U53" s="26"/>
       <c r="V53" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A54" s="32"/>
+      <c r="A54" s="26"/>
       <c r="B54" t="s">
         <v>280</v>
       </c>
-      <c r="E54" s="32"/>
+      <c r="E54" s="26"/>
       <c r="F54" t="s">
         <v>293</v>
       </c>
-      <c r="I54" s="32"/>
+      <c r="I54" s="26"/>
       <c r="J54" t="s">
         <v>288</v>
       </c>
-      <c r="M54" s="32"/>
+      <c r="M54" s="26"/>
       <c r="N54" t="s">
         <v>289</v>
       </c>
-      <c r="Q54" s="32"/>
+      <c r="Q54" s="26"/>
       <c r="R54" t="s">
         <v>290</v>
       </c>
-      <c r="U54" s="32"/>
+      <c r="U54" s="26"/>
       <c r="V54" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A55" s="32"/>
+      <c r="A55" s="26"/>
       <c r="B55" t="s">
         <v>286</v>
       </c>
-      <c r="E55" s="32"/>
+      <c r="E55" s="26"/>
       <c r="F55" t="s">
         <v>312</v>
       </c>
-      <c r="I55" s="32"/>
+      <c r="I55" s="26"/>
       <c r="J55" t="s">
         <v>306</v>
       </c>
-      <c r="M55" s="32"/>
+      <c r="M55" s="26"/>
       <c r="N55" t="s">
         <v>295</v>
       </c>
-      <c r="Q55" s="32"/>
+      <c r="Q55" s="26"/>
       <c r="R55" t="s">
         <v>296</v>
       </c>
-      <c r="U55" s="32"/>
+      <c r="U55" s="26"/>
       <c r="V55" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A56" s="32"/>
+      <c r="A56" s="26"/>
       <c r="B56" t="s">
         <v>292</v>
       </c>
-      <c r="E56" s="32"/>
+      <c r="E56" s="26"/>
       <c r="F56" t="s">
         <v>311</v>
       </c>
-      <c r="I56" s="32"/>
+      <c r="I56" s="26"/>
       <c r="J56" t="s">
         <v>57</v>
       </c>
-      <c r="M56" s="32"/>
+      <c r="M56" s="26"/>
       <c r="N56" t="s">
         <v>307</v>
       </c>
-      <c r="Q56" s="32"/>
+      <c r="Q56" s="26"/>
       <c r="R56" t="s">
         <v>302</v>
       </c>
-      <c r="U56" s="32"/>
+      <c r="U56" s="26"/>
       <c r="V56" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A57" s="32"/>
+      <c r="A57" s="26"/>
       <c r="B57" t="s">
         <v>298</v>
       </c>
-      <c r="E57" s="32"/>
+      <c r="E57" s="26"/>
       <c r="F57" t="s">
         <v>317</v>
       </c>
-      <c r="I57" s="32"/>
+      <c r="I57" s="26"/>
       <c r="J57" t="s">
         <v>282</v>
       </c>
-      <c r="M57" s="32"/>
+      <c r="M57" s="26"/>
       <c r="N57" t="s">
         <v>313</v>
       </c>
-      <c r="Q57" s="32"/>
+      <c r="Q57" s="26"/>
       <c r="R57" t="s">
         <v>308</v>
       </c>
-      <c r="U57" s="32"/>
+      <c r="U57" s="26"/>
       <c r="V57" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A58" s="32"/>
+      <c r="A58" s="26"/>
       <c r="B58" t="s">
         <v>304</v>
       </c>
-      <c r="E58" s="32"/>
+      <c r="E58" s="26"/>
       <c r="F58" t="s">
         <v>323</v>
       </c>
-      <c r="I58" s="30" t="s">
+      <c r="I58" s="25" t="s">
         <v>93</v>
       </c>
       <c r="J58" t="s">
         <v>353</v>
       </c>
-      <c r="M58" s="30" t="s">
+      <c r="M58" s="25" t="s">
         <v>93</v>
       </c>
       <c r="N58" t="s">
         <v>319</v>
       </c>
-      <c r="Q58" s="32"/>
+      <c r="Q58" s="26"/>
       <c r="R58" t="s">
         <v>314</v>
       </c>
-      <c r="U58" s="32"/>
+      <c r="U58" s="26"/>
       <c r="V58" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A59" s="32"/>
+      <c r="A59" s="26"/>
       <c r="B59" t="s">
         <v>310</v>
       </c>
-      <c r="E59" s="32"/>
+      <c r="E59" s="26"/>
       <c r="F59" t="s">
         <v>329</v>
       </c>
-      <c r="I59" s="30"/>
+      <c r="I59" s="25"/>
       <c r="J59" t="s">
         <v>318</v>
       </c>
-      <c r="M59" s="30"/>
+      <c r="M59" s="25"/>
       <c r="N59" t="s">
         <v>325</v>
       </c>
-      <c r="Q59" s="32"/>
+      <c r="Q59" s="26"/>
       <c r="R59" t="s">
         <v>320</v>
       </c>
-      <c r="U59" s="32"/>
+      <c r="U59" s="26"/>
       <c r="V59" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A60" s="32"/>
+      <c r="A60" s="26"/>
       <c r="B60" t="s">
         <v>316</v>
       </c>
-      <c r="E60" s="32"/>
+      <c r="E60" s="26"/>
       <c r="F60" t="s">
         <v>335</v>
       </c>
-      <c r="I60" s="30"/>
+      <c r="I60" s="25"/>
       <c r="J60" t="s">
         <v>106</v>
       </c>
-      <c r="M60" s="30"/>
+      <c r="M60" s="25"/>
       <c r="N60" t="s">
         <v>331</v>
       </c>
-      <c r="Q60" s="32"/>
+      <c r="Q60" s="26"/>
       <c r="R60" t="s">
         <v>326</v>
       </c>
-      <c r="U60" s="30" t="s">
+      <c r="U60" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V60" t="s">
@@ -4196,57 +4196,57 @@
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A61" s="32"/>
+      <c r="A61" s="26"/>
       <c r="B61" t="s">
         <v>322</v>
       </c>
-      <c r="E61" s="32"/>
+      <c r="E61" s="26"/>
       <c r="F61" t="s">
         <v>299</v>
       </c>
-      <c r="I61" s="30"/>
+      <c r="I61" s="25"/>
       <c r="J61" t="s">
         <v>336</v>
       </c>
-      <c r="M61" s="30"/>
+      <c r="M61" s="25"/>
       <c r="N61" t="s">
         <v>128</v>
       </c>
-      <c r="Q61" s="32"/>
+      <c r="Q61" s="26"/>
       <c r="R61" t="s">
         <v>332</v>
       </c>
-      <c r="U61" s="30"/>
+      <c r="U61" s="25"/>
       <c r="V61" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A62" s="32"/>
+      <c r="A62" s="26"/>
       <c r="B62" t="s">
         <v>305</v>
       </c>
-      <c r="E62" s="30" t="s">
+      <c r="E62" s="25" t="s">
         <v>93</v>
       </c>
       <c r="F62" t="s">
         <v>341</v>
       </c>
-      <c r="I62" s="30"/>
+      <c r="I62" s="25"/>
       <c r="J62" t="s">
         <v>324</v>
       </c>
-      <c r="M62" s="29" t="s">
+      <c r="M62" s="32" t="s">
         <v>113</v>
       </c>
       <c r="N62" t="s">
         <v>337</v>
       </c>
-      <c r="Q62" s="32"/>
+      <c r="Q62" s="26"/>
       <c r="R62" t="s">
         <v>338</v>
       </c>
-      <c r="U62" s="29" t="s">
+      <c r="U62" s="32" t="s">
         <v>113</v>
       </c>
       <c r="V62" t="s">
@@ -4254,89 +4254,89 @@
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A63" s="30" t="s">
+      <c r="A63" s="25" t="s">
         <v>93</v>
       </c>
       <c r="B63" t="s">
         <v>328</v>
       </c>
-      <c r="E63" s="30"/>
+      <c r="E63" s="25"/>
       <c r="F63" t="s">
         <v>347</v>
       </c>
-      <c r="I63" s="29" t="s">
+      <c r="I63" s="32" t="s">
         <v>113</v>
       </c>
       <c r="J63" t="s">
         <v>342</v>
       </c>
-      <c r="M63" s="29"/>
+      <c r="M63" s="32"/>
       <c r="N63" t="s">
         <v>343</v>
       </c>
-      <c r="Q63" s="32"/>
+      <c r="Q63" s="26"/>
       <c r="R63" t="s">
         <v>344</v>
       </c>
-      <c r="U63" s="29"/>
+      <c r="U63" s="32"/>
       <c r="V63" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A64" s="30"/>
+      <c r="A64" s="25"/>
       <c r="B64" t="s">
         <v>334</v>
       </c>
-      <c r="E64" s="30"/>
+      <c r="E64" s="25"/>
       <c r="F64" t="s">
         <v>359</v>
       </c>
-      <c r="I64" s="29"/>
+      <c r="I64" s="32"/>
       <c r="J64" t="s">
         <v>348</v>
       </c>
-      <c r="M64" s="29"/>
+      <c r="M64" s="32"/>
       <c r="N64" t="s">
         <v>349</v>
       </c>
-      <c r="Q64" s="30" t="s">
+      <c r="Q64" s="25" t="s">
         <v>93</v>
       </c>
       <c r="R64" t="s">
         <v>350</v>
       </c>
-      <c r="U64" s="29"/>
+      <c r="U64" s="32"/>
       <c r="V64" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A65" s="30"/>
+      <c r="A65" s="25"/>
       <c r="B65" t="s">
         <v>340</v>
       </c>
-      <c r="E65" s="29" t="s">
+      <c r="E65" s="32" t="s">
         <v>113</v>
       </c>
       <c r="F65" t="s">
         <v>365</v>
       </c>
-      <c r="I65" s="29"/>
+      <c r="I65" s="32"/>
       <c r="J65" t="s">
         <v>354</v>
       </c>
-      <c r="M65" s="26" t="s">
+      <c r="M65" s="29" t="s">
         <v>137</v>
       </c>
       <c r="N65" t="s">
         <v>355</v>
       </c>
-      <c r="Q65" s="30"/>
+      <c r="Q65" s="25"/>
       <c r="R65" t="s">
         <v>356</v>
       </c>
-      <c r="U65" s="26" t="s">
+      <c r="U65" s="29" t="s">
         <v>137</v>
       </c>
       <c r="V65" t="s">
@@ -4344,141 +4344,141 @@
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A66" s="30"/>
+      <c r="A66" s="25"/>
       <c r="B66" t="s">
         <v>346</v>
       </c>
-      <c r="E66" s="29"/>
+      <c r="E66" s="32"/>
       <c r="F66" t="s">
         <v>371</v>
       </c>
-      <c r="I66" s="29"/>
+      <c r="I66" s="32"/>
       <c r="J66" t="s">
         <v>360</v>
       </c>
-      <c r="M66" s="26"/>
+      <c r="M66" s="29"/>
       <c r="N66" t="s">
         <v>361</v>
       </c>
-      <c r="Q66" s="29" t="s">
+      <c r="Q66" s="32" t="s">
         <v>113</v>
       </c>
       <c r="R66" t="s">
         <v>362</v>
       </c>
-      <c r="U66" s="26"/>
+      <c r="U66" s="29"/>
       <c r="V66" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A67" s="30"/>
+      <c r="A67" s="25"/>
       <c r="B67" t="s">
         <v>330</v>
       </c>
-      <c r="E67" s="29"/>
+      <c r="E67" s="32"/>
       <c r="F67" t="s">
         <v>377</v>
       </c>
-      <c r="I67" s="26" t="s">
+      <c r="I67" s="29" t="s">
         <v>137</v>
       </c>
       <c r="J67" t="s">
         <v>372</v>
       </c>
-      <c r="M67" s="26"/>
+      <c r="M67" s="29"/>
       <c r="N67" t="s">
         <v>156</v>
       </c>
-      <c r="Q67" s="29"/>
+      <c r="Q67" s="32"/>
       <c r="R67" t="s">
         <v>368</v>
       </c>
-      <c r="U67" s="26"/>
+      <c r="U67" s="29"/>
       <c r="V67" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A68" s="29" t="s">
+      <c r="A68" s="32" t="s">
         <v>113</v>
       </c>
       <c r="B68" t="s">
         <v>352</v>
       </c>
-      <c r="E68" s="29"/>
+      <c r="E68" s="32"/>
       <c r="F68" t="s">
         <v>125</v>
       </c>
-      <c r="I68" s="26"/>
+      <c r="I68" s="29"/>
       <c r="J68" t="s">
         <v>384</v>
       </c>
-      <c r="M68" s="26"/>
+      <c r="M68" s="29"/>
       <c r="N68" t="s">
         <v>373</v>
       </c>
-      <c r="Q68" s="29"/>
+      <c r="Q68" s="32"/>
       <c r="R68" t="s">
         <v>374</v>
       </c>
-      <c r="U68" s="26"/>
+      <c r="U68" s="29"/>
       <c r="V68" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A69" s="29"/>
+      <c r="A69" s="32"/>
       <c r="B69" t="s">
         <v>358</v>
       </c>
-      <c r="E69" s="26" t="s">
+      <c r="E69" s="29" t="s">
         <v>137</v>
       </c>
       <c r="F69" t="s">
         <v>383</v>
       </c>
-      <c r="I69" s="26"/>
+      <c r="I69" s="29"/>
       <c r="J69" t="s">
         <v>162</v>
       </c>
-      <c r="M69" s="26"/>
+      <c r="M69" s="29"/>
       <c r="N69" t="s">
         <v>379</v>
       </c>
-      <c r="Q69" s="29"/>
+      <c r="Q69" s="32"/>
       <c r="R69" t="s">
         <v>380</v>
       </c>
-      <c r="U69" s="26"/>
+      <c r="U69" s="29"/>
       <c r="V69" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A70" s="29"/>
+      <c r="A70" s="32"/>
       <c r="B70" t="s">
         <v>364</v>
       </c>
-      <c r="E70" s="26"/>
+      <c r="E70" s="29"/>
       <c r="F70" t="s">
         <v>389</v>
       </c>
-      <c r="I70" s="26"/>
+      <c r="I70" s="29"/>
       <c r="J70" t="s">
         <v>407</v>
       </c>
-      <c r="M70" s="26"/>
+      <c r="M70" s="29"/>
       <c r="N70" t="s">
         <v>367</v>
       </c>
-      <c r="Q70" s="26" t="s">
+      <c r="Q70" s="29" t="s">
         <v>137</v>
       </c>
       <c r="R70" t="s">
         <v>386</v>
       </c>
-      <c r="U70" s="27" t="s">
+      <c r="U70" s="30" t="s">
         <v>167</v>
       </c>
       <c r="V70" t="s">
@@ -4486,171 +4486,259 @@
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A71" s="26" t="s">
+      <c r="A71" s="29" t="s">
         <v>137</v>
       </c>
       <c r="B71" t="s">
         <v>370</v>
       </c>
-      <c r="E71" s="26"/>
+      <c r="E71" s="29"/>
       <c r="F71" t="s">
         <v>395</v>
       </c>
-      <c r="I71" s="26"/>
+      <c r="I71" s="29"/>
       <c r="J71" t="s">
         <v>366</v>
       </c>
-      <c r="M71" s="27" t="s">
+      <c r="M71" s="30" t="s">
         <v>167</v>
       </c>
       <c r="N71" t="s">
         <v>385</v>
       </c>
-      <c r="Q71" s="26"/>
+      <c r="Q71" s="29"/>
       <c r="R71" t="s">
         <v>392</v>
       </c>
-      <c r="U71" s="27"/>
+      <c r="U71" s="30"/>
       <c r="V71" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A72" s="26"/>
+      <c r="A72" s="29"/>
       <c r="B72" t="s">
         <v>376</v>
       </c>
-      <c r="E72" s="26"/>
+      <c r="E72" s="29"/>
       <c r="F72" t="s">
         <v>401</v>
       </c>
-      <c r="I72" s="26"/>
+      <c r="I72" s="29"/>
       <c r="J72" t="s">
         <v>378</v>
       </c>
-      <c r="M72" s="27"/>
+      <c r="M72" s="30"/>
       <c r="N72" t="s">
         <v>391</v>
       </c>
-      <c r="Q72" s="26"/>
+      <c r="Q72" s="29"/>
       <c r="R72" t="s">
         <v>398</v>
       </c>
-      <c r="U72" s="27"/>
+      <c r="U72" s="30"/>
       <c r="V72" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A73" s="26"/>
+      <c r="A73" s="29"/>
       <c r="B73" t="s">
         <v>382</v>
       </c>
-      <c r="E73" s="27" t="s">
+      <c r="E73" s="30" t="s">
         <v>167</v>
       </c>
       <c r="F73" t="s">
         <v>406</v>
       </c>
-      <c r="I73" s="27" t="s">
+      <c r="I73" s="30" t="s">
         <v>167</v>
       </c>
       <c r="J73" t="s">
         <v>390</v>
       </c>
-      <c r="M73" s="27"/>
+      <c r="M73" s="30"/>
       <c r="N73" t="s">
         <v>397</v>
       </c>
-      <c r="Q73" s="26"/>
+      <c r="Q73" s="29"/>
       <c r="R73" t="s">
         <v>403</v>
       </c>
-      <c r="U73" s="27"/>
+      <c r="U73" s="30"/>
       <c r="V73" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A74" s="26"/>
+      <c r="A74" s="29"/>
       <c r="B74" t="s">
         <v>388</v>
       </c>
-      <c r="E74" s="27"/>
+      <c r="E74" s="30"/>
       <c r="F74" t="s">
         <v>410</v>
       </c>
-      <c r="I74" s="27"/>
+      <c r="I74" s="30"/>
       <c r="J74" t="s">
         <v>402</v>
       </c>
-      <c r="Q74" s="27" t="s">
+      <c r="Q74" s="30" t="s">
         <v>167</v>
       </c>
       <c r="R74" t="s">
-        <v>408</v>
-      </c>
-      <c r="U74" s="27"/>
+        <v>186</v>
+      </c>
+      <c r="U74" s="30"/>
       <c r="V74" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A75" s="27" t="s">
+      <c r="A75" s="30" t="s">
         <v>167</v>
       </c>
       <c r="B75" t="s">
         <v>394</v>
       </c>
-      <c r="E75" s="27"/>
+      <c r="E75" s="30"/>
       <c r="F75" t="s">
         <v>413</v>
       </c>
-      <c r="I75" s="27"/>
+      <c r="I75" s="30"/>
       <c r="J75" t="s">
         <v>411</v>
       </c>
-      <c r="Q75" s="27"/>
+      <c r="Q75" s="30"/>
       <c r="R75" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A76" s="27"/>
+      <c r="A76" s="30"/>
       <c r="B76" t="s">
         <v>400</v>
       </c>
-      <c r="I76" s="27"/>
+      <c r="I76" s="30"/>
       <c r="J76" t="s">
         <v>187</v>
       </c>
-      <c r="Q76" s="27"/>
+      <c r="Q76" s="30"/>
       <c r="R76" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A77" s="27"/>
+      <c r="A77" s="30"/>
       <c r="B77" t="s">
         <v>405</v>
       </c>
-      <c r="I77" s="27"/>
+      <c r="I77" s="30"/>
       <c r="J77" t="s">
         <v>396</v>
       </c>
-      <c r="Q77" s="27"/>
+      <c r="Q77" s="30"/>
       <c r="R77" t="s">
-        <v>415</v>
+        <v>168</v>
       </c>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A78" s="27"/>
+      <c r="A78" s="30"/>
       <c r="B78" t="s">
         <v>409</v>
       </c>
+      <c r="Q78" s="30"/>
+      <c r="R78" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q79" s="30"/>
+      <c r="R79" t="s">
+        <v>412</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="94">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="E41:E44"/>
+    <mergeCell ref="E21:E24"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="M65:M70"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="M41:M43"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="E62:E64"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="Q74:Q79"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="U40:V40"/>
+    <mergeCell ref="U44:U49"/>
+    <mergeCell ref="U60:U61"/>
+    <mergeCell ref="U50:U59"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="Q43:Q50"/>
+    <mergeCell ref="M44:M50"/>
+    <mergeCell ref="M51:M57"/>
+    <mergeCell ref="M58:M61"/>
+    <mergeCell ref="M30:M33"/>
+    <mergeCell ref="I4:I11"/>
+    <mergeCell ref="M5:M11"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="I29:I33"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="A44:A51"/>
+    <mergeCell ref="A52:A62"/>
+    <mergeCell ref="I42:I50"/>
+    <mergeCell ref="E45:E49"/>
+    <mergeCell ref="E50:E61"/>
+    <mergeCell ref="A63:A67"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="U70:U74"/>
+    <mergeCell ref="E69:E72"/>
+    <mergeCell ref="M71:M73"/>
+    <mergeCell ref="Q70:Q73"/>
+    <mergeCell ref="M62:M64"/>
+    <mergeCell ref="I63:I66"/>
+    <mergeCell ref="I73:I77"/>
+    <mergeCell ref="E73:E75"/>
+    <mergeCell ref="I67:I72"/>
+    <mergeCell ref="U29:U33"/>
+    <mergeCell ref="Q51:Q63"/>
+    <mergeCell ref="U5:U10"/>
+    <mergeCell ref="U11:U18"/>
+    <mergeCell ref="Q12:Q18"/>
+    <mergeCell ref="U62:U64"/>
+    <mergeCell ref="Q64:Q65"/>
+    <mergeCell ref="U65:U69"/>
+    <mergeCell ref="Q66:Q69"/>
+    <mergeCell ref="Q19:Q21"/>
+    <mergeCell ref="U19:U20"/>
+    <mergeCell ref="U21:U24"/>
+    <mergeCell ref="Q22:Q25"/>
+    <mergeCell ref="U25:U28"/>
+    <mergeCell ref="Q26:Q29"/>
+    <mergeCell ref="U41:U43"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="E10:E15"/>
+    <mergeCell ref="Q5:Q11"/>
+    <mergeCell ref="Q30:Q34"/>
+    <mergeCell ref="I12:I19"/>
+    <mergeCell ref="I21:I24"/>
+    <mergeCell ref="M23:M25"/>
+    <mergeCell ref="I25:I28"/>
+    <mergeCell ref="M26:M29"/>
+    <mergeCell ref="E4:E9"/>
+    <mergeCell ref="M20:M22"/>
+    <mergeCell ref="M12:M19"/>
+    <mergeCell ref="E16:E17"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A8:A15"/>
     <mergeCell ref="I51:I57"/>
@@ -4667,84 +4755,6 @@
     <mergeCell ref="M2:M4"/>
     <mergeCell ref="Q2:Q4"/>
     <mergeCell ref="U2:U4"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="E10:E15"/>
-    <mergeCell ref="Q5:Q11"/>
-    <mergeCell ref="Q30:Q34"/>
-    <mergeCell ref="I12:I19"/>
-    <mergeCell ref="U29:U33"/>
-    <mergeCell ref="Q51:Q63"/>
-    <mergeCell ref="U5:U10"/>
-    <mergeCell ref="U11:U18"/>
-    <mergeCell ref="Q12:Q18"/>
-    <mergeCell ref="U62:U64"/>
-    <mergeCell ref="Q64:Q65"/>
-    <mergeCell ref="U65:U69"/>
-    <mergeCell ref="Q66:Q69"/>
-    <mergeCell ref="Q19:Q21"/>
-    <mergeCell ref="U19:U20"/>
-    <mergeCell ref="I21:I24"/>
-    <mergeCell ref="U21:U24"/>
-    <mergeCell ref="Q22:Q25"/>
-    <mergeCell ref="M23:M25"/>
-    <mergeCell ref="I25:I28"/>
-    <mergeCell ref="U25:U28"/>
-    <mergeCell ref="M26:M29"/>
-    <mergeCell ref="Q26:Q29"/>
-    <mergeCell ref="U70:U74"/>
-    <mergeCell ref="E69:E72"/>
-    <mergeCell ref="M71:M73"/>
-    <mergeCell ref="Q70:Q73"/>
-    <mergeCell ref="M62:M64"/>
-    <mergeCell ref="I63:I66"/>
-    <mergeCell ref="I73:I77"/>
-    <mergeCell ref="E73:E75"/>
-    <mergeCell ref="I67:I72"/>
-    <mergeCell ref="E4:E9"/>
-    <mergeCell ref="M20:M22"/>
-    <mergeCell ref="M12:M19"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="A71:A74"/>
-    <mergeCell ref="I29:I33"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="A44:A51"/>
-    <mergeCell ref="A52:A62"/>
-    <mergeCell ref="I42:I50"/>
-    <mergeCell ref="E45:E49"/>
-    <mergeCell ref="E50:E61"/>
-    <mergeCell ref="A63:A67"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="M44:M50"/>
-    <mergeCell ref="M51:M57"/>
-    <mergeCell ref="M58:M61"/>
-    <mergeCell ref="M30:M33"/>
-    <mergeCell ref="I4:I11"/>
-    <mergeCell ref="M5:M11"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="U41:U43"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="U40:V40"/>
-    <mergeCell ref="U44:U49"/>
-    <mergeCell ref="U60:U61"/>
-    <mergeCell ref="U50:U59"/>
-    <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="Q43:Q50"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="E41:E44"/>
-    <mergeCell ref="E21:E24"/>
-    <mergeCell ref="Q74:Q77"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="M65:M70"/>
-    <mergeCell ref="E65:E68"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="M41:M43"/>
-    <mergeCell ref="A75:A78"/>
-    <mergeCell ref="E62:E64"/>
-    <mergeCell ref="M40:N40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4756,7 +4766,7 @@
   <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4778,38 +4788,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="E1" s="31" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="E1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="31"/>
+      <c r="F1" s="27"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="31" t="s">
+      <c r="L1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="31"/>
-      <c r="O1" s="31" t="s">
+      <c r="M1" s="27"/>
+      <c r="O1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="31"/>
-      <c r="R1" s="31" t="s">
+      <c r="P1" s="27"/>
+      <c r="R1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="31"/>
+      <c r="S1" s="27"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>635</v>
+        <v>488</v>
       </c>
       <c r="C2" t="s">
         <v>493</v>
@@ -5024,33 +5034,33 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="E17" s="31" t="s">
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="E17" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="I17" s="31" t="s">
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="I17" s="27" t="s">
         <v>605</v>
       </c>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31" t="s">
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="M17" s="31"/>
-      <c r="O17" s="31" t="s">
+      <c r="M17" s="27"/>
+      <c r="O17" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="P17" s="31"/>
-      <c r="R17" s="31" t="s">
+      <c r="P17" s="27"/>
+      <c r="R17" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="S17" s="31"/>
+      <c r="S17" s="27"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
@@ -5078,7 +5088,7 @@
         <v>487</v>
       </c>
       <c r="O18" t="s">
-        <v>488</v>
+        <v>635</v>
       </c>
       <c r="R18" t="s">
         <v>489</v>
@@ -5435,10 +5445,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B182"/>
+  <dimension ref="A1:B187"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A168" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B195" sqref="B195"/>
+      <selection activeCell="F189" sqref="F189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6518,6 +6528,35 @@
         <v>613</v>
       </c>
     </row>
+    <row r="183" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="18" t="s">
+        <v>577</v>
+      </c>
+      <c r="B184" s="19" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="9"/>
+      <c r="B185" s="20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="9"/>
+      <c r="B186" s="20" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A187" s="21" t="s">
+        <v>661</v>
+      </c>
+      <c r="B187" s="22" t="s">
+        <v>582</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
update drafted order on that tab/trade up!
</commit_message>
<xml_diff>
--- a/OffSeason.xlsx
+++ b/OffSeason.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sdwg-my.sharepoint.com/personal/john_olson_agtegra_com/Documents/Documents 1/Football/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="8_{ECA9F46E-F317-4CC4-8E17-E8E8FEC0C4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{061B4D5D-CEBD-4AF8-A8C9-04ADDF22582C}"/>
+  <xr:revisionPtr revIDLastSave="337" documentId="8_{ECA9F46E-F317-4CC4-8E17-E8E8FEC0C4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16D09D69-42A6-45BB-A92A-0930E4391361}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rosters" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="675">
   <si>
     <t>Vanja Dolas - CeeDee Nuts</t>
   </si>
@@ -2014,6 +2014,45 @@
   </si>
   <si>
     <t xml:space="preserve">Adam </t>
+  </si>
+  <si>
+    <t>2021 4.4</t>
+  </si>
+  <si>
+    <t>2022 3 Ben</t>
+  </si>
+  <si>
+    <t>Current Draft Order</t>
+  </si>
+  <si>
+    <t>John O</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>MattH</t>
+  </si>
+  <si>
+    <t>Zach</t>
+  </si>
+  <si>
+    <t>AdamW</t>
+  </si>
+  <si>
+    <t>Holland</t>
+  </si>
+  <si>
+    <t>AlanP</t>
+  </si>
+  <si>
+    <t>2022 3 Adam W</t>
+  </si>
+  <si>
+    <t>2021 2.6</t>
+  </si>
+  <si>
+    <t>2021 3.9</t>
   </si>
 </sst>
 </file>
@@ -2224,7 +2263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2256,22 +2295,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2280,6 +2307,19 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2665,8 +2705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W79"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12:N14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2682,71 +2722,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="E1" s="27" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="E1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="27"/>
+      <c r="F1" s="31"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="27"/>
+      <c r="N1" s="31"/>
       <c r="O1" s="1"/>
-      <c r="Q1" s="27" t="s">
+      <c r="Q1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="27"/>
+      <c r="R1" s="31"/>
       <c r="S1" s="1"/>
-      <c r="U1" s="27" t="s">
+      <c r="U1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="27"/>
+      <c r="V1" s="31"/>
       <c r="W1" s="1"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="M2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="N2" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="28" t="s">
+      <c r="Q2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="R2" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="28" t="s">
+      <c r="U2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="V2" t="s">
@@ -2754,89 +2794,89 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
+      <c r="A3" s="25"/>
       <c r="B3" t="s">
         <v>209</v>
       </c>
-      <c r="E3" s="28"/>
+      <c r="E3" s="25"/>
       <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="28"/>
+      <c r="I3" s="25"/>
       <c r="J3" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="28"/>
+      <c r="M3" s="25"/>
       <c r="N3" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="28"/>
+      <c r="Q3" s="25"/>
       <c r="R3" t="s">
         <v>17</v>
       </c>
-      <c r="U3" s="28"/>
+      <c r="U3" s="25"/>
       <c r="V3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="27" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="27" t="s">
         <v>20</v>
       </c>
       <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="31" t="s">
+      <c r="I4" s="27" t="s">
         <v>20</v>
       </c>
       <c r="J4" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="28"/>
+      <c r="M4" s="25"/>
       <c r="N4" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" s="28"/>
+      <c r="Q4" s="25"/>
       <c r="R4" t="s">
         <v>24</v>
       </c>
-      <c r="U4" s="28"/>
+      <c r="U4" s="25"/>
       <c r="V4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
+      <c r="A5" s="27"/>
       <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="27"/>
       <c r="F5" t="s">
         <v>227</v>
       </c>
-      <c r="I5" s="31"/>
+      <c r="I5" s="27"/>
       <c r="J5" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="M5" s="27" t="s">
         <v>20</v>
       </c>
       <c r="N5" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="31" t="s">
+      <c r="Q5" s="27" t="s">
         <v>20</v>
       </c>
       <c r="R5" t="s">
         <v>30</v>
       </c>
-      <c r="U5" s="31" t="s">
+      <c r="U5" s="27" t="s">
         <v>20</v>
       </c>
       <c r="V5" t="s">
@@ -2844,161 +2884,161 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="27"/>
       <c r="B6" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="27"/>
       <c r="F6" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="31"/>
+      <c r="I6" s="27"/>
       <c r="J6" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="31"/>
+      <c r="M6" s="27"/>
       <c r="N6" t="s">
         <v>35</v>
       </c>
-      <c r="Q6" s="31"/>
+      <c r="Q6" s="27"/>
       <c r="R6" t="s">
         <v>36</v>
       </c>
-      <c r="U6" s="31"/>
+      <c r="U6" s="27"/>
       <c r="V6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="27"/>
       <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="27"/>
       <c r="F7" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="31"/>
+      <c r="I7" s="27"/>
       <c r="J7" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="31"/>
+      <c r="M7" s="27"/>
       <c r="N7" t="s">
         <v>41</v>
       </c>
-      <c r="Q7" s="31"/>
+      <c r="Q7" s="27"/>
       <c r="R7" t="s">
         <v>42</v>
       </c>
-      <c r="U7" s="31"/>
+      <c r="U7" s="27"/>
       <c r="V7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="32" t="s">
         <v>44</v>
       </c>
       <c r="B8" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="31"/>
+      <c r="E8" s="27"/>
       <c r="F8" t="s">
         <v>52</v>
       </c>
-      <c r="I8" s="31"/>
+      <c r="I8" s="27"/>
       <c r="J8" t="s">
         <v>47</v>
       </c>
-      <c r="M8" s="31"/>
+      <c r="M8" s="27"/>
       <c r="N8" t="s">
         <v>48</v>
       </c>
-      <c r="Q8" s="31"/>
+      <c r="Q8" s="27"/>
       <c r="R8" t="s">
         <v>49</v>
       </c>
-      <c r="U8" s="31"/>
+      <c r="U8" s="27"/>
       <c r="V8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
+      <c r="A9" s="32"/>
       <c r="B9" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="31"/>
+      <c r="E9" s="27"/>
       <c r="F9" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="31"/>
+      <c r="I9" s="27"/>
       <c r="J9" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="31"/>
+      <c r="M9" s="27"/>
       <c r="N9" t="s">
         <v>54</v>
       </c>
-      <c r="Q9" s="31"/>
+      <c r="Q9" s="27"/>
       <c r="R9" t="s">
         <v>55</v>
       </c>
-      <c r="U9" s="31"/>
+      <c r="U9" s="27"/>
       <c r="V9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+      <c r="A10" s="32"/>
       <c r="B10" t="s">
         <v>281</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="32" t="s">
         <v>44</v>
       </c>
       <c r="F10" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="31"/>
+      <c r="I10" s="27"/>
       <c r="J10" t="s">
         <v>59</v>
       </c>
-      <c r="M10" s="31"/>
+      <c r="M10" s="27"/>
       <c r="N10" t="s">
         <v>60</v>
       </c>
-      <c r="Q10" s="31"/>
+      <c r="Q10" s="27"/>
       <c r="R10" t="s">
         <v>61</v>
       </c>
-      <c r="U10" s="31"/>
+      <c r="U10" s="27"/>
       <c r="V10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="32"/>
       <c r="B11" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="26"/>
+      <c r="E11" s="32"/>
       <c r="F11" t="s">
         <v>70</v>
       </c>
-      <c r="I11" s="31"/>
+      <c r="I11" s="27"/>
       <c r="J11" t="s">
         <v>65</v>
       </c>
-      <c r="M11" s="31"/>
+      <c r="M11" s="27"/>
       <c r="N11" t="s">
         <v>66</v>
       </c>
-      <c r="Q11" s="31"/>
+      <c r="Q11" s="27"/>
       <c r="R11" t="s">
         <v>67</v>
       </c>
-      <c r="U11" s="26" t="s">
+      <c r="U11" s="32" t="s">
         <v>44</v>
       </c>
       <c r="V11" t="s">
@@ -3006,225 +3046,225 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+      <c r="A12" s="32"/>
       <c r="B12" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="26"/>
+      <c r="E12" s="32"/>
       <c r="F12" t="s">
         <v>88</v>
       </c>
-      <c r="I12" s="26" t="s">
+      <c r="I12" s="32" t="s">
         <v>44</v>
       </c>
       <c r="J12" t="s">
         <v>71</v>
       </c>
-      <c r="M12" s="26" t="s">
-        <v>44</v>
-      </c>
+      <c r="M12" s="27"/>
       <c r="N12" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q12" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q12" s="32" t="s">
         <v>44</v>
       </c>
       <c r="R12" t="s">
         <v>73</v>
       </c>
-      <c r="U12" s="26"/>
+      <c r="U12" s="32"/>
       <c r="V12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="A13" s="32"/>
       <c r="B13" t="s">
         <v>270</v>
       </c>
-      <c r="E13" s="26"/>
+      <c r="E13" s="32"/>
       <c r="F13" t="s">
         <v>82</v>
       </c>
-      <c r="I13" s="26"/>
+      <c r="I13" s="32"/>
       <c r="J13" t="s">
         <v>77</v>
       </c>
-      <c r="M13" s="26"/>
+      <c r="M13" s="32" t="s">
+        <v>44</v>
+      </c>
       <c r="N13" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q13" s="26"/>
+        <v>72</v>
+      </c>
+      <c r="Q13" s="32"/>
       <c r="R13" t="s">
         <v>79</v>
       </c>
-      <c r="U13" s="26"/>
+      <c r="U13" s="32"/>
       <c r="V13" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="32"/>
       <c r="B14" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="26"/>
+      <c r="E14" s="32"/>
       <c r="F14" t="s">
         <v>95</v>
       </c>
-      <c r="I14" s="26"/>
+      <c r="I14" s="32"/>
       <c r="J14" t="s">
         <v>83</v>
       </c>
-      <c r="M14" s="26"/>
+      <c r="M14" s="32"/>
       <c r="N14" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q14" s="26"/>
+        <v>78</v>
+      </c>
+      <c r="Q14" s="32"/>
       <c r="R14" t="s">
         <v>85</v>
       </c>
-      <c r="U14" s="26"/>
+      <c r="U14" s="32"/>
       <c r="V14" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+      <c r="A15" s="32"/>
       <c r="B15" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="26"/>
+      <c r="E15" s="32"/>
       <c r="F15" t="s">
         <v>294</v>
       </c>
-      <c r="I15" s="26"/>
+      <c r="I15" s="32"/>
       <c r="J15" t="s">
         <v>89</v>
       </c>
-      <c r="M15" s="26"/>
+      <c r="M15" s="32"/>
       <c r="N15" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q15" s="26"/>
+        <v>84</v>
+      </c>
+      <c r="Q15" s="32"/>
       <c r="R15" t="s">
         <v>91</v>
       </c>
-      <c r="U15" s="26"/>
+      <c r="U15" s="32"/>
       <c r="V15" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="30" t="s">
         <v>93</v>
       </c>
       <c r="B16" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="30" t="s">
         <v>93</v>
       </c>
       <c r="F16" t="s">
         <v>101</v>
       </c>
-      <c r="I16" s="26"/>
+      <c r="I16" s="32"/>
       <c r="J16" t="s">
         <v>96</v>
       </c>
-      <c r="M16" s="26"/>
+      <c r="M16" s="32"/>
       <c r="N16" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q16" s="26"/>
+        <v>90</v>
+      </c>
+      <c r="Q16" s="32"/>
       <c r="R16" t="s">
         <v>98</v>
       </c>
-      <c r="U16" s="26"/>
+      <c r="U16" s="32"/>
       <c r="V16" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="30"/>
       <c r="B17" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="25"/>
+      <c r="E17" s="30"/>
       <c r="F17" t="s">
         <v>107</v>
       </c>
-      <c r="I17" s="26"/>
+      <c r="I17" s="32"/>
       <c r="J17" t="s">
         <v>102</v>
       </c>
-      <c r="M17" s="26"/>
+      <c r="M17" s="32"/>
       <c r="N17" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q17" s="26"/>
+        <v>97</v>
+      </c>
+      <c r="Q17" s="32"/>
       <c r="R17" t="s">
         <v>104</v>
       </c>
-      <c r="U17" s="26"/>
+      <c r="U17" s="32"/>
       <c r="V17" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="30"/>
       <c r="B18" t="s">
         <v>112</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="28" t="s">
         <v>113</v>
       </c>
       <c r="F18" t="s">
         <v>120</v>
       </c>
-      <c r="I18" s="26"/>
+      <c r="I18" s="32"/>
       <c r="J18" t="s">
         <v>108</v>
       </c>
-      <c r="M18" s="26"/>
+      <c r="M18" s="32"/>
       <c r="N18" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q18" s="26"/>
+        <v>103</v>
+      </c>
+      <c r="Q18" s="32"/>
       <c r="R18" t="s">
         <v>110</v>
       </c>
-      <c r="U18" s="26"/>
+      <c r="U18" s="32"/>
       <c r="V18" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="28" t="s">
         <v>113</v>
       </c>
       <c r="B19" t="s">
         <v>119</v>
       </c>
-      <c r="E19" s="32"/>
+      <c r="E19" s="28"/>
       <c r="F19" t="s">
         <v>126</v>
       </c>
-      <c r="I19" s="26"/>
+      <c r="I19" s="32"/>
       <c r="J19" t="s">
         <v>115</v>
       </c>
-      <c r="M19" s="26"/>
+      <c r="M19" s="32"/>
       <c r="N19" t="s">
-        <v>301</v>
-      </c>
-      <c r="Q19" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q19" s="30" t="s">
         <v>93</v>
       </c>
       <c r="R19" t="s">
         <v>117</v>
       </c>
-      <c r="U19" s="25" t="s">
+      <c r="U19" s="30" t="s">
         <v>93</v>
       </c>
       <c r="V19" t="s">
@@ -3232,11 +3272,11 @@
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
+      <c r="A20" s="28"/>
       <c r="B20" t="s">
         <v>131</v>
       </c>
-      <c r="E20" s="32"/>
+      <c r="E20" s="28"/>
       <c r="F20" t="s">
         <v>132</v>
       </c>
@@ -3246,47 +3286,45 @@
       <c r="J20" t="s">
         <v>121</v>
       </c>
-      <c r="M20" s="25" t="s">
-        <v>93</v>
-      </c>
+      <c r="M20" s="32"/>
       <c r="N20" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q20" s="25"/>
+        <v>301</v>
+      </c>
+      <c r="Q20" s="30"/>
       <c r="R20" t="s">
         <v>123</v>
       </c>
-      <c r="U20" s="25"/>
+      <c r="U20" s="30"/>
       <c r="V20" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
+      <c r="A21" s="28"/>
       <c r="B21" t="s">
         <v>114</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="26" t="s">
         <v>137</v>
       </c>
       <c r="F21" t="s">
         <v>139</v>
       </c>
-      <c r="I21" s="32" t="s">
+      <c r="I21" s="28" t="s">
         <v>113</v>
       </c>
       <c r="J21" t="s">
         <v>127</v>
       </c>
-      <c r="M21" s="25"/>
+      <c r="M21" s="32"/>
       <c r="N21" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q21" s="25"/>
+        <v>282</v>
+      </c>
+      <c r="Q21" s="30"/>
       <c r="R21" t="s">
         <v>129</v>
       </c>
-      <c r="U21" s="32" t="s">
+      <c r="U21" s="28" t="s">
         <v>113</v>
       </c>
       <c r="V21" t="s">
@@ -3294,115 +3332,117 @@
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="26" t="s">
         <v>137</v>
       </c>
       <c r="B22" t="s">
         <v>138</v>
       </c>
-      <c r="E22" s="29"/>
+      <c r="E22" s="26"/>
       <c r="F22" t="s">
         <v>145</v>
       </c>
-      <c r="I22" s="32"/>
+      <c r="I22" s="28"/>
       <c r="J22" t="s">
         <v>133</v>
       </c>
-      <c r="M22" s="25"/>
+      <c r="M22" s="30" t="s">
+        <v>93</v>
+      </c>
       <c r="N22" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q22" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q22" s="28" t="s">
         <v>113</v>
       </c>
       <c r="R22" t="s">
         <v>135</v>
       </c>
-      <c r="U22" s="32"/>
+      <c r="U22" s="28"/>
       <c r="V22" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
+      <c r="A23" s="26"/>
       <c r="B23" t="s">
         <v>144</v>
       </c>
-      <c r="E23" s="29"/>
+      <c r="E23" s="26"/>
       <c r="F23" t="s">
         <v>151</v>
       </c>
-      <c r="I23" s="32"/>
+      <c r="I23" s="28"/>
       <c r="J23" t="s">
         <v>140</v>
       </c>
-      <c r="M23" s="32" t="s">
-        <v>113</v>
-      </c>
+      <c r="M23" s="30"/>
       <c r="N23" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q23" s="32"/>
+        <v>122</v>
+      </c>
+      <c r="Q23" s="28"/>
       <c r="R23" t="s">
         <v>142</v>
       </c>
-      <c r="U23" s="32"/>
+      <c r="U23" s="28"/>
       <c r="V23" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
+      <c r="A24" s="26"/>
       <c r="B24" t="s">
         <v>150</v>
       </c>
-      <c r="E24" s="29"/>
+      <c r="E24" s="26"/>
       <c r="F24" t="s">
         <v>157</v>
       </c>
-      <c r="I24" s="32"/>
+      <c r="I24" s="28"/>
       <c r="J24" t="s">
         <v>146</v>
       </c>
-      <c r="M24" s="32"/>
+      <c r="M24" s="30"/>
       <c r="N24" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q24" s="32"/>
+        <v>134</v>
+      </c>
+      <c r="Q24" s="28"/>
       <c r="R24" t="s">
         <v>148</v>
       </c>
-      <c r="U24" s="32"/>
+      <c r="U24" s="28"/>
       <c r="V24" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+      <c r="A25" s="26"/>
       <c r="B25" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="E25" s="29" t="s">
         <v>167</v>
       </c>
       <c r="F25" t="s">
         <v>169</v>
       </c>
-      <c r="I25" s="29" t="s">
+      <c r="I25" s="26" t="s">
         <v>137</v>
       </c>
       <c r="J25" t="s">
         <v>152</v>
       </c>
-      <c r="M25" s="32"/>
+      <c r="M25" s="28" t="s">
+        <v>113</v>
+      </c>
       <c r="N25" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q25" s="32"/>
+        <v>141</v>
+      </c>
+      <c r="Q25" s="28"/>
       <c r="R25" t="s">
         <v>154</v>
       </c>
-      <c r="U25" s="29" t="s">
+      <c r="U25" s="26" t="s">
         <v>137</v>
       </c>
       <c r="V25" t="s">
@@ -3410,105 +3450,105 @@
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="29" t="s">
         <v>167</v>
       </c>
       <c r="B26" t="s">
         <v>193</v>
       </c>
-      <c r="E26" s="30"/>
+      <c r="E26" s="29"/>
       <c r="F26" t="s">
         <v>175</v>
       </c>
-      <c r="I26" s="29"/>
+      <c r="I26" s="26"/>
       <c r="J26" t="s">
         <v>158</v>
       </c>
-      <c r="M26" s="29" t="s">
-        <v>137</v>
-      </c>
+      <c r="M26" s="28"/>
       <c r="N26" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q26" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q26" s="26" t="s">
         <v>137</v>
       </c>
       <c r="R26" t="s">
         <v>160</v>
       </c>
-      <c r="U26" s="29"/>
+      <c r="U26" s="26"/>
       <c r="V26" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
+      <c r="A27" s="29"/>
       <c r="B27" t="s">
         <v>174</v>
       </c>
-      <c r="E27" s="30"/>
+      <c r="E27" s="29"/>
       <c r="F27" t="s">
         <v>181</v>
       </c>
-      <c r="I27" s="29"/>
+      <c r="I27" s="26"/>
       <c r="J27" t="s">
         <v>163</v>
       </c>
-      <c r="M27" s="29"/>
+      <c r="M27" s="28"/>
       <c r="N27" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q27" s="29"/>
+        <v>153</v>
+      </c>
+      <c r="Q27" s="26"/>
       <c r="R27" t="s">
         <v>165</v>
       </c>
-      <c r="U27" s="29"/>
+      <c r="U27" s="26"/>
       <c r="V27" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
+      <c r="A28" s="29"/>
       <c r="B28" t="s">
         <v>192</v>
       </c>
-      <c r="I28" s="29"/>
+      <c r="I28" s="26"/>
       <c r="J28" t="s">
         <v>170</v>
       </c>
-      <c r="M28" s="29"/>
+      <c r="M28" s="26" t="s">
+        <v>137</v>
+      </c>
       <c r="N28" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q28" s="29"/>
+        <v>159</v>
+      </c>
+      <c r="Q28" s="26"/>
       <c r="R28" t="s">
         <v>172</v>
       </c>
-      <c r="U28" s="29"/>
+      <c r="U28" s="26"/>
       <c r="V28" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
+      <c r="A29" s="29"/>
       <c r="B29" t="s">
         <v>180</v>
       </c>
-      <c r="I29" s="30" t="s">
+      <c r="I29" s="29" t="s">
         <v>167</v>
       </c>
       <c r="J29" t="s">
         <v>176</v>
       </c>
-      <c r="M29" s="29"/>
+      <c r="M29" s="26"/>
       <c r="N29" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q29" s="29"/>
+        <v>164</v>
+      </c>
+      <c r="Q29" s="26"/>
       <c r="R29" t="s">
         <v>178</v>
       </c>
-      <c r="U29" s="30" t="s">
+      <c r="U29" s="29" t="s">
         <v>167</v>
       </c>
       <c r="V29" t="s">
@@ -3516,131 +3556,139 @@
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="I30" s="30"/>
+      <c r="I30" s="29"/>
       <c r="J30" t="s">
         <v>182</v>
       </c>
-      <c r="M30" s="30" t="s">
-        <v>167</v>
-      </c>
+      <c r="M30" s="26"/>
       <c r="N30" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q30" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q30" s="29" t="s">
         <v>167</v>
       </c>
       <c r="R30" t="s">
         <v>184</v>
       </c>
-      <c r="U30" s="30"/>
+      <c r="U30" s="29"/>
       <c r="V30" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="I31" s="30"/>
+      <c r="I31" s="29"/>
       <c r="J31" t="s">
         <v>188</v>
       </c>
-      <c r="M31" s="30"/>
+      <c r="M31" s="26"/>
       <c r="N31" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q31" s="30"/>
+        <v>177</v>
+      </c>
+      <c r="Q31" s="29"/>
       <c r="R31" t="s">
         <v>190</v>
       </c>
-      <c r="U31" s="30"/>
+      <c r="U31" s="29"/>
       <c r="V31" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="I32" s="30"/>
+      <c r="I32" s="29"/>
       <c r="J32" t="s">
         <v>194</v>
       </c>
-      <c r="M32" s="30"/>
+      <c r="M32" s="29" t="s">
+        <v>167</v>
+      </c>
       <c r="N32" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q32" s="30"/>
+        <v>183</v>
+      </c>
+      <c r="Q32" s="29"/>
       <c r="R32" t="s">
         <v>196</v>
       </c>
-      <c r="U32" s="30"/>
+      <c r="U32" s="29"/>
       <c r="V32" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="I33" s="30"/>
+      <c r="I33" s="29"/>
       <c r="J33" t="s">
         <v>198</v>
       </c>
-      <c r="M33" s="30"/>
+      <c r="M33" s="29"/>
       <c r="N33" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q33" s="30"/>
+        <v>189</v>
+      </c>
+      <c r="Q33" s="29"/>
       <c r="R33" t="s">
         <v>200</v>
       </c>
-      <c r="U33" s="30"/>
+      <c r="U33" s="29"/>
       <c r="V33" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="Q34" s="30"/>
+      <c r="M34" s="29"/>
+      <c r="N34" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q34" s="29"/>
       <c r="R34" t="s">
         <v>202</v>
       </c>
       <c r="U34" s="3"/>
     </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="M35" s="29"/>
+      <c r="N35" t="s">
+        <v>199</v>
+      </c>
+    </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-      <c r="E40" s="27" t="s">
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="E40" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="I40" s="27" t="s">
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="I40" s="31" t="s">
         <v>605</v>
       </c>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="31"/>
       <c r="L40" s="1"/>
-      <c r="M40" s="27" t="s">
+      <c r="M40" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="N40" s="27"/>
+      <c r="N40" s="31"/>
       <c r="O40" s="1"/>
-      <c r="Q40" s="27" t="s">
+      <c r="Q40" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="R40" s="27"/>
+      <c r="R40" s="31"/>
       <c r="S40" s="1"/>
-      <c r="U40" s="27" t="s">
+      <c r="U40" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="V40" s="27"/>
+      <c r="V40" s="31"/>
       <c r="W40" s="1"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
+      <c r="A41" s="25" t="s">
         <v>6</v>
       </c>
       <c r="B41" t="s">
         <v>208</v>
       </c>
-      <c r="E41" s="28" t="s">
+      <c r="E41" s="25" t="s">
         <v>6</v>
       </c>
       <c r="F41" t="s">
@@ -3652,19 +3700,19 @@
       <c r="J41" t="s">
         <v>216</v>
       </c>
-      <c r="M41" s="28" t="s">
+      <c r="M41" s="25" t="s">
         <v>6</v>
       </c>
       <c r="N41" t="s">
         <v>211</v>
       </c>
-      <c r="Q41" s="28" t="s">
+      <c r="Q41" s="25" t="s">
         <v>6</v>
       </c>
       <c r="R41" t="s">
         <v>212</v>
       </c>
-      <c r="U41" s="28" t="s">
+      <c r="U41" s="25" t="s">
         <v>6</v>
       </c>
       <c r="V41" t="s">
@@ -3672,87 +3720,87 @@
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A42" s="28"/>
+      <c r="A42" s="25"/>
       <c r="B42" t="s">
         <v>214</v>
       </c>
-      <c r="E42" s="28"/>
+      <c r="E42" s="25"/>
       <c r="F42" t="s">
         <v>19</v>
       </c>
-      <c r="I42" s="31" t="s">
+      <c r="I42" s="27" t="s">
         <v>20</v>
       </c>
       <c r="J42" t="s">
         <v>222</v>
       </c>
-      <c r="M42" s="28"/>
+      <c r="M42" s="25"/>
       <c r="N42" t="s">
         <v>217</v>
       </c>
-      <c r="Q42" s="28"/>
+      <c r="Q42" s="25"/>
       <c r="R42" t="s">
         <v>218</v>
       </c>
-      <c r="U42" s="28"/>
+      <c r="U42" s="25"/>
       <c r="V42" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A43" s="28"/>
+      <c r="A43" s="25"/>
       <c r="B43" t="s">
         <v>220</v>
       </c>
-      <c r="E43" s="28"/>
+      <c r="E43" s="25"/>
       <c r="F43" t="s">
         <v>215</v>
       </c>
-      <c r="I43" s="31"/>
+      <c r="I43" s="27"/>
       <c r="J43" t="s">
         <v>46</v>
       </c>
-      <c r="M43" s="28"/>
+      <c r="M43" s="25"/>
       <c r="N43" t="s">
         <v>223</v>
       </c>
-      <c r="Q43" s="31" t="s">
+      <c r="Q43" s="27" t="s">
         <v>20</v>
       </c>
       <c r="R43" t="s">
         <v>224</v>
       </c>
-      <c r="U43" s="28"/>
+      <c r="U43" s="25"/>
       <c r="V43" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="27" t="s">
         <v>20</v>
       </c>
       <c r="B44" t="s">
         <v>226</v>
       </c>
-      <c r="E44" s="28"/>
+      <c r="E44" s="25"/>
       <c r="F44" t="s">
         <v>221</v>
       </c>
-      <c r="I44" s="31"/>
+      <c r="I44" s="27"/>
       <c r="J44" t="s">
         <v>245</v>
       </c>
-      <c r="M44" s="31" t="s">
+      <c r="M44" s="27" t="s">
         <v>20</v>
       </c>
       <c r="N44" t="s">
         <v>229</v>
       </c>
-      <c r="Q44" s="31"/>
+      <c r="Q44" s="27"/>
       <c r="R44" t="s">
         <v>230</v>
       </c>
-      <c r="U44" s="31" t="s">
+      <c r="U44" s="27" t="s">
         <v>20</v>
       </c>
       <c r="V44" t="s">
@@ -3760,161 +3808,163 @@
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A45" s="31"/>
+      <c r="A45" s="27"/>
       <c r="B45" t="s">
         <v>233</v>
       </c>
-      <c r="E45" s="31" t="s">
+      <c r="E45" s="27" t="s">
         <v>20</v>
       </c>
       <c r="F45" t="s">
         <v>239</v>
       </c>
-      <c r="I45" s="31"/>
+      <c r="I45" s="27"/>
       <c r="J45" t="s">
         <v>234</v>
       </c>
-      <c r="M45" s="31"/>
+      <c r="M45" s="27"/>
       <c r="N45" t="s">
         <v>235</v>
       </c>
-      <c r="Q45" s="31"/>
+      <c r="Q45" s="27"/>
       <c r="R45" t="s">
         <v>236</v>
       </c>
-      <c r="U45" s="31"/>
+      <c r="U45" s="27"/>
       <c r="V45" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A46" s="31"/>
+      <c r="A46" s="27"/>
       <c r="B46" t="s">
         <v>232</v>
       </c>
-      <c r="E46" s="31"/>
+      <c r="E46" s="27"/>
       <c r="F46" t="s">
         <v>251</v>
       </c>
-      <c r="I46" s="31"/>
+      <c r="I46" s="27"/>
       <c r="J46" t="s">
         <v>252</v>
       </c>
-      <c r="M46" s="31"/>
+      <c r="M46" s="27"/>
       <c r="N46" t="s">
         <v>241</v>
       </c>
-      <c r="Q46" s="31"/>
+      <c r="Q46" s="27"/>
       <c r="R46" t="s">
         <v>242</v>
       </c>
-      <c r="U46" s="31"/>
+      <c r="U46" s="27"/>
       <c r="V46" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
+      <c r="A47" s="27"/>
       <c r="B47" t="s">
         <v>238</v>
       </c>
-      <c r="E47" s="31"/>
+      <c r="E47" s="27"/>
       <c r="F47" t="s">
         <v>257</v>
       </c>
-      <c r="I47" s="31"/>
+      <c r="I47" s="27"/>
       <c r="J47" t="s">
         <v>258</v>
       </c>
-      <c r="M47" s="31"/>
+      <c r="M47" s="27"/>
       <c r="N47" t="s">
         <v>247</v>
       </c>
-      <c r="Q47" s="31"/>
+      <c r="Q47" s="27"/>
       <c r="R47" t="s">
         <v>248</v>
       </c>
-      <c r="U47" s="31"/>
+      <c r="U47" s="27"/>
       <c r="V47" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
+      <c r="A48" s="27"/>
       <c r="B48" t="s">
         <v>244</v>
       </c>
-      <c r="E48" s="31"/>
+      <c r="E48" s="27"/>
       <c r="F48" t="s">
         <v>263</v>
       </c>
-      <c r="I48" s="31"/>
+      <c r="I48" s="27"/>
       <c r="J48" t="s">
         <v>264</v>
       </c>
-      <c r="M48" s="31"/>
+      <c r="M48" s="27"/>
       <c r="N48" t="s">
         <v>253</v>
       </c>
-      <c r="Q48" s="31"/>
+      <c r="Q48" s="27"/>
       <c r="R48" t="s">
         <v>254</v>
       </c>
-      <c r="U48" s="31"/>
+      <c r="U48" s="27"/>
       <c r="V48" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A49" s="31"/>
+      <c r="A49" s="27"/>
       <c r="B49" t="s">
         <v>250</v>
       </c>
-      <c r="E49" s="31"/>
+      <c r="E49" s="27"/>
       <c r="F49" t="s">
         <v>240</v>
       </c>
-      <c r="I49" s="31"/>
+      <c r="I49" s="27"/>
       <c r="J49" t="s">
-        <v>228</v>
-      </c>
-      <c r="M49" s="31"/>
+        <v>246</v>
+      </c>
+      <c r="M49" s="27"/>
       <c r="N49" t="s">
         <v>259</v>
       </c>
-      <c r="Q49" s="31"/>
+      <c r="Q49" s="27"/>
       <c r="R49" t="s">
         <v>260</v>
       </c>
-      <c r="U49" s="31"/>
+      <c r="U49" s="27"/>
       <c r="V49" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A50" s="31"/>
+      <c r="A50" s="27"/>
       <c r="B50" t="s">
         <v>256</v>
       </c>
-      <c r="E50" s="26" t="s">
+      <c r="E50" s="32" t="s">
         <v>44</v>
       </c>
       <c r="F50" t="s">
         <v>269</v>
       </c>
-      <c r="I50" s="31"/>
+      <c r="I50" s="32" t="s">
+        <v>44</v>
+      </c>
       <c r="J50" t="s">
-        <v>246</v>
-      </c>
-      <c r="M50" s="31"/>
+        <v>76</v>
+      </c>
+      <c r="M50" s="27"/>
       <c r="N50" t="s">
         <v>265</v>
       </c>
-      <c r="Q50" s="31"/>
+      <c r="Q50" s="27"/>
       <c r="R50" t="s">
         <v>266</v>
       </c>
-      <c r="U50" s="26" t="s">
+      <c r="U50" s="32" t="s">
         <v>44</v>
       </c>
       <c r="V50" t="s">
@@ -3922,273 +3972,271 @@
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A51" s="31"/>
+      <c r="A51" s="27"/>
       <c r="B51" t="s">
         <v>262</v>
       </c>
-      <c r="E51" s="26"/>
+      <c r="E51" s="32"/>
       <c r="F51" t="s">
         <v>275</v>
       </c>
-      <c r="I51" s="26" t="s">
-        <v>44</v>
-      </c>
+      <c r="I51" s="32"/>
       <c r="J51" t="s">
-        <v>76</v>
-      </c>
-      <c r="M51" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="M51" s="32" t="s">
         <v>44</v>
       </c>
       <c r="N51" t="s">
         <v>271</v>
       </c>
-      <c r="Q51" s="26" t="s">
+      <c r="Q51" s="32" t="s">
         <v>44</v>
       </c>
       <c r="R51" t="s">
         <v>272</v>
       </c>
-      <c r="U51" s="26"/>
+      <c r="U51" s="32"/>
       <c r="V51" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A52" s="26" t="s">
+      <c r="A52" s="32" t="s">
         <v>44</v>
       </c>
       <c r="B52" t="s">
         <v>268</v>
       </c>
-      <c r="E52" s="26"/>
+      <c r="E52" s="32"/>
       <c r="F52" t="s">
         <v>63</v>
       </c>
-      <c r="I52" s="26"/>
+      <c r="I52" s="32"/>
       <c r="J52" t="s">
-        <v>276</v>
-      </c>
-      <c r="M52" s="26"/>
+        <v>300</v>
+      </c>
+      <c r="M52" s="32"/>
       <c r="N52" t="s">
         <v>277</v>
       </c>
-      <c r="Q52" s="26"/>
+      <c r="Q52" s="32"/>
       <c r="R52" t="s">
         <v>278</v>
       </c>
-      <c r="U52" s="26"/>
+      <c r="U52" s="32"/>
       <c r="V52" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A53" s="26"/>
+      <c r="A53" s="32"/>
       <c r="B53" t="s">
         <v>274</v>
       </c>
-      <c r="E53" s="26"/>
+      <c r="E53" s="32"/>
       <c r="F53" t="s">
         <v>287</v>
       </c>
-      <c r="I53" s="26"/>
+      <c r="I53" s="32"/>
       <c r="J53" t="s">
-        <v>300</v>
-      </c>
-      <c r="M53" s="26"/>
+        <v>288</v>
+      </c>
+      <c r="M53" s="32"/>
       <c r="N53" t="s">
         <v>283</v>
       </c>
-      <c r="Q53" s="26"/>
+      <c r="Q53" s="32"/>
       <c r="R53" t="s">
         <v>284</v>
       </c>
-      <c r="U53" s="26"/>
+      <c r="U53" s="32"/>
       <c r="V53" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A54" s="26"/>
+      <c r="A54" s="32"/>
       <c r="B54" t="s">
         <v>280</v>
       </c>
-      <c r="E54" s="26"/>
+      <c r="E54" s="32"/>
       <c r="F54" t="s">
         <v>293</v>
       </c>
-      <c r="I54" s="26"/>
+      <c r="I54" s="32"/>
       <c r="J54" t="s">
-        <v>288</v>
-      </c>
-      <c r="M54" s="26"/>
+        <v>306</v>
+      </c>
+      <c r="M54" s="32"/>
       <c r="N54" t="s">
         <v>289</v>
       </c>
-      <c r="Q54" s="26"/>
+      <c r="Q54" s="32"/>
       <c r="R54" t="s">
         <v>290</v>
       </c>
-      <c r="U54" s="26"/>
+      <c r="U54" s="32"/>
       <c r="V54" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A55" s="26"/>
+      <c r="A55" s="32"/>
       <c r="B55" t="s">
         <v>286</v>
       </c>
-      <c r="E55" s="26"/>
+      <c r="E55" s="32"/>
       <c r="F55" t="s">
         <v>312</v>
       </c>
-      <c r="I55" s="26"/>
+      <c r="I55" s="32"/>
       <c r="J55" t="s">
-        <v>306</v>
-      </c>
-      <c r="M55" s="26"/>
+        <v>57</v>
+      </c>
+      <c r="M55" s="32"/>
       <c r="N55" t="s">
         <v>295</v>
       </c>
-      <c r="Q55" s="26"/>
+      <c r="Q55" s="32"/>
       <c r="R55" t="s">
         <v>296</v>
       </c>
-      <c r="U55" s="26"/>
+      <c r="U55" s="32"/>
       <c r="V55" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A56" s="26"/>
+      <c r="A56" s="32"/>
       <c r="B56" t="s">
         <v>292</v>
       </c>
-      <c r="E56" s="26"/>
+      <c r="E56" s="32"/>
       <c r="F56" t="s">
         <v>311</v>
       </c>
-      <c r="I56" s="26"/>
+      <c r="I56" s="30" t="s">
+        <v>93</v>
+      </c>
       <c r="J56" t="s">
-        <v>57</v>
-      </c>
-      <c r="M56" s="26"/>
+        <v>353</v>
+      </c>
+      <c r="M56" s="32"/>
       <c r="N56" t="s">
         <v>307</v>
       </c>
-      <c r="Q56" s="26"/>
+      <c r="Q56" s="32"/>
       <c r="R56" t="s">
         <v>302</v>
       </c>
-      <c r="U56" s="26"/>
+      <c r="U56" s="32"/>
       <c r="V56" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A57" s="26"/>
+      <c r="A57" s="32"/>
       <c r="B57" t="s">
         <v>298</v>
       </c>
-      <c r="E57" s="26"/>
+      <c r="E57" s="32"/>
       <c r="F57" t="s">
         <v>317</v>
       </c>
-      <c r="I57" s="26"/>
+      <c r="I57" s="30"/>
       <c r="J57" t="s">
-        <v>282</v>
-      </c>
-      <c r="M57" s="26"/>
+        <v>318</v>
+      </c>
+      <c r="M57" s="32"/>
       <c r="N57" t="s">
         <v>313</v>
       </c>
-      <c r="Q57" s="26"/>
+      <c r="Q57" s="32"/>
       <c r="R57" t="s">
         <v>308</v>
       </c>
-      <c r="U57" s="26"/>
+      <c r="U57" s="32"/>
       <c r="V57" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A58" s="26"/>
+      <c r="A58" s="32"/>
       <c r="B58" t="s">
         <v>304</v>
       </c>
-      <c r="E58" s="26"/>
+      <c r="E58" s="32"/>
       <c r="F58" t="s">
         <v>323</v>
       </c>
-      <c r="I58" s="25" t="s">
-        <v>93</v>
-      </c>
+      <c r="I58" s="30"/>
       <c r="J58" t="s">
-        <v>353</v>
-      </c>
-      <c r="M58" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="M58" s="30" t="s">
         <v>93</v>
       </c>
       <c r="N58" t="s">
         <v>319</v>
       </c>
-      <c r="Q58" s="26"/>
+      <c r="Q58" s="32"/>
       <c r="R58" t="s">
         <v>314</v>
       </c>
-      <c r="U58" s="26"/>
+      <c r="U58" s="32"/>
       <c r="V58" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A59" s="26"/>
+      <c r="A59" s="32"/>
       <c r="B59" t="s">
         <v>310</v>
       </c>
-      <c r="E59" s="26"/>
+      <c r="E59" s="32"/>
       <c r="F59" t="s">
         <v>329</v>
       </c>
-      <c r="I59" s="25"/>
+      <c r="I59" s="30"/>
       <c r="J59" t="s">
-        <v>318</v>
-      </c>
-      <c r="M59" s="25"/>
+        <v>336</v>
+      </c>
+      <c r="M59" s="30"/>
       <c r="N59" t="s">
         <v>325</v>
       </c>
-      <c r="Q59" s="26"/>
+      <c r="Q59" s="32"/>
       <c r="R59" t="s">
         <v>320</v>
       </c>
-      <c r="U59" s="26"/>
+      <c r="U59" s="32"/>
       <c r="V59" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A60" s="26"/>
+      <c r="A60" s="32"/>
       <c r="B60" t="s">
         <v>316</v>
       </c>
-      <c r="E60" s="26"/>
+      <c r="E60" s="32"/>
       <c r="F60" t="s">
         <v>335</v>
       </c>
-      <c r="I60" s="25"/>
+      <c r="I60" s="30"/>
       <c r="J60" t="s">
-        <v>106</v>
-      </c>
-      <c r="M60" s="25"/>
+        <v>324</v>
+      </c>
+      <c r="M60" s="30"/>
       <c r="N60" t="s">
         <v>331</v>
       </c>
-      <c r="Q60" s="26"/>
+      <c r="Q60" s="32"/>
       <c r="R60" t="s">
         <v>326</v>
       </c>
-      <c r="U60" s="25" t="s">
+      <c r="U60" s="30" t="s">
         <v>93</v>
       </c>
       <c r="V60" t="s">
@@ -4196,57 +4244,59 @@
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A61" s="26"/>
+      <c r="A61" s="32"/>
       <c r="B61" t="s">
         <v>322</v>
       </c>
-      <c r="E61" s="26"/>
+      <c r="E61" s="32"/>
       <c r="F61" t="s">
         <v>299</v>
       </c>
-      <c r="I61" s="25"/>
+      <c r="I61" s="28" t="s">
+        <v>113</v>
+      </c>
       <c r="J61" t="s">
-        <v>336</v>
-      </c>
-      <c r="M61" s="25"/>
+        <v>342</v>
+      </c>
+      <c r="M61" s="30"/>
       <c r="N61" t="s">
         <v>128</v>
       </c>
-      <c r="Q61" s="26"/>
+      <c r="Q61" s="32"/>
       <c r="R61" t="s">
         <v>332</v>
       </c>
-      <c r="U61" s="25"/>
+      <c r="U61" s="30"/>
       <c r="V61" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A62" s="26"/>
+      <c r="A62" s="32"/>
       <c r="B62" t="s">
         <v>305</v>
       </c>
-      <c r="E62" s="25" t="s">
+      <c r="E62" s="30" t="s">
         <v>93</v>
       </c>
       <c r="F62" t="s">
         <v>341</v>
       </c>
-      <c r="I62" s="25"/>
+      <c r="I62" s="28"/>
       <c r="J62" t="s">
-        <v>324</v>
-      </c>
-      <c r="M62" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="M62" s="28" t="s">
         <v>113</v>
       </c>
       <c r="N62" t="s">
         <v>337</v>
       </c>
-      <c r="Q62" s="26"/>
+      <c r="Q62" s="32"/>
       <c r="R62" t="s">
         <v>338</v>
       </c>
-      <c r="U62" s="32" t="s">
+      <c r="U62" s="28" t="s">
         <v>113</v>
       </c>
       <c r="V62" t="s">
@@ -4254,89 +4304,89 @@
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A63" s="25" t="s">
+      <c r="A63" s="30" t="s">
         <v>93</v>
       </c>
       <c r="B63" t="s">
         <v>328</v>
       </c>
-      <c r="E63" s="25"/>
+      <c r="E63" s="30"/>
       <c r="F63" t="s">
         <v>347</v>
       </c>
-      <c r="I63" s="32" t="s">
-        <v>113</v>
-      </c>
+      <c r="I63" s="28"/>
       <c r="J63" t="s">
-        <v>342</v>
-      </c>
-      <c r="M63" s="32"/>
+        <v>354</v>
+      </c>
+      <c r="M63" s="28"/>
       <c r="N63" t="s">
         <v>343</v>
       </c>
-      <c r="Q63" s="26"/>
+      <c r="Q63" s="32"/>
       <c r="R63" t="s">
         <v>344</v>
       </c>
-      <c r="U63" s="32"/>
+      <c r="U63" s="28"/>
       <c r="V63" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A64" s="25"/>
+      <c r="A64" s="30"/>
       <c r="B64" t="s">
         <v>334</v>
       </c>
-      <c r="E64" s="25"/>
+      <c r="E64" s="30"/>
       <c r="F64" t="s">
         <v>359</v>
       </c>
-      <c r="I64" s="32"/>
+      <c r="I64" s="28"/>
       <c r="J64" t="s">
-        <v>348</v>
-      </c>
-      <c r="M64" s="32"/>
+        <v>360</v>
+      </c>
+      <c r="M64" s="28"/>
       <c r="N64" t="s">
         <v>349</v>
       </c>
-      <c r="Q64" s="25" t="s">
+      <c r="Q64" s="30" t="s">
         <v>93</v>
       </c>
       <c r="R64" t="s">
         <v>350</v>
       </c>
-      <c r="U64" s="32"/>
+      <c r="U64" s="28"/>
       <c r="V64" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A65" s="25"/>
+      <c r="A65" s="30"/>
       <c r="B65" t="s">
         <v>340</v>
       </c>
-      <c r="E65" s="32" t="s">
+      <c r="E65" s="28" t="s">
         <v>113</v>
       </c>
       <c r="F65" t="s">
         <v>365</v>
       </c>
-      <c r="I65" s="32"/>
+      <c r="I65" s="26" t="s">
+        <v>137</v>
+      </c>
       <c r="J65" t="s">
-        <v>354</v>
-      </c>
-      <c r="M65" s="29" t="s">
+        <v>372</v>
+      </c>
+      <c r="M65" s="26" t="s">
         <v>137</v>
       </c>
       <c r="N65" t="s">
         <v>355</v>
       </c>
-      <c r="Q65" s="25"/>
+      <c r="Q65" s="30"/>
       <c r="R65" t="s">
         <v>356</v>
       </c>
-      <c r="U65" s="29" t="s">
+      <c r="U65" s="26" t="s">
         <v>137</v>
       </c>
       <c r="V65" t="s">
@@ -4344,141 +4394,139 @@
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A66" s="25"/>
+      <c r="A66" s="30"/>
       <c r="B66" t="s">
         <v>346</v>
       </c>
-      <c r="E66" s="32"/>
+      <c r="E66" s="28"/>
       <c r="F66" t="s">
         <v>371</v>
       </c>
-      <c r="I66" s="32"/>
+      <c r="I66" s="26"/>
       <c r="J66" t="s">
-        <v>360</v>
-      </c>
-      <c r="M66" s="29"/>
+        <v>384</v>
+      </c>
+      <c r="M66" s="26"/>
       <c r="N66" t="s">
         <v>361</v>
       </c>
-      <c r="Q66" s="32" t="s">
+      <c r="Q66" s="28" t="s">
         <v>113</v>
       </c>
       <c r="R66" t="s">
         <v>362</v>
       </c>
-      <c r="U66" s="29"/>
+      <c r="U66" s="26"/>
       <c r="V66" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A67" s="25"/>
+      <c r="A67" s="30"/>
       <c r="B67" t="s">
         <v>330</v>
       </c>
-      <c r="E67" s="32"/>
+      <c r="E67" s="28"/>
       <c r="F67" t="s">
         <v>377</v>
       </c>
-      <c r="I67" s="29" t="s">
-        <v>137</v>
-      </c>
+      <c r="I67" s="26"/>
       <c r="J67" t="s">
-        <v>372</v>
-      </c>
-      <c r="M67" s="29"/>
+        <v>162</v>
+      </c>
+      <c r="M67" s="26"/>
       <c r="N67" t="s">
         <v>156</v>
       </c>
-      <c r="Q67" s="32"/>
+      <c r="Q67" s="28"/>
       <c r="R67" t="s">
         <v>368</v>
       </c>
-      <c r="U67" s="29"/>
+      <c r="U67" s="26"/>
       <c r="V67" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A68" s="32" t="s">
+      <c r="A68" s="28" t="s">
         <v>113</v>
       </c>
       <c r="B68" t="s">
         <v>352</v>
       </c>
-      <c r="E68" s="32"/>
+      <c r="E68" s="28"/>
       <c r="F68" t="s">
         <v>125</v>
       </c>
-      <c r="I68" s="29"/>
+      <c r="I68" s="26"/>
       <c r="J68" t="s">
-        <v>384</v>
-      </c>
-      <c r="M68" s="29"/>
+        <v>407</v>
+      </c>
+      <c r="M68" s="26"/>
       <c r="N68" t="s">
         <v>373</v>
       </c>
-      <c r="Q68" s="32"/>
+      <c r="Q68" s="28"/>
       <c r="R68" t="s">
         <v>374</v>
       </c>
-      <c r="U68" s="29"/>
+      <c r="U68" s="26"/>
       <c r="V68" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A69" s="32"/>
+      <c r="A69" s="28"/>
       <c r="B69" t="s">
         <v>358</v>
       </c>
-      <c r="E69" s="29" t="s">
+      <c r="E69" s="26" t="s">
         <v>137</v>
       </c>
       <c r="F69" t="s">
         <v>383</v>
       </c>
-      <c r="I69" s="29"/>
+      <c r="I69" s="26"/>
       <c r="J69" t="s">
-        <v>162</v>
-      </c>
-      <c r="M69" s="29"/>
+        <v>366</v>
+      </c>
+      <c r="M69" s="26"/>
       <c r="N69" t="s">
         <v>379</v>
       </c>
-      <c r="Q69" s="32"/>
+      <c r="Q69" s="28"/>
       <c r="R69" t="s">
         <v>380</v>
       </c>
-      <c r="U69" s="29"/>
+      <c r="U69" s="26"/>
       <c r="V69" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A70" s="32"/>
+      <c r="A70" s="28"/>
       <c r="B70" t="s">
         <v>364</v>
       </c>
-      <c r="E70" s="29"/>
+      <c r="E70" s="26"/>
       <c r="F70" t="s">
         <v>389</v>
       </c>
-      <c r="I70" s="29"/>
+      <c r="I70" s="26"/>
       <c r="J70" t="s">
-        <v>407</v>
-      </c>
-      <c r="M70" s="29"/>
+        <v>378</v>
+      </c>
+      <c r="M70" s="26"/>
       <c r="N70" t="s">
         <v>367</v>
       </c>
-      <c r="Q70" s="29" t="s">
+      <c r="Q70" s="26" t="s">
         <v>137</v>
       </c>
       <c r="R70" t="s">
         <v>386</v>
       </c>
-      <c r="U70" s="30" t="s">
+      <c r="U70" s="29" t="s">
         <v>167</v>
       </c>
       <c r="V70" t="s">
@@ -4486,230 +4534,195 @@
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A71" s="29" t="s">
+      <c r="A71" s="26" t="s">
         <v>137</v>
       </c>
       <c r="B71" t="s">
         <v>370</v>
       </c>
-      <c r="E71" s="29"/>
+      <c r="E71" s="26"/>
       <c r="F71" t="s">
         <v>395</v>
       </c>
-      <c r="I71" s="29"/>
+      <c r="I71" s="29" t="s">
+        <v>167</v>
+      </c>
       <c r="J71" t="s">
-        <v>366</v>
-      </c>
-      <c r="M71" s="30" t="s">
+        <v>390</v>
+      </c>
+      <c r="M71" s="29" t="s">
         <v>167</v>
       </c>
       <c r="N71" t="s">
         <v>385</v>
       </c>
-      <c r="Q71" s="29"/>
+      <c r="Q71" s="26"/>
       <c r="R71" t="s">
         <v>392</v>
       </c>
-      <c r="U71" s="30"/>
+      <c r="U71" s="29"/>
       <c r="V71" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A72" s="29"/>
+      <c r="A72" s="26"/>
       <c r="B72" t="s">
         <v>376</v>
       </c>
-      <c r="E72" s="29"/>
+      <c r="E72" s="26"/>
       <c r="F72" t="s">
         <v>401</v>
       </c>
       <c r="I72" s="29"/>
       <c r="J72" t="s">
-        <v>378</v>
-      </c>
-      <c r="M72" s="30"/>
+        <v>402</v>
+      </c>
+      <c r="M72" s="29"/>
       <c r="N72" t="s">
         <v>391</v>
       </c>
-      <c r="Q72" s="29"/>
+      <c r="Q72" s="26"/>
       <c r="R72" t="s">
         <v>398</v>
       </c>
-      <c r="U72" s="30"/>
+      <c r="U72" s="29"/>
       <c r="V72" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A73" s="29"/>
+      <c r="A73" s="26"/>
       <c r="B73" t="s">
         <v>382</v>
       </c>
-      <c r="E73" s="30" t="s">
+      <c r="E73" s="29" t="s">
         <v>167</v>
       </c>
       <c r="F73" t="s">
         <v>406</v>
       </c>
-      <c r="I73" s="30" t="s">
-        <v>167</v>
-      </c>
+      <c r="I73" s="29"/>
       <c r="J73" t="s">
-        <v>390</v>
-      </c>
-      <c r="M73" s="30"/>
+        <v>411</v>
+      </c>
+      <c r="M73" s="29"/>
       <c r="N73" t="s">
         <v>397</v>
       </c>
-      <c r="Q73" s="29"/>
+      <c r="Q73" s="26"/>
       <c r="R73" t="s">
         <v>403</v>
       </c>
-      <c r="U73" s="30"/>
+      <c r="U73" s="29"/>
       <c r="V73" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A74" s="29"/>
+      <c r="A74" s="26"/>
       <c r="B74" t="s">
         <v>388</v>
       </c>
-      <c r="E74" s="30"/>
+      <c r="E74" s="29"/>
       <c r="F74" t="s">
         <v>410</v>
       </c>
-      <c r="I74" s="30"/>
+      <c r="I74" s="29"/>
       <c r="J74" t="s">
-        <v>402</v>
-      </c>
-      <c r="Q74" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q74" s="29" t="s">
         <v>167</v>
       </c>
       <c r="R74" t="s">
         <v>186</v>
       </c>
-      <c r="U74" s="30"/>
+      <c r="U74" s="29"/>
       <c r="V74" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A75" s="30" t="s">
+      <c r="A75" s="29" t="s">
         <v>167</v>
       </c>
       <c r="B75" t="s">
         <v>394</v>
       </c>
-      <c r="E75" s="30"/>
+      <c r="E75" s="29"/>
       <c r="F75" t="s">
         <v>413</v>
       </c>
-      <c r="I75" s="30"/>
+      <c r="I75" s="29"/>
       <c r="J75" t="s">
-        <v>411</v>
-      </c>
-      <c r="Q75" s="30"/>
+        <v>396</v>
+      </c>
+      <c r="Q75" s="29"/>
       <c r="R75" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A76" s="30"/>
+      <c r="A76" s="29"/>
       <c r="B76" t="s">
         <v>400</v>
       </c>
-      <c r="I76" s="30"/>
-      <c r="J76" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q76" s="30"/>
+      <c r="Q76" s="29"/>
       <c r="R76" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A77" s="30"/>
+      <c r="A77" s="29"/>
       <c r="B77" t="s">
         <v>405</v>
       </c>
-      <c r="I77" s="30"/>
-      <c r="J77" t="s">
-        <v>396</v>
-      </c>
-      <c r="Q77" s="30"/>
+      <c r="Q77" s="29"/>
       <c r="R77" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A78" s="30"/>
+      <c r="A78" s="29"/>
       <c r="B78" t="s">
         <v>409</v>
       </c>
-      <c r="Q78" s="30"/>
+      <c r="Q78" s="29"/>
       <c r="R78" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q79" s="30"/>
+      <c r="Q79" s="29"/>
       <c r="R79" t="s">
         <v>412</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="E41:E44"/>
-    <mergeCell ref="E21:E24"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="M65:M70"/>
-    <mergeCell ref="E65:E68"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="M41:M43"/>
-    <mergeCell ref="A75:A78"/>
-    <mergeCell ref="E62:E64"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="Q74:Q79"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="U40:V40"/>
-    <mergeCell ref="U44:U49"/>
-    <mergeCell ref="U60:U61"/>
-    <mergeCell ref="U50:U59"/>
-    <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="Q43:Q50"/>
-    <mergeCell ref="M44:M50"/>
-    <mergeCell ref="M51:M57"/>
-    <mergeCell ref="M58:M61"/>
-    <mergeCell ref="M30:M33"/>
-    <mergeCell ref="I4:I11"/>
-    <mergeCell ref="M5:M11"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="A71:A74"/>
-    <mergeCell ref="I29:I33"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="A44:A51"/>
-    <mergeCell ref="A52:A62"/>
-    <mergeCell ref="I42:I50"/>
-    <mergeCell ref="E45:E49"/>
-    <mergeCell ref="E50:E61"/>
-    <mergeCell ref="A63:A67"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="U70:U74"/>
-    <mergeCell ref="E69:E72"/>
-    <mergeCell ref="M71:M73"/>
-    <mergeCell ref="Q70:Q73"/>
-    <mergeCell ref="M62:M64"/>
-    <mergeCell ref="I63:I66"/>
-    <mergeCell ref="I73:I77"/>
-    <mergeCell ref="E73:E75"/>
-    <mergeCell ref="I67:I72"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="U2:U4"/>
+    <mergeCell ref="M13:M21"/>
+    <mergeCell ref="M5:M12"/>
+    <mergeCell ref="Q5:Q11"/>
+    <mergeCell ref="Q30:Q34"/>
+    <mergeCell ref="I12:I19"/>
+    <mergeCell ref="I21:I24"/>
+    <mergeCell ref="M25:M27"/>
+    <mergeCell ref="I25:I28"/>
+    <mergeCell ref="M28:M31"/>
+    <mergeCell ref="M22:M24"/>
     <mergeCell ref="U29:U33"/>
     <mergeCell ref="Q51:Q63"/>
     <mergeCell ref="U5:U10"/>
@@ -4726,35 +4739,62 @@
     <mergeCell ref="U25:U28"/>
     <mergeCell ref="Q26:Q29"/>
     <mergeCell ref="U41:U43"/>
+    <mergeCell ref="M32:M35"/>
+    <mergeCell ref="I4:I11"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="I29:I33"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="A44:A51"/>
+    <mergeCell ref="A52:A62"/>
+    <mergeCell ref="E45:E49"/>
+    <mergeCell ref="E50:E61"/>
+    <mergeCell ref="A63:A67"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="E69:E72"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="Q74:Q79"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="U40:V40"/>
+    <mergeCell ref="U44:U49"/>
+    <mergeCell ref="U60:U61"/>
+    <mergeCell ref="U50:U59"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="Q43:Q50"/>
+    <mergeCell ref="M44:M50"/>
+    <mergeCell ref="M51:M57"/>
+    <mergeCell ref="M58:M61"/>
+    <mergeCell ref="U70:U74"/>
+    <mergeCell ref="M71:M73"/>
+    <mergeCell ref="Q70:Q73"/>
+    <mergeCell ref="M62:M64"/>
+    <mergeCell ref="M65:M70"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="M41:M43"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="E62:E64"/>
+    <mergeCell ref="I61:I64"/>
+    <mergeCell ref="I71:I75"/>
+    <mergeCell ref="E73:E75"/>
+    <mergeCell ref="I65:I70"/>
+    <mergeCell ref="I56:I60"/>
+    <mergeCell ref="I42:I49"/>
+    <mergeCell ref="I50:I55"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="E41:E44"/>
+    <mergeCell ref="E21:E24"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="E18:E20"/>
     <mergeCell ref="E25:E27"/>
     <mergeCell ref="E10:E15"/>
-    <mergeCell ref="Q5:Q11"/>
-    <mergeCell ref="Q30:Q34"/>
-    <mergeCell ref="I12:I19"/>
-    <mergeCell ref="I21:I24"/>
-    <mergeCell ref="M23:M25"/>
-    <mergeCell ref="I25:I28"/>
-    <mergeCell ref="M26:M29"/>
     <mergeCell ref="E4:E9"/>
-    <mergeCell ref="M20:M22"/>
-    <mergeCell ref="M12:M19"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A8:A15"/>
-    <mergeCell ref="I51:I57"/>
-    <mergeCell ref="I58:I62"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="U2:U4"/>
+    <mergeCell ref="A26:A29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4763,10 +4803,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S28"/>
+  <dimension ref="A1:S78"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4788,34 +4828,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="E1" s="27" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="E1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="27"/>
+      <c r="F1" s="31"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="27"/>
-      <c r="O1" s="27" t="s">
+      <c r="M1" s="31"/>
+      <c r="O1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="27"/>
-      <c r="R1" s="27" t="s">
+      <c r="P1" s="31"/>
+      <c r="R1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="27"/>
+      <c r="S1" s="31"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4837,7 +4877,7 @@
         <v>420</v>
       </c>
       <c r="L2" t="s">
-        <v>617</v>
+        <v>442</v>
       </c>
       <c r="M2" t="s">
         <v>421</v>
@@ -4875,7 +4915,7 @@
         <v>430</v>
       </c>
       <c r="L3" t="s">
-        <v>431</v>
+        <v>463</v>
       </c>
       <c r="M3" t="s">
         <v>432</v>
@@ -4909,9 +4949,6 @@
       <c r="I4" t="s">
         <v>441</v>
       </c>
-      <c r="L4" t="s">
-        <v>442</v>
-      </c>
       <c r="M4" t="s">
         <v>443</v>
       </c>
@@ -4944,11 +4981,8 @@
       <c r="I5" t="s">
         <v>452</v>
       </c>
-      <c r="L5" t="s">
-        <v>453</v>
-      </c>
       <c r="M5" t="s">
-        <v>454</v>
+        <v>477</v>
       </c>
       <c r="O5" t="s">
         <v>455</v>
@@ -4976,11 +5010,8 @@
       <c r="I6" t="s">
         <v>462</v>
       </c>
-      <c r="L6" t="s">
-        <v>463</v>
-      </c>
       <c r="M6" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="O6" t="s">
         <v>465</v>
@@ -5005,6 +5036,9 @@
       <c r="H7" t="s">
         <v>471</v>
       </c>
+      <c r="M7" t="s">
+        <v>510</v>
+      </c>
       <c r="R7" t="s">
         <v>472</v>
       </c>
@@ -5016,6 +5050,9 @@
       <c r="F8" t="s">
         <v>483</v>
       </c>
+      <c r="M8" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
@@ -5024,6 +5061,9 @@
       <c r="F9" t="s">
         <v>476</v>
       </c>
+      <c r="M9" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
@@ -5034,40 +5074,37 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="E17" s="27" t="s">
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="E17" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="I17" s="27" t="s">
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="I17" s="31" t="s">
         <v>605</v>
       </c>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27" t="s">
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="M17" s="27"/>
-      <c r="O17" s="27" t="s">
+      <c r="M17" s="31"/>
+      <c r="O17" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="P17" s="27"/>
-      <c r="R17" s="27" t="s">
+      <c r="P17" s="31"/>
+      <c r="R17" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="S17" s="27"/>
+      <c r="S17" s="31"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>448</v>
-      </c>
-      <c r="C18" t="s">
-        <v>491</v>
+        <v>509</v>
       </c>
       <c r="E18" t="s">
         <v>624</v>
@@ -5096,7 +5133,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>480</v>
+        <v>448</v>
       </c>
       <c r="C19" t="s">
         <v>514</v>
@@ -5124,6 +5161,9 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>480</v>
+      </c>
       <c r="E20" t="s">
         <v>492</v>
       </c>
@@ -5131,10 +5171,10 @@
         <v>474</v>
       </c>
       <c r="I20" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="J20" t="s">
-        <v>477</v>
+        <v>491</v>
       </c>
       <c r="O20" t="s">
         <v>504</v>
@@ -5157,10 +5197,10 @@
         <v>470</v>
       </c>
       <c r="I21" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="J21" t="s">
-        <v>478</v>
+        <v>517</v>
       </c>
       <c r="L21" t="s">
         <v>511</v>
@@ -5183,7 +5223,7 @@
         <v>500</v>
       </c>
       <c r="I22" t="s">
-        <v>509</v>
+        <v>431</v>
       </c>
       <c r="O22" t="s">
         <v>518</v>
@@ -5200,10 +5240,7 @@
         <v>508</v>
       </c>
       <c r="I23" t="s">
-        <v>516</v>
-      </c>
-      <c r="J23" t="s">
-        <v>510</v>
+        <v>626</v>
       </c>
       <c r="O23" t="s">
         <v>521</v>
@@ -5216,8 +5253,8 @@
       <c r="F24" t="s">
         <v>469</v>
       </c>
-      <c r="J24" t="s">
-        <v>517</v>
+      <c r="I24" t="s">
+        <v>453</v>
       </c>
       <c r="O24" t="s">
         <v>523</v>
@@ -5230,6 +5267,9 @@
       <c r="F25" t="s">
         <v>515</v>
       </c>
+      <c r="I25" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
@@ -5244,6 +5284,395 @@
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
         <v>526</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D31" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>1.2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>1.3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>1.4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>1.5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>1.6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>1.7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>1.8</v>
+      </c>
+      <c r="D38" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>1.9</v>
+      </c>
+      <c r="D39" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="33">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D40" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="D41" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="D42" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>2.1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D44" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D45" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>2.4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>2.5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>2.6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>2.7</v>
+      </c>
+      <c r="D49" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>2.8</v>
+      </c>
+      <c r="D50" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>2.9</v>
+      </c>
+      <c r="D51" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="33">
+        <v>2.1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>2.11</v>
+      </c>
+      <c r="D53" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>2.12</v>
+      </c>
+      <c r="D54" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>3.1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>3.2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>3.3</v>
+      </c>
+      <c r="D57" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>3.4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>3.5</v>
+      </c>
+      <c r="D59" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>3.6</v>
+      </c>
+      <c r="D60" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>3.7</v>
+      </c>
+      <c r="D61" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>3.8</v>
+      </c>
+      <c r="D62" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>3.9</v>
+      </c>
+      <c r="D63" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C64" s="33">
+        <v>3.1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>3.11</v>
+      </c>
+      <c r="D65" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>3.12</v>
+      </c>
+      <c r="D66" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D67" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <v>4.2</v>
+      </c>
+      <c r="D68" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <v>4.3</v>
+      </c>
+      <c r="D69" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D70" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <v>4.5</v>
+      </c>
+      <c r="D71" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D72" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <v>4.7</v>
+      </c>
+      <c r="D73" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <v>4.8</v>
+      </c>
+      <c r="D74" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D75" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C76" s="33">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D76" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C77">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="D77" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <v>4.12</v>
+      </c>
+      <c r="D78" t="s">
+        <v>668</v>
       </c>
     </row>
   </sheetData>
@@ -5271,7 +5700,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5445,10 +5874,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B187"/>
+  <dimension ref="A1:B199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F189" sqref="F189"/>
+    <sheetView topLeftCell="A171" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E187" sqref="E187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6557,6 +6986,76 @@
         <v>582</v>
       </c>
     </row>
+    <row r="188" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="18" t="s">
+        <v>606</v>
+      </c>
+      <c r="B189" s="19" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="9"/>
+      <c r="B190" s="20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="9"/>
+      <c r="B191" s="20" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="9"/>
+      <c r="B192" s="20" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="9"/>
+      <c r="B193" s="20" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="B194" s="20" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="9"/>
+      <c r="B195" s="20" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="21"/>
+      <c r="B196" s="22" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="18" t="s">
+        <v>606</v>
+      </c>
+      <c r="B198" s="19" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="21" t="s">
+        <v>574</v>
+      </c>
+      <c r="B199" s="22" t="s">
+        <v>663</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
updated picks to correct
2.6 is for adamw
3.9 for adamw
</commit_message>
<xml_diff>
--- a/OffSeason.xlsx
+++ b/OffSeason.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="686">
   <si>
     <t xml:space="preserve">Vanja Dolas - CeeDee Nuts</t>
   </si>
@@ -1210,156 +1210,156 @@
     <t xml:space="preserve">Grady Jarrett</t>
   </si>
   <si>
+    <t xml:space="preserve">2021 2.6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demario davis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Julian Edelman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yannick Ngakoue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shaq Thompson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quinnen Williams</t>
+  </si>
+  <si>
     <t xml:space="preserve">2021 2.8 Andrew</t>
   </si>
   <si>
-    <t xml:space="preserve">Demario davis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Julian Edelman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yannick Ngakoue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shaq Thompson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quinnen Williams</t>
+    <t xml:space="preserve">Danny Trevathan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travis Fulgham</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tremaine Edmunds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 1.7 ZachJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leighton Vander Esch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeffery Simmons</t>
   </si>
   <si>
     <t xml:space="preserve">2021 2.9 BrandonH</t>
   </si>
   <si>
-    <t xml:space="preserve">Danny Trevathan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Travis Fulgham</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tremaine Edmunds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 1.7 ZachJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leighton Vander Esch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jeffery Simmons</t>
+    <t xml:space="preserve">Kyle Van Noy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blake Jarwin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haason Reddick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 1.9 BrandonH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 1.12 Vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jerome Baker</t>
   </si>
   <si>
     <t xml:space="preserve">2021 3.5 BenL</t>
   </si>
   <si>
-    <t xml:space="preserve">Kyle Van Noy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blake Jarwin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haason Reddick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 1.9 BrandonH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 1.12 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jerome Baker</t>
+    <t xml:space="preserve">Jamie Collins Sr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malcolm Butler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brandley Chubb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 2.4 PatrickP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zach Cunningham</t>
   </si>
   <si>
     <t xml:space="preserve">2021 4.3</t>
   </si>
   <si>
-    <t xml:space="preserve">Jamie Collins Sr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malcolm Butler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brandley Chubb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 2.4 PatrickP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zach Cunningham</t>
+    <t xml:space="preserve">2021 2.11 JohnO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mike Hilton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 4.4 PatrickP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 2.12 Vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dre Greenlaw</t>
   </si>
   <si>
     <t xml:space="preserve">2021 4.9 BrandonH</t>
   </si>
   <si>
-    <t xml:space="preserve">2021 2.11 JohnO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mike Hilton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 4.4 PatrickP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 2.12 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 2.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dre Greenlaw</t>
+    <t xml:space="preserve">2021 3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fletcher Cox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 4.6AlanP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 4.1 MikeW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 3.3</t>
   </si>
   <si>
     <t xml:space="preserve">2021 5.2 AdamW</t>
   </si>
   <si>
-    <t xml:space="preserve">2021 3.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fletcher Cox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 4.6AlanP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 4.1 MikeW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 2.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 3.3</t>
+    <t xml:space="preserve">2021 3.12 Vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adrian Peterson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 5.9 BrandonH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 4.2 AdamW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 3.11 JohnO</t>
   </si>
   <si>
     <t xml:space="preserve">2021 5.12 Vanja</t>
   </si>
   <si>
-    <t xml:space="preserve">2021 3.12 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adrian Peterson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 5.9 BrandonH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 4.2 AdamW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 3.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 3.11 JohnO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 6.2 AdamW</t>
-  </si>
-  <si>
     <t xml:space="preserve">2021 5.1 MikeW</t>
   </si>
   <si>
@@ -1576,13 +1576,19 @@
     <t xml:space="preserve">2022 5 MikeR</t>
   </si>
   <si>
+    <t xml:space="preserve">2021 2.6 AlanP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 2 Vanja</t>
+  </si>
+  <si>
     <t xml:space="preserve">2022 5 AlanP</t>
   </si>
   <si>
     <t xml:space="preserve">2022 2 Patrick</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 2 Vanja</t>
+    <t xml:space="preserve">2022 4 AdamW</t>
   </si>
   <si>
     <t xml:space="preserve">2022 2 AlanP</t>
@@ -1591,7 +1597,7 @@
     <t xml:space="preserve">2022 3 BenL</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 4 AdamW</t>
+    <t xml:space="preserve">2022 5 AdamW</t>
   </si>
   <si>
     <t xml:space="preserve">2022 4 MikeW</t>
@@ -1606,16 +1612,13 @@
     <t xml:space="preserve">2021 5 MikeR</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 5 AdamW</t>
-  </si>
-  <si>
     <t xml:space="preserve">2022 4 Vanja</t>
   </si>
   <si>
     <t xml:space="preserve">2022 4 BenL</t>
   </si>
   <si>
-    <t xml:space="preserve">2021 2.6 AlanP</t>
+    <t xml:space="preserve">2021 3.9 BrandonH</t>
   </si>
   <si>
     <t xml:space="preserve">2022 5 MikeW</t>
@@ -1624,18 +1627,15 @@
     <t xml:space="preserve">2022 4 AlanP</t>
   </si>
   <si>
+    <t xml:space="preserve">2022 4 JohnO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 5 BenL</t>
+  </si>
+  <si>
     <t xml:space="preserve">2021 5 AdamW</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 4 JohnO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 3.9 BrandonH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 5 BenL</t>
-  </si>
-  <si>
     <t xml:space="preserve">2021 4.11 JohnO</t>
   </si>
   <si>
@@ -1651,12 +1651,18 @@
     <t xml:space="preserve">John O</t>
   </si>
   <si>
+    <t xml:space="preserve">Starting round 27 pick 5</t>
+  </si>
+  <si>
     <t xml:space="preserve">BenL</t>
   </si>
   <si>
     <t xml:space="preserve">Andrew</t>
   </si>
   <si>
+    <t xml:space="preserve">Page 27 end</t>
+  </si>
+  <si>
     <t xml:space="preserve">MattH</t>
   </si>
   <si>
@@ -1666,10 +1672,13 @@
     <t xml:space="preserve">Vanja</t>
   </si>
   <si>
+    <t xml:space="preserve">AdamW</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zach</t>
   </si>
   <si>
-    <t xml:space="preserve">AdamW</t>
+    <t xml:space="preserve">Page 28 end</t>
   </si>
   <si>
     <t xml:space="preserve">Holland</t>
@@ -1684,6 +1693,9 @@
     <t xml:space="preserve">*Picks moved up</t>
   </si>
   <si>
+    <t xml:space="preserve">Page 29 end</t>
+  </si>
+  <si>
     <t xml:space="preserve">AlanP</t>
   </si>
   <si>
@@ -2063,6 +2075,12 @@
   </si>
   <si>
     <t xml:space="preserve">2022 3 Ben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 2.06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Darrell Henderson</t>
   </si>
 </sst>
 </file>
@@ -2289,7 +2307,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2366,7 +2384,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2423,6 +2441,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2506,8 +2528,8 @@
   </sheetPr>
   <dimension ref="A1:AA97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L28" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W70" activeCellId="0" sqref="W70"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T47" activeCellId="0" sqref="T47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5786,15 +5808,15 @@
   </sheetPr>
   <dimension ref="A1:S90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H60" activeCellId="0" sqref="H60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B51" activeCellId="0" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.85"/>
@@ -6106,7 +6128,10 @@
         <v>516</v>
       </c>
       <c r="O18" s="0" t="s">
-        <v>395</v>
+        <v>517</v>
+      </c>
+      <c r="P18" s="0" t="s">
+        <v>518</v>
       </c>
       <c r="R18" s="0" t="s">
         <v>424</v>
@@ -6117,31 +6142,31 @@
         <v>433</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>399</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>421</v>
       </c>
-      <c r="J19" s="0" t="s">
-        <v>519</v>
-      </c>
       <c r="L19" s="0" t="s">
         <v>443</v>
       </c>
       <c r="O19" s="0" t="s">
         <v>402</v>
       </c>
+      <c r="P19" s="0" t="s">
+        <v>521</v>
+      </c>
       <c r="R19" s="0" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>440</v>
       </c>
@@ -6149,96 +6174,87 @@
         <v>406</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="I20" s="0" t="s">
         <v>428</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="O20" s="0" t="s">
         <v>409</v>
       </c>
       <c r="P20" s="0" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="R20" s="0" t="s">
         <v>438</v>
       </c>
       <c r="S20" s="0" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="0" t="s">
         <v>413</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="I21" s="0" t="s">
         <v>435</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="L21" s="15" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="O21" s="0" t="s">
         <v>416</v>
       </c>
-      <c r="P21" s="0" t="s">
-        <v>527</v>
-      </c>
       <c r="S21" s="0" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="0" t="s">
         <v>420</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>530</v>
+        <v>442</v>
       </c>
       <c r="O22" s="0" t="s">
-        <v>423</v>
+        <v>531</v>
       </c>
       <c r="S22" s="0" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="0" t="s">
         <v>427</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>532</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>442</v>
+        <v>533</v>
       </c>
       <c r="O23" s="0" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="0" t="s">
         <v>434</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>534</v>
       </c>
-      <c r="I24" s="0" t="s">
-        <v>535</v>
-      </c>
       <c r="O24" s="0" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6246,6 +6262,9 @@
         <v>441</v>
       </c>
       <c r="F25" s="0" t="s">
+        <v>535</v>
+      </c>
+      <c r="O25" s="0" t="s">
         <v>536</v>
       </c>
     </row>
@@ -6253,6 +6272,9 @@
       <c r="E26" s="15" t="s">
         <v>537</v>
       </c>
+      <c r="O26" s="0" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="15" t="s">
@@ -6276,13 +6298,16 @@
       <c r="D31" s="0" t="s">
         <v>541</v>
       </c>
+      <c r="E31" s="0" t="s">
+        <v>542</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="n">
         <v>1.2</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6290,7 +6315,7 @@
         <v>1.3</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6322,7 +6347,7 @@
         <v>1.7</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6330,7 +6355,10 @@
         <v>1.8</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>543</v>
+        <v>544</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6338,7 +6366,7 @@
         <v>1.9</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6346,7 +6374,7 @@
         <v>1.1</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6354,7 +6382,7 @@
         <v>1.11</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6362,7 +6390,7 @@
         <v>1.12</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6370,7 +6398,7 @@
         <v>2.1</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6378,7 +6406,7 @@
         <v>2.2</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6386,7 +6414,7 @@
         <v>2.3</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6394,7 +6422,7 @@
         <v>2.4</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6402,15 +6430,15 @@
         <v>2.5</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="n">
         <v>2.6</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6418,7 +6446,7 @@
         <v>2.7</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6426,7 +6454,10 @@
         <v>2.8</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>548</v>
+        <v>549</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6434,7 +6465,7 @@
         <v>2.9</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6442,7 +6473,7 @@
         <v>2.1</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6450,7 +6481,7 @@
         <v>2.11</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6458,7 +6489,7 @@
         <v>2.12</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6466,7 +6497,7 @@
         <v>3.1</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6474,7 +6505,7 @@
         <v>3.2</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6482,7 +6513,7 @@
         <v>3.3</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6490,7 +6521,7 @@
         <v>3.4</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6498,7 +6529,7 @@
         <v>3.5</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6506,10 +6537,10 @@
         <v>3.6</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>548</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>552</v>
+        <v>549</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6517,10 +6548,10 @@
         <v>3.7</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>544</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>552</v>
+        <v>546</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6528,10 +6559,13 @@
         <v>3.8</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>552</v>
+        <v>556</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6539,10 +6573,13 @@
         <v>3.9</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>550</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>552</v>
+        <v>549</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6550,10 +6587,13 @@
         <v>3.1</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>542</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>552</v>
+        <v>543</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6561,10 +6601,13 @@
         <v>3.11</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>542</v>
-      </c>
-      <c r="E65" s="0" t="s">
-        <v>552</v>
+        <v>543</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6572,10 +6615,13 @@
         <v>3.12</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>548</v>
-      </c>
-      <c r="E66" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6583,10 +6629,13 @@
         <v>4.1</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>553</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>552</v>
+        <v>557</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6594,10 +6643,13 @@
         <v>4.2</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>547</v>
-      </c>
-      <c r="E68" s="0" t="s">
-        <v>552</v>
+        <v>550</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6605,10 +6657,13 @@
         <v>4.3</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>553</v>
-      </c>
-      <c r="E69" s="0" t="s">
-        <v>552</v>
+        <v>557</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6616,10 +6671,13 @@
         <v>4.4</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>547</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>552</v>
+        <v>550</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6627,10 +6685,13 @@
         <v>4.5</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>548</v>
-      </c>
-      <c r="E71" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6638,70 +6699,52 @@
         <v>4.6</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>550</v>
-      </c>
-      <c r="E72" s="0" t="s">
-        <v>552</v>
-      </c>
-      <c r="F72" s="19" t="s">
-        <v>445</v>
-      </c>
+        <v>549</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>555</v>
+      </c>
+      <c r="G72" s="19"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="0" t="n">
         <v>4.7</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>548</v>
-      </c>
-      <c r="E73" s="0" t="s">
-        <v>552</v>
-      </c>
-      <c r="F73" s="19" t="s">
-        <v>430</v>
-      </c>
+        <v>557</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>555</v>
+      </c>
+      <c r="G73" s="19"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="0" t="n">
         <v>4.8</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>553</v>
-      </c>
-      <c r="E74" s="0" t="s">
-        <v>552</v>
-      </c>
-      <c r="F74" s="19" t="n">
-        <v>5.9</v>
-      </c>
+        <v>549</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>555</v>
+      </c>
+      <c r="G74" s="19"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C75" s="0" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>548</v>
-      </c>
-      <c r="E75" s="0" t="s">
-        <v>552</v>
-      </c>
-      <c r="F75" s="19" t="s">
-        <v>437</v>
-      </c>
+      <c r="G75" s="19"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C76" s="18" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="D76" s="0" t="s">
-        <v>548</v>
-      </c>
-      <c r="E76" s="0" t="s">
-        <v>552</v>
-      </c>
-      <c r="F76" s="19" t="s">
-        <v>444</v>
-      </c>
+      <c r="C76" s="18"/>
+      <c r="G76" s="19"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6714,7 +6757,7 @@
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F86" s="0" t="s">
-        <v>554</v>
+        <v>558</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6767,143 +6810,143 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>583</v>
+        <v>587</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>584</v>
+        <v>588</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>586</v>
+        <v>590</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>587</v>
+        <v>591</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>
@@ -6936,10 +6979,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B199"/>
+  <dimension ref="A1:B205"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A171" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E187" activeCellId="0" sqref="E187"/>
+      <selection pane="topLeft" activeCell="D190" activeCellId="0" sqref="D190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6950,23 +6993,23 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>326</v>
@@ -6981,12 +7024,12 @@
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="26"/>
       <c r="B6" s="27" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="24" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>477</v>
@@ -6994,7 +7037,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>314</v>
@@ -7002,21 +7045,21 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="26" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="24"/>
       <c r="B11" s="25" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B13" s="23" t="s">
         <v>244</v>
@@ -7025,27 +7068,27 @@
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="26"/>
       <c r="B14" s="27" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="26"/>
       <c r="B15" s="27" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="26" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="26"/>
       <c r="B17" s="27" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7056,7 +7099,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
       <c r="B20" s="23" t="s">
         <v>38</v>
@@ -7077,13 +7120,13 @@
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="26"/>
       <c r="B23" s="27" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="26"/>
       <c r="B24" s="27" t="s">
-        <v>606</v>
+        <v>610</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7092,7 +7135,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="26" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="B26" s="27" t="s">
         <v>37</v>
@@ -7125,18 +7168,18 @@
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="26"/>
       <c r="B31" s="27" t="s">
-        <v>607</v>
+        <v>611</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="24"/>
       <c r="B32" s="25" t="s">
-        <v>608</v>
+        <v>612</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="22" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B34" s="23" t="s">
         <v>276</v>
@@ -7145,7 +7188,7 @@
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="26"/>
       <c r="B35" s="27" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7156,51 +7199,51 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="24" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="22" t="s">
-        <v>611</v>
+        <v>615</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="24" t="s">
-        <v>613</v>
+        <v>617</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="22" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>615</v>
+        <v>619</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="26"/>
       <c r="B43" s="27" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="26"/>
       <c r="B44" s="27" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="26" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="B45" s="27" t="s">
         <v>493</v>
@@ -7214,21 +7257,21 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="26"/>
       <c r="B49" s="27" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="24" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B50" s="25" t="s">
         <v>226</v>
@@ -7236,7 +7279,7 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="22" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="B52" s="23" t="s">
         <v>284</v>
@@ -7250,21 +7293,21 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="26" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="B54" s="27" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="24"/>
       <c r="B55" s="25" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="22" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="B57" s="23" t="s">
         <v>478</v>
@@ -7284,7 +7327,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="26" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="B60" s="27" t="s">
         <v>296</v>
@@ -7293,29 +7336,29 @@
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="24"/>
       <c r="B61" s="25" t="s">
-        <v>622</v>
+        <v>626</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="28" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="B63" s="29" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="30"/>
       <c r="B64" s="31" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="30" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B65" s="31" t="s">
-        <v>625</v>
+        <v>629</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7327,30 +7370,30 @@
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="22" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
       <c r="B68" s="23" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="26"/>
       <c r="B69" s="27" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="24" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="B70" s="25" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="22" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
       <c r="B72" s="23" t="s">
         <v>461</v>
@@ -7358,24 +7401,24 @@
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="24" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="B73" s="25" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="22" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
       <c r="B75" s="23" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="24" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="B76" s="25" t="s">
         <v>492</v>
@@ -7384,15 +7427,15 @@
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="22" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="B78" s="23" t="s">
-        <v>632</v>
+        <v>636</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="24" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="B79" s="25" t="s">
         <v>506</v>
@@ -7401,7 +7444,7 @@
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="22" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="B81" s="23" t="s">
         <v>44</v>
@@ -7410,7 +7453,7 @@
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="26"/>
       <c r="B82" s="27" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7421,7 +7464,7 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="26" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B84" s="27" t="s">
         <v>493</v>
@@ -7436,13 +7479,13 @@
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="24"/>
       <c r="B86" s="25" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="22" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="B88" s="23" t="s">
         <v>281</v>
@@ -7451,7 +7494,7 @@
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="26"/>
       <c r="B89" s="27" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7462,22 +7505,22 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="26" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="B91" s="27" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="24"/>
       <c r="B92" s="25" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="22" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B94" s="23" t="s">
         <v>287</v>
@@ -7497,7 +7540,7 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="26" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="B97" s="27" t="s">
         <v>66</v>
@@ -7512,7 +7555,7 @@
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="22" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B100" s="23" t="s">
         <v>59</v>
@@ -7521,18 +7564,18 @@
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="26"/>
       <c r="B101" s="27" t="s">
-        <v>637</v>
+        <v>641</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="26"/>
       <c r="B102" s="27" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="26" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="B103" s="27" t="s">
         <v>102</v>
@@ -7541,16 +7584,16 @@
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="24"/>
       <c r="B104" s="25" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="22" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="B106" s="23" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7562,18 +7605,18 @@
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="26"/>
       <c r="B108" s="27" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="26"/>
       <c r="B109" s="27" t="s">
-        <v>641</v>
+        <v>645</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="26" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="B110" s="27" t="s">
         <v>294</v>
@@ -7582,42 +7625,42 @@
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="24"/>
       <c r="B111" s="25" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="22" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="B113" s="23" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="26" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="B114" s="27" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="26"/>
       <c r="B115" s="27" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="24"/>
       <c r="B116" s="25" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="22" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c r="B118" s="23" t="s">
         <v>359</v>
@@ -7625,7 +7668,7 @@
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="24" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="B119" s="25" t="s">
         <v>126</v>
@@ -7634,18 +7677,18 @@
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="22" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
       <c r="B121" s="23" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="26" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="B122" s="27" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7657,26 +7700,26 @@
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="26"/>
       <c r="B124" s="27" t="s">
-        <v>648</v>
+        <v>652</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="24"/>
       <c r="B125" s="25" t="s">
-        <v>649</v>
+        <v>653</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="0" t="s">
-        <v>650</v>
+        <v>654</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="22" t="s">
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="B128" s="23" t="s">
-        <v>652</v>
+        <v>656</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7700,12 +7743,12 @@
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="26"/>
       <c r="B132" s="27" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="26" t="s">
-        <v>653</v>
+        <v>657</v>
       </c>
       <c r="B133" s="27" t="s">
         <v>102</v>
@@ -7714,21 +7757,21 @@
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="26"/>
       <c r="B134" s="27" t="s">
-        <v>654</v>
+        <v>658</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="26"/>
       <c r="B135" s="27" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="26" t="s">
-        <v>655</v>
+        <v>659</v>
       </c>
       <c r="B136" s="27" t="s">
-        <v>652</v>
+        <v>656</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7746,27 +7789,27 @@
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="26"/>
       <c r="B139" s="27" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="26"/>
       <c r="B140" s="27" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="26"/>
       <c r="B141" s="27" t="s">
-        <v>656</v>
+        <v>660</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="26" t="s">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="B142" s="27" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7790,12 +7833,12 @@
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="26"/>
       <c r="B146" s="27" t="s">
-        <v>658</v>
+        <v>662</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="26" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
       <c r="B147" s="27" t="s">
         <v>102</v>
@@ -7804,7 +7847,7 @@
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="26"/>
       <c r="B148" s="27" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7816,21 +7859,21 @@
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="26"/>
       <c r="B150" s="27" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="26"/>
       <c r="B151" s="27" t="s">
-        <v>656</v>
+        <v>660</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="26" t="s">
-        <v>660</v>
+        <v>664</v>
       </c>
       <c r="B152" s="27" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7848,7 +7891,7 @@
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="26"/>
       <c r="B155" s="27" t="s">
-        <v>662</v>
+        <v>666</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7866,48 +7909,48 @@
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="22" t="s">
-        <v>663</v>
+        <v>667</v>
       </c>
       <c r="B159" s="23" t="s">
-        <v>664</v>
+        <v>668</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="26" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
       <c r="B160" s="27" t="s">
-        <v>666</v>
+        <v>670</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="26" t="s">
-        <v>667</v>
+        <v>671</v>
       </c>
       <c r="B161" s="27" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="26"/>
       <c r="B162" s="27" t="s">
-        <v>666</v>
+        <v>670</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="26" t="s">
-        <v>653</v>
+        <v>657</v>
       </c>
       <c r="B163" s="27" t="s">
-        <v>664</v>
+        <v>668</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="26" t="s">
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="B164" s="27" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7924,7 +7967,7 @@
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="26" t="s">
-        <v>655</v>
+        <v>659</v>
       </c>
       <c r="B167" s="27" t="s">
         <v>484</v>
@@ -7938,30 +7981,30 @@
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="24" t="s">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="B169" s="25" t="s">
-        <v>666</v>
+        <v>670</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="22" t="s">
-        <v>668</v>
+        <v>672</v>
       </c>
       <c r="B171" s="23" t="s">
-        <v>648</v>
+        <v>652</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="26"/>
       <c r="B172" s="27" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="26" t="s">
-        <v>669</v>
+        <v>673</v>
       </c>
       <c r="B173" s="27" t="s">
         <v>349</v>
@@ -7976,7 +8019,7 @@
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="22" t="s">
-        <v>670</v>
+        <v>674</v>
       </c>
       <c r="B176" s="23" t="s">
         <v>506</v>
@@ -7984,16 +8027,16 @@
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="24" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
       <c r="B177" s="25" t="s">
-        <v>671</v>
+        <v>675</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="22" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
       <c r="B179" s="23" t="s">
         <v>133</v>
@@ -8007,25 +8050,25 @@
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="26" t="s">
-        <v>672</v>
+        <v>676</v>
       </c>
       <c r="B181" s="27" t="s">
-        <v>648</v>
+        <v>652</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="24"/>
       <c r="B182" s="25" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="22" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
       <c r="B184" s="23" t="s">
-        <v>648</v>
+        <v>652</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8037,21 +8080,21 @@
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="26"/>
       <c r="B186" s="27" t="s">
-        <v>673</v>
+        <v>677</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="24" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="B187" s="25" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="22" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="B189" s="23" t="s">
         <v>133</v>
@@ -8072,7 +8115,7 @@
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="26"/>
       <c r="B192" s="27" t="s">
-        <v>675</v>
+        <v>679</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8083,7 +8126,7 @@
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="26" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c r="B194" s="27" t="s">
         <v>428</v>
@@ -8092,30 +8135,64 @@
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="26"/>
       <c r="B195" s="27" t="s">
-        <v>676</v>
+        <v>680</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="24"/>
       <c r="B196" s="25" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="22" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="B198" s="23" t="s">
-        <v>678</v>
+        <v>682</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="24" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
       <c r="B199" s="25" t="s">
-        <v>679</v>
+        <v>683</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="28" t="s">
+        <v>547</v>
+      </c>
+      <c r="B201" s="29" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="30"/>
+      <c r="B202" s="31" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="30"/>
+      <c r="B203" s="31" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="30"/>
+      <c r="B204" s="31" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="34" t="s">
+        <v>549</v>
+      </c>
+      <c r="B205" s="33" t="s">
+        <v>685</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
picks entered. emails updated
</commit_message>
<xml_diff>
--- a/OffSeason.xlsx
+++ b/OffSeason.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="732">
   <si>
     <t xml:space="preserve">Kupp My Footballs – Vanja Dolas </t>
   </si>
@@ -1324,139 +1324,139 @@
     <t xml:space="preserve">Brandon Hurd - Snow Happens</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 1 JohnO</t>
+    <t xml:space="preserve">2022 1.11</t>
   </si>
   <si>
     <t xml:space="preserve">2023 3 Adam</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 1 MikeR</t>
+    <t xml:space="preserve">2022 1.1 </t>
   </si>
   <si>
     <t xml:space="preserve">2023 1 Jared</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 1 AlanP</t>
+    <t xml:space="preserve">2022 1.4 </t>
   </si>
   <si>
     <t xml:space="preserve">2023 1 BenL</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 1 MattH</t>
+    <t xml:space="preserve">2022 1.9 </t>
   </si>
   <si>
     <t xml:space="preserve">2023 1 MattH</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 1 Andrew</t>
+    <t xml:space="preserve">2022 1.8</t>
   </si>
   <si>
     <t xml:space="preserve">2023 1 Andrew</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 1 BrandonH</t>
+    <t xml:space="preserve">2022 1.7</t>
   </si>
   <si>
     <t xml:space="preserve">2023 1 BrandonH</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 3 Jared</t>
+    <t xml:space="preserve">2022 3.5 </t>
   </si>
   <si>
     <t xml:space="preserve">2023 3 AlanP</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 1 Adam</t>
+    <t xml:space="preserve">2022 1.3</t>
   </si>
   <si>
     <t xml:space="preserve">2023 1 MikeR</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 2 Vanja</t>
+    <t xml:space="preserve">2022 2.12 </t>
   </si>
   <si>
     <t xml:space="preserve">2023 2 BenL</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 2 MattH</t>
+    <t xml:space="preserve">2022 2.9 </t>
   </si>
   <si>
     <t xml:space="preserve">2023 2 MattH</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 2 JohnO</t>
+    <t xml:space="preserve">2022 2.11</t>
   </si>
   <si>
     <t xml:space="preserve">2023 2 Andrew</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 2 BrandonH</t>
+    <t xml:space="preserve">2022 2.7</t>
   </si>
   <si>
     <t xml:space="preserve">2023 2 BrandonH</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 3 BenL</t>
+    <t xml:space="preserve">2022 3.10 </t>
   </si>
   <si>
     <t xml:space="preserve">2023 4 Vanja</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 2 Jared</t>
+    <t xml:space="preserve">2022 2.1 </t>
   </si>
   <si>
     <t xml:space="preserve">2023 1 Vanja</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 5 BenL</t>
+    <t xml:space="preserve">2022 5.10 </t>
   </si>
   <si>
     <t xml:space="preserve">2023 3 BenL</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 3 MattH</t>
+    <t xml:space="preserve">2022 3.9 </t>
   </si>
   <si>
     <t xml:space="preserve">2023 3 MattH</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 3 Andrew</t>
+    <t xml:space="preserve">2022 3.8</t>
   </si>
   <si>
     <t xml:space="preserve">2023 3 Andrew</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 3 BrandonH</t>
+    <t xml:space="preserve">2022 3.7</t>
   </si>
   <si>
     <t xml:space="preserve">2023 3 BrandonH</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 5 JohnO</t>
+    <t xml:space="preserve">2022 5.11 </t>
   </si>
   <si>
     <t xml:space="preserve">2023 5 Vanja</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 2 MikeR</t>
+    <t xml:space="preserve">2022 2.5 </t>
   </si>
   <si>
     <t xml:space="preserve">2023 1 JohnO</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 5 Vanja</t>
+    <t xml:space="preserve">2022 5.12</t>
   </si>
   <si>
     <t xml:space="preserve">2023 4 BenL</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 4 MattH</t>
+    <t xml:space="preserve">2022 4.9 </t>
   </si>
   <si>
     <t xml:space="preserve">2023 4 MattH</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 4 MikeR</t>
+    <t xml:space="preserve">2022 4.1</t>
   </si>
   <si>
     <t xml:space="preserve">2023 4 Andrew</t>
@@ -1468,7 +1468,7 @@
     <t xml:space="preserve">2023 4 BrandonH</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 5 Jared</t>
+    <t xml:space="preserve">2022 5.5 </t>
   </si>
   <si>
     <t xml:space="preserve">2023 1 Adam</t>
@@ -1477,19 +1477,19 @@
     <t xml:space="preserve">2023 5 BenL</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 5 MattH</t>
+    <t xml:space="preserve">2022 5.9 </t>
   </si>
   <si>
     <t xml:space="preserve">2023 5 MattH</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 5 Andrew</t>
+    <t xml:space="preserve">2022 5.8</t>
   </si>
   <si>
     <t xml:space="preserve">2023 5 Andrew</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 3 MikeR</t>
+    <t xml:space="preserve">2022 3.1</t>
   </si>
   <si>
     <t xml:space="preserve">2023 5 BrandonH</t>
@@ -1498,19 +1498,19 @@
     <t xml:space="preserve">2023 1 AlanP</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 4 BrandonH</t>
+    <t xml:space="preserve">2022 4.7</t>
   </si>
   <si>
     <t xml:space="preserve">2023 2 MikeR</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 4 Jared</t>
+    <t xml:space="preserve">2022 4.5</t>
   </si>
   <si>
     <t xml:space="preserve">2023 3 MikeR</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 5 BrandonH</t>
+    <t xml:space="preserve">2022 5.7</t>
   </si>
   <si>
     <t xml:space="preserve">2023 5 JohnO</t>
@@ -1534,109 +1534,112 @@
     <t xml:space="preserve">Mike Rhode - Punishers</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 4 Andrew</t>
+    <t xml:space="preserve">2022 4.3</t>
   </si>
   <si>
     <t xml:space="preserve">2023 1 JoeB</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 1 Jared</t>
+    <t xml:space="preserve">2022 1.5</t>
   </si>
   <si>
     <t xml:space="preserve">2023 2 Vanja</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 5 Adam</t>
+    <t xml:space="preserve">2022 5.3</t>
   </si>
   <si>
     <t xml:space="preserve">2023 2 Jared</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 3 AlanP</t>
+    <t xml:space="preserve">2022 3.4</t>
   </si>
   <si>
     <t xml:space="preserve">2023 3 Vanja</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 1 Zach</t>
+    <t xml:space="preserve">2022 1.2</t>
   </si>
   <si>
     <t xml:space="preserve">2023 1 Steve</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 1 JoeB</t>
+    <t xml:space="preserve">2022 1.6</t>
   </si>
   <si>
     <t xml:space="preserve">2023 2 AlanP</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 4 AlanP</t>
+    <t xml:space="preserve">2022 4.4</t>
   </si>
   <si>
     <t xml:space="preserve">2023 2 JoeB</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 1 Vanja</t>
+    <t xml:space="preserve">2022 1.12</t>
   </si>
   <si>
     <t xml:space="preserve">2023 2 Adam</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 5 AlanP</t>
+    <t xml:space="preserve">2022 5.4</t>
   </si>
   <si>
     <t xml:space="preserve">2023 3 JoeB</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 3 JoeB</t>
+    <t xml:space="preserve">2022 3 JohnO</t>
   </si>
   <si>
     <t xml:space="preserve">2023 4 Adam</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 2 Zach</t>
+    <t xml:space="preserve">2022 2.2</t>
   </si>
   <si>
     <t xml:space="preserve">2023 2 Steve</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 1 BenL</t>
+    <t xml:space="preserve">2022 1.10</t>
   </si>
   <si>
     <t xml:space="preserve">2023 2 JohnO</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 4 BenL</t>
+    <t xml:space="preserve">2022 4.6</t>
   </si>
   <si>
     <t xml:space="preserve">2023 4 JoeB</t>
   </si>
   <si>
+    <t xml:space="preserve">2022 6.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">2023 4 Jared</t>
   </si>
   <si>
     <t xml:space="preserve">2023 4 MikeR</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 3 JohnO</t>
+    <t xml:space="preserve">2022 3.11</t>
   </si>
   <si>
     <t xml:space="preserve">2023 5 Adam</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 3 Zach</t>
+    <t xml:space="preserve">2022 3.2</t>
   </si>
   <si>
     <t xml:space="preserve">2023 3 Steve</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 2 JoeB</t>
+    <t xml:space="preserve">2022 2.6</t>
   </si>
   <si>
     <t xml:space="preserve">2023 3 Jared</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 4 Adam</t>
+    <t xml:space="preserve">2022 4.8</t>
   </si>
   <si>
     <t xml:space="preserve">2023 5 JoeB</t>
@@ -1648,199 +1651,277 @@
     <t xml:space="preserve">2023 4 AlanP</t>
   </si>
   <si>
+    <t xml:space="preserve">2022 6.3</t>
+  </si>
+  <si>
     <t xml:space="preserve">2023 5 Jared</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 4 Zach</t>
+    <t xml:space="preserve">2022 4.2</t>
   </si>
   <si>
     <t xml:space="preserve">2023 4 Steve</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 2 Adam</t>
+    <t xml:space="preserve">2022 2.3</t>
   </si>
   <si>
     <t xml:space="preserve">2023 3 JohnO</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 4 JoeB</t>
+    <t xml:space="preserve">2022 4.10</t>
   </si>
   <si>
     <t xml:space="preserve">2023 5 AlanP</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 5 Zach</t>
+    <t xml:space="preserve">2022 5.2</t>
   </si>
   <si>
     <t xml:space="preserve">2023 5 Steve</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 2 AlanP</t>
+    <t xml:space="preserve">2022 2.4</t>
   </si>
   <si>
     <t xml:space="preserve">2023 4 JohnO</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 5 JoeB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 2 Andrew</t>
+    <t xml:space="preserve">2022 5.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 2.8</t>
   </si>
   <si>
     <t xml:space="preserve">2023 5 MikeR</t>
   </si>
   <si>
+    <t xml:space="preserve">2022 2.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 3.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 4.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 4 .12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 5.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Ben and John each drew something out of a hat on each end to select the first 3. Ben picked a number and John drew a name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brandon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kupp My Footballs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanja Dolas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eranievanja@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BeatinGoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steve Cohen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scohe11@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bad Juju</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benjamin Luther</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blluther7@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Trade Committee member</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VikesRock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Olson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">john.olson8734@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Col Mostert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joseph Bures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JoeyBures@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luke Bachmann</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lukeb55@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeke – A – Virus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jared Fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FieldsJared54@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magic Skol Bus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brandon Hurd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bjhurd@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Young Guns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mike Rhode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roadrunner44@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slick Daddy Club</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrew Gates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">andrewagates89@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thielen Groovy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam Wells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adamwells12@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the naked pooper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alan Powell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">powellap28@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Velociraptor Maloish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matt Holland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">king_ahab11@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Josh Jacobs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laviska Shenault</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chase Claypool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 1 John</t>
+  </si>
+  <si>
     <t xml:space="preserve">2022 2 BenL</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 3 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 4 JohnO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 4 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 5 MikeR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kupp My Footballs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vanja Dolas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eranievanja@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BeatinGoff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Steve Cohen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bad Juju</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Benjamin Luther</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blluther7@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Trade Committee member</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VikesRock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John Olson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">john.olson8734@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Col Mostert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joseph Bures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JoeyBures@hotmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luke Bachmann</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lukeb55@hotmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zeke – A – Virus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jared Fields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldsJared54@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magic Skol Bus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brandon Hurd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bjhurd@hotmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Young Guns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mike Rhode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">roadrunner44@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slick Daddy Club</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andrew Gates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">andrewagates89@hotmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thielen Groovy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adam Wells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adamwells12@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the naked pooper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alan Powell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">powellap28@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Velociraptor Maloish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matt Holland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">king_ahab11@hotmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Josh Jacobs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laviska Shenault</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chase Claypool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 1 John</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hunter Henry</t>
   </si>
   <si>
     <t xml:space="preserve">Tyler Higbee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jared</t>
   </si>
   <si>
     <t xml:space="preserve">DeAndre Hopkins</t>
@@ -1900,9 +1981,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">John</t>
-  </si>
-  <si>
     <t xml:space="preserve">DK metcalf</t>
   </si>
   <si>
@@ -1921,18 +1999,15 @@
     <t xml:space="preserve">Rhamandre Stevenson</t>
   </si>
   <si>
+    <t xml:space="preserve">2022 2 Jared</t>
+  </si>
+  <si>
     <t xml:space="preserve">JohnO</t>
   </si>
   <si>
     <t xml:space="preserve">2022 1.06</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 1.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 1.12</t>
-  </si>
-  <si>
     <t xml:space="preserve">2022 2.06</t>
   </si>
   <si>
@@ -1975,7 +2050,7 @@
     <t xml:space="preserve">2022 2.4 (alan)</t>
   </si>
   <si>
-    <t xml:space="preserve">Alan</t>
+    <t xml:space="preserve">2022 2 Andrew</t>
   </si>
   <si>
     <t xml:space="preserve">2023 1 Alan</t>
@@ -1984,7 +2059,13 @@
     <t xml:space="preserve">2023 3 Alan</t>
   </si>
   <si>
-    <t xml:space="preserve">Joe</t>
+    <t xml:space="preserve">2022 4 Andrew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 4 AlanP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 4 BenL</t>
   </si>
   <si>
     <t xml:space="preserve">2023 3 Joe</t>
@@ -2002,12 +2083,15 @@
     <t xml:space="preserve">2022 2 mikeR</t>
   </si>
   <si>
+    <t xml:space="preserve">2022 3 AlanP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 3 JoeB</t>
+  </si>
+  <si>
     <t xml:space="preserve">For</t>
   </si>
   <si>
-    <t xml:space="preserve">Adam</t>
-  </si>
-  <si>
     <t xml:space="preserve">2023 1 Adam </t>
   </si>
   <si>
@@ -2104,6 +2188,9 @@
     <t xml:space="preserve">2023 2 John</t>
   </si>
   <si>
+    <t xml:space="preserve">2022 1 Vanja</t>
+  </si>
+  <si>
     <t xml:space="preserve">Devin Bush</t>
   </si>
   <si>
@@ -2119,6 +2206,12 @@
     <t xml:space="preserve">Deion Jones</t>
   </si>
   <si>
+    <t xml:space="preserve">2022 4 Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 4 JoeB</t>
+  </si>
+  <si>
     <t xml:space="preserve">JoeB/Luke</t>
   </si>
   <si>
@@ -2153,6 +2246,9 @@
   </si>
   <si>
     <t xml:space="preserve">Khalil Herbert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 1 JohnO</t>
   </si>
 </sst>
 </file>
@@ -2364,6 +2460,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2393,10 +2493,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2521,7 +2617,7 @@
   <dimension ref="A1:V83"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2931,6 +3027,7 @@
       <c r="B14" s="0" t="s">
         <v>81</v>
       </c>
+      <c r="C14" s="8"/>
       <c r="E14" s="7"/>
       <c r="F14" s="0" t="s">
         <v>82</v>
@@ -3035,7 +3132,7 @@
       <c r="B18" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="9" t="s">
         <v>106</v>
       </c>
       <c r="F18" s="0" t="s">
@@ -3063,7 +3160,7 @@
       <c r="B19" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="E19" s="8"/>
+      <c r="E19" s="9"/>
       <c r="F19" s="0" t="s">
         <v>113</v>
       </c>
@@ -3075,7 +3172,7 @@
       <c r="N19" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="Q19" s="8" t="s">
+      <c r="Q19" s="9" t="s">
         <v>106</v>
       </c>
       <c r="R19" s="0" t="s">
@@ -3091,7 +3188,7 @@
       <c r="B20" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="8"/>
+      <c r="E20" s="9"/>
       <c r="F20" s="0" t="s">
         <v>119</v>
       </c>
@@ -3103,7 +3200,7 @@
       <c r="N20" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="Q20" s="8"/>
+      <c r="Q20" s="9"/>
       <c r="R20" s="0" t="s">
         <v>122</v>
       </c>
@@ -3117,7 +3214,7 @@
       <c r="B21" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="10" t="s">
         <v>125</v>
       </c>
       <c r="F21" s="0" t="s">
@@ -3131,7 +3228,7 @@
       <c r="N21" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="Q21" s="8"/>
+      <c r="Q21" s="9"/>
       <c r="R21" s="0" t="s">
         <v>129</v>
       </c>
@@ -3145,7 +3242,7 @@
       <c r="B22" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="E22" s="9"/>
+      <c r="E22" s="10"/>
       <c r="F22" s="0" t="s">
         <v>132</v>
       </c>
@@ -3153,13 +3250,13 @@
       <c r="J22" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="M22" s="8" t="s">
+      <c r="M22" s="9" t="s">
         <v>106</v>
       </c>
       <c r="N22" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="Q22" s="9" t="s">
+      <c r="Q22" s="10" t="s">
         <v>125</v>
       </c>
       <c r="R22" s="0" t="s">
@@ -3171,31 +3268,31 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="9" t="s">
         <v>106</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="E23" s="9"/>
+      <c r="E23" s="10"/>
       <c r="F23" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="I23" s="9" t="s">
         <v>106</v>
       </c>
       <c r="J23" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="M23" s="8"/>
+      <c r="M23" s="9"/>
       <c r="N23" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="Q23" s="9"/>
+      <c r="Q23" s="10"/>
       <c r="R23" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="U23" s="8" t="s">
+      <c r="U23" s="9" t="s">
         <v>106</v>
       </c>
       <c r="V23" s="0" t="s">
@@ -3203,59 +3300,59 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8"/>
+      <c r="A24" s="9"/>
       <c r="B24" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="11" t="s">
         <v>144</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="I24" s="8"/>
+      <c r="I24" s="9"/>
       <c r="J24" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="M24" s="9" t="s">
+      <c r="M24" s="10" t="s">
         <v>125</v>
       </c>
       <c r="N24" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="Q24" s="9"/>
+      <c r="Q24" s="10"/>
       <c r="R24" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="U24" s="8"/>
+      <c r="U24" s="9"/>
       <c r="V24" s="0" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="E25" s="10"/>
+      <c r="E25" s="11"/>
       <c r="F25" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="I25" s="9" t="s">
+      <c r="I25" s="10" t="s">
         <v>125</v>
       </c>
       <c r="J25" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="M25" s="9"/>
+      <c r="M25" s="10"/>
       <c r="N25" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="Q25" s="9"/>
+      <c r="Q25" s="10"/>
       <c r="R25" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="U25" s="9" t="s">
+      <c r="U25" s="10" t="s">
         <v>125</v>
       </c>
       <c r="V25" s="0" t="s">
@@ -3263,87 +3360,87 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="10" t="s">
         <v>125</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="E26" s="10"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="I26" s="9"/>
+      <c r="I26" s="10"/>
       <c r="J26" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="M26" s="9"/>
+      <c r="M26" s="10"/>
       <c r="N26" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="Q26" s="10" t="s">
+      <c r="Q26" s="11" t="s">
         <v>144</v>
       </c>
       <c r="R26" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="U26" s="9"/>
+      <c r="U26" s="10"/>
       <c r="V26" s="0" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9"/>
+      <c r="A27" s="10"/>
       <c r="B27" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="12" t="s">
         <v>163</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="I27" s="9"/>
+      <c r="I27" s="10"/>
       <c r="J27" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="M27" s="9"/>
+      <c r="M27" s="10"/>
       <c r="N27" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="Q27" s="10"/>
+      <c r="Q27" s="11"/>
       <c r="R27" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="U27" s="9"/>
+      <c r="U27" s="10"/>
       <c r="V27" s="0" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9"/>
+      <c r="A28" s="10"/>
       <c r="B28" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="E28" s="11"/>
+      <c r="E28" s="12"/>
       <c r="F28" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="I28" s="9"/>
+      <c r="I28" s="10"/>
       <c r="J28" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="M28" s="10" t="s">
+      <c r="M28" s="11" t="s">
         <v>144</v>
       </c>
       <c r="N28" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="Q28" s="10"/>
+      <c r="Q28" s="11"/>
       <c r="R28" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="U28" s="10" t="s">
+      <c r="U28" s="11" t="s">
         <v>144</v>
       </c>
       <c r="V28" s="0" t="s">
@@ -3351,103 +3448,103 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="11" t="s">
         <v>144</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="E29" s="11"/>
+      <c r="E29" s="12"/>
       <c r="F29" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="I29" s="10" t="s">
+      <c r="I29" s="11" t="s">
         <v>144</v>
       </c>
       <c r="J29" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="M29" s="10"/>
+      <c r="M29" s="11"/>
       <c r="N29" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="Q29" s="10"/>
+      <c r="Q29" s="11"/>
       <c r="R29" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="U29" s="10"/>
+      <c r="U29" s="11"/>
       <c r="V29" s="0" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="I30" s="10"/>
+      <c r="I30" s="11"/>
       <c r="J30" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="M30" s="10"/>
+      <c r="M30" s="11"/>
       <c r="N30" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="Q30" s="10"/>
+      <c r="Q30" s="11"/>
       <c r="R30" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="U30" s="10"/>
+      <c r="U30" s="11"/>
       <c r="V30" s="0" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="I31" s="10"/>
+      <c r="I31" s="11"/>
       <c r="J31" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="M31" s="11" t="s">
+      <c r="M31" s="12" t="s">
         <v>163</v>
       </c>
       <c r="N31" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="Q31" s="11" t="s">
+      <c r="Q31" s="12" t="s">
         <v>163</v>
       </c>
       <c r="R31" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="U31" s="10"/>
+      <c r="U31" s="11"/>
       <c r="V31" s="0" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="10"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="I32" s="11" t="s">
+      <c r="I32" s="12" t="s">
         <v>163</v>
       </c>
       <c r="J32" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="M32" s="11"/>
+      <c r="M32" s="12"/>
       <c r="N32" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="Q32" s="11"/>
+      <c r="Q32" s="12"/>
       <c r="R32" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="U32" s="11" t="s">
+      <c r="U32" s="12" t="s">
         <v>163</v>
       </c>
       <c r="V32" s="0" t="s">
@@ -3455,114 +3552,114 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="I33" s="11"/>
+      <c r="I33" s="12"/>
       <c r="J33" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="M33" s="11"/>
+      <c r="M33" s="12"/>
       <c r="N33" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="Q33" s="11"/>
+      <c r="Q33" s="12"/>
       <c r="R33" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="U33" s="11"/>
+      <c r="U33" s="12"/>
       <c r="V33" s="0" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="12" t="s">
         <v>163</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="I34" s="11"/>
+      <c r="I34" s="12"/>
       <c r="J34" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="M34" s="11"/>
+      <c r="M34" s="12"/>
       <c r="N34" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="Q34" s="11"/>
+      <c r="Q34" s="12"/>
       <c r="R34" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="U34" s="11"/>
+      <c r="U34" s="12"/>
       <c r="V34" s="0" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="11"/>
+      <c r="A35" s="12"/>
       <c r="B35" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="I35" s="11"/>
+      <c r="I35" s="12"/>
       <c r="J35" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="M35" s="11"/>
+      <c r="M35" s="12"/>
       <c r="N35" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="Q35" s="11"/>
+      <c r="Q35" s="12"/>
       <c r="R35" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="U35" s="11"/>
+      <c r="U35" s="12"/>
       <c r="V35" s="0" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="11"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="G36" s="12"/>
-      <c r="I36" s="11"/>
+      <c r="G36" s="13"/>
+      <c r="I36" s="12"/>
       <c r="J36" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="M36" s="11"/>
+      <c r="M36" s="12"/>
       <c r="N36" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="U36" s="11"/>
+      <c r="U36" s="12"/>
       <c r="V36" s="0" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11"/>
+      <c r="A37" s="12"/>
       <c r="B37" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="G37" s="12"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G38" s="12"/>
+      <c r="G38" s="13"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D39" s="12"/>
-      <c r="G39" s="12"/>
+      <c r="D39" s="13"/>
+      <c r="G39" s="13"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="G40" s="12"/>
+      <c r="A40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="G40" s="13"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12"/>
-      <c r="D41" s="12"/>
+      <c r="A41" s="13"/>
+      <c r="D41" s="13"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
@@ -4022,7 +4119,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="13" t="s">
+      <c r="A58" s="14" t="s">
         <v>106</v>
       </c>
       <c r="B58" s="0" t="s">
@@ -4040,7 +4137,7 @@
       <c r="N58" s="0" t="s">
         <v>316</v>
       </c>
-      <c r="Q58" s="8" t="s">
+      <c r="Q58" s="9" t="s">
         <v>106</v>
       </c>
       <c r="R58" s="0" t="s">
@@ -4052,7 +4149,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="10" t="s">
         <v>125</v>
       </c>
       <c r="B59" s="0" t="s">
@@ -4070,7 +4167,7 @@
       <c r="N59" s="0" t="s">
         <v>322</v>
       </c>
-      <c r="Q59" s="8"/>
+      <c r="Q59" s="9"/>
       <c r="R59" s="0" t="s">
         <v>323</v>
       </c>
@@ -4080,11 +4177,11 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="9"/>
+      <c r="A60" s="10"/>
       <c r="B60" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="E60" s="8" t="s">
+      <c r="E60" s="9" t="s">
         <v>106</v>
       </c>
       <c r="F60" s="0" t="s">
@@ -4098,7 +4195,7 @@
       <c r="N60" s="0" t="s">
         <v>328</v>
       </c>
-      <c r="Q60" s="8"/>
+      <c r="Q60" s="9"/>
       <c r="R60" s="0" t="s">
         <v>329</v>
       </c>
@@ -4108,13 +4205,13 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="9" t="s">
+      <c r="A61" s="10" t="s">
         <v>228</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>331</v>
       </c>
-      <c r="E61" s="8"/>
+      <c r="E61" s="9"/>
       <c r="F61" s="0" t="s">
         <v>332</v>
       </c>
@@ -4126,7 +4223,7 @@
       <c r="N61" s="0" t="s">
         <v>334</v>
       </c>
-      <c r="Q61" s="9" t="s">
+      <c r="Q61" s="10" t="s">
         <v>125</v>
       </c>
       <c r="R61" s="0" t="s">
@@ -4138,11 +4235,11 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="9"/>
+      <c r="A62" s="10"/>
       <c r="B62" s="0" t="s">
         <v>337</v>
       </c>
-      <c r="E62" s="9" t="s">
+      <c r="E62" s="10" t="s">
         <v>125</v>
       </c>
       <c r="F62" s="0" t="s">
@@ -4156,7 +4253,7 @@
       <c r="N62" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="Q62" s="9"/>
+      <c r="Q62" s="10"/>
       <c r="R62" s="0" t="s">
         <v>341</v>
       </c>
@@ -4166,13 +4263,13 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="9" t="s">
+      <c r="A63" s="10" t="s">
         <v>228</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>343</v>
       </c>
-      <c r="E63" s="9"/>
+      <c r="E63" s="10"/>
       <c r="F63" s="0" t="s">
         <v>344</v>
       </c>
@@ -4184,7 +4281,7 @@
       <c r="N63" s="0" t="s">
         <v>346</v>
       </c>
-      <c r="Q63" s="9"/>
+      <c r="Q63" s="10"/>
       <c r="R63" s="0" t="s">
         <v>347</v>
       </c>
@@ -4194,13 +4291,13 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="11" t="s">
         <v>144</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>349</v>
       </c>
-      <c r="E64" s="9"/>
+      <c r="E64" s="10"/>
       <c r="F64" s="0" t="s">
         <v>350</v>
       </c>
@@ -4212,11 +4309,11 @@
       <c r="N64" s="0" t="s">
         <v>352</v>
       </c>
-      <c r="Q64" s="9"/>
+      <c r="Q64" s="10"/>
       <c r="R64" s="0" t="s">
         <v>353</v>
       </c>
-      <c r="U64" s="8" t="s">
+      <c r="U64" s="9" t="s">
         <v>106</v>
       </c>
       <c r="V64" s="0" t="s">
@@ -4224,113 +4321,113 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="10"/>
+      <c r="A65" s="11"/>
       <c r="B65" s="0" t="s">
         <v>355</v>
       </c>
-      <c r="E65" s="10" t="s">
+      <c r="E65" s="11" t="s">
         <v>144</v>
       </c>
       <c r="F65" s="0" t="s">
         <v>356</v>
       </c>
-      <c r="I65" s="8" t="s">
+      <c r="I65" s="9" t="s">
         <v>106</v>
       </c>
       <c r="J65" s="0" t="s">
         <v>357</v>
       </c>
-      <c r="M65" s="8" t="s">
+      <c r="M65" s="9" t="s">
         <v>106</v>
       </c>
       <c r="N65" s="0" t="s">
         <v>358</v>
       </c>
-      <c r="Q65" s="10" t="s">
+      <c r="Q65" s="11" t="s">
         <v>144</v>
       </c>
       <c r="R65" s="0" t="s">
         <v>359</v>
       </c>
-      <c r="U65" s="8"/>
+      <c r="U65" s="9"/>
       <c r="V65" s="0" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="10"/>
+      <c r="A66" s="11"/>
       <c r="B66" s="0" t="s">
         <v>361</v>
       </c>
-      <c r="E66" s="10"/>
+      <c r="E66" s="11"/>
       <c r="F66" s="0" t="s">
         <v>362</v>
       </c>
-      <c r="I66" s="8"/>
+      <c r="I66" s="9"/>
       <c r="J66" s="0" t="s">
         <v>363</v>
       </c>
-      <c r="M66" s="8"/>
+      <c r="M66" s="9"/>
       <c r="N66" s="0" t="s">
         <v>364</v>
       </c>
-      <c r="Q66" s="10"/>
+      <c r="Q66" s="11"/>
       <c r="R66" s="0" t="s">
         <v>365</v>
       </c>
-      <c r="U66" s="8"/>
+      <c r="U66" s="9"/>
       <c r="V66" s="0" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="10"/>
+      <c r="A67" s="11"/>
       <c r="B67" s="0" t="s">
         <v>367</v>
       </c>
-      <c r="E67" s="10"/>
+      <c r="E67" s="11"/>
       <c r="F67" s="0" t="s">
         <v>368</v>
       </c>
-      <c r="I67" s="8"/>
+      <c r="I67" s="9"/>
       <c r="J67" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="M67" s="8"/>
+      <c r="M67" s="9"/>
       <c r="N67" s="0" t="s">
         <v>370</v>
       </c>
-      <c r="Q67" s="10"/>
+      <c r="Q67" s="11"/>
       <c r="R67" s="0" t="s">
         <v>371</v>
       </c>
-      <c r="U67" s="8"/>
+      <c r="U67" s="9"/>
       <c r="V67" s="0" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="10"/>
+      <c r="A68" s="11"/>
       <c r="B68" s="0" t="s">
         <v>373</v>
       </c>
-      <c r="E68" s="10"/>
+      <c r="E68" s="11"/>
       <c r="F68" s="0" t="s">
         <v>374</v>
       </c>
-      <c r="I68" s="8"/>
+      <c r="I68" s="9"/>
       <c r="J68" s="0" t="s">
         <v>375</v>
       </c>
-      <c r="M68" s="8"/>
+      <c r="M68" s="9"/>
       <c r="N68" s="0" t="s">
         <v>376</v>
       </c>
-      <c r="Q68" s="10"/>
+      <c r="Q68" s="11"/>
       <c r="R68" s="0" t="s">
         <v>377</v>
       </c>
-      <c r="U68" s="9" t="s">
+      <c r="U68" s="10" t="s">
         <v>125</v>
       </c>
       <c r="V68" s="0" t="s">
@@ -4338,87 +4435,87 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="11" t="s">
+      <c r="A69" s="12" t="s">
         <v>163</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>379</v>
       </c>
-      <c r="E69" s="11" t="s">
+      <c r="E69" s="12" t="s">
         <v>163</v>
       </c>
       <c r="F69" s="0" t="s">
         <v>380</v>
       </c>
-      <c r="I69" s="9" t="s">
+      <c r="I69" s="10" t="s">
         <v>125</v>
       </c>
       <c r="J69" s="0" t="s">
         <v>381</v>
       </c>
-      <c r="M69" s="8"/>
+      <c r="M69" s="9"/>
       <c r="N69" s="0" t="s">
         <v>382</v>
       </c>
-      <c r="Q69" s="11" t="s">
+      <c r="Q69" s="12" t="s">
         <v>163</v>
       </c>
       <c r="R69" s="0" t="s">
         <v>383</v>
       </c>
-      <c r="U69" s="9"/>
+      <c r="U69" s="10"/>
       <c r="V69" s="0" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="11"/>
+      <c r="A70" s="12"/>
       <c r="B70" s="0" t="s">
         <v>385</v>
       </c>
-      <c r="E70" s="11"/>
+      <c r="E70" s="12"/>
       <c r="F70" s="0" t="s">
         <v>386</v>
       </c>
-      <c r="I70" s="9"/>
+      <c r="I70" s="10"/>
       <c r="J70" s="0" t="s">
         <v>387</v>
       </c>
-      <c r="M70" s="8"/>
+      <c r="M70" s="9"/>
       <c r="N70" s="0" t="s">
         <v>388</v>
       </c>
-      <c r="Q70" s="11"/>
+      <c r="Q70" s="12"/>
       <c r="R70" s="0" t="s">
         <v>389</v>
       </c>
-      <c r="U70" s="9"/>
+      <c r="U70" s="10"/>
       <c r="V70" s="5" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="11"/>
+      <c r="A71" s="12"/>
       <c r="B71" s="0" t="s">
         <v>391</v>
       </c>
-      <c r="E71" s="11"/>
+      <c r="E71" s="12"/>
       <c r="F71" s="0" t="s">
         <v>392</v>
       </c>
-      <c r="I71" s="9"/>
+      <c r="I71" s="10"/>
       <c r="J71" s="0" t="s">
         <v>393</v>
       </c>
-      <c r="M71" s="8"/>
+      <c r="M71" s="9"/>
       <c r="N71" s="0" t="s">
         <v>394</v>
       </c>
-      <c r="Q71" s="11"/>
+      <c r="Q71" s="12"/>
       <c r="R71" s="0" t="s">
         <v>395</v>
       </c>
-      <c r="U71" s="10" t="s">
+      <c r="U71" s="11" t="s">
         <v>144</v>
       </c>
       <c r="V71" s="0" t="s">
@@ -4426,73 +4523,73 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="11"/>
+      <c r="A72" s="12"/>
       <c r="B72" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="I72" s="9"/>
+      <c r="I72" s="10"/>
       <c r="J72" s="0" t="s">
         <v>398</v>
       </c>
-      <c r="M72" s="9" t="s">
+      <c r="M72" s="10" t="s">
         <v>125</v>
       </c>
       <c r="N72" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="Q72" s="11"/>
+      <c r="Q72" s="12"/>
       <c r="R72" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="U72" s="10"/>
+      <c r="U72" s="11"/>
       <c r="V72" s="0" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I73" s="10" t="s">
+      <c r="I73" s="11" t="s">
         <v>144</v>
       </c>
       <c r="J73" s="0" t="s">
         <v>402</v>
       </c>
-      <c r="M73" s="9"/>
+      <c r="M73" s="10"/>
       <c r="N73" s="0" t="s">
         <v>403</v>
       </c>
-      <c r="Q73" s="11"/>
+      <c r="Q73" s="12"/>
       <c r="R73" s="0" t="s">
         <v>404</v>
       </c>
-      <c r="U73" s="10"/>
+      <c r="U73" s="11"/>
       <c r="V73" s="0" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I74" s="10"/>
+      <c r="I74" s="11"/>
       <c r="J74" s="0" t="s">
         <v>406</v>
       </c>
-      <c r="M74" s="9"/>
+      <c r="M74" s="10"/>
       <c r="N74" s="0" t="s">
         <v>407</v>
       </c>
-      <c r="U74" s="10"/>
+      <c r="U74" s="11"/>
       <c r="V74" s="0" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I75" s="10"/>
+      <c r="I75" s="11"/>
       <c r="J75" s="0" t="s">
         <v>409</v>
       </c>
-      <c r="M75" s="9"/>
+      <c r="M75" s="10"/>
       <c r="N75" s="0" t="s">
         <v>410</v>
       </c>
-      <c r="U75" s="11" t="s">
+      <c r="U75" s="12" t="s">
         <v>163</v>
       </c>
       <c r="V75" s="0" t="s">
@@ -4500,76 +4597,76 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I76" s="10"/>
+      <c r="I76" s="11"/>
       <c r="J76" s="0" t="s">
         <v>412</v>
       </c>
-      <c r="M76" s="10" t="s">
+      <c r="M76" s="11" t="s">
         <v>144</v>
       </c>
       <c r="N76" s="0" t="s">
         <v>413</v>
       </c>
-      <c r="U76" s="11"/>
+      <c r="U76" s="12"/>
       <c r="V76" s="0" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I77" s="11" t="s">
+      <c r="I77" s="12" t="s">
         <v>163</v>
       </c>
       <c r="J77" s="0" t="s">
         <v>415</v>
       </c>
-      <c r="M77" s="10"/>
+      <c r="M77" s="11"/>
       <c r="N77" s="0" t="s">
         <v>416</v>
       </c>
-      <c r="U77" s="11"/>
+      <c r="U77" s="12"/>
       <c r="V77" s="0" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="12"/>
-      <c r="D78" s="12"/>
-      <c r="G78" s="12"/>
-      <c r="I78" s="11"/>
+      <c r="A78" s="13"/>
+      <c r="D78" s="13"/>
+      <c r="G78" s="13"/>
+      <c r="I78" s="12"/>
       <c r="J78" s="0" t="s">
         <v>418</v>
       </c>
-      <c r="M78" s="10"/>
+      <c r="M78" s="11"/>
       <c r="N78" s="0" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="12"/>
-      <c r="D79" s="12"/>
-      <c r="I79" s="11"/>
+      <c r="A79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="I79" s="12"/>
       <c r="J79" s="0" t="s">
         <v>420</v>
       </c>
-      <c r="M79" s="10"/>
+      <c r="M79" s="11"/>
       <c r="N79" s="0" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="12"/>
-      <c r="I80" s="11"/>
+      <c r="A80" s="13"/>
+      <c r="I80" s="12"/>
       <c r="J80" s="0" t="s">
         <v>422</v>
       </c>
-      <c r="M80" s="10"/>
+      <c r="M80" s="11"/>
       <c r="N80" s="0" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J81" s="1"/>
-      <c r="M81" s="11" t="s">
+      <c r="M81" s="12" t="s">
         <v>163</v>
       </c>
       <c r="N81" s="0" t="s">
@@ -4577,13 +4674,13 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M82" s="11"/>
+      <c r="M82" s="12"/>
       <c r="N82" s="0" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M83" s="11"/>
+      <c r="M83" s="12"/>
       <c r="N83" s="0" t="s">
         <v>426</v>
       </c>
@@ -4702,7 +4799,7 @@
   <dimension ref="A1:T63"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5082,228 +5179,289 @@
       <c r="C19" s="0" t="s">
         <v>528</v>
       </c>
+      <c r="E19" s="0" t="s">
+        <v>529</v>
+      </c>
       <c r="F19" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="N19" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="P19" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="Q19" s="0" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="S19" s="0" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="T19" s="0" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
+      </c>
+      <c r="M20" s="0" t="s">
+        <v>542</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="P20" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="Q20" s="0" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="S20" s="0" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="T20" s="0" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="P21" s="0" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="Q21" s="0" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="S21" s="0" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="T21" s="0" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="S22" s="0" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="T22" s="0" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S23" s="0" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S24" s="0" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S25" s="0" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S26" s="0" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S27" s="0" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="14"/>
+      <c r="C29" s="15"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="14"/>
+      <c r="C30" s="15"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="14"/>
+      <c r="C31" s="15"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="14"/>
+      <c r="C32" s="15"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="14"/>
+      <c r="B33" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>563</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>564</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="14"/>
+      <c r="B34" s="0" t="s">
+        <v>565</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>566</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="14"/>
+      <c r="B35" s="0" t="s">
+        <v>567</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="14"/>
+      <c r="B36" s="0" t="s">
+        <v>569</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
+      <c r="B37" s="15" t="s">
+        <v>571</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
+      <c r="B38" s="0" t="s">
+        <v>573</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>574</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
+      <c r="B39" s="0" t="s">
+        <v>575</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>576</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
+      <c r="B40" s="0" t="s">
+        <v>577</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>578</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
+      <c r="B41" s="0" t="s">
+        <v>579</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>580</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
+      <c r="B42" s="15" t="s">
+        <v>581</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>582</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
+      <c r="B43" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
+      <c r="B44" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>586</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="15"/>
-      <c r="C58" s="14"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="15"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5343,7 +5501,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5357,151 +5515,157 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>560</v>
+        <v>587</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>588</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>563</v>
+        <v>590</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>564</v>
-      </c>
-      <c r="C2" s="16"/>
-    </row>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>591</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>565</v>
+        <v>593</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>567</v>
+        <v>594</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>595</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>568</v>
+        <v>596</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>569</v>
+        <v>597</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>570</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>571</v>
+        <v>598</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>599</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>568</v>
+        <v>596</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>572</v>
+        <v>600</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>573</v>
+        <v>601</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>574</v>
+        <v>602</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>575</v>
+        <v>603</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>577</v>
+        <v>605</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>578</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>579</v>
+        <v>606</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>580</v>
+        <v>608</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>581</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>582</v>
+        <v>609</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>610</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>583</v>
+        <v>611</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>584</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>585</v>
+        <v>612</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>586</v>
+        <v>614</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>587</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>588</v>
+        <v>615</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>616</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>589</v>
+        <v>617</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>590</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>591</v>
+        <v>618</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>592</v>
+        <v>620</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>593</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>594</v>
+        <v>621</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>622</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>568</v>
+        <v>596</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>595</v>
+        <v>623</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>596</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>597</v>
-      </c>
-    </row>
+        <v>624</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="8"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5548,53 +5712,53 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="14.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="20.18"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="15" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="14.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="16" width="20.18"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="16" width="8.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
-        <v>598</v>
+        <v>586</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>599</v>
+        <v>626</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20"/>
       <c r="B2" s="21" t="s">
-        <v>600</v>
+        <v>627</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22"/>
       <c r="B3" s="21" t="s">
-        <v>601</v>
+        <v>628</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20"/>
       <c r="B4" s="21" t="s">
-        <v>602</v>
+        <v>629</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="22"/>
       <c r="B5" s="21" t="s">
-        <v>555</v>
+        <v>630</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="22"/>
       <c r="B6" s="21" t="s">
-        <v>603</v>
+        <v>631</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="20"/>
       <c r="B7" s="21" t="s">
-        <v>604</v>
+        <v>632</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5603,100 +5767,100 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
-        <v>605</v>
+        <v>572</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>606</v>
+        <v>633</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22"/>
       <c r="B10" s="21" t="s">
-        <v>607</v>
+        <v>634</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="20"/>
       <c r="B11" s="21" t="s">
-        <v>608</v>
+        <v>635</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22"/>
       <c r="B12" s="21" t="s">
-        <v>609</v>
+        <v>636</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="20"/>
       <c r="B13" s="21" t="s">
-        <v>610</v>
+        <v>637</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="23"/>
       <c r="B14" s="24" t="s">
-        <v>611</v>
+        <v>638</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="14"/>
+      <c r="B15" s="15"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>598</v>
+        <v>586</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>612</v>
+        <v>639</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="22"/>
       <c r="B17" s="21" t="s">
-        <v>613</v>
+        <v>640</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="20"/>
       <c r="B18" s="21" t="s">
-        <v>614</v>
+        <v>641</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>615</v>
+        <v>584</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>616</v>
+        <v>642</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="20"/>
       <c r="B20" s="21" t="s">
-        <v>617</v>
+        <v>643</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="23"/>
       <c r="B21" s="24" t="s">
-        <v>618</v>
+        <v>644</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="14"/>
+      <c r="B22" s="15"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="s">
-        <v>619</v>
+        <v>645</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>620</v>
+        <v>646</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="22"/>
       <c r="B24" s="21" t="s">
-        <v>621</v>
+        <v>647</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5720,7 +5884,7 @@
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="22"/>
       <c r="B28" s="21" t="s">
-        <v>459</v>
+        <v>648</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5729,82 +5893,82 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>622</v>
+        <v>649</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>623</v>
+        <v>650</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="22"/>
       <c r="B31" s="21" t="s">
-        <v>624</v>
+        <v>525</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="20"/>
       <c r="B32" s="21" t="s">
-        <v>625</v>
+        <v>517</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22"/>
       <c r="B33" s="21" t="s">
-        <v>626</v>
+        <v>651</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="20"/>
       <c r="B34" s="21" t="s">
-        <v>627</v>
+        <v>652</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="22"/>
       <c r="B35" s="21" t="s">
-        <v>628</v>
+        <v>653</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="23"/>
       <c r="B36" s="24" t="s">
-        <v>629</v>
+        <v>654</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="14"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="18" t="s">
-        <v>615</v>
+        <v>584</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>630</v>
+        <v>655</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="20"/>
       <c r="B40" s="21" t="s">
-        <v>631</v>
+        <v>656</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22"/>
       <c r="B41" s="21" t="s">
-        <v>632</v>
+        <v>657</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="20"/>
       <c r="B42" s="21" t="s">
-        <v>633</v>
+        <v>658</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="22"/>
       <c r="B43" s="21" t="s">
-        <v>634</v>
+        <v>659</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5813,10 +5977,10 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="22" t="s">
-        <v>605</v>
+        <v>572</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>635</v>
+        <v>660</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5828,43 +5992,43 @@
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22"/>
       <c r="B47" s="21" t="s">
-        <v>603</v>
+        <v>631</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="20"/>
       <c r="B48" s="21" t="s">
-        <v>636</v>
+        <v>661</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="23"/>
       <c r="B49" s="24" t="s">
-        <v>618</v>
+        <v>644</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="18" t="s">
-        <v>637</v>
+        <v>662</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>638</v>
+        <v>663</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="20"/>
       <c r="B52" s="21" t="s">
-        <v>639</v>
+        <v>664</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="22"/>
       <c r="B53" s="21" t="s">
-        <v>553</v>
+        <v>665</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5875,142 +6039,142 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="20" t="s">
-        <v>640</v>
+        <v>570</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>641</v>
+        <v>666</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="23"/>
       <c r="B56" s="24" t="s">
-        <v>642</v>
+        <v>667</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="14"/>
-      <c r="B57" s="14"/>
+      <c r="A57" s="15"/>
+      <c r="B57" s="15"/>
     </row>
     <row r="58" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="14"/>
+      <c r="B58" s="15"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="18" t="s">
-        <v>640</v>
+        <v>570</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>503</v>
+        <v>668</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="22"/>
       <c r="B60" s="21" t="s">
-        <v>515</v>
+        <v>669</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="20"/>
       <c r="B61" s="21" t="s">
-        <v>527</v>
+        <v>670</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="23" t="s">
-        <v>643</v>
+        <v>574</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>644</v>
+        <v>671</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="14"/>
-      <c r="B63" s="14"/>
+      <c r="A63" s="15"/>
+      <c r="B63" s="15"/>
     </row>
     <row r="64" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="14"/>
+      <c r="B64" s="15"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="18" t="s">
-        <v>605</v>
+        <v>572</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>645</v>
+        <v>672</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="22"/>
       <c r="B66" s="21" t="s">
-        <v>646</v>
+        <v>673</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="22"/>
       <c r="B67" s="21" t="s">
-        <v>647</v>
+        <v>674</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="22"/>
       <c r="B68" s="21" t="s">
-        <v>648</v>
+        <v>675</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="22"/>
       <c r="B69" s="21" t="s">
-        <v>509</v>
+        <v>676</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="22"/>
       <c r="B70" s="21" t="s">
-        <v>521</v>
+        <v>677</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="22"/>
       <c r="B71" s="21" t="s">
-        <v>649</v>
+        <v>678</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="22" t="s">
-        <v>650</v>
+        <v>568</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>651</v>
+        <v>679</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="23"/>
       <c r="B73" s="24" t="s">
-        <v>652</v>
+        <v>680</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="25"/>
       <c r="B75" s="19" t="s">
-        <v>653</v>
+        <v>681</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="18" t="s">
-        <v>654</v>
+        <v>682</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>655</v>
+        <v>683</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="20"/>
       <c r="B77" s="21" t="s">
-        <v>656</v>
+        <v>684</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="20"/>
       <c r="B78" s="21" t="s">
-        <v>657</v>
+        <v>685</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6023,34 +6187,34 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="20" t="s">
-        <v>658</v>
+        <v>686</v>
       </c>
       <c r="B81" s="21" t="s">
-        <v>620</v>
+        <v>646</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="20"/>
       <c r="B82" s="21" t="s">
-        <v>659</v>
+        <v>687</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="20"/>
       <c r="B83" s="21" t="s">
-        <v>660</v>
+        <v>688</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="20"/>
       <c r="B84" s="21" t="s">
-        <v>661</v>
+        <v>689</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="20"/>
       <c r="B85" s="21" t="s">
-        <v>662</v>
+        <v>690</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6062,7 +6226,7 @@
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="20"/>
       <c r="B87" s="21" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6071,7 +6235,7 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="20" t="s">
-        <v>663</v>
+        <v>691</v>
       </c>
       <c r="B89" s="21" t="s">
         <v>482</v>
@@ -6080,19 +6244,19 @@
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="20"/>
       <c r="B90" s="21" t="s">
-        <v>659</v>
+        <v>687</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="20"/>
       <c r="B91" s="21" t="s">
-        <v>660</v>
+        <v>688</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="20"/>
       <c r="B92" s="21" t="s">
-        <v>662</v>
+        <v>690</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6104,7 +6268,7 @@
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="20"/>
       <c r="B94" s="21" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6113,22 +6277,22 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="20" t="s">
-        <v>658</v>
+        <v>686</v>
       </c>
       <c r="B96" s="21" t="s">
-        <v>636</v>
+        <v>661</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="20"/>
       <c r="B97" s="21" t="s">
-        <v>664</v>
+        <v>692</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="20"/>
       <c r="B98" s="21" t="s">
-        <v>655</v>
+        <v>683</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6137,28 +6301,28 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="20" t="s">
-        <v>665</v>
+        <v>693</v>
       </c>
       <c r="B100" s="21" t="s">
-        <v>636</v>
+        <v>661</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="20"/>
       <c r="B101" s="21" t="s">
-        <v>666</v>
+        <v>694</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="20"/>
       <c r="B102" s="21" t="s">
-        <v>667</v>
+        <v>695</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="20"/>
       <c r="B103" s="21" t="s">
-        <v>668</v>
+        <v>696</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6167,7 +6331,7 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="20" t="s">
-        <v>658</v>
+        <v>686</v>
       </c>
       <c r="B105" s="21" t="s">
         <v>482</v>
@@ -6176,7 +6340,7 @@
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="20"/>
       <c r="B106" s="21" t="s">
-        <v>618</v>
+        <v>644</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6187,22 +6351,22 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="25" t="s">
-        <v>598</v>
+        <v>586</v>
       </c>
       <c r="B109" s="19" t="s">
-        <v>669</v>
+        <v>697</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="22"/>
       <c r="B110" s="21" t="s">
-        <v>670</v>
+        <v>698</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="22"/>
       <c r="B111" s="21" t="s">
-        <v>671</v>
+        <v>699</v>
       </c>
       <c r="F111" s="26"/>
     </row>
@@ -6214,7 +6378,7 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="23" t="s">
-        <v>650</v>
+        <v>568</v>
       </c>
       <c r="B113" s="24" t="s">
         <v>518</v>
@@ -6222,58 +6386,58 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="25" t="s">
-        <v>640</v>
+        <v>570</v>
       </c>
       <c r="B115" s="19" t="s">
-        <v>553</v>
+        <v>665</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="22"/>
       <c r="B116" s="21" t="s">
-        <v>672</v>
+        <v>700</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="22"/>
       <c r="B117" s="21" t="s">
-        <v>673</v>
+        <v>701</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="22" t="s">
-        <v>619</v>
+        <v>645</v>
       </c>
       <c r="B118" s="21" t="s">
-        <v>674</v>
+        <v>702</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="22"/>
       <c r="B119" s="21" t="s">
-        <v>675</v>
+        <v>703</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="23"/>
       <c r="B120" s="24" t="s">
-        <v>676</v>
+        <v>704</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="25" t="s">
-        <v>640</v>
+        <v>570</v>
       </c>
       <c r="B122" s="19" t="s">
-        <v>677</v>
+        <v>705</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="23" t="s">
-        <v>619</v>
+        <v>645</v>
       </c>
       <c r="B123" s="24" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6284,42 +6448,42 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="25" t="s">
-        <v>605</v>
+        <v>572</v>
       </c>
       <c r="B126" s="19" t="s">
-        <v>678</v>
+        <v>706</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="22"/>
       <c r="B127" s="21" t="s">
-        <v>679</v>
+        <v>707</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="22"/>
       <c r="B128" s="21" t="s">
-        <v>680</v>
+        <v>708</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="22"/>
       <c r="B129" s="21" t="s">
-        <v>642</v>
+        <v>667</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="22"/>
       <c r="B130" s="21" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="23" t="s">
-        <v>598</v>
+        <v>586</v>
       </c>
       <c r="B131" s="24" t="s">
-        <v>681</v>
+        <v>709</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6327,18 +6491,18 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="25" t="s">
-        <v>598</v>
+        <v>586</v>
       </c>
       <c r="B133" s="19" t="s">
-        <v>555</v>
+        <v>630</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="22" t="s">
-        <v>615</v>
+        <v>584</v>
       </c>
       <c r="B134" s="21" t="s">
-        <v>682</v>
+        <v>710</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6349,10 +6513,10 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="25" t="s">
-        <v>615</v>
+        <v>584</v>
       </c>
       <c r="B137" s="19" t="s">
-        <v>555</v>
+        <v>630</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6364,78 +6528,78 @@
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="22"/>
       <c r="B139" s="21" t="s">
-        <v>603</v>
+        <v>631</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="23" t="s">
-        <v>650</v>
+        <v>568</v>
       </c>
       <c r="B140" s="24" t="s">
-        <v>648</v>
+        <v>675</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="25" t="s">
-        <v>605</v>
+        <v>572</v>
       </c>
       <c r="B142" s="19" t="s">
-        <v>604</v>
+        <v>632</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="23" t="s">
-        <v>650</v>
+        <v>568</v>
       </c>
       <c r="B143" s="24" t="s">
-        <v>555</v>
+        <v>630</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="25" t="s">
-        <v>598</v>
+        <v>586</v>
       </c>
       <c r="B145" s="19" t="s">
-        <v>660</v>
+        <v>688</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="22"/>
       <c r="B146" s="21" t="s">
-        <v>608</v>
+        <v>635</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="22"/>
       <c r="B147" s="21" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="23" t="s">
-        <v>619</v>
+        <v>645</v>
       </c>
       <c r="B148" s="24" t="s">
-        <v>517</v>
+        <v>711</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="25" t="s">
-        <v>605</v>
+        <v>572</v>
       </c>
       <c r="B150" s="19" t="s">
-        <v>634</v>
+        <v>659</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="22"/>
       <c r="B151" s="21" t="s">
-        <v>683</v>
+        <v>712</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="22" t="s">
-        <v>650</v>
+        <v>568</v>
       </c>
       <c r="B152" s="21" t="s">
         <v>494</v>
@@ -6444,21 +6608,21 @@
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="23"/>
       <c r="B153" s="24" t="s">
-        <v>670</v>
+        <v>698</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="25" t="s">
-        <v>637</v>
+        <v>662</v>
       </c>
       <c r="B155" s="19" t="s">
-        <v>684</v>
+        <v>713</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="22"/>
       <c r="B156" s="21" t="s">
-        <v>641</v>
+        <v>666</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6469,109 +6633,109 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="22" t="s">
-        <v>615</v>
+        <v>584</v>
       </c>
       <c r="B158" s="21" t="s">
-        <v>685</v>
+        <v>714</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="22"/>
       <c r="B159" s="21" t="s">
-        <v>686</v>
+        <v>715</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="23"/>
       <c r="B160" s="24" t="s">
-        <v>687</v>
+        <v>716</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="25" t="s">
-        <v>605</v>
+        <v>572</v>
       </c>
       <c r="B162" s="19" t="s">
-        <v>537</v>
+        <v>717</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="22"/>
       <c r="B163" s="21" t="s">
-        <v>546</v>
+        <v>718</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="23" t="s">
-        <v>688</v>
+        <v>719</v>
       </c>
       <c r="B164" s="24" t="s">
-        <v>689</v>
+        <v>720</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="25" t="s">
-        <v>605</v>
+        <v>572</v>
       </c>
       <c r="B166" s="19" t="s">
-        <v>690</v>
+        <v>721</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="22"/>
       <c r="B167" s="21" t="s">
-        <v>636</v>
+        <v>661</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="22"/>
       <c r="B168" s="21" t="s">
-        <v>601</v>
+        <v>628</v>
       </c>
       <c r="F168" s="26"/>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="22"/>
       <c r="B169" s="21" t="s">
-        <v>691</v>
+        <v>722</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="22"/>
       <c r="B170" s="21" t="s">
-        <v>600</v>
+        <v>627</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="22"/>
       <c r="B171" s="21" t="s">
-        <v>692</v>
+        <v>723</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="22" t="s">
-        <v>598</v>
+        <v>586</v>
       </c>
       <c r="B172" s="21" t="s">
-        <v>607</v>
+        <v>634</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="22"/>
       <c r="B173" s="21" t="s">
-        <v>693</v>
+        <v>724</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="22"/>
       <c r="B174" s="21" t="s">
-        <v>694</v>
+        <v>725</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="22"/>
       <c r="B175" s="21" t="s">
-        <v>695</v>
+        <v>726</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6588,50 +6752,50 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="18" t="s">
-        <v>598</v>
+        <v>586</v>
       </c>
       <c r="B179" s="19" t="s">
-        <v>601</v>
+        <v>628</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="22"/>
       <c r="B180" s="21" t="s">
-        <v>696</v>
+        <v>727</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="22"/>
       <c r="B181" s="21" t="s">
-        <v>697</v>
+        <v>728</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="22"/>
       <c r="B182" s="21" t="s">
-        <v>682</v>
+        <v>710</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="22" t="s">
-        <v>619</v>
+        <v>645</v>
       </c>
       <c r="B183" s="21" t="s">
-        <v>698</v>
+        <v>729</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="23"/>
       <c r="B184" s="24" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="25" t="s">
-        <v>598</v>
+        <v>586</v>
       </c>
       <c r="B186" s="19" t="s">
-        <v>666</v>
+        <v>694</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6643,21 +6807,21 @@
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="22"/>
       <c r="B188" s="21" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="22" t="s">
-        <v>605</v>
+        <v>572</v>
       </c>
       <c r="B189" s="21" t="s">
-        <v>699</v>
+        <v>730</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="22"/>
       <c r="B190" s="21" t="s">
-        <v>433</v>
+        <v>731</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
no trade pick correction
MikeR pointed out I did not move pick correctly. updated
</commit_message>
<xml_diff>
--- a/OffSeason.xlsx
+++ b/OffSeason.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="741">
   <si>
     <t xml:space="preserve">Kupp My Footballs – Vanja Dolas </t>
   </si>
@@ -1576,6 +1576,9 @@
     <t xml:space="preserve">2022 1.6</t>
   </si>
   <si>
+    <t xml:space="preserve">2023 2 JohnO</t>
+  </si>
+  <si>
     <t xml:space="preserve">2022 4.4</t>
   </si>
   <si>
@@ -1609,7 +1612,7 @@
     <t xml:space="preserve">2022 1.10</t>
   </si>
   <si>
-    <t xml:space="preserve">2023 2 JohnO</t>
+    <t xml:space="preserve">2023 3 Jared</t>
   </si>
   <si>
     <t xml:space="preserve">2022 4.6</t>
@@ -1639,7 +1642,7 @@
     <t xml:space="preserve">2022 2.6</t>
   </si>
   <si>
-    <t xml:space="preserve">2023 3 Jared</t>
+    <t xml:space="preserve">2023 3 JohnO</t>
   </si>
   <si>
     <t xml:space="preserve">2022 4.8</t>
@@ -1666,7 +1669,7 @@
     <t xml:space="preserve">2022 2.3</t>
   </si>
   <si>
-    <t xml:space="preserve">2023 3 JohnO</t>
+    <t xml:space="preserve">2023 4 JohnO</t>
   </si>
   <si>
     <t xml:space="preserve">2022 4.10</t>
@@ -1684,16 +1687,13 @@
     <t xml:space="preserve">2022 2.4</t>
   </si>
   <si>
-    <t xml:space="preserve">2023 4 JohnO</t>
+    <t xml:space="preserve">2023 5 MikeR</t>
   </si>
   <si>
     <t xml:space="preserve">2022 5.6</t>
   </si>
   <si>
     <t xml:space="preserve">2022 2.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5 MikeR</t>
   </si>
   <si>
     <t xml:space="preserve">2022 2.10</t>
@@ -4832,7 +4832,7 @@
   <dimension ref="A1:T63"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5176,136 +5176,133 @@
         <v>516</v>
       </c>
       <c r="T17" s="0" t="s">
-        <v>434</v>
+        <v>517</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="P18" s="0" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="Q18" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="S18" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="T18" s="0" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="P19" s="0" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="Q19" s="0" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="S19" s="0" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="T19" s="0" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="P20" s="0" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="Q20" s="0" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="S20" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="T20" s="0" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="P21" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="Q21" s="0" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="S21" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="T21" s="0" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="S22" s="0" t="s">
-        <v>555</v>
-      </c>
-      <c r="T22" s="0" t="s">
         <v>556</v>
       </c>
     </row>
@@ -5316,7 +5313,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S24" s="0" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5944,13 +5941,13 @@
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="22"/>
       <c r="B31" s="21" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="20"/>
       <c r="B32" s="21" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6268,7 +6265,7 @@
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="20"/>
       <c r="B87" s="21" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6310,7 +6307,7 @@
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="20"/>
       <c r="B94" s="21" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6415,7 +6412,7 @@
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="22"/>
       <c r="B112" s="21" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6517,7 +6514,7 @@
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="22"/>
       <c r="B130" s="21" t="s">
-        <v>538</v>
+        <v>529</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6614,7 +6611,7 @@
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="22"/>
       <c r="B147" s="21" t="s">
-        <v>538</v>
+        <v>529</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6829,7 +6826,7 @@
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="23"/>
       <c r="B184" s="24" t="s">
-        <v>538</v>
+        <v>529</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6849,7 +6846,7 @@
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="22"/>
       <c r="B188" s="21" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7027,13 +7024,13 @@
         <v>567</v>
       </c>
       <c r="B219" s="21" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="23"/>
       <c r="B220" s="24" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="F220" s="26"/>
     </row>

</xml_diff>

<commit_message>
4 trade / 4 team trade explained
Jared	2022 3.10
BenL	2023 3 BenL
	
Jared	2022 2.5
	2023 3 BenL
MikeR	2022 2.8
	2023 2 John
	
	
Jared	2022 2.8
MattH	2023 2 MattH
	
John 	2022 1.4
	2022 1.11
Jared	2022 1.5
	2022 3.5
	2023 2 Alan
	2023 2 John
	2023 2 Vanja
	2023 2 MattH
</commit_message>
<xml_diff>
--- a/OffSeason.xlsx
+++ b/OffSeason.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Rosters" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="755">
   <si>
     <t xml:space="preserve">Kupp My Footballs – Vanja Dolas </t>
   </si>
@@ -1366,334 +1366,337 @@
     <t xml:space="preserve">2023 3 JohnO</t>
   </si>
   <si>
+    <t xml:space="preserve">2022 1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1 MikeR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 2.12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2 BenL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 2.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3 MattH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 2.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2 Andrew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 2.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2 BrandonH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 4 JohnO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 3.5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1 Vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 3.10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2 Jared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 2.9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 4 MattH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 3.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3 Andrew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 3.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3 BrandonH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 4 Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 6.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1 JohnO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 5.10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 3.9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5 MattH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 4.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 4 Andrew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 3.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 4 BrandonH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 4 Jared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1 Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 5.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 4 BenL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 4.9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 5.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5 Andrew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5 BrandonH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 4 Vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1 AlanP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5 BenL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 5.9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 4.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5 Vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2 MikeR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 4.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2 Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 5.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2 Vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2 AlanP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2 MattH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2 JohnO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3 JoeB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3 Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3 MikeR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5 JohnO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joe Bures - colonel mostert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jared Fields - Injured Reserve Team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alan Powell - The Naked Pooper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam Wells - Thielen Groovy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BeatinGoff – Steven Cohen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mike Rhode - Punishers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 4.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1 JoeB</t>
+  </si>
+  <si>
     <t xml:space="preserve">2022 1.4 </t>
   </si>
   <si>
-    <t xml:space="preserve">2023 1 MikeR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 2.12 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2 BenL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 2.9 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2 MattH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 2.11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2 Andrew</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 2.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2 BrandonH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4 JohnO</t>
+    <t xml:space="preserve">2023 6 Jared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 5.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3 Vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 3.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5 Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1 Steve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3 BenL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 4.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2 JoeB</t>
   </si>
   <si>
     <t xml:space="preserve">2022 1.11</t>
   </si>
   <si>
-    <t xml:space="preserve">2023 1 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 5.10 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2 Jared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 3.9 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3 MattH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 3.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3 Andrew</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 3.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3 BrandonH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4 Adam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1 JohnO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 5.12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3 BenL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 4.9 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4 MattH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 4.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4 Andrew</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 3.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4 BrandonH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4 Jared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1 Adam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4 BenL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 5.9 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5 MattH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 5.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5 Andrew</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 3.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5 BrandonH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1 AlanP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5 BenL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 4.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2 MikeR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 4.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2 Adam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 5.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3 JoeB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3 Adam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3 MikeR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5 JohnO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joe Bures - colonel mostert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jared Fields - Injured Reserve Team</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alan Powell - The Naked Pooper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adam Wells - Thielen Groovy</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BeatinGoff – Steven Cohen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mike Rhode - Punishers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 4.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1 JoeB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 1.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 5.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 3.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5 Adam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1 Steve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 1.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2 JohnO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 4.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2 JoeB</t>
+    <t xml:space="preserve">2022 5.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 4 MikeR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 3.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5 Jared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2 Steve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 1.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3 Jared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 4.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 4 JoeB</t>
   </si>
   <si>
     <t xml:space="preserve">2022 1.12</t>
   </si>
   <si>
-    <t xml:space="preserve">2023 2 AlanP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 5.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4 MikeR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 3.11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5 Jared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 2.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2 Steve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 1.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3 Jared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 4.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4 JoeB</t>
+    <t xml:space="preserve">2023 4 AlanP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 3.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3 Steve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 2.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5 MikeR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 4.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5 JoeB</t>
   </si>
   <si>
     <t xml:space="preserve">2022 2.1 </t>
   </si>
   <si>
-    <t xml:space="preserve">2023 4 AlanP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 3.12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 3.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3 Steve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 2.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 4.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5 JoeB</t>
+    <t xml:space="preserve">2023 5 AlanP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 6.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 4.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 4 Steve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 4.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 6.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 5.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5 Steve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 5.6</t>
   </si>
   <si>
     <t xml:space="preserve">2022 2.5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 6 Jared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5 AlanP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 6.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 4.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4 Steve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 2.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 4.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 3.5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 5.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5 Steve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 2.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5 MikeR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 5.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 3.10 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 2.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 6.5</t>
   </si>
   <si>
     <t xml:space="preserve">2022 2.10</t>
@@ -2307,6 +2310,15 @@
   <si>
     <t xml:space="preserve">Nick bosa</t>
   </si>
+  <si>
+    <t xml:space="preserve">MattH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 3.5</t>
+  </si>
 </sst>
 </file>
 
@@ -2315,7 +2327,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2348,6 +2360,15 @@
     </font>
     <font>
       <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -2484,7 +2505,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2593,6 +2614,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2673,8 +2710,8 @@
   </sheetPr>
   <dimension ref="A1:V87"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4862,10 +4899,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T63"/>
+  <dimension ref="A1:T67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5034,13 +5071,13 @@
       <c r="C5" s="0" t="s">
         <v>468</v>
       </c>
+      <c r="E5" s="0" t="s">
+        <v>469</v>
+      </c>
       <c r="F5" s="0" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>470</v>
-      </c>
-      <c r="J5" s="0" t="s">
         <v>471</v>
       </c>
       <c r="L5" s="0" t="s">
@@ -5069,13 +5106,13 @@
       <c r="F6" s="0" t="s">
         <v>479</v>
       </c>
+      <c r="I6" s="0" t="s">
+        <v>480</v>
+      </c>
       <c r="J6" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="M6" s="0" t="s">
         <v>482</v>
       </c>
       <c r="O6" s="0" t="s">
@@ -5101,397 +5138,396 @@
       <c r="J7" s="0" t="s">
         <v>489</v>
       </c>
+      <c r="L7" s="0" t="s">
+        <v>490</v>
+      </c>
       <c r="R7" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F9" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F10" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F11" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F12" s="0" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F13" s="0" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F14" s="0" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="0" t="s">
+        <v>502</v>
+      </c>
+    </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="E16" s="3" t="s">
-        <v>501</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="I16" s="3" t="s">
-        <v>502</v>
-      </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="M16" s="3" t="s">
+      <c r="F16" s="0" t="s">
         <v>503</v>
       </c>
-      <c r="N16" s="3"/>
-      <c r="P16" s="3" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F17" s="0" t="s">
         <v>504</v>
-      </c>
-      <c r="Q16" s="3"/>
-      <c r="S16" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="T16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
-        <v>506</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>507</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>508</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>509</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>510</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>511</v>
-      </c>
-      <c r="M17" s="0" t="s">
-        <v>512</v>
-      </c>
-      <c r="N17" s="0" t="s">
-        <v>513</v>
-      </c>
-      <c r="P17" s="0" t="s">
-        <v>514</v>
-      </c>
-      <c r="Q17" s="0" t="s">
-        <v>515</v>
-      </c>
-      <c r="S17" s="0" t="s">
-        <v>516</v>
-      </c>
-      <c r="T17" s="0" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>518</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>519</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>520</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>521</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>522</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>523</v>
-      </c>
-      <c r="M18" s="0" t="s">
-        <v>524</v>
-      </c>
-      <c r="N18" s="0" t="s">
-        <v>525</v>
-      </c>
-      <c r="P18" s="0" t="s">
-        <v>526</v>
-      </c>
-      <c r="Q18" s="0" t="s">
-        <v>527</v>
-      </c>
-      <c r="S18" s="0" t="s">
-        <v>528</v>
-      </c>
-      <c r="T18" s="0" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="s">
-        <v>530</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>531</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>532</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>533</v>
-      </c>
-      <c r="M19" s="0" t="s">
-        <v>534</v>
-      </c>
-      <c r="P19" s="0" t="s">
-        <v>535</v>
-      </c>
-      <c r="Q19" s="0" t="s">
-        <v>536</v>
-      </c>
-      <c r="S19" s="0" t="s">
-        <v>537</v>
-      </c>
-    </row>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
-        <v>538</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>539</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>540</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>541</v>
-      </c>
-      <c r="K20" s="0" t="s">
-        <v>542</v>
-      </c>
-      <c r="M20" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="P20" s="0" t="s">
-        <v>544</v>
-      </c>
-      <c r="Q20" s="0" t="s">
-        <v>545</v>
-      </c>
-      <c r="S20" s="0" t="s">
-        <v>546</v>
-      </c>
+      <c r="A20" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="E20" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="I20" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="M20" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="N20" s="3"/>
+      <c r="P20" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="Q20" s="3"/>
+      <c r="S20" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="T20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>547</v>
+        <v>511</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>512</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>548</v>
+        <v>513</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="K21" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>517</v>
+      </c>
+      <c r="N21" s="0" t="s">
+        <v>518</v>
       </c>
       <c r="P21" s="0" t="s">
-        <v>549</v>
+        <v>519</v>
       </c>
       <c r="Q21" s="0" t="s">
-        <v>550</v>
+        <v>520</v>
       </c>
       <c r="S21" s="0" t="s">
-        <v>551</v>
+        <v>521</v>
       </c>
       <c r="T21" s="0" t="s">
-        <v>552</v>
+        <v>522</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>528</v>
+      </c>
+      <c r="N22" s="0" t="s">
+        <v>529</v>
+      </c>
+      <c r="P22" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="Q22" s="0" t="s">
+        <v>531</v>
+      </c>
+      <c r="S22" s="0" t="s">
+        <v>532</v>
+      </c>
+      <c r="T22" s="0" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
+        <v>534</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>535</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>537</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="P23" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="Q23" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="S23" s="0" t="s">
+        <v>541</v>
+      </c>
+      <c r="T23" s="0" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="s">
+        <v>543</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>545</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>546</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="P24" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="Q24" s="0" t="s">
+        <v>549</v>
+      </c>
+      <c r="S24" s="0" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>551</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>552</v>
+      </c>
+      <c r="P25" s="0" t="s">
         <v>553</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="Q25" s="0" t="s">
         <v>554</v>
       </c>
-      <c r="S22" s="0" t="s">
+      <c r="S25" s="0" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E23" s="0" t="s">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
         <v>556</v>
       </c>
-      <c r="S23" s="0" t="s">
+      <c r="S26" s="0" t="s">
         <v>557</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S24" s="0" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S25" s="0" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S26" s="0" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S27" s="0" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S28" s="0" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S29" s="0" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S30" s="0" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="15"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="15"/>
-    </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="15"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="15"/>
-    </row>
+      <c r="S31" s="0" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="15"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="15"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="15"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="15"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
         <v>562</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="C37" s="15" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
+      <c r="D37" s="0" t="s">
         <v>564</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
-        <v>568</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
-        <v>578</v>
+      <c r="B41" s="15" t="s">
+        <v>571</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="15" t="s">
-        <v>580</v>
+      <c r="B42" s="0" t="s">
+        <v>573</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
+        <v>577</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="s">
+        <v>579</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="15" t="s">
+        <v>581</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0" t="s">
+        <v>583</v>
+      </c>
+      <c r="C47" s="15" t="s">
         <v>584</v>
       </c>
-      <c r="C44" s="15" t="s">
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
+      <c r="C48" s="15" t="s">
+        <v>586</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="15"/>
@@ -5516,9 +5552,6 @@
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
-      <c r="L54" s="0" t="n">
-        <v>12</v>
-      </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="15"/>
@@ -5533,14 +5566,33 @@
       <c r="C57" s="15"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="16"/>
+      <c r="B58" s="15"/>
       <c r="C58" s="15"/>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="L58" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="15"/>
+      <c r="C60" s="15"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="15"/>
+      <c r="C61" s="15"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="16"/>
+      <c r="C62" s="15"/>
+    </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A1:C1"/>
@@ -5549,12 +5601,12 @@
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="R1:S1"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="S20:T20"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5588,151 +5640,151 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>597</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>598</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>599</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>596</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>597</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>598</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5777,10 +5829,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A215" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D239" activeCellId="0" sqref="D239"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A228" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D253" activeCellId="0" sqref="D253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5792,46 +5844,46 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20"/>
       <c r="B2" s="21" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22"/>
       <c r="B3" s="21" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20"/>
       <c r="B4" s="21" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="22"/>
       <c r="B5" s="21" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="22"/>
       <c r="B6" s="21" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="20"/>
       <c r="B7" s="21" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5840,40 +5892,40 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22"/>
       <c r="B10" s="21" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="20"/>
       <c r="B11" s="21" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22"/>
       <c r="B12" s="21" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="20"/>
       <c r="B13" s="21" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="23"/>
       <c r="B14" s="24" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5881,42 +5933,42 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="22"/>
       <c r="B17" s="21" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="20"/>
       <c r="B18" s="21" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="20"/>
       <c r="B20" s="21" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="23"/>
       <c r="B21" s="24" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5924,16 +5976,16 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="22"/>
       <c r="B24" s="21" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5945,19 +5997,19 @@
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="22"/>
       <c r="B26" s="21" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="22"/>
       <c r="B27" s="21" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="22"/>
       <c r="B28" s="21" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5966,46 +6018,46 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="22"/>
       <c r="B31" s="21" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="20"/>
       <c r="B32" s="21" t="s">
-        <v>520</v>
+        <v>536</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22"/>
       <c r="B33" s="21" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="20"/>
       <c r="B34" s="21" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="22"/>
       <c r="B35" s="21" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="23"/>
       <c r="B36" s="24" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6014,34 +6066,34 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="18" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="20"/>
       <c r="B40" s="21" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22"/>
       <c r="B41" s="21" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="20"/>
       <c r="B42" s="21" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="22"/>
       <c r="B43" s="21" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6050,10 +6102,10 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="22" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6065,19 +6117,19 @@
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22"/>
       <c r="B47" s="21" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="20"/>
       <c r="B48" s="21" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="23"/>
       <c r="B49" s="24" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6086,22 +6138,22 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="18" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="20"/>
       <c r="B52" s="21" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="22"/>
       <c r="B53" s="21" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6112,16 +6164,16 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="20" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="23"/>
       <c r="B56" s="24" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6133,30 +6185,30 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="18" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="22"/>
       <c r="B60" s="21" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="20"/>
       <c r="B61" s="21" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="23" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6168,86 +6220,86 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="18" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="22"/>
       <c r="B66" s="21" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="22"/>
       <c r="B67" s="21" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="22"/>
       <c r="B68" s="21" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="22"/>
       <c r="B69" s="21" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="22"/>
       <c r="B70" s="21" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="22"/>
       <c r="B71" s="21" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="22" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="23"/>
       <c r="B73" s="24" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="25"/>
       <c r="B75" s="19" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="18" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="20"/>
       <c r="B77" s="21" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="20"/>
       <c r="B78" s="21" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6260,40 +6312,40 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="20" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B81" s="21" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="20"/>
       <c r="B82" s="21" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="20"/>
       <c r="B83" s="21" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="20"/>
       <c r="B84" s="21" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="20"/>
       <c r="B85" s="21" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="20"/>
       <c r="B86" s="21" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6308,7 +6360,7 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="20" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="B89" s="21" t="s">
         <v>479</v>
@@ -6317,25 +6369,25 @@
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="20"/>
       <c r="B90" s="21" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="20"/>
       <c r="B91" s="21" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="20"/>
       <c r="B92" s="21" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="20"/>
       <c r="B93" s="21" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6350,22 +6402,22 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="20" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B96" s="21" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="20"/>
       <c r="B97" s="21" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="20"/>
       <c r="B98" s="21" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6374,28 +6426,28 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="20" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="B100" s="21" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="20"/>
       <c r="B101" s="21" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="20"/>
       <c r="B102" s="21" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="20"/>
       <c r="B103" s="21" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6404,7 +6456,7 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="20" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B105" s="21" t="s">
         <v>479</v>
@@ -6413,7 +6465,7 @@
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="20"/>
       <c r="B106" s="21" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6424,93 +6476,93 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="25" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B109" s="19" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="22"/>
       <c r="B110" s="21" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="22"/>
       <c r="B111" s="21" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="F111" s="26"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="22"/>
       <c r="B112" s="21" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="23" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B113" s="24" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="25" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B115" s="19" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="22"/>
       <c r="B116" s="21" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="22"/>
       <c r="B117" s="21" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="22" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B118" s="21" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="22"/>
       <c r="B119" s="21" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="23"/>
       <c r="B120" s="24" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="25" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B122" s="19" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="23" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B123" s="24" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6521,42 +6573,42 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="25" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B126" s="19" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="22"/>
       <c r="B127" s="21" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="22"/>
       <c r="B128" s="21" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="22"/>
       <c r="B129" s="21" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="22"/>
       <c r="B130" s="21" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="23" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B131" s="24" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6564,317 +6616,317 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="25" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B133" s="19" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="22" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B134" s="21" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="23"/>
       <c r="B135" s="24" t="s">
-        <v>509</v>
+        <v>497</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="25" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B137" s="19" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="22"/>
       <c r="B138" s="21" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="22"/>
       <c r="B139" s="21" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="23" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B140" s="24" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="25" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B142" s="19" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="23" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B143" s="24" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="25" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B145" s="19" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="22"/>
       <c r="B146" s="21" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="22"/>
       <c r="B147" s="21" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="23" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B148" s="24" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="25" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B150" s="19" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="22"/>
       <c r="B151" s="21" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="22" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B152" s="21" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="23"/>
       <c r="B153" s="24" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="25" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B155" s="19" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="22"/>
       <c r="B156" s="21" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="22"/>
       <c r="B157" s="21" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="22" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B158" s="21" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="22"/>
       <c r="B159" s="21" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="23"/>
       <c r="B160" s="24" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="25" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B162" s="19" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="22"/>
       <c r="B163" s="21" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="23" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="B164" s="24" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="25" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B166" s="19" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="22"/>
       <c r="B167" s="21" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="22"/>
       <c r="B168" s="21" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="F168" s="26"/>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="22"/>
       <c r="B169" s="21" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="22"/>
       <c r="B170" s="21" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="22"/>
       <c r="B171" s="21" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="22" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B172" s="21" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="22"/>
       <c r="B173" s="21" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="22"/>
       <c r="B174" s="21" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="22"/>
       <c r="B175" s="21" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="22"/>
       <c r="B176" s="21" t="s">
-        <v>509</v>
+        <v>497</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="23"/>
       <c r="B177" s="24" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="18" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B179" s="19" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="22"/>
       <c r="B180" s="21" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="22"/>
       <c r="B181" s="21" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="22"/>
       <c r="B182" s="21" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="22" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B183" s="21" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="23"/>
       <c r="B184" s="24" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="25" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B186" s="19" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="22"/>
       <c r="B187" s="21" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6885,22 +6937,22 @@
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="22" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B189" s="21" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="22"/>
       <c r="B190" s="21" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="23"/>
       <c r="B191" s="24" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6911,10 +6963,10 @@
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="25" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B194" s="19" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6925,140 +6977,140 @@
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="23" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B196" s="24" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="25" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B198" s="19" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="22"/>
       <c r="B199" s="21" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="22" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B200" s="21" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="22"/>
       <c r="B201" s="21" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="22"/>
       <c r="B202" s="21" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="23"/>
       <c r="B203" s="24" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="25" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B205" s="19" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="22"/>
       <c r="B206" s="21" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="23" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B207" s="24" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="25" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B209" s="19" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="22"/>
       <c r="B210" s="21" t="s">
-        <v>458</v>
+        <v>525</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="22"/>
       <c r="B211" s="21" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="22" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B212" s="21" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="22"/>
       <c r="B213" s="21" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="23"/>
       <c r="B214" s="24" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="25" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B216" s="19" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="22"/>
       <c r="B217" s="21" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="22"/>
       <c r="B218" s="21" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="22" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B219" s="21" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7070,82 +7122,82 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="25" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B222" s="19" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="23" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B223" s="24" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="E223" s="26"/>
       <c r="F223" s="26"/>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="25" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B225" s="19" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="22" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B226" s="21" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="23"/>
       <c r="B227" s="24" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="25" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B229" s="19" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="22"/>
       <c r="B230" s="21" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="22"/>
       <c r="B231" s="21" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="22"/>
       <c r="B232" s="21" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="22"/>
       <c r="B233" s="21" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="22" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B234" s="21" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7162,29 +7214,29 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="25" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B238" s="19" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="22" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B239" s="21" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="23"/>
       <c r="B240" s="24" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="25" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B242" s="19" t="s">
         <v>437</v>
@@ -7193,44 +7245,223 @@
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="22"/>
       <c r="B243" s="21" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="22" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B244" s="21" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="23"/>
       <c r="B245" s="24" t="s">
-        <v>750</v>
-      </c>
-    </row>
+        <v>751</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="25" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B247" s="19" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="22" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B248" s="21" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="23"/>
       <c r="B249" s="24" t="s">
-        <v>653</v>
-      </c>
+        <v>654</v>
+      </c>
+      <c r="F249" s="27"/>
+      <c r="G249" s="0"/>
+    </row>
+    <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F250" s="27"/>
+      <c r="G250" s="0"/>
+    </row>
+    <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="25" t="s">
+        <v>572</v>
+      </c>
+      <c r="B251" s="19" t="s">
+        <v>746</v>
+      </c>
+      <c r="F251" s="27"/>
+      <c r="G251" s="0"/>
+    </row>
+    <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="23" t="s">
+        <v>733</v>
+      </c>
+      <c r="B252" s="24" t="s">
+        <v>522</v>
+      </c>
+      <c r="F252" s="27"/>
+      <c r="G252" s="0"/>
+    </row>
+    <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F253" s="27"/>
+      <c r="G253" s="0"/>
+    </row>
+    <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="28" t="s">
+        <v>572</v>
+      </c>
+      <c r="B254" s="29" t="s">
+        <v>741</v>
+      </c>
+      <c r="F254" s="0"/>
+      <c r="G254" s="0"/>
+    </row>
+    <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="22"/>
+      <c r="B255" s="21" t="s">
+        <v>522</v>
+      </c>
+      <c r="F255" s="0"/>
+      <c r="G255" s="0"/>
+    </row>
+    <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="B256" s="21" t="s">
+        <v>451</v>
+      </c>
+      <c r="F256" s="0"/>
+      <c r="G256" s="0"/>
+    </row>
+    <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="23"/>
+      <c r="B257" s="24" t="s">
+        <v>710</v>
+      </c>
+      <c r="F257" s="0"/>
+      <c r="G257" s="0"/>
+    </row>
+    <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F258" s="0"/>
+      <c r="G258" s="0"/>
+    </row>
+    <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="0"/>
+      <c r="B259" s="0"/>
+      <c r="F259" s="0"/>
+      <c r="G259" s="0"/>
+    </row>
+    <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="18" t="s">
+        <v>572</v>
+      </c>
+      <c r="B260" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="F260" s="0"/>
+      <c r="G260" s="0"/>
+    </row>
+    <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="30" t="s">
+        <v>752</v>
+      </c>
+      <c r="B261" s="24" t="s">
+        <v>499</v>
+      </c>
+      <c r="F261" s="0"/>
+      <c r="G261" s="0"/>
+    </row>
+    <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="0"/>
+      <c r="B262" s="0"/>
+      <c r="F262" s="0"/>
+      <c r="G262" s="0"/>
+    </row>
+    <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="25" t="s">
+        <v>753</v>
+      </c>
+      <c r="B263" s="19" t="s">
+        <v>750</v>
+      </c>
+      <c r="F263" s="27"/>
+      <c r="G263" s="0"/>
+    </row>
+    <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="22"/>
+      <c r="B264" s="21" t="s">
+        <v>525</v>
+      </c>
+      <c r="F264" s="27"/>
+      <c r="G264" s="0"/>
+    </row>
+    <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="22" t="s">
+        <v>572</v>
+      </c>
+      <c r="B265" s="21" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="22"/>
+      <c r="B266" s="21" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="22"/>
+      <c r="B267" s="21" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="22"/>
+      <c r="B268" s="21" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="22"/>
+      <c r="B269" s="21" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="23"/>
+      <c r="B270" s="24" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="0"/>
+      <c r="B271" s="0"/>
+    </row>
+    <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="0"/>
+      <c r="B272" s="0"/>
+    </row>
+    <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="0"/>
+      <c r="B273" s="0"/>
+    </row>
+    <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="0"/>
+      <c r="B274" s="0"/>
+    </row>
+    <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="0"/>
+      <c r="B275" s="0"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
Trades needed post draft
</commit_message>
<xml_diff>
--- a/OffSeason.xlsx
+++ b/OffSeason.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Rosters" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Picks" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Managers" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Off-Season Trades" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Post Draft trades" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="806">
   <si>
     <t xml:space="preserve">Kupp My Footballs – Vanja Dolas </t>
   </si>
@@ -1789,6 +1790,9 @@
     <t xml:space="preserve">MikeR</t>
   </si>
   <si>
+    <t xml:space="preserve">End 26</t>
+  </si>
+  <si>
     <t xml:space="preserve">12) </t>
   </si>
   <si>
@@ -1798,7 +1802,16 @@
     <t xml:space="preserve">Holland</t>
   </si>
   <si>
+    <t xml:space="preserve">End 27</t>
+  </si>
+  <si>
     <t xml:space="preserve">AdamW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End 28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End 29</t>
   </si>
   <si>
     <t xml:space="preserve">← not needed anymore</t>
@@ -2352,6 +2365,150 @@
   <si>
     <t xml:space="preserve">2023 2 Ben</t>
   </si>
+  <si>
+    <t xml:space="preserve">Trades</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Vanja </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2023 3 vanja</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Alan </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2023 3 alan</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanja 2023 1 vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John 2023 3 John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanja 2023 2 vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John 2023 4 JohnO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanja 2023 late pick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam 2023 4 adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jared 2023 Jared 4th</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John late pick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jared 2023 1 Jared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MikeR 2023 1 Mike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MikeR 2023 2 Mike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MikeR 2023 3 Mike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam 2023 1 Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam 2023 2 adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam 2023 3 adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alan 2023 1 alan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alan 2023 2 Alan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrew 2023 1 Andrew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matt 2023 1 Matt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matt 2023 2 matt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JoeB 2023 3 Joe/Luke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ben 2023 2 BenL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steve 2023 1 Steve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ben Late pick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steve 2023 2 Steve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jared 2023 2 Jared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alan late pick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MikeR 2023 4 Mike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jared 2023 5 Jared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam late pick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jared 2023 3 Jared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MikeR late pick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BenL2023 3 BenL</t>
+  </si>
 </sst>
 </file>
 
@@ -2361,7 +2518,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2394,9 +2551,10 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF00A933"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
@@ -2414,6 +2572,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -2628,11 +2792,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2768,8 +2932,8 @@
   </sheetPr>
   <dimension ref="A1:AA105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C61" activeCellId="0" sqref="C61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B27" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G48" activeCellId="0" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6057,8 +6221,8 @@
   </sheetPr>
   <dimension ref="A1:T134"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I99" activeCellId="0" sqref="I99"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T23" activeCellId="0" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6116,13 +6280,13 @@
       <c r="B2" s="18" t="s">
         <v>478</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="19" t="s">
         <v>479</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="19" t="s">
         <v>480</v>
       </c>
       <c r="I2" s="0" t="s">
@@ -6148,19 +6312,19 @@
       <c r="B3" s="18" t="s">
         <v>483</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="19" t="s">
         <v>484</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="19" t="s">
         <v>485</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="19" t="s">
         <v>486</v>
       </c>
       <c r="L3" s="0" t="s">
@@ -6183,19 +6347,19 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="19" t="s">
         <v>490</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="19" t="s">
         <v>491</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" s="19" t="s">
         <v>492</v>
       </c>
       <c r="L4" s="0" t="s">
@@ -6218,7 +6382,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="19" t="s">
         <v>497</v>
       </c>
       <c r="E5" s="18" t="s">
@@ -6230,7 +6394,7 @@
       <c r="I5" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="J5" s="19" t="s">
         <v>500</v>
       </c>
       <c r="L5" s="0" t="s">
@@ -6253,10 +6417,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="19" t="s">
         <v>504</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="19" t="s">
         <v>505</v>
       </c>
       <c r="I6" s="0" t="s">
@@ -6282,10 +6446,10 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="19" t="s">
         <v>510</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="19" t="s">
         <v>511</v>
       </c>
       <c r="J7" s="0" t="s">
@@ -6302,10 +6466,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="19" t="s">
         <v>516</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="19" t="s">
         <v>517</v>
       </c>
       <c r="L8" s="18" t="s">
@@ -6316,7 +6480,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="19" t="s">
         <v>520</v>
       </c>
       <c r="R9" s="18" t="s">
@@ -6324,27 +6488,27 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="19" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="19" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="19" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="19" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="19" t="s">
         <v>526</v>
       </c>
     </row>
@@ -6354,17 +6518,17 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="19" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="0" t="s">
+      <c r="F17" s="19" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="19" t="s">
         <v>530</v>
       </c>
     </row>
@@ -6424,7 +6588,7 @@
       <c r="J23" s="18" t="s">
         <v>540</v>
       </c>
-      <c r="K23" s="0" t="s">
+      <c r="K23" s="19" t="s">
         <v>541</v>
       </c>
       <c r="M23" s="0" t="s">
@@ -6436,13 +6600,13 @@
       <c r="P23" s="0" t="s">
         <v>407</v>
       </c>
-      <c r="Q23" s="0" t="s">
+      <c r="Q23" s="19" t="s">
         <v>543</v>
       </c>
       <c r="S23" s="0" t="s">
         <v>408</v>
       </c>
-      <c r="T23" s="0" t="s">
+      <c r="T23" s="19" t="s">
         <v>544</v>
       </c>
     </row>
@@ -6465,7 +6629,7 @@
       <c r="M24" s="0" t="s">
         <v>419</v>
       </c>
-      <c r="N24" s="0" t="s">
+      <c r="N24" s="19" t="s">
         <v>548</v>
       </c>
       <c r="P24" s="0" t="s">
@@ -6477,7 +6641,7 @@
       <c r="S24" s="0" t="s">
         <v>414</v>
       </c>
-      <c r="T24" s="0" t="s">
+      <c r="T24" s="19" t="s">
         <v>550</v>
       </c>
     </row>
@@ -6601,22 +6765,22 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="19"/>
+      <c r="C35" s="20"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="19"/>
+      <c r="C36" s="20"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="19"/>
+      <c r="C37" s="20"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="19"/>
+      <c r="C38" s="20"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
         <v>561</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="C39" s="20" t="s">
         <v>562</v>
       </c>
       <c r="D39" s="0" t="s">
@@ -6627,7 +6791,7 @@
       <c r="B40" s="0" t="s">
         <v>564</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="C40" s="20" t="s">
         <v>565</v>
       </c>
     </row>
@@ -6635,7 +6799,7 @@
       <c r="B41" s="0" t="s">
         <v>566</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="20" t="s">
         <v>567</v>
       </c>
     </row>
@@ -6643,21 +6807,21 @@
       <c r="B42" s="0" t="s">
         <v>568</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C42" s="20" t="s">
         <v>569</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="20" t="s">
         <v>570</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C43" s="20" t="s">
         <v>571</v>
       </c>
       <c r="G43" s="0" t="s">
         <v>572</v>
       </c>
-      <c r="H43" s="20" t="s">
+      <c r="H43" s="5" t="s">
         <v>573</v>
       </c>
     </row>
@@ -6665,7 +6829,7 @@
       <c r="B44" s="0" t="s">
         <v>574</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="C44" s="20" t="s">
         <v>575</v>
       </c>
       <c r="G44" s="0" t="n">
@@ -6679,7 +6843,7 @@
       <c r="B45" s="0" t="s">
         <v>577</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C45" s="20" t="s">
         <v>578</v>
       </c>
       <c r="G45" s="0" t="n">
@@ -6693,7 +6857,7 @@
       <c r="B46" s="0" t="s">
         <v>579</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C46" s="20" t="s">
         <v>580</v>
       </c>
       <c r="G46" s="0" t="n">
@@ -6707,7 +6871,7 @@
       <c r="B47" s="0" t="s">
         <v>582</v>
       </c>
-      <c r="C47" s="19" t="s">
+      <c r="C47" s="20" t="s">
         <v>583</v>
       </c>
       <c r="G47" s="0" t="n">
@@ -6718,10 +6882,10 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="19" t="s">
+      <c r="B48" s="20" t="s">
         <v>584</v>
       </c>
-      <c r="C48" s="19" t="s">
+      <c r="C48" s="20" t="s">
         <v>581</v>
       </c>
       <c r="G48" s="0" t="n">
@@ -6735,7 +6899,7 @@
       <c r="B49" s="0" t="s">
         <v>585</v>
       </c>
-      <c r="C49" s="19" t="s">
+      <c r="C49" s="20" t="s">
         <v>586</v>
       </c>
       <c r="G49" s="0" t="n">
@@ -6744,13 +6908,16 @@
       <c r="H49" s="0" t="s">
         <v>587</v>
       </c>
+      <c r="I49" s="0" t="s">
+        <v>588</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>588</v>
-      </c>
-      <c r="C50" s="19" t="s">
         <v>589</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>590</v>
       </c>
       <c r="G50" s="0" t="n">
         <v>1.7</v>
@@ -6760,8 +6927,8 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
       <c r="G51" s="0" t="n">
         <v>1.8</v>
       </c>
@@ -6770,18 +6937,18 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
       <c r="G52" s="0" t="n">
         <v>1.9</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="19"/>
-      <c r="C53" s="19"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
       <c r="G53" s="21" t="n">
         <v>1.1</v>
       </c>
@@ -6790,18 +6957,18 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
       <c r="G54" s="0" t="n">
         <v>1.11</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="19"/>
-      <c r="C55" s="19"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
       <c r="G55" s="0" t="n">
         <v>1.12</v>
       </c>
@@ -6810,8 +6977,8 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="19"/>
-      <c r="C56" s="19"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
       <c r="G56" s="0" t="n">
         <v>2.1</v>
       </c>
@@ -6820,8 +6987,8 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="19"/>
-      <c r="C57" s="19"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
       <c r="G57" s="0" t="n">
         <v>2.2</v>
       </c>
@@ -6830,8 +6997,8 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="19"/>
-      <c r="C58" s="19"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="20"/>
       <c r="G58" s="0" t="n">
         <v>2.3</v>
       </c>
@@ -6840,8 +7007,8 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="19"/>
-      <c r="C59" s="19"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="20"/>
       <c r="G59" s="0" t="n">
         <v>2.4</v>
       </c>
@@ -6850,8 +7017,8 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="19"/>
-      <c r="C60" s="19"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="20"/>
       <c r="G60" s="0" t="n">
         <v>2.5</v>
       </c>
@@ -6860,18 +7027,21 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="19"/>
-      <c r="C61" s="19"/>
+      <c r="B61" s="20"/>
+      <c r="C61" s="20"/>
       <c r="G61" s="0" t="n">
         <v>2.6</v>
       </c>
       <c r="H61" s="0" t="s">
         <v>571</v>
       </c>
+      <c r="I61" s="0" t="s">
+        <v>592</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="19"/>
-      <c r="C62" s="19"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="20"/>
       <c r="G62" s="0" t="n">
         <v>2.7</v>
       </c>
@@ -6880,23 +7050,23 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="19"/>
-      <c r="C63" s="19"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="20"/>
       <c r="G63" s="0" t="n">
         <v>2.8</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="22"/>
-      <c r="C64" s="19"/>
+      <c r="C64" s="20"/>
       <c r="G64" s="0" t="n">
         <v>2.9</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6952,7 +7122,7 @@
         <v>3.4</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6968,7 +7138,10 @@
         <v>3.6</v>
       </c>
       <c r="H73" s="0" t="s">
-        <v>591</v>
+        <v>593</v>
+      </c>
+      <c r="I73" s="0" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6984,7 +7157,7 @@
         <v>3.8</v>
       </c>
       <c r="H75" s="0" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7000,7 +7173,7 @@
         <v>3.1</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7008,7 +7181,7 @@
         <v>3.11</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7066,6 +7239,9 @@
       <c r="H85" s="0" t="s">
         <v>565</v>
       </c>
+      <c r="I85" s="0" t="s">
+        <v>595</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G86" s="0" t="n">
@@ -7104,7 +7280,7 @@
         <v>4.11</v>
       </c>
       <c r="H90" s="0" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7168,7 +7344,7 @@
         <v>5.7</v>
       </c>
       <c r="I98" s="0" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7394,151 +7570,151 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>607</v>
+        <v>611</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>608</v>
+        <v>612</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>611</v>
+        <v>615</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>613</v>
+        <v>617</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>615</v>
+        <v>619</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>622</v>
+        <v>626</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>625</v>
+        <v>629</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7598,46 +7774,46 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>632</v>
+        <v>636</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26"/>
       <c r="B2" s="27" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="28"/>
       <c r="B3" s="27" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26"/>
       <c r="B4" s="27" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="28"/>
       <c r="B5" s="27" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="28"/>
       <c r="B6" s="27" t="s">
-        <v>637</v>
+        <v>641</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26"/>
       <c r="B7" s="27" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7649,60 +7825,60 @@
         <v>571</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="28"/>
       <c r="B10" s="27" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="26"/>
       <c r="B11" s="27" t="s">
-        <v>641</v>
+        <v>645</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="28"/>
       <c r="B12" s="27" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="26"/>
       <c r="B13" s="27" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="19"/>
+      <c r="B15" s="20"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="24" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="28"/>
       <c r="B17" s="27" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="26"/>
       <c r="B18" s="27" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7710,36 +7886,36 @@
         <v>586</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>648</v>
+        <v>652</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="26"/>
       <c r="B20" s="27" t="s">
-        <v>649</v>
+        <v>653</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="29"/>
       <c r="B21" s="30" t="s">
-        <v>650</v>
+        <v>654</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="19"/>
+      <c r="B22" s="20"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="s">
         <v>587</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>651</v>
+        <v>655</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="28"/>
       <c r="B24" s="27" t="s">
-        <v>652</v>
+        <v>656</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7763,7 +7939,7 @@
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="28"/>
       <c r="B28" s="27" t="s">
-        <v>653</v>
+        <v>657</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7775,7 +7951,7 @@
         <v>576</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>654</v>
+        <v>658</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7793,29 +7969,29 @@
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="28"/>
       <c r="B33" s="27" t="s">
-        <v>655</v>
+        <v>659</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="26"/>
       <c r="B34" s="27" t="s">
-        <v>656</v>
+        <v>660</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="28"/>
       <c r="B35" s="27" t="s">
-        <v>657</v>
+        <v>661</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="29"/>
       <c r="B36" s="30" t="s">
-        <v>658</v>
+        <v>662</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="19"/>
+      <c r="A37" s="20"/>
       <c r="B37" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7823,31 +7999,31 @@
         <v>586</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="26"/>
       <c r="B40" s="27" t="s">
-        <v>660</v>
+        <v>664</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="28"/>
       <c r="B41" s="27" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="26"/>
       <c r="B42" s="27" t="s">
-        <v>662</v>
+        <v>666</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="28"/>
       <c r="B43" s="27" t="s">
-        <v>663</v>
+        <v>667</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7859,7 +8035,7 @@
         <v>571</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>664</v>
+        <v>668</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7871,43 +8047,43 @@
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="28"/>
       <c r="B47" s="27" t="s">
-        <v>637</v>
+        <v>641</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="26"/>
       <c r="B48" s="27" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="29"/>
       <c r="B49" s="30" t="s">
-        <v>650</v>
+        <v>654</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="19"/>
-      <c r="B50" s="19"/>
+      <c r="A50" s="20"/>
+      <c r="B50" s="20"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="24" t="s">
-        <v>666</v>
+        <v>670</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>667</v>
+        <v>671</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="26"/>
       <c r="B52" s="27" t="s">
-        <v>668</v>
+        <v>672</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="28"/>
       <c r="B53" s="27" t="s">
-        <v>669</v>
+        <v>673</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7921,40 +8097,40 @@
         <v>569</v>
       </c>
       <c r="B55" s="27" t="s">
-        <v>670</v>
+        <v>674</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="29"/>
       <c r="B56" s="30" t="s">
-        <v>671</v>
+        <v>675</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="19"/>
-      <c r="B57" s="19"/>
+      <c r="A57" s="20"/>
+      <c r="B57" s="20"/>
     </row>
     <row r="58" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="19"/>
+      <c r="B58" s="20"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="24" t="s">
         <v>569</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>672</v>
+        <v>676</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="28"/>
       <c r="B60" s="27" t="s">
-        <v>673</v>
+        <v>677</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="26"/>
       <c r="B61" s="27" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7962,58 +8138,58 @@
         <v>575</v>
       </c>
       <c r="B62" s="30" t="s">
-        <v>675</v>
+        <v>679</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="19"/>
-      <c r="B63" s="19"/>
+      <c r="A63" s="20"/>
+      <c r="B63" s="20"/>
     </row>
     <row r="64" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="19"/>
+      <c r="B64" s="20"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="24" t="s">
         <v>571</v>
       </c>
       <c r="B65" s="25" t="s">
-        <v>676</v>
+        <v>680</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="28"/>
       <c r="B66" s="27" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="28"/>
       <c r="B67" s="27" t="s">
-        <v>678</v>
+        <v>682</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="28"/>
       <c r="B68" s="27" t="s">
-        <v>679</v>
+        <v>683</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="28"/>
       <c r="B69" s="27" t="s">
-        <v>680</v>
+        <v>684</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="28"/>
       <c r="B70" s="27" t="s">
-        <v>681</v>
+        <v>685</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="28"/>
       <c r="B71" s="27" t="s">
-        <v>682</v>
+        <v>686</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8021,39 +8197,39 @@
         <v>567</v>
       </c>
       <c r="B72" s="27" t="s">
-        <v>683</v>
+        <v>687</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="29"/>
       <c r="B73" s="30" t="s">
-        <v>684</v>
+        <v>688</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="31"/>
       <c r="B75" s="25" t="s">
-        <v>685</v>
+        <v>689</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="24" t="s">
-        <v>686</v>
+        <v>690</v>
       </c>
       <c r="B76" s="25" t="s">
-        <v>687</v>
+        <v>691</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="26"/>
       <c r="B77" s="27" t="s">
-        <v>688</v>
+        <v>692</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="26"/>
       <c r="B78" s="27" t="s">
-        <v>689</v>
+        <v>693</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8066,34 +8242,34 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="26" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
       <c r="B81" s="27" t="s">
-        <v>651</v>
+        <v>655</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="26"/>
       <c r="B82" s="27" t="s">
-        <v>691</v>
+        <v>695</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="26"/>
       <c r="B83" s="27" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="26"/>
       <c r="B84" s="27" t="s">
-        <v>693</v>
+        <v>697</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="26"/>
       <c r="B85" s="27" t="s">
-        <v>694</v>
+        <v>698</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8114,7 +8290,7 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="26" t="s">
-        <v>695</v>
+        <v>699</v>
       </c>
       <c r="B89" s="27" t="s">
         <v>505</v>
@@ -8123,19 +8299,19 @@
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="26"/>
       <c r="B90" s="27" t="s">
-        <v>691</v>
+        <v>695</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="26"/>
       <c r="B91" s="27" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="26"/>
       <c r="B92" s="27" t="s">
-        <v>694</v>
+        <v>698</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8156,22 +8332,22 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="26" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
       <c r="B96" s="27" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="26"/>
       <c r="B97" s="27" t="s">
-        <v>696</v>
+        <v>700</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="26"/>
       <c r="B98" s="27" t="s">
-        <v>687</v>
+        <v>691</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8180,28 +8356,28 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="26" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="B100" s="27" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="26"/>
       <c r="B101" s="27" t="s">
-        <v>698</v>
+        <v>702</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="26"/>
       <c r="B102" s="27" t="s">
-        <v>699</v>
+        <v>703</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="26"/>
       <c r="B103" s="27" t="s">
-        <v>700</v>
+        <v>704</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8210,7 +8386,7 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="26" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
       <c r="B105" s="27" t="s">
         <v>505</v>
@@ -8219,7 +8395,7 @@
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="26"/>
       <c r="B106" s="27" t="s">
-        <v>650</v>
+        <v>654</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8230,22 +8406,22 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="31" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B109" s="25" t="s">
-        <v>701</v>
+        <v>705</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="28"/>
       <c r="B110" s="27" t="s">
-        <v>702</v>
+        <v>706</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="28"/>
       <c r="B111" s="27" t="s">
-        <v>703</v>
+        <v>707</v>
       </c>
       <c r="F111" s="13"/>
     </row>
@@ -8268,19 +8444,19 @@
         <v>569</v>
       </c>
       <c r="B115" s="25" t="s">
-        <v>669</v>
+        <v>673</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="28"/>
       <c r="B116" s="27" t="s">
-        <v>704</v>
+        <v>708</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="28"/>
       <c r="B117" s="27" t="s">
-        <v>705</v>
+        <v>709</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8288,19 +8464,19 @@
         <v>587</v>
       </c>
       <c r="B118" s="27" t="s">
-        <v>706</v>
+        <v>710</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="28"/>
       <c r="B119" s="27" t="s">
-        <v>707</v>
+        <v>711</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="29"/>
       <c r="B120" s="30" t="s">
-        <v>708</v>
+        <v>712</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8308,7 +8484,7 @@
         <v>569</v>
       </c>
       <c r="B122" s="25" t="s">
-        <v>709</v>
+        <v>713</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8330,25 +8506,25 @@
         <v>571</v>
       </c>
       <c r="B126" s="25" t="s">
-        <v>710</v>
+        <v>714</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="28"/>
       <c r="B127" s="27" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="28"/>
       <c r="B128" s="27" t="s">
-        <v>712</v>
+        <v>716</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="28"/>
       <c r="B129" s="27" t="s">
-        <v>671</v>
+        <v>675</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8359,10 +8535,10 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="29" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B131" s="30" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8370,10 +8546,10 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="31" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B133" s="25" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8381,7 +8557,7 @@
         <v>586</v>
       </c>
       <c r="B134" s="27" t="s">
-        <v>714</v>
+        <v>718</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8395,7 +8571,7 @@
         <v>586</v>
       </c>
       <c r="B137" s="25" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8407,7 +8583,7 @@
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="28"/>
       <c r="B139" s="27" t="s">
-        <v>637</v>
+        <v>641</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8415,7 +8591,7 @@
         <v>567</v>
       </c>
       <c r="B140" s="30" t="s">
-        <v>679</v>
+        <v>683</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8423,7 +8599,7 @@
         <v>571</v>
       </c>
       <c r="B142" s="25" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8431,21 +8607,21 @@
         <v>567</v>
       </c>
       <c r="B143" s="30" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="31" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B145" s="25" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="28"/>
       <c r="B146" s="27" t="s">
-        <v>641</v>
+        <v>645</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8459,7 +8635,7 @@
         <v>587</v>
       </c>
       <c r="B148" s="30" t="s">
-        <v>715</v>
+        <v>719</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8467,13 +8643,13 @@
         <v>571</v>
       </c>
       <c r="B150" s="25" t="s">
-        <v>663</v>
+        <v>667</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="28"/>
       <c r="B151" s="27" t="s">
-        <v>716</v>
+        <v>720</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8487,21 +8663,21 @@
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="29"/>
       <c r="B153" s="30" t="s">
-        <v>702</v>
+        <v>706</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="31" t="s">
-        <v>666</v>
+        <v>670</v>
       </c>
       <c r="B155" s="25" t="s">
-        <v>717</v>
+        <v>721</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="28"/>
       <c r="B156" s="27" t="s">
-        <v>670</v>
+        <v>674</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8515,19 +8691,19 @@
         <v>586</v>
       </c>
       <c r="B158" s="27" t="s">
-        <v>718</v>
+        <v>722</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="28"/>
       <c r="B159" s="27" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="29"/>
       <c r="B160" s="30" t="s">
-        <v>720</v>
+        <v>724</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8535,21 +8711,21 @@
         <v>571</v>
       </c>
       <c r="B162" s="25" t="s">
-        <v>721</v>
+        <v>725</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="28"/>
       <c r="B163" s="27" t="s">
-        <v>722</v>
+        <v>726</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="29" t="s">
-        <v>723</v>
+        <v>727</v>
       </c>
       <c r="B164" s="30" t="s">
-        <v>724</v>
+        <v>728</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8557,64 +8733,64 @@
         <v>571</v>
       </c>
       <c r="B166" s="25" t="s">
-        <v>725</v>
+        <v>729</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="28"/>
       <c r="B167" s="27" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="28"/>
       <c r="B168" s="27" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="F168" s="13"/>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="28"/>
       <c r="B169" s="27" t="s">
-        <v>726</v>
+        <v>730</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="28"/>
       <c r="B170" s="27" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="28"/>
       <c r="B171" s="27" t="s">
-        <v>727</v>
+        <v>731</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="28" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B172" s="27" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="28"/>
       <c r="B173" s="27" t="s">
-        <v>728</v>
+        <v>732</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="28"/>
       <c r="B174" s="27" t="s">
-        <v>729</v>
+        <v>733</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="28"/>
       <c r="B175" s="27" t="s">
-        <v>730</v>
+        <v>734</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8631,28 +8807,28 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="24" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B179" s="25" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="28"/>
       <c r="B180" s="27" t="s">
-        <v>731</v>
+        <v>735</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="28"/>
       <c r="B181" s="27" t="s">
-        <v>732</v>
+        <v>736</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="28"/>
       <c r="B182" s="27" t="s">
-        <v>714</v>
+        <v>718</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8660,7 +8836,7 @@
         <v>587</v>
       </c>
       <c r="B183" s="27" t="s">
-        <v>733</v>
+        <v>737</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8671,10 +8847,10 @@
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="31" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B186" s="25" t="s">
-        <v>698</v>
+        <v>702</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8694,13 +8870,13 @@
         <v>571</v>
       </c>
       <c r="B189" s="27" t="s">
-        <v>734</v>
+        <v>738</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="28"/>
       <c r="B190" s="27" t="s">
-        <v>735</v>
+        <v>739</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8720,7 +8896,7 @@
         <v>569</v>
       </c>
       <c r="B194" s="25" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8731,10 +8907,10 @@
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="29" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
       <c r="B196" s="30" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8742,13 +8918,13 @@
         <v>571</v>
       </c>
       <c r="B198" s="25" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="28"/>
       <c r="B199" s="27" t="s">
-        <v>724</v>
+        <v>728</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8756,25 +8932,25 @@
         <v>569</v>
       </c>
       <c r="B200" s="27" t="s">
-        <v>739</v>
+        <v>743</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="28"/>
       <c r="B201" s="27" t="s">
-        <v>740</v>
+        <v>744</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="28"/>
       <c r="B202" s="27" t="s">
-        <v>741</v>
+        <v>745</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="29"/>
       <c r="B203" s="30" t="s">
-        <v>675</v>
+        <v>679</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8796,15 +8972,15 @@
         <v>586</v>
       </c>
       <c r="B207" s="30" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="31" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B209" s="25" t="s">
-        <v>743</v>
+        <v>747</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8824,19 +9000,19 @@
         <v>586</v>
       </c>
       <c r="B212" s="27" t="s">
-        <v>717</v>
+        <v>721</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="28"/>
       <c r="B213" s="27" t="s">
-        <v>744</v>
+        <v>748</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="29"/>
       <c r="B214" s="30" t="s">
-        <v>745</v>
+        <v>749</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8844,19 +9020,19 @@
         <v>571</v>
       </c>
       <c r="B216" s="25" t="s">
-        <v>728</v>
+        <v>732</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="28"/>
       <c r="B217" s="27" t="s">
-        <v>708</v>
+        <v>712</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="28"/>
       <c r="B218" s="27" t="s">
-        <v>741</v>
+        <v>745</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8879,15 +9055,15 @@
         <v>587</v>
       </c>
       <c r="B222" s="25" t="s">
-        <v>705</v>
+        <v>709</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="29" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B223" s="30" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="E223" s="13"/>
       <c r="F223" s="13"/>
@@ -8897,7 +9073,7 @@
         <v>569</v>
       </c>
       <c r="B225" s="25" t="s">
-        <v>746</v>
+        <v>750</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8905,7 +9081,7 @@
         <v>571</v>
       </c>
       <c r="B226" s="27" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8916,34 +9092,34 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="31" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B229" s="25" t="s">
-        <v>734</v>
+        <v>738</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="28"/>
       <c r="B230" s="27" t="s">
-        <v>748</v>
+        <v>752</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="28"/>
       <c r="B231" s="27" t="s">
-        <v>749</v>
+        <v>753</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="28"/>
       <c r="B232" s="27" t="s">
-        <v>750</v>
+        <v>754</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="28"/>
       <c r="B233" s="27" t="s">
-        <v>705</v>
+        <v>709</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8951,7 +9127,7 @@
         <v>571</v>
       </c>
       <c r="B234" s="27" t="s">
-        <v>698</v>
+        <v>702</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8971,7 +9147,7 @@
         <v>567</v>
       </c>
       <c r="B238" s="25" t="s">
-        <v>751</v>
+        <v>755</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8979,13 +9155,13 @@
         <v>569</v>
       </c>
       <c r="B239" s="27" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="29"/>
       <c r="B240" s="30" t="s">
-        <v>707</v>
+        <v>711</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8999,30 +9175,30 @@
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="28"/>
       <c r="B243" s="27" t="s">
-        <v>753</v>
+        <v>757</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="28" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
       <c r="B244" s="27" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="29"/>
       <c r="B245" s="30" t="s">
-        <v>755</v>
+        <v>759</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="31" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B247" s="25" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9030,13 +9206,13 @@
         <v>587</v>
       </c>
       <c r="B248" s="27" t="s">
-        <v>656</v>
+        <v>660</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="29"/>
       <c r="B249" s="30" t="s">
-        <v>658</v>
+        <v>662</v>
       </c>
       <c r="F249" s="32"/>
       <c r="G249" s="0"/>
@@ -9050,14 +9226,14 @@
         <v>571</v>
       </c>
       <c r="B251" s="25" t="s">
-        <v>750</v>
+        <v>754</v>
       </c>
       <c r="F251" s="32"/>
       <c r="G251" s="0"/>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="29" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
       <c r="B252" s="30" t="s">
         <v>544</v>
@@ -9074,7 +9250,7 @@
         <v>571</v>
       </c>
       <c r="B254" s="25" t="s">
-        <v>745</v>
+        <v>749</v>
       </c>
       <c r="F254" s="0"/>
       <c r="G254" s="0"/>
@@ -9100,7 +9276,7 @@
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="29"/>
       <c r="B257" s="30" t="s">
-        <v>714</v>
+        <v>718</v>
       </c>
       <c r="F257" s="0"/>
       <c r="G257" s="0"/>
@@ -9127,7 +9303,7 @@
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="33" t="s">
-        <v>756</v>
+        <v>760</v>
       </c>
       <c r="B261" s="30" t="s">
         <v>526</v>
@@ -9143,10 +9319,10 @@
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="31" t="s">
-        <v>757</v>
+        <v>761</v>
       </c>
       <c r="B263" s="25" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
       <c r="F263" s="32"/>
       <c r="G263" s="0"/>
@@ -9170,19 +9346,19 @@
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="28"/>
       <c r="B266" s="27" t="s">
-        <v>758</v>
+        <v>762</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="28"/>
       <c r="B267" s="27" t="s">
-        <v>705</v>
+        <v>709</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="28"/>
       <c r="B268" s="27" t="s">
-        <v>714</v>
+        <v>718</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9231,7 +9407,7 @@
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="29" t="s">
-        <v>756</v>
+        <v>760</v>
       </c>
       <c r="B276" s="30" t="s">
         <v>520</v>
@@ -9242,7 +9418,7 @@
         <v>571</v>
       </c>
       <c r="B278" s="25" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9250,7 +9426,7 @@
         <v>587</v>
       </c>
       <c r="B279" s="27" t="s">
-        <v>745</v>
+        <v>749</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9276,7 +9452,7 @@
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="28"/>
       <c r="B284" s="27" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9284,7 +9460,7 @@
         <v>586</v>
       </c>
       <c r="B285" s="30" t="s">
-        <v>759</v>
+        <v>763</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9303,40 +9479,40 @@
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="28" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
       <c r="B289" s="27" t="s">
-        <v>760</v>
+        <v>764</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="28"/>
       <c r="B290" s="27" t="s">
-        <v>761</v>
+        <v>765</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="28"/>
       <c r="B291" s="27" t="s">
-        <v>762</v>
+        <v>766</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="28"/>
       <c r="B292" s="27" t="s">
-        <v>763</v>
+        <v>767</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="28"/>
       <c r="B293" s="27" t="s">
-        <v>764</v>
+        <v>768</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="29"/>
       <c r="B294" s="30" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -9347,6 +9523,239 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.2"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>771</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>773</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>775</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>777</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>777</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>780</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>794</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>796</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>796</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>799</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>801</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>803</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>804</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>805</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
pick #'s and trade
John 	2023 2.1
Ben	        2023 2.4
	        2024 3 Ben
</commit_message>
<xml_diff>
--- a/OffSeason.xlsx
+++ b/OffSeason.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="657">
   <si>
     <t xml:space="preserve">Where’s your Kupp Now– Vanja Dolas </t>
   </si>
@@ -1346,42 +1346,42 @@
     <t xml:space="preserve">2024 1 John</t>
   </si>
   <si>
+    <t xml:space="preserve">2023 1.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 1 Vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 2 Ben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 1 Mike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 1 Joe/Luke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 3 Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 1 Adam</t>
+  </si>
+  <si>
     <t xml:space="preserve">2023 1.11</t>
   </si>
   <si>
-    <t xml:space="preserve">2024 1 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 2 Ben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2.11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 1 Mike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 1 Joe/Luke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 3 Adam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 1 Adam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1.10</t>
-  </si>
-  <si>
     <t xml:space="preserve">2024 2 Alan</t>
   </si>
   <si>
@@ -1418,69 +1418,69 @@
     <t xml:space="preserve">2024 2 Jared</t>
   </si>
   <si>
+    <t xml:space="preserve">2023 2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 4 Ben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 4 Mike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 4.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 3 Joe/Luke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 5 Vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 1 Jared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 2 Vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 5 Ben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 5 Mike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 4 Joe/Luke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 1 Ben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 3 Vanja</t>
+  </si>
+  <si>
     <t xml:space="preserve">2023 2.12</t>
   </si>
   <si>
-    <t xml:space="preserve">2024 4 Ben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 4 Mike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 3 Joe/Luke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 5 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 1 Jared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 2 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 5 Ben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 5 Mike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 4 Joe/Luke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 1 Ben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 3 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2.10</t>
-  </si>
-  <si>
     <t xml:space="preserve">2024 5 Joe/Luke</t>
   </si>
   <si>
@@ -1493,16 +1493,16 @@
     <t xml:space="preserve">2024 3 John</t>
   </si>
   <si>
+    <t xml:space="preserve">2023 3.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 2 John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 4 John</t>
+  </si>
+  <si>
     <t xml:space="preserve">2023 3.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 2 John</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 4 John</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3.7</t>
   </si>
   <si>
     <t xml:space="preserve">2024 5 John</t>
@@ -2402,7 +2402,7 @@
   <dimension ref="A1:Z89"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4638,7 +4638,7 @@
   <dimension ref="A1:BG125"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5564,7 +5564,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A98" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I130" activeCellId="0" sqref="I130"/>
+      <selection pane="topLeft" activeCell="F135" activeCellId="0" sqref="F135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6400,6 +6400,28 @@
       <c r="A142" s="25"/>
       <c r="B142" s="28" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="19" t="s">
+        <v>643</v>
+      </c>
+      <c r="B144" s="20" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="23" t="s">
+        <v>653</v>
+      </c>
+      <c r="B145" s="24" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="25"/>
+      <c r="B146" s="28" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
missed 2 keepers on Joe/Luke's team
</commit_message>
<xml_diff>
--- a/OffSeason.xlsx
+++ b/OffSeason.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="690">
   <si>
     <t xml:space="preserve">Where’s your Kupp Now– Vanja Dolas </t>
   </si>
@@ -503,1104 +503,1104 @@
     <t xml:space="preserve">Kameron Curl</t>
   </si>
   <si>
+    <t xml:space="preserve">Deatrich Wise Jr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dre’Mont Jones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jake ferguson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myles Garrett</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montez Sweat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fred Warner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xavier Mckinney</t>
+  </si>
+  <si>
     <t xml:space="preserve">Matthew Judon</t>
   </si>
   <si>
-    <t xml:space="preserve">Dre’Mont Jones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jake ferguson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Myles Garrett</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Montez Sweat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fred Warner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xavier Mckinney</t>
+    <t xml:space="preserve">B.J. Hill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minkah Fitzpatrick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maxx Crosby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danielle Hunter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kwity Paye</t>
   </si>
   <si>
     <t xml:space="preserve">Alex Singleton</t>
   </si>
   <si>
-    <t xml:space="preserve">B.J. Hill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minkah Fitzpatrick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maxx Crosby</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Danielle Hunter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kwity Paye</t>
+    <t xml:space="preserve">Myles Jack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grant Delpit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quay Walker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foye Oluokun </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Ojabo</t>
   </si>
   <si>
     <t xml:space="preserve">Cole Holcomb</t>
   </si>
   <si>
-    <t xml:space="preserve">Myles Jack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grant Delpit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quay Walker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Foye Oluokun </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David Ojabo</t>
+    <t xml:space="preserve">Devine Deablo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyle Dugger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devin White</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jordyn Brooks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travon Walker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zaire Franklin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taysom Hill (TE/QB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aaron Donald</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeremiah Owusu-Koramoah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isaiah Simmons</t>
   </si>
   <si>
     <t xml:space="preserve">2023 1.7</t>
   </si>
   <si>
-    <t xml:space="preserve">Devine Deablo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kyle Dugger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Devin White</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jordyn Brooks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Travon Walker</t>
+    <t xml:space="preserve">Darrell Henderson Jr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demarcus Lawrence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nick Bolton</t>
   </si>
   <si>
     <t xml:space="preserve">2023 2.7</t>
   </si>
   <si>
-    <t xml:space="preserve">Taysom Hill (TE/QB)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aaron Donald</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jeremiah Owusu-Koramoah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isaiah Simmons</t>
+    <t xml:space="preserve">Russell Gage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logan Wilson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2.11</t>
   </si>
   <si>
     <t xml:space="preserve">2023 4.7</t>
   </si>
   <si>
-    <t xml:space="preserve">Darrell Henderson Jr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demarcus Lawrence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2.12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nick Bolton</t>
+    <t xml:space="preserve">Ben Showronek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bobby Wagner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3.8</t>
   </si>
   <si>
     <t xml:space="preserve">2023 5.7</t>
   </si>
   <si>
-    <t xml:space="preserve">Russell Gage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logan Wilson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1.11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2.11</t>
+    <t xml:space="preserve">Sammy Watkins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demario Davis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5.8</t>
   </si>
   <si>
     <t xml:space="preserve">2023 6.7</t>
   </si>
   <si>
-    <t xml:space="preserve">Ben Showronek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bobby Wagner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1.12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3.8</t>
+    <t xml:space="preserve">Noah Brown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jamison Crowder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nyheim Hines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DeeJay Dallas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mike Boone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dontrell Hilliard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JaMycal Hasty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marcus Mariota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeff Driskel (QB, TE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom Brady </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Julio Jones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robbie Anderson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O.J. Howard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Donovan wilson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Velociraptor Maloish - Matt Holland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slick Daddy Club - Andrew Gates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FoldingTableRepairMan - Steve Cohen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the naked pooper - Alan Powell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magik Skol Bus - Brandon Hurd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thielen Groovy - Adam Wells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J.J. Watt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Josh Allen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joe Burrow </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dak Prescott </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kirk Cousins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aaron Rodgers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel Jones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hassan Haskins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Justin Herbert </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Derek Carr </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jimmy Garoppolo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tua Tagovailoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ryan Tannehill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James Conner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malik Davis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alvin Kamara </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tony Pollard </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antonio Gibson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kenneth Gainwell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Montgomery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alexander Mattison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quez Watkins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christian McCaffrey </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kareem Hunt </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brian Robinson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ty Chandler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AJ Dillon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jerick Mckinnon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chris Moore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jaylen Warren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tyler Allgeier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jamaal Williams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keaontay Ingram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devin Singletary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James robinson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devin Duvernay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matt Breida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James Cook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terry McLaurin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eli Mitchell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clyde Edwards-Helaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mike Evans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel Bellinger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">George Pickens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D’Onta Foreman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keenan Allen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gabe Davis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joshua Kelley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam Thielen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harrison Bryant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tee Higgins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diontae Johnson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marquise Brown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brandon Aiyuk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mike Williams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Donovan Peoples-Jones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jordan Whitehead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jakobi Meyers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allen Lazard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zay Jones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terrace Marshall Jr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael Pittman Jr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Micheal Gallup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pat Surtain Jr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deebo Samuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kendrick Bourne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DJ Chark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Darnell Mooney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treylon Burks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curtis Samuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malik Willis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skyy Moore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tyler Lockett</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robert Woods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isaiah Hodgins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jerry Jeudy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K.J. Osborn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mike White</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rondale Moore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noah Fant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DeVante Parker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Odell Beckham Jr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marquez Valdes-Scantling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Richie James</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zonovan Knight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WanDale Robinson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C.J. Uzomah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courtland Sutton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brandin Cooks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Romeo Doubs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juwan Johnson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Van Jefferson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rahod Bateman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin Byard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evan Engram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mike Gesicki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hunter Renfrow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hunter Henry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Bell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dalton Schultz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eddie Jackson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zach Ertz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greg Dulcich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gerald Everett</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tyler Higbee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jermaine Johnson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Austin Hooper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J.C. Jackson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Richie Grant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Irv Smith Jr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hayden Hurst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harrison Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trey Hendrickson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isaiah Likely</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aidan Hutchinson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tyrann Mathieu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talanoa Hufanga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trey McBride</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rayshawn Jenkins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J.D. Mckissic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jordan Poyer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Josh Sweat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quinnen Williams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jevon Holland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Justin Simmons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Damar Hamlin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travis Homer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sauce Gardner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dexter Lawrence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kenny Clark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jessie Bates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vonn Bell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Javon Hargrave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DeAndre Carter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rasul Douglas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C.J. Mosley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T.J. Watt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jonathan Allen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jalen Thompson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grover Stewart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KJ Hamler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denico Autry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roquan Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eric Kendricks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kayvon Thibodeaux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chris Jones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linval Joseph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vita Vea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dre Greenlaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matt Milano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">George Karlaftis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christian Wilkins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bobby Okereke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zach Sieler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Derrick Brown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khalil Mack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quincy Williams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patrick Queen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brian Burns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Germaine Pratt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jack Sanborn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Micah Parsons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De’Vondre Campbell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tremaine Edmunds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T.J. Edwards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Willie Gay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gardner Minshew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lavonte David</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bradley Chubb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shaq Thompson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cordarrelle Patterson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zaven Collins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 4.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 4.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pete Werner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Long Jr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latavius Muray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shaquille Leonard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chubba Hubbard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shaquil Barrett</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 6.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 4.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isaiah Spiller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 7.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 6.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 4.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joshua Palmer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 4.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 8.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 7.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 4.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Julian Love</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trevon Diggs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DeShon Elliot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frank Clark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rashaan Evans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devin Lloyd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tyler Heinicke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kenyan Drake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tony Jones Jr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isaiah McKenzie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kenny Golladay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fletcher Cox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tae Crowder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jalen Ramsey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaiir Elam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jordan Phillips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rex Burkhead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caleb Huntley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corey Davis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allen Robinson II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robert tonyan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roger McCreary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calais Campbell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christian Kirksey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harold Landry III</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alex Anzalone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drue Tranquill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raheem Mostert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zack Moss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael Carter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jordan Mason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tyrion Davis-Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chase Edmonds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyren Williams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyle Phillips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laviska Shenault Jr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tyler Boyd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jarvis Landry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 6 Vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 4 Vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 1 John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 2 Jared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 2 Steve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 1 Mike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 1 Joe/Luke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 4 Jared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 1 Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 2 Vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 3 Steve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 3 Mike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 2 Joe/Luke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 4 Ben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 1 Alan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 2 Ben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 4 John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 4 Mike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 3 Joe/Luke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 5 Vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 1 Jared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 2 Mike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 5 Ben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 5 Mike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 4 Joe/Luke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 5 John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 1 Ben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 3 Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 5 Joe/Luke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 1 Vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 3 Vanja</t>
   </si>
   <si>
     <t xml:space="preserve">2023 7.7</t>
   </si>
   <si>
-    <t xml:space="preserve">Sammy Watkins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demario Davis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3.12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5.8</t>
+    <t xml:space="preserve">2024 2 Alan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 3 John</t>
   </si>
   <si>
     <t xml:space="preserve">2023 8.7</t>
   </si>
   <si>
-    <t xml:space="preserve">Noah Brown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jamison Crowder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nyheim Hines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DeeJay Dallas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mike Boone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dontrell Hilliard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JaMycal Hasty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marcus Mariota</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jeff Driskel (QB, TE)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tom Brady </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Julio Jones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robbie Anderson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O.J. Howard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Donovan wilson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Velociraptor Maloish - Matt Holland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slick Daddy Club - Andrew Gates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FoldingTableRepairMan - Steve Cohen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the naked pooper - Alan Powell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magik Skol Bus - Brandon Hurd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thielen Groovy - Adam Wells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J.J. Watt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Josh Allen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joe Burrow </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dak Prescott </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kirk Cousins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aaron Rodgers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daniel Jones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hassan Haskins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Justin Herbert </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Derek Carr </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jimmy Garoppolo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tua Tagovailoa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ryan Tannehill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">James Conner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malik Davis </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alvin Kamara </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tony Pollard </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antonio Gibson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kenneth Gainwell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David Montgomery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alexander Mattison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quez Watkins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christian McCaffrey </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kareem Hunt </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brian Robinson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ty Chandler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AJ Dillon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jerick Mckinnon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chris Moore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jaylen Warren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tyler Allgeier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jamaal Williams</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keaontay Ingram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Devin Singletary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">James robinson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Devin Duvernay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matt Breida</t>
-  </si>
-  <si>
-    <t xml:space="preserve">James Cook</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terry McLaurin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eli Mitchell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clyde Edwards-Helaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mike Evans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daniel Bellinger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">George Pickens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D’Onta Foreman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keenan Allen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gabe Davis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joshua Kelley</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adam Thielen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harrison Bryant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tee Higgins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diontae Johnson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marquise Brown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brandon Aiyuk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mike Williams</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Donovan Peoples-Jones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zaire Franklin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jakobi Meyers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allen Lazard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zay Jones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terrace Marshall Jr.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Michael Pittman Jr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Micheal Gallup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jordan Whitehead</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deebo Samuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kendrick Bourne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DJ Chark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Darnell Mooney</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treylon Burks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Curtis Samuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pat Surtain Jr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skyy Moore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tyler Lockett</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robert Woods</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isaiah Hodgins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jerry Jeudy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K.J. Osborn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deatrich Wise Jr.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rondale Moore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Noah Fant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DeVante Parker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Odell Beckham Jr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marquez Valdes-Scantling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Richie James</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malik Willis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WanDale Robinson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C.J. Uzomah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Courtland Sutton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brandin Cooks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Romeo Doubs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juwan Johnson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mike White</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rahod Bateman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kevin Byard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Evan Engram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mike Gesicki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hunter Renfrow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hunter Henry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zonovan Knight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dalton Schultz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eddie Jackson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zach Ertz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Greg Dulcich</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerald Everett</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tyler Higbee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Van Jefferson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Austin Hooper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J.C. Jackson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Richie Grant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Irv Smith Jr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hayden Hurst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harrison Smith</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David Bell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isaiah Likely</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aidan Hutchinson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tyrann Mathieu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Talanoa Hufanga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trey McBride</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rayshawn Jenkins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jermaine Johnson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jordan Poyer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Josh Sweat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quinnen Williams</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jevon Holland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Justin Simmons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Damar Hamlin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trey Hendrickson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sauce Gardner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dexter Lawrence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kenny Clark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jessie Bates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vonn Bell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Javon Hargrave</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J.D. Mckissic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rasul Douglas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C.J. Mosley</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T.J. Watt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jonathan Allen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jalen Thompson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grover Stewart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Travis Homer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Denico Autry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roquan Smith</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eric Kendricks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kayvon Thibodeaux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chris Jones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DeAndre Carter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vita Vea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dre Greenlaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matt Milano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">George Karlaftis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christian Wilkins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bobby Okereke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KJ Hamler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Derrick Brown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Khalil Mack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quincy Williams</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patrick Queen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brian Burns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Germaine Pratt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linval Joseph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Micah Parsons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">De’Vondre Campbell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tremaine Edmunds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T.J. Edwards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Willie Gay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zach Sieler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lavonte David</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bradley Chubb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shaq Thompson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jack Sanborn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zaven Collins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pete Werner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David Long Jr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gardner Minshew</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shaquille Leonard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3.11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cordarrelle Patterson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shaquil Barrett</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 6.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Latavius Muray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 7.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 6.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chubba Hubbard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 8.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 7.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isaiah Spiller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joshua Palmer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Julian Love</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trevon Diggs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DeShon Elliot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frank Clark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rashaan Evans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Devin Lloyd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tyler Heinicke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kenyan Drake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tony Jones Jr.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isaiah McKenzie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kenny Golladay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fletcher Cox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tae Crowder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jalen Ramsey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kaiir Elam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jordan Phillips</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rex Burkhead</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caleb Huntley</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corey Davis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allen Robinson II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robert tonyan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roger McCreary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calais Campbell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christian Kirksey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harold Landry III</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alex Anzalone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drue Tranquill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raheem Mostert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zack Moss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Michael Carter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jordan Mason</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tyrion Davis-Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chase Edmonds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kyren Williams</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kyle Phillips</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laviska Shenault Jr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tyler Boyd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jarvis Landry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 6 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 4 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 1 John</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 2 Jared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 2 Steve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 1 Mike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 1 Joe/Luke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 4 Jared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 1 Adam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 2 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 3 Steve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 3 Mike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 2 Joe/Luke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 4 Ben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 1 Alan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 2 Ben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 4 John</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 4 Mike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 3 Joe/Luke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 5 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 1 Jared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 2 Mike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 5 Ben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 5 Mike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 4 Joe/Luke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5 John</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 1 Ben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 3 Adam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 5 Joe/Luke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 1 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 3 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 2 Alan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 3 John</t>
-  </si>
-  <si>
     <t xml:space="preserve">2024 2 Adam</t>
   </si>
   <si>
@@ -1884,6 +1884,9 @@
   </si>
   <si>
     <t xml:space="preserve">roadrunner44@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ausinrhode47@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Slick Daddy Club</t>
@@ -2530,7 +2533,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA114"/>
+  <dimension ref="A1:AA112"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G60" activeCellId="0" sqref="G60"/>
@@ -3641,9 +3644,7 @@
       <c r="U22" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="V22" s="14" t="s">
-        <v>156</v>
-      </c>
+      <c r="V22" s="13"/>
       <c r="W22" s="0" t="s">
         <v>159</v>
       </c>
@@ -3690,7 +3691,9 @@
       <c r="U23" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="V23" s="14"/>
+      <c r="V23" s="14" t="s">
+        <v>156</v>
+      </c>
       <c r="W23" s="0" t="s">
         <v>166</v>
       </c>
@@ -3790,6 +3793,7 @@
       <c r="U25" s="4" t="n">
         <v>24</v>
       </c>
+      <c r="V25" s="14"/>
       <c r="W25" s="0" t="s">
         <v>180</v>
       </c>
@@ -3835,6 +3839,7 @@
       <c r="U26" s="4" t="n">
         <v>25</v>
       </c>
+      <c r="V26" s="14"/>
       <c r="W26" s="0" t="s">
         <v>187</v>
       </c>
@@ -5824,16 +5829,6 @@
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA112" s="0" t="s">
         <v>489</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA113" s="0" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA114" s="0" t="s">
-        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -5880,8 +5875,8 @@
   </sheetPr>
   <dimension ref="A1:BG125"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H74" activeCellId="0" sqref="H74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5936,199 +5931,199 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>197</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>191</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>171</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="M2" s="7" t="s">
         <v>207</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="BG2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>204</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>198</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>178</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>214</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="BG3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>211</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>205</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>185</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="M4" s="7" t="s">
         <v>221</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="BG4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>218</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>212</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>192</v>
       </c>
       <c r="K5" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q5" s="0" t="s">
         <v>514</v>
-      </c>
-      <c r="N5" s="0" t="s">
-        <v>515</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q5" s="0" t="s">
-        <v>516</v>
       </c>
       <c r="BG5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>219</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>199</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="BG6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="0" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>206</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>215</v>
+        <v>521</v>
       </c>
       <c r="BG7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="0" t="s">
+        <v>522</v>
+      </c>
+      <c r="H8" s="0" t="s">
         <v>523</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>524</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>213</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>222</v>
+        <v>524</v>
       </c>
       <c r="BG8" s="0"/>
     </row>
@@ -7013,7 +7008,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
+      <selection pane="topLeft" activeCell="Q15" activeCellId="0" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7127,51 +7122,56 @@
         <v>619</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
         <v>620</v>
       </c>
-      <c r="B10" s="0" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>621</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="B11" s="0" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="C11" s="10" t="s">
         <v>623</v>
       </c>
-      <c r="B11" s="0" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>624</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="B12" s="0" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="C12" s="10" t="s">
         <v>626</v>
       </c>
-      <c r="B12" s="0" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>627</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="B13" s="0" t="s">
         <v>628</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="C13" s="10" t="s">
+        <v>629</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>629</v>
-      </c>
-      <c r="B13" s="0" t="s">
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>630</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="B14" s="0" t="s">
         <v>631</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>632</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7196,10 +7196,10 @@
     <hyperlink ref="C7" r:id="rId6" display="FieldsJared54@gmail.com"/>
     <hyperlink ref="C8" r:id="rId7" display="bjhurd@hotmail.com"/>
     <hyperlink ref="C9" r:id="rId8" display="roadrunner44@gmail.com"/>
-    <hyperlink ref="C10" r:id="rId9" display="andrewagates89@hotmail.com"/>
-    <hyperlink ref="C11" r:id="rId10" display="adamwells12@gmail.com"/>
-    <hyperlink ref="C12" r:id="rId11" display="powellap28@gmail.com"/>
-    <hyperlink ref="C13" r:id="rId12" display="king_ahab11@hotmail.com"/>
+    <hyperlink ref="C11" r:id="rId9" display="andrewagates89@hotmail.com"/>
+    <hyperlink ref="C12" r:id="rId10" display="adamwells12@gmail.com"/>
+    <hyperlink ref="C13" r:id="rId11" display="powellap28@gmail.com"/>
+    <hyperlink ref="C14" r:id="rId12" display="king_ahab11@hotmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -7231,13 +7231,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="23" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B1" s="24"/>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>73</v>
@@ -7246,7 +7246,7 @@
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="27"/>
       <c r="B3" s="26" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7258,13 +7258,13 @@
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="27"/>
       <c r="B5" s="26" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="27"/>
       <c r="B6" s="26" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7282,13 +7282,13 @@
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="27"/>
       <c r="B9" s="26" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="27"/>
       <c r="B10" s="26" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7303,40 +7303,40 @@
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="25" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="27"/>
       <c r="B14" s="26" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="27"/>
       <c r="B15" s="26" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="27"/>
       <c r="B16" s="26" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="27"/>
       <c r="B17" s="26" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="27"/>
       <c r="B18" s="26" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7345,7 +7345,7 @@
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="25" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>284</v>
@@ -7354,13 +7354,13 @@
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="27"/>
       <c r="B21" s="26" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="27"/>
       <c r="B22" s="26" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7369,7 +7369,7 @@
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="25" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>182</v>
@@ -7390,13 +7390,13 @@
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="27"/>
       <c r="B27" s="26" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="27"/>
       <c r="B28" s="26" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7411,28 +7411,28 @@
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="25" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="27"/>
       <c r="B32" s="26" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="27"/>
       <c r="B33" s="26" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="27"/>
       <c r="B34" s="26" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7444,7 +7444,7 @@
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="27"/>
       <c r="B36" s="26" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7456,13 +7456,13 @@
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="27"/>
       <c r="B38" s="26" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="27"/>
       <c r="B39" s="26" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7471,22 +7471,22 @@
     </row>
     <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="25" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="27"/>
       <c r="B42" s="26" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="27"/>
       <c r="B43" s="26" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7495,22 +7495,22 @@
     </row>
     <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="25" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="27"/>
       <c r="B46" s="26" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="27"/>
       <c r="B47" s="26" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7519,7 +7519,7 @@
     </row>
     <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="25" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B49" s="26" t="s">
         <v>284</v>
@@ -7528,13 +7528,13 @@
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="27"/>
       <c r="B50" s="26" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="27"/>
       <c r="B51" s="26" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7546,25 +7546,25 @@
     <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="27"/>
       <c r="B53" s="26" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="27"/>
       <c r="B54" s="26" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="27"/>
       <c r="B55" s="26" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="27"/>
       <c r="B56" s="26" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7576,7 +7576,7 @@
     <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="29"/>
       <c r="B58" s="30" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7584,18 +7584,18 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="23" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="27" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B61" s="31" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7612,7 +7612,7 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="23" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B65" s="33" t="s">
         <v>527</v>
@@ -7621,13 +7621,13 @@
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="27"/>
       <c r="B66" s="31" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="27"/>
       <c r="B67" s="31" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7638,7 +7638,7 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="27" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B69" s="28" t="s">
         <v>162</v>
@@ -7650,7 +7650,7 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="27" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B71" s="28" t="s">
         <v>162</v>
@@ -7658,7 +7658,7 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="27" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B72" s="31" t="s">
         <v>387</v>
@@ -7667,7 +7667,7 @@
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="27"/>
       <c r="B73" s="31" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7676,15 +7676,15 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="27" t="s">
+        <v>667</v>
+      </c>
+      <c r="B75" s="31" t="s">
         <v>666</v>
-      </c>
-      <c r="B75" s="31" t="s">
-        <v>665</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="27" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="B76" s="31" t="s">
         <v>527</v>
@@ -7693,13 +7693,13 @@
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="27"/>
       <c r="B77" s="31" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="29"/>
       <c r="B78" s="32" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7712,7 +7712,7 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="27" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B81" s="28" t="s">
         <v>373</v>
@@ -7721,7 +7721,7 @@
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="29"/>
       <c r="B82" s="32" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7729,12 +7729,12 @@
         <v>576</v>
       </c>
       <c r="B84" s="24" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="27" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B85" s="28" t="s">
         <v>393</v>
@@ -7743,7 +7743,7 @@
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="29"/>
       <c r="B86" s="32" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7751,7 +7751,7 @@
         <v>581</v>
       </c>
       <c r="B88" s="24" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7762,37 +7762,37 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="27" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B90" s="28" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="29"/>
       <c r="B91" s="32" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="23" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B93" s="24" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="29" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B94" s="32" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="23" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B96" s="33" t="s">
         <v>25</v>
@@ -7801,38 +7801,38 @@
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="27"/>
       <c r="B97" s="31" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="27"/>
       <c r="B98" s="31" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="27"/>
       <c r="B99" s="31" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="27" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B100" s="31" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="29"/>
       <c r="B101" s="32" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="23" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B103" s="33" t="s">
         <v>61</v>
@@ -7847,12 +7847,12 @@
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="27"/>
       <c r="B105" s="31" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="27" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B106" s="31" t="s">
         <v>22</v>
@@ -7867,7 +7867,7 @@
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="27"/>
       <c r="B108" s="31" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7881,7 +7881,7 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="23" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B111" s="24" t="s">
         <v>46</v>
@@ -7890,13 +7890,13 @@
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="27"/>
       <c r="B112" s="28" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="27"/>
       <c r="B113" s="28" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7907,7 +7907,7 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="29" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B115" s="32" t="s">
         <v>31</v>
@@ -7915,10 +7915,10 @@
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="23" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B117" s="24" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7929,10 +7929,10 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="29" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B119" s="32" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7940,15 +7940,15 @@
         <v>576</v>
       </c>
       <c r="B121" s="24" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="27" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B122" s="28" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7960,7 +7960,7 @@
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="29"/>
       <c r="B124" s="32" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7968,21 +7968,21 @@
         <v>576</v>
       </c>
       <c r="B126" s="24" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="27" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B127" s="28" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="27"/>
       <c r="B128" s="28" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8004,21 +8004,21 @@
         <v>581</v>
       </c>
       <c r="B132" s="28" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="29"/>
       <c r="B133" s="32" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="23" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B135" s="24" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8029,15 +8029,15 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="29" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B137" s="32" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="23" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B140" s="24" t="s">
         <v>171</v>
@@ -8048,7 +8048,7 @@
         <v>570</v>
       </c>
       <c r="B141" s="28" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8059,7 +8059,7 @@
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="23" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B144" s="24" t="s">
         <v>185</v>
@@ -8081,7 +8081,7 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="23" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B148" s="24" t="s">
         <v>191</v>
@@ -8092,13 +8092,13 @@
         <v>577</v>
       </c>
       <c r="B149" s="28" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="29"/>
       <c r="B150" s="32" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8118,7 +8118,7 @@
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="27"/>
       <c r="B154" s="28" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8132,13 +8132,13 @@
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="27"/>
       <c r="B156" s="28" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="29"/>
       <c r="B157" s="32" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8154,12 +8154,12 @@
         <v>577</v>
       </c>
       <c r="B160" s="32" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="23" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="B162" s="24" t="s">
         <v>395</v>
@@ -8168,7 +8168,7 @@
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="27"/>
       <c r="B163" s="28" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8180,7 +8180,7 @@
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="27"/>
       <c r="B165" s="28" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8209,7 +8209,7 @@
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="27"/>
       <c r="B170" s="28" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8223,13 +8223,13 @@
         <v>580</v>
       </c>
       <c r="B172" s="28" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="29"/>
       <c r="B173" s="32" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8243,27 +8243,27 @@
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="27"/>
       <c r="B176" s="28" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="27"/>
       <c r="B177" s="28" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="27" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="B178" s="28" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="29"/>
       <c r="B179" s="32" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8371,7 +8371,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
2nd commit. need cleaning still
</commit_message>
<xml_diff>
--- a/OffSeason.xlsx
+++ b/OffSeason.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="544">
   <si>
     <t xml:space="preserve">Massage Envy – Vanja Dolas</t>
   </si>
@@ -1655,280 +1655,7 @@
     <t xml:space="preserve">king_ahab11@hotmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">4 team trade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vanja sends</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Damien Harris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Michael Gallup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Darrell Henderson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">James Robinson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1 Jared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 1 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vanja receives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 John 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4 Jared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tracy Walker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JK Dobbins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Micheal Thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skylar Thompson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jared sends</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Michael thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jared receives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Javon Hargrave</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John sends</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 John 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 Mike 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John Receives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 Adam 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 Adam 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 Adam 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adam Sends</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adam Receives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Damien harris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vanja </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3 Alan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jared </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yannick Ngakoue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John Sends</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 2 John</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 3 Adam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 4 John</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alan Sends</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alan Receives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2 Matt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jared Sends</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jessie Bates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deforest Buckner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 2 Mike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3 Mike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 3 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jake Ferguson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 3 John</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keontay Ingram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2 Adam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2 Alan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 2 Jared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">christian Watson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andre Cisco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Justyn Ross</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3 Andrew</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 1 Alan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1 Mike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Irv Smith Jr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 2 Alan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3 Jared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3 Adam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 3 Jared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 4 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 1 Jared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1 Vanja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 1 Ben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 2.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 3 Ben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 1.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 John 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 2 Ben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 4 Ben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Damar Hamlin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Javon Hargreaves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 3.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jamall Williams</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 5.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 2 Steve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 3 Steve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 4 Jared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vanja`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Filled out when final cuts happen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 1 Adam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 2 Adam</t>
+    <t xml:space="preserve">Coming Day after Super Bowl!!!!!</t>
   </si>
 </sst>
 </file>
@@ -1995,7 +1722,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2050,12 +1777,6 @@
         <bgColor rgb="FF0563C1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBF0041"/>
-        <bgColor rgb="FFC9211E"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="8">
     <border diagonalUp="false" diagonalDown="false">
@@ -2075,13 +1796,6 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
       <right/>
-      <top style="hair"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="hair"/>
       <top style="hair"/>
       <bottom/>
       <diagonal/>
@@ -2114,6 +1828,13 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -2143,7 +1864,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2224,8 +1945,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -2236,27 +1957,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2264,19 +1993,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2304,7 +2029,7 @@
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FFBF0041"/>
+      <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF0070C0"/>
       <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
@@ -2361,7 +2086,7 @@
   <dimension ref="B1:Y83"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5091,10 +4816,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:H263"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J161" activeCellId="0" sqref="J161"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5108,1038 +4833,754 @@
       <c r="A1" s="20" t="s">
         <v>543</v>
       </c>
-      <c r="B1" s="21"/>
-    </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
-        <v>544</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24"/>
-      <c r="B3" s="23" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24"/>
-      <c r="B4" s="23" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24"/>
-      <c r="B5" s="23" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24"/>
-      <c r="B6" s="23" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24"/>
-      <c r="B7" s="23" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24"/>
-      <c r="B8" s="23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24"/>
-      <c r="B9" s="23" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="24"/>
-      <c r="B10" s="23" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24"/>
-      <c r="B11" s="23" t="s">
-        <v>190</v>
-      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22" t="s">
-        <v>551</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="24"/>
-      <c r="B14" s="23" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24"/>
-      <c r="B15" s="23" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24"/>
-      <c r="B16" s="23" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="24"/>
-      <c r="B17" s="23" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="24"/>
-      <c r="B18" s="23" t="s">
-        <v>557</v>
-      </c>
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="22" t="s">
-        <v>558</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="24"/>
-      <c r="B21" s="23" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="24"/>
-      <c r="B22" s="23" t="s">
-        <v>559</v>
-      </c>
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="21"/>
+      <c r="B21" s="22"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="21"/>
+      <c r="B22" s="22"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="24"/>
-      <c r="B23" s="25"/>
-    </row>
-    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="22" t="s">
-        <v>560</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="24"/>
-      <c r="B25" s="23" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="24"/>
-      <c r="B26" s="23" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="24"/>
-      <c r="B27" s="23" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="24"/>
-      <c r="B28" s="23" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="24"/>
-      <c r="B29" s="23" t="s">
-        <v>190</v>
-      </c>
+      <c r="A23" s="21"/>
+      <c r="B23" s="23"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="24"/>
+      <c r="B24" s="22"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="21"/>
+      <c r="B25" s="22"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="21"/>
+      <c r="B26" s="22"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="21"/>
+      <c r="B27" s="22"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="21"/>
+      <c r="B28" s="22"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="21"/>
+      <c r="B29" s="22"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="24"/>
-      <c r="B30" s="25"/>
-    </row>
-    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="22" t="s">
-        <v>562</v>
-      </c>
-      <c r="B31" s="23" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="24"/>
-      <c r="B32" s="23" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="24"/>
-      <c r="B33" s="23" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="24"/>
-      <c r="B34" s="23" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="24"/>
-      <c r="B35" s="23" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="24"/>
-      <c r="B36" s="23" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="24"/>
-      <c r="B37" s="23" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="24"/>
-      <c r="B38" s="23" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="24"/>
-      <c r="B39" s="23" t="s">
-        <v>553</v>
-      </c>
+      <c r="A30" s="21"/>
+      <c r="B30" s="23"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="24"/>
+      <c r="B31" s="22"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="21"/>
+      <c r="B32" s="22"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="21"/>
+      <c r="B33" s="22"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="21"/>
+      <c r="B34" s="22"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="21"/>
+      <c r="B35" s="22"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="21"/>
+      <c r="B36" s="22"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="21"/>
+      <c r="B37" s="22"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="21"/>
+      <c r="B38" s="22"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="21"/>
+      <c r="B39" s="22"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="24"/>
-      <c r="B40" s="25"/>
-    </row>
-    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="22" t="s">
-        <v>565</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="24"/>
-      <c r="B42" s="23" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="24"/>
-      <c r="B43" s="23" t="s">
-        <v>568</v>
-      </c>
+      <c r="A40" s="21"/>
+      <c r="B40" s="23"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="24"/>
+      <c r="B41" s="22"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="21"/>
+      <c r="B42" s="22"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="21"/>
+      <c r="B43" s="22"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="24"/>
-      <c r="B44" s="25"/>
-    </row>
-    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="22" t="s">
-        <v>569</v>
-      </c>
-      <c r="B45" s="23" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="24"/>
-      <c r="B46" s="23" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="24"/>
-      <c r="B47" s="23" t="s">
-        <v>568</v>
-      </c>
+      <c r="A44" s="21"/>
+      <c r="B44" s="23"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="24"/>
+      <c r="B45" s="22"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="21"/>
+      <c r="B46" s="22"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="21"/>
+      <c r="B47" s="22"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="24"/>
-      <c r="B48" s="25"/>
-    </row>
-    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="22" t="s">
-        <v>570</v>
-      </c>
-      <c r="B49" s="23" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="24"/>
-      <c r="B50" s="23" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="24"/>
-      <c r="B51" s="23" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="24"/>
-      <c r="B52" s="23" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="24"/>
-      <c r="B53" s="23" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="24"/>
-      <c r="B54" s="23" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="24"/>
-      <c r="B55" s="23" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="24"/>
-      <c r="B56" s="23" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="24"/>
-      <c r="B57" s="23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="26"/>
-      <c r="B58" s="27" t="s">
-        <v>563</v>
-      </c>
+      <c r="A48" s="21"/>
+      <c r="B48" s="23"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="24"/>
+      <c r="B49" s="22"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="21"/>
+      <c r="B50" s="22"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="21"/>
+      <c r="B51" s="22"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="21"/>
+      <c r="B52" s="22"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="21"/>
+      <c r="B53" s="22"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="21"/>
+      <c r="B54" s="22"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="21"/>
+      <c r="B55" s="22"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="21"/>
+      <c r="B56" s="22"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="21"/>
+      <c r="B57" s="22"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="25"/>
+      <c r="B58" s="26"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="20" t="s">
-        <v>572</v>
-      </c>
-      <c r="B60" s="21" t="s">
-        <v>573</v>
-      </c>
+      <c r="A60" s="27"/>
+      <c r="B60" s="28"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="24" t="s">
-        <v>574</v>
-      </c>
-      <c r="B61" s="28" t="s">
-        <v>183</v>
-      </c>
+      <c r="A61" s="21"/>
+      <c r="B61" s="29"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="24"/>
-      <c r="B62" s="28" t="s">
-        <v>386</v>
-      </c>
+      <c r="A62" s="21"/>
+      <c r="B62" s="29"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="26"/>
-      <c r="B63" s="29" t="s">
-        <v>575</v>
-      </c>
+      <c r="A63" s="25"/>
+      <c r="B63" s="30"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="20" t="s">
-        <v>576</v>
-      </c>
-      <c r="B65" s="30" t="s">
-        <v>577</v>
-      </c>
+      <c r="A65" s="27"/>
+      <c r="B65" s="31"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="24"/>
-      <c r="B66" s="28" t="s">
-        <v>578</v>
-      </c>
+      <c r="A66" s="21"/>
+      <c r="B66" s="29"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="24"/>
-      <c r="B67" s="28" t="s">
-        <v>579</v>
-      </c>
+      <c r="A67" s="21"/>
+      <c r="B67" s="29"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="24"/>
-      <c r="B68" s="28" t="s">
-        <v>398</v>
-      </c>
+      <c r="A68" s="21"/>
+      <c r="B68" s="29"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="24" t="s">
-        <v>565</v>
-      </c>
-      <c r="B69" s="25" t="s">
-        <v>175</v>
-      </c>
+      <c r="A69" s="21"/>
+      <c r="B69" s="23"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="24"/>
-      <c r="B70" s="25"/>
+      <c r="A70" s="21"/>
+      <c r="B70" s="23"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="24" t="s">
-        <v>580</v>
-      </c>
-      <c r="B71" s="25" t="s">
-        <v>175</v>
-      </c>
+      <c r="A71" s="21"/>
+      <c r="B71" s="23"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="24" t="s">
-        <v>581</v>
-      </c>
-      <c r="B72" s="28" t="s">
-        <v>398</v>
-      </c>
+      <c r="A72" s="21"/>
+      <c r="B72" s="29"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="24"/>
-      <c r="B73" s="28" t="s">
-        <v>582</v>
-      </c>
+      <c r="A73" s="21"/>
+      <c r="B73" s="29"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="24"/>
-      <c r="B74" s="25"/>
+      <c r="A74" s="21"/>
+      <c r="B74" s="23"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="24" t="s">
-        <v>583</v>
-      </c>
-      <c r="B75" s="28" t="s">
-        <v>582</v>
-      </c>
+      <c r="A75" s="21"/>
+      <c r="B75" s="29"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="24" t="s">
-        <v>560</v>
-      </c>
-      <c r="B76" s="28" t="s">
-        <v>577</v>
-      </c>
+      <c r="A76" s="21"/>
+      <c r="B76" s="29"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="24"/>
-      <c r="B77" s="28" t="s">
-        <v>578</v>
-      </c>
+      <c r="A77" s="21"/>
+      <c r="B77" s="29"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="26"/>
-      <c r="B78" s="29" t="s">
-        <v>579</v>
-      </c>
+      <c r="A78" s="25"/>
+      <c r="B78" s="30"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="20" t="s">
-        <v>475</v>
-      </c>
-      <c r="B80" s="21" t="s">
-        <v>162</v>
-      </c>
+      <c r="A80" s="27"/>
+      <c r="B80" s="28"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="24" t="s">
-        <v>574</v>
-      </c>
-      <c r="B81" s="25" t="s">
-        <v>584</v>
-      </c>
+      <c r="A81" s="21"/>
+      <c r="B81" s="23"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="26"/>
-      <c r="B82" s="29" t="s">
-        <v>573</v>
-      </c>
+      <c r="A82" s="25"/>
+      <c r="B82" s="30"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="20" t="s">
-        <v>475</v>
-      </c>
-      <c r="B84" s="21" t="s">
-        <v>585</v>
-      </c>
+      <c r="A84" s="27"/>
+      <c r="B84" s="28"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="24" t="s">
-        <v>572</v>
-      </c>
-      <c r="B85" s="25" t="s">
-        <v>386</v>
-      </c>
+      <c r="A85" s="21"/>
+      <c r="B85" s="23"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="26"/>
-      <c r="B86" s="29" t="s">
-        <v>553</v>
-      </c>
+      <c r="A86" s="25"/>
+      <c r="B86" s="30"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="20" t="s">
-        <v>586</v>
-      </c>
-      <c r="B88" s="21" t="s">
-        <v>587</v>
-      </c>
+      <c r="A88" s="27"/>
+      <c r="B88" s="28"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="24"/>
-      <c r="B89" s="25" t="s">
-        <v>204</v>
-      </c>
+      <c r="A89" s="21"/>
+      <c r="B89" s="23"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="24" t="s">
-        <v>572</v>
-      </c>
-      <c r="B90" s="25" t="s">
-        <v>552</v>
-      </c>
+      <c r="A90" s="21"/>
+      <c r="B90" s="23"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="26"/>
-      <c r="B91" s="29" t="s">
-        <v>588</v>
-      </c>
+      <c r="A91" s="25"/>
+      <c r="B91" s="30"/>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="20" t="s">
-        <v>572</v>
-      </c>
-      <c r="B93" s="21" t="s">
-        <v>589</v>
-      </c>
+      <c r="A93" s="27"/>
+      <c r="B93" s="28"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="26" t="s">
-        <v>574</v>
-      </c>
-      <c r="B94" s="29" t="s">
-        <v>590</v>
-      </c>
+      <c r="A94" s="25"/>
+      <c r="B94" s="30"/>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="20" t="s">
-        <v>591</v>
-      </c>
-      <c r="B96" s="30" t="s">
-        <v>25</v>
-      </c>
+      <c r="A96" s="27"/>
+      <c r="B96" s="31"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="24"/>
-      <c r="B97" s="28" t="s">
-        <v>592</v>
-      </c>
+      <c r="A97" s="21"/>
+      <c r="B97" s="29"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="24"/>
-      <c r="B98" s="28" t="s">
-        <v>593</v>
-      </c>
+      <c r="A98" s="21"/>
+      <c r="B98" s="29"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="24"/>
-      <c r="B99" s="28" t="s">
-        <v>594</v>
-      </c>
+      <c r="A99" s="21"/>
+      <c r="B99" s="29"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="24" t="s">
-        <v>574</v>
-      </c>
-      <c r="B100" s="28" t="s">
-        <v>550</v>
-      </c>
+      <c r="A100" s="21"/>
+      <c r="B100" s="29"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="26"/>
-      <c r="B101" s="29" t="s">
-        <v>595</v>
-      </c>
+      <c r="A101" s="25"/>
+      <c r="B101" s="30"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="20" t="s">
-        <v>572</v>
-      </c>
-      <c r="B103" s="30" t="s">
-        <v>44</v>
-      </c>
+      <c r="A103" s="27"/>
+      <c r="B103" s="31"/>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="24"/>
-      <c r="B104" s="28" t="s">
-        <v>85</v>
-      </c>
+      <c r="A104" s="21"/>
+      <c r="B104" s="29"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="24"/>
-      <c r="B105" s="28" t="s">
-        <v>596</v>
-      </c>
+      <c r="A105" s="21"/>
+      <c r="B105" s="29"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="24" t="s">
-        <v>574</v>
-      </c>
-      <c r="B106" s="28" t="s">
-        <v>17</v>
-      </c>
+      <c r="A106" s="21"/>
+      <c r="B106" s="29"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="24"/>
-      <c r="B107" s="28" t="s">
-        <v>171</v>
-      </c>
+      <c r="A107" s="21"/>
+      <c r="B107" s="29"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="24"/>
-      <c r="B108" s="28" t="s">
-        <v>597</v>
-      </c>
+      <c r="A108" s="21"/>
+      <c r="B108" s="29"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="26"/>
-      <c r="B109" s="29" t="s">
-        <v>42</v>
-      </c>
+      <c r="A109" s="25"/>
+      <c r="B109" s="30"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F110" s="13"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="20" t="s">
-        <v>591</v>
-      </c>
-      <c r="B111" s="21" t="s">
-        <v>29</v>
-      </c>
+      <c r="A111" s="27"/>
+      <c r="B111" s="28"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="24"/>
-      <c r="B112" s="25" t="s">
-        <v>550</v>
-      </c>
+      <c r="A112" s="21"/>
+      <c r="B112" s="23"/>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="24"/>
-      <c r="B113" s="25" t="s">
-        <v>420</v>
-      </c>
+      <c r="A113" s="21"/>
+      <c r="B113" s="23"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="24"/>
-      <c r="B114" s="25" t="s">
-        <v>598</v>
-      </c>
+      <c r="A114" s="21"/>
+      <c r="B114" s="23"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="26" t="s">
-        <v>574</v>
-      </c>
-      <c r="B115" s="29" t="s">
-        <v>57</v>
-      </c>
+      <c r="A115" s="25"/>
+      <c r="B115" s="30"/>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="20" t="s">
-        <v>574</v>
-      </c>
-      <c r="B117" s="21" t="s">
-        <v>578</v>
-      </c>
+      <c r="A117" s="27"/>
+      <c r="B117" s="28"/>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="24"/>
-      <c r="B118" s="25" t="s">
-        <v>599</v>
-      </c>
+      <c r="A118" s="21"/>
+      <c r="B118" s="23"/>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="26" t="s">
-        <v>572</v>
-      </c>
-      <c r="B119" s="29" t="s">
-        <v>600</v>
-      </c>
+      <c r="A119" s="25"/>
+      <c r="B119" s="30"/>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="20" t="s">
-        <v>475</v>
-      </c>
-      <c r="B121" s="21" t="s">
-        <v>601</v>
-      </c>
+      <c r="A121" s="27"/>
+      <c r="B121" s="28"/>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="24" t="s">
-        <v>591</v>
-      </c>
-      <c r="B122" s="25" t="s">
-        <v>602</v>
-      </c>
+      <c r="A122" s="21"/>
+      <c r="B122" s="23"/>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="24"/>
-      <c r="B123" s="25" t="s">
-        <v>603</v>
-      </c>
+      <c r="A123" s="21"/>
+      <c r="B123" s="23"/>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="26"/>
-      <c r="B124" s="29" t="s">
-        <v>248</v>
-      </c>
+      <c r="A124" s="25"/>
+      <c r="B124" s="30"/>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="20" t="s">
-        <v>475</v>
-      </c>
-      <c r="B126" s="21" t="s">
-        <v>604</v>
-      </c>
+      <c r="A126" s="27"/>
+      <c r="B126" s="28"/>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="24" t="s">
-        <v>574</v>
-      </c>
-      <c r="B127" s="25" t="s">
-        <v>605</v>
-      </c>
+      <c r="A127" s="21"/>
+      <c r="B127" s="23"/>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="24"/>
-      <c r="B128" s="25" t="s">
-        <v>606</v>
-      </c>
+      <c r="A128" s="21"/>
+      <c r="B128" s="23"/>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="26"/>
-      <c r="B129" s="29" t="s">
-        <v>607</v>
-      </c>
+      <c r="A129" s="25"/>
+      <c r="B129" s="30"/>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="20" t="s">
-        <v>608</v>
-      </c>
-      <c r="B131" s="21" t="s">
-        <v>228</v>
-      </c>
+      <c r="A131" s="27"/>
+      <c r="B131" s="28"/>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="24" t="s">
-        <v>586</v>
-      </c>
-      <c r="B132" s="25" t="s">
-        <v>65</v>
-      </c>
+      <c r="A132" s="21"/>
+      <c r="B132" s="23"/>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="26"/>
-      <c r="B133" s="29" t="s">
-        <v>609</v>
-      </c>
+      <c r="A133" s="25"/>
+      <c r="B133" s="30"/>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="20" t="s">
-        <v>574</v>
-      </c>
-      <c r="B135" s="21" t="s">
-        <v>610</v>
-      </c>
+      <c r="A135" s="27"/>
+      <c r="B135" s="28"/>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="24"/>
-      <c r="B136" s="25" t="s">
-        <v>577</v>
-      </c>
+      <c r="A136" s="21"/>
+      <c r="B136" s="23"/>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="26" t="s">
-        <v>591</v>
-      </c>
-      <c r="B137" s="29" t="s">
-        <v>611</v>
-      </c>
+      <c r="A137" s="25"/>
+      <c r="B137" s="30"/>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="20" t="s">
-        <v>591</v>
-      </c>
-      <c r="B140" s="21" t="s">
-        <v>612</v>
-      </c>
+      <c r="A140" s="27"/>
+      <c r="B140" s="28"/>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="24" t="s">
-        <v>608</v>
-      </c>
-      <c r="B141" s="25" t="s">
-        <v>613</v>
-      </c>
+      <c r="A141" s="21"/>
+      <c r="B141" s="23"/>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="26"/>
-      <c r="B142" s="29" t="s">
-        <v>119</v>
-      </c>
+      <c r="A142" s="25"/>
+      <c r="B142" s="30"/>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="20" t="s">
-        <v>591</v>
-      </c>
-      <c r="B144" s="21" t="s">
-        <v>614</v>
-      </c>
+      <c r="A144" s="27"/>
+      <c r="B144" s="28"/>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="24" t="s">
-        <v>608</v>
-      </c>
-      <c r="B145" s="25" t="s">
-        <v>615</v>
-      </c>
+      <c r="A145" s="21"/>
+      <c r="B145" s="23"/>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="26"/>
-      <c r="B146" s="29" t="s">
-        <v>616</v>
-      </c>
+      <c r="A146" s="25"/>
+      <c r="B146" s="30"/>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="20" t="s">
-        <v>591</v>
-      </c>
-      <c r="B148" s="21" t="s">
-        <v>617</v>
-      </c>
+      <c r="A148" s="27"/>
+      <c r="B148" s="28"/>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="24" t="s">
-        <v>432</v>
-      </c>
-      <c r="B149" s="25" t="s">
-        <v>550</v>
-      </c>
+      <c r="A149" s="21"/>
+      <c r="B149" s="23"/>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="26"/>
-      <c r="B150" s="29" t="s">
-        <v>604</v>
-      </c>
+      <c r="A150" s="25"/>
+      <c r="B150" s="30"/>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="20" t="s">
-        <v>432</v>
-      </c>
-      <c r="B152" s="21" t="s">
-        <v>127</v>
-      </c>
+      <c r="A152" s="27"/>
+      <c r="B152" s="28"/>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="24"/>
-      <c r="B153" s="25" t="s">
-        <v>211</v>
-      </c>
+      <c r="A153" s="21"/>
+      <c r="B153" s="23"/>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="24"/>
-      <c r="B154" s="25" t="s">
-        <v>618</v>
-      </c>
+      <c r="A154" s="21"/>
+      <c r="B154" s="23"/>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="24" t="s">
-        <v>608</v>
-      </c>
-      <c r="B155" s="25" t="s">
-        <v>184</v>
-      </c>
+      <c r="A155" s="21"/>
+      <c r="B155" s="23"/>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="24"/>
-      <c r="B156" s="25" t="s">
-        <v>619</v>
-      </c>
+      <c r="A156" s="21"/>
+      <c r="B156" s="23"/>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="26"/>
-      <c r="B157" s="29" t="s">
-        <v>620</v>
-      </c>
+      <c r="A157" s="25"/>
+      <c r="B157" s="30"/>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="20" t="s">
-        <v>475</v>
-      </c>
-      <c r="B159" s="21" t="s">
-        <v>607</v>
-      </c>
+      <c r="A159" s="27"/>
+      <c r="B159" s="28"/>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="26" t="s">
-        <v>432</v>
-      </c>
-      <c r="B160" s="29" t="s">
-        <v>593</v>
-      </c>
+      <c r="A160" s="25"/>
+      <c r="B160" s="30"/>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="20" t="s">
-        <v>621</v>
-      </c>
-      <c r="B162" s="21" t="s">
-        <v>403</v>
-      </c>
+      <c r="A162" s="27"/>
+      <c r="B162" s="28"/>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="24"/>
-      <c r="B163" s="25" t="s">
-        <v>289</v>
-      </c>
+      <c r="A163" s="21"/>
+      <c r="B163" s="23"/>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="24"/>
-      <c r="B164" s="25" t="s">
-        <v>622</v>
-      </c>
+      <c r="A164" s="21"/>
+      <c r="B164" s="23"/>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="24"/>
-      <c r="B165" s="25" t="s">
-        <v>623</v>
-      </c>
+      <c r="A165" s="21"/>
+      <c r="B165" s="23"/>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="24"/>
-      <c r="B166" s="25" t="s">
-        <v>624</v>
-      </c>
+      <c r="A166" s="21"/>
+      <c r="B166" s="23"/>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="26" t="s">
-        <v>474</v>
-      </c>
-      <c r="B167" s="29" t="s">
-        <v>545</v>
-      </c>
+      <c r="A167" s="25"/>
+      <c r="B167" s="30"/>
       <c r="F167" s="13"/>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="20" t="s">
-        <v>608</v>
-      </c>
-      <c r="B169" s="21" t="s">
-        <v>55</v>
-      </c>
+      <c r="A169" s="27"/>
+      <c r="B169" s="28"/>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="24"/>
-      <c r="B170" s="25" t="s">
-        <v>625</v>
-      </c>
+      <c r="A170" s="21"/>
+      <c r="B170" s="23"/>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="24"/>
-      <c r="B171" s="25" t="s">
-        <v>626</v>
-      </c>
+      <c r="A171" s="21"/>
+      <c r="B171" s="23"/>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="24" t="s">
-        <v>434</v>
-      </c>
-      <c r="B172" s="25" t="s">
-        <v>627</v>
-      </c>
+      <c r="A172" s="21"/>
+      <c r="B172" s="23"/>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="26"/>
-      <c r="B173" s="29" t="s">
-        <v>628</v>
-      </c>
+      <c r="A173" s="25"/>
+      <c r="B173" s="30"/>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="20" t="s">
-        <v>432</v>
-      </c>
-      <c r="B175" s="21" t="s">
-        <v>545</v>
-      </c>
+      <c r="A175" s="27"/>
+      <c r="B175" s="28"/>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="24"/>
-      <c r="B176" s="25" t="s">
-        <v>620</v>
-      </c>
+      <c r="A176" s="21"/>
+      <c r="B176" s="23"/>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="24"/>
-      <c r="B177" s="25" t="s">
-        <v>629</v>
-      </c>
+      <c r="A177" s="21"/>
+      <c r="B177" s="23"/>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="24" t="s">
-        <v>630</v>
-      </c>
-      <c r="B178" s="25" t="s">
-        <v>587</v>
-      </c>
+      <c r="A178" s="21"/>
+      <c r="B178" s="23"/>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="26"/>
-      <c r="B179" s="29" t="s">
-        <v>578</v>
-      </c>
+      <c r="A179" s="25"/>
+      <c r="B179" s="30"/>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E191" s="13"/>
@@ -6152,23 +5593,23 @@
       <c r="F222" s="13"/>
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F248" s="31"/>
+      <c r="F248" s="32"/>
       <c r="G248" s="0"/>
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F249" s="31"/>
+      <c r="F249" s="32"/>
       <c r="G249" s="0"/>
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F250" s="31"/>
+      <c r="F250" s="32"/>
       <c r="G250" s="0"/>
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F251" s="31"/>
+      <c r="F251" s="32"/>
       <c r="G251" s="0"/>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F252" s="31"/>
+      <c r="F252" s="32"/>
       <c r="G252" s="0"/>
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6208,15 +5649,17 @@
       <c r="G261" s="0"/>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F262" s="31"/>
+      <c r="F262" s="32"/>
       <c r="G262" s="0"/>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F263" s="31"/>
+      <c r="F263" s="32"/>
       <c r="G263" s="0"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H20"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6232,10 +5675,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6245,117 +5688,208 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A1" s="33"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+    </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>430</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>472</v>
-      </c>
+      <c r="A4" s="33"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="32" t="s">
-        <v>471</v>
-      </c>
+      <c r="A5" s="33"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>632</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>633</v>
-      </c>
+      <c r="A6" s="33"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="32" t="s">
-        <v>601</v>
-      </c>
+      <c r="A7" s="33"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="33"/>
       <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="32" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+    </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="32" t="s">
-        <v>604</v>
-      </c>
+      <c r="A11" s="33"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="32" t="s">
-        <v>634</v>
-      </c>
+      <c r="A12" s="33"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="32" t="s">
-        <v>616</v>
-      </c>
+      <c r="A13" s="33"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>432</v>
-      </c>
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="32"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="32" t="s">
-        <v>619</v>
-      </c>
+      <c r="A16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="32" t="s">
-        <v>587</v>
-      </c>
+      <c r="A17" s="33"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="32" t="s">
-        <v>578</v>
-      </c>
+      <c r="A18" s="33"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="32" t="s">
-        <v>589</v>
-      </c>
+      <c r="A19" s="33"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="33"/>
       <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>608</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>627</v>
-      </c>
+      <c r="A21" s="33"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
-        <v>628</v>
-      </c>
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="33"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="33"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="33"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="33"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+    </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Cleaned File. Ready for off season
</commit_message>
<xml_diff>
--- a/OffSeason.xlsx
+++ b/OffSeason.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="599">
   <si>
     <t xml:space="preserve">Massage Envy – Vanja Dolas</t>
   </si>
@@ -80,6 +80,9 @@
     <t xml:space="preserve">Justin Fields</t>
   </si>
   <si>
+    <t xml:space="preserve">RB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jamaal Williams</t>
   </si>
   <si>
@@ -119,9 +122,6 @@
     <t xml:space="preserve">Kendre Miller</t>
   </si>
   <si>
-    <t xml:space="preserve">RB</t>
-  </si>
-  <si>
     <t xml:space="preserve">Austin Ekeler</t>
   </si>
   <si>
@@ -191,6 +191,9 @@
     <t xml:space="preserve">Isiah Pacheco</t>
   </si>
   <si>
+    <t xml:space="preserve">WR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Courtland Sutton</t>
   </si>
   <si>
@@ -230,9 +233,6 @@
     <t xml:space="preserve">Robert Woods</t>
   </si>
   <si>
-    <t xml:space="preserve">WR</t>
-  </si>
-  <si>
     <t xml:space="preserve">DeAndre Hopkins</t>
   </si>
   <si>
@@ -347,6 +347,9 @@
     <t xml:space="preserve">CeeDee Lamb</t>
   </si>
   <si>
+    <t xml:space="preserve">TE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dalton Shultz</t>
   </si>
   <si>
@@ -377,9 +380,6 @@
     <t xml:space="preserve">Joshua Palmer</t>
   </si>
   <si>
-    <t xml:space="preserve">TE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Travis Kelce</t>
   </si>
   <si>
@@ -404,6 +404,9 @@
     <t xml:space="preserve">Kadarius Toney</t>
   </si>
   <si>
+    <t xml:space="preserve">DB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jordan Poyer</t>
   </si>
   <si>
@@ -452,9 +455,6 @@
     <t xml:space="preserve">Richie grant</t>
   </si>
   <si>
-    <t xml:space="preserve">DB</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jaquan Brisker</t>
   </si>
   <si>
@@ -479,6 +479,9 @@
     <t xml:space="preserve">Dalton Kincaid</t>
   </si>
   <si>
+    <t xml:space="preserve">DL</t>
+  </si>
+  <si>
     <t xml:space="preserve">Micah Parsons</t>
   </si>
   <si>
@@ -533,6 +536,9 @@
     <t xml:space="preserve">Brian Branch</t>
   </si>
   <si>
+    <t xml:space="preserve">LB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Shaquille Leonard</t>
   </si>
   <si>
@@ -545,9 +551,6 @@
     <t xml:space="preserve">Leonard Floyd</t>
   </si>
   <si>
-    <t xml:space="preserve">DL</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aaron Donald</t>
   </si>
   <si>
@@ -620,9 +623,6 @@
     <t xml:space="preserve">T.J. Watt</t>
   </si>
   <si>
-    <t xml:space="preserve">LB</t>
-  </si>
-  <si>
     <t xml:space="preserve">Azeez Al-Shaair</t>
   </si>
   <si>
@@ -1334,78 +1334,168 @@
     <t xml:space="preserve">Ben 1</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 1 John</t>
+  </si>
+  <si>
     <t xml:space="preserve">Matt H 1</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 1 Vanja</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mike rhode 1</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 1 Ben</t>
+  </si>
+  <si>
     <t xml:space="preserve">JohnO 1</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 1 Jared</t>
+  </si>
+  <si>
     <t xml:space="preserve">Holland 2</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 1 Matt Holland</t>
+  </si>
+  <si>
     <t xml:space="preserve">Steve 1</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 1 Steve</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vanja 1</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 2 John</t>
+  </si>
+  <si>
     <t xml:space="preserve">John 5</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 2 Vanja</t>
+  </si>
+  <si>
     <t xml:space="preserve">Steve 2</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 2 Ben</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vanja 2</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 2 Jared</t>
+  </si>
+  <si>
     <t xml:space="preserve">Holland 3</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 2 Matt Holland</t>
+  </si>
+  <si>
     <t xml:space="preserve">Steve 4</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 2 Steve</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alan 1</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 3 John</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vanja 5</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 3 Vanja</t>
+  </si>
+  <si>
     <t xml:space="preserve">JohnO 4 </t>
   </si>
   <si>
+    <t xml:space="preserve">2025 3 Ben</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rhode 2</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 3 Jared</t>
+  </si>
+  <si>
     <t xml:space="preserve">Holland 4</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 3 Matt Holland</t>
+  </si>
+  <si>
     <t xml:space="preserve">Steve 5</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 3 Steve</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adam 1</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 4 John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 4 Vanja</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ben 5</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 4 Ben</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ben 3</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 4 Jared</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adam 4</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 4 Matt Holland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 4 Steve</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jared 1</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 5 John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 5 Vanja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 5 Ben</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alan 3</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 5 Jared</t>
+  </si>
+  <si>
     <t xml:space="preserve">Holland 5</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 5 Matt Holland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 5 Steve</t>
+  </si>
+  <si>
     <t xml:space="preserve">JohnO 2</t>
   </si>
   <si>
@@ -1463,64 +1553,139 @@
     <t xml:space="preserve">Joe Luke</t>
   </si>
   <si>
-    <t xml:space="preserve">no picks</t>
+    <t xml:space="preserve">2024 6 as needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 1 Rhode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 1 Adam</t>
   </si>
   <si>
     <t xml:space="preserve">Andrew 3</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 1 Alan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brandon 1</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 1 Brandon</t>
+  </si>
+  <si>
     <t xml:space="preserve">Andrew 1</t>
   </si>
   <si>
     <t xml:space="preserve">Joe/Luke 1</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 1 Joe/Luke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 2 Rhode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 2 Adam</t>
+  </si>
+  <si>
     <t xml:space="preserve">Steve 3</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 2 Alan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brandon 2</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 2 Brandon</t>
+  </si>
+  <si>
     <t xml:space="preserve">Andrew 2</t>
   </si>
   <si>
     <t xml:space="preserve">Joe/Luke2</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 2 Joe/Luke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 3 Rhode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 3 Adam</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alan 4</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 3 Alan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brandon 3</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 3 Brandon</t>
+  </si>
+  <si>
     <t xml:space="preserve">Andrew 4</t>
   </si>
   <si>
     <t xml:space="preserve">Joe/Luke 3</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 3 Joe/Luke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 4 Rhode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 4 Adam</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rhode 4</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 4 Alan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brandon 4</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 4 Brandon</t>
+  </si>
+  <si>
     <t xml:space="preserve">Andrew 5</t>
   </si>
   <si>
     <t xml:space="preserve">JohnO 3</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 4 Joe/Luke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 5 Rhode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 5 Adam</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alan 5</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 5 Alan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brandon 5</t>
   </si>
   <si>
+    <t xml:space="preserve">2025 5 Brandon</t>
+  </si>
+  <si>
     <t xml:space="preserve">Joe/Luke 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 5 Joe/Luke</t>
   </si>
   <si>
     <t xml:space="preserve">Adam 5</t>
@@ -1778,7 +1943,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1796,41 +1961,6 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
       <right/>
-      <top style="hair"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="hair"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right/>
-      <top/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="hair"/>
-      <top/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="hair"/>
       <top style="hair"/>
       <bottom/>
       <diagonal/>
@@ -1864,7 +1994,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1949,59 +2079,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2085,8 +2167,8 @@
   </sheetPr>
   <dimension ref="B1:Y83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B79" activeCellId="0" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2155,19 +2237,27 @@
       <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="3"/>
+      <c r="J2" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="K2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="3"/>
+      <c r="N2" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="O2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="3"/>
+      <c r="R2" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="S2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="3"/>
+      <c r="V2" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="W2" s="0" t="s">
         <v>12</v>
       </c>
@@ -2193,66 +2283,74 @@
       <c r="S3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="V3" s="3"/>
+      <c r="V3" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="W3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="3"/>
       <c r="C4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R4" s="3"/>
       <c r="S4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="V4" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="V4" s="5"/>
       <c r="W4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3"/>
       <c r="C5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="O5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="R5" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="S5" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="V5" s="5"/>
       <c r="W5" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="5" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>32</v>
@@ -2284,7 +2382,7 @@
         <v>38</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>39</v>
@@ -2353,66 +2451,72 @@
       <c r="S9" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="V9" s="6"/>
+      <c r="V9" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="W9" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="5"/>
       <c r="C10" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="R10" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="S10" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="V10" s="6"/>
       <c r="W10" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="5"/>
       <c r="C11" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="J11" s="6"/>
+        <v>64</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="K11" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R11" s="6"/>
       <c r="S11" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="V11" s="6"/>
       <c r="W11" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="6" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>69</v>
@@ -2451,7 +2555,9 @@
       <c r="K13" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="N13" s="6"/>
+      <c r="N13" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="O13" s="0" t="s">
         <v>78</v>
       </c>
@@ -2471,7 +2577,7 @@
       </c>
       <c r="D14" s="7"/>
       <c r="F14" s="6" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>82</v>
@@ -2580,52 +2686,54 @@
       <c r="G18" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="J18" s="8"/>
+      <c r="J18" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="K18" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="R18" s="6"/>
       <c r="S18" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="V18" s="6"/>
       <c r="W18" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="6"/>
       <c r="C19" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N19" s="6"/>
       <c r="O19" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="R19" s="6"/>
       <c r="S19" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="V19" s="6"/>
       <c r="W19" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="8" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>118</v>
@@ -2660,80 +2768,90 @@
       <c r="G21" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="J21" s="9"/>
+      <c r="J21" s="9" t="s">
+        <v>126</v>
+      </c>
       <c r="K21" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="N21" s="6"/>
       <c r="O21" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="R21" s="6"/>
       <c r="S21" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="V21" s="6"/>
       <c r="W21" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="8"/>
       <c r="C22" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N22" s="6"/>
       <c r="O22" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="R22" s="8"/>
+        <v>134</v>
+      </c>
+      <c r="R22" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="S22" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="V22" s="8"/>
+        <v>135</v>
+      </c>
+      <c r="V22" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="W22" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="8"/>
       <c r="C23" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="N23" s="8"/>
+        <v>139</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="O23" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R23" s="8"/>
       <c r="S23" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="V23" s="9"/>
+        <v>141</v>
+      </c>
+      <c r="V23" s="9" t="s">
+        <v>126</v>
+      </c>
       <c r="W23" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="9" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>143</v>
@@ -2768,214 +2886,232 @@
       <c r="G25" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="J25" s="10"/>
+      <c r="J25" s="10" t="s">
+        <v>151</v>
+      </c>
       <c r="K25" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="N25" s="8"/>
       <c r="O25" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="R25" s="8"/>
       <c r="S25" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="V25" s="9"/>
       <c r="W25" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="9"/>
       <c r="C26" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="J26" s="10"/>
       <c r="K26" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="N26" s="9"/>
+        <v>158</v>
+      </c>
+      <c r="N26" s="9" t="s">
+        <v>126</v>
+      </c>
       <c r="O26" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="R26" s="9"/>
+        <v>159</v>
+      </c>
+      <c r="R26" s="9" t="s">
+        <v>126</v>
+      </c>
       <c r="S26" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="V26" s="10"/>
+        <v>160</v>
+      </c>
+      <c r="V26" s="10" t="s">
+        <v>151</v>
+      </c>
       <c r="W26" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="9"/>
       <c r="C27" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J27" s="10"/>
       <c r="K27" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N27" s="9"/>
       <c r="O27" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="R27" s="9"/>
       <c r="S27" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="V27" s="10"/>
       <c r="W27" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="9"/>
       <c r="C28" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="J28" s="11"/>
+        <v>169</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>170</v>
+      </c>
       <c r="K28" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="N28" s="9"/>
       <c r="O28" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="R28" s="9"/>
       <c r="S28" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="V28" s="10"/>
       <c r="W28" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="10" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J29" s="11"/>
       <c r="K29" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="N29" s="10"/>
+        <v>177</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>151</v>
+      </c>
       <c r="O29" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="R29" s="9"/>
       <c r="S29" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="V29" s="10"/>
       <c r="W29" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="10"/>
       <c r="C30" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J30" s="11"/>
       <c r="K30" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N30" s="10"/>
       <c r="O30" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="R30" s="10"/>
+        <v>184</v>
+      </c>
+      <c r="R30" s="10" t="s">
+        <v>151</v>
+      </c>
       <c r="S30" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="V30" s="11"/>
+        <v>185</v>
+      </c>
+      <c r="V30" s="11" t="s">
+        <v>170</v>
+      </c>
       <c r="W30" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="10"/>
       <c r="C31" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J31" s="11"/>
       <c r="K31" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="N31" s="10"/>
       <c r="O31" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="R31" s="10"/>
       <c r="S31" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="V31" s="11"/>
       <c r="W31" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="10"/>
       <c r="C32" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="J32" s="11"/>
       <c r="K32" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="N32" s="11"/>
+        <v>195</v>
+      </c>
+      <c r="N32" s="11" t="s">
+        <v>170</v>
+      </c>
       <c r="O32" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="R32" s="10"/>
       <c r="S32" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="V32" s="11"/>
       <c r="W32" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="11" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>199</v>
@@ -2988,7 +3124,9 @@
       <c r="O33" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="R33" s="11"/>
+      <c r="R33" s="11" t="s">
+        <v>170</v>
+      </c>
       <c r="S33" s="0" t="s">
         <v>202</v>
       </c>
@@ -3025,7 +3163,7 @@
         <v>209</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="G35" s="0" t="s">
         <v>210</v>
@@ -3129,27 +3267,39 @@
       <c r="W45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="3"/>
+      <c r="B46" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C46" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="F46" s="3"/>
+      <c r="F46" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="G46" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="J46" s="3"/>
+      <c r="J46" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="K46" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="N46" s="3"/>
+      <c r="N46" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="O46" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="R46" s="3"/>
+      <c r="R46" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="S46" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="V46" s="3"/>
+      <c r="V46" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="W46" s="0" t="s">
         <v>233</v>
       </c>
@@ -3181,11 +3331,15 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="5"/>
+      <c r="B48" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="C48" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="F48" s="5"/>
+      <c r="F48" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="G48" s="0" t="s">
         <v>241</v>
       </c>
@@ -3197,7 +3351,7 @@
       <c r="O48" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="R48" s="5"/>
+      <c r="R48" s="3"/>
       <c r="S48" s="0" t="s">
         <v>244</v>
       </c>
@@ -3215,7 +3369,9 @@
       <c r="G49" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="J49" s="5"/>
+      <c r="J49" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K49" s="0" t="s">
         <v>248</v>
       </c>
@@ -3223,7 +3379,9 @@
       <c r="O49" s="0" t="s">
         <v>249</v>
       </c>
-      <c r="R49" s="5"/>
+      <c r="R49" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="S49" s="0" t="s">
         <v>250</v>
       </c>
@@ -3246,7 +3404,7 @@
       <c r="K50" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="N50" s="5"/>
+      <c r="N50" s="3"/>
       <c r="O50" s="0" t="s">
         <v>255</v>
       </c>
@@ -3272,7 +3430,9 @@
       <c r="K51" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="N51" s="5"/>
+      <c r="N51" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="O51" s="0" t="s">
         <v>261</v>
       </c>
@@ -3306,7 +3466,9 @@
       <c r="S52" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="V52" s="5"/>
+      <c r="V52" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="W52" s="0" t="s">
         <v>269</v>
       </c>
@@ -3328,7 +3490,7 @@
       <c r="O53" s="0" t="s">
         <v>273</v>
       </c>
-      <c r="R53" s="6"/>
+      <c r="R53" s="5"/>
       <c r="S53" s="0" t="s">
         <v>274</v>
       </c>
@@ -3346,7 +3508,9 @@
       <c r="G54" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="J54" s="6"/>
+      <c r="J54" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="K54" s="0" t="s">
         <v>278</v>
       </c>
@@ -3354,7 +3518,9 @@
       <c r="O54" s="0" t="s">
         <v>279</v>
       </c>
-      <c r="R54" s="6"/>
+      <c r="R54" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="S54" s="0" t="s">
         <v>280</v>
       </c>
@@ -3390,7 +3556,9 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="6"/>
+      <c r="B56" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="C56" s="0" t="s">
         <v>288</v>
       </c>
@@ -3420,7 +3588,9 @@
       <c r="C57" s="0" t="s">
         <v>294</v>
       </c>
-      <c r="F57" s="6"/>
+      <c r="F57" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="G57" s="0" t="s">
         <v>295</v>
       </c>
@@ -3454,7 +3624,9 @@
       <c r="K58" s="0" t="s">
         <v>302</v>
       </c>
-      <c r="N58" s="6"/>
+      <c r="N58" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="O58" s="0" t="s">
         <v>303</v>
       </c>
@@ -3462,7 +3634,9 @@
       <c r="S58" s="0" t="s">
         <v>304</v>
       </c>
-      <c r="V58" s="6"/>
+      <c r="V58" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="W58" s="0" t="s">
         <v>305</v>
       </c>
@@ -3510,7 +3684,7 @@
       <c r="O60" s="0" t="s">
         <v>315</v>
       </c>
-      <c r="R60" s="8"/>
+      <c r="R60" s="6"/>
       <c r="S60" s="0" t="s">
         <v>316</v>
       </c>
@@ -3520,7 +3694,9 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="8"/>
+      <c r="B61" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="C61" s="0" t="s">
         <v>318</v>
       </c>
@@ -3536,7 +3712,9 @@
       <c r="O61" s="0" t="s">
         <v>321</v>
       </c>
-      <c r="R61" s="8"/>
+      <c r="R61" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="S61" s="0" t="s">
         <v>322</v>
       </c>
@@ -3588,7 +3766,7 @@
       <c r="O63" s="0" t="s">
         <v>333</v>
       </c>
-      <c r="R63" s="9"/>
+      <c r="R63" s="8"/>
       <c r="S63" s="0" t="s">
         <v>334</v>
       </c>
@@ -3606,7 +3784,9 @@
       <c r="G64" s="0" t="s">
         <v>337</v>
       </c>
-      <c r="J64" s="8"/>
+      <c r="J64" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="K64" s="0" t="s">
         <v>338</v>
       </c>
@@ -3614,7 +3794,9 @@
       <c r="O64" s="0" t="s">
         <v>339</v>
       </c>
-      <c r="R64" s="9"/>
+      <c r="R64" s="9" t="s">
+        <v>126</v>
+      </c>
       <c r="S64" s="0" t="s">
         <v>340</v>
       </c>
@@ -3624,7 +3806,9 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="9"/>
+      <c r="B65" s="9" t="s">
+        <v>126</v>
+      </c>
       <c r="C65" s="0" t="s">
         <v>342</v>
       </c>
@@ -3654,7 +3838,9 @@
       <c r="C66" s="0" t="s">
         <v>348</v>
       </c>
-      <c r="F66" s="8"/>
+      <c r="F66" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="G66" s="0" t="s">
         <v>349</v>
       </c>
@@ -3670,7 +3856,9 @@
       <c r="S66" s="0" t="s">
         <v>352</v>
       </c>
-      <c r="V66" s="8"/>
+      <c r="V66" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="W66" s="0" t="s">
         <v>353</v>
       </c>
@@ -3684,15 +3872,21 @@
       <c r="G67" s="0" t="s">
         <v>355</v>
       </c>
-      <c r="J67" s="9"/>
+      <c r="J67" s="9" t="s">
+        <v>126</v>
+      </c>
       <c r="K67" s="0" t="s">
         <v>356</v>
       </c>
-      <c r="N67" s="8"/>
+      <c r="N67" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="O67" s="0" t="s">
         <v>357</v>
       </c>
-      <c r="R67" s="10"/>
+      <c r="R67" s="10" t="s">
+        <v>151</v>
+      </c>
       <c r="S67" s="0" t="s">
         <v>358</v>
       </c>
@@ -3728,11 +3922,15 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="10"/>
+      <c r="B69" s="10" t="s">
+        <v>151</v>
+      </c>
       <c r="C69" s="0" t="s">
         <v>366</v>
       </c>
-      <c r="F69" s="9"/>
+      <c r="F69" s="9" t="s">
+        <v>126</v>
+      </c>
       <c r="G69" s="0" t="s">
         <v>367</v>
       </c>
@@ -3766,7 +3964,9 @@
       <c r="K70" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="N70" s="9"/>
+      <c r="N70" s="9" t="s">
+        <v>126</v>
+      </c>
       <c r="O70" s="0" t="s">
         <v>375</v>
       </c>
@@ -3774,7 +3974,9 @@
       <c r="S70" s="0" t="s">
         <v>376</v>
       </c>
-      <c r="V70" s="9"/>
+      <c r="V70" s="9" t="s">
+        <v>126</v>
+      </c>
       <c r="W70" s="0" t="s">
         <v>377</v>
       </c>
@@ -3788,7 +3990,9 @@
       <c r="G71" s="0" t="s">
         <v>379</v>
       </c>
-      <c r="J71" s="10"/>
+      <c r="J71" s="10" t="s">
+        <v>151</v>
+      </c>
       <c r="K71" s="4" t="s">
         <v>380</v>
       </c>
@@ -3796,7 +4000,9 @@
       <c r="O71" s="0" t="s">
         <v>381</v>
       </c>
-      <c r="R71" s="11"/>
+      <c r="R71" s="11" t="s">
+        <v>170</v>
+      </c>
       <c r="S71" s="0" t="s">
         <v>382</v>
       </c>
@@ -3810,7 +4016,9 @@
       <c r="C72" s="0" t="s">
         <v>384</v>
       </c>
-      <c r="F72" s="10"/>
+      <c r="F72" s="10" t="s">
+        <v>151</v>
+      </c>
       <c r="G72" s="0" t="s">
         <v>385</v>
       </c>
@@ -3832,7 +4040,9 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="11"/>
+      <c r="B73" s="11" t="s">
+        <v>170</v>
+      </c>
       <c r="C73" s="0" t="s">
         <v>390</v>
       </c>
@@ -3844,7 +4054,9 @@
       <c r="K73" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="N73" s="10"/>
+      <c r="N73" s="10" t="s">
+        <v>151</v>
+      </c>
       <c r="O73" s="0" t="s">
         <v>393</v>
       </c>
@@ -3852,7 +4064,9 @@
       <c r="S73" s="0" t="s">
         <v>394</v>
       </c>
-      <c r="V73" s="10"/>
+      <c r="V73" s="10" t="s">
+        <v>151</v>
+      </c>
       <c r="W73" s="0" t="s">
         <v>395</v>
       </c>
@@ -3866,7 +4080,9 @@
       <c r="G74" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="J74" s="11"/>
+      <c r="J74" s="11" t="s">
+        <v>170</v>
+      </c>
       <c r="K74" s="4" t="s">
         <v>398</v>
       </c>
@@ -3888,7 +4104,9 @@
       <c r="C75" s="0" t="s">
         <v>402</v>
       </c>
-      <c r="F75" s="11"/>
+      <c r="F75" s="11" t="s">
+        <v>170</v>
+      </c>
       <c r="G75" s="0" t="s">
         <v>403</v>
       </c>
@@ -3944,11 +4162,15 @@
       <c r="K77" s="0" t="s">
         <v>414</v>
       </c>
-      <c r="N77" s="11"/>
+      <c r="N77" s="11" t="s">
+        <v>170</v>
+      </c>
       <c r="O77" s="0" t="s">
         <v>415</v>
       </c>
-      <c r="V77" s="11"/>
+      <c r="V77" s="11" t="s">
+        <v>170</v>
+      </c>
       <c r="W77" s="0" t="s">
         <v>416</v>
       </c>
@@ -4018,7 +4240,7 @@
       <c r="B83" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="94">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="J1:K1"/>
@@ -4027,19 +4249,43 @@
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="F2:F6"/>
-    <mergeCell ref="V2:V4"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="N2:N4"/>
+    <mergeCell ref="R2:R4"/>
+    <mergeCell ref="V3:V8"/>
+    <mergeCell ref="J4:J10"/>
+    <mergeCell ref="N5:N12"/>
+    <mergeCell ref="R5:R9"/>
     <mergeCell ref="B6:B11"/>
     <mergeCell ref="F7:F13"/>
+    <mergeCell ref="V9:V21"/>
+    <mergeCell ref="R10:R21"/>
+    <mergeCell ref="J11:J17"/>
     <mergeCell ref="B12:B19"/>
+    <mergeCell ref="N13:N22"/>
     <mergeCell ref="F14:F21"/>
+    <mergeCell ref="J18:J20"/>
     <mergeCell ref="B20:B23"/>
+    <mergeCell ref="J21:J24"/>
     <mergeCell ref="F22:F25"/>
-    <mergeCell ref="R22:R24"/>
+    <mergeCell ref="R22:R25"/>
+    <mergeCell ref="N23:N25"/>
+    <mergeCell ref="V23:V25"/>
     <mergeCell ref="B24:B28"/>
+    <mergeCell ref="J25:J27"/>
     <mergeCell ref="F26:F28"/>
+    <mergeCell ref="N26:N28"/>
+    <mergeCell ref="R26:R29"/>
+    <mergeCell ref="V26:V29"/>
+    <mergeCell ref="J28:J32"/>
     <mergeCell ref="B29:B32"/>
     <mergeCell ref="F29:F34"/>
+    <mergeCell ref="N29:N31"/>
+    <mergeCell ref="R30:R32"/>
+    <mergeCell ref="V30:V34"/>
+    <mergeCell ref="N32:N35"/>
     <mergeCell ref="B33:B38"/>
+    <mergeCell ref="R33:R38"/>
     <mergeCell ref="F35:F38"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="F45:G45"/>
@@ -4047,7 +4293,48 @@
     <mergeCell ref="N45:O45"/>
     <mergeCell ref="R45:S45"/>
     <mergeCell ref="V45:W45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="J46:J48"/>
+    <mergeCell ref="N46:N50"/>
+    <mergeCell ref="R46:R48"/>
+    <mergeCell ref="V46:V51"/>
+    <mergeCell ref="B48:B55"/>
+    <mergeCell ref="F48:F56"/>
+    <mergeCell ref="J49:J53"/>
+    <mergeCell ref="R49:R53"/>
+    <mergeCell ref="N51:N57"/>
+    <mergeCell ref="V52:V57"/>
+    <mergeCell ref="J54:J63"/>
+    <mergeCell ref="R54:R60"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="F57:F65"/>
+    <mergeCell ref="N58:N66"/>
+    <mergeCell ref="V58:V65"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="R61:R63"/>
+    <mergeCell ref="J64:J66"/>
+    <mergeCell ref="R64:R66"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="F66:F68"/>
+    <mergeCell ref="V66:V69"/>
+    <mergeCell ref="J67:J70"/>
+    <mergeCell ref="N67:N69"/>
+    <mergeCell ref="R67:R70"/>
+    <mergeCell ref="B69:B72"/>
+    <mergeCell ref="F69:F71"/>
+    <mergeCell ref="N70:N72"/>
+    <mergeCell ref="V70:V72"/>
+    <mergeCell ref="J71:J73"/>
+    <mergeCell ref="R71:R75"/>
+    <mergeCell ref="F72:F74"/>
+    <mergeCell ref="B73:B78"/>
+    <mergeCell ref="N73:N76"/>
+    <mergeCell ref="V73:V76"/>
+    <mergeCell ref="J74:J80"/>
     <mergeCell ref="F75:F78"/>
+    <mergeCell ref="N77:N80"/>
+    <mergeCell ref="V77:V81"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4067,7 +4354,7 @@
   <dimension ref="A1:BG125"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4124,155 +4411,245 @@
       <c r="A2" s="0" t="s">
         <v>435</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>436</v>
+      </c>
       <c r="D2" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>438</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>437</v>
+        <v>439</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>440</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>438</v>
+        <v>441</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>442</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>439</v>
+        <v>443</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>444</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>440</v>
+        <v>445</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>446</v>
       </c>
       <c r="BG2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>441</v>
+        <v>447</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>448</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>442</v>
+        <v>449</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>450</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>443</v>
+        <v>451</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>452</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>444</v>
+        <v>453</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>454</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>445</v>
+        <v>455</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>456</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>446</v>
+        <v>457</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>458</v>
       </c>
       <c r="BG3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>447</v>
+        <v>459</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>460</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>448</v>
+        <v>461</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>462</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>449</v>
+        <v>463</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>464</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>450</v>
+        <v>465</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>466</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>451</v>
+        <v>467</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>468</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>452</v>
+        <v>469</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>470</v>
       </c>
       <c r="BG4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>453</v>
+        <v>471</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>473</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>454</v>
+        <v>474</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>475</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>455</v>
+        <v>476</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>477</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>456</v>
+        <v>478</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>480</v>
       </c>
       <c r="BG5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>457</v>
+        <v>481</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>484</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>458</v>
+        <v>485</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>486</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>459</v>
+        <v>487</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>489</v>
       </c>
       <c r="BG6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>460</v>
+        <v>490</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>461</v>
+        <v>491</v>
       </c>
       <c r="BG7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>462</v>
+        <v>492</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>463</v>
+        <v>493</v>
       </c>
       <c r="BG8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>464</v>
+        <v>494</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>465</v>
+        <v>495</v>
       </c>
       <c r="BG9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>466</v>
+        <v>496</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>467</v>
+        <v>497</v>
       </c>
       <c r="BG10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>468</v>
+        <v>498</v>
       </c>
       <c r="BG11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>469</v>
+        <v>499</v>
       </c>
       <c r="BG12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>470</v>
+        <v>500</v>
       </c>
       <c r="BG13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>471</v>
+        <v>501</v>
       </c>
       <c r="BG14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>472</v>
+        <v>502</v>
       </c>
       <c r="BG15" s="0"/>
     </row>
@@ -4293,141 +4670,231 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>473</v>
+        <v>503</v>
       </c>
       <c r="B21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>474</v>
+        <v>504</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="14"/>
       <c r="G21" s="1" t="s">
-        <v>475</v>
+        <v>505</v>
       </c>
       <c r="H21" s="1"/>
       <c r="J21" s="1" t="s">
-        <v>476</v>
+        <v>506</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="14"/>
       <c r="M21" s="1" t="s">
-        <v>477</v>
+        <v>507</v>
       </c>
       <c r="N21" s="1"/>
       <c r="P21" s="1" t="s">
-        <v>478</v>
+        <v>508</v>
       </c>
       <c r="Q21" s="1"/>
       <c r="BG21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>479</v>
+        <v>509</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>510</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>479</v>
+        <v>509</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>511</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>480</v>
+        <v>512</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>513</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>481</v>
+        <v>514</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>515</v>
       </c>
       <c r="M22" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="N22" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="P22" s="0" t="s">
+        <v>517</v>
+      </c>
+      <c r="Q22" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="BG22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>522</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="N23" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="P23" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q23" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="BG23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="s">
+        <v>528</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>529</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>531</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>532</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>533</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>534</v>
+      </c>
+      <c r="N24" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="P24" s="0" t="s">
+        <v>535</v>
+      </c>
+      <c r="Q24" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="BG24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>537</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>541</v>
+      </c>
+      <c r="K25" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="M25" s="0" t="s">
+        <v>543</v>
+      </c>
+      <c r="N25" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="P25" s="0" t="s">
+        <v>544</v>
+      </c>
+      <c r="Q25" s="0" t="s">
+        <v>545</v>
+      </c>
+      <c r="BG25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>546</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>549</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>550</v>
+      </c>
+      <c r="K26" s="0" t="s">
+        <v>551</v>
+      </c>
+      <c r="N26" s="0" t="s">
         <v>482</v>
       </c>
-      <c r="P22" s="0" t="s">
-        <v>483</v>
-      </c>
-      <c r="BG22" s="0"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G23" s="0" t="s">
-        <v>484</v>
-      </c>
-      <c r="J23" s="0" t="s">
-        <v>485</v>
-      </c>
-      <c r="M23" s="0" t="s">
-        <v>486</v>
-      </c>
-      <c r="P23" s="0" t="s">
-        <v>487</v>
-      </c>
-      <c r="BG23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G24" s="0" t="s">
-        <v>488</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>489</v>
-      </c>
-      <c r="M24" s="0" t="s">
-        <v>490</v>
-      </c>
-      <c r="P24" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="BG24" s="0"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G25" s="0" t="s">
-        <v>492</v>
-      </c>
-      <c r="J25" s="0" t="s">
-        <v>493</v>
-      </c>
-      <c r="M25" s="0" t="s">
-        <v>494</v>
-      </c>
-      <c r="P25" s="0" t="s">
-        <v>495</v>
-      </c>
-      <c r="BG25" s="0"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G26" s="0" t="s">
-        <v>496</v>
-      </c>
-      <c r="J26" s="0" t="s">
-        <v>497</v>
-      </c>
       <c r="P26" s="0" t="s">
-        <v>498</v>
+        <v>552</v>
+      </c>
+      <c r="Q26" s="0" t="s">
+        <v>553</v>
       </c>
       <c r="BG26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G27" s="0" t="s">
-        <v>499</v>
+        <v>554</v>
       </c>
       <c r="P27" s="0" t="s">
-        <v>500</v>
+        <v>555</v>
       </c>
       <c r="BG27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G28" s="0" t="s">
-        <v>501</v>
+        <v>556</v>
       </c>
       <c r="BG28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>502</v>
+        <v>557</v>
       </c>
       <c r="BG29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>503</v>
+        <v>558</v>
       </c>
       <c r="BG30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>504</v>
+        <v>559</v>
       </c>
       <c r="BG31" s="0"/>
     </row>
@@ -4626,151 +5093,151 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>505</v>
+        <v>560</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>506</v>
+        <v>561</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>507</v>
+        <v>562</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>508</v>
+        <v>563</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>509</v>
+        <v>564</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>510</v>
+        <v>565</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>511</v>
+        <v>566</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>512</v>
+        <v>567</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>513</v>
+        <v>568</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>514</v>
+        <v>569</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>515</v>
+        <v>570</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>429</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>516</v>
+        <v>571</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>514</v>
+        <v>569</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>517</v>
+        <v>572</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>518</v>
+        <v>573</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>519</v>
+        <v>574</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>520</v>
+        <v>575</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>521</v>
+        <v>576</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>522</v>
+        <v>577</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>523</v>
+        <v>578</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>524</v>
+        <v>579</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>525</v>
+        <v>580</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>526</v>
+        <v>581</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>527</v>
+        <v>582</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>528</v>
+        <v>583</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>529</v>
+        <v>584</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>530</v>
+        <v>585</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>531</v>
+        <v>586</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>532</v>
+        <v>587</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>533</v>
+        <v>588</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>534</v>
+        <v>589</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>535</v>
+        <v>590</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>536</v>
+        <v>591</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>537</v>
+        <v>592</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>538</v>
+        <v>593</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>539</v>
+        <v>594</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>514</v>
+        <v>569</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>540</v>
+        <v>595</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>541</v>
+        <v>596</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>542</v>
+        <v>597</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4819,7 +5286,7 @@
   <dimension ref="A1:H263"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4831,7 +5298,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>543</v>
+        <v>598</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -5032,555 +5499,307 @@
       <c r="H20" s="20"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22"/>
+      <c r="B21" s="21"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="21"/>
-      <c r="B22" s="22"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="21"/>
-      <c r="B23" s="23"/>
+      <c r="B22" s="21"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="24"/>
-      <c r="B24" s="22"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="21"/>
-      <c r="B25" s="22"/>
+      <c r="B25" s="21"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="21"/>
-      <c r="B26" s="22"/>
+      <c r="B26" s="21"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="21"/>
-      <c r="B27" s="22"/>
+      <c r="B27" s="21"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="21"/>
-      <c r="B28" s="22"/>
+      <c r="B28" s="21"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="21"/>
-      <c r="B29" s="22"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="21"/>
-      <c r="B30" s="23"/>
+      <c r="B29" s="21"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="24"/>
-      <c r="B31" s="22"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="21"/>
-      <c r="B32" s="22"/>
+      <c r="B32" s="21"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="21"/>
-      <c r="B33" s="22"/>
+      <c r="B33" s="21"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="21"/>
-      <c r="B34" s="22"/>
+      <c r="B34" s="21"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="21"/>
-      <c r="B35" s="22"/>
+      <c r="B35" s="21"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="21"/>
-      <c r="B36" s="22"/>
+      <c r="B36" s="21"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="21"/>
-      <c r="B37" s="22"/>
+      <c r="B37" s="21"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="21"/>
-      <c r="B38" s="22"/>
+      <c r="B38" s="21"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="21"/>
-      <c r="B39" s="22"/>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="21"/>
-      <c r="B40" s="23"/>
+      <c r="B39" s="21"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="24"/>
-      <c r="B41" s="22"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="21"/>
-      <c r="B42" s="22"/>
+      <c r="B42" s="21"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="21"/>
-      <c r="B43" s="22"/>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="21"/>
-      <c r="B44" s="23"/>
+      <c r="B43" s="21"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="24"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="21"/>
+      <c r="B45" s="21"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="21"/>
-      <c r="B46" s="22"/>
+      <c r="B46" s="21"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="21"/>
-      <c r="B47" s="22"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="21"/>
-      <c r="B48" s="23"/>
+      <c r="B47" s="21"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="24"/>
-      <c r="B49" s="22"/>
+      <c r="A49" s="21"/>
+      <c r="B49" s="21"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="21"/>
-      <c r="B50" s="22"/>
+      <c r="B50" s="21"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="21"/>
-      <c r="B51" s="22"/>
+      <c r="B51" s="21"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="21"/>
-      <c r="B52" s="22"/>
+      <c r="B52" s="21"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="21"/>
-      <c r="B53" s="22"/>
+      <c r="B53" s="21"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="21"/>
-      <c r="B54" s="22"/>
+      <c r="B54" s="21"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="21"/>
-      <c r="B55" s="22"/>
+      <c r="B55" s="21"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="21"/>
-      <c r="B56" s="22"/>
+      <c r="B56" s="21"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="21"/>
-      <c r="B57" s="22"/>
+      <c r="B57" s="21"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="25"/>
-      <c r="B58" s="26"/>
+      <c r="B58" s="21"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="27"/>
-      <c r="B60" s="28"/>
+      <c r="A60" s="15"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="21"/>
-      <c r="B61" s="29"/>
+      <c r="B61" s="15"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="21"/>
-      <c r="B62" s="29"/>
+      <c r="B62" s="15"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="25"/>
-      <c r="B63" s="30"/>
+      <c r="B63" s="15"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="27"/>
-      <c r="B65" s="31"/>
+      <c r="A65" s="15"/>
+      <c r="B65" s="15"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="21"/>
-      <c r="B66" s="29"/>
+      <c r="B66" s="15"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="21"/>
-      <c r="B67" s="29"/>
+      <c r="B67" s="15"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="21"/>
-      <c r="B68" s="29"/>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="21"/>
-      <c r="B69" s="23"/>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="21"/>
-      <c r="B70" s="23"/>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="21"/>
-      <c r="B71" s="23"/>
+      <c r="B68" s="15"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="21"/>
-      <c r="B72" s="29"/>
+      <c r="B72" s="15"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="21"/>
-      <c r="B73" s="29"/>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="21"/>
-      <c r="B74" s="23"/>
+      <c r="B73" s="15"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="21"/>
-      <c r="B75" s="29"/>
+      <c r="B75" s="15"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="21"/>
-      <c r="B76" s="29"/>
+      <c r="B76" s="15"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="21"/>
-      <c r="B77" s="29"/>
+      <c r="B77" s="15"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="25"/>
-      <c r="B78" s="30"/>
+      <c r="B78" s="15"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="27"/>
-      <c r="B80" s="28"/>
-    </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="21"/>
-      <c r="B81" s="23"/>
+      <c r="A80" s="15"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="25"/>
-      <c r="B82" s="30"/>
+      <c r="B82" s="15"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="27"/>
-      <c r="B84" s="28"/>
-    </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="21"/>
-      <c r="B85" s="23"/>
+      <c r="A84" s="15"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="25"/>
-      <c r="B86" s="30"/>
+      <c r="B86" s="15"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="27"/>
-      <c r="B88" s="28"/>
-    </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="21"/>
-      <c r="B89" s="23"/>
-    </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="21"/>
-      <c r="B90" s="23"/>
+      <c r="A88" s="15"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="25"/>
-      <c r="B91" s="30"/>
+      <c r="B91" s="15"/>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="27"/>
-      <c r="B93" s="28"/>
+      <c r="A93" s="15"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="25"/>
-      <c r="B94" s="30"/>
+      <c r="B94" s="15"/>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="27"/>
-      <c r="B96" s="31"/>
+      <c r="A96" s="15"/>
+      <c r="B96" s="15"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="21"/>
-      <c r="B97" s="29"/>
+      <c r="B97" s="15"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="21"/>
-      <c r="B98" s="29"/>
+      <c r="B98" s="15"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="21"/>
-      <c r="B99" s="29"/>
+      <c r="B99" s="15"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="21"/>
-      <c r="B100" s="29"/>
+      <c r="B100" s="15"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="25"/>
-      <c r="B101" s="30"/>
+      <c r="B101" s="15"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="27"/>
-      <c r="B103" s="31"/>
+      <c r="A103" s="15"/>
+      <c r="B103" s="15"/>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="21"/>
-      <c r="B104" s="29"/>
+      <c r="B104" s="15"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="21"/>
-      <c r="B105" s="29"/>
+      <c r="B105" s="15"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="21"/>
-      <c r="B106" s="29"/>
+      <c r="B106" s="15"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="21"/>
-      <c r="B107" s="29"/>
+      <c r="B107" s="15"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="21"/>
-      <c r="B108" s="29"/>
+      <c r="B108" s="15"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="25"/>
-      <c r="B109" s="30"/>
+      <c r="B109" s="15"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F110" s="13"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="27"/>
-      <c r="B111" s="28"/>
-    </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="21"/>
-      <c r="B112" s="23"/>
-    </row>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="21"/>
-      <c r="B113" s="23"/>
-    </row>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="21"/>
-      <c r="B114" s="23"/>
+      <c r="A111" s="15"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="25"/>
-      <c r="B115" s="30"/>
+      <c r="B115" s="15"/>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="27"/>
-      <c r="B117" s="28"/>
-    </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="21"/>
-      <c r="B118" s="23"/>
+      <c r="A117" s="15"/>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="25"/>
-      <c r="B119" s="30"/>
+      <c r="B119" s="15"/>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="27"/>
-      <c r="B121" s="28"/>
-    </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="21"/>
-      <c r="B122" s="23"/>
-    </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="21"/>
-      <c r="B123" s="23"/>
+      <c r="A121" s="15"/>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="25"/>
-      <c r="B124" s="30"/>
+      <c r="B124" s="15"/>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="27"/>
-      <c r="B126" s="28"/>
-    </row>
-    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="21"/>
-      <c r="B127" s="23"/>
-    </row>
-    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="21"/>
-      <c r="B128" s="23"/>
+      <c r="A126" s="15"/>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="25"/>
-      <c r="B129" s="30"/>
+      <c r="B129" s="15"/>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="27"/>
-      <c r="B131" s="28"/>
-    </row>
-    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="21"/>
-      <c r="B132" s="23"/>
+      <c r="A131" s="15"/>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="25"/>
-      <c r="B133" s="30"/>
+      <c r="B133" s="15"/>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="27"/>
-      <c r="B135" s="28"/>
-    </row>
-    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="21"/>
-      <c r="B136" s="23"/>
+      <c r="A135" s="15"/>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="25"/>
-      <c r="B137" s="30"/>
+      <c r="B137" s="15"/>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="27"/>
-      <c r="B140" s="28"/>
-    </row>
-    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="21"/>
-      <c r="B141" s="23"/>
+      <c r="A140" s="15"/>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="25"/>
-      <c r="B142" s="30"/>
+      <c r="B142" s="15"/>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="27"/>
-      <c r="B144" s="28"/>
-    </row>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="21"/>
-      <c r="B145" s="23"/>
+      <c r="A144" s="15"/>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="25"/>
-      <c r="B146" s="30"/>
+      <c r="B146" s="15"/>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="27"/>
-      <c r="B148" s="28"/>
-    </row>
-    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="21"/>
-      <c r="B149" s="23"/>
+      <c r="A148" s="15"/>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="25"/>
-      <c r="B150" s="30"/>
+      <c r="B150" s="15"/>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="27"/>
-      <c r="B152" s="28"/>
-    </row>
-    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="21"/>
-      <c r="B153" s="23"/>
-    </row>
-    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="21"/>
-      <c r="B154" s="23"/>
-    </row>
-    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="21"/>
-      <c r="B155" s="23"/>
-    </row>
-    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="21"/>
-      <c r="B156" s="23"/>
+      <c r="A152" s="15"/>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="25"/>
-      <c r="B157" s="30"/>
+      <c r="B157" s="15"/>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="27"/>
-      <c r="B159" s="28"/>
+      <c r="A159" s="15"/>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="25"/>
-      <c r="B160" s="30"/>
+      <c r="B160" s="15"/>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="27"/>
-      <c r="B162" s="28"/>
-    </row>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="21"/>
-      <c r="B163" s="23"/>
-    </row>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="21"/>
-      <c r="B164" s="23"/>
-    </row>
-    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="21"/>
-      <c r="B165" s="23"/>
-    </row>
-    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="21"/>
-      <c r="B166" s="23"/>
+      <c r="A162" s="15"/>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="25"/>
-      <c r="B167" s="30"/>
+      <c r="B167" s="15"/>
       <c r="F167" s="13"/>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="27"/>
-      <c r="B169" s="28"/>
-    </row>
-    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="21"/>
-      <c r="B170" s="23"/>
-    </row>
-    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="21"/>
-      <c r="B171" s="23"/>
-    </row>
-    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="21"/>
-      <c r="B172" s="23"/>
+      <c r="A169" s="15"/>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="25"/>
-      <c r="B173" s="30"/>
+      <c r="B173" s="15"/>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="27"/>
-      <c r="B175" s="28"/>
-    </row>
-    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="21"/>
-      <c r="B176" s="23"/>
-    </row>
-    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="21"/>
-      <c r="B177" s="23"/>
-    </row>
-    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="21"/>
-      <c r="B178" s="23"/>
+      <c r="A175" s="15"/>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="25"/>
-      <c r="B179" s="30"/>
+      <c r="B179" s="15"/>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E191" s="13"/>
@@ -5593,23 +5812,23 @@
       <c r="F222" s="13"/>
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F248" s="32"/>
+      <c r="F248" s="22"/>
       <c r="G248" s="0"/>
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F249" s="32"/>
+      <c r="F249" s="22"/>
       <c r="G249" s="0"/>
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F250" s="32"/>
+      <c r="F250" s="22"/>
       <c r="G250" s="0"/>
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F251" s="32"/>
+      <c r="F251" s="22"/>
       <c r="G251" s="0"/>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F252" s="32"/>
+      <c r="F252" s="22"/>
       <c r="G252" s="0"/>
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5649,11 +5868,11 @@
       <c r="G261" s="0"/>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F262" s="32"/>
+      <c r="F262" s="22"/>
       <c r="G262" s="0"/>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F263" s="32"/>
+      <c r="F263" s="22"/>
       <c r="G263" s="0"/>
     </row>
   </sheetData>
@@ -5675,7 +5894,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="B1:B43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
@@ -5687,209 +5906,61 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.19"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="33"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-    </row>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
+      <c r="B4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="33"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
+      <c r="B5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="33"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
+      <c r="B6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="33"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-    </row>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="33"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-    </row>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="33"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="33"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="33"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="33"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-    </row>
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="33"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="33"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="33"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="33"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="33"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="33"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="33"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="33"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="33"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="33"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="33"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-    </row>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>